<commit_message>
Updating results from laptop and gitignore
</commit_message>
<xml_diff>
--- a/results/embedding/spreadsheet25_embedding_pegasus_0.xlsx
+++ b/results/embedding/spreadsheet25_embedding_pegasus_0.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -54,18 +54,86 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -358,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS7"/>
+  <dimension ref="A1:AK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,160 +497,120 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>full_embed_l</t>
+          <t>heur_avgl_l</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>full_embed_n</t>
+          <t>heur_avgl_n</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>full_length_l</t>
+          <t>heur_avgt_l</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>full_length_n</t>
+          <t>heur_avgt_n</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
-          <t>full_time_l</t>
+          <t>heur_best_embed_l</t>
         </is>
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>full_time_n</t>
+          <t>heur_best_embed_n</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
         <is>
-          <t>heur_avgl_l</t>
+          <t>heur_best_length_l</t>
         </is>
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>heur_avgl_n</t>
+          <t>heur_best_length_n</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>heur_avgt_l</t>
+          <t>heur_best_time_l</t>
         </is>
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>heur_avgt_n</t>
+          <t>heur_best_time_n</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
         <is>
-          <t>heur_best_embed_l</t>
+          <t>heur_lengths_l</t>
         </is>
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>heur_best_embed_n</t>
+          <t>heur_lengths_n</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
         <is>
-          <t>heur_best_length_l</t>
+          <t>heur_stdevl_l</t>
         </is>
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>heur_best_length_n</t>
+          <t>heur_stdevl_n</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
         <is>
-          <t>heur_best_time_l</t>
+          <t>heur_succ_l</t>
         </is>
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>heur_best_time_n</t>
+          <t>heur_succ_n</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
         <is>
-          <t>heur_embeds_l</t>
+          <t>heur_times_l</t>
         </is>
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>heur_embeds_n</t>
+          <t>heur_times_n</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
         <is>
-          <t>heur_lengths_l</t>
+          <t>n_edges_l</t>
         </is>
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>heur_lengths_n</t>
+          <t>n_edges_n</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
         <is>
-          <t>heur_stdevl_l</t>
+          <t>n_nodes_l</t>
         </is>
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>heur_stdevl_n</t>
+          <t>n_nodes_n</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
         <is>
-          <t>heur_succ_l</t>
+          <t>nodes_l</t>
         </is>
       </c>
       <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>heur_succ_n</t>
-        </is>
-      </c>
-      <c r="AL1" s="1" t="inlineStr">
-        <is>
-          <t>heur_times_l</t>
-        </is>
-      </c>
-      <c r="AM1" s="1" t="inlineStr">
-        <is>
-          <t>heur_times_n</t>
-        </is>
-      </c>
-      <c r="AN1" s="1" t="inlineStr">
-        <is>
-          <t>n_edges_l</t>
-        </is>
-      </c>
-      <c r="AO1" s="1" t="inlineStr">
-        <is>
-          <t>n_edges_n</t>
-        </is>
-      </c>
-      <c r="AP1" s="1" t="inlineStr">
-        <is>
-          <t>n_nodes_l</t>
-        </is>
-      </c>
-      <c r="AQ1" s="1" t="inlineStr">
-        <is>
-          <t>n_nodes_n</t>
-        </is>
-      </c>
-      <c r="AR1" s="1" t="inlineStr">
-        <is>
-          <t>nodes_l</t>
-        </is>
-      </c>
-      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>nodes_n</t>
         </is>
@@ -606,7 +634,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>[(0, 1), (0, 0), (1, 1), (2, 2)]</t>
+          <t>[(0, 1)]</t>
         </is>
       </c>
       <c r="G2" t="n">
@@ -621,14 +649,14 @@
         <v>0.002534468157697533</v>
       </c>
       <c r="J2" t="n">
-        <v>0.6190476190476191</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="K2" t="n">
         <v>1.333333333333333</v>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[(0, 1), (0, 's_0_1'), (0, 's_0_0'), (0, 0), (1, 's_0_1'), (1, 's_1_1'), (1, 1), ('s_0_1', 's_0_1'), ('s_0_0', 's_0_0'), ('s_1_1', 's_1_1'), (2, 's_2_2'), (2, 2), ('s_2_2', 's_2_2')]</t>
+          <t>[(0, 1), (0, 's_0_1'), (0, 0), (1, 's_0_1'), (1, 1), ('s_0_1', 's_0_1'), (2, 2)]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -636,122 +664,90 @@
           <t>[(0, 1), (0, 0), (1, 1), (2, 2)]</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>{0: [548, 549, 4352], 1: [4367, 564, 563], 2: [517, 518, 4382], 3: [532, 533, 4397], 4: [4412, 488], 5: [503, 4427], 6: [4441, 4442, 457, 458], 7: [472, 4456, 4457, 473], 8: [579, 4532, 578], 9: [593, 4547, 594], 10: [608, 4502], 11: [4517, 623], 12: [428, 4471, 4472]}</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>{0: [4934, 2590], 1: [4949, 2605], 2: [2561, 4964], 3: [4979, 2576]}</t>
-        </is>
+      <c r="N2" t="n">
+        <v>4</v>
+      </c>
+      <c r="O2" t="n">
+        <v>3</v>
       </c>
       <c r="P2" t="n">
-        <v>37</v>
+        <v>0.03637886047363281</v>
       </c>
       <c r="Q2" t="n">
-        <v>8</v>
-      </c>
-      <c r="R2" t="n">
-        <v>221.3675539493561</v>
-      </c>
-      <c r="S2" t="n">
-        <v>54.19483518600464</v>
+        <v>0.0387723445892334</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>{0: [4498], 1: [2498], 's_0_1': [4483], 2: [631]}</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>{0: [174], 1: [4665], 2: [727]}</t>
+        </is>
       </c>
       <c r="T2" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="U2" t="n">
         <v>3</v>
       </c>
       <c r="V2" t="n">
-        <v>0.02719783782958984</v>
+        <v>0.03643989562988281</v>
       </c>
       <c r="W2" t="n">
-        <v>0.02245426177978516</v>
+        <v>0.05267167091369629</v>
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>{0: [5105], 1: [971], 's_0_1': [986], 's_0_0': [1001], 's_1_1': [5074], 2: [4350], 's_2_2': [262]}</t>
+          <t>[4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4, 4]</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>{0: [5641], 1: [359], 2: [726]}</t>
+          <t>[3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3]</t>
         </is>
       </c>
       <c r="Z2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>[0.03643989562988281, 0.05018925666809082, 0.05527520179748535, 0.04685068130493164, 0.03385806083679199, 0.029694795608520508, 0.036782026290893555, 0.040480852127075195, 0.03377723693847656, 0.028940677642822266, 0.028774499893188477, 0.03701972961425781, 0.029392004013061523, 0.028326749801635742, 0.03949856758117676, 0.03359484672546387, 0.030651330947875977, 0.02689957618713379, 0.031090497970581055, 0.02824544906616211, 0.02921319007873535, 0.03763151168823242, 0.03494596481323242, 0.04285311698913574, 0.0344233512878418, 0.040009498596191406, 0.04013395309448242, 0.0499265193939209, 0.03130841255187988, 0.03017878532409668, 0.036004066467285156, 0.03964877128601074, 0.03160834312438965, 0.03783249855041504, 0.04027056694030762, 0.03220534324645996, 0.04602622985839844, 0.031774044036865234, 0.027753829956054688, 0.03634047508239746, 0.036417245864868164, 0.038011789321899414, 0.038373708724975586, 0.04147958755493164, 0.03449654579162598, 0.04930448532104492, 0.031505584716796875, 0.03223776817321777, 0.044441938400268555, 0.03849387168884277, 0.03526163101196289, 0.03072667121887207, 0.038992881774902344, 0.03917098045349121, 0.03705644607543945, 0.042092084884643555, 0.042890071868896484, 0.04234623908996582, 0.03311562538146973, 0.0613560676574707, 0.05500960350036621, 0.05959653854370117, 0.0332026481628418, 0.043999433517456055, 0.03751206398010254, 0.04583120346069336, 0.04283404350280762, 0.04162883758544922, 0.03597307205200195, 0.03817439079284668, 0.03809833526611328, 0.04633378982543945, 0.031001806259155273, 0.042673349380493164, 0.030371665954589844, 0.03407931327819824, 0.03511810302734375, 0.059177398681640625, 0.042879581451416016, 0.05757617950439453, 0.03713798522949219, 0.03353524208068848, 0.03161048889160156, 0.03012990951538086, 0.03434181213378906, 0.03291177749633789, 0.03014206886291504, 0.0359959602355957, 0.02913689613342285, 0.026050806045532227, 0.02863311767578125, 0.039299726486206055, 0.0438840389251709, 0.029363393783569336, 0.0326695442199707, 0.04404807090759277, 0.033814191818237305, 0.0337986946105957, 0.036115407943725586, 0.0421140193939209]</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>[0.05267167091369629, 0.03606748580932617, 0.03778553009033203, 0.031976938247680664, 0.0355837345123291, 0.03499579429626465, 0.04675793647766113, 0.04025697708129883, 0.08804917335510254, 0.053986549377441406, 0.05891060829162598, 0.045092105865478516, 0.05089712142944336, 0.04537248611450195, 0.04838299751281738, 0.04060673713684082, 0.04150199890136719, 0.04821038246154785, 0.04338526725769043, 0.038580894470214844, 0.0343780517578125, 0.038292884826660156, 0.03551220893859863, 0.043840885162353516, 0.04336357116699219, 0.04575395584106445, 0.03216910362243652, 0.03383135795593262, 0.04115104675292969, 0.06128406524658203, 0.0461573600769043, 0.04688382148742676, 0.056194305419921875, 0.05626034736633301, 0.03115248680114746, 0.036394596099853516, 0.03739809989929199, 0.028683900833129883, 0.04053759574890137, 0.04780220985412598, 0.04904437065124512, 0.041730642318725586, 0.034313201904296875, 0.03269457817077637, 0.04080605506896973, 0.04074525833129883, 0.03877902030944824, 0.04902076721191406, 0.03264188766479492, 0.03137993812561035, 0.03108692169189453, 0.03623509407043457, 0.027086496353149414, 0.0362086296081543, 0.045205116271972656, 0.047196149826049805, 0.03706645965576172, 0.04755711555480957, 0.04587721824645996, 0.04298543930053711, 0.03831982612609863, 0.04903125762939453, 0.0419461727142334, 0.05499553680419922, 0.030585050582885742, 0.04509162902832031, 0.0319514274597168, 0.03126835823059082, 0.03353476524353027, 0.04542732238769531, 0.03822040557861328, 0.02910757064819336, 0.027399778366088867, 0.02561473846435547, 0.03668212890625, 0.04300332069396973, 0.038765668869018555, 0.03162527084350586, 0.04141426086425781, 0.041165828704833984, 0.03218817710876465, 0.03528714179992676, 0.034088134765625, 0.036989450454711914, 0.04440903663635254, 0.03541970252990723, 0.037499189376831055, 0.035813093185424805, 0.04645943641662598, 0.04324054718017578, 0.0441288948059082, 0.03911185264587402, 0.04614591598510742, 0.03673219680786133, 0.0294649600982666, 0.029333829879760742, 0.02910161018371582, 0.030271291732788086, 0.02729964256286621, 0.026276350021362305]</t>
+        </is>
+      </c>
+      <c r="AF2" t="n">
         <v>7</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AG2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI2" t="n">
         <v>3</v>
       </c>
-      <c r="AB2" t="n">
-        <v>0.03017973899841309</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.02548623085021973</v>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>[{0: [5105], 1: [971], 's_0_1': [986], 's_0_0': [1001], 's_1_1': [5074], 2: [4350], 's_2_2': [262]}, {0: [3256], 1: [346], 's_0_1': [331], 's_0_0': [316], 's_1_1': [3166], 2: [5416], 's_2_2': [403]}, {0: [5593], 1: [2489], 's_0_1': [2474], 's_0_0': [2504], 's_1_1': [5547], 2: [2588], 's_2_2': [4483]}, {0: [5688], 1: [644], 's_0_1': [659], 's_0_0': [614], 's_1_1': [5567], 2: [2570], 's_2_2': [3913]}, {0: [5399], 1: [5384], 's_0_1': [2713], 's_0_0': [5398], 's_1_1': [2698], 2: [2559], 's_2_2': [4589]}, {0: [1505], 1: [4012], 's_0_1': [1520], 's_0_0': [4028], 's_1_1': [4013], 2: [3578], 's_2_2': [1698]}, {0: [2087], 1: [2072], 's_0_1': [3431], 's_0_0': [2088], 's_1_1': [3461], 2: [5256], 's_2_2': [5255]}, {0: [5477], 1: [5462], 's_0_1': [554], 's_0_0': [463], 's_1_1': [508], 2: [720], 's_2_2': [2913]}, {0: [2605], 1: [2590], 's_0_1': [4843], 's_0_0': [5008], 's_1_1': [4858], 2: [452], 's_2_2': [3406]}, {0: [5593], 1: [2519], 's_0_1': [2504], 's_0_0': [5608], 's_1_1': [5668], 2: [4937], 's_2_2': [551]}, {0: [3061], 1: [3076], 's_0_1': [390], 's_0_0': [360], 's_1_1': [375], 2: [3575], 's_2_2': [1128]}, {0: [1358], 1: [1373], 's_0_1': [4597], 's_0_0': [4507], 's_1_1': [4612], 2: [1146], 's_2_2': [4280]}, {0: [1831], 1: [3219], 's_0_1': [3234], 's_0_0': [3189], 's_1_1': [1936], 2: [1181], 's_2_2': [5061]}, {0: [2745], 1: [3044], 's_0_1': [2730], 's_0_0': [2939], 's_1_1': [2715], 2: [2455], 's_2_2': [2440]}, {0: [3375], 1: [3360], 's_0_1': [227], 's_0_0': [286], 's_1_1': [256], 2: [2769], 's_2_2': [2784]}, {0: [824], 1: [5644], 's_0_1': [5659], 's_0_0': [5568], 's_1_1': [5643], 2: [5439], 's_2_2': [1738]}, {0: [5328], 1: [642], 's_0_1': [5313], 's_0_0': [598], 's_1_1': [5223], 2: [993], 's_2_2': [1008]}, {0: [5005], 1: [2080], 's_0_1': [4990], 's_0_0': [2126], 's_1_1': [2079], 2: [5283], 's_2_2': [5284]}, {0: [3250], 1: [1981], 's_0_1': [1996], 's_0_0': [2026], 's_1_1': [3190], 2: [5388], 's_2_2': [703]}, {0: [3380], 1: [1112], 's_0_1': [1127], 's_0_0': [1052], 's_1_1': [3365], 2: [1162], 's_2_2': [4445]}, {0: [1343], 1: [4641], 's_0_1': [4626], 's_0_0': [4506], 's_1_1': [1389], 2: [2421], 's_2_2': [4228]}, {0: [3256], 1: [316], 's_0_1': [3241], 's_0_0': [406], 's_1_1': [3210], 2: [2577], 's_2_2': [5114]}, {0: [3997], 1: [1446], 's_0_1': [1461], 's_0_0': [1400], 's_1_1': [4087], 2: [3875], 's_2_2': [935]}, {0: [5081], 1: [5096], 's_0_1': [2111], 's_0_0': [2202], 's_1_1': [2126], 2: [3516], 's_2_2': [1187]}, {0: [247], 1: [4365], 's_0_1': [4350], 's_0_0': [4455], 's_1_1': [233], 2: [68], 's_2_2': [4605]}, {0: [147], 1: [5265], 's_0_1': [5250], 's_0_0': [5280], 's_1_1': [267], 2: [695], 's_2_2': [3933]}, {0: [2196], 1: [4091], 's_0_1': [2211], 's_0_0': [4136], 's_1_1': [4090], 2: [4885], 's_2_2': [2020]}, {0: [3349], 1: [3334], 's_0_1': [857], 's_0_0': [902], 's_1_1': [811], 2: [485], 's_2_2': [484]}, {0: [4634], 1: [4649], 's_0_1': [2829], 's_0_0': [4633], 's_1_1': [2844], 2: [2624], 's_2_2': [5578]}, {0: [1546], 1: [1531], 's_0_1': [3232], 's_0_0': [3278], 's_1_1': [3382], 2: [3136], 's_2_2': [3137]}, {0: [4035], 1: [65], 's_0_1': [80], 's_0_0': [125], 's_1_1': [4065], 2: [5421], 's_2_2': [1243]}, {0: [2828], 1: [4484], 's_0_1': [4499], 's_0_0': [4469], 's_1_1': [2798], 2: [676], 's_2_2': [3227]}, {0: [5151], 1: [5136], 's_0_1': [1196], 's_0_0': [1181], 's_1_1': [1287], 2: [2918], 's_2_2': [2919]}, {0: [1496], 1: [4973], 's_0_1': [1481], 's_0_0': [4912], 's_1_1': [1601], 2: [4756], 's_2_2': [279]}, {0: [4782], 1: [2215], 's_0_1': [2200], 's_0_0': [2290], 's_1_1': [4811], 2: [4518], 's_2_2': [758]}, {0: [3020], 1: [1080], 's_0_1': [3005], 's_0_0': [1095], 's_1_1': [3065], 2: [863], 's_2_2': [4519]}, {0: [4599], 1: [1688], 's_0_1': [1703], 's_0_0': [1674], 's_1_1': [4614], 2: [3678], 's_2_2': [574]}, {0: [4407], 1: [4392], 's_0_1': [2257], 's_0_0': [2272], 's_1_1': [2242], 2: [4186], 's_2_2': [321]}, {0: [3979], 1: [3964], 's_0_1': [920], 's_0_0': [860], 's_1_1': [965], 2: [5413], 's_2_2': [2488]}, {0: [2308], 1: [5412], 's_0_1': [5427], 's_0_0': [5366], 's_1_1': [2293], 2: [5002], 's_2_2': [1540]}, {0: [429], 1: [4772], 's_0_1': [4787], 's_0_0': [4742], 's_1_1': [444], 2: [4730], 's_2_2': [1074]}, {0: [1327], 1: [1342], 's_0_1': [4446], 's_0_0': [4356], 's_1_1': [4387], 2: [4174], 's_2_2': [952]}, {0: [2726], 1: [2711], 's_0_1': [5054], 's_0_0': [5024], 's_1_1': [5009], 2: [4193], 's_2_2': [4194]}, {0: [1352], 1: [3457], 's_0_1': [1367], 's_0_0': [3517], 's_1_1': [1382], 2: [4662], 's_2_2': [2484]}, {0: [4985], 1: [5000], 's_0_1': [1091], 's_0_0': [1136], 's_1_1': [1165], 2: [2290], 's_2_2': [4811]}, {0: [681], 1: [4218], 's_0_1': [666], 's_0_0': [4053], 's_1_1': [606], 2: [3192], 's_2_2': [2326]}, {0: [499], 1: [3782], 's_0_1': [3797], 's_0_0': [500], 's_1_1': [469], 2: [5522], 's_2_2': [524]}, {0: [3670], 1: [1878], 's_0_1': [1863], 's_0_0': [1968], 's_1_1': [3639], 2: [5271], 's_2_2': [1242]}, {0: [1187], 1: [1172], 's_0_1': [3545], 's_0_0': [3486], 's_1_1': [3426], 2: [3204], 's_2_2': [1921]}, {0: [3306], 1: [1127], 's_0_1': [3321], 's_0_0': [1262], 's_1_1': [3290], 2: [4267], 's_2_2': [1447]}, {0: [1144], 1: [3785], 's_0_1': [1159], 's_0_0': [1143], 's_1_1': [3786], 2: [3302], 's_2_2': [392]}, {0: [4424], 1: [2617], 's_0_1': [4439], 's_0_0': [2708], 's_1_1': [4303], 2: [887], 's_2_2': [886]}, {0: [2663], 1: [2648], 's_0_1': [4483], 's_0_0': [2662], 's_1_1': [2649], 2: [922], 's_2_2': [4189]}, {0: [71], 1: [86], 's_0_1': [5100], 's_0_0': [5145], 's_1_1': [87], 2: [5011], 's_2_2': [416]}, {0: [2624], 1: [5684], 's_0_1': [2639], 's_0_0': [5624], 's_1_1': [2594], 2: [3875], 's_2_2': [964]}, {0: [535], 1: [4937], 's_0_1': [520], 's_0_0': [4862], 's_1_1': [566], 2: [2233], 's_2_2': [5396]}, {0: [287], 1: [3540], 's_0_1': [272], 's_0_0': [3481], 's_1_1': [318], 2: [3154], 's_2_2': [795]}, {0: [4312], 1: [1522], 's_0_1': [1507], 's_0_0': [1567], 's_1_1': [4357], 2: [5308], 's_2_2': [2502]}, {0: [3240], 1: [91], 's_0_1': [3255], 's_0_0': [166], 's_1_1': [92], 2: [35], 's_2_2': [3870]}, {0: [3111], 1: [1320], 's_0_1': [3096], 's_0_0': [1200], 's_1_1': [3066], 2: [2342], 's_2_2': [2341]}, {0: [4238], 1: [4253], 's_0_1': [1551], 's_0_0': [1627], 's_1_1': [1642], 2: [2461], 's_2_2': [3207]}, {0: [1822], 1: [1807], 's_0_1': [4254], 's_0_0': [4284], 's_1_1': [4314], 2: [2004], 's_2_2': [4645]}, {0: [4404], 1: [4389], 's_0_1': [1687], 's_0_0': [4405], 's_1_1': [1732], 2: [2960], 's_2_2': [2961]}, {0: [3746], 1: [2223], 's_0_1': [2238], 's_0_0': [2149], 's_1_1': [3581], 2: [4627], 's_2_2': [1449]}, {0: [100], 1: [4965], 's_0_1': [115], 's_0_0': [4950], 's_1_1': [4966], 2: [4064], 's_2_2': [2556]}, {0: [5201], 1: [2142], 's_0_1': [5216], 's_0_0': [2157], 's_1_1': [5261], 2: [3661], 's_2_2': [273]}, {0: [3109], 1: [3094], 's_0_1': [960], 's_0_0': [3108], 's_1_1': [946], 2: [4153], 's_2_2': [2481]}, {0: [570], 1: [2943], 's_0_1': [2958], 's_0_0': [3062], 's_1_1': [2942], 2: [2324], 's_2_2': [5667]}, {0: [5323], 1: [2457], 's_0_1': [5338], 's_0_0': [2383], 's_1_1': [5233], 2: [437], 's_2_2': [3556]}, {0: [2596], 1: [3329], 's_0_1': [3314], 's_0_0': [3388], 's_1_1': [3328], 2: [4607], 's_2_2': [564]}, {0: [873], 1: [3679], 's_0_1': [3664], 's_0_0': [3604], 's_1_1': [3680], 2: [4711], 's_2_2': [385]}, {0: [3753], 1: [3768], 's_0_1': [784], 's_0_0': [769], 's_1_1': [709], 2: [3586], 's_2_2': [483]}, {0: [5446], 1: [328], 's_0_1': [5431], 's_0_0': [404], 's_1_1': [329], 2: [2315], 's_2_2': [3957]}, {0: [5435], 1: [1094], 's_0_1': [1109], 's_0_0': [1078], 's_1_1': [5555], 2: [1286], 's_2_2': [4971]}, {0: [5405], 1: [1108], 's_0_1': [5420], 's_0_0': [1123], 's_1_1': [5270], 2: [2019], 's_2_2': [2034]}, {0: [3314], 1: [2641], 's_0_1': [2656], 's_0_0': [3329], 's_1_1': [2642], 2: [524], 's_2_2': [523]}, {0: [1411], 1: [3172], 's_0_1': [1426], 's_0_0': [3232], 's_1_1': [1306], 2: [3873], 's_2_2': [680]}, {0: [2270], 1: [4017], 's_0_1': [4002], 's_0_0': [4091], 's_1_1': [2405], 2: [4793], 's_2_2': [1539]}, {0: [1509], 1: [4657], 's_0_1': [1524], 's_0_0': [4807], 's_1_1': [4658], 2: [4167], 's_2_2': [2406]}, {0: [689], 1: [5613], 's_0_1': [5628], 's_0_0': [5522], 's_1_1': [644], 2: [5085], 's_2_2': [5086]}, {0: [3975], 1: [3960], 's_0_1': [110], 's_0_0': [95], 's_1_1': [200], 2: [58], 's_2_2': [5295]}, {0: [3127], 1: [1456], 's_0_1': [1441], 's_0_0': [1425], 's_1_1': [3172], 2: [4667], 's_2_2': [654]}, {0: [4344], 1: [4329], 's_0_1': [1762], 's_0_0': [1792], 's_1_1': [1717], 2: [4940], 's_2_2': [956]}, {0: [5438], 1: [1603], 's_0_1': [5453], 's_0_0': [1618], 's_1_1': [1602], 2: [1105], 's_2_2': [4760]}, {0: [693], 1: [3513], 's_0_1': [3528], 's_0_0': [3543], 's_1_1': [663], 2: [447], 's_2_2': [5191]}, {0: [4493], 1: [1598], 's_0_1': [4478], 's_0_0': [1733], 's_1_1': [4538], 2: [3435], 's_2_2': [152]}, {0: [3189], 1: [1860], 's_0_1': [3204], 's_0_0': [1771], 's_1_1': [1875], 2: [3986], 's_2_2': [2105]}, {0: [3766], 1: [3751], 's_0_1': [394], 's_0_0': [454], 's_1_1': [409], 2: [1562], 's_2_2': [3412]}, {0: [3296], 1: [3281], 's_0_1': [2236], 's_0_0': [2207], 's_1_1': [2131], 2: [3502], 's_2_2': [1458]}, {0: [3935], 1: [1160], 's_0_1': [3950], 's_0_0': [1055], 's_1_1': [3995], 2: [877], 's_2_2': [4324]}, {0: [5603], 1: [1649], 's_0_1': [5588], 's_0_0': [1544], 's_1_1': [5438], 2: [5702], 's_2_2': [5701]}, {0: [1025], 1: [1040], 's_0_1': [3919], 's_0_0': [3934], 's_1_1': [3890], 2: [4365], 's_2_2': [218]}, {0: [4676], 1: [4661], 's_0_1': [2289], 's_0_0': [2154], 's_1_1': [2259], 2: [414], 's_2_2': [4607]}, {0: [3584], 1: [2673], 's_0_1': [2688], 's_0_0': [3599], 's_1_1': [3689], 2: [2136], 's_2_2': [4166]}, {0: [2711], 1: [5039], 's_0_1': [2726], 's_0_0': [4949], 's_1_1': [2756], 2: [102], 's_2_2': [5250]}, {0: [4654], 1: [924], 's_0_1': [4669], 's_0_0': [4655], 's_1_1': [4609], 2: [4648], 's_2_2': [2529]}, {0: [5441], 1: [5456], 's_0_1': [2248], 's_0_0': [2143], 's_1_1': [2189], 2: [4884], 's_2_2': [4869]}, {0: [4465], 1: [4450], 's_0_1': [1958], 's_0_0': [2047], 's_1_1': [1973], 2: [1149], 's_2_2': [4700]}, {0: [3044], 1: [3059], 's_0_1': [2670], 's_0_0': [3043], 's_1_1': [2730], 2: [4045], 's_2_2': [4046]}, {0: [1782], 1: [1797], 's_0_1': [5289], 's_0_0': [5304], 's_1_1': [5169], 2: [2186], 's_2_2': [4901]}]</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>[{0: [5641], 1: [359], 2: [726]}, {0: [3437], 1: [527], 2: [4435]}, {0: [5716], 1: [5701], 2: [5369]}, {0: [2353], 1: [5412], 2: [2046]}, {0: [1816], 1: [3129], 2: [3084]}, {0: [3368], 1: [1742], 2: [3697]}, {0: [3370], 1: [2117], 2: [4929]}, {0: [3565], 1: [3550], 2: [5315]}, {0: [4317], 1: [2377], 2: [3297]}, {0: [4314], 1: [1852], 2: [1792]}, {0: [5086], 1: [296], 2: [4910]}, {0: [3312], 1: [2207], 2: [3714]}, {0: [2231], 1: [5066], 2: [3148]}, {0: [5381], 1: [2308], 2: [4113]}, {0: [1015], 1: [4834], 2: [2630]}, {0: [5018], 1: [5017], 2: [2572]}, {0: [2466], 1: [2481], 2: [894]}, {0: [2089], 1: [3836], 2: [3668]}, {0: [3049], 1: [3034], 2: [750]}, {0: [4365], 1: [172], 2: [4985]}, {0: [5357], 1: [553], 2: [4855]}, {0: [318], 1: [303], 2: [4336]}, {0: [2714], 1: [5444], 2: [993]}, {0: [3637], 1: [1353], 2: [4504]}, {0: [5120], 1: [1016], 2: [1904]}, {0: [5117], 1: [552], 2: [1564]}, {0: [5462], 1: [448], 2: [2023]}, {0: [89], 1: [5670], 2: [3513]}, {0: [2762], 1: [3419], 2: [5595]}, {0: [4212], 1: [2331], 2: [867]}, {0: [3067], 1: [1515], 2: [65]}, {0: [2338], 1: [5322], 2: [2292]}, {0: [807], 1: [5223], 2: [3927]}, {0: [3315], 1: [32], 2: [2084]}, {0: [2001], 1: [1986], 2: [2324]}, {0: [1071], 1: [4160], 2: [5183]}, {0: [2827], 1: [4304], 2: [2309]}, {0: [1115], 1: [3920], 2: [3335]}, {0: [537], 1: [5207], 2: [170]}, {0: [3391], 1: [422], 2: [1513]}, {0: [348], 1: [3541], 2: [3306]}, {0: [1249], 1: [3711], 2: [2363]}, {0: [3329], 1: [2656], 2: [3138]}, {0: [3384], 1: [1802], 2: [5272]}, {0: [1833], 1: [3474], 2: [1982]}, {0: [1864], 1: [3834], 2: [5158]}, {0: [54], 1: [55], 2: [4610]}, {0: [2137], 1: [4301], 2: [2953]}, {0: [2623], 1: [5398], 2: [2325]}, {0: [5706], 1: [1364], 2: [3529]}, {0: [1549], 1: [3907], 2: [1792]}, {0: [98], 1: [4575], 2: [4631]}, {0: [5622], 1: [2294], 2: [3219]}, {0: [4352], 1: [4367], 2: [1707]}, {0: [4773], 1: [624], 2: [4759]}, {0: [2429], 1: [5698], 2: [5016]}, {0: [1286], 1: [5031], 2: [5659]}, {0: [5427], 1: [2398], 2: [1809]}, {0: [3355], 1: [1982], 2: [4081]}, {0: [508], 1: [5386], 2: [2160]}, {0: [3333], 1: [631], 2: [3723]}, {0: [3268], 1: [2476], 2: [2489]}, {0: [609], 1: [4788], 2: [310]}, {0: [3754], 1: [1039], 2: [192]}, {0: [2243], 1: [4587], 2: [4232]}, {0: [880], 1: [4894], 2: [5656]}, {0: [262], 1: [4335], 2: [339]}, {0: [56], 1: [57], 2: [713]}, {0: [308], 1: [4576], 2: [1855]}, {0: [1063], 1: [1064], 2: [5370]}, {0: [5315], 1: [5314], 2: [1548]}, {0: [4063], 1: [2420], 2: [1612]}, {0: [4370], 1: [1118], 2: [3122]}, {0: [886], 1: [3169], 2: [4191]}, {0: [2376], 1: [4152], 2: [1943]}, {0: [422], 1: [3451], 2: [4657]}, {0: [167], 1: [3420], 2: [5218]}, {0: [5153], 1: [1587], 2: [3816]}, {0: [3155], 1: [3154], 2: [5198]}, {0: [1656], 1: [4013], 2: [2357]}, {0: [3444], 1: [1877], 2: [4809]}, {0: [1600], 1: [4913], 2: [5161]}, {0: [1793], 1: [4464], 2: [1562]}, {0: [902], 1: [3439], 2: [92]}, {0: [4986], 1: [1271], 2: [561]}, {0: [1898], 1: [4570], 2: [3435]}, {0: [2194], 1: [2193], 2: [5047]}, {0: [4430], 1: [1058], 2: [1359]}, {0: [1565], 1: [3878], 2: [4284]}, {0: [3107], 1: [541], 2: [2336]}, {0: [3130], 1: [1875], 2: [415]}, {0: [3752], 1: [514], 2: [5509]}, {0: [2445], 1: [3133], 2: [199]}, {0: [4196], 1: [4195], 2: [1777]}, {0: [217], 1: [4320], 2: [3929]}, {0: [5230], 1: [1947], 2: [1967]}, {0: [507], 1: [5297], 2: [4005]}, {0: [5322], 1: [5323], 2: [5194]}, {0: [5066], 1: [2231], 2: [4370]}, {0: [5218], 1: [2577], 2: [2605]}]</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>[7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7, 7]</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>[3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3, 3]</t>
-        </is>
-      </c>
-      <c r="AH2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL2" t="inlineStr">
-        <is>
-          <t>[0.030179738998413086, 0.027634620666503906, 0.027518033981323242, 0.028872013092041016, 0.02881455421447754, 0.0292665958404541, 0.028983592987060547, 0.026899099349975586, 0.026875734329223633, 0.02669525146484375, 0.0285186767578125, 0.027209043502807617, 0.026941299438476562, 0.027033090591430664, 0.027041912078857422, 0.027267932891845703, 0.02688288688659668, 0.027051210403442383, 0.026915788650512695, 0.026973247528076172, 0.027236461639404297, 0.027063846588134766, 0.02718663215637207, 0.02695012092590332, 0.026915788650512695, 0.026921987533569336, 0.026950359344482422, 0.02723217010498047, 0.026756763458251953, 0.027448177337646484, 0.02889704704284668, 0.028675556182861328, 0.02899169921875, 0.028959035873413086, 0.027031421661376953, 0.02705240249633789, 0.027219057083129883, 0.02714991569519043, 0.027014732360839844, 0.026778459548950195, 0.02703380584716797, 0.027252912521362305, 0.026929855346679688, 0.027326107025146484, 0.027379274368286133, 0.02736377716064453, 0.028927087783813477, 0.027282238006591797, 0.028811216354370117, 0.02703690528869629, 0.027136564254760742, 0.027024030685424805, 0.02741861343383789, 0.026749610900878906, 0.026821613311767578, 0.02691340446472168, 0.026871442794799805, 0.027143239974975586, 0.026824951171875, 0.026970386505126953, 0.027450084686279297, 0.029267549514770508, 0.02952289581298828, 0.02980208396911621, 0.02687215805053711, 0.028677701950073242, 0.028985977172851562, 0.0271756649017334, 0.026958703994750977, 0.027975082397460938, 0.026993751525878906, 0.027152538299560547, 0.028226375579833984, 0.027033329010009766, 0.027005672454833984, 0.027146577835083008, 0.027265548706054688, 0.027364253997802734, 0.029158830642700195, 0.02886509895324707, 0.031243562698364258, 0.027921676635742188, 0.027980804443359375, 0.029407262802124023, 0.02698373794555664, 0.02713179588317871, 0.02702784538269043, 0.028736114501953125, 0.02902698516845703, 0.029222965240478516, 0.0275118350982666, 0.027113676071166992, 0.026997089385986328, 0.026896953582763672, 0.02682185173034668, 0.02841973304748535, 0.027118921279907227, 0.027544736862182617, 0.028968334197998047, 0.028212547302246094]</t>
-        </is>
-      </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>[0.025486230850219727, 0.02268362045288086, 0.022454261779785156, 0.022408008575439453, 0.022467851638793945, 0.02263641357421875, 0.022504806518554688, 0.022542715072631836, 0.022507905960083008, 0.022461414337158203, 0.022410869598388672, 0.022401094436645508, 0.022406816482543945, 0.02242136001586914, 0.022498130798339844, 0.022493839263916016, 0.02423095703125, 0.02435755729675293, 0.022673845291137695, 0.023160934448242188, 0.022780179977416992, 0.02248859405517578, 0.022459745407104492, 0.022498369216918945, 0.024350404739379883, 0.023152828216552734, 0.0266420841217041, 0.025170564651489258, 0.028417110443115234, 0.023915529251098633, 0.022542715072631836, 0.022258520126342773, 0.02231740951538086, 0.022211074829101562, 0.022321224212646484, 0.024295330047607422, 0.02428436279296875, 0.024291515350341797, 0.022376060485839844, 0.022581100463867188, 0.023366451263427734, 0.022454261779785156, 0.02221989631652832, 0.02292799949645996, 0.022272348403930664, 0.022258758544921875, 0.022230148315429688, 0.022325992584228516, 0.022321462631225586, 0.022270679473876953, 0.02232670783996582, 0.022262096405029297, 0.02227783203125, 0.024129867553710938, 0.024201154708862305, 0.022238492965698242, 0.022290468215942383, 0.02253246307373047, 0.02232670783996582, 0.022429466247558594, 0.0242159366607666, 0.02258157730102539, 0.02228832244873047, 0.022344350814819336, 0.022646665573120117, 0.022347211837768555, 0.022279739379882812, 0.02233743667602539, 0.022312641143798828, 0.022938966751098633, 0.02530956268310547, 0.023166656494140625, 0.022485017776489258, 0.022417068481445312, 0.02305126190185547, 0.0225372314453125, 0.02233433723449707, 0.022556543350219727, 0.022413969039916992, 0.02245354652404785, 0.022334575653076172, 0.02240753173828125, 0.022374391555786133, 0.022440671920776367, 0.02234172821044922, 0.022346019744873047, 0.02232503890991211, 0.022362947463989258, 0.022333621978759766, 0.022294282913208008, 0.022235631942749023, 0.0223388671875, 0.022253751754760742, 0.0242307186126709, 0.02429509162902832, 0.024320125579833984, 0.022528648376464844, 0.022342443466186523, 0.02234506607055664, 0.02361750602722168]</t>
-        </is>
-      </c>
-      <c r="AN2" t="n">
-        <v>13</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>4</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>7</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>3</v>
-      </c>
-      <c r="AR2" t="inlineStr">
-        <is>
-          <t>[0, 1, 's_0_1', 's_0_0', 's_1_1', 2, 's_2_2']</t>
-        </is>
-      </c>
-      <c r="AS2" t="inlineStr">
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>[0, 1, 's_0_1', 2]</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
         <is>
           <t>[0, 1, 2]</t>
         </is>
@@ -770,12 +766,12 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>[0, 3, 7, 8, 2, 5, 6, 9, 4, 1]</t>
+          <t>[0, 3, 7, 8, 2, 5, 4, 9, 6, 1]</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>[(0, 3), (0, 7), (0, 8), (0, 0), (3, 2), (3, 5), (3, 7), (3, 8), (3, 3), (7, 7), (8, 2), (8, 8), (2, 2), (5, 6), (5, 9), (5, 5), (6, 6), (9, 4), (9, 9), (4, 4), (1, 1)]</t>
+          <t>[(0, 3), (0, 7), (0, 8), (3, 2), (3, 5), (3, 7), (3, 8), (8, 2), (5, 6), (5, 9), (4, 9)]</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -790,14 +786,14 @@
         <v>0.002534468157697533</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1591397849462366</v>
+        <v>0.2571428571428571</v>
       </c>
       <c r="K3" t="n">
         <v>0.4666666666666667</v>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[(0, 3), (0, 's_0_3'), (0, 7), (0, 's_0_7'), (0, 8), (0, 's_0_8'), (0, 's_0_0'), (0, 0), (3, 's_0_3'), (3, 2), (3, 's_3_2'), (3, 5), (3, 's_3_5'), (3, 7), (3, 's_3_7'), (3, 8), (3, 's_3_8'), (3, 's_3_3'), (3, 3), ('s_0_3', 's_0_3'), (7, 's_0_7'), (7, 's_3_7'), (7, 's_7_7'), (7, 7), ('s_0_7', 's_0_7'), (8, 's_0_8'), (8, 's_3_8'), (8, 2), (8, 's_8_2'), (8, 's_8_8'), (8, 8), ('s_0_8', 's_0_8'), ('s_0_0', 's_0_0'), (2, 's_3_2'), (2, 's_8_2'), (2, 's_2_2'), (2, 2), ('s_3_2', 's_3_2'), (5, 's_3_5'), (5, 6), (5, 's_5_6'), (5, 9), (5, 's_5_9'), (5, 's_5_5'), (5, 5), ('s_3_5', 's_3_5'), ('s_3_7', 's_3_7'), ('s_3_8', 's_3_8'), ('s_3_3', 's_3_3'), ('s_7_7', 's_7_7'), ('s_8_2', 's_8_2'), ('s_8_8', 's_8_8'), ('s_2_2', 's_2_2'), (6, 's_5_6'), (6, 's_6_6'), (6, 6), ('s_5_6', 's_5_6'), (9, 's_5_9'), (9, 4), (9, 's_9_4'), (9, 's_9_9'), (9, 9), ('s_5_9', 's_5_9'), ('s_5_5', 's_5_5'), ('s_6_6', 's_6_6'), (4, 's_9_4'), (4, 's_4_4'), (4, 4), ('s_9_4', 's_9_4'), ('s_9_9', 's_9_9'), ('s_4_4', 's_4_4'), (1, 's_1_1'), (1, 1), ('s_1_1', 's_1_1')]</t>
+          <t>[(0, 3), (0, 's_0_3'), (0, 7), (0, 's_0_7'), (0, 8), (0, 's_0_8'), (0, 0), (3, 's_0_3'), (3, 2), (3, 's_2_3'), (3, 5), (3, 's_3_5'), (3, 7), (3, 's_3_7'), (3, 8), (3, 's_3_8'), (3, 3), ('s_0_3', 's_0_3'), (7, 's_0_7'), (7, 's_3_7'), (7, 7), ('s_0_7', 's_0_7'), (8, 's_0_8'), (8, 's_3_8'), (8, 2), (8, 's_2_8'), (8, 8), ('s_0_8', 's_0_8'), (2, 's_2_3'), (2, 's_2_8'), (2, 2), ('s_2_3', 's_2_3'), (5, 's_3_5'), (5, 6), (5, 's_5_6'), (5, 9), (5, 's_5_9'), (5, 5), ('s_3_5', 's_3_5'), ('s_3_7', 's_3_7'), ('s_3_8', 's_3_8'), ('s_2_8', 's_2_8'), (6, 's_5_6'), (6, 6), ('s_5_6', 's_5_6'), (9, 4), (9, 's_5_9'), (9, 's_4_9'), (9, 9), ('s_5_9', 's_5_9'), (4, 's_4_9'), (4, 4), ('s_4_9', 's_4_9'), (1, 1)]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
@@ -805,122 +801,90 @@
           <t>[(0, 3), (0, 7), (0, 8), (0, 0), (3, 2), (3, 5), (3, 7), (3, 8), (3, 3), (7, 7), (8, 2), (8, 8), (2, 2), (5, 6), (5, 9), (5, 5), (6, 6), (9, 4), (9, 9), (4, 4), (1, 1)]</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>{0: [1029, 1032, 1028, 1031, 1034, 1027, 1033, 5585, 1030], 1: [1044, 1047, 1043, 1046, 1049, 1042, 1048, 5600, 1045], 2: [1002, 5554, 1001, 998, 1004, 997, 1003, 1000, 999], 3: [1012, 1018, 1014, 1017, 1013, 1016, 5569, 1019, 1015], 4: [5524, 969, 972, 968, 971, 967, 973, 970], 5: [5539, 986, 983, 982, 985, 988, 984, 987], 6: [939, 942, 941, 938, 944, 5495, 943, 940], 7: [954, 957, 953, 956, 959, 5510, 958, 955], 8: [910, 909, 912, 5465, 908, 911, 5464, 914, 913], 9: [5480, 927, 5479, 926, 923, 929, 928, 925, 924], 10: [880, 877, 883, 879, 882, 5435, 878, 881, 5434], 11: [5449, 893, 895, 892, 898, 894, 897, 5450, 896], 12: [847, 853, 850, 849, 852, 5405, 848, 851, 5404], 13: [5420, 863, 866, 5419, 862, 865, 868, 867, 864], 14: [821, 5373, 820, 817, 823, 818, 819, 822, 5374], 15: [835, 834, 837, 5389, 833, 836, 5388, 832, 838], 16: [5358, 805, 803, 802, 804, 807, 5359, 806], 17: [763, 5315, 760, 759, 762, 5314, 758, 761], 18: [778, 5330, 775, 774, 777, 5329, 773, 776], 19: [1061, 1058, 5285, 1057, 1060, 1059, 5284, 1062], 20: [1076, 1073, 5300, 1072, 1075, 1074, 5299, 1077], 21: [730, 5255, 733, 729, 5254, 732, 728, 5253, 731], 22: [746, 745, 5270, 748, 744, 5269, 747, 743, 5268], 23: [699, 702, 5223, 698, 5225, 701, 697, 700, 5224], 24: [1092, 5195, 1089, 5194, 1088, 1091, 1090, 5193], 25: [5209, 1107, 1104, 5208, 1103, 1106, 5210, 1105], 26: [5177, 670, 5180, 669, 5179, 672, 671, 668, 5178, 667], 27: [5134, 654, 5133, 656, 653, 652, 5135, 655], 28: [607, 5104, 610, 5103, 609, 5105, 611, 608], 29: [624, 5120, 5119, 623, 626, 622, 625, 5118], 30: [5075, 580, 5074, 579, 582, 581, 5073, 578, 5072], 31: [5090, 595, 5089, 594, 597, 593, 596, 5088, 5087], 32: [549, 5042, 5045, 5044, 548, 551, 550, 5043], 33: [5059, 564, 566, 5058, 563, 5057, 5060, 565], 34: [517, 5014, 519, 5013, 518, 521, 5015, 520, 5012], 35: [534, 5027, 533, 5030, 536, 532, 5029, 535, 5028], 36: [4999, 1118, 4998, 1121, 1120, 5000, 4997, 1119], 37: [4953, 4956, 488, 491, 4952, 490, 4955, 487, 4954, 489], 38: [504, 503, 4969, 506, 4968, 505, 4971, 502, 4970, 4967], 39: [4939, 459, 4938, 458, 4941, 460, 457, 4940, 4937], 40: [4910, 1147, 4907, 1150, 1149, 4909, 4908, 1148], 41: [4861, 429, 4864, 428, 4863, 427, 430, 4865, 4862], 42: [4878, 445, 442, 4877, 4880, 4876, 444, 4879, 443], 43: [4834, 4833, 399, 4832, 4835, 398, 4831, 400], 44: [414, 4850, 413, 4847, 4846, 415, 4849, 4848], 45: [4803, 1179, 4805, 1178, 4802, 1177, 4801, 4804], 46: [1193, 4818, 4817, 4820, 1192, 4816, 1194, 4819], 47: [4383, 1210, 4386, 1209, 4382, 4385, 1208, 4384, 1207], 48: [1224, 1223, 4399, 1222, 4398, 1225, 4401, 4400, 4397], 49: [4776, 1239, 4775, 4772, 1238, 4774, 1240, 4773], 50: [4788, 4791, 1254, 4790, 4787, 1253, 4789, 1255], 51: [4745, 4742, 370, 4741, 4744, 369, 4743, 4746, 368], 52: [4759, 4758, 384, 4761, 4757, 383, 4760, 385, 4756], 53: [4413, 4416, 4412, 339, 4415, 4411, 338, 4414], 54: [4429, 353, 4428, 4431, 4430, 4427, 354, 4426], 55: [4446, 4443, 308, 4442, 4445, 4441, 4444, 309, 4440], 56: [4456, 324, 4459, 323, 4455, 4458, 4461, 4460, 4457], 57: [4471, 4474, 4470, 4473, 278, 4476, 279, 4475, 4472], 58: [293, 4488, 4485, 4491, 4487, 4490, 4486, 294, 4489], 59: [4503, 1285, 4502, 4505, 4501, 1284, 4504, 1283, 4506], 60: [4535, 248, 4534, 4531, 4530, 4536, 4533, 249, 4532], 61: [4547, 4550, 4546, 4549, 264, 4545, 4551, 4548, 263], 62: [4562, 4565, 4561, 220, 4564, 4566, 219, 4563], 63: [235, 4577, 4580, 4576, 234, 4579, 4581, 4578], 64: [4713, 4716, 190, 4715, 4712, 189, 4711, 4714, 4710], 65: [4725, 4728, 4731, 205, 4730, 4727, 204, 4726, 4729], 66: [4594, 4591, 4597, 4590, 4596, 4593, 1299, 4592, 4595], 67: [4610, 4609, 4606, 4612, 4605, 4611, 4608, 1314, 4607], 68: [4686, 1328, 4685, 4682, 4681, 4684, 1329, 4683, 4680], 69: [4701, 4700, 4697, 1344, 4696, 1343, 4699, 4695, 4698], 70: [4623, 4620, 4626, 4622, 159, 4625, 4621, 4624], 71: [4637, 4640, 4636, 4639, 174, 4635, 4641, 4638], 72: [4652, 4655, 4651, 4654, 1359, 4650, 4656, 4653], 73: [4669, 4666, 4665, 4671, 4668, 1374, 4667, 4670]}</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>{0: [815, 4083, 814], 1: [829, 830, 4098], 2: [846, 845, 844, 4054], 3: [4069, 861, 859, 860], 4: [874, 875, 3784], 5: [3799, 889, 890], 6: [4024, 905, 906], 7: [921, 4039, 920], 8: [935, 3814, 936], 9: [950, 951, 3829], 10: [3844, 3845, 785, 784], 11: [799, 3859, 800, 3860], 12: [3874, 3875, 964, 965], 13: [979, 3889, 3890, 980], 14: [3903, 3904, 995, 994], 15: [3919, 1010, 1009, 3918], 16: [3995, 756, 3994, 3993, 755], 17: [4008, 771, 4010, 770, 4009], 18: [3933, 3934, 1025], 19: [1040, 3948, 3949], 20: [1055, 3963, 3964, 3965]}</t>
-        </is>
+      <c r="N3" t="n">
+        <v>23.3</v>
+      </c>
+      <c r="O3" t="n">
+        <v>10.06</v>
       </c>
       <c r="P3" t="n">
-        <v>637</v>
+        <v>0.06836831569671631</v>
       </c>
       <c r="Q3" t="n">
-        <v>76</v>
-      </c>
-      <c r="R3" t="n">
-        <v>4225.969753742218</v>
-      </c>
-      <c r="S3" t="n">
-        <v>452.5838611125946</v>
+        <v>0.04203236103057861</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>{0: [5293], 3: [2383, 5338], 's_0_3': [2548], 7: [2457], 's_0_7': [2442], 8: [5308], 's_0_8': [2487], 2: [2412], 's_2_3': [5262], 5: [5382], 's_3_5': [2398], 's_3_7': [5352], 's_3_8': [2533], 's_2_8': [2427], 6: [2473], 's_5_6': [2488], 9: [2413], 's_5_9': [2428], 4: [5532], 's_4_9': [5547], 1: [3995]}</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>{0: [3257], 3: [556], 7: [3242], 8: [541], 2: [3092], 5: [557], 6: [3362], 9: [542], 4: [3332], 1: [3338]}</t>
+        </is>
       </c>
       <c r="T3" t="n">
-        <v>34.03</v>
+        <v>22</v>
       </c>
       <c r="U3" t="n">
-        <v>10.05</v>
+        <v>10</v>
       </c>
       <c r="V3" t="n">
-        <v>0.06755757331848145</v>
+        <v>0.06227636337280273</v>
       </c>
       <c r="W3" t="n">
-        <v>0.03254795074462891</v>
+        <v>0.03936648368835449</v>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>{0: [1041], 3: [4084, 1026], 's_0_3': [4160], 7: [4070], 's_0_7': [4055], 8: [4129], 's_0_8': [4114], 's_0_0': [1042], 2: [876], 's_3_2': [4099], 5: [980], 's_3_5': [965], 's_3_7': [1010], 's_3_8': [936], 's_3_3': [1027], 's_7_7': [1101], 's_8_2': [891], 's_8_8': [4128], 's_2_2': [875], 6: [3964], 's_5_6': [3979], 9: [4009], 's_5_9': [3994], 's_5_5': [979], 's_6_6': [3963], 4: [860], 's_9_4': [845], 's_9_9': [890], 's_4_4': [859], 1: [2754], 's_1_1': [4664]}</t>
+          <t>[23, 23, 23, 23, 23, 23, 23, 24, 23, 23, 23, 24, 23, 24, 24, 24, 23, 23, 25, 23, 23, 23, 24, 23, 24, 23, 22, 24, 25, 22, 23, 22, 24, 24, 23, 24, 23, 23, 23, 22, 24, 24, 23, 23, 23, 24, 23, 23, 23, 22, 23, 24, 24, 23, 23, 24, 23, 23, 24, 22, 22, 23, 22, 24, 23, 22, 23, 23, 23, 23, 24, 23, 24, 24, 25, 23, 25, 24, 23, 22, 24, 24, 23, 24, 23, 25, 22, 24, 24, 23, 22, 23, 23, 23, 23, 24, 22, 25, 24, 24]</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>{0: [3273], 3: [3288], 7: [661], 8: [646], 2: [631], 5: [676], 6: [3182], 9: [3168], 4: [645], 1: [4583]}</t>
+          <t>[10, 10, 11, 10, 10, 10, 10, 11, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 11, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 11, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 11, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 11, 10, 10, 10]</t>
         </is>
       </c>
       <c r="Z3" t="n">
-        <v>32</v>
+        <v>0.7719841941125453</v>
       </c>
       <c r="AA3" t="n">
+        <v>0.238683256575942</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>[0.06680846214294434, 0.06308293342590332, 0.055959224700927734, 0.06317734718322754, 0.07065510749816895, 0.07420706748962402, 0.07491469383239746, 0.05736565589904785, 0.06447219848632812, 0.058936357498168945, 0.06556010246276855, 0.0663912296295166, 0.06081533432006836, 0.07217931747436523, 0.07563614845275879, 0.0790705680847168, 0.05961132049560547, 0.07245993614196777, 0.07137560844421387, 0.06914472579956055, 0.08166384696960449, 0.07405567169189453, 0.0691995620727539, 0.07204890251159668, 0.06163740158081055, 0.05668807029724121, 0.062276363372802734, 0.06222939491271973, 0.0663156509399414, 0.06130099296569824, 0.06726765632629395, 0.06101846694946289, 0.06682586669921875, 0.07203912734985352, 0.07382392883300781, 0.07200026512145996, 0.09375977516174316, 0.06413984298706055, 0.06720948219299316, 0.06740522384643555, 0.06487560272216797, 0.0691690444946289, 0.06067943572998047, 0.06968379020690918, 0.06142163276672363, 0.06150078773498535, 0.07119584083557129, 0.06239175796508789, 0.06627559661865234, 0.06278371810913086, 0.07505273818969727, 0.06486630439758301, 0.07592940330505371, 0.07747268676757812, 0.0596623420715332, 0.06558036804199219, 0.06383442878723145, 0.06385254859924316, 0.0821983814239502, 0.07003355026245117, 0.09078264236450195, 0.07369780540466309, 0.0620265007019043, 0.07950806617736816, 0.08900737762451172, 0.0681924819946289, 0.09499907493591309, 0.06025242805480957, 0.06940579414367676, 0.05719900131225586, 0.07444429397583008, 0.06987500190734863, 0.06879138946533203, 0.0659947395324707, 0.06289219856262207, 0.06911659240722656, 0.06504607200622559, 0.06718611717224121, 0.06085491180419922, 0.07019352912902832, 0.08492422103881836, 0.09294581413269043, 0.06885552406311035, 0.07056045532226562, 0.07089376449584961, 0.0687570571899414, 0.07191038131713867, 0.06854414939880371, 0.0633389949798584, 0.07742953300476074, 0.07398033142089844, 0.07018017768859863, 0.06602072715759277, 0.06671881675720215, 0.06118488311767578, 0.05907726287841797, 0.07779192924499512, 0.07265138626098633, 0.07779765129089355, 0.06482863426208496]</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>[0.03936648368835449, 0.037180185317993164, 0.03802657127380371, 0.043132781982421875, 0.0433964729309082, 0.03679203987121582, 0.04218029975891113, 0.04325675964355469, 0.04586458206176758, 0.037412166595458984, 0.03960990905761719, 0.046222686767578125, 0.04733633995056152, 0.04956221580505371, 0.046228647232055664, 0.03690075874328613, 0.0450742244720459, 0.040986061096191406, 0.03487420082092285, 0.03901052474975586, 0.03946828842163086, 0.0400390625, 0.03655886650085449, 0.042359352111816406, 0.03661847114562988, 0.04894375801086426, 0.06447815895080566, 0.047765254974365234, 0.05279421806335449, 0.05185270309448242, 0.06025528907775879, 0.05333900451660156, 0.05978560447692871, 0.05836915969848633, 0.05086326599121094, 0.06649947166442871, 0.07354450225830078, 0.055681705474853516, 0.04960322380065918, 0.04159951210021973, 0.04342341423034668, 0.04268312454223633, 0.03925681114196777, 0.04822182655334473, 0.05246400833129883, 0.05830550193786621, 0.0505070686340332, 0.04474043846130371, 0.04038810729980469, 0.03919410705566406, 0.03990650177001953, 0.049504995346069336, 0.043808698654174805, 0.04823732376098633, 0.04013800621032715, 0.037740230560302734, 0.05503654479980469, 0.05848956108093262, 0.04427075386047363, 0.038056373596191406, 0.038901329040527344, 0.04359912872314453, 0.03811287879943848, 0.04129457473754883, 0.035460472106933594, 0.04227638244628906, 0.03806710243225098, 0.040047407150268555, 0.04224252700805664, 0.037294626235961914, 0.0379338264465332, 0.039846181869506836, 0.041492462158203125, 0.04171156883239746, 0.04206252098083496, 0.03746342658996582, 0.0409235954284668, 0.03624105453491211, 0.042002201080322266, 0.03515815734863281, 0.0357663631439209, 0.04357266426086426, 0.04690432548522949, 0.044374704360961914, 0.04709005355834961, 0.03716611862182617, 0.04102134704589844, 0.04649639129638672, 0.036386966705322266, 0.04935932159423828, 0.036266326904296875, 0.042788028717041016, 0.039566993713378906, 0.03487420082092285, 0.0359807014465332, 0.036577701568603516, 0.03949379920959473, 0.03859210014343262, 0.043891191482543945, 0.03915667533874512]</t>
+        </is>
+      </c>
+      <c r="AF3" t="n">
+        <v>54</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI3" t="n">
         <v>10</v>
       </c>
-      <c r="AB3" t="n">
-        <v>0.06525468826293945</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>0.03455877304077148</v>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">[{0: [3709], 3: [3768, 844], 's_0_3': [769], 7: [3694], 's_0_7': [813], 8: [859, 3844], 's_0_8': [889], 's_0_0': [828], 2: [3859], 's_3_2': [799], 5: [693, 694], 's_3_5': [3738], 's_3_7': [754], 's_3_8': [3784], 's_3_3': [845], 's_7_7': [798], 's_8_2': [829], 's_8_8': [3843], 's_2_2': [814], 6: [708], 's_5_6': [709], 9: [3783], 's_5_9': [3798], 's_5_5': [692], 's_6_6': [3528], 4: [634], 's_9_4': [649], 's_9_9': [739], 's_4_4': [3917], 1: [1843], 's_1_1': [5305]}, {0: [1115, 3965], 3: [3876, 1265], 's_0_3': [3966], 7: [3846], 's_0_7': [1130], 8: [3890, 3891], 's_0_8': [1025], 's_0_0': [1145], 2: [1220], 's_3_2': [3981], 5: [3936], 's_3_5': [1250], 's_3_7': [1174], 's_3_8': [3875], 's_3_3': [3816], 's_7_7': [3845], 's_8_2': [1205], 's_8_8': [3889], 's_2_2': [3950], 6: [1325], 's_5_6': [1340], 9: [3951], 's_5_9': [1385], 's_5_5': [3937], 's_6_6': [3996], 4: [1370], 's_9_4': [1355], 's_9_9': [1235], 's_4_4': [4101], 1: [3206], 's_1_1': [2281]}, {0: [5357, 583], 3: [688, 5313], 's_0_3': [598], 7: [627], 's_0_7': [5267], 8: [5283, 733], 's_0_8': [657], 's_0_0': [5252], 2: [5418], 's_3_2': [673], 5: [568, 5312], 's_3_5': [5372], 's_3_7': [612], 's_3_8': [5328], 's_3_3': [689], 's_7_7': [5192], 's_8_2': [5403], 's_8_8': [5268], 's_2_2': [658], 6: [5327], 's_5_6': [523], 9: [403], 's_5_9': [418], 's_5_5': [538], 's_6_6': [508], 4: [5356], 's_9_4': [5341], 's_9_9': [5401], 's_4_4': [432], 1: [2088], 's_1_1': [3611]}, {0: [5577, 2414], 3: [5710, 5712, 5711], 's_0_3': [2429], 7: [2444], 's_0_7': [5683], 8: [5576, 2279], 's_0_8': [5637], 's_0_0': [2369], 2: [2264], 's_3_2': [5726], 5: [5725, 5724, 5723], 's_3_5': [5709], 's_3_7': [5727], 's_3_8': [2249], 's_3_3': [2459], 's_7_7': [5698], 's_8_2': [5561], 's_8_8': [2204], 's_2_2': [5592], 6: [1739], 's_5_6': [5708], 9: [1874], 's_5_9': [1889], 's_5_5': [2069], 's_6_6': [5558], 4: [5650], 's_9_4': [5665], 's_9_9': [5680], 's_4_4': [1949], 1: [721], 's_1_1': [3198]}, {0: [3430], 3: [3490, 1967], 's_0_3': [1922], 7: [3445], 's_0_7': [2042], 8: [1997, 3340], 's_0_8': [1982], 's_0_0': [3431], 2: [1952], 's_3_2': [3400], 5: [3520, 1877], 's_3_5': [3505], 's_3_7': [1907], 's_3_8': [3415], 's_3_3': [3491], 's_7_7': [3444], 's_8_2': [3370], 's_8_8': [1891], 's_2_2': [3460], 6: [1848], 's_5_6': [3564], 9: [1953], 's_5_9': [3535], 's_5_5': [3521], 's_6_6': [3459], 4: [1968], 's_9_4': [3655], 's_9_9': [3610], 's_4_4': [3670], 1: [4702], 's_1_1': [1464]}, {0: [1041], 3: [4084, 1026], 's_0_3': [4160], 7: [4070], 's_0_7': [4055], 8: [4129], 's_0_8': [4114], 's_0_0': [1042], 2: [876], 's_3_2': [4099], 5: [980], 's_3_5': [965], 's_3_7': [1010], 's_3_8': [936], 's_3_3': [1027], 's_7_7': [1101], 's_8_2': [891], 's_8_8': [4128], 's_2_2': [875], 6: [3964], 's_5_6': [3979], 9: [4009], 's_5_9': [3994], 's_5_5': [979], 's_6_6': [3963], 4: [860], 's_9_4': [845], 's_9_9': [890], 's_4_4': [859], 1: [2754], 's_1_1': [4664]}, {0: [3073], 3: [3044, 3043, 2490], 's_0_3': [2595], 7: [2550], 's_0_7': [2565], 8: [3042, 2430], 's_0_8': [2445], 's_0_0': [2535], 2: [3103], 's_3_2': [2580], 5: [3059], 's_3_5': [2730], 's_3_7': [3013], 's_3_8': [3088], 's_3_3': [3148], 's_7_7': [2969], 's_8_2': [2460], 's_8_8': [3057], 's_2_2': [3102], 6: [2790], 's_5_6': [2805], 9: [2775], 's_5_9': [2760], 's_5_5': [2700], 's_6_6': [2791], 4: [3194], 's_9_4': [3209], 's_9_9': [3119], 's_4_4': [2731], 1: [185], 's_1_1': [3945]}, {0: [1020, 3095], 3: [930, 3034], 's_0_3': [3004], 7: [3049], 's_0_7': [990], 8: [2990], 's_0_8': [1050], 's_0_0': [3140], 2: [2975], 's_3_2': [1035], 5: [1080, 3035], 's_3_5': [2945], 's_3_7': [960], 's_3_8': [945], 's_3_3': [885], 's_7_7': [915], 's_8_2': [1065], 's_8_8': [2991], 's_2_2': [2976], 6: [1140], 's_5_6': [3050], 9: [2930], 's_5_9': [1110], 's_5_5': [2960], 's_6_6': [3110], 4: [2915], 's_9_4': [1095], 's_9_9': [2931], 's_4_4': [2914], 1: [1151], 's_1_1': [5136]}, {0: [402], 3: [5176, 492], 's_0_3': [5206], 7: [5132], 's_0_7': [5147], 8: [5221, 372], 's_0_8': [5071], 's_0_0': [5117], 2: [5191], 's_3_2': [387], 5: [5267], 's_3_5': [507], 's_3_7': [446], 's_3_8': [357], 's_3_3': [493], 's_7_7': [5133], 's_8_2': [342], 's_8_8': [297], 's_2_2': [447], 6: [477], 's_5_6': [462], 9: [5252], 's_5_9': [598], 's_5_5': [627], 's_6_6': [5297], 4: [522], 's_9_4': [537], 's_9_9': [553], 's_4_4': [5237], 1: [4374], 's_1_1': [1838]}, {0: [4485], 3: [248, 4545], 's_0_3': [158], 7: [4470], 's_0_7': [293], 8: [4440, 173], 's_0_8': [203], 's_0_0': [308], 2: [4500], 's_3_2': [98], 5: [4620, 234], 's_3_5': [4530], 's_3_7': [263], 's_3_8': [247], 's_3_3': [249], 's_7_7': [4471], 's_8_2': [218], 's_8_8': [4560], 's_2_2': [188], 6: [189], 's_5_6': [4695], 9: [4606], 's_5_9': [309], 's_5_5': [159], 's_6_6': [4635], 4: [354], 's_9_4': [339], 's_9_9': [369], 's_4_4': [4756], 1: [3926], 's_1_1': [2210]}, {0: [3678], 3: [3648, 678], 's_0_3': [739], 7: [693], 's_0_7': [708], 8: [633], 's_0_8': [648], 's_0_0': [618], 2: [3618], 's_3_2': [663], 5: [769, 3753], 's_3_5': [724], 's_3_7': [3633], 's_3_8': [3587], 's_3_3': [3513], 's_7_7': [694], 's_8_2': [3603], 's_8_8': [3693], 's_2_2': [753], 6: [859], 's_5_6': [3738], 9: [784], 's_5_9': [3768], 's_5_5': [3723], 's_6_6': [3799], 4: [799], 's_9_4': [3844], 's_9_9': [3813], 's_4_4': [3859], 1: [2591], 's_1_1': [5159]}, {0: [5587], 3: [5617, 1514], 's_0_3': [1424], 7: [5512, 1409], 's_0_7': [1454], 8: [1379], 's_0_8': [5602], 's_0_0': [5586], 2: [5557, 5556], 's_3_2': [1364], 5: [5572, 1544], 's_3_5': [5618], 's_3_7': [1394], 's_3_8': [5632], 's_3_3': [5678], 's_7_7': [1333], 's_8_2': [5571], 's_8_8': [1378], 's_2_2': [5555], 6: [5663], 's_5_6': [1559], 9: [5588], 's_5_9': [5603], 's_5_5': [5693], 's_6_6': [1619], 4: [1634], 's_9_4': [1649], 's_9_9': [1589], 's_4_4': [5528], 1: [3698], 's_1_1': [1594]}, {0: [3215, 1216], 3: [3200, 3201], 's_0_3': [1201], 7: [1111], 's_0_7': [3230], 8: [3185], 's_0_8': [1051], 's_0_0': [3321], 2: [1155], 's_3_2': [1140], 5: [1320, 3066], 's_3_5': [1170], 's_3_7': [1126], 's_3_8': [1066], 's_3_3': [1350], 's_7_7': [1112], 's_8_2': [1185, 3035], 's_8_8': [3186], 's_2_2': [3065], 6: [1290], 's_5_6': [1305], 9: [1215], 's_5_9': [1200], 's_5_5': [1260], 's_6_6': [3081], 4: [3005], 's_9_4': [3020], 's_9_9': [2976], 's_4_4': [1095], 1: [2729], 's_1_1': [2728]}, {0: [4535], 3: [4505, 1043], 's_0_3': [1058], 7: [1148], 's_0_7': [1163], 8: [1013], 's_0_8': [4550], 's_0_0': [4536], 2: [4580], 's_3_2': [1028], 5: [4430], 's_3_5': [4415], 's_3_7': [4520], 's_3_8': [4489], 's_3_3': [1133], 's_7_7': [4596], 's_8_2': [998], 's_8_8': [4610], 's_2_2': [4579], 6: [1103], 's_5_6': [1088], 9: [953], 's_5_9': [938], 's_5_5': [4429], 's_6_6': [1104], 4: [4444], 's_9_4': [4459], 's_9_9': [954], 's_4_4': [982], 1: [4331], 's_1_1': [2212]}, {0: [4228, 2481], 3: [2542, 4258], 's_0_3': [2527], 7: [2451], 's_0_7': [4168], 8: [2421], 's_0_8': [4213], 's_0_0': [4063], 2: [2377, 4182], 's_3_2': [2392], 5: [2347, 4257], 's_3_5': [4348, 4347], 's_3_7': [4183], 's_3_8': [2406], 's_3_3': [2541], 's_7_7': [2452], 's_8_2': [4197], 's_8_8': [4287], 's_2_2': [2316], 6: [2226], 's_5_6': [2241], 9: [2287], 's_5_9': [4332], 's_5_5': [4227], 's_6_6': [2227], 4: [4271], 's_9_4': [4286], 's_9_9': [2288], 's_4_4': [2152], 1: [790], 's_1_1': [791]}, {0: [5580, 179], 3: [329, 5550], 's_0_3': [254], 7: [209], 's_0_7': [5505], 8: [5535], 's_0_8': [239], 's_0_0': [134], 2: [314], 's_3_2': [5641], 5: [284], 's_3_5': [5626], 's_3_7': [194], 's_3_8': [164], 's_3_3': [5491], 's_7_7': [5490], 's_8_2': [5520], 's_8_8': [224], 's_2_2': [5596], 6: [5581], 's_5_6': [299], 9: [269, 5700], 's_5_9': [5686], 's_5_5': [5671], 's_6_6': [374], 4: [5716, 5701], 's_9_4': [5715], 's_9_9': [5595], 's_4_4': [5702], 1: [2666], 's_1_1': [5054]}, {0: [5237, 477], 3: [568, 5267], 's_0_3': [5282], 7: [5327], 's_0_7': [5312], 8: [5252], 's_0_8': [537], 's_0_0': [567], 2: [492], 's_3_2': [5297], 5: [627, 5283], 's_3_5': [583], 's_3_7': [553], 's_3_8': [462], 's_3_3': [598], 's_7_7': [508], 's_8_2': [507], 's_8_8': [5251], 's_2_2': [5147], 6: [657], 's_5_6': [5357], 9: [5313], 's_5_9': [612], 's_5_5': [717], 's_6_6': [658], 4: [5328], 's_9_4': [718], 's_9_9': [703], 's_4_4': [688], 1: [1216], 's_1_1': [1217]}, {0: [3465, 257], 3: [227, 3420], 's_0_3': [242], 7: [107], 's_0_7': [3450], 8: [152], 's_0_8': [3390], 's_0_0': [256], 2: [3435], 's_3_2': [182], 5: [212], 's_3_5': [3360], 's_3_7': [92], 's_3_8': [3405], 's_3_3': [137], 's_7_7': [3525], 's_8_2': [167], 's_8_8': [153], 's_2_2': [3436], 6: [3270], 's_5_6': [3285], 9: [3331], 's_5_9': [3346], 's_5_5': [213], 's_6_6': [136], 4: [377], 's_9_4': [362], 's_9_9': [286], 's_4_4': [3361], 1: [4672], 's_1_1': [1419]}, {0: [169], 3: [154, 3750], 's_0_3': [3840], 7: [124, 3690], 's_0_7': [3810], 8: [3780], 's_0_8': [3795], 's_0_0': [3855], 2: [184], 's_3_2': [3735], 5: [289, 3826], 's_3_5': [3765], 's_3_7': [3705], 's_3_8': [259], 's_3_3': [214], 's_7_7': [93], 's_8_2': [199], 's_8_8': [3781], 's_2_2': [3630], 6: [274], 's_5_6': [3886], 9: [288, 3720], 's_5_9': [304], 's_5_5': [395], 's_6_6': [275], 4: [258], 's_9_4': [3676], 's_9_9': [3721], 's_4_4': [3570], 1: [1277], 's_1_1': [3291]}, {0: [860], 3: [875, 3889], 's_0_3': [3994], 7: [845], 's_0_7': [4009], 8: [815, 3964], 's_0_8': [3948], 's_0_0': [859], 2: [3979], 's_3_2': [905], 5: [770], 's_3_5': [755], 's_3_7': [3874], 's_3_8': [4024], 's_3_3': [3934], 's_7_7': [846], 's_8_2': [890], 's_8_8': [4039], 's_2_2': [935], 6: [3903], 's_5_6': [3918], 9: [3963], 's_5_9': [3978], 's_5_5': [3844], 's_6_6': [740], 4: [785], 's_9_4': [800], 's_9_9': [695], 's_4_4': [4054], 1: [1839], 's_1_1': [4585]}, {0: [2532, 5248], 3: [2577], 's_0_3': [5233], 7: [2562], 's_0_7': [5098], 8: [2547, 5083], 's_0_8': [5158], 's_0_0': [5113], 2: [5173], 's_3_2': [5188], 5: [5129], 's_3_5': [5114], 's_3_7': [5218], 's_3_8': [5203], 's_3_3': [5144], 's_7_7': [5159], 's_8_2': [2591], 's_8_8': [2441], 's_2_2': [5172], 6: [2651], 's_5_6': [2666], 9: [2727], 's_5_9': [2712], 's_5_5': [2621], 's_6_6': [4993], 4: [5189], 's_9_4': [5174], 's_9_9': [5084], 's_4_4': [2816], 1: [265], 's_1_1': [250]}, {0: [181, 3210], 3: [3166, 226], 's_0_3': [3090], 7: [3225], 's_0_7': [166], 8: [211], 's_0_8': [3105], 's_0_0': [286], 2: [3180], 's_3_2': [240], 5: [212, 227], 's_3_5': [346, 3316], 's_3_7': [301], 's_3_8': [3255], 's_3_3': [3167], 's_7_7': [271], 's_8_2': [3195], 's_8_8': [3240], 's_2_2': [285], 6: [3285], 's_5_6': [3270], 9: [228], 's_5_9': [213], 's_5_5': [3360], 's_6_6': [106], 4: [3481], 's_9_4': [3496], 's_9_9': [3570], 's_4_4': [272], 1: [3329], 's_1_1': [3328]}, {0: [1904, 5695], 3: [5589, 1874], 's_0_3': [5680], 7: [1889], 's_0_7': [5559], 8: [1919, 5574], 's_0_8': [5605], 's_0_0': [5620], 2: [5665], 's_3_2': [5650], 5: [1739], 's_3_5': [5604], 's_3_7': [5619], 's_3_8': [1829], 's_3_3': [1859], 's_7_7': [1888], 's_8_2': [1934], 's_8_8': [5635], 's_2_2': [1949], 6: [5664], 's_5_6': [5649], 9: [1724], 's_5_9': [5634], 's_5_5': [1738], 's_6_6': [1769], 4: [5558], 's_9_4': [5573], 's_9_9': [5679], 's_4_4': [1709], 1: [1038], 's_1_1': [3515]}, {0: [4398, 743], 3: [713, 4488], 's_0_3': [4443], 7: [4413], 's_0_7': [637], 8: [4503], 's_0_8': [728], 's_0_0': [667], 2: [4518], 's_3_2': [758], 5: [698], 's_3_5': [4458], 's_3_7': [4428], 's_3_8': [803], 's_3_3': [4489], 's_7_7': [593], 's_8_2': [683], 's_8_8': [4502], 's_2_2': [773], 6: [4563], 's_5_6': [4578], 9: [4533], 's_5_9': [4548], 's_5_5': [697], 's_6_6': [608], 4: [729], 's_9_4': [744], 's_9_9': [759], 's_4_4': [4593], 1: [557], 's_1_1': [3362]}, {0: [2526, 4168], 3: [4153, 2541], 's_0_3': [2466], 7: [4108], 's_0_7': [2496], 8: [4123], 's_0_8': [2511], 's_0_0': [4169], 2: [2601], 's_3_2': [4138], 5: [2435, 4078], 's_3_5': [2481], 's_3_7': [2571], 's_3_8': [2556], 's_3_3': [2542], 's_7_7': [2585], 's_8_2': [2586], 's_8_8': [2631], 's_2_2': [4273], 6: [4003], 's_5_6': [4018], 9: [2420], 's_5_9': [4033], 's_5_5': [3973], 's_6_6': [2510], 4: [2405], 's_9_4': [4017], 's_9_9': [4002], 's_4_4': [2406], 1: [4496], 's_1_1': [2183]}, {0: [190], 3: [235, 4800], 's_0_3': [4875], 7: [4710], 's_0_7': [4725], 8: [4815], 's_0_8': [205], 's_0_0': [4785], 2: [279], 's_3_2': [4741], 5: [4845], 's_3_5': [175], 's_3_7': [264], 's_3_8': [249], 's_3_3': [236], 's_7_7': [144], 's_8_2': [294], 's_8_8': [4816], 's_2_2': [4650], 6: [295], 's_5_6': [280], 9: [4830], 's_5_9': [325], 's_5_5': [4846], 's_6_6': [4906], 4: [265], 's_9_4': [250], 's_9_9': [310], 's_4_4': [4860], 1: [34], 's_1_1': [3660]}, {0: [4297], 3: [4312, 1582], 's_0_3': [1432], 7: [1447], 's_0_7': [1462], 8: [1552], 's_0_8': [1537], 's_0_0': [4298], 2: [4343], 's_3_2': [1567], 5: [1477], 's_3_5': [1492], 's_3_7': [4282], 's_3_8': [4373], 's_3_3': [4313], 's_7_7': [4222], 's_8_2': [4328], 's_8_8': [1551], 's_2_2': [1642], 6: [4238], 's_5_6': [4253], 9: [4177], 's_5_9': [4192], 's_5_5': [4327], 's_6_6': [1521], 4: [1416], 's_9_4': [1431], 's_9_9': [4176], 's_4_4': [4132], 1: [5227], 's_1_1': [1422]}, {0: [714], 3: [4728, 669], 's_0_3': [4608], 7: [4713, 804], 's_0_7': [4653], 8: [789, 4668], 's_0_8': [4683], 's_0_0': [4623], 2: [699], 's_3_2': [4593], 5: [4743, 4742], 's_3_5': [654], 's_3_7': [775], 's_3_8': [4667], 's_3_3': [4622], 's_7_7': [4803], 's_8_2': [4698], 's_8_8': [864], 's_2_2': [698], 6: [429], 's_5_6': [444], 9: [489], 's_5_9': [504], 's_5_5': [4744], 's_6_6': [4711], 4: [4727], 's_9_4': [4712], 's_9_9': [4621], 's_4_4': [550], 1: [4421], 's_1_1': [2092]}, {0: [4473], 3: [818, 4488], 's_0_3': [743], 7: [848], 's_0_7': [863], 8: [758, 4458], 's_0_8': [773], 's_0_0': [4472], 2: [698], 's_3_2': [713], 5: [4563, 4564], 's_3_5': [803], 's_3_7': [4504], 's_3_8': [817], 's_3_3': [4609], 's_7_7': [849], 's_8_2': [4443], 's_8_8': [787], 's_2_2': [697], 6: [774], 's_5_6': [4579], 9: [4578], 's_5_9': [653], 's_5_5': [878], 's_6_6': [4698], 4: [668], 's_9_4': [683], 's_9_9': [594], 's_4_4': [4457], 1: [5289], 's_1_1': [1737]}, {0: [1513, 5527], 3: [1589, 5572], 's_0_3': [5498], 7: [5542], 's_0_7': [1424], 8: [1559, 1558], 's_0_8': [5377], 's_0_0': [5526], 2: [5648], 's_3_2': [5663], 5: [5633, 1694], 's_3_5': [5573], 's_3_7': [1469], 's_3_8': [5618], 's_3_3': [5588], 's_7_7': [5541], 's_8_2': [1544], 's_8_8': [5453], 's_2_2': [5647], 6: [1709], 's_5_6': [5558], 9: [1604], 's_5_9': [5603], 's_5_5': [1693], 's_6_6': [1708], 4: [5528], 's_9_4': [1619], 's_9_9': [5543], 's_4_4': [1754], 1: [3954], 's_1_1': [1775]}, {0: [4439], 3: [2587, 4453], 's_0_3': [2602], 7: [4424], 's_0_7': [2632], 8: [2663, 4468], 's_0_8': [2573], 's_0_0': [2558], 2: [2513], 's_3_2': [2498], 5: [2437, 4452], 's_3_5': [4348], 's_3_7': [2617], 's_3_8': [2543], 's_3_3': [4363], 's_7_7': [2678], 's_8_2': [4483], 's_8_8': [4589], 's_2_2': [4513], 6: [4408], 's_5_6': [2422], 9: [4438], 's_5_9': [2407], 's_5_5': [2468], 's_6_6': [4407], 4: [2393], 's_9_4': [4423], 's_9_9': [2378], 's_4_4': [4512], 1: [2337], 's_1_1': [5187]}, {0: [217], 3: [232, 4231], 's_0_3': [4320], 7: [4260], 's_0_7': [4275], 8: [261, 4201], 's_0_8': [4246], 's_0_0': [218], 2: [4216], 's_3_2': [382], 5: [4170], 's_3_5': [246], 's_3_7': [322], 's_3_8': [367], 's_3_3': [4335], 's_7_7': [157], 's_8_2': [336], 's_8_8': [4140], 's_2_2': [321], 6: [156], 's_5_6': [171], 9: [141], 's_5_9': [4185], 's_5_5': [187], 's_6_6': [4080], 4: [4065], 's_9_4': [126], 's_9_9': [140], 's_4_4': [36], 1: [334], 's_1_1': [3841]}, {0: [2129], 3: [5501, 2114], 's_0_3': [5560], 7: [5591], 's_0_7': [5606], 8: [2084, 5651], 's_0_8': [5666], 's_0_0': [5530], 2: [2159], 's_3_2': [5516], 5: [5500], 's_3_5': [5545, 2009], 's_3_7': [2189], 's_3_8': [2144], 's_3_3': [2024], 's_7_7': [2234], 's_8_2': [5636], 's_8_8': [5681], 's_2_2': [2158], 6: [1918], 's_5_6': [5515], 9: [1888], 's_5_9': [1873], 's_5_5': [1934], 's_6_6': [1903], 4: [5439, 1723], 's_9_4': [5454], 's_9_9': [5409], 's_4_4': [5528], 1: [590], 's_1_1': [3962]}, {0: [4218, 621], 3: [606, 4127], 's_0_3': [651], 7: [4142], 's_0_7': [4157], 8: [666], 's_0_8': [4112], 's_0_0': [622], 2: [576, 4097], 's_3_2': [561], 5: [604, 605], 's_3_5': [4082, 516], 's_3_7': [531], 's_3_8': [4203], 's_3_3': [4277], 's_7_7': [501], 's_8_2': [4053], 's_8_8': [667], 's_2_2': [3992], 6: [3902], 's_5_6': [3917], 9: [4023], 's_5_9': [620], 's_5_5': [3858], 's_6_6': [619], 4: [741], 's_9_4': [4038], 's_9_9': [695], 's_4_4': [4098], 1: [3702], 's_1_1': [2253]}, {0: [1553, 4642], 3: [4507, 1508], 's_0_3': [4598], 7: [4492], 's_0_7': [1538], 8: [1494, 4568], 's_0_8': [4627], 's_0_0': [4523], 2: [4537], 's_3_2': [1373], 5: [1463], 's_3_5': [4522], 's_3_7': [1418], 's_3_8': [1523], 's_3_3': [4613], 's_7_7': [4493], 's_8_2': [1479], 's_8_8': [1629], 's_2_2': [4536], 6: [1448], 's_5_6': [4387], 9: [4372, 4371], 's_5_9': [4357], 's_5_5': [4447], 's_6_6': [4417], 4: [1252], 's_9_4': [1237], 's_9_9': [1207], 's_4_4': [4386], 1: [3595], 's_1_1': [3580]}, {0: [1480, 4748], 3: [4747, 1450], 's_0_3': [4852], 7: [4867], 's_0_7': [1495], 8: [4717], 's_0_8': [1524], 's_0_0': [4837], 2: [1404], 's_3_2': [4762], 5: [4807], 's_3_5': [1465], 's_3_7': [4882], 's_3_8': [1419], 's_3_3': [1329], 's_7_7': [1405], 's_8_2': [1389], 's_8_8': [1509], 's_2_2': [4626], 6: [1539], 's_5_6': [1554], 9: [1570], 's_5_9': [4822], 's_5_5': [4806], 's_6_6': [4657], 4: [4778], 's_9_4': [4793], 's_9_9': [4898], 's_4_4': [4779], 1: [472], 's_1_1': [471]}, {0: [331, 3316], 3: [301, 3271], 's_0_3': [377], 7: [286], 's_0_7': [3301], 8: [316], 's_0_8': [3166], 's_0_0': [362], 2: [3241], 's_3_2': [421], 5: [151, 3180], 's_3_5': [3210], 's_3_7': [3225], 's_3_8': [3286], 's_3_3': [392], 's_7_7': [3331], 's_8_2': [3256], 's_8_8': [317], 's_2_2': [391], 6: [181], 's_5_6': [196], 9: [255], 's_5_9': [240], 's_5_5': [3150], 's_6_6': [3135], 4: [3136], 's_9_4': [3121], 's_9_9': [3045], 's_4_4': [361], 1: [3104], 's_1_1': [2701]}, {0: [3206, 2220], 3: [2206], 's_0_3': [3191], 7: [3101], 's_0_7': [2176], 8: [2356, 3132], 's_0_8': [3207], 's_0_0': [3071], 2: [3162], 's_3_2': [3177], 5: [3221], 's_3_5': [3236], 's_3_7': [3116], 's_3_8': [2191], 's_3_3': [3251], 's_7_7': [2130], 's_8_2': [2250], 's_8_8': [3192], 's_2_2': [2311], 6: [2266], 's_5_6': [2251], 9: [2296], 's_5_9': [2281], 's_5_5': [3222], 's_6_6': [3282], 4: [3327], 's_9_4': [3312], 's_9_9': [2295], 's_4_4': [2342], 1: [95], 's_1_1': [4005]}, {0: [2678], 3: [4529, 2723], 's_0_3': [4454], 7: [4484], 's_0_7': [2693], 8: [2663, 4514], 's_0_8': [4559], 's_0_0': [4544], 2: [4439], 's_3_2': [2648], 5: [2767, 2768], 's_3_5': [2783], 's_3_7': [2753], 's_3_8': [2618], 's_3_3': [4528], 's_7_7': [2813], 's_8_2': [4424], 's_8_8': [4468], 's_2_2': [2632], 6: [4649], 's_5_6': [4634], 9: [4364], 's_5_9': [2782], 's_5_5': [2769], 's_6_6': [2709], 4: [2738], 's_9_4': [4379], 's_9_9': [2662], 's_4_4': [2739], 1: [3162], 's_1_1': [2281]}, {0: [4756], 3: [324, 4681], 's_0_3': [279], 7: [354], 's_0_7': [4741], 8: [385, 384], 's_0_8': [370], 's_0_0': [235], 2: [4696], 's_3_2': [414], 5: [443, 444], 's_3_5': [4726], 's_3_7': [339], 's_3_8': [4711], 's_3_3': [325], 's_7_7': [355], 's_8_2': [369], 's_8_8': [383], 's_2_2': [4697], 6: [4562], 's_5_6': [4577], 9: [428], 's_5_9': [4607], 's_5_5': [4531], 's_6_6': [473], 4: [4621], 's_9_4': [4636], 's_9_9': [4592], 's_4_4': [4620], 1: [5543], 's_1_1': [1634]}, {0: [2716], 3: [3179, 2610], 's_0_3': [3134], 7: [2701], 's_0_7': [3224], 8: [3269, 2611], 's_0_8': [3254], 's_0_0': [2715], 2: [2671], 's_3_2': [3164], 5: [3104], 's_3_5': [2625], 's_3_7': [3119], 's_3_8': [2656], 's_3_3': [2641], 's_7_7': [2702], 's_8_2': [3329], 's_8_8': [3373], 's_2_2': [3314], 6: [2670], 's_5_6': [2685], 9: [2760], 's_5_9': [2775], 's_5_5': [2731], 's_6_6': [2984], 4: [3044], 's_9_4': [3059], 's_9_9': [3089], 's_4_4': [2730], 1: [1669], 's_1_1': [3684]}, {0: [3495], 3: [3420, 92], 's_0_3': [137], 7: [167], 's_0_7': [152], 8: [3465, 107], 's_0_8': [183], 's_0_0': [122], 2: [3435], 's_3_2': [227], 5: [3480, 3481], 's_3_5': [242], 's_3_7': [3450], 's_3_8': [3510], 's_3_3': [3421], 's_7_7': [168], 's_8_2': [257], 's_8_8': [213], 's_2_2': [3436], 6: [302], 's_5_6': [317], 9: [378], 's_5_9': [3496], 's_5_5': [287], 's_6_6': [3375], 4: [363], 's_9_4': [3586], 's_9_9': [3451], 's_4_4': [3571], 1: [526], 's_1_1': [3257]}, {0: [3232, 1531], 3: [1681, 3293], 's_0_3': [3233], 7: [3263], 's_0_7': [1546], 8: [1561], 's_0_8': [3217], 's_0_0': [1501], 2: [3308, 1576], 's_3_2': [1606], 5: [3383], 's_3_5': [1637], 's_3_7': [1591], 's_3_8': [3278], 's_3_3': [3294], 's_7_7': [1636], 's_8_2': [3202], 's_8_8': [1562], 's_2_2': [3307], 6: [1667], 's_5_6': [1652], 9: [1607], 's_5_9': [3368], 's_5_5': [3384], 's_6_6': [3354], 4: [3473], 's_9_4': [3458], 's_9_9': [3353], 's_4_4': [1547], 1: [2363], 's_1_1': [4527]}, {0: [1110], 3: [1200, 2976], 's_0_3': [3005], 7: [1080, 3050], 's_0_7': [3020], 8: [2961, 1125], 's_0_8': [3080], 's_0_0': [2930], 2: [2991], 's_3_2': [1230], 5: [3096], 's_3_5': [3111], 's_3_7': [1215], 's_3_8': [3035], 's_3_3': [3066], 's_7_7': [3065], 's_8_2': [1260], 's_8_8': [2962], 's_2_2': [2992], 6: [1185], 's_5_6': [1170], 9: [1276], 's_5_9': [1261], 's_5_5': [1306], 's_6_6': [3185], 4: [3171], 's_9_4': [3156], 's_9_9': [3186], 's_4_4': [1126], 1: [4857], 's_1_1': [2485]}, {0: [5113, 2547], 3: [5218, 2577, 5159], 's_0_3': [5248], 7: [5158], 's_0_7': [5143], 8: [5083], 's_0_8': [2516], 's_0_0': [2501], 2: [2562], 's_3_2': [5114], 5: [2667], 's_3_5': [5144], 's_3_7': [2517], 's_3_8': [2532], 's_3_3': [2727], 's_7_7': [2502], 's_8_2': [5098], 's_8_8': [2486], 's_2_2': [5129], 6: [5188], 's_5_6': [5173], 9: [2622, 5234], 's_5_9': [5309], 's_5_5': [5264], 's_6_6': [2636], 4: [5249], 's_9_4': [2682], 's_9_9': [5233], 's_4_4': [2637], 1: [3415], 's_1_1': [1997]}, {0: [5268, 748], 3: [642, 5253], 's_0_3': [733], 7: [778], 's_0_7': [5358], 8: [5283], 's_0_8': [717], 's_0_0': [702], 2: [5298], 's_3_2': [657], 5: [671, 672], 's_3_5': [5192], 's_3_7': [792, 5284], 's_3_8': [687], 's_3_3': [641], 's_7_7': [5418], 's_8_2': [612], 's_8_8': [627], 's_2_2': [5299], 6: [5088], 's_5_6': [686], 9: [5133], 's_5_9': [5148], 's_5_5': [5103], 's_6_6': [732], 4: [626], 's_9_4': [611], 's_9_9': [597], 's_4_4': [5012], 1: [4855], 's_1_1': [2080]}, {0: [633, 3663], 3: [3693], 's_0_3': [574], 7: [724], 's_0_7': [3648], 8: [664, 3722], 's_0_8': [648], 's_0_0': [693], 2: [3708], 's_3_2': [679], 5: [694], 's_3_5': [709], 's_3_7': [739], 's_3_8': [618], 's_3_3': [3692], 's_7_7': [3768], 's_8_2': [603], 's_8_8': [3767], 's_2_2': [3709], 6: [3798], 's_5_6': [3783], 9: [3858], 's_5_9': [3843], 's_5_5': [3723], 's_6_6': [784], 4: [649], 's_9_4': [634], 's_9_9': [725], 's_4_4': [3828], 1: [3190], 's_1_1': [1981]}, {0: [4943], 3: [1570, 4898], 's_0_3': [1600], 7: [4928], 's_0_7': [1631], 8: [1540, 4852], 's_0_8': [1525], 's_0_0': [4944], 2: [1555], 's_3_2': [4837], 5: [1615], 's_3_5': [4913], 's_3_7': [1646], 's_3_8': [4868], 's_3_3': [1705], 's_7_7': [4927], 's_8_2': [4987], 's_8_8': [1480], 's_2_2': [1554], 6: [4778], 's_5_6': [4793], 9: [4853], 's_5_9': [4838], 's_5_5': [1616], 's_6_6': [1630], 4: [1675], 's_9_4': [1660], 's_9_9': [1720], 's_4_4': [4749], 1: [92], 's_1_1': [3420]}, {0: [1433], 3: [4492, 1448], 's_0_3': [4432], 7: [4522], 's_0_7': [4507], 8: [4447, 1522], 's_0_8': [4462], 's_0_0': [4537], 2: [1463], 's_3_2': [4477], 5: [4417], 's_3_5': [1418], 's_3_7': [1508], 's_3_8': [1523], 's_3_3': [1538], 's_7_7': [1373], 's_8_2': [4357], 's_8_8': [4448], 's_2_2': [1464], 6: [1403], 's_5_6': [1388], 9: [1313], 's_5_9': [1298], 's_5_5': [4416], 's_6_6': [4582], 4: [4461], 's_9_4': [4446], 's_9_9': [1314], 's_4_4': [4460], 1: [2414], 's_1_1': [5712]}, {0: [3901, 424], 3: [3946, 425], 's_0_3': [365], 7: [500], 's_0_7': [3916], 8: [395], 's_0_8': [3887], 's_0_0': [454], 2: [410], 's_3_2': [3961], 5: [455], 's_3_5': [470], 's_3_7': [4022], 's_3_8': [3976], 's_3_3': [3991], 's_7_7': [3992], 's_8_2': [3826], 's_8_8': [3857], 's_2_2': [3872], 6: [3977], 's_5_6': [3962], 9: [4081], 's_5_9': [4096], 's_5_5': [4007], 's_6_6': [590], 4: [411], 's_9_4': [396], 's_9_9': [440], 's_4_4': [4052], 1: [4396], 's_1_1': [233]}, {0: [4360, 1927], 3: [4299, 1867], 's_0_3': [4390], 7: [4359, 1838], 's_0_7': [4405], 8: [4314], 's_0_8': [1942], 's_0_0': [1957], 2: [1897], 's_3_2': [4420], 5: [1928, 4464], 's_3_5': [4449], 's_3_7': [1777], 's_3_8': [1822], 's_3_3': [1866], 's_7_7': [1747], 's_8_2': [1912], 's_8_8': [1852], 's_2_2': [4375], 6: [4555], 's_5_6': [4540], 9: [4585], 's_5_9': [4570], 's_5_5': [1943], 's_6_6': [1958], 4: [2004], 's_9_4': [1989], 's_9_9': [4584], 's_4_4': [4615], 1: [5371], 's_1_1': [5372]}, {0: [722, 3348], 3: [3303, 676], 's_0_3': [737], 7: [616], 's_0_7': [3333], 8: [572, 3377], 's_0_8': [3318], 's_0_0': [662], 2: [631], 's_3_2': [3273], 5: [3212], 's_3_5': [661], 's_3_7': [601], 's_3_8': [646], 's_3_3': [3168], 's_7_7': [617], 's_8_2': [3362], 's_8_8': [3376], 's_2_2': [630], 6: [586], 's_5_6': [571], 9: [556], 's_5_9': [541], 's_5_5': [3213], 's_6_6': [3182], 4: [3257], 's_9_4': [3242], 's_9_9': [3197], 's_4_4': [526], 1: [3411], 's_1_1': [3410]}, {0: [2439], 3: [4768, 2530], 's_0_3': [4783], 7: [4723], 's_0_7': [4738], 8: [4693, 2454], 's_0_8': [4812], 's_0_0': [2440], 2: [4753], 's_3_2': [2469], 5: [4813], 's_3_5': [2545], 's_3_7': [2514], 's_3_8': [4798], 's_3_3': [4843], 's_7_7': [4722], 's_8_2': [2499], 's_8_8': [2544], 's_2_2': [2424], 6: [2634], 's_5_6': [2619], 9: [2604], 's_5_9': [4828], 's_5_5': [4814], 's_6_6': [4769], 4: [2589], 's_9_4': [4678], 's_9_9': [2603], 's_4_4': [4663], 1: [2118], 's_1_1': [3611]}, {0: [3412], 3: [1427, 3382], 's_0_3': [1472], 7: [1577], 's_0_7': [3397], 8: [3352, 1412], 's_0_8': [1442], 's_0_0': [1502], 2: [3427], 's_3_2': [1487], 5: [1516], 's_3_5': [3367], 's_3_7': [1562], 's_3_8': [1457], 's_3_3': [3381], 's_7_7': [3503], 's_8_2': [1382], 's_8_8': [1351], 's_2_2': [1367], 6: [3353], 's_5_6': [3338], 9: [3308], 's_5_9': [1501], 's_5_5': [3277], 's_6_6': [1592], 4: [3323], 's_9_4': [1637], 's_9_9': [3307], 's_4_4': [1622], 1: [3428], 's_1_1': [1652]}, {0: [2369, 5607], 3: [2428, 5547], 's_0_3': [5442], 7: [2384], 's_0_7': [5592], 8: [5637, 2339], 's_0_8': [2279], 's_0_0': [5606], 2: [2323, 2324], 's_3_2': [5457], 5: [5546, 5531], 's_3_5': [5532], 's_3_7': [5503], 's_3_8': [2429], 's_3_3': [2443], 's_7_7': [5473], 's_8_2': [5622], 's_8_8': [5667], 's_2_2': [5367], 6: [2144], 's_5_6': [2159], 9: [2233], 's_5_9': [2248], 's_5_5': [2263], 's_6_6': [2143], 4: [5517], 's_9_4': [5502], 's_9_9': [5381], 's_4_4': [2204], 1: [5492], 's_1_1': [478]}, {0: [750, 2989], 3: [3062, 3064, 3063], 's_0_3': [885], 7: [855], 's_0_7': [3003], 8: [735, 2988], 's_0_8': [3018], 's_0_0': [751], 2: [570], 's_3_2': [585], 5: [945], 's_3_5': [3079], 's_3_7': [840], 's_3_8': [720], 's_3_3': [3065], 's_7_7': [3094], 's_8_2': [2943], 's_8_8': [2987], 's_2_2': [2958], 6: [3004], 's_5_6': [3019], 9: [3049], 's_5_9': [3034], 's_5_5': [2914], 's_6_6': [3005], 4: [915], 's_9_4': [900], 's_9_9': [1005], 's_4_4': [916], 1: [3098], 's_1_1': [1621]}, {0: [3326], 3: [2041, 3311], 's_0_3': [2071], 7: [2027], 's_0_7': [2012], 8: [2116], 's_0_8': [2101], 's_0_0': [2056], 2: [2177, 3281], 's_3_2': [2162], 5: [3250, 1936], 's_3_5': [3265], 's_3_7': [3370], 's_3_8': [3220], 's_3_3': [3312], 's_7_7': [3415], 's_8_2': [3296], 's_8_8': [2115], 's_2_2': [2192], 6: [3234], 's_5_6': [1921], 9: [3310], 's_5_9': [3325], 's_5_5': [1937], 's_6_6': [1831], 4: [1966], 's_9_4': [1951], 's_9_9': [3309], 's_4_4': [3190], 1: [5017], 's_1_1': [1586]}, {0: [2656, 2657], 3: [3359, 2552], 's_0_3': [3403], 7: [3314], 's_0_7': [2641], 8: [3388], 's_0_8': [3373], 's_0_0': [3494], 2: [2596], 's_3_2': [3329], 5: [2702], 's_3_5': [3344], 's_3_7': [2626], 's_3_8': [2567], 's_3_3': [2687], 's_7_7': [2671], 's_8_2': [2581], 's_8_8': [2492], 's_2_2': [2595], 6: [3449], 's_5_6': [3434], 9: [3374], 's_5_9': [2717], 's_5_5': [2701], 's_6_6': [2777], 4: [2732], 's_9_4': [2747], 's_9_9': [2806], 's_4_4': [2731], 1: [5491], 's_1_1': [5492]}, {0: [3114], 3: [3129, 1816], 's_0_3': [1740], 7: [1801], 's_0_7': [3099], 8: [3219, 1831], 's_0_8': [1846], 's_0_0': [3115], 2: [3249], 's_3_2': [3264], 5: [1785, 3069], 's_3_5': [1710], 's_3_7': [3234], 's_3_8': [3204], 's_3_3': [3128], 's_7_7': [1802], 's_8_2': [1861], 's_8_8': [1936], 's_2_2': [3248], 6: [1845], 's_5_6': [3024], 9: [1815], 's_5_9': [3054], 's_5_5': [1875], 's_6_6': [2934], 4: [2979], 's_9_4': [1800], 's_9_9': [3084], 's_4_4': [2980], 1: [4534], 's_1_1': [954]}, {0: [2660], 3: [3914, 3913], 's_0_3': [2720, 3989], 7: [3928], 's_0_7': [2645], 8: [2495, 3943], 's_0_8': [3958], 's_0_0': [4019], 2: [2570], 's_3_2': [2555], 5: [2629, 3809], 's_3_5': [2764], 's_3_7': [2584], 's_3_8': [2540], 's_3_3': [2735], 's_7_7': [3927], 's_8_2': [3988], 's_8_8': [3898], 's_2_2': [2569], 6: [2659], 's_5_6': [2644], 9: [2689], 's_5_9': [3854], 's_5_5': [3778], 's_6_6': [3704], 4: [2674], 's_9_4': [3779], 's_9_9': [3764], 's_4_4': [3734], 1: [5474], 's_1_1': [2608]}, {0: [1050], 3: [930, 1095, 2975], 's_0_3': [3035], 7: [3020], 's_0_7': [3005], 8: [3125, 1020], 's_0_8': [3095], 's_0_0': [3110], 2: [3080], 's_3_2': [3079], 5: [2974, 885], 's_3_5': [3064], 's_3_7': [1080], 's_3_8': [3034], 's_3_3': [3065], 's_7_7': [1200], 's_8_2': [1005], 's_8_8': [960], 's_2_2': [1155], 6: [915], 's_5_6': [2989], 9: [3094], 's_5_9': [840], 's_5_5': [3139], 's_6_6': [2959], 4: [901], 's_9_4': [916], 's_9_9': [855], 's_4_4': [900], 1: [1557], 's_1_1': [5303]}, {0: [2358, 3462], 3: [3552, 2313], 's_0_3': [2312], 7: [2417], 's_0_7': [2402], 8: [3627], 's_0_8': [3612], 's_0_0': [2327], 2: [2373], 's_3_2': [3582], 5: [2298, 3642], 's_3_5': [3537], 's_3_7': [3567], 's_3_8': [2343], 's_3_3': [2314], 's_7_7': [3447], 's_8_2': [2388], 's_8_8': [3626], 's_2_2': [3523], 6: [3657], 's_5_6': [2268], 9: [2359], 's_5_9': [3672], 's_5_5': [3581], 's_6_6': [2389], 4: [2344], 's_9_4': [3717], 's_9_9': [3807], 's_4_4': [2345], 1: [4413], 's_1_1': [593]}, {0: [405], 3: [375, 2942, 2941], 's_0_3': [2911], 7: [390], 's_0_7': [2926], 8: [3031, 3030], 's_0_8': [3046], 's_0_0': [2987], 2: [210], 's_3_2': [2956], 5: [555], 's_3_5': [2957], 's_3_7': [3016], 's_3_8': [225], 's_3_3': [2943], 's_7_7': [391], 's_8_2': [3045], 's_8_8': [150], 's_2_2': [2925], 6: [3047], 's_5_6': [3032], 9: [3063, 3062], 's_5_9': [540], 's_5_5': [2927], 's_6_6': [645], 4: [3078], 's_9_4': [630], 's_9_9': [465], 's_4_4': [750], 1: [1893], 's_1_1': [3610]}, {0: [2482], 3: [2527, 4258], 's_0_3': [4348], 7: [2467], 's_0_7': [4393], 8: [4272, 2406], 's_0_8': [4287], 's_0_0': [4408], 2: [2421], 's_3_2': [4228], 5: [2662, 4273], 's_3_5': [2542], 's_3_7': [4333], 's_3_8': [2436], 's_3_3': [2528], 's_7_7': [2468], 's_8_2': [4213], 's_8_8': [4197], 's_2_2': [2422], 6: [4394], 's_5_6': [4409], 9: [2557], 's_5_9': [2572], 's_5_5': [2586], 's_6_6': [2632], 4: [4244], 's_9_4': [4259], 's_9_9': [2558], 's_4_4': [2707], 1: [5073], 's_1_1': [777]}, {0: [388, 5311, 313], 3: [5446, 448], 's_0_3': [5431], 7: [463, 5371], 's_0_7': [5386], 8: [5401], 's_0_8': [373], 's_0_0': [5461], 2: [403, 5416], 's_3_2': [404], 5: [419], 's_3_5': [5507], 's_3_7': [5492], 's_3_8': [328], 's_3_3': [449], 's_7_7': [5447], 's_8_2': [418], 's_8_8': [5400], 's_2_2': [5251], 6: [5551], 's_5_6': [5566], 9: [5581], 's_5_9': [5596], 's_5_5': [5536], 's_6_6': [464], 4: [314], 's_9_4': [329], 's_9_9': [359], 's_4_4': [5535], 1: [5195], 's_1_1': [5196]}, {0: [130], 3: [175, 4785], 's_0_3': [4770], 7: [4875], 's_0_7': [4860], 8: [145], 's_0_8': [4905], 's_0_0': [129], 2: [4935], 's_3_2': [160], 5: [4755, 114], 's_3_5': [69], 's_3_7': [190], 's_3_8': [4890], 's_3_3': [4845], 's_7_7': [115], 's_8_2': [4920], 's_8_8': [146], 's_2_2': [56], 6: [4680], 's_5_6': [99], 9: [174], 's_5_9': [4710], 's_5_5': [113], 's_6_6': [4681], 4: [4650], 's_9_4': [4665], 's_9_9': [4620], 's_4_4': [264], 1: [3645], 's_1_1': [108]}, {0: [1399], 3: [3697, 1310, 1309], 's_0_3': [3712], 7: [3771], 's_0_7': [3756], 8: [3847], 's_0_8': [1384], 's_0_0': [1400], 2: [3862], 's_3_2': [1295], 5: [1338], 's_3_5': [3651], 's_3_7': [1294], 's_3_8': [1429], 's_3_3': [1459], 's_7_7': [1249], 's_8_2': [1339], 's_8_8': [3848], 's_2_2': [3861], 6: [1323], 's_5_6': [3591], 9: [3682], 's_5_9': [3667], 's_5_5': [3636], 's_6_6': [1322], 4: [1428], 's_9_4': [1413], 's_9_9': [1353], 's_4_4': [1427], 1: [5223], 's_1_1': [5222]}, {0: [4602, 2228], 3: [4692, 2319], 's_0_3': [2364], 7: [2289], 's_0_7': [4631], 8: [2349, 4662], 's_0_8': [4587], 's_0_0': [2227], 2: [2394], 's_3_2': [4707], 5: [4737], 's_3_5': [2274], 's_3_7': [4752], 's_3_8': [4647], 's_3_3': [2304], 's_7_7': [4676], 's_8_2': [4557], 's_8_8': [2469], 's_2_2': [4573], 6: [2350], 's_5_6': [2365], 9: [2395], 's_5_9': [4722], 's_5_5': [4736], 's_6_6': [4797], 4: [2380], 's_9_4': [4842], 's_9_9': [4812], 's_4_4': [4783], 1: [1755], 's_1_1': [3038]}, {0: [1971, 4120], 3: [1956, 4075], 's_0_3': [4180], 7: [4105], 's_0_7': [2031], 8: [4150], 's_0_8': [2001], 's_0_0': [2076], 2: [1941], 's_3_2': [4060], 5: [4014, </t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>[{0: [3273], 3: [3288], 7: [661], 8: [646], 2: [631], 5: [676], 6: [3182], 9: [3168], 4: [645], 1: [4583]}, {0: [3612], 3: [3627], 7: [2328], 8: [2358], 2: [2343], 5: [3628], 6: [2478], 9: [2463], 4: [3643], 1: [750]}, {0: [606], 3: [4157], 7: [621], 8: [4142], 2: [516], 5: [4156], 6: [291], 9: [441], 4: [4171], 1: [4974]}, {0: [2120], 3: [2105], 7: [3971], 8: [4046], 2: [4031], 5: [3940], 6: [2015], 9: [2090], 4: [4001], 1: [4554]}, {0: [1384], 3: [3817], 7: [1399], 8: [3832], 2: [1414], 5: [1354], 6: [1355], 9: [3921], 4: [3922], 1: [4865]}, {0: [4915], 3: [4900], 7: [1960], 8: [2036], 2: [2021], 5: [1930], 6: [4870], 9: [4885], 4: [1915], 1: [5516]}, {0: [1852], 3: [1837], 7: [4225], 8: [4269], 2: [4284], 5: [4299], 6: [1807], 9: [1927], 4: [4314], 1: [3485]}, {0: [1231], 3: [1246], 7: [3321], 8: [3186], 2: [3201], 5: [3156], 6: [3171], 9: [1261], 4: [3246], 1: [3210]}, {0: [614], 3: [5702], 7: [629], 8: [5717], 2: [644], 5: [5701], 6: [464], 9: [479], 4: [5551], 1: [5295]}, {0: [1645], 3: [1630], 7: [4718], 8: [4868], 2: [4883], 5: [4778], 6: [4793], 9: [1480], 4: [4732], 1: [1719]}, {0: [1441], 3: [3142], 7: [1456], 8: [3127], 2: [1291], 5: [1335], 6: [3111], 9: [1336], 4: [3381], 1: [4759]}, {0: [2534], 3: [5533], 7: [2549], 8: [5548], 2: [2579], 5: [2564], 6: [5519], 9: [5504], 4: [2638], 1: [4783]}, {0: [119], 3: [104], 7: [5625], 8: [5655], 2: [5640], 5: [5685], 6: [89], 9: [74], 4: [5670], 1: [1938]}, {0: [5680], 3: [1919], 7: [5695], 8: [1904], 2: [5650], 5: [5574], 6: [5573], 9: [1859], 4: [5515], 1: [2490]}, {0: [3286], 3: [3271], 7: [331], 8: [362], 2: [377], 5: [346], 6: [3256], 9: [3211], 4: [496], 1: [3373]}, {0: [5670], 3: [119], 7: [5685], 8: [104], 2: [5655], 5: [5580], 6: [179], 9: [239], 4: [5430], 1: [5272]}, {0: [210], 3: [375, 2941], 7: [2956], 8: [225], 2: [2971], 5: [3001], 6: [405], 9: [345], 4: [3136], 1: [4962]}, {0: [5459], 3: [5444], 7: [2729], 8: [2759], 2: [2744], 5: [2653], 6: [5324], 9: [5414], 4: [2698], 1: [3167]}, {0: [1808], 3: [4389], 7: [1823], 8: [4404], 2: [1777], 5: [1792], 6: [1793], 9: [4314], 4: [1912], 1: [1254]}, {0: [4297], 3: [1537, 4373], 7: [4312], 8: [1582], 2: [1567], 5: [1673], 6: [1672], 9: [4358], 4: [4357], 1: [3749]}, {0: [1324], 3: [1339], 7: [3877], 8: [3862], 2: [3847], 5: [3816], 6: [1234], 9: [1295], 4: [1296], 1: [1179]}, {0: [1824], 3: [1809], 7: [4599], 8: [4539], 2: [4554], 5: [1808], 6: [4524], 9: [4479], 4: [1778], 1: [4946]}, {0: [3078], 3: [2988, 720], 7: [675], 8: [3063], 2: [735], 5: [2987], 6: [510], 9: [525], 4: [3047], 1: [203]}, {0: [1275], 3: [1260], 7: [3036], 8: [3066], 2: [3081], 5: [2916], 6: [2931], 9: [2917], 4: [2918], 1: [4009]}, {0: [4099], 3: [4084], 7: [965], 8: [921], 2: [906], 5: [951], 6: [952], 9: [4025], 4: [1086], 1: [3753]}, {0: [911], 3: [926], 7: [4954], 8: [5044], 2: [5059], 5: [925], 6: [4849], 9: [4759], 4: [834], 1: [536]}, {0: [4995], 3: [4980], 7: [295], 8: [221], 2: [236], 5: [161], 6: [5055], 9: [5085], 4: [237], 1: [4458]}, {0: [4022], 3: [515], 7: [4037], 8: [530], 2: [3932], 5: [3962], 6: [3961], 9: [620], 4: [4053], 1: [4279]}, {0: [4226], 3: [2032], 7: [4211], 8: [2017], 2: [4241], 5: [4195], 6: [1956], 9: [4194], 4: [1822], 1: [1381]}, {0: [4652], 3: [594], 7: [4667], 8: [579], 2: [4637], 5: [593], 6: [4428], 9: [4517], 4: [563], 1: [4563]}, {0: [631], 3: [3303], 7: [646], 8: [3318], 2: [661], 5: [616], 6: [617], 9: [3257], 4: [3242], 1: [4768]}, {0: [5691], 3: [1184], 7: [5676], 8: [1199], 2: [5705], 5: [5586], 6: [1289], 9: [1334], 4: [1349], 1: [1837]}, {0: [3313], 3: [2446], 7: [3328], 8: [2431], 2: [3358], 5: [3387], 6: [2416], 9: [3386], 4: [2221], 1: [1460]}, {0: [3324], 3: [3309], 7: [1741], 8: [1696], 2: [1681], 5: [1726], 6: [3218], 9: [3249], 4: [1831], 1: [2805]}, {0: [2354], 3: [2369], 7: [5577], 8: [5517], 2: [5502], 5: [5547], 6: [2413], 9: [2474], 4: [2473], 1: [5262]}, {0: [3614], 3: [3629], 7: [2778], 8: [2703], 2: [2718], 5: [2688], 6: [3524], 9: [3599], 4: [3598], 1: [1880]}, {0: [3708], 3: [603], 7: [3693], 8: [618], 2: [3678], 5: [3617], 6: [543], 9: [498], 4: [3556], 1: [4956]}, {0: [3856], 3: [244], 7: [3841], 8: [259], 2: [3750], 5: [3871], 6: [305], 9: [274], 4: [3796], 1: [2231]}, {0: [1043], 3: [1028], 7: [4474], 8: [4535], 2: [4550], 5: [4415], 6: [938], 9: [967], 4: [4309], 1: [63]}, {0: [3906], 3: [3816, 1339], 7: [1280], 8: [3921], 2: [1324], 5: [3892], 6: [1295], 9: [3891], 4: [1265], 1: [332]}, {0: [338], 3: [353], 7: [4471], 8: [4531], 2: [4546], 5: [4561], 6: [384], 9: [293], 4: [4501], 1: [5608]}, {0: [740], 3: [725], 7: [3903], 8: [3978], 2: [3963], 5: [3828], 6: [649], 9: [664], 4: [665], 1: [2099]}, {0: [5280], 3: [193], 7: [5295], 8: [208], 2: [5325], 5: [5340], 6: [238], 9: [223], 4: [5355], 1: [2411]}, {0: [4776], 3: [1120], 7: [4791], 8: [1135], 2: [4820], 5: [4761], 6: [4760], 9: [1224], 4: [4701], 1: [621]}, {0: [5016], 3: [5031], 7: [1256], 8: [1406], 2: [1391], 5: [1286], 6: [1285], 9: [4896], 4: [1225], 1: [591]}, {0: [4808], 3: [4823], 7: [1615], 8: [1660], 2: [1675], 5: [1765], 6: [4884], 9: [4794], 4: [1825], 1: [2474]}, {0: [5089], 3: [5074], 7: [912], 8: [896], 2: [881], 5: [866], 6: [4969], 9: [851], 4: [4998], 1: [1590]}, {0: [4238], 3: [1521], 7: [4253], 8: [1506], 2: [4208], 5: [4177], 6: [1356], 9: [4178], 4: [4193], 1: [280]}, {0: [4214], 3: [2557], 7: [4229], 8: [2572], 2: [4183], 5: [4288], 6: [2647], 9: [2601], 4: [4153], 1: [258]}, {0: [3242], 3: [556], 7: [3257], 8: [541], 2: [3197], 5: [555], 6: [2987], 9: [2972], 4: [390], 1: [5130]}, {0: [2462], 3: [3358], 7: [2477], 8: [3343], 2: [2372], 5: [2507], 6: [3478], 9: [3493], 4: [2538], 1: [2442]}, {0: [4232], 3: [547], 7: [4247], 8: [562], 2: [4217], 5: [4307], 6: [652], 9: [532], 4: [4292], 1: [5363]}, {0: [3160], 3: [1936], 7: [3175], 8: [1921], 2: [3265], 5: [3204], 6: [1905], 9: [1771], 4: [3189], 1: [2957]}, {0: [4556], 3: [2199], 7: [4541], 8: [2214], 2: [4646], 5: [4691], 6: [2094], 9: [2079], 4: [4675], 1: [1691]}, {0: [3800], 3: [1054], 7: [3785], 8: [1069], 2: [3770], 5: [3815], 6: [1144], 9: [1039], 4: [3724], 1: [2719]}, {0: [4504], 3: [4519], 7: [863], 8: [833], 2: [818], 5: [923], 6: [4459], 9: [4474], 4: [4489], 1: [609]}, {0: [2191], 3: [2206], 7: [3147], 8: [3162], 2: [3177], 5: [3132], 6: [3131], 9: [2341], 4: [3267], 1: [3160]}, {0: [725], 3: [3948], 7: [740], 8: [3933], 2: [845], 5: [800], 6: [785], 9: [4039], 4: [860], 1: [2500]}, {0: [3612], 3: [3627], 7: [2343], 8: [2268], 2: [2253], 5: [2313], 6: [3657], 9: [3582], 4: [2448], 1: [4286]}, {0: [5611], 3: [5626], 7: [359], 8: [329], 2: [314], 5: [344], 6: [5536], 9: [5551], 4: [5566], 1: [1147]}, {0: [1410], 3: [3082], 7: [1425], 8: [3067], 2: [1455], 5: [1380], 6: [1395], 9: [3051], 4: [1350], 1: [4259]}, {0: [4203], 3: [4218], 7: [621], 8: [651], 2: [636], 5: [696], 6: [4068], 9: [4113], 4: [726], 1: [4483]}, {0: [1043], 3: [4415], 7: [1028], 8: [4430], 2: [967], 5: [938], 6: [4489], 9: [4519], 4: [878], 1: [2983]}, {0: [1107], 3: [5105], 7: [1092], 8: [5120], 2: [1076], 5: [1031], 6: [5075], 9: [5014], 4: [971], 1: [4856]}, {0: [2423], 3: [2408], 7: [4573], 8: [4542], 2: [4557], 5: [4647], 6: [2469], 9: [2453], 4: [2452], 1: [1796]}, {0: [866], 3: [5044], 7: [851], 8: [5059], 2: [911], 5: [5045], 6: [1031], 9: [1061], 4: [5015], 1: [4288]}, {0: [4672], 3: [4657], 7: [1464], 8: [1494], 2: [1479], 5: [4658], 6: [1674], 9: [4659], 4: [1899], 1: [1609]}, {0: [2979], 3: [1770], 7: [2994], 8: [1785], 2: [3114], 5: [3054], 6: [3039], 9: [3053], 4: [1590], 1: [4385]}, {0: [1358], 3: [1373], 7: [4597], 8: [4582], 2: [4567], 5: [4626], 6: [1269], 9: [1404], 4: [4612], 1: [3566]}, {0: [859], 3: [844], 7: [3859], 8: [3814], 2: [3829], 5: [3799], 6: [949], 9: [3798], 4: [664], 1: [325]}, {0: [4540], 3: [2048], 7: [4555], 8: [2063], 2: [4645], 5: [4571], 6: [4572], 9: [2184], 4: [4676], 1: [2571]}, {0: [5345], 3: [5360], 7: [1078], 8: [1123], 2: [1138], 5: [1197], 6: [5210], 9: [5256], 4: [1288], 1: [1926]}, {0: [3807], 3: [2299], 7: [3792], 8: [2284], 2: [3776], 5: [3852], 6: [2224], 9: [2239], 4: [3806], 1: [2817]}, {0: [5325], 3: [5310], 7: [178], 8: [43], 2: [58], 5: [148], 6: [5400], 9: [5415], 4: [118], 1: [3956]}, {0: [960], 3: [975], 7: [3034], 8: [3109], 2: [3094], 5: [3199], 6: [1005], 9: [931], 4: [932], 1: [178]}, {0: [3219], 3: [1876], 7: [3234], 8: [1861], 2: [3384], 5: [3310], 6: [1966], 9: [3325], 4: [1951], 1: [3221]}, {0: [5002], 3: [4987], 7: [1586], 8: [1451], 2: [1466], 5: [1496], 6: [1495], 9: [4943], 4: [1600], 1: [1976]}, {0: [5479], 3: [5464], 7: [808], 8: [929], 2: [914], 5: [764], 6: [779], 9: [5509], 4: [823], 1: [3512]}, {0: [398], 3: [4351], 7: [413], 8: [4366], 2: [277], 5: [442], 6: [443], 9: [441], 4: [426], 1: [3799]}, {0: [1793], 3: [1778], 7: [4449], 8: [4434], 2: [4419], 5: [4524], 6: [1823], 9: [1853], 4: [1854], 1: [905]}, {0: [2747], 3: [2732], 7: [3449], 8: [3419], 2: [3404], 5: [3434], 6: [2627], 9: [2642], 4: [2643], 1: [4244]}, {0: [2965], 3: [1995], 7: [2950], 8: [1980], 2: [3085], 5: [2980], 6: [2979], 9: [1965], 4: [3070], 1: [2625]}, {0: [2636], 3: [2621], 7: [5144], 8: [5099], 2: [5084], 5: [5173], 6: [2532], 9: [2577], 4: [5083], 1: [737]}, {0: [2001], 3: [4045], 7: [1986], 8: [4030], 2: [1880], 5: [1925], 6: [3954], 9: [4000], 4: [3999], 1: [2167]}, {0: [658], 3: [643], 7: [5537], 8: [5372], 2: [5387], 5: [5433], 6: [5434], 9: [764], 4: [5448], 1: [2684]}, {0: [5127], 3: [2321], 7: [5112], 8: [2336], 2: [5097], 5: [5037], 6: [2426], 9: [2411], 4: [5187], 1: [3436]}, {0: [548], 3: [563], 7: [4487], 8: [4397], 2: [4382], 5: [4352], 6: [4353], 9: [578], 4: [4517], 1: [3992]}, {0: [4460], 3: [1177], 7: [4445], 8: [1192], 2: [4416], 5: [1178], 6: [4611], 9: [4506], 4: [1193], 1: [3029]}, {0: [1772], 3: [1787], 7: [3354], 8: [3504], 2: [3489], 5: [3399], 6: [3398], 9: [1847], 4: [1832], 1: [194]}, {0: [1025], 3: [1040], 7: [3965], 8: [4040], 2: [4025], 5: [1039], 6: [3710], 9: [3785], 4: [1114], 1: [858]}, {0: [2726], 3: [2711], 7: [5009], 8: [4964], 2: [4979], 5: [5024], 6: [2846], 9: [2741], 4: [2740], 1: [3504]}, {0: [1431], 3: [4192], 7: [1416], 8: [4177], 2: [1521], 5: [1386], 6: [4072], 9: [4222], 4: [1297], 1: [3601]}, {0: [2092], 3: [4376], 7: [2077], 8: [4361], 2: [2213], 5: [2183], 6: [4421], 9: [4496], 4: [4481], 1: [1823]}, {0: [1606], 3: [1651, 3233], 7: [3218], 8: [1591], 2: [3203], 5: [1650], 6: [3038], 9: [3023], 4: [1740], 1: [3714]}, {0: [1335], 3: [1320], 7: [3201], 8: [3127], 2: [3142], 5: [3081], 6: [1230], 9: [3066], 4: [1290], 1: [1790]}, {0: [5690], 3: [5675], 7: [974], 8: [1004], 2: [1019], 5: [989], 6: [5569], 9: [5584], 4: [5599], 1: [115]}, {0: [170], 3: [155], 7: [3990], 8: [3960], 2: [3975], 5: [4035], 6: [125], 9: [186], 4: [4125], 1: [4198]}, {0: [5661], 3: [5646], 7: [1214], 8: [1169], 2: [1154], 5: [5647], 6: [1364], 9: [1394], 4: [5512], 1: [1398]}, {0: [3972], 3: [3987], 7: [2315], 8: [2360], 2: [2345], 5: [2300], 6: [3941], 9: [4017], 4: [2376], 1: [5283]}, {0: [2304], 3: [2289], 7: [4752], 8: [4737], 2: [4722], 5: [4631], 6: [2273], 9: [2139], 4: [4691], 1: [3748]}]</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>[34, 34, 35, 37, 34, 32, 34, 34, 33, 34, 33, 35, 35, 32, 36, 35, 34, 33, 35, 33, 33, 35, 34, 33, 34, 32, 32, 35, 34, 35, 34, 33, 35, 36, 35, 33, 34, 33, 34, 34, 33, 34, 34, 34, 35, 35, 33, 33, 33, 33, 35, 34, 33, 33, 36, 35, 34, 33, 34, 35, 35, 34, 35, 34, 36, 33, 33, 34, 34, 35, 34, 32, 34, 34, 36, 34, 34, 34, 35, 35, 34, 36, 34, 33, 34, 35, 33, 34, 35, 33, 33, 33, 35, 33, 35, 34, 33, 34, 34, 34]</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>[10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 11, 10, 10, 11, 10, 10, 11, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 11, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 10, 11, 10, 10, 10, 10, 10, 10]</t>
-        </is>
-      </c>
-      <c r="AH3" t="n">
-        <v>1.019556251265691</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>0.2190429135575903</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL3" t="inlineStr">
-        <is>
-          <t>[0.06984519958496094, 0.06853437423706055, 0.06811738014221191, 0.13138771057128906, 0.06470155715942383, 0.06525468826293945, 0.10083341598510742, 0.07143759727478027, 0.06528949737548828, 0.0742197036743164, 0.06391716003417969, 0.06442904472351074, 0.06348395347595215, 0.06671357154846191, 0.06952047348022461, 0.10572290420532227, 0.062467336654663086, 0.06014275550842285, 0.06584835052490234, 0.06183028221130371, 0.060778141021728516, 0.06789660453796387, 0.06136965751647949, 0.06287503242492676, 0.06726574897766113, 0.06099200248718262, 0.07400727272033691, 0.0757589340209961, 0.07913970947265625, 0.07289004325866699, 0.0825955867767334, 0.06287932395935059, 0.06751108169555664, 0.07165765762329102, 0.07882070541381836, 0.07353782653808594, 0.06813526153564453, 0.06232094764709473, 0.07119178771972656, 0.0749974250793457, 0.06043386459350586, 0.07106351852416992, 0.06658267974853516, 0.06232762336730957, 0.06501197814941406, 0.06529450416564941, 0.06378006935119629, 0.07217025756835938, 0.06702327728271484, 0.0689401626586914, 0.07009291648864746, 0.06259679794311523, 0.0645289421081543, 0.06157875061035156, 0.06485581398010254, 0.08320379257202148, 0.06815218925476074, 0.06760406494140625, 0.07789278030395508, 0.07126641273498535, 0.11800503730773926, 0.06667494773864746, 0.08067440986633301, 0.06645679473876953, 0.0640108585357666, 0.07017922401428223, 0.08061385154724121, 0.06556582450866699, 0.08311104774475098, 0.06459784507751465, 0.07005834579467773, 0.061223506927490234, 0.0720674991607666, 0.06400394439697266, 0.06548452377319336, 0.06347823143005371, 0.07304167747497559, 0.06199955940246582, 0.07892942428588867, 0.07347249984741211, 0.06727814674377441, 0.06738662719726562, 0.0717308521270752, 0.06270909309387207, 0.07044410705566406, 0.07180142402648926, 0.06848692893981934, 0.0796966552734375, 0.06819868087768555, 0.08461809158325195, 0.07037639617919922, 0.0633852481842041, 0.07919716835021973, 0.06432485580444336, 0.06438851356506348, 0.061383962631225586, 0.0630643367767334, 0.06589674949645996, 0.06073498725891113, 0.06940960884094238]</t>
-        </is>
-      </c>
-      <c r="AM3" t="inlineStr">
-        <is>
-          <t>[0.034558773040771484, 0.03331565856933594, 0.03128385543823242, 0.031441450119018555, 0.033467769622802734, 0.03136467933654785, 0.03355121612548828, 0.031439781188964844, 0.03072500228881836, 0.03154444694519043, 0.031324148178100586, 0.03167414665222168, 0.03615856170654297, 0.03183794021606445, 0.031369924545288086, 0.03221559524536133, 0.031386613845825195, 0.03356313705444336, 0.033776283264160156, 0.034665822982788086, 0.03256535530090332, 0.04671764373779297, 0.03143429756164551, 0.03222298622131348, 0.03146004676818848, 0.031581878662109375, 0.03562140464782715, 0.033721923828125, 0.03331351280212402, 0.03874945640563965, 0.03160691261291504, 0.03253054618835449, 0.03121328353881836, 0.035611867904663086, 0.031038284301757812, 0.032660722732543945, 0.0327606201171875, 0.031838178634643555, 0.033660173416137695, 0.03237128257751465, 0.031534433364868164, 0.033622026443481445, 0.03301548957824707, 0.03700375556945801, 0.031595468521118164, 0.033601999282836914, 0.03338932991027832, 0.03371930122375488, 0.033087730407714844, 0.0346674919128418, 0.033046722412109375, 0.03193235397338867, 0.03436279296875, 0.03519701957702637, 0.03369259834289551, 0.031581878662109375, 0.03165793418884277, 0.03146982192993164, 0.031208515167236328, 0.03128528594970703, 0.03455710411071777, 0.032573699951171875, 0.03468823432922363, 0.0334775447845459, 0.034125566482543945, 0.03277754783630371, 0.03160691261291504, 0.032013893127441406, 0.034013986587524414, 0.03561282157897949, 0.033943891525268555, 0.033263206481933594, 0.03305220603942871, 0.03144526481628418, 0.031301259994506836, 0.031419992446899414, 0.03137040138244629, 0.03107619285583496, 0.031244277954101562, 0.03349113464355469, 0.03212547302246094, 0.030991315841674805, 0.031199932098388672, 0.031766653060913086, 0.031256914138793945, 0.03128409385681152, 0.03501462936401367, 0.034789085388183594, 0.033315420150756836, 0.0334019660949707, 0.03289937973022461, 0.034448862075805664, 0.03154444694519043, 0.03175759315490723, 0.03274726867675781, 0.03081679344177246, 0.031906843185424805, 0.031133174896240234, 0.03420543670654297, 0.03187155723571777]</t>
-        </is>
-      </c>
-      <c r="AN3" t="n">
-        <v>74</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>21</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>31</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>10</v>
-      </c>
-      <c r="AR3" t="inlineStr">
-        <is>
-          <t>[0, 3, 's_0_3', 7, 's_0_7', 8, 's_0_8', 's_0_0', 2, 's_3_2', 5, 's_3_5', 's_3_7', 's_3_8', 's_3_3', 's_7_7', 's_8_2', 's_8_8', 's_2_2', 6, 's_5_6', 9, 's_5_9', 's_5_5', 's_6_6', 4, 's_9_4', 's_9_9', 's_4_4', 1, 's_1_1']</t>
-        </is>
-      </c>
-      <c r="AS3" t="inlineStr">
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>[0, 3, 's_0_3', 7, 's_0_7', 8, 's_0_8', 2, 's_2_3', 5, 's_3_5', 's_3_7', 's_3_8', 's_2_8', 6, 's_5_6', 9, 's_5_9', 4, 's_4_9', 1]</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
         <is>
           <t>[0, 3, 7, 8, 2, 5, 6, 9, 4, 1]</t>
         </is>
@@ -939,12 +903,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>[0, 3, 11, 12, 2, 5, 10, 6, 8, 14, 16, 17, 18, 1, 4, 9, 13, 15, 7, 19]</t>
+          <t>[0, 3, 11, 12, 1, 6, 10, 13, 2, 5, 8, 18, 4, 16, 14, 9, 17, 7, 15, 19]</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>[(0, 3), (0, 11), (0, 12), (0, 0), (3, 2), (3, 5), (3, 10), (3, 3), (11, 6), (11, 8), (11, 10), (11, 14), (11, 16), (11, 17), (11, 18), (11, 11), (12, 1), (12, 4), (12, 8), (12, 9), (12, 16), (12, 18), (12, 12), (2, 6), (2, 5), (2, 8), (2, 18), (2, 2), (5, 10), (5, 4), (5, 14), (5, 5), (10, 1), (10, 8), (10, 9), (10, 15), (10, 10), (6, 1), (6, 9), (6, 13), (6, 17), (6, 6), (8, 9), (8, 16), (8, 8), (14, 7), (14, 19), (14, 14), (16, 18), (16, 4), (16, 7), (16, 17), (16, 16), (17, 7), (17, 17), (18, 13), (18, 18), (1, 13), (1, 1), (4, 4), (9, 9), (13, 13), (15, 19), (15, 15), (7, 7), (19, 19)]</t>
+          <t>[(0, 3), (0, 11), (0, 12), (3, 2), (3, 5), (3, 10), (11, 6), (11, 8), (11, 10), (11, 14), (11, 16), (11, 17), (11, 18), (12, 1), (12, 4), (12, 8), (12, 9), (12, 16), (12, 18), (1, 6), (1, 10), (1, 13), (6, 2), (6, 9), (6, 13), (6, 17), (10, 5), (10, 8), (10, 9), (10, 15), (13, 18), (2, 5), (2, 8), (2, 18), (5, 4), (5, 14), (8, 9), (8, 16), (18, 16), (4, 16), (16, 7), (16, 17), (14, 7), (14, 19), (17, 7), (15, 19)]</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -959,143 +923,107 @@
         <v>0.002534468157697533</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0667578659370725</v>
+        <v>0.0951048951048951</v>
       </c>
       <c r="K4" t="n">
         <v>0.3473684210526316</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[(0, 3), (0, 's_0_3'), (0, 11), (0, 's_0_11'), (0, 12), (0, 's_0_12'), (0, 's_0_0'), (0, 0), (3, 's_0_3'), (3, 2), (3, 's_3_2'), (3, 5), (3, 's_3_5'), (3, 10), (3, 's_3_10'), (3, 's_3_3'), (3, 3), ('s_0_3', 's_0_3'), (11, 's_0_11'), (11, 6), (11, 's_11_6'), (11, 8), (11, 's_11_8'), (11, 10), (11, 's_11_10'), (11, 14), (11, 's_11_14'), (11, 16), (11, 's_11_16'), (11, 17), (11, 's_11_17'), (11, 18), (11, 's_11_18'), (11, 's_11_11'), (11, 11), ('s_0_11', 's_0_11'), (12, 's_0_12'), (12, 1), (12, 's_12_1'), (12, 4), (12, 's_12_4'), (12, 8), (12, 's_12_8'), (12, 9), (12, 's_12_9'), (12, 16), (12, 's_12_16'), (12, 18), (12, 's_12_18'), (12, 's_12_12'), (12, 12), ('s_0_12', 's_0_12'), ('s_0_0', 's_0_0'), (2, 's_3_2'), (2, 6), (2, 's_2_6'), (2, 5), (2, 's_2_5'), (2, 8), (2, 's_2_8'), (2, 18), (2, 's_2_18'), (2, 's_2_2'), (2, 2), ('s_3_2', 's_3_2'), (5, 's_3_5'), (5, 's_2_5'), (5, 10), (5, 's_5_10'), (5, 4), (5, 's_5_4'), (5, 14), (5, 's_5_14'), (5, 's_5_5'), (5, 5), ('s_3_5', 's_3_5'), (10, 's_3_10'), (10, 's_11_10'), (10, 's_5_10'), (10, 1), (10, 's_10_1'), (10, 8), (10, 's_10_8'), (10, 9), (10, 's_10_9'), (10, 15), (10, 's_10_15'), (10, 's_10_10'), (10, 10), ('s_3_10', 's_3_10'), ('s_3_3', 's_3_3'), (6, 's_11_6'), (6, 's_2_6'), (6, 1), (6, 's_6_1'), (6, 9), (6, 's_6_9'), (6, 13), (6, 's_6_13'), (6, 17), (6, 's_6_17'), (6, 's_6_6'), (6, 6), ('s_11_6', 's_11_6'), (8, 's_11_8'), (8, 's_12_8'), (8, 's_2_8'), (8, 's_10_8'), (8, 9), (8, 's_8_9'), (8, 16), (8, 's_8_16'), (8, 's_8_8'), (8, 8), ('s_11_8', 's_11_8'), ('s_11_10', 's_11_10'), (14, 's_11_14'), (14, 's_5_14'), (14, 7), (14, 's_14_7'), (14, 19), (14, 's_14_19'), (14, 's_14_14'), (14, 14), ('s_11_14', 's_11_14'), (16, 's_11_16'), (16, 's_12_16'), (16, 's_8_16'), (16, 18), (16, 's_16_18'), (16, 4), (16, 's_16_4'), (16, 7), (16, 's_16_7'), (16, 17), (16, 's_16_17'), (16, 's_16_16'), (16, 16), ('s_11_16', 's_11_16'), (17, 's_11_17'), (17, 's_6_17'), (17, 's_16_17'), (17, 7), (17, 's_17_7'), (17, 's_17_17'), (17, 17), ('s_11_17', 's_11_17'), (18, 's_11_18'), (18, 's_12_18'), (18, 's_2_18'), (18, 's_16_18'), (18, 13), (18, 's_18_13'), (18, 's_18_18'), (18, 18), ('s_11_18', 's_11_18'), ('s_11_11', 's_11_11'), (1, 's_12_1'), (1, 's_10_1'), (1, 's_6_1'), (1, 13), (1, 's_1_13'), (1, 's_1_1'), (1, 1), ('s_12_1', 's_12_1'), (4, 's_12_4'), (4, 's_5_4'), (4, 's_16_4'), (4, 's_4_4'), (4, 4), ('s_12_4', 's_12_4'), ('s_12_8', 's_12_8'), (9, 's_12_9'), (9, 's_10_9'), (9, 's_6_9'), (9, 's_8_9'), (9, 's_9_9'), (9, 9), ('s_12_9', 's_12_9'), ('s_12_16', 's_12_16'), ('s_12_18', 's_12_18'), ('s_12_12', 's_12_12'), ('s_2_6', 's_2_6'), ('s_2_5', 's_2_5'), ('s_2_8', 's_2_8'), ('s_2_18', 's_2_18'), ('s_2_2', 's_2_2'), ('s_5_10', 's_5_10'), ('s_5_4', 's_5_4'), ('s_5_14', 's_5_14'), ('s_5_5', 's_5_5'), ('s_10_1', 's_10_1'), ('s_10_8', 's_10_8'), ('s_10_9', 's_10_9'), (15, 's_10_15'), (15, 19), (15, 's_15_19'), (15, 's_15_15'), (15, 15), ('s_10_15', 's_10_15'), ('s_10_10', 's_10_10'), ('s_6_1', 's_6_1'), ('s_6_9', 's_6_9'), (13, 's_6_13'), (13, 's_18_13'), (13, 's_1_13'), (13, 's_13_13'), (13, 13), ('s_6_13', 's_6_13'), ('s_6_17', 's_6_17'), ('s_6_6', 's_6_6'), ('s_8_9', 's_8_9'), ('s_8_16', 's_8_16'), ('s_8_8', 's_8_8'), (7, 's_14_7'), (7, 's_16_7'), (7, 's_17_7'), (7, 's_7_7'), (7, 7), ('s_14_7', 's_14_7'), (19, 's_14_19'), (19, 's_15_19'), (19, 's_19_19'), (19, 19), ('s_14_19', 's_14_19'), ('s_14_14', 's_14_14'), ('s_16_18', 's_16_18'), ('s_16_4', 's_16_4'), ('s_16_7', 's_16_7'), ('s_16_17', 's_16_17'), ('s_16_16', 's_16_16'), ('s_17_7', 's_17_7'), ('s_17_17', 's_17_17'), ('s_18_13', 's_18_13'), ('s_18_18', 's_18_18'), ('s_1_13', 's_1_13'), ('s_1_1', 's_1_1'), ('s_4_4', 's_4_4'), ('s_9_9', 's_9_9'), ('s_13_13', 's_13_13'), ('s_15_19', 's_15_19'), ('s_15_15', 's_15_15'), ('s_7_7', 's_7_7'), ('s_19_19', 's_19_19')]</t>
+          <t>[(0, 3), (0, 's_0_3'), (0, 11), (0, 's_0_11'), (0, 12), (0, 's_0_12'), (0, 0), (3, 's_0_3'), (3, 2), (3, 's_2_3'), (3, 5), (3, 's_3_5'), (3, 10), (3, 's_3_10'), (3, 3), ('s_0_3', 's_0_3'), (11, 's_0_11'), (11, 6), (11, 's_6_11'), (11, 8), (11, 's_8_11'), (11, 10), (11, 's_10_11'), (11, 14), (11, 's_11_14'), (11, 16), (11, 's_11_16'), (11, 17), (11, 's_11_17'), (11, 18), (11, 's_11_18'), (11, 11), ('s_0_11', 's_0_11'), (12, 's_0_12'), (12, 1), (12, 's_1_12'), (12, 4), (12, 's_4_12'), (12, 8), (12, 's_8_12'), (12, 9), (12, 's_9_12'), (12, 16), (12, 's_12_16'), (12, 18), (12, 's_12_18'), (12, 12), ('s_0_12', 's_0_12'), (2, 6), (2, 's_2_3'), (2, 's_2_6'), (2, 5), (2, 's_2_5'), (2, 8), (2, 's_2_8'), (2, 18), (2, 's_2_18'), (2, 2), ('s_2_3', 's_2_3'), (5, 10), (5, 's_3_5'), (5, 's_5_10'), (5, 's_2_5'), (5, 4), (5, 's_4_5'), (5, 14), (5, 's_5_14'), (5, 5), ('s_3_5', 's_3_5'), (10, 1), (10, 's_3_10'), (10, 's_10_11'), (10, 's_1_10'), (10, 's_5_10'), (10, 8), (10, 's_8_10'), (10, 9), (10, 's_9_10'), (10, 15), (10, 's_10_15'), (10, 10), ('s_3_10', 's_3_10'), (6, 1), (6, 's_6_11'), (6, 's_1_6'), (6, 's_2_6'), (6, 9), (6, 's_6_9'), (6, 13), (6, 's_6_13'), (6, 17), (6, 's_6_17'), (6, 6), ('s_6_11', 's_6_11'), (8, 's_8_11'), (8, 's_8_12'), (8, 's_8_10'), (8, 's_2_8'), (8, 9), (8, 's_8_9'), (8, 16), (8, 's_8_16'), (8, 8), ('s_8_11', 's_8_11'), ('s_10_11', 's_10_11'), (14, 's_11_14'), (14, 's_5_14'), (14, 7), (14, 's_7_14'), (14, 19), (14, 's_14_19'), (14, 14), ('s_11_14', 's_11_14'), (16, 18), (16, 4), (16, 's_11_16'), (16, 's_12_16'), (16, 's_8_16'), (16, 's_16_18'), (16, 's_4_16'), (16, 7), (16, 's_7_16'), (16, 17), (16, 's_16_17'), (16, 16), ('s_11_16', 's_11_16'), (17, 's_11_17'), (17, 's_6_17'), (17, 's_16_17'), (17, 7), (17, 's_7_17'), (17, 17), ('s_11_17', 's_11_17'), (18, 13), (18, 's_11_18'), (18, 's_12_18'), (18, 's_13_18'), (18, 's_2_18'), (18, 's_16_18'), (18, 18), ('s_11_18', 's_11_18'), (1, 's_1_12'), (1, 's_1_6'), (1, 's_1_10'), (1, 13), (1, 's_1_13'), (1, 1), ('s_1_12', 's_1_12'), (4, 's_4_12'), (4, 's_4_5'), (4, 's_4_16'), (4, 4), ('s_4_12', 's_4_12'), ('s_8_12', 's_8_12'), (9, 's_9_12'), (9, 's_6_9'), (9, 's_9_10'), (9, 's_8_9'), (9, 9), ('s_9_12', 's_9_12'), ('s_12_16', 's_12_16'), ('s_12_18', 's_12_18'), ('s_1_6', 's_1_6'), ('s_1_10', 's_1_10'), (13, 's_1_13'), (13, 's_6_13'), (13, 's_13_18'), (13, 13), ('s_1_13', 's_1_13'), ('s_2_6', 's_2_6'), ('s_6_9', 's_6_9'), ('s_6_13', 's_6_13'), ('s_6_17', 's_6_17'), ('s_5_10', 's_5_10'), ('s_8_10', 's_8_10'), ('s_9_10', 's_9_10'), (15, 's_10_15'), (15, 19), (15, 's_15_19'), (15, 15), ('s_10_15', 's_10_15'), ('s_13_18', 's_13_18'), ('s_2_5', 's_2_5'), ('s_2_8', 's_2_8'), ('s_2_18', 's_2_18'), ('s_4_5', 's_4_5'), ('s_5_14', 's_5_14'), ('s_8_9', 's_8_9'), ('s_8_16', 's_8_16'), ('s_16_18', 's_16_18'), ('s_4_16', 's_4_16'), (7, 's_7_16'), (7, 's_7_14'), (7, 's_7_17'), (7, 7), ('s_7_16', 's_7_16'), ('s_16_17', 's_16_17'), ('s_7_14', 's_7_14'), (19, 's_14_19'), (19, 's_15_19'), (19, 19), ('s_14_19', 's_14_19'), ('s_7_17', 's_7_17'), ('s_15_19', 's_15_19')]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>[(0, 3), (0, 11), (0, 12), (0, 0), (3, 2), (3, 5), (3, 10), (3, 3), (11, 6), (11, 8), (11, 10), (11, 14), (11, 16), (11, 17), (11, 18), (11, 11), (12, 1), (12, 4), (12, 8), (12, 9), (12, 16), (12, 18), (12, 12), (2, 6), (2, 5), (2, 8), (2, 18), (2, 2), (5, 10), (5, 4), (5, 14), (5, 5), (10, 1), (10, 8), (10, 9), (10, 15), (10, 10), (6, 1), (6, 9), (6, 13), (6, 17), (6, 6), (8, 9), (8, 16), (8, 8), (14, 7), (14, 19), (14, 14), (16, 18), (16, 4), (16, 7), (16, 17), (16, 16), (17, 7), (17, 17), (18, 13), (18, 18), (1, 13), (1, 1), (4, 4), (9, 9), (15, 19), (15, 15), (13, 13), (7, 7), (19, 19)]</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>{0: [1055, 1058, 1054, 1057, 1060, 1056, 1059, 3785], 1: [1070, 1073, 1069, 1072, 3800, 1075, 1071, 1074], 2: [1086, 1089, 1085, 1088, 1087, 3815, 1090], 3: [1101, 1104, 1100, 1103, 1102, 3830, 1105], 4: [1029, 1028, 1025, 1024, 1027, 1030, 3845, 1026], 5: [1041, 1044, 1043, 1040, 1039, 1042, 1045, 3860], 6: [995, 998, 994, 997, 3875, 1000, 996, 999], 7: [1012, 1011, 1014, 1013, 3890, 1010, 1009, 1015], 8: [4834, 966, 969, 968, 965, 4835, 964, 967, 970], 9: [980, 983, 4850, 979, 982, 985, 4849, 981, 984], 10: [1115, 1118, 3919, 1116, 1120, 1117, 3920, 1119], 11: [939, 935, 3934, 938, 937, 940, 936, 3935], 12: [954, 953, 950, 3950, 952, 955, 951, 3949], 13: [1147, 3965, 1149, 1146, 3964, 1145, 1148], 14: [1161, 1164, 3980, 1160, 1163, 1162, 3979], 15: [3995, 3994, 923, 922, 925, 921, 924], 16: [1176, 4025, 1179, 1175, 4024, 1178, 1177, 4026], 17: [1190, 1193, 4040, 1192, 4039, 1191, 1194, 4041], 18: [1210, 4056, 1209, 4055, 1206, 1208, 4054, 1207], 19: [1224, 4071, 1223, 4070, 1222, 1225, 4069, 1221], 20: [1236, 1239, 4086, 1238, 4085, 1237, 1240, 4084], 21: [1251, 1255, 4100, 1254, 4099, 1253, 1252, 4101], 22: [1267, 1270, 1266, 4115, 1269, 4114, 1268, 4116], 23: [1285, 1282, 4130, 1281, 1284, 4129, 1283, 4131], 24: [880, 4146, 877, 876, 879, 4145, 878, 4144], 25: [4176, 1300, 1297, 4175, 4174, 1299, 1298], 26: [4189, 1315, 1312, 4191, 1314, 4190, 1313], 27: [4206, 847, 850, 846, 849, 4205, 848, 4204, 4207], 28: [4221, 863, 861, 862, 865, 4220, 864, 4219, 4222], 29: [1328, 4235, 4234, 1327, 4237, 1326, 1329, 4236], 30: [4251, 1342, 4250, 1341, 1344, 4249, 4252, 1343], 31: [4263, 4266, 1357, 4265, 1356, 1359, 4264, 1358], 32: [4281, 4278, 1372, 1371, 4280, 1374, 4279, 1373], 33: [4296, 4293, 817, 4295, 819, 4294, 818], 34: [4310, 834, 4309, 4311, 833, 4308, 832], 35: [4327, 4323, 802, 4326, 804, 4325, 803, 4324], 36: [4354, 760, 4357, 4353, 759, 4356, 758, 4355], 37: [4371, 4368, 775, 774, 4370, 773, 4369, 4372], 38: [4383, 4386, 730, 4385, 729, 4384, 728, 4387], 39: [4402, 745, 4399, 4398, 4401, 744, 4400, 743], 40: [699, 4803, 4806, 4805, 698, 700, 4804], 41: [4818, 4821, 715, 4820, 714, 4819, 713], 42: [4417, 4413, 1390, 4416, 1389, 4415, 1388, 4414], 43: [4429, 4432, 4428, 1405, 4431, 4430, 1404, 1403], 44: [4446, 4443, 1420, 1419, 4445, 1418, 4444, 4447], 45: [1433, 4459, 4462, 4458, 1435, 4461, 4460, 1434], 46: [4477, 1448, 4474, 4473, 1450, 4476, 1449, 4475], 47: [4492, 4488, 4491, 1463, 1465, 4490, 1464, 4489], 48: [4503, 670, 669, 4505, 4504, 4507, 668, 4506], 49: [4535, 654, 4534, 4537, 4536, 653, 4533], 50: [4776, 4775, 609, 4777, 4774, 608, 4773], 51: [4788, 624, 4791, 4790, 623, 4792, 4789], 52: [4568, 4565, 4564, 4567, 1480, 4566, 4563, 1479], 53: [4583, 4580, 1495, 4579, 1494, 4582, 4581, 4578], 54: [580, 4745, 4748, 579, 4744, 4747, 4743, 4746], 55: [4759, 595, 4758, 594, 4761, 4760, 4763, 4762], 56: [4713, 1509, 4716, 4715, 4712, 1508, 4717, 4714], 57: [4728, 1523, 4731, 4730, 4727, 1524, 4732, 4729], 58: [4686, 4685, 1538, 4682, 4688, 4684, 4687, 1539, 4683], 59: [4701, 4700, 4697, 4703, 4702, 1554, 4699, 1553, 4698], 60: [549, 4652, 4655, 4654, 4657, 4656, 4653], 61: [4669, 564, 4672, 4671, 4668, 4667, 4670], 62: [4623, 4626, 519, 4622, 4625, 4624, 4627], 63: [4637, 4640, 534, 4639, 4642, 4641, 4638], 64: [4598, 4594, 4597, 4596, 4593, 4592, 4595, 489], 65: [4610, 504, 4613, 4609, 4612, 4611, 4608, 4607]}</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+          <t>[(0, 3), (0, 11), (0, 12), (0, 0), (3, 2), (3, 5), (3, 10), (3, 3), (11, 6), (11, 8), (11, 10), (11, 14), (11, 16), (11, 17), (11, 18), (11, 11), (12, 1), (12, 4), (12, 8), (12, 9), (12, 16), (12, 18), (12, 12), (2, 6), (2, 5), (2, 8), (2, 18), (2, 2), (5, 10), (5, 4), (5, 14), (5, 5), (10, 1), (10, 8), (10, 9), (10, 15), (10, 10), (6, 1), (6, 9), (6, 13), (6, 17), (6, 6), (8, 9), (8, 16), (8, 8), (14, 7), (14, 19), (14, 14), (16, 18), (16, 4), (16, 7), (16, 17), (16, 16), (17, 7), (17, 17), (18, 13), (18, 18), (1, 13), (1, 1), (4, 4), (9, 9), (13, 13), (15, 19), (15, 15), (7, 7), (19, 19)]</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
+        <v>100.32</v>
+      </c>
+      <c r="O4" t="n">
+        <v>27.41</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.5914666652679443</v>
       </c>
       <c r="Q4" t="n">
-        <v>516</v>
+        <v>0.1129571199417114</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="S4" t="n">
-        <v>3267.796339511871</v>
+          <t>{0: [5322, 5321], 3: [5336, 2143], 's_0_3': [2067], 11: [5382, 2338, 2339], 's_0_11': [2323], 12: [5517, 2247, 2248], 's_0_12': [5337], 2: [2189, 2188], 's_2_3': [5471], 5: [5366, 5292, 2232], 's_3_5': [2158], 10: [2234, 2233, 5381], 's_3_10': [5426], 6: [2293, 5411, 5412], 's_6_11': [2368], 8: [5502, 5501], 's_8_11': [2324], 's_10_11': [5652], 14: [2533, 5367, 5368], 's_11_14': [5383], 16: [2369, 5547, 2442, 2443], 's_11_16': [5352], 17: [5397, 2398], 's_11_17': [2473], 18: [5606, 2354, 5607], 's_11_18': [5532], 1: [2278], 's_1_12': [5487], 4: [5217, 5216], 's_4_12': [5201], 's_8_12': [2204], 9: [2308, 2309], 's_9_12': [5351], 's_12_16': [5546], 's_12_18': [5472], 's_2_6': [2173], 's_2_5': [5261], 's_2_8': [2174], 's_2_18': [5591], 's_5_10': [2218], 's_4_5': [2292], 's_5_14': [5293], 's_1_10': [5531], 's_8_10': [2098, 5380], 's_9_10': [5576], 15: [5668, 5667], 's_10_15': [2249], 's_1_6': [5427], 's_6_9': [5396], 13: [5442], 's_6_13': [2413], 's_6_17': [2353], 's_8_9': [2294], 's_8_16': [5503], 7: [5338], 's_7_14': [2412], 19: [2503, 2504], 's_14_19': [5353], 's_16_18': [5592], 's_4_16': [5202], 's_7_16': [2457], 's_16_17': [5308], 's_7_17': [2488], 's_13_18': [2384], 's_1_13': [2263], 's_15_19': [5653]}</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>{0: [3297], 3: [3296], 11: [2251], 12: [2282, 2281], 2: [2221], 5: [2236], 10: [3371, 2192], 6: [3357, 2342], 8: [3386], 14: [3236], 16: [2266, 3252], 17: [3282], 18: [3342], 1: [3312], 4: [3221], 9: [2297], 15: [2177], 13: [2357], 7: [2296], 19: [2176]}</t>
+        </is>
       </c>
       <c r="T4" t="n">
-        <v>122.97</v>
+        <v>93</v>
       </c>
       <c r="U4" t="n">
-        <v>27.61</v>
+        <v>24</v>
       </c>
       <c r="V4" t="n">
-        <v>0.5125343799591064</v>
+        <v>0.628427267074585</v>
       </c>
       <c r="W4" t="n">
-        <v>0.08079135417938232</v>
+        <v>0.12129807472229</v>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>{0: [3435, 212], 3: [136, 137], 's_0_3': [3270], 11: [257, 256, 3301], 's_0_11': [3316], 12: [422, 272, 3436], 's_0_12': [3390], 's_0_0': [211], 2: [3676, 122, 123, 3675], 's_3_2': [3420], 5: [167, 3480], 's_3_5': [3330], 10: [213, 91, 92, 3465], 's_3_10': [3495], 's_3_3': [121], 6: [3496, 379, 378], 's_11_6': [377], 8: [3630, 168, 3555], 's_11_8': [3540], 's_11_10': [3300], 14: [3361, 3360], 's_11_14': [271], 16: [318, 316, 317, 3331], 's_11_16': [3210], 17: [332, 331], 's_11_17': [3346], 18: [348, 3511], 's_11_18': [242], 's_11_11': [3302], 1: [408, 3450, 3451], 's_12_1': [407], 4: [3405], 's_12_4': [3406], 's_12_8': [3556], 9: [3481, 228], 's_12_9': [3482], 's_12_16': [3526], 's_12_18': [3541], 's_12_12': [423], 's_2_6': [364], 's_2_5': [3345], 's_2_8': [108], 's_2_18': [3510], 's_2_2': [49], 's_5_10': [198], 's_5_4': [152], 's_5_14': [3375], 's_5_5': [48], 's_10_1': [183], 's_10_8': [3570], 's_10_9': [3600], 15: [106], 's_10_15': [3255], 's_10_10': [3525], 's_6_1': [3497], 's_6_9': [347], 13: [3616], 's_6_13': [3601], 's_6_17': [3466], 's_6_6': [3691], 's_8_9': [229], 's_8_16': [303], 's_8_8': [3645], 7: [436, 3256], 's_14_7': [286], 19: [3315, 197], 's_14_19': [182], 's_14_14': [451], 's_16_18': [3631], 's_16_4': [227], 's_16_7': [3241], 's_16_17': [3286], 's_16_16': [3225], 's_17_7': [3226], 's_17_17': [3196], 's_18_13': [333], 's_18_18': [3586], 's_1_13': [363], 's_1_1': [3452], 's_4_4': [287], 's_9_9': [3615], 's_15_19': [3285], 's_15_15': [105], 's_13_13': [438], 's_7_7': [301], 's_19_19': [61]}</t>
+          <t>[97, 106, 107, 95, 107, 95, 96, 102, 101, 119, 104, 98, 97, 104, 101, 98, 99, 103, 97, 108, 99, 96, 104, 107, 94, 97, 100, 107, 101, 99, 100, 93, 100, 98, 105, 100, 101, 96, 93, 94, 108, 103, 100, 100, 96, 114, 96, 101, 97, 95, 98, 98, 104, 96, 96, 99, 107, 94, 103, 96, 96, 102, 94, 101, 99, 97, 102, 103, 103, 99, 104, 98, 97, 103, 102, 103, 100, 105, 95, 104, 100, 96, 97, 94, 105, 97, 109, 98, 97, 115, 102, 95, 107, 96, 97, 96, 100, 97, 102, 106]</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>{0: [3417], 3: [2462], 11: [3538, 2432], 12: [2417], 2: [3493], 5: [2477], 10: [3477, 3478], 6: [2388], 8: [2402], 14: [2478], 16: [3523, 2447], 17: [3552], 18: [3508], 1: [3462], 4: [3402], 9: [3567, 2343], 15: [2358], 13: [2373], 7: [2463], 19: [3582]}</t>
+          <t>[27, 27, 26, 27, 28, 28, 27, 26, 27, 28, 29, 30, 27, 27, 27, 27, 28, 29, 30, 28, 28, 27, 33, 29, 26, 26, 27, 27, 27, 30, 26, 28, 24, 27, 27, 29, 25, 28, 26, 30, 27, 27, 28, 29, 26, 27, 26, 27, 25, 27, 28, 26, 27, 29, 29, 30, 29, 27, 27, 27, 28, 26, 25, 26, 28, 30, 27, 28, 28, 26, 28, 26, 27, 28, 28, 27, 25, 27, 25, 28, 26, 31, 25, 31, 29, 27, 26, 25, 29, 26, 27, 27, 28, 26, 26, 26, 30, 26, 28, 30]</t>
         </is>
       </c>
       <c r="Z4" t="n">
-        <v>114</v>
+        <v>4.86977899649948</v>
       </c>
       <c r="AA4" t="n">
-        <v>24</v>
+        <v>1.557614078057083</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.5746102333068848</v>
+        <v>1</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.07222604751586914</v>
+        <v>1</v>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>[{0: [3964, 920], 3: [950], 's_0_3': [3919], 11: [3829, 3830, 3891, 1130], 's_0_11': [3814], 12: [1160, 815, 4009, 4010], 's_0_12': [921], 's_0_0': [3963], 2: [875, 3934], 's_3_2': [3904], 5: [935, 934, 3784], 's_3_5': [3860], 10: [4040, 3950, 3875, 1055], 's_3_10': [951], 's_3_3': [3845], 6: [1281, 4071, 3935, 1145], 's_11_6': [1144], 8: [1040, 3890], 's_11_8': [964], 's_11_10': [3920, 1205], 14: [3740, 3710, 1069], 's_11_14': [3785, 1129], 16: [3979, 3980, 3981], 's_11_16': [1265], 17: [1280], 's_11_17': [3846], 18: [3965, 4099, 995], 's_11_18': [994], 's_11_11': [3828], 1: [4026, 1190], 's_12_1': [4056], 4: [3948, 829, 830], 's_12_4': [814], 's_12_8': [1025], 9: [3995, 1086], 's_12_9': [3994], 's_12_16': [890], 's_12_18': [906], 's_12_12': [4024], 's_2_6': [4070, 980], 's_2_5': [874], 's_2_8': [3889], 's_2_18': [876], 's_2_2': [905], 's_5_10': [3949], 's_5_4': [3799], 's_5_14': [3739], 's_5_5': [844], 's_10_1': [4041], 's_10_8': [979], 's_10_9': [1101], 15: [1054, 3800], 's_10_15': [1009], 's_10_10': [3951], 's_6_1': [3996], 's_6_9': [1116], 13: [4084, 4085], 's_6_13': [1206], 's_6_17': [3936], 's_6_6': [1146], 's_8_9': [1085], 's_8_16': [1100], 's_8_8': [1041], 7: [1219, 3876, 1220], 's_14_7': [3770], 19: [3725], 's_14_19': [1143], 's_14_14': [1039], 's_16_18': [1070], 's_16_4': [860], 's_16_7': [1235], 's_16_17': [3966], 's_16_16': [1310], 's_17_7': [3861], 's_17_17': [3906], 's_18_13': [936], 's_18_18': [4098], 's_1_13': [4100], 's_1_1': [1191], 's_4_4': [695], 's_9_9': [4115], 's_15_19': [1099], 's_15_15': [3695], 's_13_13': [1071], 's_7_7': [1250], 's_19_19': [1188]}, {0: [913, 837, 5269], 3: [836, 702, 5163], 's_0_3': [867], 11: [822, 823, 5537, 5538], 's_0_11': [5329], 12: [643, 5404, 5403], 's_0_12': [958], 's_0_0': [5270], 2: [628, 5283, 627], 's_3_2': [5298], 5: [852, 5284, 5208], 's_3_5': [732], 10: [5253, 5358, 807], 's_3_10': [806], 's_3_3': [791], 6: [779, 5447, 5448], 's_11_6': [704, 5568], 8: [748, 5373], 's_11_8': [793], 's_11_10': [5299], 14: [5239, 882], 's_11_14': [5224], 16: [5464, 5523, 5463, 749], 's_11_16': [5522], 17: [914, 5479], 's_11_17': [5494], 18: [5493, 613], 's_11_18': [689], 's_11_11': [5536], 1: [642, 5357, 538], 's_12_1': [5402], 4: [5419, 853], 's_12_4': [973], 's_12_8': [778], 9: [5313, 703], 's_12_9': [688], 's_12_16': [658], 's_12_18': [5508], 's_12_12': [943, 5300], 's_2_6': [5432], 's_2_5': [5207], 's_2_8': [5372], 's_2_18': [612], 's_2_2': [5282], 's_5_10': [717], 's_5_4': [928], 's_5_14': [5134], 's_5_5': [5285], 's_10_1': [657, 5268], 's_10_8': [733], 's_10_9': [5314], 15: [687], 's_10_15': [672], 's_10_10': [5252], 's_6_1': [673], 's_6_9': [5433], 13: [5387, 493, 5386], 's_6_13': [463], 's_6_17': [5449], 's_6_6': [478], 's_8_9': [718], 's_8_16': [808, 5418], 's_8_8': [838], 7: [5359, 883], 's_14_7': [987], 19: [5148, 5149], 's_14_19': [897], 's_14_14': [912], 's_16_18': [719], 's_16_4': [854], 's_16_7': [898], 's_16_17': [929], 's_16_16': [5524], 's_17_7': [5434], 's_17_17': [5569], 's_18_13': [5417], 's_18_18': [674], 's_1_13': [5327], 's_1_1': [537], 's_4_4': [5420], 's_9_9': [583], 's_15_19': [5133], 's_15_15': [5162], 's_13_13': [403], 's_7_7': [5360], 's_19_19': [762]}, {0: [5182, 1302, 5181], 3: [5138, 1573, 1572], 's_0_3': [5137], 11: [5452, 5451, 1228, 1227, 5226], 's_0_11': [1287], 12: [1258, 5286, 1257], 's_0_12': [5166], 's_0_0': [5107], 2: [5288, 1392, 5287], 's_3_2': [1587], 5: [5318, 1484, 1483], 's_3_5': [1482], 10: [5317, 1423, 1558, 5392], 's_3_10': [5468], 's_3_3': [5139], 6: [1438, 5333, 1362, 5332], 's_11_6': [5227], 8: [1393, 5360, 5361], 's_11_8': [1197, 5345], 's_11_10': [1332], 14: [1454, 5542], 's_11_14': [1528], 16: [5526, 5316, 1274, 1273], 's_11_16': [1289], 17: [1363], 's_11_17': [5437], 18: [5257, 5256], 's_11_18': [1212], 's_11_11': [1272], 1: [5376, 5378, 5377], 's_12_1': [1243], 4: [5422, 5421], 's_12_4': [1288], 's_12_8': [1167], 9: [1303, 5406], 's_12_9': [5271], 's_12_16': [5481], 's_12_18': [1242], 's_12_12': [5301], 's_2_6': [5242], 's_2_5': [1542], 's_2_8': [1347], 's_2_18': [1407], 's_2_2': [5289], 's_5_10': [5498], 's_5_4': [5513, 1513], 's_5_14': [5587], 's_5_5': [5572], 's_10_1': [5393], 's_10_8': [1377], 's_10_9': [1422, 5302], 15: [5453], 's_10_15': [5438], 's_10_10': [1557], 's_6_1': [1618], 's_6_9': [5346], 13: [5272, 1498], 's_6_13': [5362], 's_6_17': [5482], 's_6_6': [5334], 's_8_9': [1318], 's_8_16': [1123], 's_8_8': [1108], 7: [5467, 1378], 's_14_7': [5497], 19: [5528, 1693, 5543], 's_14_19': [5527], 's_14_14': [5602], 's_16_18': [1182], 's_16_4': [1333], 's_16_7': [5541], 's_16_17': [5391], 's_16_16': [5586], 's_17_7': [5407], 's_17_17': [5512], 's_18_13': [1437], 's_18_18': [5255], 's_1_13': [1453], 's_1_1': [1753], 's_4_4': [1198], 's_9_9': [5405], 's_15_19': [1634], 's_15_15': [5454], 's_13_13': [1499], 's_7_7': [1319], 's_19_19': [5408]}, {0: [5115], 3: [5175, 207, 5070], 's_0_3': [192], 11: [4996, 4995, 160, 161], 's_0_11': [176], 12: [4741, 4740, 42, 41, 40], 's_0_12': [57], 's_0_0': [86], 2: [5101, 295, 5056, 296], 's_3_2': [5160], 5: [5055, 130, 131], 's_3_5': [146], 10: [101, 4906, 4905, 100], 's_3_10': [5100], 's_3_3': [5190], 6: [235, 356, 236, 4951], 's_11_6': [5040], 8: [4936, 114, 115, 4935], 's_11_8': [4950], 's_11_10': [4890], 14: [370, 4875, 4876], 's_11_14': [265], 16: [159, 4711, 205, 4710], 's_11_16': [206], 17: [4815], 's_11_17': [175], 18: [4726, 386, 385], 's_11_18': [371], 's_11_11': [460], 1: [339, 341, 340], 's_12_1': [354], 4: [4785], 's_12_4': [69], 's_12_8': [144, 4695], 9: [4966, 4965], 's_12_9': [56], 's_12_16': [174], 's_12_18': [324], 's_12_12': [39], 's_2_6': [5086], 's_2_5': [251], 's_2_8': [294, 4681, 4680], 's_2_18': [4891], 's_2_2': [297], 's_5_10': [191], 's_5_4': [4770], 's_5_14': [145], 's_5_5': [129], 's_10_1': [4920, 4921], 's_10_8': [250], 's_10_9': [280], 15: [445], 's_10_15': [430], 's_10_10': [355], 's_6_1': [5116], 's_6_9': [311], 13: [401, 4981], 's_6_13': [4980], 's_6_17': [220], 's_6_6': [357], 's_8_9': [221], 's_8_16': [4725], 's_8_8': [85], 7: [4845, 325], 's_14_7': [4771], 19: [4846], 's_14_19': [415], 's_14_14': [4877], 's_16_18': [429], 's_16_4': [99], 's_16_7': [4830], 's_16_17': [279], 's_16_16': [4712], 's_17_7': [310], 's_17_17': [264], 's_18_13': [5011], 's_18_18': [4727], 's_1_13': [5026], 's_1_1': [4651], 's_4_4': [84], 's_9_9': [70], 's_15_19': [4831], 's_15_15': [444], 's_13_13': [402], 's_7_7': [326], 's_19_19': [490]}, {0: [2316, 4062], 3: [4197, 2286], 's_0_3': [4077], 11: [2225, 2227, 2226], 's_0_11': [2240], 12: [4151, 2271, 4152], 's_0_12': [2270], 's_0_0': [2255], 2: [2151, 4136], 's_3_2': [4196], 5: [4181, 4182, 2406, 2407], 's_3_5': [2421], 10: [4317, 2287, 4316], 's_3_10': [2392], 's_3_3': [4198], 6: [2257, 4227, 2256], 's_11_6': [4451], 8: [2181, 2182, 4301], 's_11_8': [4331], 's_11_10': [2242], 14: [4378, 4376, 4377], 's_11_14': [4361], 16: [4270, 4271, 4272, 2482], 's_11_16': [4286], 17: [4407, 4408], 's_11_17': [4392], 18: [4257, 2196, 2197], 's_11_18': [4032], 's_11_11': [3986], 1: [2348, 2346, 2347], 's_12_1': [2361], 4: [2091, 4120], 's_12_4': [2121], 's_12_8': [4166], 9: [2272, 4347], 's_12_9': [2301, 2302], 's_12_16': [2076], 's_12_18': [2211], 's_12_12': [4153], 's_2_6': [4226], 's_2_5': [4137, 4122], 's_2_8': [4061], 's_2_18': [4106], 's_2_2': [4211], 's_5_10': [2167], 's_5_4': [2106], 's_5_14': [2422], 's_5_5': [4228], 's_10_1': [4302], 's_10_8': [2152], 's_10_9': [2377], 15: [2452], 's_10_15': [2437], 's_10_10': [2288], 's_6_1': [4362], 's_6_9': [4466], 13: [2362], 's_6_13': [4332], 's_6_17': [2198, 4437], 's_6_6': [2241], 's_8_9': [4346], 's_8_16': [2137], 's_8_8': [4300], 7: [2512, 4348], 's_14_7': [2587], 19: [2393, 4452], 's_14_19': [2378], 's_14_14': [2558], 's_16_18': [2212], 's_16_4': [2061], 's_16_7': [4258], 's_16_17': [4393], 's_16_16': [2002], 's_17_7': [2467], 's_17_17': [4409], 's_18_13': [4212], 's_18_18': [4047], 's_1_13': [2363], 's_1_1': [4497], 's_4_4': [2092], 's_9_9': [2273], 's_15_19': [4467], 's_15_15': [4423], 's_13_13': [4287], 's_7_7': [2557], 's_19_19': [2483]}, {0: [3247, 3246], 3: [1336, 3352], 's_0_3': [1366], 11: [3128, 1290, 1291, 3127], 's_0_11': [3261], 12: [1486, 3397, 1487], 's_0_12': [3262], 's_0_0': [1186], 2: [3308, 3307], 's_3_2': [1292], 5: [1516, 1351, 3277], 's_3_5': [3366], 10: [3142, 3337, 1456, 1457], 's_3_10': [1321], 's_3_3': [1337], 6: [3216, 1382, 1381, 1380], 's_11_6': [2992], 8: [1411, 3172, 1412], 's_11_8': [1306], 's_11_10': [1320], 14: [1350, 3068, 3067], 's_11_14': [3051], 16: [1546, 3037, 1545, 3187], 's_11_16': [3036], 17: [3021, 1455, 3022], 's_11_17': [2977], 18: [1621, 1606, 3158], 's_11_18': [1530], 's_11_11': [3126], 1: [3097], 's_12_1': [1471], 4: [3353], 's_12_4': [1562], 's_12_8': [3173], 9: [3442], 's_12_9': [1517], 's_12_16': [3217], 's_12_18': [3323], 's_12_12': [3398], 's_2_6': [1396], 's_2_5': [1442], 's_2_8': [1426], 's_2_18': [1591], 's_2_2': [1307], 's_5_10': [3322], 's_5_4': [1501], 's_5_14': [1515], 's_5_5': [3276], 's_10_1': [1441], 's_10_8': [3382], 's_10_9': [1427], 15: [3053, 1425, 3052], 's_10_15': [1410], 's_10_10': [3336], 's_6_1': [1395], 's_6_9': [1397], 13: [3113, 3111, 3112], 's_6_13': [1276], 's_6_17': [3006], 's_6_6': [1231], 's_8_9': [3427], 's_8_16': [3367], 's_8_8': [3457], 7: [1470], 's_14_7': [3082], 19: [1665], 's_14_19': [1650], 's_14_14': [3066], 's_16_18': [3263], 's_16_4': [1531], 's_16_7': [1485], 's_16_17': [1560], 's_16_16': [3202], 's_17_7': [2932], 's_17_17': [1230], 's_18_13': [1605], 's_18_18': [3233], 's_1_13': [1500], 's_1_1': [3098], 's_4_4': [1607], 's_9_9': [1502], 's_15_19': [3038], 's_15_15': [3054], 's_13_13': [1170], 's_7_7': [2978], 's_19_19': [2918]}, {0: [740, 3918], 3: [665, 710, 4023], 's_0_3': [3963], 11: [3903, 4159, 861, 860], 's_0_11': [799], 12: [515, 3948, 785, 3947], 's_0_12': [3917], 's_0_0': [770, 769], 2: [4038, 4039], 's_3_2': [726], 5: [681, 576, 4053], 's_3_5': [591], 10: [741, 846, 4113], 's_3_10': [711], 's_3_3': [3873], 6: [4009, 890], 's_11_6': [3904], 8: [829, 4054, 830], 's_11_8': [3784, 859], 's_11_10': [4204], 14: [4218, 4220, 4219], 's_11_14': [876], 16: [4099, 4098, 620, 4097], 's_11_16': [906], 17: [4025, 936], 's_11_17': [951], 18: [800, 3977, 3978, 755], 's_11_18': [3889], 's_11_11': [814], 1: [3994, 845], 's_12_1': [3933], 4: [3992], 's_12_4': [530], 's_12_8': [3753, 784], 9: [816, 815], 's_12_9': [4069], 's_12_16': [3932], 's_12_18': [575], 's_12_12': [3872], 's_2_6': [875], 's_2_5': [605], 's_2_8': [756], 's_2_18': [680], 's_2_2': [695], 's_5_10': [696, 4158], 's_5_4': [561, 4127], 's_5_14': [4203, 636], 's_5_5': [682], 's_10_1': [3993], 's_10_8': [771], 's_10_9': [4083], 15: [4189], 's_10_15': [4174], 's_10_10': [742], 's_6_1': [965], 's_6_9': [4024], 13: [3874, 920], 's_6_13': [3919], 's_6_17': [980], 's_6_6': [889], 's_8_9': [3964], 's_8_16': [891], 's_8_8': [3799], 7: [4129, 1026], 's_14_7': [1056, 4070], 19: [937], 's_14_19': [4205], 's_14_14': [772], 's_16_18': [3962], 's_16_4': [4007], 's_16_7': [1041], 's_16_17': [1010], 's_16_16': [621], 's_17_7': [4084], 's_17_17': [1086], 's_18_13': [3859], 's_18_18': [485], 's_1_13': [3979], 's_1_1': [921], 's_4_4': [3991, 396], 's_9_9': [4278], 's_15_19': [952], 's_15_15': [4188], 's_13_13': [3814], 's_7_7': [1025], 's_19_19': [938]}, {0: [625, 4953], 3: [5117, 686, 5118], 's_0_3': [701], 11: [386, 4892, 4891], 's_0_11': [610], 12: [4981, 521, 640, 4982], 's_0_12': [655], 's_0_0': [746], 2: [4846, 445, 446], 's_3_2': [431], 5: [5042, 506, 505], 's_3_5': [5043], 10: [582, 580, 581], 's_3_10': [4968], 's_3_3': [732], 6: [4862, 4861, 296, 295], 's_11_6': [355], 8: [4996, 460, 4877], 's_11_8': [371], 's_11_10': [596], 14: [325, 4816, 4815], 's_11_14': [340, 4801], 16: [4952, 4951], 's_11_16': [280], 17: [221, 4921], 's_11_17': [4890], 18: [4922, 416], 's_11_18': [5011], 's_11_11': [387], 1: [5087, 5086], 's_12_1': [5072], 4: [536], 's_12_4': [5012], 's_12_8': [4997], 9: [535, 670, 4832], 's_12_9': [4847], 's_12_16': [356], 's_12_18': [520], 's_12_12': [4863], 's_2_6': [400], 's_2_5': [5041], 's_2_8': [4937], 's_2_18': [4906], 's_2_2': [5161], 's_5_10': [5057], 's_5_4': [5102], 's_5_14': [490], 's_5_5': [611], 's_10_1': [597], 's_10_8': [4907], 's_10_9': [4817], 15: [4712, 4711], 's_10_15': [4727], 's_10_10': [4743], 's_6_1': [281], 's_6_9': [595], 13: [552, 550, 551], 's_6_13': [565], 's_6_17': [5010], 's_6_6': [5146], 's_8_9': [4772, 459], 's_8_16': [491], 's_8_8': [4995], 7: [250, 249], 's_14_7': [4845], 19: [429], 's_14_19': [444], 's_14_14': [190], 's_16_18': [475], 's_16_4': [4967], 's_16_7': [4966], 's_16_17': [265], 's_16_16': [4950], 's_17_7': [4980], 's_17_17': [5055], 's_18_13': [566], 's_18_18': [430], 's_1_13': [567], 's_1_1': [5085], 's_4_4': [537], 's_9_9': [4773], 's_15_19': [4726], 's_15_15': [354], 's_13_13': [5177], 's_7_7': [248], 's_19_19': [428]}, {0: [541], 3: [3213, 3212], 's_0_3': [3227], 11: [3257, 601, 3349, 3347, 3348], 's_0_11': [542], 12: [3152, 3196, 3077, 465], 's_0_12': [540], 's_0_0': [3197], 2: [645, 766, 767, 3093], 's_3_2': [646], 5: [676, 3243], 's_3_5': [796], 10: [3242, 3124, 3123, 586], 's_3_10': [721, 3228], 's_3_3': [856], 6: [3423, 3422, 466, 467], 's_11_6': [662], 8: [3182, 556], 's_11_8': [557], 's_11_10': [587], 14: [781, 3319], 's_11_14': [3334], 16: [497, 3181, 496], 's_11_16': [482], 17: [3467, 512], 's_11_17': [527], 18: [436, 3138, 3137, 435], 's_11_18': [421, 3256], 's_11_11': [737], 1: [450, 451], 's_12_1': [3031], 4: [481, 3318, 3317], 's_12_4': [511], 's_12_8': [3092, 600], 9: [617, 615, 616], 's_12_9': [3062], 's_12_16': [376], 's_12_18': [3076], 's_12_12': [585], 's_2_6': [3438], 's_2_5': [3168], 's_2_8': [3183], 's_2_18': [705], 's_2_2': [3393], 's_5_10': [736], 's_5_4': [631], 's_5_14': [3273], 's_5_5': [3288], 's_10_1': [3122], 's_10_8': [630], 's_10_9': [3153], 15: [780, 3154], 's_10_15': [810], 's_10_10': [840], 's_6_1': [3211], 's_6_9': [602], 13: [526, 3302], 's_6_13': [3272], 's_6_17': [3437], 's_6_6': [632], 's_8_9': [3107], 's_8_16': [3167], 's_8_8': [555], 7: [3363, 3361, 3362], 's_14_7': [3378], 19: [886], 's_14_19': [871], 's_14_14': [782], 's_16_18': [391], 's_16_4': [346, 3316], 's_16_7': [3376], 's_16_17': [3482], 's_16_16': [3497, 3496], 's_17_7': [3377], 's_17_17': [3407], 's_18_13': [525], 's_18_18': [3136], 's_1_13': [3287], 's_1_1': [452], 's_4_4': [572], 's_9_9': [3542], 's_15_19': [3169], 's_15_15': [795], 's_13_13': [3301], 's_7_7': [3364], 's_19_19': [3229]}, {0: [1770, 3324, 1771], 3: [1817, 3294, 1876], 's_0_3': [1756], 11: [3129, 1651, 3131, 3130], 's_0_11': [1652], 12: [1860, 3190, 3189], 's_0_12': [1786], 's_0_0': [1681], 2: [3399, 3400], 's_3_2': [1802], 5: [3369, 3354, 1787], 's_3_5': [1726], 10: [1636, 3233, 1861, 3234], 's_3_10': [3264], 's_3_3': [3295], 6: [1831, 3311, 3099, 3310, 1832], 's_11_6': [1875], 8: [2012, 2011, 3115, 3114, 1816], 's_11_8': [3146], 's_11_10': [3248], 14: [3069, 1711, 1710], 's_11_14': [3188], 16: [3084, 1935, 1905, 3085], 's_11_16': [1965], 17: [2994, 1785], 's_11_17': [1650], 18: [3086, 2117, 2115, 2116], 's_11_18': [2981, 2145], 's_11_11': [3132], 1: [3250, 1921], 's_12_1': [1981], 4: [3070, 1891, 1890], 's_12_4': [2055], 's_12_8': [2026], 9: [1845, 1846], 's_12_9': [3039], 's_12_16': [3160], 's_12_18': [2101], 's_12_12': [3191], 's_2_6': [1997], 's_2_5': [3414], 's_2_8': [2027], 's_2_18': [3415], 's_2_2': [1892, 3535], 's_5_10': [1696], 's_5_4': [3355], 's_5_14': [3368], 's_5_5': [3474, 1862], 's_10_1': [1936], 's_10_8': [3235], 's_10_9': [3325, 1847], 15: [1591, 1590], 's_10_15': [3098], 's_10_10': [1606], 's_6_1': [2056], 's_6_9': [3249], 13: [3266, 1966, 3265], 's_6_13': [2071], 's_6_17': [1740], 's_6_6': [1906], 's_8_9': [3219], 's_8_16': [3100], 's_8_8': [3280], 7: [1815], 's_14_7': [1800], 19: [3038], 's_14_19': [1725], 's_14_14': [3279], 's_16_18': [2010, 3010], 's_16_4': [3175], 's_16_7': [3054], 's_16_17': [2995], 's_16_16': [2980], 's_17_7': [3024], 's_17_17': [3009], 's_18_13': [3251], 's_18_18': [3101], 's_1_13': [1996], 's_1_1': [3204], 's_4_4': [3071], 's_9_9': [2950], 's_15_19': [3053], 's_15_15': [1592], 's_13_13': [2176], 's_7_7': [2919], 's_19_19': [1635]}, {0: [3704, 2582, 2583], 3: [3643], 's_0_3': [2554], 11: [2673, 3854, 2674], 's_0_11': [2584], 12: [3418, 2658, 2657], 's_0_12': [3494], 's_0_0': [3478], 2: [3538, 2493], 's_3_2': [2463], 5: [3463, 2524, 2523], 's_3_5': [2539], 10: [3614, 2598, 3613], 's_3_10': [3658], 's_3_3': [3642], 6: [2703, 3583, 3584], 's_11_6': [3554], 8: [2644, 3568, 2643], 's_11_8': [3824], 's_11_10': [2599], 14: [2494, 3763, 3764], 's_11_14': [2614], 16: [2748, 3659, 2749], 's_11_16': [3809], 17: [2793, 3779, 2794], 's_11_17': [2689], 18: [2628, 3688, 3689], 's_11_18': [2629], 's_11_11': [2555], 1: [2718, 3539], 's_12_1': [3524], 4: [2627, 3464], 's_12_4': [3403], 's_12_8': [2642], 9: [2613, 2612], 's_12_9': [3449], 's_12_16': [3434, 2747], 's_12_18': [3598], 's_12_12': [3388], 's_2_6': [2538], 's_2_5': [2432], 's_2_8': [2508], 's_2_18': [2478], 's_2_2': [2402], 's_5_10': [3748], 's_5_4': [3553], 's_5_14': [3793], 's_5_5': [3778], 's_10_1': [2568], 's_10_8': [2597], 's_10_9': [3719], 15: [2448, 3597], 's_10_15': [2433], 's_10_10': [3612], 's_6_1': [2553], 's_6_9': [3479], 13: [2688], 's_6_13': [3569], 's_6_17': [2808], 's_6_6': [2823], 's_8_9': [3629], 's_8_16': [3644], 's_8_8': [3567], 7: [3749, 2824], 's_14_7': [2839], 19: [2418, 3703], 's_14_19': [3718], 's_14_14': [3762], 's_16_18': [2719], 's_16_4': [2733], 's_16_7': [2778], 's_16_17': [2704], 's_16_16': [3794], 's_17_7': [3734], 's_17_17': [3914], 's_18_13': [3674], 's_18_18': [2389], 's_1_13': [3599], 's_1_1': [2717], 's_4_4': [2626], 's_9_9': [2611], 's_15_19': [3582], 's_15_15': [2358], 's_13_13': [2687], 's_7_7': [2734], 's_19_19': [3747]}, {0: [2597, 2596], 3: [3493, 3494], 's_0_3': [2553, 3478], 11: [3298, 2702, 3299], 's_0_11': [2581], 12: [2719, 3509, 3569, 2718], 's_0_12': [3539], 's_0_0': [2598], 2: [3463, 3464, 2523], 's_3_2': [2492], 5: [3524, 3403, 2627], 's_3_5': [2507], 10: [3644, 3418, 2613, 2611, 2612], 's_3_10': [2582], 's_3_3': [2462], 6: [2643, 2641, 2642], 's_11_6': [3314], 8: [2747, 2748, 2749], 's_11_8': [3374], 's_11_10': [2522], 14: [2821, 3209, 3404, 2822], 's_11_14': [2732], 16: [2716, 3554, 3419, 2717, 2792], 's_11_16': [3329], 17: [3164, 2701], 's_11_17': [2671], 18: [2538, 3628, 2703, 3629], 's_11_18': [2537], 's_11_11': [2446], 1: [2508, 3568], 's_12_1': [2568], 4: [3599, 2673], 's_12_4': [3584], 's_12_8': [3809], 9: [2762, 2567, 3434, 3433], 's_12_9': [2777], 's_12_16': [2823], 's_12_18': [3508], 's_12_12': [3719], 's_2_6': [2657], 's_2_5': [3523], 's_2_8': [3794, 2524, 3793], 's_2_18': [3538], 's_2_2': [3462], 's_5_10': [2552], 's_5_4': [2688], 's_5_14': [3479, 2687], 's_5_5': [3402], 's_10_1': [3748, 2509], 's_10_8': [3659], 's_10_9': [3344], 15: [2610, 3089], 's_10_15': [2626, 2625], 's_10_10': [3238], 's_6_1': [3583], 's_6_9': [3359], 13: [2658], 's_6_13': [3689], 's_6_17': [3269], 's_6_6': [2644], 's_8_9': [3449], 's_8_16': [3284], 's_8_8': [2750], 7: [3224, 2806], 's_14_7': [2731], 19: [2775], 's_14_19': [3194], 's_14_14': [2820], 's_16_18': [3553], 's_16_4': [2733], 's_16_7': [2791], 's_16_17': [3104], 's_16_16': [3134], 's_17_7': [3239], 's_17_17': [2580], 's_18_13': [3614], 's_18_18': [2539], 's_1_13': [3598], 's_1_1': [3643], 's_4_4': [2778], 's_9_9': [3388], 's_15_19': [2760], 's_15_15': [2715], 's_13_13': [2659], 's_7_7': [3223], 's_19_19': [3059]}, {0: [4539], 3: [4405, 1853, 1854], 's_0_3': [4554], 11: [4464, 1748, 1732, 4463], 's_0_11': [1733], 12: [1717, 1718, 4599], 's_0_12': [1824], 's_0_0': [1868], 2: [4420, 1898, 1897], 's_3_2': [4600], 5: [4525, 4523, 4524], 's_3_5': [4509], 10: [1837, 4449, 1838], 's_3_10': [1839], 's_3_3': [4689], 6: [1943, 1942, 4299], 's_11_6': [1867], 8: [1794, 1793, 4419], 's_11_8': [4434], 's_11_10': [4374], 14: [1643, 1642], 's_11_14': [4448], 16: [4358, 1674, 1673], 's_11_16': [4478], 17: [4390, 4388, 4389], 's_11_17': [1747], 18: [4314, 1702, 4313], 's_11_18': [1687], 's_11_11': [1731], 1: [4344, 1777], 's_12_1': [4404], 4: [1659, 4508, 1658], 's_12_4': [4614], 's_12_8': [1779], 9: [4494, 4493], 's_12_9': [1688], 's_12_16': [4359], 's_12_18': [4298], 's_12_12': [1764], 's_2_6': [4375], 's_2_5': [4510], 's_2_8': [4629], 's_2_18': [1912], 's_2_2': [4421], 's_5_10': [1778], 's_5_4': [1598], 's_5_14': [1628], 's_5_5': [2063], 's_10_1': [4269], 's_10_8': [1823], 's_10_9': [1928], 15: [4193, 4194], 's_10_15': [1852], 's_10_10': [4179], 's_6_1': [4345], 's_6_9': [4479], 13: [1807, 4239], 's_6_13': [4240], 's_6_17': [1927], 's_6_6': [4300], 's_8_9': [1763], 's_8_16': [4584], 's_8_8': [4749], 7: [1552, 4343], 's_14_7': [4403], 19: [1627], 's_14_19': [4208], 's_14_14': [4283], 's_16_18': [4373], 's_16_4': [4643], 's_16_7': [1672], 's_16_17': [1537], 's_16_16': [4658], 's_17_7': [1567], 's_17_17': [1957], 's_18_13': [1657], 's_18_18': [1701], 's_1_13': [1792], 's_1_1': [1762], 's_4_4': [4507], 's_9_9': [1883], 's_15_19': [4178], 's_15_15': [4192], 's_13_13': [1716], 's_7_7': [4462], 's_19_19': [4238]}, {0: [3751, 3750], 3: [3781, 334], 's_0_3': [394], 11: [319, 411, 4006, 320], 's_0_11': [304], 12: [155, 3915, 274, 3826], 's_0_12': [154], 's_0_0': [199], 2: [3856, 365], 's_3_2': [364], 5: [3812, 3811], 's_3_5': [439], 10: [288, 289, 290, 4080], 's_3_10': [3706], 's_3_3': [409], 6: [380, 381, 4066], 's_11_6': [4067], 8: [245, 3841, 244], 's_11_8': [3900], 's_11_10': [3930], 14: [498, 499, 4037, 500], 's_11_14': [4007], 16: [336, 3886, 335], 's_11_16': [4141], 17: [4081], 's_11_17': [425], 18: [3961, 305], 's_11_18': [440], 's_11_11': [318], 1: [231, 4005], 's_12_1': [170], 4: [454, 3916], 's_12_4': [3827], 's_12_8': [3825], 9: [156, 216, 4095], 's_12_9': [201, 4020], 's_12_16': [259], 's_12_18': [3945], 's_12_12': [200], 's_2_6': [3931], 's_2_5': [349], 's_2_8': [3871], 's_2_18': [3976], 's_2_2': [3946], 's_5_10': [3796, 424], 's_5_4': [395], 's_5_14': [484], 's_5_5': [575], 's_10_1': [186], 's_10_8': [3765], 's_10_9': [171], 15: [3601], 's_10_15': [273], 's_10_10': [3631], 's_6_1': [4051], 's_6_9': [306], 13: [4021], 's_6_13': [275], 's_6_17': [366], 's_6_6': [382, 4186], 's_8_9': [3990], 's_8_16': [215], 's_8_8': [243], 7: [396, 4156], 's_14_7': [4022], 19: [3586, 348], 's_14_19': [3571], 's_14_14': [3512], 's_16_18': [3991], 's_16_4': [3887], 's_16_7': [4111], 's_16_17': [4096], 's_16_16': [4216], 's_17_7': [351], 's_17_17': [455], 's_18_13': [350], 's_18_18': [3962], 's_1_13': [4036], 's_1_1': [4140], 's_4_4': [3857], 's_9_9': [4110], 's_15_19': [3616], 's_15_15': [303], 's_13_13': [260], 's_7_7': [276], 's_19_19': [363]}, {0: [5508, 5448, 734], 3: [5480, 779, 5479], 's_0_3': [5509], 11: [688, 689, 5387, 5388], 's_0_11': [733], 12: [5492, 884, 5493, 5494], 's_0_12': [749], 's_0_0': [5449], 2: [5599, 5598], 's_3_2': [914], 5: [958, 959, 5554], 's_3_5': [944], 10: [5567, 5569, 869, 5568], 's_3_10': [764], 's_3_3': [1048], 6: [5628, 704, 703], 's_11_6': [5313], 8: [5583, 569, 5582], 's_11_8': [568], 's_11_10': [868], 14: [5269, 748, 5268], 's_11_14': [778], 16: [5537, 5539, 5538], 's_11_16': [5522], 17: [673, 628, 5463], 's_11_17': [5328], 18: [5689, 823, 824], 's_11_18': [5373], 's_11_11': [553, 5402], 1: [809, 808], 's_12_1': [5659], 4: [5524], 's_12_4': [929], 's_12_8': [524], 9: [613, 614, 5643], 's_12_9': [719], 's_12_16': [643], 's_12_18': [5614], 's_12_12': [463], 's_2_6': [644], 's_2_5': [974], 's_2_8': [5597], 's_2_18': [5584], 's_2_2': [989], 's_5_10': [1004], 's_5_4': [1049], 's_5_14': [5254], 's_5_5': [5389], 's_10_1': [5523], 's_10_8': [629], 's_10_9': [659], 15: [538, 539], 's_10_15': [5552], 's_10_10': [5570], 's_6_1': [5553], 's_6_9': [5478], 13: [794], 's_6_13': [5613], 's_6_17': [718], 's_6_6': [5358], 's_8_9': [5447], 's_8_16': [554], 's_8_8': [5477], 7: [793, 5418], 's_14_7': [763], 19: [5357, 642], 's_14_19': [5283], 's_14_14': [987], 's_16_18': [838], 's_16_4': [1018], 's_16_7': [658], 's_16_17': [674], 's_16_16': [5536], 's_17_7': [5403], 's_17_17': [627], 's_18_13': [5644], 's_18_18': [5404], 's_1_13': [5718], 's_1_1': [807], 's_4_4': [5525], 's_9_9': [5673], 's_15_19': [523], 's_15_15': [5507], 's_13_13': [5674], 's_7_7': [5419], 's_19_19': [5192]}, {0: [4373, 4312, 1537], 3: [4388, 1552], 's_0_3': [4297], 11: [4597, 1462, 1463, 4657, 1464], 's_0_11': [1447], 12: [1614, 4628, 1674, 1673], 's_0_12': [4358, 1582], 's_0_0': [1432], 2: [4462, 4672, 1584, 1583], 's_3_2': [4447], 5: [4417, 4418], 's_3_5': [1628], 10: [4372, 4342, 1523, 1522], 's_3_10': [1507], 's_3_3': [4328], 6: [1419, 1343, 4612], 's_11_6': [4567], 8: [4598, 1629], 's_11_8': [1494], 's_11_10': [4492], 14: [1315, 1313, 1314], 's_11_14': [4402], 16: [1598, 4763, 1524, 1599], 's_11_16': [1509], 17: [1359, 4702], 's_11_17': [1479], 18: [1554, 4718, 4717], 's_11_18': [1539], 's_11_11': [4432], 1: [4626, 1553, 4627], 's_12_1': [4508], 4: [4523, 1613], 's_12_4': [1688], 's_12_8': [4599], 9: [4553, 4476, 1538, 4477], 's_12_9': [1703], 's_12_16': [4478], 's_12_18': [4703], 's_12_12': [1615], 's_2_6': [1434], 's_2_5': [1568], 's_2_8': [4673], 's_2_18': [4748], 's_2_2': [4433], 's_5_10': [1372], 's_5_4': [1643], 's_5_14': [1298], 's_5_5': [1327], 's_10_1': [4583], 's_10_8': [1508], 's_10_9': [4642], 15: [4507, 1403], 's_10_15': [4537], 's_10_10': [4403], 's_6_1': [1373], 's_6_9': [4491], 13: [1404], 's_6_13': [4747], 's_6_17': [1449], 's_6_6': [1342], 's_8_9': [4613], 's_8_16': [4658], 's_8_8': [4643, 4644], 7: [4807, 4806], 's_14_7': [1300], 19: [4582], 's_14_19': [1299], 's_14_14': [4686], 's_16_18': [1645], 's_16_4': [4463], 's_16_7': [4822], 's_16_17': [4762], 's_16_16': [1525], 's_17_7': [1374], 's_17_17': [4792], 's_18_13': [4732], 's_18_18': [4716], 's_1_13': [4641], 's_1_1': [1269], 's_4_4': [4493], 's_9_9': [1268], 's_15_19': [1418], 's_15_15': [4461], 's_13_13': [4656], 's_7_7': [1285], 's_19_19': [4581]}, {0: [4798], 3: [4978, 2545, 2546], 's_0_3': [2530], 11: [2306, 2305, 4872, 4769, 4768, 2380], 's_0_11': [2439], 12: [4662, 4797, 2319, 2320], 's_0_12': [2454], 's_0_0': [2424], 2: [4977, 2350, 2351], 's_3_2': [5022, 5023], 5: [2289, 2290, 2291, 5053, 5052], 's_3_5': [2531], 10: [2501, 2410, 4963], 's_3_10': [5008], 's_3_3': [4993], 6: [4811, 2274, 4813, 4812], 's_11_6': [2604], 8: [4841, 4842], 's_11_8': [4856], 's_11_10': [4962], 14: [5172, 2381, 2382], 's_11_14': [5082], 16: [4859, 4858, 2395, 4857], 's_11_16': [2710], 17: [2650, 4827, 4828], 's_11_17': [2589], 18: [2275, 4888, 4887], 's_11_18': [5006], 's_11_11': [5036], 1: [4783, 2409], 's_12_1': [4692], 4: [4722], 's_12_4': [2259], 's_12_8': [2200], 9: [2365, 4917, 2366], 's_12_9': [2364], 's_12_16': [2394], 's_12_18': [4932], 's_12_12': [4617], 's_2_6': [4752], 's_2_5': [2321], 's_2_8': [2260], 's_2_18': [4947], 's_2_2': [5007], 's_5_10': [2411], 's_5_4': [2304], 's_5_14': [2441], 's_5_5': [5054], 's_10_1': [2500], 's_10_8': [2455], 's_10_9': [4902], 15: [2517, 2502], 's_10_15': [2516], 's_10_10': [5038], 's_6_1': [4707], 's_6_9': [4782], 13: [2484, 2485], 's_6_13': [2515, 4903], 's_6_17': [4826], 's_6_6': [4676], 's_8_9': [2335], 's_8_16': [4843], 's_8_8': [2230], 7: [2440, 4948, 4949], 's_14_7': [4933], 19: [5143], 's_14_19': [2397], 's_14_14': [5247], 's_16_18': [2590], 's_16_4': [4737], 's_16_7': [2680], 's_16_17': [2470], 's_16_16': [2755], 's_17_7': [2665], 's_17_17': [2634], 's_18_13': [4873], 's_18_18': [4889], 's_1_13': [4753], 's_1_1': [4784], 's_4_4': [4723], 's_9_9': [4918], 's_15_19': [5158], 's_15_15': [5218], 's_13_13': [4693], 's_7_7': [2561], 's_19_19': [2487]}, {0: [1636, 3248], 3: [1651, 3113], 's_0_3': [3233], 11: [1816, 3128, 3264, 3129], 's_0_11': [3249], 12: [3202, 3203, 1710, 3084], 's_0_12': [1591], 's_0_0': [1546], 2: [1605, 3278, 1606], 's_3_2': [1652], 5: [3098, 1860, 3099], 's_3_5': [1545], 10: [3187, 3189, 3188], 's_3_10': [1530], 's_3_3': [3218], 6: [1470, 3262, 3143, 1471], 's_11_6': [1500], 8: [1741, 3309, 3308], 's_11_8': [1817], 's_11_10': [1801], 14: [3130], 's_11_14': [1905, 3204], 16: [3040, 3039, 1786, 1785], 's_11_16': [1815], 17: [2980, 2979, 2978, 1560], 's_11_17': [1755], 18: [3067, 1740, 3068, 3069], 's_11_18': [1575], 's_11_11': [3127], 1: [3217, 1426], 's_12_1': [1456], 4: [1846, 1845], 's_12_4': [1800, 2934], 's_12_8': [1756], 9: [3158, 1576], 's_12_9': [1486], 's_12_16': [3114], 's_12_18': [1725], 's_12_12': [1515], 's_2_6': [3173], 's_2_5': [1590], 's_2_8': [1531], 's_2_18': [3038], 's_2_2': [1667], 's_5_10': [1831], 's_5_4': [3175], 's_5_14': [1875], 's_5_5': [3160], 's_10_1': [1411], 's_10_8': [1771], 's_10_9': [1621], 15: [1890, 3100], 's_10_15': [1935, 1936], 's_10_10': [3186], 's_6_1': [3247], 's_6_9': [3263], 13: [1440, 1441], 's_6_13': [3022], 's_6_17': [3052], 's_6_6': [3261], 's_8_9': [3323], 's_8_16': [3324], 's_8_8': [1637], 7: [1995, 1996], 's_14_7': [1981], 19: [1950], 's_14_19': [1965], 's_14_14': [3131], 's_16_18': [1770], 's_16_4': [3219], 's_16_7': [1980], 's_16_17': [2994], 's_16_16': [2100], 's_17_7': [2995], 's_17_17': [1620], 's_18_13': [3082], 's_18_18': [1380], 's_1_13': [3172], 's_1_1': [3322], 's_4_4': [1847], 's_9_9': [1577], 's_15_19': [3070], 's_15_15': [2011], 's_13_13': [3097], 's_7_7': [3250], 's_19_19': [3010]}, {0: [1273, 5331], 3: [5195, 5301, 1152], 's_0_3': [1167], 11: [1123, 1124, 5600, 5599], 's_0_11': [5316], 12: [5419, 5421, 5420], 's_0_12': [1288], 's_0_0': [1197], 2: [5344, 5300, 972], 's_3_2': [5194], 5: [1064, 5330, 1062, 1063], 's_3_5': [5270], 10: [1138, 5555, 1139], 's_3_10': [5286], 's_3_3': [5225], 6: [973, 5375, 5374], 's_11_6': [974], 8: [1108, 1109], 's_11_8': [5585], 's_11_10': [1169], 14: [5615, 5614, 989], 's_11_14': [869], 16: [5480, 958, 959], 's_11_16': [5584], 17: [5494, 1049, 5495], 's_11_17': [1079], 18: [1033, 5451, 5450], 's_11_18': [1034], 's_11_11': [824], 1: [1228, 5496, 1229], 's_12_1': [5406], 4: [943], 's_12_4': [5404], 's_12_8': [5405], 9: [1153, 5391, 5390], 's_12_9': [1318], 's_12_16': [1078], 's_12_18': [1333], 's_12_12': [823], 's_2_6': [928], 's_2_5': [1077], 's_2_8': [5285], 's_2_18': [1032], 's_2_2': [5224], 's_5_10': [5255], 's_5_4': [5315], 's_5_14': [5630], 's_5_5': [5135], 's_10_1': [1214], 's_10_8': [5345], 's_10_9': [5481], 15: [5435, 5510, 1003], 's_10_15': [5511], 's_10_10': [1199], 's_6_1': [1168], 's_6_9': [5389], 13: [1183], 's_6_13': [1198], 's_6_17': [988], 's_6_6': [5373], 's_8_9': [5525], 's_8_16': [5465], 's_8_8': [1107], 7: [5569], 's_14_7': [884], 19: [899, 5539], 's_14_19': [5629], 's_14_14': [5613], 's_16_18': [1048], 's_16_4': [5254], 's_16_7': [944], 's_16_17': [5554], 's_16_16': [1018], 's_17_7': [914], 's_17_17': [779], 's_18_13': [1289, 5466], 's_18_18': [5452], 's_1_13': [5540], 's_1_1': [5497], 's_4_4': [5359], 's_9_9': [1303], 's_15_19': [5524], 's_15_15': [1094], 's_13_13': [1182], 's_7_7': [929], 's_19_19': [5659]}, {0: [3351, 3350], 3: [1021, 1022], 's_0_3': [1037], 11: [1185, 1186, 3366, 3365], 's_0_11': [1277], 12: [1217, 1216, 3200], 's_0_12': [1202], 's_0_0': [3349], 2: [3307, 3306, 3290, 1127], 's_3_2': [3425], 5: [961, 3305], 's_3_5': [1036], 10: [3170, 3185, 1066], 's_3_10': [3155], 's_3_3': [3485], 6: [3322, 1306, 1307], 's_11_6': [1321], 8: [1246, 3171], 's_11_8': [1170], 's_11_10': [1067], 14: [3260, 3364, 1006], 's_11_14': [1141], 16: [3051, 3050, 1155], 's_11_16': [3035], 17: [1200, 3096], 's_11_17': [3066], 18: [3276, 1335, 3352, 1336], 's_11_18': [3081], 's_11_11': [1187], 1: [3216, 3215], 's_12_1': [1081], 4: [3095, 1051, 1050], 's_12_4': [1126], 's_12_8': [3321], 9: [3246, 3230, 1171], 's_12_9': [3380], 's_12_16': [1215], 's_12_18': [3201], 's_12_12': [3486], 's_2_6': [1381], 's_2_5': [991], 's_2_8': [3291], 's_2_18': [1457], 's_2_2': [1128], 's_5_10': [960], 's_5_4': [3320], 's_5_14': [3379], 's_5_5': [3274], 's_10_1': [1096], 's_10_8': [1140], 's_10_9': [1201], 15: [946], 's_10_15': [3184], 's_10_10': [1065], 's_6_1': [1396], 's_6_9': [3231], 13: [1351], 's_6_13': [3337], 's_6_17': [1291], 's_6_6': [1305], 's_8_9': [1261], 's_8_16': [1245], 's_8_8': [3172], 7: [1111, 3126], 's_14_7': [3245], 19: [3259], 's_14_19': [976], 's_14_14': [872], 's_16_18': [1320], 's_16_4': [3080], 's_16_7': [1110], 's_16_17': [1230], 's_16_16': [3052], 's_17_7': [1276], 's_17_17': [2976], 's_18_13': [3277], 's_18_18': [1397], 's_1_13': [1366], 's_1_1': [3217], 's_4_4': [3065], 's_9_9': [1172], 's_15_19': [3244], 's_15_15': [3109], 's_13_13': [1352], 's_7_7': [3125], 's_19_19': [841]}, {0: [3859], 3: [3844, 3949, 905], 's_0_3': [920], 11: [3648, 799, 798], 's_0_11': [784], 12: [828, 3784, 829], 's_0_12': [844], 's_0_0': [3858], 2: [858, 859], 's_3_2': [3814], 5: [935, 934, 3634, 3633], 's_3_5': [3979], 10: [3679, 770, 768, 769], 's_3_10': [3889], 's_3_3': [3843], 6: [3588, 693], 's_11_6': [783], 8: [754, 888, 3664], 's_11_8': [3694], 's_11_10': [3918], 14: [663, 3572], 's_11_14': [648], 16: [3767, 3769, 3768], 's_11_16': [739], 17: [3693, 709, 708], 's_11_17': [3723], 18: [375</t>
+          <t>[0.4502110481262207, 0.6539931297302246, 0.6342546939849854, 0.5765764713287354, 0.45978569984436035, 0.5229392051696777, 0.8218913078308105, 0.7702312469482422, 0.32209348678588867, 0.5405776500701904, 0.6063034534454346, 0.6518127918243408, 0.5762143135070801, 0.6785781383514404, 0.5116004943847656, 0.43817663192749023, 1.1837928295135498, 0.5114941596984863, 0.5014247894287109, 0.5668797492980957, 0.7437584400177002, 0.42513132095336914, 0.46575379371643066, 0.36464715003967285, 0.3763923645019531, 0.7482883930206299, 0.5095193386077881, 0.4515037536621094, 0.6108694076538086, 1.4214000701904297, 0.7503049373626709, 0.628427267074585, 0.694866418838501, 0.8316972255706787, 0.5552382469177246, 0.6596577167510986, 0.5038280487060547, 0.7931625843048096, 0.6546320915222168, 0.8139102458953857, 0.43482542037963867, 0.608361005783081, 0.9599189758300781, 0.28572797775268555, 0.44753098487854004, 0.5242187976837158, 0.7232894897460938, 0.6355948448181152, 0.706214189529419, 0.42676591873168945, 0.6697943210601807, 0.3870687484741211, 0.8257710933685303, 0.7373766899108887, 0.3851940631866455, 0.8503875732421875, 0.49191784858703613, 0.6762058734893799, 0.8147919178009033, 0.4063143730163574, 0.5447747707366943, 0.4998655319213867, 0.9120974540710449, 0.9275097846984863, 0.5821094512939453, 0.8596441745758057, 0.9285600185394287, 0.5761959552764893, 0.5502474308013916, 0.30994319915771484, 0.5434191226959229, 0.31845617294311523, 0.6405274868011475, 0.8142311573028564, 0.5059583187103271, 0.3720431327819824, 0.6623663902282715, 0.7689919471740723, 0.39272403717041016, 0.6505298614501953, 0.6329653263092041, 0.5016603469848633, 0.9069333076477051, 0.9182701110839844, 0.4827585220336914, 0.9428369998931885, 0.3238260746002197, 0.7632532119750977, 0.9964950084686279, 0.361053466796875, 0.7888312339782715, 0.7805309295654297, 0.4834263324737549, 0.8818089962005615, 0.5279583930969238, 0.4584617614746094, 0.3662412166595459, 0.5000991821289062, 0.379345178604126, 0.6008238792419434]</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>[{0: [5285], 3: [5224, 987], 11: [5374, 958], 12: [1002, 5359], 2: [5329, 837], 5: [972, 5269], 10: [5315], 6: [5389, 898], 8: [5330], 14: [913], 16: [943, 5419], 17: [988], 18: [883], 1: [1048], 4: [5300], 9: [1033], 15: [5314], 13: [5344], 7: [5404], 19: [928]}, {0: [325], 3: [4921], 11: [4876, 370], 12: [4906, 340], 2: [4831, 355], 5: [4936], 10: [4800, 310], 6: [415], 8: [385, 4771], 14: [295], 16: [339, 4726], 17: [4711], 18: [4846, 400], 1: [4801], 4: [279, 280], 9: [4861], 15: [175], 13: [4816], 7: [294], 19: [4845]}, {0: [4077], 3: [2211], 11: [4076], 12: [2196, 4001], 2: [4090, 4091], 5: [4121, 2151], 10: [4106, 2166], 6: [4120, 2106], 8: [2181], 14: [4061], 16: [4046, 2090], 17: [2031], 18: [2075], 1: [4151], 4: [2150], 9: [4166], 15: [2240], 13: [2076], 7: [2016], 19: [4062]}, {0: [4055, 980], 3: [936], 11: [3994, 3993], 12: [4054], 2: [4098, 4099], 5: [4159, 951], 10: [4009], 6: [785, 4024], 8: [906], 14: [4158, 741], 16: [4069, 756], 17: [771], 18: [815], 1: [830], 4: [861], 9: [921], 15: [4008], 13: [3933], 7: [4143], 19: [726]}, {0: [5470], 3: [1918], 11: [1994, 5530], 12: [1978, 5455], 2: [5500], 5: [5515, 5516], 10: [1903, 5440], 6: [5501, 2129], 8: [2009, 5605], 14: [2039], 16: [5560, 2024], 17: [2114], 18: [1964, 1963], 1: [2053], 4: [1979], 9: [2069, 2068], 15: [5485], 13: [5545], 7: [5575], 19: [5486]}, {0: [1373], 3: [1418, 4567], 11: [4491, 1268], 12: [4506, 4507], 2: [1343, 1342], 5: [1328, 1327], 10: [4416, 4417], 6: [4461], 8: [1403, 4476], 14: [4356], 16: [1313], 17: [4446], 18: [4432, 1388], 1: [1253], 4: [4521], 9: [1238], 15: [1147], 13: [4431, 1283], 7: [1298], 19: [4355]}, {0: [5636], 3: [5621], 11: [2159, 5531], 12: [2233, 2234], 2: [5561, 2249], 5: [2144], 10: [5666, 2084], 6: [2174], 8: [5591], 14: [5651], 16: [5546, 2189], 17: [5501], 18: [2248], 1: [2083, 5456], 4: [5576], 9: [5606], 15: [5696], 13: [5441], 7: [2129, 5516], 19: [2099]}, {0: [5514], 3: [5513], 11: [1708, 1709], 12: [1754], 2: [1634, 5558], 5: [1619], 10: [5633, 1604], 6: [1724, 5649], 8: [1739, 5573], 14: [1618, 5438], 16: [5528, 1649], 17: [1694, 5588], 18: [1769, 5664], 1: [5618, 5619], 4: [5543], 9: [5634], 15: [1603], 13: [1799], 7: [1693], 19: [5453]}, {0: [511, 510], 3: [3047], 11: [3257, 586], 12: [3227], 2: [616, 615], 5: [525, 3032], 10: [3168, 645], 6: [3197], 8: [646, 3212], 14: [3107], 16: [3242, 556], 17: [541], 18: [601], 1: [661], 4: [526], 9: [571], 15: [3167], 13: [3318, 676], 7: [3092], 19: [450]}, {0: [3183], 3: [751], 11: [3228, 840, 841], 12: [810], 2: [3124], 5: [3139], 10: [765, 766], 6: [3244, 916], 8: [780, 3198], 14: [885, 2974], 16: [3093, 3094], 17: [3109], 18: [3079, 855], 1: [3154], 4: [825], 9: [3169], 15: [2928], 13: [856], 7: [870], 19: [750]}, {0: [2382], 3: [5082], 11: [2441, 5113], 12: [2381, 5007], 2: [4992, 2336], 5: [5097], 10: [2426], 6: [2456, 2455], 8: [5022], 14: [5098], 16: [4963, 2486], 17: [5083], 18: [2440], 1: [4842, 2425], 4: [2397, 2396], 9: [5037], 15: [5158], 13: [4857], 7: [2471], 19: [2547]}, {0: [1855], 3: [4734], 11: [4824], 12: [4885, 4884], 2: [4794, 1825], 5: [4704, 1734], 10: [1884, 4780], 6: [1914, 4795], 8: [4854, 1840], 14: [4823], 16: [1780, 4869], 17: [4809], 18: [1810, 4764], 1: [1990], 4: [1735], 9: [1945], 15: [4719], 13: [4765], 7: [4808, 1765], 19: [1719]}, {0: [784], 3: [785], 11: [3873, 3874], 12: [3813], 2: [3978], 5: [4008, 800], 10: [860, 3933], 6: [3903, 710], 8: [725], 14: [665], 16: [649, 3828], 17: [575, 3902], 18: [755], 1: [770], 4: [799], 9: [740], 15: [3932], 13: [3963], 7: [3888], 19: [3947]}, {0: [3200, 1111], 3: [3230], 11: [3261, 1201], 12: [1231, 3156], 2: [1126, 3171], 5: [3185, 1051], 10: [3215], 6: [1246], 8: [1216], 14: [3290, 3291], 16: [3306], 17: [3321], 18: [1262, 1261], 1: [3216], 4: [1140, 1141], 9: [1171, 3246], 15: [1096], 13: [3231], 7: [1186], 19: [1097]}, {0: [360], 3: [3016, 495], 11: [390, 3031], 12: [435, 3061], 2: [3046], 5: [330, 3091], 10: [3122, 391], 6: [465, 3181], 8: [420], 14: [3001], 16: [3076], 17: [376, 375], 18: [345], 1: [3196], 4: [315], 9: [3167], 15: [300, 3121], 13: [346], 7: [405, 2911], 19: [3000]}, {0: [257], 3: [3526], 11: [3555], 12: [258, 3645], 2: [3511], 5: [213, 3600], 10: [3525, 153], 6: [3510, 183], 8: [318, 3585], 14: [242, 243], 16: [168, 3630], 17: [199, 198], 18: [228, 229], 1: [138], 4: [93], 9: [3570], 15: [154], 13: [3615], 7: [3540], 19: [3720]}, {0: [890], 3: [3919], 11: [3933, 3934], 12: [814, 3889], 2: [3949, 1040], 5: [3904], 10: [905], 6: [964, 965], 8: [920], 14: [4010, 1025], 16: [845, 3979], 17: [980], 18: [875], 1: [3814], 4: [3903], 9: [3829], 15: [3964], 13: [3754, 874], 7: [4009], 19: [3965]}, {0: [4498], 3: [2648], 11: [2558], 12: [2602, 2603], 2: [2663], 5: [4574, 2723, 2724], 10: [4424], 6: [4453], 8: [4468, 2632], 14: [4364, 4363], 16: [2513, 4513], 17: [4378, 2528], 18: [4483], 1: [4528, 2573], 4: [2588], 9: [2587], 15: [2708], 13: [2543], 7: [2512], 19: [4379]}, {0: [3417], 3: [2462], 11: [3538, 2432], 12: [2417], 2: [3493], 5: [2477], 10: [3477, 3478], 6: [2388], 8: [2402], 14: [2478], 16: [3523, 2447], 17: [3552], 18: [3508], 1: [3462], 4: [3402], 9: [3567, 2343], 15: [2358], 13: [2373], 7: [2463], 19: [3582]}, {0: [4373], 3: [1552], 11: [4418, 1628], 12: [4508, 1673], 2: [1537], 5: [4403], 10: [1507, 4433], 6: [4388], 8: [4448, 4447], 14: [4462, 1522], 16: [4493, 1658], 17: [1598, 1597], 18: [4358], 1: [1582, 1583], 4: [4404], 9: [1643], 15: [4372], 13: [1567], 7: [4463], 19: [1448]}, {0: [3607], 3: [1518, 3698], 11: [1474, 1473], 12: [3562, 1488], 2: [1548], 5: [3652, 3653], 10: [1444, 3637], 6: [3547, 1547], 8: [1489, 3668], 14: [1639, 3713], 16: [1608, 3533], 17: [3518], 18: [3592, 3593], 1: [1443], 4: [1563], 9: [3667, 1428], 15: [3697], 13: [1458], 7: [1638], 19: [3712]}, {0: [3471], 3: [3470], 11: [1172, 3426], 12: [3456, 1187], 2: [1128], 5: [1113], 10: [1157, 3516], 6: [1247, 3501], 8: [3486], 14: [3410, 1112], 16: [1203, 1202], 17: [1217], 18: [3531], 1: [3561, 1278], 4: [3545], 9: [1263], 15: [3425], 13: [1248], 7: [3365], 19: [1082]}, {0: [367], 3: [4321], 11: [487, 4306], 12: [456, 4261], 2: [412], 5: [4336, 427], 10: [337, 336], 6: [4231, 4232], 8: [4276], 14: [397], 16: [441, 442], 17: [4171, 382], 18: [4247], 1: [352], 4: [426], 9: [4126, 471], 15: [4081], 13: [4246], 7: [4291], 19: [396]}, {0: [5232], 3: [2397], 11: [5187, 2367], 12: [2337, 2336], 2: [2291, 5082], 5: [5113, 2382], 10: [5143, 2411], 6: [2426], 8: [2366, 5052], 14: [5217], 16: [2261, 5157], 17: [5097], 18: [5127], 1: [2441, 5037], 4: [5112], 9: [5067], 15: [5172], 13: [5128], 7: [2352], 19: [2322]}, {0: [1603], 3: [5318], 11: [5303, 1602], 12: [1617, 1618], 2: [5319, 1707], 5: [5243, 1542], 10: [1557], 6: [5363, 1648], 8: [5273], 14: [1572], 16: [5153, 1587], 17: [1647, 5183], 18: [5289, 5288], 1: [5333], 4: [5228], 9: [5258], 15: [5212], 13: [1633], 7: [5182], 19: [5197]}, {0: [611], 3: [5103], 11: [582, 5177], 12: [656, 5027], 2: [597], 5: [626, 5072], 10: [5118, 732], 6: [5207, 687], 8: [5133], 14: [567], 16: [5012, 641], 17: [551, 552], 18: [5162], 1: [671, 686], 4: [521], 9: [5148], 15: [5088], 13: [672], 7: [566], 19: [5087]}, {0: [1008, 3710], 3: [1068, 1069], 11: [1158, 3635], 12: [3711, 1219], 2: [3725], 5: [1173, 3575], 10: [1188, 3740], 6: [1129], 8: [1114], 14: [3590], 16: [1264, 3681], 17: [3666], 18: [1143], 1: [1084, 3755], 4: [1218], 9: [3696], 15: [1099], 13: [3650], 7: [1203], 19: [1098]}, {0: [2598], 3: [2583, 3628], 11: [2597], 12: [2493, 3598], 2: [2568], 5: [3583], 10: [3478, 2538], 6: [3539], 8: [2508, 3568], 14: [3463, 2523], 16: [3553], 17: [3403, 2627], 18: [3524, 2643], 1: [3509, 2553], 4: [2658], 9: [3538], 15: [2492], 13: [2703], 7: [2582], 19: [3493]}, {0: [2989], 3: [885], 11: [870, 3094], 12: [750, 3048], 2: [915, 3079], 5: [3019, 930], 10: [3034, 3033], 6: [3064, 975], 8: [810], 14: [931], 16: [3124, 840], 17: [855], 18: [2974], 1: [3049], 4: [3018], 9: [825], 15: [990], 13: [900], 7: [3109], 19: [3155]}, {0: [4393], 3: [4392], 11: [2393], 12: [4362, 2422], 2: [2363], 5: [2272, 4422], 10: [4407, 4408], 6: [4482], 8: [4377, 2257], 14: [4451, 4452], 16: [4437, 4438], 17: [2318, 4527], 18: [4467, 2483], 1: [2348], 4: [4423], 9: [2378], 15: [2452], 13: [4497], 7: [2288], 19: [2437]}, {0: [2668], 3: [5383], 11: [2623, 5459], 12: [5548, 2669], 2: [2638], 5: [5444, 2653], 10: [2593, 5474], 6: [5489], 8: [5504], 14: [2788], 16: [5594, 2729], 17: [2714], 18: [5519], 1: [2564], 4: [2654], 9: [2608], 15: [2683], 13: [2579], 7: [5549], 19: [5399]}, {0: [4290], 3: [322], 11: [217, 4320], 12: [187], 2: [4245, 4246], 5: [307], 10: [4305, 232], 6: [126, 127], 8: [4260, 291], 14: [246, 4231], 16: [202], 17: [4170], 18: [157, 4230], 1: [4335], 4: [4275], 9: [4200, 4201], 15: [4216], 13: [142], 7: [4185], 19: [367]}, {0: [2599], 3: [3808, 2449], 11: [3899, 3898], 12: [3927, 3928], 2: [3838], 5: [2434], 10: [3883], 6: [3943, 2540], 8: [2525], 14: [2555, 3823], 16: [3988, 2465], 17: [2495], 18: [2585, 2584], 1: [2510], 4: [3912], 9: [2419, 3853], 15: [3884], 13: [3913], 7: [3973], 19: [2570]}, {0: [1349, 5647], 3: [1409], 11: [5586, 1319], 12: [5571], 2: [5512, 5511], 5: [1424, 5497], 10: [5601, 5602], 6: [1274, 5526], 8: [1259], 14: [5587], 16: [5556], 17: [1333, 1334], 18: [1289], 1: [1394], 4: [1304], 9: [1244], 15: [1499], 13: [5541], 7: [5706, 1364], 19: [1484]}, {0: [692], 3: [3378], 11: [631, 3333], 12: [737, 3423], 2: [752, 3408], 5: [707], 10: [3362, 3363], 6: [587, 3407], 8: [722, 3438], 14: [3453, 662], 16: [646, 3288], 17: [3303], 18: [3273], 1: [572, 3318], 4: [3348], 9: [677], 15: [616], 13: [3272], 7: [661], 19: [3377]}, {0: [2479], 3: [3538, 2478], 11: [2418, 3747], 12: [3703], 2: [3673], 5: [2508], 10: [3658, 3657], 6: [3688, 2493], 8: [2374], 14: [3597, 3598], 16: [3718], 17: [2433], 18: [3748, 2524], 1: [2539], 4: [2509], 9: [2389], 15: [2298], 13: [3643], 7: [2448], 19: [3596]}, {0: [991], 3: [3350], 11: [1127, 3290], 12: [1082, 3320], 2: [1067], 5: [3335], 10: [3245, 1006], 6: [1066, 3230], 8: [1052, 1051], 14: [3336], 16: [3380], 17: [3351, 1141], 18: [3365], 1: [1081], 4: [1097], 9: [3305], 15: [1111], 13: [3215, 1186], 7: [1202], 19: [1112]}, {0: [5214], 3: [5215], 11: [1872, 5290], 12: [1917], 2: [5199, 5200], 5: [5350, 2097], 10: [1963, 1962], 6: [1947], 8: [5260, 1977], 14: [1993], 16: [2008, 5305], 17: [1933, 1932], 18: [1902], 1: [2067, 5245], 4: [5321, 5320], 9: [5230], 15: [5455], 13: [5275], 7: [5425], 19: [1994]}, {0: [4547], 3: [579], 11: [623, 4487], 12: [4548], 2: [4622, 594], 5: [4578], 10: [4563], 6: [4608], 8: [653], 14: [668], 16: [4533, 4532], 17: [4472, 608], 18: [744, 4593], 1: [729, 4623], 4: [698], 9: [638], 15: [713], 13: [699], 7: [683], 19: [4413]}, {0: [2360], 3: [3942], 11: [3987, 3988], 12: [3897, 3898], 2: [3957], 5: [2315], 10: [2330, 3972], 6: [2480, 3927], 8: [2390], 14: [4002, 2405], 16: [2510, 3883], 17: [4003, 2495], 18: [2465], 1: [2345], 4: [3882], 9: [2375], 15: [2270], 13: [3912], 7: [4033], 19: [4017]}, {0: [544], 3: [545], 11: [3722], 12: [634, 3767], 2: [3827], 5: [560], 10: [529, 3812], 6: [604, 603], 8: [514, 3752], 14: [559], 16: [3693, 574], 17: [618], 18: [3828, 664], 1: [590, 3858], 4: [575, 3917], 9: [619], 15: [484], 13: [3843], 7: [3647], 19: [483, 3662]}, {0: [1266, 4011], 3: [4116], 11: [1370, 4086], 12: [1325], 2: [1296], 5: [4131], 10: [1400, 1401], 6: [4072, 1311], 8: [1355, 4101], 14: [1236], 16: [1341, 1340], 17: [3996, 1281], 18: [4042], 1: [4027], 4: [1326], 9: [4057], 15: [4207], 13: [1461], 7: [4146], 19: [4206]}, {0: [988], 3: [987, 5315], 11: [1048, 5389], 12: [5419], 2: [5344], 5: [1033], 10: [5359], 6: [958, 5374], 8: [898], 14: [5330], 16: [5405, 5404], 17: [1018], 18: [943], 1: [913], 4: [5420], 9: [883], 15: [1017], 13: [5254], 7: [5450, 1063], 19: [1002]}, {0: [1672], 3: [4178], 11: [4313], 12: [1792, 4254], 2: [1642, 4283], 5: [1701], 10: [1657, 4224], 6: [1762, 4329], 8: [1717, 1716], 14: [1702], 16: [4389, 1687], 17: [1732], 18: [1747], 1: [1807], 4: [1686], 9: [4239], 15: [1658], 13: [4344], 7: [4298], 19: [4448]}, {0: [2626], 3: [3314], 11: [2717, 3344], 12: [3464, 2627], 2: [2702], 5: [2641, 3329], 10: [3433, 2552], 6: [3404, 2732], 8: [3419, 3418], 14: [2596], 16: [2657], 17: [3373, 3374], 18: [3449], 1: [3434], 4: [2642], 9: [3403], 15: [2582], 13: [2687], 7: [3388], 19: [2597]}, {0: [5350], 3: [2067], 11: [5395, 2008], 12: [2038, 5275], 2: [5260], 5: [1977, 5230], 10: [5291, 5290], 6: [1962, 5305], 8: [2023], 14: [1978], 16: [5336, 5335], 17: [1963], 18: [2053, 2052], 1: [1917], 4: [1902], 9: [5306], 15: [2082], 13: [5245], 7: [5320], 19: [5365]}, {0: [1187, 3410], 3: [1217], 11: [3321, 1186], 12: [1082, 3351, 3350], 2: [1202], 5: [3426, 1307], 10: [3381, 3380], 6: [1201, 3306], 8: [3365], 14: [3291], 16: [1112], 17: [1127], 18: [3336], 1: [1262], 4: [3425], 9: [1141], 15: [1171], 13: [1277], 7: [3290], 19: [3276]}, {0: [3010, 3009], 3: [1980], 11: [1815], 12: [2979, 1770], 2: [3084, 3085], 5: [1995], 10: [2950, 2949], 6: [1740, 2994], 8: [1800], 14: [3024, 3025], 16: [1845, 3054], 17: [3069], 18: [1905, 3039], 1: [1650], 4: [2980], 9: [1665, 2964], 15: [2948, 1620], 13: [3038], 7: [1785], 19: [3023]}, {0: [2422], 3: [4317], 11: [2407, 2406], 12: [2497, 4408], 2: [2393, 2392], 5: [4302], 10: [2377, 4228], 6: [4213], 8: [4258], 14: [2362, 4347], 16: [2482, 4272], 17: [2421], 18: [4393], 1: [2496], 4: [2467], 9: [2528, 2527], 15: [4332], 13: [2511, 2512], 7: [4287], 19: [2272]}, {0: [2729], 3: [5594], 11: [5504, 2638], 12: [5473, 5474], 2: [2714], 5: [5608, 5609], 10: [2669], 6: [5444], 8: [5519, 2608], 14: [2579], 16: [2564, 5533], 17: [2623], 18: [5489], 1: [2668, 5459], 4: [2534], 9: [2654, 2653], 15: [5563], 13: [2698], 7: [5548], 19: [5578]}, {0: [4733], 3: [4732], 11: [1645, 4793], 12: [1554], 2: [1495], 5: [4717, 4718], 10: [1480], 6: [4852, 1570], 8: [4823, 4822], 14: [1630], 16: [1540, 1539], 17: [4868], 18: [4778, 1615], 1: [1555, 4837], 4: [4657, 1434], 9: [4807], 15: [4763], 13: [4913], 7: [4883], 19: [4748]}, {0: [5588], 3: [5589], 11: [1694], 12: [5648, 1604], 2: [1739], 5: [5634, 1754], 10: [1769, 5604, 5603], 6: [5708, 5707], 8: [5664, 5663], 14: [5633], 16: [5573, 1619], 17: [1709], 18: [5558], 1: [1559], 4: [5543], 9: [1544], 15: [1589], 13: [1514, 5557], 7: [5618], 19: [1574]}, {0: [4594], 3: [894], 11: [909], 12: [954, 4595], 2: [879], 5: [4729, 969], 10: [4685, 4684], 6: [4639], 8: [4699], 14: [4669], 16: [939, 4534], 17: [4624], 18: [4654], 1: [1044], 4: [968], 9: [983, 984], 15: [999], 13: [1029], 7: [924], 19: [1014]}, {0: [487], 3: [4486, 488], 11: [4306, 427], 12: [4381, 4382], 2: [4396, 368], 5: [503, 4456], 10: [563, 4427], 6: [4366], 8: [4397], 14: [457], 16: [472, 4441], 17: [442], 18: [338, 337], 1: [398], 4: [383], 9: [413], 15: [533], 13: [4351], 7: [4291], 19: [4412]}, {0: [3351], 3: [1277], 11: [1382, 3352], 12: [3336, 3337], 2: [3396], 5: [3291, 1262], 10: [3381], 6: [3411], 8: [1397, 3366], 14: [1336], 16: [3307, 1366], 17: [1292], 18: [1307], 1: [1232], 4: [1321], 9: [1247], 15: [1351], 13: [1337, 3441], 7: [3322], 19: [3216]}, {0: [1024], 3: [3800], 11: [1085, 3860], 12: [3814, 3815], 2: [1099, 1100], 5: [3785], 10: [1054], 6: [3830], 8: [950, 3845], 14: [1009], 16: [3919, 979], 17: [994], 18: [1115, 3920], 1: [3755, 1159], 4: [859, 3784], 9: [1069], 15: [3710], 13: [1144], 7: [3769], 19: [1008]}, {0: [1362], 3: [5317], 11: [5287, 5286, 1288], 12: [5272, 1377], 2: [1393], 5: [5332], 10: [1332], 6: [1273, 5376], 8: [5346], 14: [5331, 1243], 16: [5302, 1318], 17: [5421], 18: [5391, 1378], 1: [5271], 4: [1453], 9: [5361], 15: [5256], 13: [1303], 7: [5406], 19: [1242]}, {0: [2957, 405], 3: [2972], 11: [540, 3017], 12: [3031, 450], 2: [510], 5: [2987], 10: [3016, 495], 6: [3062, 3061], 8: [3077], 14: [555], 16: [3032, 585], 17: [570], 18: [3047, 3046], 1: [345], 4: [3107, 525], 9: [3076, 360], 15: [3092], 13: [330], 7: [2927], 19: [556]}, {0: [98], 3: [4560, 189], 11: [173, 4530], 12: [248, 4500], 2: [4665], 5: [4635, 324], 10: [204], 6: [174, 159], 8: [234, 4545], 14: [4455, 323], 16: [263], 17: [4485, 158], 18: [219, 4561], 1: [249, 4695], 4: [4606], 9: [113, 4605], 15: [203], 13: [4650], 7: [4470], 19: [4440]}, {0: [759, 4638], 3: [4683], 11: [864], 12: [729, 4623], 2: [699], 5: [4698], 10: [804, 4668], 6: [4758, 4759], 8: [4653], 14: [4699], 16: [4594, 849], 17: [4744], 18: [4608, 4609], 1: [730, 4713], 4: [774], 9: [714], 15: [834], 13: [669], 7: [879], 19: [4684]}, {0: [1330], 3: [1329], 11: [4851], 12: [4867, 4866], 2: [4806], 5: [1344], 10: [1285, 4716], 6: [1255], 8: [4731, 1270], 14: [1345], 16: [1316, 1315], 17: [1375, 4836], 18: [1300], 1: [1239, 1240], 4: [4777, 1420], 9: [4881], 15: [1286], 13: [4821], 7: [4942], 19: [4986]}, {0: [305], 3: [3900], 11: [200, 3945], 12: [4006, 366], 2: [215, 3930], 5: [155, 3915], 10: [320], 6: [260], 8: [3961, 275], 14: [3885], 16: [245, 4066], 17: [3975], 18: [290], 1: [4036], 4: [4005], 9: [321, 4051], 15: [3871], 13: [4021], 7: [3960, 125], 19: [3870]}, {0: [969], 3: [4729, 4730], 11: [968, 4595], 12: [954, 4654], 2: [1044, 1043], 5: [4715], 10: [1013, 1014], 6: [4624], 8: [4565], 14: [1074], 16: [4580, 998], 17: [983], 18: [4535, 4534], 1: [4639], 4: [999], 9: [4669, 939], 15: [4520], 13: [909], 7: [4610], 19: [1073]}, {0: [1785], 3: [3084], 11: [1801, 3114], 12: [1786], 2: [1710, 1711], 5: [1770, 3069], 10: [1845, 1846], 6: [1875, 3099], 8: [1831, 3249], 14: [1860], 16: [3234], 17: [3264, 1876], 18: [3218, 3219], 1: [3189], 4: [1771], 9: [3204], 15: [3175], 13: [1816], 7: [1861], 19: [3160]}, {0: [3311, 3310], 3: [1921], 11: [3175, 1951], 12: [2041, 3235], 2: [3250], 5: [1936], 10: [3161, 3160], 6: [2056, 3220], 8: [1981], 14: [3325], 16: [1982, 3295], 17: [3280], 18: [1966], 1: [2011], 4: [1906, 3234], 9: [1996], 15: [2146], 13: [3265], 7: [1891], 19: [3326]}, {0: [665], 3: [3993], 11: [604, 3873], 12: [3978, 725], 2: [680], 5: [4008], 10: [695], 6: [3902], 8: [4023, 710], 14: [741, 740], 16: [3843, 590, 591], 17: [575], 18: [3888], 1: [3917, 3918], 4: [726, 4053], 9: [3903], 15: [696], 13: [619], 7: [3858], 19: [4128]}, {0: [842], 3: [917, 3334], 11: [3470, 3469], 12: [3424], 2: [887], 5: [3409], 10: [857, 3408], 6: [3453, 3454], 8: [3484, 812], 14: [1037], 16: [977, 3439], 17: [962], 18: [872, 3349], 1: [782, 3423], 4: [902], 9: [827], 15: [3378], 13: [3348, 692], 7: [3485], 19: [3379]}, {0: [3548], 3: [1712], 11: [3458, 1638], 12: [3578, 1653], 2: [3563], 5: [3398, 1727], 10: [3488, 3489], 6: [1697], 8: [1668], 14: [1607], 16: [3593], 17: [3608, 1698], 18: [1623], 1: [3534, 1682], 4: [1728], 9: [3504], 15: [1592], 13: [3473], 7: [1608], 19: [3338]}, {0: [982], 3: [4294], 11: [4354], 12: [4324], 2: [4309], 5: [4249, 922], 10: [892, 4384], 6: [952, 953], 8: [4308, 862], 14: [923], 16: [4369, 967], 17: [938], 18: [877], 1: [4264, 937], 4: [847], 9: [4339], 15: [893], 13: [4279], 7: [4444], 19: [4474]}, {0: [885], 3: [3063, 3064], 11: [1020, 3034], 12: [705, 3004, 3003], 2: [750], 5: [3078, 3079], 10: [2989, 915], 6: [2974, 2975], 8: [2959, 900], 14: [870], 16: [3048, 3049], 17: [945], 18: [3033], 1: [840], 4: [735], 9: [765], 15: [916], 13: [855], 7: [3019, 1035], 19: [3094]}, {0: [3901], 3: [454, 3782], 11: [424], 12: [410, 3826], 2: [3812, 499], 5: [484], 10: [3766], 6: [3811], 8: [334, 3751], 14: [3857], 16: [469, 3887], 17: [439], 18: [3916, 500], 1: [365, 364], 4: [3827], 9: [349], 15: [3767], 13: [380], 7: [3842], 19: [514]}, {0: [2445], 3: [2446], 11: [2386, 3178], 12: [3207, 2326], 2: [3237], 5: [2461, 3253], 10: [2506, 3268], 6: [2416, 3252], 8: [2476], 14: [2536], 16: [2371, 3163], 17: [2415], 18: [3222], 1: [3267], 4: [3192], 9: [3312, 3313], 15: [2566], 13: [2341], 7: [3148], 19: [3103]}, {0: [900], 3: [901], 11: [2974, 870], 12: [3079], 2: [3094], 5: [916], 10: [3139], 6: [3064, 960], 8: [3048, 840], 14: [871, 3199], 16: [930, 3049], 17: [3034], 18: [885], 1: [810], 4: [915], 9: [825], 15: [795], 13: [3109], 7: [990], 19: [3154]}, {0: [1228, 5421], 3: [5481], 11: [1198, 1199], 12: [1229, 5496], 2: [5450, 1139], 5: [1124], 10: [5466, 1168], 6: [1274, 5451], 8: [5540], 14: [5511], 16: [1214, 5646], 17: [5601], 18: [5570], 1: [1289], 4: [5555], 9: [1183], 15: [5375], 13: [5571], 7: [1259], 19: [1153]}, {0: [583], 3: [582], 11: [5298], 12: [5267, 5268], 2: [5133], 5: [5222, 597], 10: [642, 5207], 6: [672, 5192], 8: [687], 14: [612], 16: [5283, 748], 17: [627], 18: [702], 1: [657], 4: [598], 9: [5253], 15: [537], 13: [5223], 7: [5328], 19: [5252]}, {0: [855, 3094], 3: [825], 11: [766, 3139], 12: [3093], 2: [3198], 5: [841, 3169], 10: [3154, 3153], 6: [721, 3138], 8: [780], 14: [3214, 901], 16: [736, 3183], 17: [3228], 18: [795], 1: [645], 4: [751], 9: [630, 3063], 15: [810], 13: [3108], 7: [3213], 19: [3124]}, {0: [2638], 3: [2637], 11: [5383, 5384], 12: [5429], 2: [5324], 5: [2622, 5264], 10: [5279, 2758], 6: [5444, 2668], 8: [2713], 14: [2623], 16: [5354, 2683], 17: [2653, 5474], 18: [2698], 1: [2772, 2773], 4: [2743], 9: [5414], 15: [5399], 13: [5459], 7: [5489], 19: [5398]}, {0: [2678], 3: [4514], 11: [2692, 2693], 12: [4454, 2782], 2: [2723, 2722], 5: [4529], 10: [4484, 2753], 6: [4379], 8: [4469], 14: [4574, 2618], 16: [2767, 4304], 17: [2677], 18: [4334], 1: [4364], 4: [2783, 2768], 9: [2738], 15: [2754], 13: [2647], 7: [2617, 4349], 19: [4544]}, {0: [4462], 3: [1537], 11: [1568], 12: [4477, 1448], 2: [1598, 4418], 5: [1552], 10: [4447], 6: [4523, 4522], 8: [4492, 1583], 14: [4433], 16: [1538, 4583], 17: [4508], 18: [1508, 4568], 1: [1433], 4: [1553], 9: [1418], 15: [4448], 13: [4507], 7: [1613], 19: [1628]}, {0: [4276], 3: [382, 381], 11: [337, 336], 12: [441], 2: [367], 5: [366], 10: [4111, 456], 6: [246, 4231], 8: [397, 4261], 14: [4156], 16: [4186, 276], 17: [4216], 18: [4171], 1: [4246, 4247], 4: [4141], 9: [4232], 15: [4126], 13: [291], 7: [306], 19: [426]}, {0: [2527], 3: [4318, 4317], 11: [4258, 2467], 12: [2406, 4213], 2: [4302], 5: [2317], 10: [2347, 4257], 6: [4228, 2377], 8: [4287, 2362], 14: [4362, 4363], 16: [2452, 2451], 17: [2436], 18: [4393, 2407], 1: [2392, 4332], 4: [4272], 9: [4197], 15: [2256], 13: [4347], 7: [2437], 19: [2257]}, {0: [3045], 3: [240], 11: [225, 226], 12: [165, 2970], 2: [3030, 210], 5: [255], 10: [3105, 120], 6: [90, 3075], 8: [2985, 2986], 14: [3180], 16: [3195, 180, 181], 17: [3090], 18: [3000], 1: [3135], 4: [3060], 9: [135], 15: [3120], 13: [150], 7: [211], 19: [196]}, {0: [754], 3: [755], 11: [3753], 12: [3738, 859], 2: [3829, 3828], 5: [3948, 725], 10: [3813, 784], 6: [829], 8: [3843, 694], 14: [740, 739], 16: [3768], 17: [814], 18: [844], 1: [3814], 4: [724], 9: [3844], 15: [679], 13: [3784, 964], 7: [799, 3903], 19: [3693]}, {0: [3404], 3: [2732], 11: [3449, 2777], 12: [2702, 2703], 2: [2748, 2733], 5: [2747], 10: [3389, 2687], 6: [2762, 3554], 8: [2657, 3464], 14: [3418, 3419], 16: [2718, 2717], 17: [3434], 18: [2778, 3614], 1: [2688, 3569], 4: [3299], 9: [3479], 15: [3388], 13: [2673], 7: [2627, 3509], 19: [2507]}, {0: [4545, 98], 3: [4560], 11: [99, 4740], 12: [4680, 219], 2: [204, 205], 5: [4575], 10: [69, 4590, 68], 6: [4710], 8: [4755, 174], 14: [54, 55], 16: [4695, 234], 17: [144], 18: [4770, 114], 1: [129], 4: [4576], 9: [159], 15: [70, 4920], 13: [4725], 7: [4605, 4606], 19: [56]}, {0: [806], 3: [5012, 5013], 11: [686, 5058], 12: [747, 5073], 2: [611], 5: [5027], 10: [641], 6: [5177, 687], 8: [5087, 5088], 14: [5057, 626], 16: [597, 5103], 17: [656], 18: [5118], 1: [5133], 4: [671], 9: [732, 5148], 15: [4968, 640], 13: [582], 7: [5162], 19: [596]}, {0: [4504], 3: [4519], 11: [982, 983], 12: [953], 2: [878], 5: [893], 10: [923, 4474], 6: [4459], 8: [4444], 14: [4549], 16: [4430, 1043], 17: [4565, 1028], 18: [4414, 4415], 1: [967, 4354], 4: [4489], 9: [938], 15: [924], 13: [908], 7: [4550], 19: [909]}, {0: [5217], 3: [2487], 11: [5218, 2502], 12: [2457, 5263], 2: [5233], 5: [5172, 2472], 10: [5278], 6: [2532], 8: [5353, 2607], 14: [5173], 16: [5309, 5308], 17: [2517, 5203], 18: [2592], 1: [2547, 2548], 4: [5293], 9: [2533], 15: [2578], 13: [5248], 7: [2667], 19: [2577]}, {0: [5444], 3: [2623], 11: [2653, 2654], 12: [5474, 2714], 2: [2638], 5: [5519], 10: [5504], 6: [2549, 5548], 8: [5533, 2564], 14: [5654, 2699], 16: [5608, 5609], 17: [2669], 18: [2759, 5459], 1: [2593], 4: [2729], 9: [2579], 15: [2684], 13: [5458], 7: [5594], 19: [5639]}, {0: [3479], 3: [2703], 11: [2612, 3568], 12: [3553, 2627], 2: [3584, 3583], 5: [2718], 10: [3494, 3493], 6: [3463, 2523], 8: [2553], 14: [3509], 16: [3539], 17: [2597], 18: [2658], 1: [2538], 4: [3524], 9: [2568], 15: [2492], 13: [3598], 7: [2582], 19: [3508]}, {0: [5315], 3: [943], 11: [958, 5404], 12: [853, 5314], 2: [5389, 5388], 5: [5344, 883], 10: [5419, 823], 6: [5434, 838], 8: [868], 14: [913], 16: [5449, 898], 17: [988], 18: [5359, 928], 1: [5479], 4: [5329], 9: [5464], 15: [5509], 13: [929], 7: [5374], 19: [914]}, {0: [3473], 3: [3472], 11: [3503, 1638], 12: [1562, 1563], 2: [1473], 5: [3458, 3457], 10: [1517], 6: [1532, 3518], 8: [1502, 3533], 14: [1577], 16: [3547, 3548], 17: [1547], 18: [3563, 3562], 1: [3488], 4: [3577, 1443], 9: [3412], 15: [1516], 13: [1488], 7: [1697, 3428], 19: [3353]}, {0: [900], 3: [901], 11: [855, 2974], 12: [3048, 3049], 2: [3139], 5: [916], 10: [3124], 6: [3079, 825], 8: [840], 14: [3094], 16: [870, 2989], 17: [3064], 18: [766, 765], 1: [810], 4: [915], 9: [3033, 780], 15: [751], 13: [3169], 7: [885], 19: [3093]}, {0: [3934], 3: [3933], 11: [4024, 890], 12: [3964, 965], 2: [3874, 755], 5: [3948], 10: [845], 6: [875], 8: [860], 14: [800], 16: [3979, 905], 17: [3889], 18: [921, 920], 1: [3994], 4: [3949], 9: [4040, 4039], 15: [846], 13: [4009], 7: [799, 3844], 19: [4098]}, {0: [4091], 3: [4092], 11: [2255, 4002], 12: [2286, 2285], 2: [4033, 2420], 5: [2361, 4017], 10: [2316, 2315], 6: [2330, 3942], 8: [4032], 14: [2405], 16: [2270, 3941], 17: [3972], 18: [3956, 3957], 1: [3882], 4: [4077], 9: [4047], 15: [3912], 13: [2345], 7: [3987], 19: [2404]}, {0: [2622, 5279], 3: [5324], 11: [2713], 12: [2743], 2: [5368, 2578], 5: [5413, 2563], 10: [5294, 2728], 6: [5339, 2683], 8: [5383, 5384], 14: [5309], 16: [2758, 5354], 17: [2682, 5264], 18: [5369], 1: [5429], 4: [5414], 9: [5399], 15: [2607], 13: [2698], 7: [5353, 2637], 19: [2592]}, {0: [4510], 3: [2018], 11: [2123, 4511], 12: [1988, 4525], 2: [2033], 5: [4421], 10: [2077, 4465], 6: [4495], 8: [4450], 14: [2138], 16: [4526, 2108], 17: [2093], 18: [4480], 1: [1973], 4: [4435, 4436], 9: [2003], 15: [4361], 13: [1958], 7: [4541], 19: [2137]}, {0: [1613], 3: [4523], 11: [1553, 4553], 12: [1748, 4478], 2: [4508], 5: [1568], 10: [1598, 4538], 6: [1629, 1628], 8: [1688], 14: [4492], 16: [4569, 4568], 17: [4583], 18: [1703], 1: [1643, 1644], 4: [4477, 1583], 9: [4493], 15: [4537], 13: [4643], 7: [1508], 19: [1523]}, {0: [2025], 3: [3055], 11: [3069, 3070], 12: [1980, 2934, 2935], 2: [3054, 3039], 5: [3040, 2100], 10: [1995], 6: [1935, 3024], 8: [2950, 1845], 14: [1965], 16: [1815, 3009], 17: [1785], 18: [1800], 1: [3085], 4: [3010], 9: [2980], 15: [3025], 13: [1770, 3084], 7: [2994, 2995], 19: [1950]}, {0: [4904], 3: [4919], 11: [2620, 4874], 12: [5054, 2711], 2: [2635], 5: [2785, 4889], 10: [2665], 6: [2726, 4964], 8: [4949], 14: [2770], 16: [2696, 2695], 17: [4784, 2725], 18: [4979], 1: [2666], 4: [4994], 9: [4934], 15: [4858], 13: [2651], 7: [4844], 19: [4859]}]</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>[120, 122, 124, 125, 119, 117, 124, 119, 126, 130, 116, 129, 117, 118, 121, 124, 126, 123, 120, 116, 116, 119, 123, 123, 118, 122, 130, 125, 134, 122, 126, 120, 117, 119, 129, 122, 125, 122, 121, 120, 120, 128, 119, 127, 119, 122, 129, 126, 135, 121, 140, 116, 120, 126, 128, 120, 127, 120, 132, 125, 123, 121, 126, 125, 122, 131, 121, 121, 130, 120, 124, 128, 118, 126, 122, 127, 114, 119, 120, 125, 118, 128, 123, 126, 130, 129, 116, 128, 119, 120, 127, 117, 121, 118, 124, 120, 122, 125, 120, 114]</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>[27, 28, 26, 27, 29, 29, 27, 30, 28, 28, 27, 29, 26, 29, 29, 29, 27, 28, 24, 28, 31, 27, 28, 28, 28, 28, 28, 28, 27, 28, 25, 28, 28, 28, 29, 26, 27, 29, 26, 27, 29, 27, 25, 26, 27, 27, 27, 30, 28, 27, 28, 28, 25, 28, 26, 28, 27, 29, 31, 27, 27, 28, 28, 28, 27, 28, 29, 26, 26, 30, 27, 27, 25, 27, 25, 28, 27, 28, 26, 27, 30, 28, 28, 31, 32, 29, 26, 27, 27, 25, 28, 29, 26, 27, 28, 29, 25, 27, 30, 26]</t>
-        </is>
+          <t>[0.09520602226257324, 0.08703923225402832, 0.09760046005249023, 0.10655784606933594, 0.1267383098602295, 0.094146728515625, 0.1403803825378418, 0.10686278343200684, 0.11140155792236328, 0.08872723579406738, 0.13907241821289062, 0.15697216987609863, 0.11703228950500488, 0.1490330696105957, 0.09217286109924316, 0.13637995719909668, 0.12264394760131836, 0.10451316833496094, 0.08827447891235352, 0.10185909271240234, 0.10840129852294922, 0.08845710754394531, 0.10123586654663086, 0.08147001266479492, 0.08848357200622559, 0.08611011505126953, 0.15886592864990234, 0.10787558555603027, 0.09978890419006348, 0.08283257484436035, 0.08082127571105957, 0.08673763275146484, 0.12129807472229004, 0.14767956733703613, 0.11916804313659668, 0.16100502014160156, 0.10946512222290039, 0.12639617919921875, 0.09757423400878906, 0.09884786605834961, 0.11069273948669434, 0.1134805679321289, 0.1276850700378418, 0.09356904029846191, 0.11177682876586914, 0.0995645523071289, 0.13976025581359863, 0.07574701309204102, 0.12483739852905273, 0.11542654037475586, 0.10942411422729492, 0.09108710289001465, 0.1004793643951416, 0.1159367561340332, 0.10324430465698242, 0.13640141487121582, 0.09070777893066406, 0.11549901962280273, 0.08538627624511719, 0.09530234336853027, 0.1273667812347412, 0.14591646194458008, 0.13364458084106445, 0.15953969955444336, 0.11968183517456055, 0.18318748474121094, 0.29433727264404297, 0.20604681968688965, 0.18437600135803223, 0.26734280586242676, 0.11322855949401855, 0.10810470581054688, 0.12176108360290527, 0.18955731391906738, 0.09653592109680176, 0.08722186088562012, 0.11263227462768555, 0.09167027473449707, 0.11643600463867188, 0.11027979850769043, 0.1116337776184082, 0.11011981964111328, 0.16233181953430176, 0.1126856803894043, 0.0989992618560791, 0.11635494232177734, 0.11966896057128906, 0.21372222900390625, 0.16256356239318848, 0.15913915634155273, 0.23912358283996582, 0.14125871658325195, 0.12815427780151367, 0.12548828125, 0.14086627960205078, 0.13566303253173828, 0.10464048385620117, 0.14752817153930664, 0.13604521751403809, 0.09958338737487793]</t>
+        </is>
+      </c>
+      <c r="AF4" t="n">
+        <v>204</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>66</v>
       </c>
       <c r="AH4" t="n">
-        <v>4.810457883663992</v>
+        <v>66</v>
       </c>
       <c r="AI4" t="n">
-        <v>1.476379683447645</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL4" t="inlineStr">
-        <is>
-          <t>[0.37943482398986816, 0.2866518497467041, 0.6917383670806885, 0.5072712898254395, 0.6033849716186523, 1.067507028579712, 0.5240542888641357, 0.8396542072296143, 0.6447725296020508, 0.6044974327087402, 0.3788580894470215, 0.6053798198699951, 0.748420238494873, 0.7403531074523926, 0.4807932376861572, 0.6815633773803711, 0.3832719326019287, 0.5514261722564697, 0.5927004814147949, 0.4826669692993164, 0.42610979080200195, 1.0954439640045166, 0.509218692779541, 0.43115782737731934, 0.4388570785522461, 0.47623610496520996, 0.5332615375518799, 0.4718620777130127, 0.45472192764282227, 0.37665557861328125, 0.48537254333496094, 0.6054191589355469, 0.5735030174255371, 0.3295564651489258, 0.5158500671386719, 0.4621396064758301, 0.6934695243835449, 0.3642456531524658, 0.5374112129211426, 0.8657915592193604, 0.6407628059387207, 0.8317234516143799, 0.43688201904296875, 0.340146541595459, 0.882810115814209, 0.6079807281494141, 0.3193831443786621, 0.3712637424468994, 0.6145443916320801, 0.2529458999633789, 0.4616997241973877, 0.46785736083984375, 0.7277305126190186, 0.4092433452606201, 0.566563606262207, 0.40837764739990234, 0.7034614086151123, 0.8625736236572266, 0.3970375061035156, 0.4251739978790283, 0.29934191703796387, 0.47804689407348633, 0.37171483039855957, 0.7491374015808105, 0.442126989364624, 0.42440056800842285, 0.8651182651519775, 0.6202259063720703, 0.3335881233215332, 0.9824023246765137, 0.2909069061279297, 0.3142271041870117, 0.6087071895599365, 0.4713118076324463, 0.42252349853515625, 0.4567840099334717, 0.5746102333068848, 0.6694941520690918, 0.5061674118041992, 0.6283061504364014, 0.28967738151550293, 0.5514647960662842, 0.6323750019073486, 0.46350646018981934, 0.4573183059692383, 0.28313541412353516, 0.527536153793335, 0.8392691612243652, 0.5478699207305908, 0.5599591732025146, 0.4629812240600586, 0.48627519607543945, 0.5163142681121826, 0.4974181652069092, 0.5750088691711426, 0.5309691429138184, 0.78739333152771, 0.8572907447814941, 0.2813377380371094, 0.7764542102813721]</t>
-        </is>
-      </c>
-      <c r="AM4" t="inlineStr">
-        <is>
-          <t>[0.0830392837524414, 0.08367514610290527, 0.09111690521240234, 0.07859468460083008, 0.06644940376281738, 0.07959747314453125, 0.09669804573059082, 0.07183003425598145, 0.07573843002319336, 0.08671784400939941, 0.07218527793884277, 0.07769322395324707, 0.07464051246643066, 0.0957038402557373, 0.07085132598876953, 0.07239532470703125, 0.09827423095703125, 0.07327604293823242, 0.07222604751586914, 0.09220218658447266, 0.08648061752319336, 0.09028744697570801, 0.08344292640686035, 0.07769632339477539, 0.09019160270690918, 0.08451271057128906, 0.09006118774414062, 0.07038617134094238, 0.07058238983154297, 0.08233189582824707, 0.07339072227478027, 0.0950479507446289, 0.0784308910369873, 0.08841085433959961, 0.07923293113708496, 0.08462285995483398, 0.11686491966247559, 0.06958150863647461, 0.07272076606750488, 0.08823895454406738, 0.07561564445495605, 0.06910991668701172, 0.06843948364257812, 0.10489630699157715, 0.081146240234375, 0.08441329002380371, 0.08158183097839355, 0.06591534614562988, 0.09607648849487305, 0.07554507255554199, 0.07479238510131836, 0.07259011268615723, 0.08018231391906738, 0.1068263053894043, 0.08837294578552246, 0.0894622802734375, 0.07352185249328613, 0.10450053215026855, 0.0748445987701416, 0.08803296089172363, 0.07839679718017578, 0.0901343822479248, 0.08279705047607422, 0.10148453712463379, 0.10391497611999512, 0.08843493461608887, 0.07546401023864746, 0.07512879371643066, 0.10061812400817871, 0.07764506340026855, 0.0914757251739502, 0.07466459274291992, 0.08064603805541992, 0.07054686546325684, 0.08766317367553711, 0.10877060890197754, 0.07289576530456543, 0.11530804634094238, 0.0875856876373291, 0.0862894058227539, 0.0925590991973877, 0.08056235313415527, 0.07719898223876953, 0.10322809219360352, 0.07176685333251953, 0.07548284530639648, 0.07774782180786133, 0.07218074798583984, 0.06859993934631348, 0.07620358467102051, 0.0736539363861084, 0.08093667030334473, 0.07362771034240723, 0.08978390693664551, 0.07831120491027832, 0.06976938247680664, 0.09194231033325195, 0.09136176109313965, 0.09071063995361328, 0.09120988845825195]</t>
-        </is>
-      </c>
-      <c r="AN4" t="n">
-        <v>244</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>66</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>86</v>
-      </c>
-      <c r="AQ4" t="n">
         <v>20</v>
       </c>
-      <c r="AR4" t="inlineStr">
-        <is>
-          <t>[0, 3, 's_0_3', 11, 's_0_11', 12, 's_0_12', 's_0_0', 2, 's_3_2', 5, 's_3_5', 10, 's_3_10', 's_3_3', 6, 's_11_6', 8, 's_11_8', 's_11_10', 14, 's_11_14', 16, 's_11_16', 17, 's_11_17', 18, 's_11_18', 's_11_11', 1, 's_12_1', 4, 's_12_4', 's_12_8', 9, 's_12_9', 's_12_16', 's_12_18', 's_12_12', 's_2_6', 's_2_5', 's_2_8', 's_2_18', 's_2_2', 's_5_10', 's_5_4', 's_5_14', 's_5_5', 's_10_1', 's_10_8', 's_10_9', 15, 's_10_15', 's_10_10', 's_6_1', 's_6_9', 13, 's_6_13', 's_6_17', 's_6_6', 's_8_9', 's_8_16', 's_8_8', 7, 's_14_7', 19, 's_14_19', 's_14_14', 's_16_18', 's_16_4', 's_16_7', 's_16_17', 's_16_16', 's_17_7', 's_17_17', 's_18_13', 's_18_18', 's_1_13', 's_1_1', 's_4_4', 's_9_9', 's_13_13', 's_15_19', 's_15_15', 's_7_7', 's_19_19']</t>
-        </is>
-      </c>
-      <c r="AS4" t="inlineStr">
-        <is>
-          <t>[0, 3, 11, 12, 2, 5, 10, 6, 8, 14, 16, 17, 18, 1, 4, 9, 15, 13, 7, 19]</t>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>[0, 3, 's_0_3', 11, 's_0_11', 12, 's_0_12', 2, 's_2_3', 5, 's_3_5', 10, 's_3_10', 6, 's_6_11', 8, 's_8_11', 's_10_11', 14, 's_11_14', 16, 's_11_16', 17, 's_11_17', 18, 's_11_18', 1, 's_1_12', 4, 's_4_12', 's_8_12', 9, 's_9_12', 's_12_16', 's_12_18', 's_1_6', 's_1_10', 13, 's_1_13', 's_2_6', 's_6_9', 's_6_13', 's_6_17', 's_5_10', 's_8_10', 's_9_10', 15, 's_10_15', 's_13_18', 's_2_5', 's_2_8', 's_2_18', 's_4_5', 's_5_14', 's_8_9', 's_8_16', 's_16_18', 's_4_16', 7, 's_7_16', 's_16_17', 's_7_14', 19, 's_14_19', 's_7_17', 's_15_19']</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>[0, 3, 11, 12, 2, 5, 10, 6, 8, 14, 16, 17, 18, 1, 4, 9, 13, 15, 7, 19]</t>
         </is>
       </c>
     </row>
@@ -1112,12 +1040,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>[0, 2, 6, 7, 8, 13, 16, 19, 20, 23, 25, 26, 27, 3, 9, 11, 21, 28, 14, 17, 24, 5, 10, 15, 29, 12, 1, 4, 22, 18]</t>
+          <t>[0, 2, 6, 7, 8, 13, 16, 19, 20, 23, 25, 26, 27, 1, 5, 12, 15, 21, 28, 3, 9, 11, 10, 14, 24, 4, 18, 22, 17, 29]</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>[(0, 2), (0, 6), (0, 7), (0, 8), (0, 13), (0, 16), (0, 19), (0, 20), (0, 23), (0, 25), (0, 26), (0, 27), (0, 0), (2, 3), (2, 9), (2, 11), (2, 19), (2, 20), (2, 21), (2, 25), (2, 27), (2, 28), (2, 2), (6, 13), (6, 14), (6, 17), (6, 20), (6, 25), (6, 6), (7, 3), (7, 14), (7, 21), (7, 24), (7, 27), (7, 28), (7, 7), (8, 3), (8, 5), (8, 10), (8, 14), (8, 15), (8, 16), (8, 23), (8, 29), (8, 8), (13, 12), (13, 25), (13, 13), (16, 1), (16, 4), (16, 5), (16, 14), (16, 17), (16, 19), (16, 20), (16, 22), (16, 29), (16, 16), (19, 3), (19, 4), (19, 5), (19, 9), (19, 15), (19, 20), (19, 28), (19, 19), (20, 3), (20, 4), (20, 9), (20, 11), (20, 14), (20, 18), (20, 27), (20, 20), (23, 10), (23, 11), (23, 21), (23, 22), (23, 24), (23, 28), (23, 29), (23, 23), (25, 11), (25, 15), (25, 26), (25, 28), (25, 25), (26, 5), (26, 9), (26, 26), (27, 4), (27, 10), (27, 18), (27, 27), (3, 10), (3, 14), (3, 24), (3, 3), (9, 15), (9, 11), (9, 14), (9, 22), (9, 9), (11, 21), (11, 22), (11, 11), (21, 1), (21, 5), (21, 4), (21, 14), (21, 21), (28, 1), (28, 5), (28, 24), (28, 28), (14, 17), (14, 14), (17, 15), (17, 17), (24, 24), (5, 1), (5, 18), (5, 22), (5, 5), (10, 18), (10, 29), (10, 10), (15, 1), (15, 15), (29, 29), (12, 1), (12, 18), (12, 12), (1, 1), (4, 4), (22, 22), (18, 18)]</t>
+          <t>[(0, 2), (0, 6), (0, 7), (0, 8), (0, 13), (0, 16), (0, 19), (0, 20), (0, 23), (0, 25), (0, 26), (0, 27), (2, 3), (2, 9), (2, 11), (2, 19), (2, 20), (2, 21), (2, 25), (2, 27), (2, 28), (6, 13), (6, 14), (6, 17), (6, 20), (6, 25), (7, 3), (7, 14), (7, 21), (7, 24), (7, 27), (7, 28), (8, 3), (8, 5), (8, 10), (8, 14), (8, 15), (8, 16), (8, 23), (8, 29), (13, 12), (13, 25), (16, 1), (16, 4), (16, 5), (16, 14), (16, 17), (16, 19), (16, 20), (16, 22), (16, 29), (19, 3), (19, 4), (19, 5), (19, 9), (19, 15), (19, 20), (19, 28), (20, 3), (20, 4), (20, 9), (20, 11), (20, 14), (20, 18), (20, 27), (23, 10), (23, 11), (23, 21), (23, 22), (23, 24), (23, 28), (23, 29), (25, 11), (25, 15), (25, 26), (25, 28), (26, 5), (26, 9), (27, 4), (27, 10), (27, 18), (1, 5), (1, 12), (1, 15), (1, 21), (1, 28), (5, 18), (5, 21), (5, 22), (5, 28), (12, 18), (15, 9), (15, 17), (21, 4), (21, 11), (21, 14), (28, 24), (3, 10), (3, 14), (3, 24), (9, 11), (9, 14), (9, 22), (11, 22), (10, 18), (10, 29), (14, 17)]</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -1132,14 +1060,14 @@
         <v>0.002534468157697533</v>
       </c>
       <c r="J5" t="n">
-        <v>0.03737104105042926</v>
+        <v>0.04916273078574496</v>
       </c>
       <c r="K5" t="n">
         <v>0.3149425287356322</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[(0, 2), (0, 's_0_2'), (0, 6), (0, 's_0_6'), (0, 7), (0, 's_0_7'), (0, 8), (0, 's_0_8'), (0, 13), (0, 's_0_13'), (0, 16), (0, 's_0_16'), (0, 19), (0, 's_0_19'), (0, 20), (0, 's_0_20'), (0, 23), (0, 's_0_23'), (0, 25), (0, 's_0_25'), (0, 26), (0, 's_0_26'), (0, 27), (0, 's_0_27'), (0, 's_0_0'), (0, 0), (2, 's_0_2'), (2, 3), (2, 's_2_3'), (2, 9), (2, 's_2_9'), (2, 11), (2, 's_2_11'), (2, 19), (2, 's_2_19'), (2, 20), (2, 's_2_20'), (2, 21), (2, 's_2_21'), (2, 25), (2, 's_2_25'), (2, 27), (2, 's_2_27'), (2, 28), (2, 's_2_28'), (2, 's_2_2'), (2, 2), ('s_0_2', 's_0_2'), (6, 's_0_6'), (6, 13), (6, 's_6_13'), (6, 14), (6, 's_6_14'), (6, 17), (6, 's_6_17'), (6, 20), (6, 's_6_20'), (6, 25), (6, 's_6_25'), (6, 's_6_6'), (6, 6), ('s_0_6', 's_0_6'), (7, 's_0_7'), (7, 3), (7, 's_7_3'), (7, 14), (7, 's_7_14'), (7, 21), (7, 's_7_21'), (7, 24), (7, 's_7_24'), (7, 27), (7, 's_7_27'), (7, 28), (7, 's_7_28'), (7, 's_7_7'), (7, 7), ('s_0_7', 's_0_7'), (8, 's_0_8'), (8, 3), (8, 's_8_3'), (8, 5), (8, 's_8_5'), (8, 10), (8, 's_8_10'), (8, 14), (8, 's_8_14'), (8, 15), (8, 's_8_15'), (8, 16), (8, 's_8_16'), (8, 23), (8, 's_8_23'), (8, 29), (8, 's_8_29'), (8, 's_8_8'), (8, 8), ('s_0_8', 's_0_8'), (13, 's_0_13'), (13, 's_6_13'), (13, 12), (13, 's_13_12'), (13, 25), (13, 's_13_25'), (13, 's_13_13'), (13, 13), ('s_0_13', 's_0_13'), (16, 's_0_16'), (16, 's_8_16'), (16, 1), (16, 's_16_1'), (16, 4), (16, 's_16_4'), (16, 5), (16, 's_16_5'), (16, 14), (16, 's_16_14'), (16, 17), (16, 's_16_17'), (16, 19), (16, 's_16_19'), (16, 20), (16, 's_16_20'), (16, 22), (16, 's_16_22'), (16, 29), (16, 's_16_29'), (16, 's_16_16'), (16, 16), ('s_0_16', 's_0_16'), (19, 's_0_19'), (19, 's_2_19'), (19, 's_16_19'), (19, 3), (19, 's_19_3'), (19, 4), (19, 's_19_4'), (19, 5), (19, 's_19_5'), (19, 9), (19, 's_19_9'), (19, 15), (19, 's_19_15'), (19, 20), (19, 's_19_20'), (19, 28), (19, 's_19_28'), (19, 's_19_19'), (19, 19), ('s_0_19', 's_0_19'), (20, 's_0_20'), (20, 's_2_20'), (20, 's_6_20'), (20, 's_16_20'), (20, 's_19_20'), (20, 3), (20, 's_20_3'), (20, 4), (20, 's_20_4'), (20, 9), (20, 's_20_9'), (20, 11), (20, 's_20_11'), (20, 14), (20, 's_20_14'), (20, 18), (20, 's_20_18'), (20, 27), (20, 's_20_27'), (20, 's_20_20'), (20, 20), ('s_0_20', 's_0_20'), (23, 's_0_23'), (23, 's_8_23'), (23, 10), (23, 's_23_10'), (23, 11), (23, 's_23_11'), (23, 21), (23, 's_23_21'), (23, 22), (23, 's_23_22'), (23, 24), (23, 's_23_24'), (23, 28), (23, 's_23_28'), (23, 29), (23, 's_23_29'), (23, 's_23_23'), (23, 23), ('s_0_23', 's_0_23'), (25, 's_0_25'), (25, 's_2_25'), (25, 's_6_25'), (25, 's_13_25'), (25, 11), (25, 's_25_11'), (25, 15), (25, 's_25_15'), (25, 26), (25, 's_25_26'), (25, 28), (25, 's_25_28'), (25, 's_25_25'), (25, 25), ('s_0_25', 's_0_25'), (26, 's_0_26'), (26, 's_25_26'), (26, 5), (26, 's_26_5'), (26, 9), (26, 's_26_9'), (26, 's_26_26'), (26, 26), ('s_0_26', 's_0_26'), (27, 's_0_27'), (27, 's_2_27'), (27, 's_7_27'), (27, 's_20_27'), (27, 4), (27, 's_27_4'), (27, 10), (27, 's_27_10'), (27, 18), (27, 's_27_18'), (27, 's_27_27'), (27, 27), ('s_0_27', 's_0_27'), ('s_0_0', 's_0_0'), (3, 's_2_3'), (3, 's_7_3'), (3, 's_8_3'), (3, 's_19_3'), (3, 's_20_3'), (3, 10), (3, 's_3_10'), (3, 14), (3, 's_3_14'), (3, 24), (3, 's_3_24'), (3, 's_3_3'), (3, 3), ('s_2_3', 's_2_3'), (9, 's_2_9'), (9, 's_19_9'), (9, 's_20_9'), (9, 's_26_9'), (9, 15), (9, 's_9_15'), (9, 11), (9, 's_9_11'), (9, 14), (9, 's_9_14'), (9, 22), (9, 's_9_22'), (9, 's_9_9'), (9, 9), ('s_2_9', 's_2_9'), (11, 's_2_11'), (11, 's_20_11'), (11, 's_23_11'), (11, 's_25_11'), (11, 's_9_11'), (11, 21), (11, 's_11_21'), (11, 22), (11, 's_11_22'), (11, 's_11_11'), (11, 11), ('s_2_11', 's_2_11'), ('s_2_19', 's_2_19'), ('s_2_20', 's_2_20'), (21, 's_2_21'), (21, 's_7_21'), (21, 's_23_21'), (21, 's_11_21'), (21, 1), (21, 's_21_1'), (21, 5), (21, 's_21_5'), (21, 4), (21, 's_21_4'), (21, 14), (21, 's_21_14'), (21, 's_21_21'), (21, 21), ('s_2_21', 's_2_21'), ('s_2_25', 's_2_25'), ('s_2_27', 's_2_27'), (28, 's_2_28'), (28, 's_7_28'), (28, 's_19_28'), (28, 's_23_28'), (28, 's_25_28'), (28, 1), (28, 's_28_1'), (28, 5), (28, 's_28_5'), (28, 24), (28, 's_28_24'), (28, 's_28_28'), (28, 28), ('s_2_28', 's_2_28'), ('s_2_2', 's_2_2'), ('s_6_13', 's_6_13'), (14, 's_6_14'), (14, 's_7_14'), (14, 's_8_14'), (14, 's_16_14'), (14, 's_20_14'), (14, 's_3_14'), (14, 's_9_14'), (14, 's_21_14'), (14, 17), (14, 's_14_17'), (14, 's_14_14'), (14, 14), ('s_6_14', 's_6_14'), (17, 's_6_17'), (17, 's_16_17'), (17, 's_14_17'), (17, 15), (17, 's_17_15'), (17, 's_17_17'), (17, 17), ('s_6_17', 's_6_17'), ('s_6_20', 's_6_20'), ('s_6_25', 's_6_25'), ('s_6_6', 's_6_6'), ('s_7_3', 's_7_3'), ('s_7_14', 's_7_14'), ('s_7_21', 's_7_21'), (24, 's_7_24'), (24, 's_23_24'), (24, 's_3_24'), (24, 's_28_24'), (24, 's_24_24'), (24, 24), ('s_7_24', 's_7_24'), ('s_7_27', 's_7_27'), ('s_7_28', 's_7_28'), ('s_7_7', 's_7_7'), ('s_8_3', 's_8_3'), (5, 's_8_5'), (5, 's_16_5'), (5, 's_19_5'), (5, 's_26_5'), (5, 's_21_5'), (5, 's_28_5'), (5, 1), (5, 's_5_1'), (5, 18), (5, 's_5_18'), (5, 22), (5, 's_5_22'), (5, 's_5_5'), (5, 5), ('s_8_5', 's_8_5'), (10, 's_8_10'), (10, 's_23_10'), (10, 's_27_10'), (10, 's_3_10'), (10, 18), (10, 's_10_18'), (10, 29), (10, 's_10_29'), (10, 's_10_10'), (10, 10), ('s_8_10', 's_8_10'), ('s_8_14', 's_8_14'), (15, 's_8_15'), (15, 's_19_15'), (15, 's_25_15'), (15, 's_9_15'), (15, 's_17_15'), (15, 1), (15, 's_15_1'), (15, 's_15_15'), (15, 15), ('s_8_15', 's_8_15'), ('s_8_16', 's_8_16'), ('s_8_23', 's_8_23'), (29, 's_8_29'), (29, 's_16_29'), (29, 's_23_29'), (29, 's_10_29'), (29, 's_29_29'), (29, 29), ('s_8_29', 's_8_29'), ('s_8_8', 's_8_8'), (12, 's_13_12'), (12, 1), (12, 's_12_1'), (12, 18), (12, 's_12_18'), (12, 's_12_12'), (12, 12), ('s_13_12', 's_13_12'), ('s_13_25', 's_13_25'), ('s_13_13', 's_13_13'), (1, 's_16_1'), (1, 's_21_1'), (1, 's_28_1'), (1, 's_5_1'), (1, 's_15_1'), (1, 's_12_1'), (1, 's_1_1'), (1, 1), ('s_16_1', 's_16_1'), (4, 's_16_4'), (4, 's_19_4'), (4, 's_20_4'), (4, 's_27_4'), (4, 's_21_4'), (4, 's_4_4'), (4, 4), ('s_16_4', 's_16_4'), ('s_16_5', 's_16_5'), ('s_16_14', 's_16_14'), ('s_16_17', 's_16_17'), ('s_16_19', 's_16_19'), ('s_16_20', 's_16_20'), (22, 's_16_22'), (22, 's_23_22'), (22, 's_9_22'), (22, 's_11_22'), (22, 's_5_22'), (22, 's_22_22'), (22, 22), ('s_16_22', 's_16_22'), ('s_16_29', 's_16_29'), ('s_16_16', 's_16_16'), ('s_19_3', 's_19_3'), ('s_19_4', 's_19_4'), ('s_19_5', 's_19_5'), ('s_19_9', 's_19_9'), ('s_19_15', 's_19_15'), ('s_19_20', 's_19_20'), ('s_19_28', 's_19_28'), ('s_19_19', 's_19_19'), ('s_20_3', 's_20_3'), ('s_20_4', 's_20_4'), ('s_20_9', 's_20_9'), ('s_20_11', 's_20_11'), ('s_20_14', 's_20_14'), (18, 's_20_18'), (18, 's_27_18'), (18, 's_5_18'), (18, 's_10_18'), (18, 's_12_18'), (18, 's_18_18'), (18, 18), ('s_20_18', 's_20_18'), ('s_20_27', 's_20_27'), ('s_20_20', 's_20_20'), ('s_23_10', 's_23_10'), ('s_23_11', 's_23_11'), ('s_23_21', 's_23_21'), ('s_23_22', 's_23_22'), ('s_23_24', 's_23_24'), ('s_23_28', 's_23_28'), ('s_23_29', 's_23_29'), ('s_23_23', 's_23_23'), ('s_25_11', 's_25_11'), ('s_25_15', 's_25_15'), ('s_25_26', 's_25_26'), ('s_25_28', 's_25_28'), ('s_25_25', 's_25_25'), ('s_26_5', 's_26_5'), ('s_26_9', 's_26_9'), ('s_26_26', 's_26_26'), ('s_27_4', 's_27_4'), ('s_27_10', 's_27_10'), ('s_27_18', 's_27_18'), ('s_27_27', 's_27_27'), ('s_3_10', 's_3_10'), ('s_3_14', 's_3_14'), ('s_3_24', 's_3_24'), ('s_3_3', 's_3_3'), ('s_9_15', 's_9_15'), ('s_9_11', 's_9_11'), ('s_9_14', 's_9_14'), ('s_9_22', 's_9_22'), ('s_9_9', 's_9_9'), ('s_11_21', 's_11_21'), ('s_11_22', 's_11_22'), ('s_11_11', 's_11_11'), ('s_21_1', 's_21_1'), ('s_21_5', 's_21_5'), ('s_21_4', 's_21_4'), ('s_21_14', 's_21_14'), ('s_21_21', 's_21_21'), ('s_28_1', 's_28_1'), ('s_28_5', 's_28_5'), ('s_28_24', 's_28_24'), ('s_28_28', 's_28_28'), ('s_14_17', 's_14_17'), ('s_14_14', 's_14_14'), ('s_17_15', 's_17_15'), ('s_17_17', 's_17_17'), ('s_24_24', 's_24_24'), ('s_5_1', 's_5_1'), ('s_5_18', 's_5_18'), ('s_5_22', 's_5_22'), ('s_5_5', 's_5_5'), ('s_10_18', 's_10_18'), ('s_10_29', 's_10_29'), ('s_10_10', 's_10_10'), ('s_15_1', 's_15_1'), ('s_15_15', 's_15_15'), ('s_29_29', 's_29_29'), ('s_12_1', 's_12_1'), ('s_12_18', 's_12_18'), ('s_12_12', 's_12_12'), ('s_1_1', 's_1_1'), ('s_4_4', 's_4_4'), ('s_22_22', 's_22_22'), ('s_18_18', 's_18_18')]</t>
+          <t>[(0, 2), (0, 's_0_2'), (0, 6), (0, 's_0_6'), (0, 7), (0, 's_0_7'), (0, 8), (0, 's_0_8'), (0, 13), (0, 's_0_13'), (0, 16), (0, 's_0_16'), (0, 19), (0, 's_0_19'), (0, 20), (0, 's_0_20'), (0, 23), (0, 's_0_23'), (0, 25), (0, 's_0_25'), (0, 26), (0, 's_0_26'), (0, 27), (0, 's_0_27'), (0, 0), (2, 's_0_2'), (2, 3), (2, 's_2_3'), (2, 9), (2, 's_2_9'), (2, 11), (2, 's_2_11'), (2, 19), (2, 's_2_19'), (2, 20), (2, 's_2_20'), (2, 21), (2, 's_2_21'), (2, 25), (2, 's_2_25'), (2, 27), (2, 's_2_27'), (2, 28), (2, 's_2_28'), (2, 2), ('s_0_2', 's_0_2'), (6, 's_0_6'), (6, 13), (6, 's_6_13'), (6, 14), (6, 's_6_14'), (6, 17), (6, 's_6_17'), (6, 20), (6, 's_6_20'), (6, 25), (6, 's_6_25'), (6, 6), ('s_0_6', 's_0_6'), (7, 's_0_7'), (7, 3), (7, 's_3_7'), (7, 14), (7, 's_7_14'), (7, 21), (7, 's_7_21'), (7, 24), (7, 's_7_24'), (7, 27), (7, 's_7_27'), (7, 28), (7, 's_7_28'), (7, 7), ('s_0_7', 's_0_7'), (8, 's_0_8'), (8, 3), (8, 's_3_8'), (8, 5), (8, 's_5_8'), (8, 10), (8, 's_8_10'), (8, 14), (8, 's_8_14'), (8, 15), (8, 's_8_15'), (8, 16), (8, 's_8_16'), (8, 23), (8, 's_8_23'), (8, 29), (8, 's_8_29'), (8, 8), ('s_0_8', 's_0_8'), (13, 's_0_13'), (13, 's_6_13'), (13, 12), (13, 's_12_13'), (13, 25), (13, 's_13_25'), (13, 13), ('s_0_13', 's_0_13'), (16, 's_0_16'), (16, 's_8_16'), (16, 1), (16, 's_1_16'), (16, 4), (16, 's_4_16'), (16, 5), (16, 's_5_16'), (16, 14), (16, 's_14_16'), (16, 17), (16, 's_16_17'), (16, 19), (16, 's_16_19'), (16, 20), (16, 's_16_20'), (16, 22), (16, 's_16_22'), (16, 29), (16, 's_16_29'), (16, 16), ('s_0_16', 's_0_16'), (19, 's_0_19'), (19, 's_2_19'), (19, 's_16_19'), (19, 3), (19, 's_3_19'), (19, 4), (19, 's_4_19'), (19, 5), (19, 's_5_19'), (19, 9), (19, 's_9_19'), (19, 15), (19, 's_15_19'), (19, 20), (19, 's_19_20'), (19, 28), (19, 's_19_28'), (19, 19), ('s_0_19', 's_0_19'), (20, 's_0_20'), (20, 's_2_20'), (20, 's_6_20'), (20, 's_16_20'), (20, 's_19_20'), (20, 3), (20, 's_3_20'), (20, 4), (20, 's_4_20'), (20, 9), (20, 's_9_20'), (20, 11), (20, 's_11_20'), (20, 14), (20, 's_14_20'), (20, 18), (20, 's_18_20'), (20, 27), (20, 's_20_27'), (20, 20), ('s_0_20', 's_0_20'), (23, 's_0_23'), (23, 's_8_23'), (23, 10), (23, 's_10_23'), (23, 11), (23, 's_11_23'), (23, 21), (23, 's_21_23'), (23, 22), (23, 's_22_23'), (23, 24), (23, 's_23_24'), (23, 28), (23, 's_23_28'), (23, 29), (23, 's_23_29'), (23, 23), ('s_0_23', 's_0_23'), (25, 's_0_25'), (25, 's_2_25'), (25, 's_6_25'), (25, 's_13_25'), (25, 11), (25, 's_11_25'), (25, 15), (25, 's_15_25'), (25, 26), (25, 's_25_26'), (25, 28), (25, 's_25_28'), (25, 25), ('s_0_25', 's_0_25'), (26, 's_0_26'), (26, 's_25_26'), (26, 5), (26, 's_5_26'), (26, 9), (26, 's_9_26'), (26, 26), ('s_0_26', 's_0_26'), (27, 's_0_27'), (27, 's_2_27'), (27, 's_7_27'), (27, 's_20_27'), (27, 4), (27, 's_4_27'), (27, 10), (27, 's_10_27'), (27, 18), (27, 's_18_27'), (27, 27), ('s_0_27', 's_0_27'), (3, 's_2_3'), (3, 's_3_7'), (3, 's_3_8'), (3, 's_3_19'), (3, 's_3_20'), (3, 10), (3, 's_3_10'), (3, 14), (3, 's_3_14'), (3, 24), (3, 's_3_24'), (3, 3), ('s_2_3', 's_2_3'), (9, 15), (9, 's_2_9'), (9, 's_9_19'), (9, 's_9_20'), (9, 's_9_26'), (9, 's_9_15'), (9, 11), (9, 's_9_11'), (9, 14), (9, 's_9_14'), (9, 22), (9, 's_9_22'), (9, 9), ('s_2_9', 's_2_9'), (11, 21), (11, 's_2_11'), (11, 's_11_20'), (11, 's_11_23'), (11, 's_11_25'), (11, 's_11_21'), (11, 's_9_11'), (11, 22), (11, 's_11_22'), (11, 11), ('s_2_11', 's_2_11'), ('s_2_19', 's_2_19'), ('s_2_20', 's_2_20'), (21, 1), (21, 5), (21, 's_2_21'), (21, 's_7_21'), (21, 's_21_23'), (21, 's_1_21'), (21, 's_5_21'), (21, 4), (21, 's_4_21'), (21, 's_11_21'), (21, 14), (21, 's_14_21'), (21, 21), ('s_2_21', 's_2_21'), ('s_2_25', 's_2_25'), ('s_2_27', 's_2_27'), (28, 1), (28, 5), (28, 's_2_28'), (28, 's_7_28'), (28, 's_19_28'), (28, 's_23_28'), (28, 's_25_28'), (28, 's_1_28'), (28, 's_5_28'), (28, 24), (28, 's_24_28'), (28, 28), ('s_2_28', 's_2_28'), ('s_6_13', 's_6_13'), (14, 's_6_14'), (14, 's_7_14'), (14, 's_8_14'), (14, 's_14_16'), (14, 's_14_20'), (14, 's_14_21'), (14, 's_3_14'), (14, 's_9_14'), (14, 17), (14, 's_14_17'), (14, 14), ('s_6_14', 's_6_14'), (17, 15), (17, 's_6_17'), (17, 's_16_17'), (17, 's_15_17'), (17, 's_14_17'), (17, 17), ('s_6_17', 's_6_17'), ('s_6_20', 's_6_20'), ('s_6_25', 's_6_25'), ('s_3_7', 's_3_7'), ('s_7_14', 's_7_14'), ('s_7_21', 's_7_21'), (24, 's_7_24'), (24, 's_23_24'), (24, 's_24_28'), (24, 's_3_24'), (24, 24), ('s_7_24', 's_7_24'), ('s_7_27', 's_7_27'), ('s_7_28', 's_7_28'), ('s_3_8', 's_3_8'), (5, 1), (5, 's_5_8'), (5, 's_5_16'), (5, 's_5_19'), (5, 's_5_26'), (5, 's_1_5'), (5, 18), (5, 's_5_18'), (5, 's_5_21'), (5, 22), (5, 's_5_22'), (5, 's_5_28'), (5, 5), ('s_5_8', 's_5_8'), (10, 's_8_10'), (10, 's_10_23'), (10, 's_10_27'), (10, 's_3_10'), (10, 18), (10, 's_10_18'), (10, 29), (10, 's_10_29'), (10, 10), ('s_8_10', 's_8_10'), ('s_8_14', 's_8_14'), (15, 1), (15, 's_8_15'), (15, 's_15_19'), (15, 's_15_25'), (15, 's_1_15'), (15, 's_9_15'), (15, 's_15_17'), (15, 15), ('s_8_15', 's_8_15'), ('s_8_16', 's_8_16'), ('s_8_23', 's_8_23'), (29, 's_8_29'), (29, 's_16_29'), (29, 's_23_29'), (29, 's_10_29'), (29, 29), ('s_8_29', 's_8_29'), (12, 1), (12, 's_12_13'), (12, 's_1_12'), (12, 18), (12, 's_12_18'), (12, 12), ('s_12_13', 's_12_13'), ('s_13_25', 's_13_25'), (1, 's_1_16'), (1, 's_1_5'), (1, 's_1_12'), (1, 's_1_15'), (1, 's_1_21'), (1, 's_1_28'), (1, 1), ('s_1_16', 's_1_16'), (4, 's_4_16'), (4, 's_4_19'), (4, 's_4_20'), (4, 's_4_27'), (4, 's_4_21'), (4, 4), ('s_4_16', 's_4_16'), ('s_5_16', 's_5_16'), ('s_14_16', 's_14_16'), ('s_16_17', 's_16_17'), ('s_16_19', 's_16_19'), ('s_16_20', 's_16_20'), (22, 's_16_22'), (22, 's_22_23'), (22, 's_5_22'), (22, 's_9_22'), (22, 's_11_22'), (22, 22), ('s_16_22', 's_16_22'), ('s_16_29', 's_16_29'), ('s_3_19', 's_3_19'), ('s_4_19', 's_4_19'), ('s_5_19', 's_5_19'), ('s_9_19', 's_9_19'), ('s_15_19', 's_15_19'), ('s_19_20', 's_19_20'), ('s_19_28', 's_19_28'), ('s_3_20', 's_3_20'), ('s_4_20', 's_4_20'), ('s_9_20', 's_9_20'), ('s_11_20', 's_11_20'), ('s_14_20', 's_14_20'), (18, 's_18_20'), (18, 's_18_27'), (18, 's_5_18'), (18, 's_12_18'), (18, 's_10_18'), (18, 18), ('s_18_20', 's_18_20'), ('s_20_27', 's_20_27'), ('s_10_23', 's_10_23'), ('s_11_23', 's_11_23'), ('s_21_23', 's_21_23'), ('s_22_23', 's_22_23'), ('s_23_24', 's_23_24'), ('s_23_28', 's_23_28'), ('s_23_29', 's_23_29'), ('s_11_25', 's_11_25'), ('s_15_25', 's_15_25'), ('s_25_26', 's_25_26'), ('s_25_28', 's_25_28'), ('s_5_26', 's_5_26'), ('s_9_26', 's_9_26'), ('s_4_27', 's_4_27'), ('s_10_27', 's_10_27'), ('s_18_27', 's_18_27'), ('s_1_5', 's_1_5'), ('s_1_12', 's_1_12'), ('s_1_15', 's_1_15'), ('s_1_21', 's_1_21'), ('s_1_28', 's_1_28'), ('s_5_18', 's_5_18'), ('s_5_21', 's_5_21'), ('s_5_22', 's_5_22'), ('s_5_28', 's_5_28'), ('s_12_18', 's_12_18'), ('s_9_15', 's_9_15'), ('s_15_17', 's_15_17'), ('s_4_21', 's_4_21'), ('s_11_21', 's_11_21'), ('s_14_21', 's_14_21'), ('s_24_28', 's_24_28'), ('s_3_10', 's_3_10'), ('s_3_14', 's_3_14'), ('s_3_24', 's_3_24'), ('s_9_11', 's_9_11'), ('s_9_14', 's_9_14'), ('s_9_22', 's_9_22'), ('s_11_22', 's_11_22'), ('s_10_18', 's_10_18'), ('s_10_29', 's_10_29'), ('s_14_17', 's_14_17')]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -1147,130 +1075,90 @@
           <t>[(0, 2), (0, 6), (0, 7), (0, 8), (0, 13), (0, 16), (0, 19), (0, 20), (0, 23), (0, 25), (0, 26), (0, 27), (0, 0), (2, 3), (2, 9), (2, 11), (2, 19), (2, 20), (2, 21), (2, 25), (2, 27), (2, 28), (2, 2), (6, 13), (6, 14), (6, 17), (6, 20), (6, 25), (6, 6), (7, 3), (7, 14), (7, 21), (7, 24), (7, 27), (7, 28), (7, 7), (8, 3), (8, 5), (8, 10), (8, 14), (8, 15), (8, 16), (8, 23), (8, 29), (8, 8), (13, 12), (13, 25), (13, 13), (16, 1), (16, 4), (16, 5), (16, 14), (16, 17), (16, 19), (16, 20), (16, 22), (16, 29), (16, 16), (19, 3), (19, 4), (19, 5), (19, 9), (19, 15), (19, 20), (19, 28), (19, 19), (20, 3), (20, 4), (20, 9), (20, 11), (20, 14), (20, 18), (20, 27), (20, 20), (23, 10), (23, 11), (23, 21), (23, 22), (23, 24), (23, 28), (23, 29), (23, 23), (25, 11), (25, 15), (25, 26), (25, 28), (25, 25), (26, 5), (26, 9), (26, 26), (27, 4), (27, 10), (27, 18), (27, 27), (3, 10), (3, 14), (3, 24), (3, 3), (9, 15), (9, 11), (9, 14), (9, 22), (9, 9), (11, 21), (11, 22), (11, 11), (21, 1), (21, 5), (21, 4), (21, 14), (21, 21), (28, 1), (28, 5), (28, 24), (28, 28), (14, 17), (14, 14), (17, 15), (17, 17), (24, 24), (5, 1), (5, 18), (5, 22), (5, 5), (10, 18), (10, 29), (10, 10), (15, 1), (15, 15), (29, 29), (12, 1), (12, 18), (12, 12), (1, 1), (4, 4), (22, 22), (18, 18)]</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="N5" t="n">
+        <v>252.33</v>
+      </c>
+      <c r="O5" t="n">
+        <v>64.33</v>
+      </c>
+      <c r="P5" t="n">
+        <v>3.832803606987</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.4339594841003418</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>{0: [1104, 4580, 4371, 1222, 1223, 4581], 2: [4506, 4505, 4504, 969, 968], 's_0_2': [1313], 6: [4355, 1058, 1057], 's_0_6': [4295], 7: [4926, 1207, 1208, 1209, 1210, 4835], 's_0_7': [4251], 8: [910, 4818, 1013, 1014, 4819], 's_0_8': [4685], 13: [892, 4535, 893, 4534], 's_0_13': [4536], 16: [982, 983, 1030, 1029, 4940, 4624], 's_0_16': [1028], 19: [1044, 4597, 4594, 4596, 4595], 's_0_19': [1178], 20: [4564, 1193, 4567, 4566, 4565], 's_0_20': [4582], 23: [4653, 4700, 1000, 4654, 999], 's_0_23': [939], 25: [1253, 1073, 4430, 4431], 's_0_25': [1252], 26: [1238, 1239], 's_0_26': [1237], 27: [759, 4446, 4579, 878, 4445, 4444], 's_0_27': [1327], 3: [863, 4925, 4924, 865, 864], 's_2_3': [970], 9: [4640, 4641, 4626, 1298, 1299], 's_2_9': [1328], 11: [4670, 1118, 1119], 's_2_11': [1133], 's_2_19': [1043], 's_2_20': [833], 21: [4805, 1164, 1162, 1163], 's_2_21': [1148], 's_2_25': [1268], 's_2_27': [4489], 28: [1075, 4716, 4714, 1074, 4715], 's_2_28': [984], 's_6_13': [4354], 14: [4549, 997, 4551, 4550, 998], 's_6_14': [4325], 17: [4400], 's_6_17': [4385], 's_6_20': [4475], 's_6_25': [1072], 's_3_7': [985, 4834], 's_7_14': [4341, 4340], 's_7_21': [1225], 24: [4894, 1150, 4895], 's_7_24': [1121], 's_7_27': [4460], 's_7_28': [4731], 's_3_8': [895], 5: [4848, 4849, 4761, 4760, 940], 's_5_8': [730], 10: [834, 4668], 's_8_10': [4744], 's_8_14': [4474], 15: [4520, 1090, 1089, 1088], 's_8_15': [4730], 's_8_16': [4639], 's_8_23': [804], 29: [955, 879, 4729], 's_8_29': [4879], 12: [819, 818], 's_12_13': [4519], 's_13_25': [4429], 1: [4789, 1105, 4790], 's_1_16': [1106], 4: [1283, 4610, 4611, 1284], 's_4_16': [954], 's_5_16': [941], 's_14_16': [4459], 's_16_17': [967], 's_16_19': [909], 's_16_20': [924], 22: [1059, 1060], 's_16_22': [4865], 's_16_29': [956], 's_3_19': [1045], 's_4_19': [4612], 's_5_19': [1224], 's_9_19': [1389], 's_15_19': [4745], 's_19_20': [1464], 's_19_28': [849], 's_3_20': [848], 's_4_20': [1269], 's_9_20': [1373], 's_11_20': [1194], 's_14_20': [1343], 18: [4563, 4623, 700, 698, 699], 's_18_20': [803], 's_20_27': [1403], 's_10_23': [744], 's_11_23': [4669], 's_21_23': [4804], 's_22_23': [4880], 's_23_24': [1149], 's_23_28': [894], 's_23_29': [4699], 's_11_25': [4416], 's_15_25': [4490], 's_25_26': [4476], 's_25_28': [1254], 's_5_26': [4746], 's_9_26': [4686], 's_4_27': [4609], 's_10_27': [774], 's_18_27': [4578], 's_3_10': [4939, 835], 's_3_14': [4415, 4414], 's_3_24': [911], 's_9_15': [4521], 's_9_11': [4671], 's_9_14': [1314], 's_9_22': [4625], 's_11_21': [1120], 's_11_22': [4655], 's_1_21': [4820], 's_5_21': [1179], 's_4_21': [4386], 's_14_21': [4370], 's_1_28': [925], 's_5_28': [1285], 's_24_28': [4910], 's_14_17': [1012], 's_15_17': [1103], 's_1_5': [760], 's_5_18': [4833], 's_5_22': [4775], 's_10_18': [714], 's_10_29': [4684], 's_1_15': [4850], 's_1_12': [4774], 's_12_18': [4473]}</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>{0: [1031, 957, 5120], 2: [1045, 1046], 6: [912, 5179], 7: [4940, 956], 8: [5150, 1106, 1107], 13: [5119], 16: [866, 4955, 4954], 19: [881, 941, 5014], 20: [911, 4999, 1000], 23: [1076, 4910, 1075], 25: [5105, 5104], 26: [1016], 27: [4984], 3: [4894, 4895], 9: [5030, 5029], 11: [5090, 1001], 21: [5044, 5045], 28: [4970, 851, 4969], 14: [985, 986], 17: [5089], 24: [1015], 5: [5060, 5059], 10: [4925, 970], 15: [971], 29: [1091], 12: [927], 1: [5074, 821], 4: [896], 22: [1061], 18: [4909, 926]}</t>
         </is>
       </c>
       <c r="T5" t="n">
-        <v>291.57</v>
+        <v>234</v>
       </c>
       <c r="U5" t="n">
-        <v>64.23999999999999</v>
+        <v>57</v>
       </c>
       <c r="V5" t="n">
-        <v>3.418953895568848</v>
+        <v>5.844826698303223</v>
       </c>
       <c r="W5" t="n">
-        <v>0.3388093709945679</v>
+        <v>0.4316649436950684</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>{0: [623, 4608, 1012, 1013, 4610, 4609], 2: [877, 878, 879, 880, 4939], 's_0_2': [4624], 6: [4488, 609, 608, 4489, 4563, 713], 's_0_6': [4502], 7: [1089, 1088, 802, 4399, 4400], 's_0_7': [4355], 8: [1058, 4579, 4581, 4580], 's_0_8': [983], 13: [637, 638], 's_0_13': [4637], 16: [4667, 4668, 4520, 1043, 1044, 4669], 's_0_16': [684], 19: [938, 939, 909, 984, 4654], 's_0_19': [1029], 20: [895, 894, 892, 4279, 893], 's_0_20': [1011], 23: [4505, 1120, 1118, 1119], 's_0_23': [4611], 25: [4759, 4548, 804, 803], 's_0_25': [4594], 26: [4533, 729, 730], 's_0_26': [4593], 27: [847, 4340, 4339], 's_0_27': [4325], 's_0_0': [4607], 3: [997, 4549, 998, 4550, 1163], 's_2_3': [4309], 9: [4817, 4819, 4818], 's_2_9': [850], 11: [4776, 4775, 910, 4774], 's_2_11': [911], 's_2_19': [4639], 's_2_20': [4249], 21: [835, 834, 908, 4504, 833], 's_2_21': [4894], 's_2_25': [805], 's_2_27': [4324], 28: [4683, 4685, 4684], 's_2_28': [4699], 's_2_2': [926], 's_6_13': [4472], 14: [863, 4414, 4413, 595, 594, 593], 's_6_14': [4788], 17: [4697, 534], 's_6_17': [4727], 's_6_20': [4384, 773], 's_6_25': [668], 's_6_6': [4562], 's_7_3': [4535], 's_7_14': [4458], 's_7_21': [832], 24: [1074, 4640], 's_7_24': [4625], 's_7_27': [4338], 's_7_28': [1104], 's_7_7': [4655], 's_8_3': [924], 5: [955, 817, 818, 4534, 954], 's_8_5': [968], 10: [4295, 4445, 1162], 's_8_10': [1208], 's_8_14': [848], 15: [774, 4653, 4712, 4713, 789], 's_8_15': [4564], 's_8_16': [1238, 4521], 's_8_23': [4460], 29: [4475, 1133], 's_8_29': [1193], 's_8_8': [1269], 12: [4353], 's_13_12': [652], 's_13_25': [653], 's_13_13': [636], 1: [4638, 743, 744], 's_16_1': [714], 4: [4444, 967], 's_16_4': [4430], 's_16_5': [4745], 's_16_14': [4652], 's_16_17': [579], 's_16_19': [1014], 's_16_20': [1042], 22: [4804, 4865, 1045], 's_16_22': [969], 's_16_29': [1103], 's_16_16': [549], 's_19_3': [4474], 's_19_4': [953], 's_19_5': [4729], 's_19_9': [940], 's_19_15': [4714], 's_19_20': [4459], 's_19_28': [999], 's_19_19': [4790], 's_20_3': [996], 's_20_4': [966], 's_20_9': [4924, 865], 's_20_11': [4849], 's_20_14': [4519], 18: [4370, 4368, 4369], 's_20_18': [1027], 's_20_27': [952], 's_20_20': [981], 's_23_10': [1117], 's_23_11': [4791], 's_23_21': [4879, 4880], 's_23_22': [4805], 's_23_24': [4715], 's_23_28': [4700], 's_23_29': [1148], 's_23_23': [4761], 's_25_11': [775], 's_25_15': [4789], 's_25_26': [4758], 's_25_28': [4698], 's_25_25': [759], 's_26_5': [4623], 's_26_9': [4803], 's_26_26': [4863], 's_27_4': [982], 's_27_10': [1087], 's_27_18': [1072], 's_27_27': [4293], 's_3_10': [4294], 's_3_14': [4415], 's_3_24': [4596, 4595], 's_3_3': [1164], 's_9_15': [565], 's_9_11': [1030], 's_9_14': [4802], 's_9_22': [925], 's_9_9': [670], 's_11_21': [4864], 's_11_22': [1060], 's_11_11': [1179], 's_21_1': [4503], 's_21_5': [4429], 's_21_4': [923], 's_21_14': [4473], 's_21_21': [4833], 's_28_1': [699], 's_28_5': [819], 's_28_24': [1059], 's_28_28': [669], 's_14_17': [4682], 's_14_14': [578], 's_17_15': [504], 's_17_17': [4742], 's_24_24': [4730], 's_5_1': [4443], 's_5_18': [4354], 's_5_22': [4834], 's_5_5': [956], 's_10_18': [1057], 's_10_29': [4401], 's_10_10': [1192], 's_15_1': [745], 's_15_15': [790], 's_29_29': [1132], 's_12_1': [728], 's_12_18': [712], 's_12_12': [758], 's_1_1': [4383], 's_4_4': [1028], 's_22_22': [4895], 's_18_18': [697]}</t>
+          <t>[244, 254, 236, 270, 257, 254, 255, 247, 250, 241, 246, 248, 240, 242, 263, 241, 264, 247, 274, 243, 266, 240, 240, 291, 262, 244, 259, 242, 264, 261, 237, 241, 259, 249, 247, 274, 239, 238, 255, 245, 268, 262, 239, 238, 247, 249, 259, 238, 274, 243, 257, 263, 253, 238, 242, 240, 246, 237, 249, 234, 257, 281, 264, 254, 251, 277, 253, 238, 265, 250, 258, 251, 245, 243, 256, 257, 276, 264, 258, 263, 243, 240, 270, 243, 260, 243, 254, 249, 265, 260, 243, 253, 251, 244, 253, 243, 248, 246, 259, 260]</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>{0: [5383, 2773, 5384], 2: [5414, 5413], 6: [2563], 7: [2608, 5474], 8: [2744, 5444], 13: [2578], 16: [2714, 2713, 5369], 19: [5458, 2503, 5368], 20: [2564, 2683, 5489], 23: [5534], 25: [2548, 5398], 26: [2533], 27: [2623], 3: [2654, 2653], 9: [5428, 5429], 11: [5399, 2788], 21: [2728, 2729], 28: [2699, 2593, 5504], 14: [2698, 5324], 17: [5339], 24: [5533], 5: [5609, 5608, 2534], 10: [2684, 2638, 5519], 15: [2669, 2668], 29: [5549], 12: [2579], 1: [5579, 5578], 4: [5459], 22: [2758, 2759], 18: [5548]}</t>
+          <t>[74, 68, 64, 63, 74, 66, 67, 71, 57, 60, 62, 62, 60, 69, 70, 60, 60, 61, 62, 61, 68, 68, 69, 61, 71, 60, 58, 63, 59, 60, 64, 65, 63, 67, 65, 66, 70, 60, 60, 57, 68, 62, 65, 69, 65, 63, 72, 62, 58, 63, 69, 59, 67, 71, 68, 59, 70, 63, 64, 69, 65, 72, 69, 59, 62, 66, 61, 64, 70, 64, 71, 67, 67, 63, 66, 65, 64, 67, 60, 63, 63, 62, 67, 62, 57, 66, 63, 62, 64, 66, 59, 59, 66, 61, 63, 65, 65, 63, 63, 61]</t>
         </is>
       </c>
       <c r="Z5" t="n">
-        <v>257</v>
+        <v>11.56104133578272</v>
       </c>
       <c r="AA5" t="n">
-        <v>56</v>
+        <v>4.022801174918951</v>
       </c>
       <c r="AB5" t="n">
-        <v>4.920925140380859</v>
+        <v>1</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.2361710071563721</v>
+        <v>1</v>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>[{0: [3963, 3962, 455, 456, 4261, 337], 2: [4218, 4217, 443, 442, 4185, 4186, 441], 's_0_2': [367], 6: [652, 651, 4187, 4188], 's_0_6': [4262], 7: [4081, 4082, 156, 4080], 's_0_7': [605], 8: [3960, 3961, 427, 426, 425], 's_0_8': [4321], 13: [4293, 757, 755, 756], 's_0_13': [3978], 16: [3886, 3887, 515, 4157, 4156, 516], 's_0_16': [530], 19: [4125, 4126, 353, 352, 4336, 396, 397], 's_0_19': [4096], 20: [3946, 470, 471, 4247, 532, 533], 's_0_20': [485], 23: [3975, 4246, 246, 245], 's_0_23': [382], 25: [4290, 4292, 4291], 's_0_25': [4306], 26: [487, 383, 4352, 4351], 's_0_26': [502], 27: [440, 500, 680, 4023, 4022], 's_0_27': [665], 's_0_0': [4052, 4053], 3: [4112, 380, 381, 4111], 's_2_3': [666], 9: [4470, 4471, 4487, 473, 4486], 's_2_9': [4621], 11: [247, 4440, 4577, 4576, 308], 's_2_11': [428], 's_2_19': [501], 's_2_20': [4412], 21: [4245, 4200, 4320, 186, 187], 's_2_21': [4170], 's_2_25': [202], 's_2_27': [681], 28: [4155, 262, 261], 's_2_28': [111], 's_2_2': [4219], 's_6_13': [4143], 14: [4201, 561, 563, 562, 4202], 's_6_14': [4277], 17: [4172, 696, 4173], 's_6_17': [711], 's_6_20': [4232, 4233], 's_6_25': [667, 4248], 's_6_6': [786], 's_7_3': [531], 's_7_14': [4097], 's_7_21': [157], 24: [4051, 260], 's_7_24': [4050], 's_7_27': [576], 's_7_28': [231], 's_7_7': [4083], 's_8_3': [3976], 5: [124, 125, 126, 4140, 292, 291, 4141], 's_8_5': [290], 10: [3901, 305, 185, 3900], 's_8_10': [170], 's_8_14': [4382], 15: [4171, 412, 413, 4397, 4398], 's_8_15': [4456], 's_8_16': [424], 's_8_23': [200], 29: [350, 4005, 4006], 's_8_29': [110], 's_8_8': [215], 12: [3916, 3918, 3917], 's_13_12': [770], 's_13_25': [4307, 4308], 's_13_13': [4249], 1: [322, 335, 4110, 321, 320, 4036], 's_16_1': [336], 4: [546, 4065, 4066, 4067], 's_16_4': [4037], 's_16_5': [3885], 's_16_14': [560], 's_16_17': [4158], 's_16_19': [486], 's_16_20': [517], 22: [278, 276, 277], 's_16_22': [274, 275], 's_16_29': [4007], 's_16_16': [3888], 's_19_3': [351], 's_19_4': [201], 's_19_5': [4411], 's_19_9': [4381, 233], 's_19_15': [398], 's_19_20': [395], 's_19_28': [4426], 's_19_19': [4501], 's_20_3': [3931], 's_20_4': [547], 's_20_9': [4532], 's_20_11': [518], 's_20_14': [4502], 18: [411, 3812, 410, 3811], 's_20_18': [365], 's_20_27': [3947], 's_20_20': [534], 's_23_10': [3930], 's_23_11': [307], 's_23_21': [4260, 172], 's_23_22': [4231], 's_23_24': [3945], 's_23_28': [4216], 's_23_29': [3990], 's_23_23': [244], 's_25_11': [457, 4441], 's_25_15': [682], 's_25_26': [622], 's_25_28': [4305], 's_25_25': [637], 's_26_5': [4366], 's_26_9': [368], 's_26_26': [548], 's_27_4': [3992], 's_27_10': [3902], 's_27_18': [679, 3767, 529], 's_27_27': [726], 's_3_10': [4021], 's_3_14': [4127], 's_3_24': [366], 's_3_3': [379], 's_9_15': [578], 's_9_11': [248], 's_9_14': [4472], 's_9_22': [4485], 's_9_9': [338], 's_11_21': [188], 's_11_22': [4455], 's_11_11': [234], 's_21_1': [4035], 's_21_5': [4020], 's_21_4': [141], 's_21_14': [232], 's_21_21': [37], 's_28_1': [4275], 's_28_5': [96], 's_28_24': [216], 's_28_28': [263], 's_14_17': [4203], 's_14_14': [564], 's_17_15': [697], 's_17_17': [577], 's_24_24': [4095], 's_5_1': [4396], 's_5_18': [3810], 's_5_22': [293], 's_5_5': [3690], 's_10_18': [304], 's_10_29': [3991], 's_10_10': [184], 's_15_1': [306], 's_15_15': [4399], 's_29_29': [349], 's_12_1': [3915], 's_12_18': [590], 's_12_12': [649], 's_1_1': [319], 's_4_4': [171], 's_22_22': [4606], 's_18_18': [3827]}, {0: [1605, 1606, 3353, 3400, 3399, 3398, 1607], 2: [2146, 1652, 3309, 3311, 3310], 's_0_2': [3278], 6: [3503, 1803, 1653, 3504], 's_0_6': [1592], 7: [2041, 3537, 3536, 3506, 2042], 's_0_7': [2072], 8: [3053, 3160, 1740, 1966, 1965, 3084, 3085], 's_0_8': [3038], 13: [3473], 's_0_13': [1562], 16: [1999, 1998, 1997, 3175, 1875, 1996], 's_0_16': [3069, 3068], 19: [3340, 3729, 1893, 1892, 1891], 's_0_19': [1952], 20: [3609, 3204, 1860, 3203, 1863, 1862, 1861], 's_0_20': [3188], 23: [3116, 3415, 1982, 3115, 1981], 's_0_23': [2057], 25: [3383, 1622, 1547, 3444, 3443], 's_0_25': [3338], 26: [3639, 1742, 3578, 1743], 's_0_26': [1608], 27: [3249, 1726, 3535, 3534, 1727], 's_0_27': [3233], 's_0_0': [1516], 3: [3219, 2161, 1936, 3266, 3265], 's_2_3': [3236], 9: [1771, 3369, 1773, 1772], 's_2_9': [1906], 11: [2012, 3429, 3341, 3430], 's_2_11': [1847], 's_2_19': [1876], 's_2_20': [1651], 21: [3564, 2088, 3565, 2086, 2087], 's_2_21': [3296], 's_2_25': [3308], 's_2_27': [3413], 28: [1922, 3445, 2148, 2147, 3446], 's_2_28': [2177], 's_2_2': [2145], 's_6_13': [1638], 14: [3280, 3281, 2162, 1788, 3594, 3595, 2163, 3596], 's_6_14': [3579], 17: [3114, 1787, 1785, 1786], 's_6_17': [3459], 's_6_20': [3608], 's_6_25': [3488], 's_6_6': [3502], 's_7_3': [2056], 's_7_14': [2298], 's_7_21': [2013], 24: [2208, 2206, 2207], 's_7_24': [3522], 's_7_27': [3250], 's_7_28': [2133], 's_7_7': [2313], 's_8_3': [1951], 5: [1711, 1969, 1968, 1967, 1712, 3489, 3490], 's_8_5': [1710], 10: [1831, 3100, 3099], 's_8_10': [1755], 's_8_14': [1921], 15: [3325, 3324, 3414, 1817], 's_8_15': [1741], 's_8_16': [1995], 's_8_23': [2055], 29: [3130, 1890], 's_8_29': [1950], 's_8_8': [3025], 12: [1682, 1681], 's_13_12': [1697], 's_13_25': [1577], 's_13_13': [3472], 1: [3550, 1907, 3548, 3549], 's_16_1': [3505], 4: [3670, 1953], 's_16_4': [1984], 's_16_5': [3805], 's_16_14': [3295], 's_16_17': [3039], 's_16_19': [3655], 's_16_20': [1846], 22: [3370, 2117, 3190, 2116], 's_16_22': [3220], 's_16_29': [3054], 's_16_16': [3760], 's_19_3': [3234], 's_19_4': [1834], 's_19_5': [3640], 's_19_9': [1774], 's_19_15': [1937], 's_19_20': [3700], 's_19_28': [3685, 3686], 's_19_19': [3728], 's_20_3': [1816], 's_20_4': [3610], 's_20_9': [3474], 's_20_11': [1877], 's_20_14': [1878], 18: [1621, 3264, 3263], 's_20_18': [1591], 's_20_27': [1758], 's_20_20': [1864], 's_23_10': [3101], 's_23_11': [2102], 's_23_21': [3385], 's_23_22': [2070], 's_23_24': [2191], 's_23_28': [3416], 's_23_29': [1935], 's_23_23': [2176], 's_25_11': [3428], 's_25_15': [1832], 's_25_26': [1757], 's_25_28': [3384], 's_25_25': [3382], 's_26_5': [1713], 's_26_9': [3624], 's_26_26': [1744], 's_27_4': [1923], 's_27_10': [1725], 's_27_18': [3248], 's_27_27': [1728], 's_3_10': [2026], 's_3_14': [3326, 2101], 's_3_24': [3191], 's_3_3': [2160], 's_9_15': [3294], 's_9_11': [1802], 's_9_14': [3669], 's_9_22': [3189], 's_9_9': [3654], 's_11_21': [3431], 's_11_22': [2071], 's_11_11': [2011], 's_21_1': [2028], 's_21_5': [1833], 's_21_4': [3580], 's_21_14': [3611], 's_21_21': [3745], 's_28_1': [3460], 's_28_5': [3355], 's_28_24': [3566], 's_28_28': [3656], 's_14_17': [3279], 's_14_14': [2221], 's_17_15': [3354], 's_17_17': [3024], 's_24_24': [3162], 's_5_1': [1848], 's_5_18': [3218], 's_5_22': [3491], 's_5_5': [3820], 's_10_18': [1801], 's_10_29': [1905], 's_10_10': [3098], 's_15_1': [1818], 's_15_15': [3323], 's_29_29': [3070, 1980], 's_12_1': [3563], 's_12_18': [1696], 's_12_12': [3368], 's_1_1': [3547], 's_4_4': [1954], 's_22_22': [3161], 's_18_18': [3173]}, {0: [5041, 838, 837, 836, 5044, 5404, 5043, 5042], 2: [778, 791, 5070, 777, 5071, 5072, 701, 5073], 's_0_2': [5119], 6: [5101, 5102, 656, 5103], 's_0_6': [311], 7: [357, 5175, 431, 5176], 's_0_7': [5056], 8: [807, 5299, 5344, 914, 913], 's_0_8': [5464], 13: [281, 5131, 388, 387], 's_0_13': [386], 16: [5389, 5388, 598, 597, 5493, 613, 5387], 's_0_16': [596], 19: [5027, 641, 644, 5088, 643, 642], 's_0_19': [5089], 20: [5012, 523, 5222, 521, 522], 's_0_20': [551], 23: [313, 5476, 5480, 5477, 749, 5479, 5478], 's_0_23': [823], 25: [5284, 5281, 446, 447, 5283, 5282], 's_0_25': [822], 26: [5373, 5328, 733], 's_0_26': [5358], 27: [5239, 853, 852, 5147, 5148, 5149], 's_0_27': [5329], 's_0_0': [926], 3: [5265, 5269, 5266, 5268, 5267], 's_2_3': [702], 9: [5402, 5538, 748, 793, 5403], 's_2_9': [5418], 11: [869, 868, 4967, 867, 866, 4969, 4968], 's_2_11': [5013], 's_2_19': [5118], 's_2_20': [671], 21: [4952, 401, 5507, 404, 403, 402], 's_2_21': [506], 's_2_25': [5086], 's_2_27': [5134], 28: [222, 5567, 5566, 5550, 5551, 224, 223], 's_2_28': [5085], 's_2_2': [131], 's_6_13': [266], 14: [5236, 5237, 5298, 5207, 626, 627], 's_6_14': [657], 17: [5162, 5163], 's_6_17': [552], 's_6_20': [536], 's_6_25': [5117], 's_6_6': [655], 's_7_3': [177], 's_7_14': [432], 's_7_21': [5191], 24: [5370, 192, 193], 's_7_24': [207], 's_7_27': [5146], 's_7_28': [5160], 's_7_7': [356], 's_8_3': [882], 5: [539, 5463, 5597, 5599, 5598, 734], 's_8_5': [929], 10: [988, 5315, 987], 's_8_10': [5419], 's_8_14': [5208], 15: [5432, 5433, 673, 5223, 672], 's_8_15': [5253], 's_8_16': [763], 's_8_23': [898], 29: [1033], 's_8_29': [5359], 's_8_8': [1002], 12: [493, 5386], 's_13_12': [5341], 's_13_25': [5132], 's_13_13': [5311], 1: [448, 478, 5491, 569, 5492], 's_16_1': [5417], 4: [492, 5087, 491], 's_16_4': [582], 's_16_5': [704], 's_16_14': [5133], 's_16_17': [5177], 's_16_19': [5508], 's_16_20': [5192], 22: [808, 809, 5584, 674, 5583], 's_16_22': [689], 's_16_29': [5374], 's_16_16': [1003], 's_19_3': [568, 5357], 's_19_4': [5026], 's_19_5': [659], 's_19_9': [658], 's_19_15': [732], 's_19_20': [686], 's_19_28': [5552], 's_19_19': [5702], 's_20_3': [477, 5297], 's_20_4': [5252], 's_20_9': [5537, 524], 's_20_11': [581], 's_20_14': [5057], 18: [5449, 5447, 5448], 's_20_18': [538], 's_20_27': [537], 's_20_20': [4982], 's_23_10': [1078], 's_23_11': [5523], 's_23_21': [5401], 's_23_22': [944], 's_23_24': [253], 's_23_28': [5385], 's_23_29': [1048], 's_23_23': [1018], 's_25_11': [445], 's_25_15': [792], 's_25_26': [583], 's_25_28': [238], 's_25_25': [267], 's_26_5': [688], 's_26_9': [703], 's_26_26': [612], 's_27_4': [507], 's_27_10': [972], 's_27_18': [5434], 's_27_27': [942], 's_3_10': [943], 's_3_14': [282], 's_3_24': [208], 's_3_3': [5270], 's_9_15': [5313], 's_9_11': [5509], 's_9_14': [628], 's_9_22': [794], 's_9_9': [553], 's_11_21': [430], 's_11_22': [854], 's_11_11': [790], 's_21_1': [5506], 's_21_5': [509], 's_21_4': [5161], 's_21_14': [5221], 's_21_21': [4951], 's_28_1': [449], 's_28_5': [614], 's_28_24': [5190], 's_28_28': [5520], 's_14_17': [687], 's_14_14': [5235], 's_17_15': [762], 's_17_17': [5164], 's_24_24': [5310], 's_5_1': [5582], 's_5_18': [718], 's_5_22': [719], 's_5_5': [5596], 's_10_18': [973], 's_10_29': [5465], 's_10_10': [5194], 's_15_1': [554], 's_15_15': [5224], 's_29_29': [5420], 's_12_1': [494], 's_12_18': [508], 's_12_12': [5462], 's_1_1': [359], 's_4_4': [5206], 's_22_22': [899], 's_18_18': [5446]}, {0: [2293, 2294, 5548, 5547, 5546], 2: [5383, 5426, 2594, 5427, 5428, 2593], 's_0_2': [2608], 6: [2414, 2504, 5653], 's_0_6': [2489], 7: [5128, 5127, 5276, 5381, 2203, 2202], 's_0_7': [2308], 8: [5202, 5530, 5531, 2427, 2428, 5532], 's_0_8': [2339], 13: [5395, 5607, 5606, 2113, 2114], 's_0_13': [5667, 2264], 16: [5441, 2174, 2173, 2172, 5171, 5172, 5173, 2547], 's_0_16': [5576], 19: [5471, 5470, 2683, 5474, 5473, 2323, 5472], 's_0_19': [2384], 20: [2532, 5578, 5292, 2534, 5293, 2533], 's_0_20': [2669], 23: [5214, 2082, 5215, 2219, 2218, 2217, 5216], 's_0_23': [5487], 25: [1904, 5635, 5637, 5636, 5638, 2129], 's_0_25': [2309], 26: [2159, 2158], 's_0_26': [5652, 5651], 27: [5353, 5351, 2353, 5352], 's_0_27': [5366], 's_0_0': [5322], 3: [5397, 5082, 5097, 2383, 2382], 's_2_3': [5398], 9: [1993, 1933, 5409, 5410, 5413, 5412, 5411], 's_2_9': [2548], 11: [2639, 1887, 1888, 1889, 5724, 5725, 5726, 5727, 5728], 's_2_11': [5669], 's_2_19': [5384], 's_2_20': [2609], 21: [2638, 5459, 5458, 5455, 2263, 5456, 5457], 's_2_21': [5429], 's_2_25': [5623], 's_2_27': [2578], 28: [5545, 5380, 2098, 2096, 2097], 's_2_28': [2128], 's_2_2': [2592], 's_6_13': [5608], 14: [5577, 5187, 2369, 2367, 2368], 's_6_14': [2444, 5698], 17: [5590, 5592, 5591], 's_6_17': [5593], 's_6_20': [5503], 's_6_25': [2474], 's_6_6': [5683], 's_7_3': [2291, 5112], 's_7_14': [5307], 's_7_21': [5396], 24: [5096], 's_7_24': [2246], 's_7_27': [5382], 's_7_28': [5126], 's_7_7': [2112], 's_8_3': [5308], 5: [2144, 5275, 5516, 2067, 2068], 's_8_5': [2189], 10: [5277, 5232, 2307], 's_8_10': [2412], 's_8_14': [2426], 15: [5560, 1964, 5515, 1994], 's_8_15': [1979], 's_8_16': [2248], 's_8_23': [5217], 29: [5262, 2292], 's_8_29': [5247], 's_8_8': [5338, 2457], 12: [2022, 2023], 's_13_12': [5336], 's_13_25': [2324], 's_13_13': [5350], 1: [5170, 2007, 2009, 5425, 2008], 's_16_1': [5440], 4: [2623, 5203, 2622], 's_16_4': [2502], 's_16_5': [5321], 's_16_14': [2472], 's_16_17': [2204], 's_16_19': [2233], 's_16_20': [5188], 22: [5291, 1843, 5290], 's_16_22': [2142], 's_16_29': [2337], 's_16_16': [2636], 's_19_3': [5367], 's_19_4': [2714, 5504], 's_19_5': [2039], 's_19_9': [2338], 's_19_15': [1903], 's_19_20': [2579], 's_19_28': [2053], 's_19_19': [5399], 's_20_3': [5113], 's_20_4': [5218], 's_20_9': [5323, 2518], 's_20_11': [5563], 's_20_14': [2487, 5143], 18: [2232, 5230, 5231], 's_20_18': [2247], 's_20_27': [2442], 's_20_20': [5579], 's_23_10': [5157], 's_23_11': [1872], 's_23_21': [5502], 's_23_22': [1902], 's_23_24': [2187], 's_23_28': [5261], 's_23_29': [5142], 's_23_23': [1782], 's_25_11': [5695], 's_25_15': [1949], 's_25_26': [5666], 's_25_28': [2099], 's_25_25': [5620], 's_26_5': [5501], 's_26_9': [2143], 's_26_26': [2157], 's_27_4': [5368], 's_27_10': [2398], 's_27_18': [5337], 's_27_27': [2188], 's_3_10': [2352], 's_3_14': [2456, 5098], 's_3_24': [5081], 's_3_3': [5083], 's_9_15': [1873], 's_9_11': [5335], 's_9_14': [5517, 2278], 's_9_22': [2038], 's_9_9': [1753], 's_11_21': [5454], 's_11_22': [5320], 's_11_11': [1874], 's_21_1': [1963], 's_21_5': [2083], 's_21_4': [2637], 's_21_14': [5442], 's_21_21': [5489], 's_28_1': [5185], 's_28_5': [5486], 's_28_24': [2081], 's_28_28': [5111], 's_14_17': [2354], 's_14_14': [2366], 's_17_15': [1934], 's_17_17': [2249], 's_24_24': [2111], 's_5_1': [5260], 's_5_18': [1962], 's_5_22': [5274], 's_5_5': [2066], 's_10_18': [5201], 's_10_29': [5186], 's_10_10': [5278], 's_15_1': [5485], 's_15_15': [2024], 's_29_29': [5263], 's_12_1': [5080], 's_12_18': [5245], 's_12_12': [2021], 's_1_1': [5125], 's_4_4': [5339], 's_22_22': [5379], 's_18_18': [5229]}, {0: [1376, 1377, 1378, 1375, 5540, 1259, 5541], 2: [1258, 5315, 5316, 5332, 1167, 5331], 's_0_2': [5361], 6: [1364, 1709, 5588, 5586, 5587], 's_0_6': [1244], 7: [5405, 5420, 1168, 5482, 5481], 's_0_7': [5542, 1454], 8: [1466, 1467, 5196, 5198, 5197], 's_0_8': [4972], 13: [1409, 5646, 5648, 5647], 's_0_13': [1379], 16: [1542, 1346, 5137, 5138, 5046, 1617, 5243], 's_0_16': [4942, 1345], 19: [5122, 5136, 1152, 5121, 1150, 1151], 's_0_19': [5000, 5001, 1330], 20: [5285, 5288, 1407, 1304, 1303, 5286, 5287], 's_0_20': [1362], 23: [1572, 1076, 1078, 1077, 5180, 5181, 5182], 's_0_23': [1079], 25: [1184, 1183, 1182, 1240, 1241, 5106, 1181], 's_0_25': [5511], 26: [1255, 4851], 's_0_26': [1360, 4912], 27: [5390, 5391, 5392], 's_0_27': [1153], 's_0_0': [5539], 3: [1212, 5450, 5451, 5256, 1332, 1333], 's_2_3': [1257], 9: [1285, 1286, 1288, 1287], 's_2_9': [5376], 11: [1196, 5271, 5195, 1197], 's_2_11': [5345], 's_2_19': [5225], 's_2_20': [943], 21: [1166, 5077, 5076, 1093, 1092, 5075], 's_2_21': [5255], 's_2_25': [5466], 's_2_27': [1318], 28: [5270, 1033, 1032, 1031, 4987, 4986, 4985, 4984], 's_2_28': [5240], 's_2_2': [958], 's_6_13': [1229], 14: [1499, 5406, 1497, 1498, 5408, 5407], 's_6_14': [1484], 17: [5543, 1708, 1706, 1707], 's_6_17': [1634], 's_6_20': [1319], 's_6_25': [1199], 's_6_6': [5589], 's_7_3': [1003], 's_7_14': [1393], 's_7_21': [5375], 24: [5465, 1018], 's_7_24': [5480], 's_7_27': [1363], 's_7_28': [1046, 1047, 1048], 's_7_7': [5419], 's_8_3': [5211], 5: [4836, 1391, 1390, 5108, 5107, 1406], 's_8_5': [4927], 10: [1453, 1663, 1557, 5257, 5258], 's_8_10': [1662], 's_8_14': [5212], 15: [5018, 1256, 5017, 5016], 's_8_15': [1632, 1631], 's_8_16': [1317], 's_8_23': [1392], 29: [5183, 1602, 5273], 's_8_29': [5213], 's_8_8': [1752], 12: [1514, 5422, 1513], 's_13_12': [5663], 's_13_25': [5661], 's_13_13': [1559], 1: [1436, 1438, 1437], 's_16_1': [1361, 5062], 4: [5061, 5060, 1138, 1136, 1137], 's_16_4': [5045], 's_16_5': [1452], 's_16_14': [5153], 's_16_17': [5139], 's_16_19': [1211], 's_16_20': [5242], 22: [5030, 5031], 's_16_22': [1316], 's_16_29': [1587], 's_16_16': [5244], 's_19_3': [1227], 's_19_4': [4910], 's_19_5': [4880, 4881, 1315], 's_19_9': [5151], 's_19_15': [4971], 's_19_20': [1242], 's_19_28': [5135], 's_19_19': [4850, 4849], 's_20_3': [5526], 's_20_4': [5301], 's_20_9': [5166], 's_20_11': [1347], 's_20_14': [1633], 18: [5362, 1482, 1483], 's_20_18': [5272], 's_20_27': [1273], 's_20_20': [5284], 's_23_10': [1422], 's_23_11': [1062], 's_23_21': [5330], 's_23_22': [1061], 's_23_24': [1063], 's_23_28': [4970], 's_23_29': [5228], 's_23_23': [5150], 's_25_11': [1122], 's_25_15': [5091], 's_25_26': [4776], 's_25_28': [5105], 's_25_25': [5496], 's_26_5': [4806], 's_26_9': [4926], 's_26_26': [1254], 's_27_4': [1123], 's_27_10': [5393], 's_27_18': [5377], 's_27_27': [1558], 's_3_10': [5317], 's_3_14': [1198], 's_3_24': [5435], 's_3_3': [1289], 's_9_15': [4956], 's_9_11': [5226], 's_9_14': [5421], 's_9_22': [1271], 's_9_9': [4896], 's_11_21': [5210], 's_11_22': [5015], 's_11_11': [5194], 's_21_1': [5167, 1511], 's_21_5': [1302], 's_21_4': [5360], 's_21_14': [5092], 's_21_21': [1016], 's_28_1': [5002], 's_28_5': [1556, 1555], 's_28_24': [5389], 's_28_28': [881, 882], 's_14_17': [5423], 's_14_14': [5498, 1574], 's_17_15': [1691], 's_17_17': [1754], 's_24_24': [988], 's_5_1': [4957], 's_5_18': [5123], 's_5_22': [1331], 's_5_5': [1405], 's_10_18': [5347], 's_10_29': [5303], 's_10_10': [5348], 's_15_1': [5032], 's_15_15': [1646], 's_29_29': [1603], 's_12_1': [5437], 's_12_18': [1423], 's_12_12': [5678], 's_1_1': [5227], 's_4_4': [1139], 's_22_22': [5029], 's_18_18': [5363]}, {0: [385, 384, 4696, 189, 4695], 2: [4590, 4591, 415, 4711, 354], 's_0_2': [219], 6: [204, 4905, 207, 205, 206], 's_0_6': [159, 4710], 7: [293, 294, 4892, 4891, 295], 's_0_7': [4531], 8: [4802, 4803, 371, 370, 4801], 's_0_8': [4846], 13: [99, 4965, 100], 's_0_13': [4680], 16: [507, 5072, 506, 505, 504, 4697, 4698], 's_0_16': [4636], 19: [4666, 431, 430, 429], 's_0_19': [414], 20: [249, 746, 745, 4728, 4725, 4726, 4727], 's_0_20': [144], 23: [640, 4862, 4861, 4863], 's_0_23': [4876], 25: [174, 175, 5011, 176, 5010], 's_0_25': [4620], 26: [129, 130, 4785], 's_0_26': [114], 27: [263, 264, 265, 4953, 4952, 4951], 's_0_27': [4545], 's_0_0': [4560], 3: [565, 4650, 4652, 4651, 534, 4742], 's_2_3': [234], 9: [4770, 552, 551, 4771, 4772, 550], 's_2_9': [4787], 11: [5088, 5087, 5086, 310, 309, 311], 's_2_11': [4606], 's_2_19': [339], 's_2_20': [324], 21: [4966, 4996, 281, 4995, 279, 280], 's_2_21': [278], 's_2_25': [4605], 's_2_27': [4741], 28: [386, 355, 4907, 4906], 's_2_28': [4816], 's_2_2': [113], 's_6_13': [4755], 14: [489, 490, 5131, 222, 221, 4937, 4936], 's_6_14': [5085], 17: [5235, 5237, 5236], 's_6_17': [5220], 's_6_20': [190], 's_6_25': [5115], 's_6_6': [5190], 's_7_3': [566], 's_7_14': [325], 's_7_21': [4800], 24: [520, 4847], 's_7_24': [610], 's_7_27': [4470], 's_7_28': [4921], 's_7_7': [4980], 's_8_3': [624], 5: [161, 669, 670, 160, 4830, 4831, 4832], 's_8_5': [4817], 10: [5012, 4878, 656, 654, 655], 's_8_10': [775], 's_8_14': [372], 15: [5041, 447, 5102, 446], 's_8_15': [5026], 's_8_16': [789], 's_8_23': [715], 29: [760, 759], 's_8_29': [4818], 's_8_8': [834], 12: [5130, 191, 192], 's_13_12': [4950], 's_13_25': [4935], 's_13_13': [115], 1: [5057, 5056, 5055], 's_16_1': [626], 4: [4968, 4967], 's_16_4': [491], 's_16_5': [684], 's_16_14': [4682], 's_16_17': [492], 's_16_19': [5161], 's_16_20': [4712], 22: [5222, 4788, 597, 595, 596], 's_16_22': [5042, 581], 's_16_29': [4683], 's_16_16': [508], 's_19_3': [400, 399], 's_19_4': [445], 's_19_5': [4667], 's_19_9': [5132], 's_19_15': [5147], 's_19_20': [4665], 's_19_28': [4981], 's_19_19': [432], 's_20_3': [609], 's_20_4': [731], 's_20_9': [235], 's_20_11': [4756], 's_20_14': [4938], 18: [5178, 5177, 250, 251, 5175, 5176], 's_20_18': [747], 's_20_27': [248], 's_20_20': [4729], 's_23_10': [700], 's_23_11': [805, 806], 's_23_21': [4997], 's_23_22': [4982], 's_23_24': [535], 's_23_28': [4908], 's_23_29': [730, 4833], 's_23_23': [4864], 's_25_11': [341], 's_25_15': [326], 's_25_26': [4875], 's_25_28': [401], 's_25_25': [173], 's_26_5': [4860], 's_26_9': [40], 's_26_26': [4920], 's_27_4': [671], 's_27_10': [521], 's_27_18': [266], 's_27_27': [262], 's_3_10': [4743], 's_3_14': [4592], 's_3_24': [519], 's_3_3': [579], 's_9_15': [567], 's_9_11': [5027, 641], 's_9_14': [4877], 's_9_22': [5207], 's_9_9': [84], 's_11_21': [4845], 's_11_22': [582], 's_11_11': [777], 's_21_1': [236], 's_21_5': [4815], 's_21_4': [460], 's_21_14': [5116], 's_21_21': [5071], 's_28_1': [416], 's_28_5': [475], 's_28_24': [625], 's_28_28': [356, 357], 's_14_17': [237], 's_14_14': [327], 's_17_15': [402], 's_17_17': [537], 's_24_24': [580], 's_5_1': [146, 5100], 's_5_18': [162], 's_5_22': [4758], 's_5_5': [668], 's_10_18': [5162], 's_10_29': [4713], 's_10_10': [653], 's_15_1': [296], 's_15_15': [5327], 's_29_29': [4594], 's_12_1': [116], 's_12_18': [5160], 's_12_12': [86], 's_1_1': [131, 132], 's_4_4': [716], 's_22_22': [4789], 's_18_18': [791]}, {0: [4504, 4818, 834, 4307, 4308, 832, 833], 2: [712, 4742, 4743, 4458, 713, 714], 's_0_2': [4443], 6: [952, 4399, 817, 982, 4324], 's_0_6': [4444, 923], 7: [682, 684, 683], 's_0_7': [667], 8: [4669, 4773, 895, 4775, 894, 4774], 's_0_8': [4594], 13: [847, 4338, 4340, 4339], 's_0_13': [772], 16: [4517, 4518, 4519, 910, 4520, 909, 908], 's_0_16': [983], 19: [4803, 863, 864, 4833, 4908, 4909, 4802, 865], 's_0_19': [4429], 20: [4248, 4249, 940, 4247, 892, 893, 939, 4549], 's_0_20': [562], 23: [4609, 803, 4651, 4652, 4653, 4610, 729, 4548], 's_0_23': [4623], 25: [4382, 757, 532, 759, 758, 4368, 4367], 's_0_25': [637], 26: [775, 4862, 760, 4863], 's_0_26': [700], 27: [4535, 4684, 4685, 4683, 1104], 's_0_27': [984, 4714], 's_0_0': [547], 3: [1045, 1044, 1043, 4415, 4414, 4413], 's_2_3': [743], 9: [4607, 534, 4849, 4848, 4847, 535], 's_2_9': [730], 11: [415, 414, 412, 413], 's_2_11': [400], 's_2_19': [715], 's_2_20': [848], 21: [4744, 594, 789, 4696, 4697, 4698], 's_2_21': [459], 's_2_25': [802], 's_2_27': [699], 28: [383, 669, 4637, 670, 472, 4636, 4456, 384], 's_2_28': [4638], 's_2_2': [728], 's_6_13': [4325], 14: [4728, 4729, 877, 878, 880, 879], 's_6_14': [4309], 17: [518, 517, 4264, 4263, 4262], 's_6_17': [4250, 996], 's_6_20': [4459], 's_6_25': [773], 's_6_6': [4220], 's_7_3': [652, 4233, 651], 's_7_14': [4713], 's_7_21': [4593], 24: [4442, 668], 's_7_24': [4457], 's_7_27': [4533, 4534], 's_7_28': [4608], 's_7_7': [681], 's_8_3': [4939, 4940], 5: [4756, 4758, 745, 4565, 4757, 4564, 744, 4563], 's_8_5': [654], 10: [1029, 4654], 's_8_10': [1014], 's_8_14': [925], 15: [548, 625, 624, 4487, 623], 's_8_15': [4788], 's_8_16': [4834], 's_8_23': [4772, 444], 29: [1075, 1073, 4760, 1074], 's_8_29': [1030, 4925], 's_8_8': [896], 12: [4383, 4385, 4384], 's_13_12': [1027], 's_13_25': [787], 's_13_13': [1117], 1: [580, 578, 579], 's_16_1': [4502], 4: [820, 818, 819], 's_16_4': [4789], 's_16_5': [924], 's_16_14': [4879], 's_16_17': [4577, 473], 's_16_19': [911], 's_16_20': [4579], 22: [550, 549, 503, 4562], 's_16_22': [458], 's_16_29': [4505], 's_16_16': [1118], 's_19_3': [4910], 's_19_4': [4894], 's_19_5': [746], 's_19_9': [655], 's_19_15': [4907], 's_19_20': [941], 's_19_28': [609, 608, 4578, 638], 's_19_19': [805], 's_20_3': [938], 's_20_4': [4864], 's_20_9': [955], 's_20_11': [4232], 's_20_14': [4819], 18: [4580, 953, 954], 's_20_18': [4369], 's_20_27': [4550], 's_20_20': [922], 's_23_10': [4595], 's_23_11': [504, 4592], 's_23_21': [849], 's_23_22': [4667], 's_23_24': [4503], 's_23_28': [564], 's_23_29': [1059], 's_23_23': [998], 's_25_11': [4397], 's_25_15': [622], 's_25_26': [774], 's_25_28': [4366], 's_25_25': [4188], 's_26_5': [4878], 's_26_9': [790], 's_26_26': [761], 's_27_4': [4699], 's_27_10': [4655], 's_27_18': [1089], 's_27_27': [4686], 's_3_10': [4715], 's_3_14': [4489], 's_3_24': [4428], 's_3_3': [1088], 's_9_15': [4892], 's_9_11': [4787], 's_9_14': [4727], 's_9_22': [4877], 's_9_9': [4937], 's_11_21': [4681], 's_11_22': [4471], 's_11_11': [4217], 's_21_1': [4547], 's_21_5': [489], 's_21_4': [4668], 's_21_14': [804], 's_21_21': [4695], 's_28_1': [4622], 's_28_5': [354], 's_28_24': [4441], 's_28_28': [4546], 's_14_17': [4279], 's_14_14': [4294], 's_17_15': [4532], 's_17_17': [4261], 's_24_24': [607], 's_5_1': [595], 's_5_18': [1028], 's_5_22': [565], 's_5_5': [235], 's_10_18': [4624], 's_10_29': [969], 's_10_10': [999], 's_15_1': [4817], 's_15_15': [4968], 's_29_29': [4460], 's_12_1': [593], 's_12_18': [4400], 's_12_12': [967], 's_1_1': [4832], 's_4_4': [4969], 's_22_22': [4427], 's_18_18': [4474, 1013]}, {0: [1794, 2091, 2092, 4643, 4644, 2093, 4645], 2: [4437, 2228, 4345, 4346, 2227], 's_0_2': [4376], 6: [4720, 1945, 4599, 4600, 1944], 's_0_6': [4719], 7: [1718, 1853, 1763, 4524], 's_0_7': [1764], 8: [1852, 4254, 4256, 1866, 1972, 4255], 's_0_8': [2076], 13: [1899, 2019, 4705], 's_0_13': [4571], 16: [4510, 1825, 1822, 1824, 1823, 4509], 's_0_16': [4764], 19: [4511, 4315, 2079, 4527, 4526, 2077, 2078], 's_0_19': [4495], 20: [4811, 1911, 1912, 4435, 2003, 4810, 2005, 2004], 's_0_20': [2094], 23: [1973, 4239, 1792, 4540, 4539, 1793], 's_0_23': [1839], 25: [2063, 2349, 4602, 4601], 's_0_25': [2124], 26: [4541, 2243], 's_0_26': [4646], 27: [2226, 4181, 1838, 1837, 4210, 2106, 4211], 's_0_27': [4151], 's_0_0': [4628], 3: [4360, 4314, 4448, 4449, 1897], 's_2_3': [1927], 9: [1959, 4630, 4617, 4631, 2259, 2257, 2258], 's_2_9': [4347], 11: [2062, 4466, 4465], 's_2_11': [2303], 's_2_19': [2318], 's_2_20': [4826, 2229], 21: [4405, 1987, 1988, 1990, 1989], 's_2_21': [4301, 4300], 's_2_25': [2348], 's_2_27': [2197], 28: [4587, 2184, 4584, 4585, 4586], 's_2_28': [4556], 's_2_2': [2363], 's_6_13': [1974], 14: [4765, 1867, 1868, 4734, 1869], 's_6_14': [4629], 17: [4749, 4689, 1779], 's_6_17': [4614], 's_6_20': [4885], 's_6_25': [4690, 2034], 's_6_6': [4870], 's_7_3': [4463], 's_7_14': [4420], 's_7_21': [4390], 24: [4493, 1748], 's_7_24': [4554], 's_7_27': [4374], 's_7_28': [1733], 's_7_7': [4569], 's_8_3': [1942], 5: [4479, 4480, 2182, 2183, 4481], 's_8_5': [2167], 10: [1761, 4283, 1777, 4329, 1762], 's_8_10': [1686], 's_8_14': [4344], 15: [4750, 4751, 2137, 2138, 2139], 's_8_15': [2152], 's_8_16': [4269], 's_8_23': [1701], 29: [4209, 1731], 's_8_29': [4149], 's_8_8': [4134], 12: [4674, 4673, 1629], 's_13_12': [1914], 's_13_25': [4707, 4706], 's_13_13': [1900], 1: [1898, 4659, 1855, 4615, 1854], 's_16_1': [4869], 4: [2212, 2213, 2214, 2215, 4841, 4840, 4839], 's_16_4': [4854], 's_16_5': [1808], 's_16_14': [4824], 's_16_17': [1810], 's_16_19': [4450, 2033], 's_16_20': [4299], 22: [2046, 2048, 2047], 's_16_22': [4525], 's_16_29': [4194], 's_16_16': [4508], 's_19_3': [4361], 's_19_4': [2080], 's_19_5': [2198], 's_19_9': [2273], 's_19_15': [4691], 's_19_20': [4675], 's_19_28': [2333], 's_19_19': [2393], 's_20_3': [1928], 's_20_4': [2170], 's_20_9': [2274], 's_20_11': [2123, 4436], 's_20_14': [4795], 18: [4226, 1628, 4224, 4225, 1643, 1642, 4223], 's_20_18': [2002], 's_20_27': [4180], 's_20_20': [1960], 's_23_10': [4389], 's_23_11': [4464], 's_23_21': [4240], 's_23_22': [4555], 's_23_24': [1747], 's_23_28': [1778], 's_23_29': [1716], 's_23_23': [4538], 's_25_11': [2289, 2288], 's_25_15': [2154], 's_25_26': [2169], 's_25_28': [2364], 's_25_25': [4557], 's_26_5': [4496], 's_26_9': [4542], 's_26_26': [4572], 's_27_4': [4212], 's_27_10': [4284], 's_27_18': [1971], 's_27_27': [1836], 's_3_10': [1807], 's_3_14': [4359], 's_3_24': [1673], 's_3_3': [1687], 's_9_15': [2109], 's_9_11': [2272], 's_9_14': [4735, 4736, 4737, 2304], 's_9_22': [4422, 4421], 's_9_9': [4332], 's_11_21': [4375], 's_11_22': [2061], 's_11_11': [4467], 's_21_1': [4780], 's_21_5': [4196, 4195], 's_21_4': [4855], 's_21_14': [4570], 's_21_21': [1986], 's_28_1': [1809], 's_28_5': [1883], 's_28_24': [1688], 's_28_28': [4661], 's_14_17': [1749], 's_14_14': [1870], 's_17_15': [1884], 's_17_17': [1780], 's_24_24': [4492], 's_5_1': [1913], 's_5_18': [4478], 's_5_22': [4241], 's_5_5': [4482], 's_10_18': [1746], 's_10_29': [4118], 's_10_10': [4328], 's_15_1': [1840], 's_15_15': [4766], 's_29_29': [4133], 's_12_1': [4658], 's_12_18': [1644], 's_12_12': [4568], 's_1_1': [4660], 's_4_4': [2290], 's_22_22': [4150], 's_18_18': [4238]}, {0: [5139, 5183, 1559, 1752, 1753, 5393, 5392, 1558], 2: [1347, 1693, 5409, 5408, 5407, 1438, 5317], 's_0_2': [1618], 6: [5587, 1633, 5603, 1634, 5588], 's_0_6': [5513], 7: [5439, 5167, 5168, 1768, 1767], 's_0_7': [1721], 8: [5394, 2098, 1992, 1993, 5395], 's_0_8': [5140], 13: [1482, 1484, 1483], 's_0_13': [5542], 16: [1782, 1783, 1784, 5651, 5650, 1781, 5649], 's_0_16': [5229], 19: [1604, 1332, 5332, 5379, 5378, 1603, 5333], 's_0_19': [5663], 20: [5528, 1706, 1707, 1709, 1708], 's_0_20': [5633], 23: [5272, 5545, 5544, 1873, 1872, 5273, 5274], 's_0_23': [1663], 25: [5290, 1318, 5228, 1557, 5289, 5287, 5288], 's_0_25': [5391], 26: [5063, 1647, 1646], 's_0_26': [5198], 27: [5470, 1918, 2022, 2023, 5469, 5425], 's_0_27': [5468], 's_0_0': [5722], 3: [1573, 5185, 5184, 1827, 5154, 5153, 1572], 's_2_3': [5377], 9: [1662, 1377, 5242, 5245, 5244, 5243], 's_2_9': [1378], 11: [1452, 5557, 5363, 5362, 1454, 1453], 's_2_11': [5482], 's_2_19': [5226], 's_2_20': [5543], 21: [5364, 1799, 1798], 's_2_21': [5484], 's_2_25': [5406], 's_2_27': [1888], 28: [1423, 5258, 5257, 1421, 1422], 's_2_28': [5302, 1303], 's_2_2': [5196], 's_6_13': [1499], 14: [1844, 1977, 5455, 1978, 5453, 5454], 's_6_14': [1649], 17: [5604, 1919, 5605], 's_6_17': [5589], 's_6_20': [1619], 's_6_25': [1632], 's_6_6': [1409], 's_7_3': [1541], 's_7_14': [1814], 's_7_21': [5424], 24: [1602, 5137, 5138], 's_7_24': [1511], 's_7_27': [5440], 's_7_28': [5182], 's_7_7': [5166], 's_8_3': [2007], 5: [1916, 1648, 1917, 5305, 5303, 5304], 's_8_5': [5125], 10: [2068, 2066, 2067], 's_8_10': [5471], 's_8_14': [5380], 15: [1964, 1843, 5320, 1962, 1963], 's_8_15': [5350, 2097, 5200], 's_8_16': [2099], 's_8_23': [1828], 29: [2129, 5530], 's_8_29': [2083], 's_8_8': [5396], 12: [5212, 5214, 5213], 's_13_12': [5197], 's_13_25': [5227], 's_13_13': [5108], 1: [1796, 5259, 1797], 's_16_1': [5034], 4: [1738, 5499], 's_16_4': [1769], 's_16_5': [5169], 's_16_14': [5574], 's_16_17': [1934], 's_16_19': [5648], 's_16_20': [1694], 22: [1736, 5334, 1737], 's_16_22': [5079], 's_16_29': [2114], 's_16_16': [2084], 's_19_3': [5423], 's_19_4': [5498], 's_19_5': [1813], 's_19_9': [5346], 's_19_15': [1858], 's_19_20': [5573], 's_19_28': [5256], 's_19_19': [5241], 's_20_3': [5438], 's_20_4': [1754], 's_20_9': [5078], 's_20_11': [5527], 's_20_14': [5529], 18: [5199, 1857, 5111, 5109, 5110], 's_20_18': [1691], 's_20_27': [1723], 's_20_20': [1705], 's_23_10': [5275], 's_23_11': [1542], 's_23_21': [5634, 1874], 's_23_22': [1678], 's_23_24': [1617], 's_23_28': [1587], 's_23_29': [2024], 's_23_23': [5546], 's_25_11': [5347], 's_25_15': [2008], 's_25_26': [1556], 's_25_28': [1407], 's_25_25': [5421], 's_26_5': [5065, 5064], 's_26_9': [1661], 's_26_26': [1676], 's_27_4': [1664], 's_27_10': [5306], 's_27_18': [5126], 's_27_27': [5156], 's_3_10': [5170], 's_3_14': [5155], 's_3_24': [1497], 's_3_3': [2127], 's_9_15': [1902], 's_9_11': [5361], 's_9_14': [5230], 's_9_22': [5124], 's_9_9': [1362], 's_11_21': [5559, 5558], 's_11_22': [5348], 's_11_11': [5556], 's_21_1': [1887], 's_21_5': [5335, 1948, 1949], 's_21_4': [5514], 's_21_14': [1933], 's_21_21': [5619], 's_28_1': [5092, 5094, 5093], 's_28_5': [1498], 's_28_24': [1392], 's_28_28': [5047], 's_14_17': [2009], 's_14_14': [1976], 's_17_15': [5620], 's_17_17': [5695], 's_24_24': [1361], 's_5_1': [5019], 's_5_18': [1901], 's_5_22': [5318, 5319], 's_5_5': [1932], 's_10_18': [2051], 's_10_29': [2053], 's_10_10': [2065], 's_15_1': [5260], 's_15_15': [5485], 's_29_29': [5531], 's_12_1': [1722], 's_12_18': [1842], 's_12_12': [5211], 's_1_1': [1795], 's_4_4': [1739], 's_22_22': [1735], 's_18_18': [2126]}, {0: [545, 3975, 3976, 3977, 3979, 800, 3978], 2: [3961, 3826, 394, 397, 396, 395], 's_0_2': [275], 6: [3990, 246, 244, 245], 's_0_6': [110], 7: [3886, 322, 321, 3887, 320], 's_0_7': [410], 8: [861, 4098, 4096, 4097], 's_0_8': [4054], 13: [200, 201], 's_0_13': [95, 4035], 16: [562, 3915, 561, 559, 560, 3917, 3916], 's_0_16': [170], 19: [3751, 3752, 4127, 4203, 606, 605, 604], 's_0_19': [3812], 20: [140, 139, 335, 334, 3782, 3780, 3781], 's_0_20': [3960], 23: [4008, 455, 4007, 622, 621, 620], 's_0_23': [785], 25: [3903, 3902, 3901, 367, 366, 3810, 3811, 365], 's_0_25': [770], 26: [830, 829], 's_0_26': [4069], 27: [578, 577, 576, 454, 575, 3827], 's_0_27': [3857], 's_0_0': [905], 3: [4021, 382, 4126, 381], 's_2_3': [4306], 9: [3930, 681, 680, 3931, 3933, 3932], 's_2_9': [425], 11: [3873, 515, 424, 3872], 's_2_11': [3796], 's_2_19': [3962], 's_2_20': [349], 21: [483, 216, 215, 3842, 485, 3841, 484], 's_2_21': [3736], 's_2_25': [4321], 's_2_</t>
+          <t>[3.7486672401428223, 3.2997848987579346, 3.50231671333313, 3.830021619796753, 2.8458261489868164, 5.034237384796143, 5.237394094467163, 4.117889881134033, 4.204772472381592, 3.7167563438415527, 3.503901958465576, 2.615175247192383, 4.641017436981201, 5.309628248214722, 4.511427402496338, 4.201631307601929, 5.135687351226807, 4.481101751327515, 3.056804656982422, 4.003279447555542, 3.446746349334717, 3.7230582237243652, 3.6940524578094482, 3.0889265537261963, 4.297009468078613, 5.627837419509888, 2.6536855697631836, 4.723609685897827, 2.5015830993652344, 4.390609502792358, 6.73119592666626, 6.019072532653809, 1.982302188873291, 3.8369739055633545, 2.6873185634613037, 3.231222629547119, 3.8173375129699707, 3.048194408416748, 6.196512937545776, 4.442905902862549, 3.313537359237671, 3.6383519172668457, 3.5401535034179688, 3.6836256980895996, 2.3695626258850098, 4.154680013656616, 4.107636451721191, 3.720176935195923, 3.315965175628662, 4.45398211479187, 3.2890005111694336, 3.000593662261963, 2.039433002471924, 8.401562452316284, 5.467447757720947, 3.835585594177246, 4.490511894226074, 5.20222806930542, 4.406318664550781, 5.844826698303223, 5.150283336639404, 1.796618938446045, 3.764124870300293, 3.765232801437378, 4.898018836975098, 3.0719804763793945, 5.554632663726807, 5.855252265930176, 4.607200622558594, 3.637012004852295, 2.464157819747925, 3.4758670330047607, 3.590684413909912, 4.565398931503296, 4.689794301986694, 3.883978843688965, 2.1173622608184814, 2.0722708702087402, 6.596177577972412, 2.7360033988952637, 2.788992166519165, 3.4303998947143555, 5.585094690322876, 4.338639974594116, 5.202486276626587, 3.8994200229644775, 3.5459132194519043, 3.234038829803467, 4.9994049072265625, 3.5465917587280273, 4.972442388534546, 3.881234884262085, 4.93268895149231, 3.7092955112457275, 3.1465742588043213, 4.442399740219116, 5.950220823287964, 2.865309715270996, 5.299416780471802, 2.654939651489258]</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>[{0: [1119, 4370, 1118], 2: [4489, 4490], 6: [1268, 4611, 1269], 7: [4550], 8: [4625, 1192, 1193], 13: [4386], 16: [4521, 4520, 1028], 19: [1088], 20: [1163, 4475], 23: [4581, 4580], 25: [4401, 1133], 26: [1147], 27: [1057, 1058], 3: [1089, 1178, 4640], 9: [4445, 1208], 11: [4431, 1223], 21: [4430, 1043], 28: [4355, 1013, 1012], 14: [4536, 4535], 17: [4461, 1238], 24: [4610, 1104], 5: [4416, 4415], 10: [4566, 4565], 15: [4460], 29: [1148], 12: [4385], 1: [1103], 4: [4505], 22: [4551, 1253], 18: [1072, 1073]}, {0: [4124, 4123], 2: [2511, 4184, 4183], 6: [4153, 4259, 2586], 7: [2706, 4064], 8: [4094, 2721, 2722], 13: [2526, 2525], 16: [4108, 2751, 4109], 19: [3989, 2675, 2676], 20: [4169, 2616], 23: [2556, 4049, 2645], 25: [4078, 2496], 26: [2541], 27: [4139, 2781], 3: [2690, 2691], 9: [4168, 4229, 2601], 11: [4138], 21: [2646, 4079], 28: [4093, 2615], 14: [2661, 4214], 17: [2752, 2662, 4334], 24: [4034], 5: [4004, 2600, 4003], 10: [2780, 3974], 15: [4198, 4199], 29: [4019], 12: [3943, 3944], 1: [2630, 2631], 4: [4154], 22: [2571], 18: [2766, 2765]}, {0: [5641, 5640, 5505, 179], 2: [5566, 269, 5565], 6: [5415, 103, 104], 7: [178, 5355], 8: [299, 5611, 5612, 494], 13: [118], 16: [344, 374, 5551], 19: [268, 5536, 5535], 20: [5656, 253, 254], 23: [224, 5492, 5490, 5491], 25: [5431, 194, 5430], 26: [5520, 5521], 27: [313, 314], 3: [5610, 163, 164], 9: [5581, 329], 11: [5580], 21: [239, 328, 5476], 28: [5356, 403, 404], 14: [5550, 5475, 209], 17: [5460, 5461], 24: [463, 5370, 5371], 5: [5477, 449, 448], 10: [5626, 5625, 149], 15: [5462, 5507, 419], 29: [359], 12: [5445], 1: [5446], 4: [5506], 22: [5596, 5595], 18: [5400, 5401, 148]}, {0: [508, 478, 5447], 2: [523, 5477], 6: [328, 5402, 5401], 7: [448, 5492], 8: [5463, 463, 5462], 13: [5446], 16: [5508, 614, 613], 19: [568, 5537, 569], 20: [553, 5417], 23: [509, 5521], 25: [5431, 5433, 5432], 26: [673, 5448], 27: [447, 5313, 5312], 3: [5372, 5371], 9: [539, 5387, 538], 11: [5582, 554], 21: [524, 5522], 28: [404, 5552, 5551], 14: [5493, 628], 17: [5478, 5403, 703], 24: [494, 493], 5: [688, 689], 10: [418, 419], 15: [659, 658], 29: [5507], 12: [373, 374], 1: [5566, 5567], 4: [5418, 643, 642], 22: [5598, 5597], 18: [5357, 5356]}, {0: [1656, 1655, 3895, 3894], 2: [1671, 4044], 6: [3865, 3864], 7: [3983, 3984], 8: [1894, 1895], 13: [1699], 16: [4103, 1880, 4104], 19: [1746, 1745], 20: [4164, 1805, 1806], 23: [3954, 1850], 25: [1685, 1684], 26: [1610, 3998], 27: [1715, 3819, 1714], 3: [1790, 4030, 4029], 9: [1821, 3999], 11: [1851, 4074, 4075], 21: [4045, 1865], 28: [1670, 3880, 3879], 14: [1835, 1836, 4089], 17: [1910, 1909], 24: [1775], 5: [3939, 3938], 10: [3908, 3909], 15: [4060, 4059], 29: [3924, 1879], 12: [3849], 1: [3969, 1729, 1730], 4: [4014], 22: [4000, 1940, 1941], 18: [1820]}, {0: [2081, 5155, 5156], 2: [5305, 2082, 5306], 6: [1842, 1902, 5214], 7: [2143, 5201, 2142], 8: [2126, 5276, 2127], 13: [1932], 16: [2096, 2008, 2007, 5185], 19: [5215, 2112], 20: [2023, 5230, 2022], 23: [2156, 5080, 5081], 25: [5140, 1947], 26: [1962], 27: [5126, 2188, 2187], 3: [5231], 9: [5170, 2052, 2051], 11: [1993, 1992], 21: [5260, 5261, 2157], 28: [2217, 5245, 5246], 14: [2097, 5336, 5335], 17: [1872, 5320], 24: [2202], 5: [2066, 5275, 2067], 10: [2173, 2172], 15: [5200, 5199], 29: [5096], 12: [5290], 1: [1977], 4: [5141], 22: [5095], 18: [5291]}, {0: [5401, 329, 328], 2: [209, 208, 5355], 6: [5580, 5581], 7: [254, 5385, 253], 8: [374, 5476], 13: [419, 5341, 418], 16: [404, 5596, 5595], 19: [5446, 194, 5445], 20: [5536, 179, 5535], 23: [5431, 5492, 448], 25: [164, 5340, 163], 26: [5400], 27: [5566, 5565], 3: [5520, 223, 224], 9: [5460, 5505, 118], 11: [5490, 5491], 21: [313, 314], 28: [5430, 178], 14: [5611, 5506, 344], 17: [5610, 104], 24: [5371, 5370], 5: [5641, 268, 269], 10: [359, 5521], 15: [5475, 103], 29: [5477, 478], 12: [5356, 508], 1: [5415, 403, 5416], 4: [299, 5550], 22: [5462, 239, 5461], 18: [5642, 509]}, {0: [2156, 5095, 5096], 2: [5066, 2202, 2201], 6: [2141], 7: [5050, 5141, 2051], 8: [5127, 2081, 5126], 13: [4991], 16: [5142, 2246, 5186], 19: [5082, 5081], 20: [2187, 5112, 5111], 23: [5201, 5200, 2022], 25: [4976, 2216, 4977], 26: [2217], 27: [2111, 5051], 3: [2096], 9: [2352, 5157], 11: [4962, 2306, 2307], 21: [2157, 5171], 28: [5036, 2172, 2171], 14: [2142, 5156], 17: [2066, 5021, 5020], 24: [2021, 5035], 5: [5231, 2367, 5232], 10: [5170, 2112], 15: [2322, 5022, 2321], 29: [5185], 12: [5005, 5006], 1: [2260, 5097, 2261], 4: [2231], 22: [2292], 18: [2127, 2126]}, {0: [816, 4175, 4174], 2: [4189, 1087, 4190], 6: [4251, 4310, 1117], 7: [4160, 4159], 8: [877, 4235, 4234], 13: [4340, 1132], 16: [4370, 1027, 1026], 19: [4099, 1041], 20: [4055, 1057, 1056], 23: [4280, 937, 4279], 25: [922, 4325, 4324], 26: [876, 4219], 27: [997, 4145, 996], 3: [1011, 1010], 9: [4220], 11: [1072, 1071], 21: [4115, 1146], 28: [4144, 892, 891], 14: [1101, 3995, 1102, 1103], 17: [4250], 24: [4084, 936], 5: [981, 4114], 10: [4294, 1012], 15: [952, 951], 29: [4309], 12: [1042], 1: [4265, 4264], 4: [1086, 4070], 22: [4205], 18: [982, 4385]}, {0: [1274, 5480, 5481], 2: [1152, 1153], 6: [1124, 5435], 7: [1139, 1138], 8: [1303, 5406, 1183], 13: [1259, 5496], 16: [1228, 5315, 5316], 19: [5270, 1109, 1108], 20: [1063, 1182, 5345], 23: [5421, 1198], 25: [5540, 1168], 26: [1094], 27: [1273, 5286], 3: [5256, 5255], 9: [5450, 1003], 11: [5330, 1048, 5420], 21: [1197, 5331], 28: [5376, 5375], 14: [5405, 1123], 17: [1033], 24: [5301, 1288], 5: [1093, 5361, 5360], 10: [5287, 1318], 15: [5465, 5466], 29: [1319, 5451], 12: [1258], 1: [1243], 4: [1167], 22: [5389, 5390], 18: [5346]}, {0: [4010, 1250, 4011], 2: [1086, 4026, 4025], 6: [1235, 3996], 7: [3935, 1191, 1190], 8: [4042, 1370, 3951], 13: [1280, 3981], 16: [1160, 4072, 4071], 19: [4056, 1175], 20: [4041, 1101, 4040], 23: [1340, 4176, 1341], 25: [4131, 1281], 26: [1267, 1266], 27: [3934, 995], 3: [3950, 1221, 1220], 9: [1205, 1206, 4221], 11: [4116, 4115], 21: [4175, 1070, 1071], 28: [1176, 4130, 1056], 14: [4145, 1296, 4146], 17: [1311], 24: [4191], 5: [4086, 4085], 10: [1310, 3965, 3966], 15: [4101, 1251], 29: [1325], 12: [3980], 1: [1145, 4100], 4: [4070, 4055], 22: [1236], 18: [4084, 1010]}, {0: [2713, 5278, 5279], 2: [2668, 5339], 6: [5308, 2548], 7: [5294, 2728, 5399], 8: [2623, 2622], 13: [2487], 16: [2638, 2637, 5203], 19: [5234, 2683, 2682], 20: [5414, 2518, 5413], 23: [2563, 5309], 25: [5263, 2607], 26: [5352, 2457], 27: [2653, 5324], 3: [2698, 5474], 9: [2817, 5353, 5354], 11: [5368], 21: [2577, 2578], 28: [5264, 2667], 14: [2608, 2533, 5398], 17: [2532, 2547], 24: [2697], 5: [5249, 5248], 10: [2593, 5383], 15: [5218, 5219], 29: [5533, 2564], 12: [5233], 1: [5144, 2562], 4: [5428, 5429], 22: [2592], 18: [5323, 2502, 2503]}, {0: [1335, 3051], 2: [1275, 1276], 6: [3142], 7: [3127, 3126], 8: [3021, 1396, 1395], 13: [3067, 1380], 16: [3035, 1320, 3036], 19: [1260, 1261], 20: [1306, 3111], 23: [3050, 2977, 2976, 1215], 25: [3231, 1350, 1351], 26: [3276, 1336], 27: [2991, 1230], 3: [1245, 3096], 9: [1231, 3201], 11: [3230, 3246, 1216], 21: [1140, 3171], 28: [1410, 1411, 3261, 3262], 14: [3172, 1291], 17: [3037, 1456, 1455], 24: [3097, 1425], 5: [3186, 1201, 3185], 10: [3005, 3006], 15: [3217, 3216], 29: [1290], 12: [3066], 1: [3215, 1185, 1186], 4: [3081, 3156, 1170], 22: [3200, 1065, 1066], 18: [1200]}, {0: [3476, 3400, 2087], 2: [3507, 2072, 3506], 6: [1952], 7: [2193, 3566], 8: [3430, 2177, 3431], 13: [1967], 16: [2148, 2146, 2147], 19: [2028, 3311, 2027], 20: [3490, 2013, 3491], 23: [2117, 3342, 3341], 25: [3416, 3415], 26: [1997], 27: [1968, 3565], 3: [3521, 2178], 9: [2102, 3370], 11: [3492, 2282, 3371], 21: [2163, 2162], 28: [3312, 2207, 2208], 14: [1892, 3461, 3460], 17: [3445, 3446], 24: [2118, 3626], 5: [1982, 3280, 3281], 10: [2056, 2057], 15: [2012], 29: [2116, 3326], 12: [1966], 1: [3296, 3295], 4: [3536, 3535], 22: [3386, 3385], 18: [3250, 2042, 2041]}, {0: [3854, 2644], 2: [2629, 3928], 6: [2645, 3988, 3989], 7: [2614, 2613], 8: [2688, 2689], 13: [2570], 16: [3748, 2674, 3749], 19: [3929, 2704, 2705], 20: [2540, 2539, 3734, 3733], 23: [3718, 2719, 3719], 25: [2555, 3823], 26: [2599], 27: [2628, 3704], 3: [3764, 2569, 3763], 9: [3914, 3913], 11: [2510, 2509], 21: [3793, 3794], 28: [3809, 2464, 3808], 14: [3824, 2734, 2735], 17: [2675, 3974], 24: [2554, 3689], 5: [3839, 2434, 3838], 10: [3674], 15: [2720, 3869], 29: [3644, 2673], 12: [3884], 1: [2659, 2660], 4: [2749, 3659, 2778], 22: [2495, 2494], 18: [2584, 2583]}, {0: [2743, 5279, 5278], 2: [2668, 5429], 6: [2729, 5369, 2728], 7: [2563], 8: [5263, 2457], 13: [5234, 2757, 2758], 16: [2607, 2608], 19: [5533, 2637, 2638], 20: [5413, 5414], 23: [5339, 2592], 25: [2788, 5399], 26: [5354, 2683], 27: [2502, 5428, 2503], 3: [5353, 2548], 9: [2623, 5444], 11: [2697, 2698], 21: [2564, 2653, 5489], 28: [2713, 5383, 5384], 14: [5474, 2578, 2579], 17: [5368], 24: [5308, 5309], 5: [5323, 5324], 10: [5338], 15: [2533, 5398], 29: [5248, 2442], 12: [2517, 5233], 1: [5458, 2518], 4: [2593], 22: [2622, 5294], 18: [2472, 2473]}, {0: [5529, 5530], 2: [5544, 1844], 6: [2098, 2099], 7: [1964, 5635], 8: [5365, 2114, 2113], 13: [2083], 16: [1978, 1979, 5665], 19: [5454, 2039, 5455], 20: [5559, 1994, 5560], 23: [2053, 5379, 5380], 25: [5470, 2068, 5471], 26: [1873], 27: [1934], 3: [5545, 2024], 9: [5485, 2009], 11: [5439, 5440], 21: [1919, 1918], 28: [1904, 1903], 14: [5606, 5605], 17: [5666, 2084], 24: [5501, 5500], 5: [5515, 5516], 10: [1933, 2023, 5410], 15: [5575, 2069], 29: [1963], 12: [2143, 5426], 1: [5620, 5621, 2144], 4: [5590], 22: [1889, 1888], 18: [5425, 1949, 1948]}, {0: [4055, 756, 4054], 2: [830, 3994], 6: [696, 4128], 7: [1041, 4070], 8: [936, 935], 13: [785, 786], 16: [816, 3979, 815], 19: [4039, 906], 20: [845, 4219, 846], 23: [3934, 1010], 25: [771, 4083], 26: [4158], 27: [921, 920, 4069], 3: [965, 4009], 9: [3993, 800, 801], 11: [4025, 4024], 21: [981, 980], 28: [951, 4084], 14: [4099, 4098], 17: [741, 4113], 24: [4010, 995], 5: [861, 4159], 10: [890, 3949], 15: [4144, 4143], 29: [950], 12: [4174, 4173], 1: [4189, 876], 4: [905, 3964], 22: [3933, 860], 18: [891]}, {0: [4746, 1120], 2: [1254, 4611], 6: [4730, 4731], 7: [4670, 1179], 8: [4836, 1105, 4835], 13: [4656, 1239], 16: [1225, 4777, 4776], 19: [1194, 4701], 20: [1224, 4596], 23: [1210, 4805], 25: [1285, 1284], 26: [4866, 4865], 27: [4640, 1119], 3: [4760, 4761], 9: [1345, 1344, 4686], 11: [4806, 1269, 1270], 21: [4551, 1209, 1208], 28: [1255, 4792, 4791], 14: [4716, 4715, 1135], 17: [1329], 24: [1164], 5: [1314, 1315], 10: [1060, 1059], 15: [4821, 4820], 29: [4850], 12: [4641], 1: [1299, 1300], 4: [4655, 1149], 22: [4881], 18: [4626, 4625]}, {0: [1218, 3754, 3755, 1219], 2: [3724, 1038, 1039], 6: [3575, 1068], 7: [3739, 1024, 3845], 8: [1099, 3770, 1204], 13: [3665, 3666], 16: [1174, 1173, 3740], 19: [1084, 3725], 20: [3815, 1069], 23: [1143, 1144], 25: [949, 3680], 26: [3786, 1279, 3681], 27: [3860, 3861], 3: [3695, 978], 9: [1009, 3800, 3801], 11: [3830, 3769, 994], 21: [3635, 993], 28: [3784, 3785], 14: [1053, 1054], 17: [3621, 3620], 24: [3920, 3919, 979], 5: [3876, 1129, 1130], 10: [3696, 1234], 15: [3650, 1008], 29: [3846], 12: [1188], 1: [3711, 1114], 4: [1159, 1158], 22: [3890, 3891], 18: [3816, 1189]}, {0: [3269, 2506, 3268], 2: [3299, 3298], 6: [2596, 3223], 7: [2701, 3284, 2702], 8: [2536, 3343, 2537], 13: [3222, 2446], 16: [2551, 2552, 3388], 19: [3163, 2671, 3164], 20: [2625, 2626], 23: [2507, 3434, 3433], 25: [3328, 2491], 26: [3238], 27: [3254, 2656], 3: [2717, 3313, 3314], 9: [2611, 2610], 11: [3359, 2431, 3358], 21: [3404, 2567, 3403], 28: [3193, 2642, 2641], 14: [3344], 17: [2581], 24: [3449], 5: [2522, 2521], 10: [3253, 2477, 2476], 15: [2580, 3208], 29: [3387, 2462], 12: [2445], 1: [2566, 3118], 4: [3329], 22: [3373, 3372], 18: [3178, 3179]}, {0: [2584, 4018, 2585], 2: [2480, 4003], 6: [2465, 2466], 7: [2555, 3958], 8: [3988, 3989], 13: [2556, 4153], 16: [3943, 2630], 19: [2496, 2495], 20: [2510, 4048], 23: [2661, 4019, 2660], 25: [4168, 2526], 26: [2541], 27: [3898, 3899], 3: [3974, 3973], 9: [2434, 4063, 2435], 11: [2721, 4033, 4034], 21: [4004, 2645], 28: [2600, 4108], 14: [3913, 2540, 3883], 17: [2390, 3942], 24: [3959, 4109, 2780], 5: [4093, 2615], 10: [2675], 15: [4078, 2450], 29: [3884, 2570], 12: [2571], 1: [4079, 2646], 4: [3928, 2525], 22: [4064], 18: [2690, 4049]}, {0: [1541, 5094, 5093], 2: [5124, 5123], 6: [1571, 5078], 7: [1735, 1736], 8: [1707, 1705, 1706], 13: [1601], 16: [1691, 5153, 5154], 19: [5184, 1827], 20: [5079, 1721], 23: [5003, 1632, 1631], 25: [5108, 1556], 26: [5182], 27: [5049, 1796], 3: [1751, 5109], 9: [5183, 1616, 1617], 11: [5018, 1511, 5017], 21: [1662, 4929, 1661], 28: [1647, 5169, 5168], 14: [5064, 5063], 17: [1586, 1587], 24: [1646, 4988], 5: [1572, 5229, 5228], 10: [4959, 4958], 15: [1557, 5244, 5243], 29: [1690], 12: [4974, 4973], 1: [1812, 1811], 4: [1797, 5139], 22: [5138], 18: [1782, 1781]}, {0: [4728, 4863, 760], 2: [655, 654], 6: [4593, 684, 4637], 7: [4818, 4774, 804], 8: [4802, 4803], 13: [700, 699], 16: [640, 564, 4847, 565], 19: [670, 4832], 20: [4742, 669, 4743], 23: [774, 775], 25: [4712, 4713], 26: [4727], 27: [4759, 4758], 3: [624, 4773], 9: [4817, 609], 11: [789, 4683, 4682], 21: [4653, 4652], 28: [4878, 4877, 745], 14: [834, 4667, 4668], 17: [549], 24: [4833, 715], 5: [519, 520], 10: [4789, 730, 4788], 15: [550], 29: [850, 4848], 12: [625, 4938], 1: [534, 535, 4862], 4: [579, 580], 22: [4697, 4698], 18: [4907, 596, 595]}, {0: [168, 3390, 167], 2: [198, 3450], 6: [3570, 153], 7: [3585, 318], 8: [422, 3435, 3436], 13: [3540], 16: [3465, 3466], 19: [212, 213], 20: [243, 242, 3420], 23: [303, 302], 25: [228, 227], 26: [3405], 27: [272, 3526, 3525], 3: [423, 3615, 3616], 9: [256, 197, 3360], 11: [3481, 257], 21: [3556, 3555], 28: [3600, 3601], 14: [182, 183], 17: [152, 3345], 24: [273, 3676], 5: [288, 287, 3496], 10: [408, 3451], 15: [377, 3346], 29: [3331, 347], 12: [333, 3541], 1: [378], 4: [363, 3511], 22: [317], 18: [3421, 332]}, {0: [5555, 5554, 944], 2: [5524, 1033, 1034], 6: [974, 5660], 7: [5419, 943], 8: [5511, 5510], 13: [1064], 16: [5374, 1019, 1018], 19: [5569, 1004, 5630], 20: [5599, 5600], 23: [1063, 1094, 5465], 25: [5661, 1214, 5525], 26: [1109], 27: [838, 884, 5494], 3: [959, 958], 9: [1124, 5585], 11: [1139, 5435], 21: [1048, 5389], 28: [1079, 1078, 5420], 14: [988, 5584, 989], 17: [5705, 5704], 24: [5315], 5: [5480, 1003], 10: [5495], 15: [1169, 1168], 29: [973], 12: [5540, 1153], 1: [5405], 4: [898, 899], 22: [5450], 18: [5539, 1049]}, {0: [704, 5538, 793], 2: [822, 824, 823], 6: [807, 809, 808], 7: [733, 734], 8: [5644, 659, 5643], 13: [792, 5314], 16: [643, 644, 5659, 5658], 19: [5509, 5508], 20: [5553, 869], 23: [674, 5448, 673], 25: [778, 5372, 5373], 26: [838], 27: [5568], 3: [5388, 719, 718], 9: [898, 779, 5464], 11: [868, 5449], 21: [853, 5328, 5329], 28: [763, 5523, 764], 14: [748, 5583, 749], 17: [5433], 24: [5357, 5358], 5: [883, 5494, 884], 10: [794, 5598], 15: [5463, 658], 29: [5628], 12: [913], 1: [5403, 5404], 4: [854], 22: [5419, 5418], 18: [5569, 5599, 914]}, {0: [5120, 5014, 5013, 1031], 2: [820, 821], 6: [957], 7: [4970, 956], 8: [776, 806, 5043], 13: [5193, 1032, 5194], 16: [5134, 5119, 762], 19: [896, 5059], 20: [5075, 851, 5074], 23: [835, 4998, 716], 25: [791, 5224, 5163, 867], 26: [942], 27: [4955, 4954], 3: [911, 4969], 9: [5089], 11: [5028, 866], 21: [5044, 836], 28: [927, 926, 4894], 14: [5149, 5150, 5029, 986], 17: [5135], 24: [4909], 5: [777, 5105, 5104], 10: [805, 4924, 4925], 15: [971, 5178, 5179], 29: [761], 12: [5240], 1: [837, 912, 5239], 4: [881], 22: [701, 5088], 18: [1091, 1092]}, {0: [2491, 3164, 3163], 2: [2461, 2460], 6: [2551], 7: [3102, 2371], 8: [2983, 2506, 2505], 13: [2581, 3253], 16: [3087, 3088, 2580], 19: [3057, 2400], 20: [2445, 3118], 23: [3208, 2521], 25: [3237, 3238], 26: [2595, 2596], 27: [2415, 3042, 2370], 3: [2386, 3133], 9: [2610, 3179, 3178], 11: [2536, 3268], 21: [3147, 3148], 28: [2310, 3207, 2311], 14: [2490, 3104, 3103], 17: [2550, 3013], 24: [3223, 3222], 5: [2295, 3072, 3073], 10: [3192, 3193], 15: [2476, 3012, 2475], 29: [3043, 2625], 12: [2326, 3252], 1: [2325], 4: [2430], 22: [2566, 2565], 18: [3117, 2356]}, {0: [2769, 4723, 4724], 2: [2498, 4753, 2499], 6: [4739, 2679], 7: [2529, 2530], 8: [2439, 4603, 2438], 13: [2724, 2725], 16: [2694, 4618, 4619], 19: [2664, 4633], 20: [4678, 4679], 23: [2514, 4528, 2513], 25: [4769, 2469, 4768], 26: [2709, 2710], 27: [2604, 4663], 3: [2545, 2544], 9: [2589, 4754], 11: [2619, 4483, 2618], 21: [4558, 4559], 28: [4648, 4647], 14: [2739, 4693, 4694], 17: [4709], 24: [2394, 4573], 5: [4588, 2633, 4589], 10: [4708], 15: [2649, 4604], 29: [2483, 2484], 12: [4574], 1: [2603], 4: [2559], 22: [2588], 18: [2574]}, {0: [1515, 3308, 1516], 2: [3323, 3322], 6: [1576], 7: [1500, 3097], 8: [1545, 1546], 13: [1622, 3293], 16: [1456, 3232], 19: [3247, 1426], 20: [3263, 1396, 3262], 23: [3142, 3143], 25: [3187, 1606, 3188], 26: [3307, 1411], 27: [1591, 3173], 3: [3382, 1486, 1487], 9: [1381], 11: [3186, 1292, 1291], 21: [1350, 3352, 1351], 28: [1472, 1471], 14: [3202, 3201], 17: [1561], 24: [3128], 5: [3216, 3217], 10: [1621, 3158], 15: [3278, 3277], 29: [1531, 1530], 12: [1637], 1: [1501, 3353], 4: [3172], 22: [3231, 1306], 18: [3218, 1636]}, {0: [3714, 3715], 2: [3728, 3578, 1713], 6: [1908, 3744], 7: [3669, 1804], 8: [3593, 1759, 1758], 13: [1984, 3655], 16: [3774, 3773, 1669], 19: [1773, 1774, 3699], 20: [1728, 3743], 23: [1789, 3804], 25: [1893, 3579], 26: [3700], 27: [1654], 3: [1743, 1744], 9: [1878, 3609], 11: [3624, 1788], 21: [1819, 3654], 28: [1924, 3729], 14: [3638, 3640, 3639], 17: [1938, 1939], 24: [3758, 3759], 5: [3819, 1834, 1835], 10: [1655, 3864], 15: [1848, 3594], 29: [1714, 3849], 12: [3790, 1999], 1: [3685, 1849], 4: [3684], 22: [1864, 1863], 18: [3788, 1729, 3789]}, {0: [425, 4037], 2: [4157, 546], 6: [4022], 7: [4053, 4038, 620], 8: [411], 13: [3962, 530], 16: [4067, 4066], 19: [471, 470], 20: [456, 455], 23: [381, 4097, 4096], 25: [500, 501], 26: [4217, 426], 27: [545, 3947, 3946], 3: [4007, 4006], 9: [547, 441, 4202], 11: [4126, 4127], 21: [4082, 531], 28: [3992, 591], 14: [440, 4052], 17: [485, 486], 24: [605], 5: [351, 4112, 4111], 10: [335, 3991], 15: [4142, 4141], 29: [396], 12: [3932], 1: [561, 560], 4: [365, 4081, 366], 22: [516], 18: [3931, 350]}, {0: [3288, 3287], 2: [3423, 691, 692], 6: [3182, 3183, 781, 780], 7: [797, 796], 8: [3437, 541, 542], 13: [451, 571, 3242], 16: [722, 3272, 3273], 19: [752, 751], 20: [3319, 767, 3349], 23: [556, 646, 3212], 25: [600, 3333, 601], 26: [616], 27: [3408, 737], 3: [857, 3438, 3439], 9: [3378, 3377, 587], 11: [3318], 21: [3468, 661, 662], 28: [3138, 721, 3243], 14: [3362, 3363], 17: [811, 3274, 841], 24: [856, 3213], 5: [3228, 631, 3227], 10: [572, 647, 3407], 15: [586, 3198, 3197], 29: [557], 12: [496, 497], 1: [3167, 676, 3168], 4: [3393, 707], 22: [3303], 18: [3347, 3348]}, {0: [4992, 2485, 2486], 2: [4902, 2546, 4903], 6: [4842], 7: [4948], 8: [4887, 2410], 13: [4827, 2350], 16: [2366, 4917], 19: [2395, 2396], 20: [4962, 4963, 2455], 23: [4873, 4872], 25: [2470], 26: [2471], 27: [4947, 2351], 3: [4933], 9: [2321, 5007, 5008], 11: [2605, 4888], 21: [2531, 4753, 2530], 28: [2516, 4783, 2515], 14: [2424, 2425], 17: [2365, 4722], 24: [2500], 5: [4977, 4978], 10: [2275, 4932], 15: [4812, 2320], 29: [2305], 12: [4857], 1: [2381, 2380], 4: [2456, 5023, 5022], 22: [4918, 2440], 18: [4856, 2260]}, {0: [1302, 1301, 4896], 2: [5107, 5106], 6: [1271], 7: [1182, 5241], 8: [1376, 5181], 13: [5046], 16: [5031], 19: [1331, 1330], 20: [1392, 4986, 1391], 23: [1452, 5077, 5076], 25: [4957, 1211, 4956], 26: [1345], 27: [1317, 5122], 3: [5166, 1272], 9: [1436, 4972], 11: [5062, 1421], 21: [5061, 1181], 28: [5091, 1287], 14: [1242, 4971, 1241], 17: [1286], 24: [5227, 5226], 5: [1346, 5016], 10: [5136, 5137], 15: [5001, 1375], 29: [1361], 12: [1196], 1: [1256, 5121], 4: [1316, 4911], 22: [1406], 18: [5151, 5152]}, {0: [4370, 1222, 4371], 2: [1089, 4505, 1088], 6: [1177, 4445], 7: [4430, 4369, 953], 8: [4355, 1057], 13: [4295], 16: [1133, 4520], 19: [4535, 1072, 1073], 20: [4444, 1027, 1028], 23: [1148, 1147], 25: [4459, 1192, 4460], 26: [1223], 27: [1012, 4415], 3: [998, 997], 9: [4566, 4565], 11: [4550, 1043], 21: [4490, 4489], 28: [4400, 4401], 14: [4580, 1058], 17: [4521, 1178, 4581], 24: [4386, 4385], 5: [1103, 4475], 10: [4340], 15: [4280, 1208, 1207], 29: [4416, 1162], 12: [1132], 1: [1118, 1117], 4: [4474, 1013], 22: [1163], 18: [1102, 4325]}, {0: [5082, 2426, 2425], 2: [2261, 5052], 6: [5127, 5202, 2352], 7: [4871, 4872], 8: [5006, 5007], 13: [2441, 5187], 16: [2410, 2411, 5036, 5037], 19: [4902, 2381], 20: [2351, 5022], 23: [2471, 4962, 4963], 25: [5097, 2382], 26: [2291], 27: [4857, 2396, 2395], 3: [2365, 2366], 9: [5066, 5067], 11: [2321, 4977], 21: [2260], 28: [2335, 2336], 14: [4947, 2231, 2230], 17: [2246, 5112], 24: [2275, 4887], 5: [2201, 2290, 4932], 10: [4992], 15: [2305, 2306], 29: [2486], 12: [2440], 1: [4841, 4842], 4: [4917], 22: [2216], 18: [2456, 4933, 2455]}, {0: [5503, 5502, 2278], 2: [5532, 5531], 6: [5473, 5472], 7: [5381, 5382], 8: [2413, 2412], 13: [2219, 2218], 16: [5411, 5412], 19: [2339, 2338], 20: [2383, 2384, 5547], 23: [2204, 5308, 5307, 2203], 25: [5487, 2263], 26: [2324, 5517], 27: [5428, 2474, 2473], 3: [5397, 2428], 9: [2369, 2294, 5607], 11: [5546], 21: [5426, 2174, 2173], 28: [5322, 2354, 2353], 14: [5442, 2233, 5441], 17: [2293], 24: [2368], 5: [5366, 2323, 5367], 10: [2427, 5323], 15: [5457], 29: [5262, 2398], 12: [5351], 1: [5396, 2308], 4: [5427], 22: [5576, 2158, 2159], 18: [5352]}, {0: [2577, 2502, 5248], 2: [5428, 2487, 2488], 6: [5098], 7: [2667, 5188], 8: [5339, 5338, 2442], 13: [5084, 5083], 16: [5309, 5308], 19: [2563, 2562], 20: [5173, 2548, 2547], 23: [2533, 5293, 5294], 25: [2456, 2457, 5323], 26: [2503], 27: [5143, 2532], 3: [5218, 5217], 9: [5383, 2593], 11: [2518, 5353], 21: [5233, 2622, 5234], 28: [2697, 5278, 5279], 14: [2591, 2592], 17: [2607, 2606], 24: [2517], 5: [2636, 5368, 2637], 10: [2382, 2383], 15: [2653, 5324], 29: [2398], 12: [2727], 1: [2728, 5264], 4: [5263, 2472], 22: [2578], 18: [5113, 5114]}, {0: [5235, 222], 2: [252, 251], 6: [177, 5145], 7: [5220, 131, 132], 8: [5085, 311, 5086], 13: [5265, 162], 16: [192, 191, 4890], 19: [5131, 5130], 20: [42, 5116, 5115], 23: [221, 5025], 25: [312, 5175], 26: [5146], 27: [161, 5070], 3: [5055, 101], 9: [5010, 296], 11: [5190, 326, 327], 21: [250, 4950, 4951], 28: [265, 267, 266], 14: [206, 207], 17: [5160], 24: [5040], 5: [5101, 236, 237], 10: [176], 15: [280, 281], 29: [4980], 12: [146, 147], 1: [4965, 4966], 4: [115, 116], 22: [295, 4995], 18: [5100]}, {0: [3496, 542, 543, 3497], 2: [421, 3317], 6: [3481, 347], 7: [3332], 8: [482, 3467], 13: [378], 16: [3407, 377, 3406], 19: [362, 3287, 3286], 20: [3362, 451, 3361], 23: [3422, 3421], 25: [3451, 422], 26: [331, 332], 27: [3452, 526, 527], 3: [557, 3347], 9: [436, 3271], 11: [3436, 407], 21: [392], 28: [496, 3482, 497], 14: [466, 3376], 17: [3375, 256, 3346], 24: [512], 5: [3391], 10: [3437], 15: [3466, 286, 287], 29: [617], 12: [3556], 1: [467, 3527, 393], 4: [572, 3302, 3303], 22: [437], 18: [452]}, {0: [2153, 2151, 2152], 2: [2168, 2167, 4346], 6: [4197, 4196, 2197], 7: [4376, 2122], 8: [4315, 2272, 4316], 13: [4226, 2136], 16: [4332, 4331], 19: [2288, 4286, 2287], 20: [4271, 2302], 23: [4450, 4451], 25: [2137, 2198, 4361], 26: [4526], 27: [4257, 4256], 3: [4241, 2182], 9: [2213, 2212], 11: [2303, 4466], 21: [2227], 28: [4512, 2123, 4511], 14: [2107, 4300, 4301], 17: [4302, 2362], 24: [2183], 5: [2243, 2241, 2242], 10: [2091, 2092], 15: [2363, 4407], 29: [2077], 12: [4227], 1: [2347, 4422, 2348], 4: [2317, 4392], 22: [4437, 2257], 18: [4151, 2226]}, {0: [3687, 3686], 2: [3716, 2179], 6: [2133, 3536], 7: [2238, 3611], 8: [3522, 2194, 2193], 13: [2118], 16: [3672, 2344], 19: [2253, 3776, 2254], 20: [2149, 3671, 2148], 23: [3806, 2209], 25: [3641, 2359, 3642], 26: [2313, 3612], 27: [2088], 3: [3566, 2164, 2163], 9: [3761, 2298, 2299], 11: [3791, 3792], 21: [3717, 2284], 28: [3732, 3731], 14: [2283, 3596], 17: [2343, 3537], 24: [3746], 5: [3852, 2329, 3657, 2328], 10: [2208, 3626], 15: [3627, 2358], 29: [2223, 3656], 12: [3580], 1: [3581, 2268], 4: [3701, 3702], 22: [3807], 18: [3851, 2073, 2074]}, {0: [1426, 1427], 2: [3322, 1307, 3441], 6: [1381, 3172], 7: [3487, 1337, 1336], 8: [1547, 3411, 3412], 13: [1411], 16: [1501, 3397, 1502], 19: [3427, 3426], 20: [1382, 3353, 3352], 23: [3502, 3503], 25: [3276, 3277], 26: [3457, 1397, 1396], 27: [3338, 3337], 3: [1292, 3366], 9: [3442], 11: [1457, 1458], 21: [1577, 3381, 3382], 28: [1321, 1322, 3532], 14: [3307, 1442], 17: [1441, 3247], 24: [1293], 5: [1352, 3262, 1351], 10: [3367, 1562], 15: [1366, 1367], 29: [3488], 12: [3217], 1: [1546, 3231, 3232], 4: [1472], 22: [3472, 1412], 18: [1516]}, {0: [3756, 3755], 2: [1248, 3861, 1249], 6: [3876, 1129, 1130], 7: [1099, 3605, 1098], 8: [3680, 1114, 3681], 13: [1189], 16: [3726, 1054, 3725], 19: [3711, 1219], 20: [1204, 3770], 23: [1279, 3651, 1203], 25: [3621, 1173, 1174], 26: [1339, 1338], 27: [1159, 1158], 3: [1144, 1143], 9: [3801], 11: [1309, 3786], 21: [3740, 3741], 28: [1218, 3606], 14: [1069, 3800], 17: [3815], 24: [3575], 5: [1188, 3636], 10: [3650], 15: [1233, 1234, 3816], 29: [3545, 1053], 12: [3921, 1085, 3920], 1: [1323, 1324], 4: [3696, 1264], 22: [1294], 18: [1084, 3635]}, {0: [3495, 198], 2: [3600, 3601], 6: [3540, 242], 7: [3585], 8: [243, 3616, 3615], 13: [3496], 16: [167, 168], 19: [393, 3465, 3466], 20: [3525, 183], 23: [3720, 199], 25: [3510, 378, 3511], 26: [3480, 3481], 27: [213, 3555], 3: [228, 3570], 9: [92, 93], 11: [3645, 138], 21: [257, 258], 28: [287, 288], 14: [3630, 153], 17: [152, 3420], 24: [273], 5: [303, 302, 3390], 10: [319, 318], 15: [108, 107], 29: [169, 3735], 12: [272], 1: [3435, 3436], 4: [3450], 22: [3661, 3660], 18: [3526]}, {0: [5383, 2773, 5384], 2: [5414, 5413], 6: [2563], 7: [2608, 5474], 8: [2744, 5444], 13: [2578], 16: [2714, 2713, 5369], 19: [5458, 2503, 5368], 20: [2564, 2683, 5489], 23: [5534], 25: [2548, 5398], 26: [2533], 27: [2623], 3: [2654, 2653], 9: [5428, 5429], 11: [5399, 2788], 21: [2728, 2729], 28: [2699, 2593, 5504], 14: [2698, 5324], 17: [5339], 24: [5533], 5: [5609, 5608, 2534], 10: [2684, 2638, 5519], 15: [2669, 2668], 29: [5549], 12: [2579], 1: [5579, 5578], 4: [5459], 22: [2758, 2759], 18: [5548]}, {0: [2490, 2371, 3148], 2: [2551, 3118], 6: [2446, 2445], 7: [3133, 3134], 8: [2520, 2998], 13: [3222], 16: [2476, 2475], 19: [2580, 3088], 20: [3208, 3207], 23: [2656, 3013, 2655], 25: [3237, 3238], 26: [2386], 27: [2400, 3117], 3: [3058, 2595], 9: [2505, 3163, 2506], 11: [3223, 2641], 21: [2535, 2536], 28: [3164, 2566], 14: [3073, 2430], 17: [3057], 24: [2625, 3179], 5: [2521, 3102, 3103], 10: [3042, 3043], 15: [2461, 2460], 29: [3012, 2385], 12: [2416], 1: [3267, 3268], 4: [3192, 3193], 22: [3253, 3254], 18: [2415]}, {0: [2845, 4993, 4994, 2846], 2: [2770, 4904], 6: [4813, 4814], 7: [2605, 4964], 8: [5068, 2545, 2546], 13: [2831, 2830], 16: [5024, 5023], 19: [2666, 2665], 20: [2740, 4919, 2741], 23: [5008, 2590], 25: [2725, 4859], 26: [4829], 27: [2711], 3: [4873, 2620, 4874], 9: [2680, 4934], 11: [4888, 4889], 21: [4949, 2651, 2650], 28: [4844, 4843], 14: [2500, 2576, 4918], 17: [2516, 2515], 24: [4858], 5: [5069, 2755, 2756], 10: [4978, 4979], 15: [4784, 4783], 29: [2531], 12: [5009], 1: [2696, 2695], 4: [2621, 5054], 22: [2635, 2636], 18: [2726]}, {0: [2628, 3658, 3659], 2: [2582, 2583], 6: [2704, 2703], 7: [2524, 2523], 8: [3613, 3614], 13: [2749, 3749], 16: [2688, 3523, 3524], 19: [3689], 20: [3673, 3674], 23: [3568, 2644, 2643], 25: [3704, 2689], 26: [3719], 27: [3463, 2539, 2538], 3: [3598, 2613], 9: [2554, 3494, 2553], 11: [2597, 2598], 21: [2508, 3583], 28: [2719, 3733, 3734], 14: [3554, 3553, 2658], 17: [3509, 2627], 24: [3748], 5: [3584, 2674, 2673], 10: [2748, 3464, 2612], 15: [2569, 2568], 29: [3569, 2733], 12: [2778], 1: [3643, 3644], 4: [3688, 2493], 22: [3539], 18: [2433, 3628, 3629]}, {0: [91, 3060, 90], 2: [3090, 3091], 6: [151, 150], 7: [240, 376, 3151], 8: [212, 3286, 3285], 13: [3166, 3165], 16: [167, 165, 166], 19: [391, 3240, 3241], 20: [182, 3120, 181], 23: [3315, 227, 3316], 25: [3045, 255], 26: [180], 27: [120, 3150, 121], 3: [3435, 361, 362, 3436], 9: [195, 196], 11: [106, 105, 3105], 21: [3195, 226], 28: [285, 286], 14: [317, 316, 3180], 17: [3000, 211, 210], 24: [3331, 377], 5: [271, 3030, 270], 10: [137, 136], 15: [3210, 256], 29: [3420], 12: [301], 1: [3225], 4: [3255], 22: [3375, 197, 3270], 18: [3301, 3300]}, {0: [4802, 715, 4803], 2: [4817, 4818, 865], 6: [4787, 624, 4788], 7: [4699, 834], 8: [4758, 4683, 714], 13: [4907, 535], 16: [4878, 774, 775], 19: [4848, 760], 20: [925, 4774, 4773], 23: [745, 744], 25: [581, 4743, 580], 26: [4938], 27: [4714, 819], 3: [864, 4759], 9: [4833, 670, 4832], 11: [729, 730], 21: [804, 4653], 28: [759, 4698, 654], 14: [4789, 790, 789], 17: [4728, 4727], 24: [833, 4638], 5: [699, 700], 10: [4623, 849], 15: [4847, 595], 29: [4594, 4593], 12: [534], 1: [4712, 4713], 4: [4744], 22: [4863], 18: [609, 4668, 4667]}, {0: [3433, 2523, 2522], 2: [3537, 3538], 6: [3388, 3387], 7: [3493, 3494], 8: [2448, 3613, 3612], 13: [3373], 16: [2463, 2462], 19: [3523, 3522], 20: [2446, 3463, 2447], 23: [3628, 2418, 3627], 25: [2492, 2388, 3508], 26: [3432, 2402], 27: [3539, 2582], 3: [2507, 2508], 9: [3597, 2343, 3462], 11: [3567, 2328], 21: [2417, 3417], 28: [2537, 2538], 14: [3643, 2477, 2478], 17: [3372], 24: [3598, 2568], 5: [3553, 2313, 3552], 10: [3568, 2493], 15: [2372, 2373], 29: [3673], 12: [2642], 1: [2312, 3402, 3403], 4: [2432, 3478], 22: [3582], 18: [3509, 2597]}, {0: [5470, 1738, 5469], 2: [1693, 5484], 6: [1754, 5543], 7: [5409], 8: [5379, 5378], 13: [1708], 16: [1844, 1843], 19: [5515, 5514], 20: [5574, 5573, 1664], 23: [1753, 5454], 25: [5529, 5528], 26: [1918, 5544], 27: [1769, 1768], 3: [1724, 1723], 9: [5559, 1829], 11: [1784, 1783], 21: [1799, 1798], 28: [1814, 1813], 14: [5589, 1888, 1889], 17: [5604], 24: [5424], 5: [1903, 5364, 1902], 10: [1618, 5393], 15: [1859, 1858], 29: [1873, 5394], 12: [1707], 1: [5335, 5334], 4: [5500, 5499], 22: [5440, 5439], 18: [1663, 5363]}, {0: [1737, 5199, 5198], 2: [5229, 1752], 6: [5168, 1767], 7: [1916, 1917], 8: [5260, 1902], 13: [5124, 1736], 16: [1947, 5184], 19: [1782, 5304], 20: [1827, 5244], 23: [5154, 1932, 5155], 25: [5228, 1706, 1707], 26: [1828, 5334], 27: [1857, 5140], 3: [1872, 5305], 9: [1722, 5319], 11: [5139, 1721], 21: [5364, 1797, 1798], 28: [5289, 2008, 5290], 14: [5213, 5214], 17: [5183, 1617], 24: [5335, 1933], 5: [5275, 5274], 10: [1977], 15: [5258, 5259], 29: [5230], 12: [1961, 5125], 1: [1842, 1843], 4: [5169], 22: [1813, 1812], 18: [5245, 1962]}, {0: [1701, 4134, 4133], 2: [4313, 1672, 4193], 6: [4178, 1596], 7: [1716], 8: [1776, 4164], 13: [1595, 1641, 3998], 16: [4180, 4089, 1942, 1941], 19: [4209, 4210], 20: [1657, 4255, 4254], 23: [1851, 1852], 25: [4103, 1626, 1627], 26: [4059, 1656], 27: [4240, 4239], 3: [1822, 4224], 9: [1761, 1762], 11: [4328, 4329], 21: [4195, 4194, 1807], 28: [4119, 1686, 4118], 14: [1730, 1731, 4179], 17: [4088], 24: [4283, 4284], 5: [1792, 1791], 10: [1866, 4225], 15: [1746], 29: [1926, 4104], 12: [3999], 1: [1806, 4074], 4: [1987], 22: [4345, 4344], 18: [4149, 1837, 1836]}, {0: [5625, 359, 5626], 2: [178, 5565, 179], 6: [5507, 5551, 404], 7: [119, 118], 8: [5610, 164], 13: [449], 16: [149, 5656, 5655], 19: [328, 5520, 329], 20: [209, 284, 5550], 23: [104, 103], 25: [374, 5566], 26: [5491], 27: [5640, 5641], 3: [194, 5595], 9: [223, 224], 11: [5461, 5460], 21: [239, 5400, 238], 28: [5430, 5431], 14: [5505, 5506], 17: [344], 24: [5445], 5: [253, 254], 10: [5581, 134, 5580], 15: [5536, 5535], 29: [5490], 12: [5611], 1: [314, 5476, 313], 4: [268, 269], 22: [148, 5415], 18: [5700, 299]}, {0: [2342, 3342], 2: [3417, 2357], 6: [3401, 3402], 7: [3433, 3431, 3432], 8: [2326, 3282], 13: [2282], 16: [3298, 2416, 3297], 19: [3371, 3372], 20: [2327, 3387], 23: [2537, 3312, 3313], 25: [2207, 3357], 26: [3237, 2221, 3236], 27: [3447], 3: [2311, 3492, 2312], 9: [2432, 2431], 11: [3358, 2477], 21: [2371, 2372], 28: [2192, 3327], 14: [2447, 2446, 3222], 17: [2462, 2461], 24: [2236, 2237], 5: [3328, 2401], 10: [2297, 2296], 15: [2251, 3268, 3267], 29: [2281], 12: [2267, 3462], 1: [3252, 2266], 4: [2387], 22: [3343], 18: [3477, 2402]}, {0: [3121, 315], 2: [2986, 300], 6: [226, 3225], 7: [331, 330], 8: [316, 3151, 3152], 13: [196, 3120, 3135], 16: [465, 3030, 3031], 19: [390, 3046, 3045], 20: [3016, 3015, 151, 150], 23: [3211, 376], 25: [3136], 26: [285, 3195], 27: [3000, 3001], 3: [3075, 435, 3076], 9: [3060, 3061], 11: [361, 360], 21: [3091, 3090], 28: [345, 346], 14: [3180, 420, 3181], 17: [255, 3105], 24: [3196], 5: [211, 210, 2971], 10: [2926, 406, 405], 15: [240], 29: [481,</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>[283, 276, 287, 290, 298, 287, 308, 296, 294, 297, 283, 287, 297, 290, 301, 300, 297, 288, 321, 289, 283, 281, 300, 293, 309, 296, 282, 286, 292, 295, 293, 300, 296, 299, 304, 287, 302, 307, 282, 304, 308, 292, 285, 294, 272, 300, 319, 294, 291, 272, 282, 299, 257, 288, 320, 314, 304, 302, 298, 270, 273, 297, 292, 280, 308, 292, 304, 284, 292, 293, 286, 307, 280, 279, 275, 277, 268, 289, 287, 278, 275, 293, 282, 296, 284, 298, 273, 309, 302, 302, 294, 305, 284, 275, 287, 284, 322, 276, 277, 277]</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>[57, 63, 75, 69, 66, 65, 74, 67, 67, 61, 68, 63, 69, 67, 67, 64, 64, 62, 62, 69, 65, 62, 66, 69, 63, 62, 69, 68, 66, 62, 60, 64, 60, 74, 59, 57, 63, 62, 64, 63, 62, 61, 65, 64, 63, 63, 58, 56, 59, 62, 65, 70, 67, 64, 59, 62, 66, 63, 62, 65, 63, 64, 64, 67, 68, 57, 61, 66, 63, 64, 68, 63, 67, 64, 63, 64, 67, 66, 64, 67, 57, 59, 68, 63, 62, 64, 65, 62, 65, 61, 69, 62, 63, 66, 61, 70, 69, 67, 65, 63]</t>
-        </is>
+          <t>[0.43790197372436523, 0.29109740257263184, 0.3628957271575928, 0.5000371932983398, 0.40633583068847656, 0.5413732528686523, 0.5681824684143066, 0.6886806488037109, 0.43166494369506836, 0.6890051364898682, 0.40560483932495117, 0.6389975547790527, 0.4929225444793701, 0.3388712406158447, 0.35364532470703125, 0.28182387351989746, 0.6980695724487305, 0.7775890827178955, 0.5675585269927979, 0.42776966094970703, 0.5137007236480713, 0.38126420974731445, 0.30324316024780273, 0.31589651107788086, 0.28351378440856934, 0.3891875743865967, 0.9675722122192383, 0.4672560691833496, 0.5978488922119141, 0.6069943904876709, 0.5449545383453369, 0.30135059356689453, 0.3872551918029785, 0.487654447555542, 0.32912182807922363, 0.39521336555480957, 0.4404256343841553, 0.3940906524658203, 0.5722963809967041, 0.4740912914276123, 0.48481011390686035, 0.4880352020263672, 0.47109556198120117, 0.3081967830657959, 0.46303439140319824, 0.4737236499786377, 0.4587440490722656, 0.49025511741638184, 0.5244808197021484, 0.37601327896118164, 0.27509403228759766, 0.32550907135009766, 0.3618929386138916, 0.31834840774536133, 0.5485777854919434, 0.3165903091430664, 0.34184694290161133, 0.3034369945526123, 0.23914504051208496, 0.522768497467041, 0.5856828689575195, 0.298417329788208, 0.30766749382019043, 0.6256814002990723, 0.33991527557373047, 0.43581604957580566, 0.5073769092559814, 0.37531113624572754, 0.3929309844970703, 0.4303891658782959, 0.4418823719024658, 0.44947075843811035, 0.4481809139251709, 0.35050249099731445, 0.4437844753265381, 0.4320073127746582, 0.5012457370758057, 0.5129454135894775, 0.4735860824584961, 0.32694387435913086, 0.4642648696899414, 0.43210291862487793, 0.4913051128387451, 0.6667547225952148, 0.43091583251953125, 0.3340620994567871, 0.2976415157318115, 0.48481011390686035, 0.18768930435180664, 0.282428503036499, 0.2653357982635498, 0.6306841373443604, 0.26485347747802734, 0.39127016067504883, 0.4632604122161865, 0.4243202209472656, 0.28519558906555176, 0.607280969619751, 0.48711514472961426, 0.2624239921569824]</t>
+        </is>
+      </c>
+      <c r="AF5" t="n">
+        <v>458</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>137</v>
       </c>
       <c r="AH5" t="n">
-        <v>12.41557754019384</v>
+        <v>137</v>
       </c>
       <c r="AI5" t="n">
-        <v>3.635181626073924</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL5" t="inlineStr">
-        <is>
-          <t>[2.2233123779296875, 3.4120991230010986, 3.8074657917022705, 2.5724363327026367, 3.6705703735351562, 3.821805477142334, 2.292283058166504, 4.622916221618652, 2.2876882553100586, 3.2191104888916016, 2.486034870147705, 4.3210060596466064, 5.021400213241577, 3.7358641624450684, 3.090468645095825, 2.5019071102142334, 3.059701919555664, 5.370641231536865, 3.277167558670044, 3.7866785526275635, 3.8121039867401123, 4.408235311508179, 3.2281017303466797, 2.476410150527954, 4.474546670913696, 2.7250092029571533, 5.781745910644531, 4.222081184387207, 3.156346559524536, 3.4747531414031982, 4.506195545196533, 5.474774360656738, 4.102116823196411, 2.466559648513794, 2.280759572982788, 2.6594927310943604, 3.3332576751708984, 3.264777660369873, 2.7342612743377686, 1.8815319538116455, 4.077101230621338, 3.994239091873169, 5.407686710357666, 2.8750455379486084, 3.1716222763061523, 5.386113405227661, 3.02703857421875, 2.9229207038879395, 3.6584293842315674, 4.0879175662994385, 3.1384220123291016, 3.338932752609253, 4.920925140380859, 3.9468204975128174, 3.347482204437256, 3.519200563430786, 5.667027950286865, 4.912498235702515, 3.801935911178589, 3.922013759613037, 5.929867744445801, 6.098344802856445, 3.4504480361938477, 2.9880428314208984, 3.1652143001556396, 3.8425731658935547, 3.061265468597412, 2.829416513442993, 3.8994524478912354, 3.1394081115722656, 5.42831015586853, 3.685781240463257, 3.819176197052002, 4.285881042480469, 4.85956072807312, 2.972353935241699, 2.7506754398345947, 3.4308016300201416, 2.7323837280273438, 3.816976547241211, 1.6548855304718018, 3.2221896648406982, 4.582113027572632, 4.19099760055542, 2.4995334148406982, 2.2553062438964844, 3.4258086681365967, 2.7914376258850098, 2.3579912185668945, 2.1453235149383545, 3.158961772918701, 2.4495275020599365, 5.692134380340576, 4.4762046337127686, 3.830447196960449, 2.657573938369751, 2.1207387447357178, 2.3720216751098633, 2.4316704273223877, 5.308555364608765]</t>
-        </is>
-      </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>[0.45374393463134766, 0.21282625198364258, 0.430736780166626, 0.4023292064666748, 0.31514596939086914, 0.29555630683898926, 0.38770365715026855, 0.39917802810668945, 0.3541445732116699, 0.46730899810791016, 0.42319583892822266, 0.3730013370513916, 0.39435744285583496, 0.35608959197998047, 0.20439863204956055, 0.38802504539489746, 0.2963714599609375, 0.30933141708374023, 0.5440442562103271, 0.25840187072753906, 0.32647228240966797, 0.3185389041900635, 0.34126734733581543, 0.37319231033325195, 0.30982279777526855, 0.2673172950744629, 0.22429752349853516, 0.25432515144348145, 0.30526280403137207, 0.41175103187561035, 0.592160701751709, 0.3367595672607422, 0.330214262008667, 0.27158427238464355, 0.42022252082824707, 0.41843438148498535, 0.3479733467102051, 0.30002808570861816, 0.30118584632873535, 0.2937479019165039, 0.2803981304168701, 0.2277977466583252, 0.339414119720459, 0.33820462226867676, 0.43838047981262207, 0.2236032485961914, 0.3478736877441406, 0.23617100715637207, 0.21548223495483398, 0.37265539169311523, 0.17891645431518555, 0.21231865882873535, 0.29375553131103516, 0.38429713249206543, 0.3832218647003174, 0.3562133312225342, 0.37212467193603516, 0.297229528427124, 0.38990020751953125, 0.32021164894104004, 0.38049817085266113, 0.34173011779785156, 0.3438589572906494, 0.19196343421936035, 0.34245967864990234, 0.6411280632019043, 0.3688333034515381, 0.25975990295410156, 0.4787774085998535, 0.27491259574890137, 0.23705458641052246, 0.4966084957122803, 0.49439382553100586, 0.3962690830230713, 0.3225739002227783, 0.32091355323791504, 0.23037314414978027, 0.48914480209350586, 0.27787280082702637, 0.41176605224609375, 0.22906208038330078, 0.38193297386169434, 0.2263336181640625, 0.2747669219970703, 0.36293697357177734, 0.6221156120300293, 0.2796058654785156, 0.3184962272644043, 0.3470487594604492, 0.33299779891967773, 0.2997760772705078, 0.40738415718078613, 0.5458803176879883, 0.29934144020080566, 0.2747962474822998, 0.4342315196990967, 0.3479580879211426, 0.3193356990814209, 0.20530176162719727, 0.3678102493286133]</t>
-        </is>
-      </c>
-      <c r="AN5" t="n">
-        <v>518</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>137</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>167</v>
-      </c>
-      <c r="AQ5" t="n">
         <v>30</v>
       </c>
-      <c r="AR5" t="inlineStr">
-        <is>
-          <t>[0, 2, 's_0_2', 6, 's_0_6', 7, 's_0_7', 8, 's_0_8', 13, 's_0_13', 16, 's_0_16', 19, 's_0_19', 20, 's_0_20', 23, 's_0_23', 25, 's_0_25', 26, 's_0_26', 27, 's_0_27', 's_0_0', 3, 's_2_3', 9, 's_2_9', 11, 's_2_11', 's_2_19', 's_2_20', 21, 's_2_21', 's_2_25', 's_2_27', 28, 's_2_28', 's_2_2', 's_6_13', 14, 's_6_14', 17, 's_6_17', 's_6_20', 's_6_25', 's_6_6', 's_7_3', 's_7_14', 's_7_21', 24, 's_7_24', 's_7_27', 's_7_28', 's_7_7', 's_8_3', 5, 's_8_5', 10, 's_8_10', 's_8_14', 15, 's_8_15', 's_8_16', 's_8_23', 29, 's_8_29', 's_8_8', 12, 's_13_12', 's_13_25', 's_13_13', 1, 's_16_1', 4, 's_16_4', 's_16_5', 's_16_14', 's_16_17', 's_16_19', 's_16_20', 22, 's_16_22', 's_16_29', 's_16_16', 's_19_3', 's_19_4', 's_19_5', 's_19_9', 's_19_15', 's_19_20', 's_19_28', 's_19_19', 's_20_3', 's_20_4', 's_20_9', 's_20_11', 's_20_14', 18, 's_20_18', 's_20_27', 's_20_20', 's_23_10', 's_23_11', 's_23_21', 's_23_22', 's_23_24', 's_23_28', 's_23_29', 's_23_23', 's_25_11', 's_25_15', 's_25_26', 's_25_28', 's_25_25', 's_26_5', 's_26_9', 's_26_26', 's_27_4', 's_27_10', 's_27_18', 's_27_27', 's_3_10', 's_3_14', 's_3_24', 's_3_3', 's_9_15', 's_9_11', 's_9_14', 's_9_22', 's_9_9', 's_11_21', 's_11_22', 's_11_11', 's_21_1', 's_21_5', 's_21_4', 's_21_14', 's_21_21', 's_28_1', 's_28_5', 's_28_24', 's_28_28', 's_14_17', 's_14_14', 's_17_15', 's_17_17', 's_24_24', 's_5_1', 's_5_18', 's_5_22', 's_5_5', 's_10_18', 's_10_29', 's_10_10', 's_15_1', 's_15_15', 's_29_29', 's_12_1', 's_12_18', 's_12_12', 's_1_1', 's_4_4', 's_22_22', 's_18_18']</t>
-        </is>
-      </c>
-      <c r="AS5" t="inlineStr">
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>[0, 2, 's_0_2', 6, 's_0_6', 7, 's_0_7', 8, 's_0_8', 13, 's_0_13', 16, 's_0_16', 19, 's_0_19', 20, 's_0_20', 23, 's_0_23', 25, 's_0_25', 26, 's_0_26', 27, 's_0_27', 3, 's_2_3', 9, 's_2_9', 11, 's_2_11', 's_2_19', 's_2_20', 21, 's_2_21', 's_2_25', 's_2_27', 28, 's_2_28', 's_6_13', 14, 's_6_14', 17, 's_6_17', 's_6_20', 's_6_25', 's_3_7', 's_7_14', 's_7_21', 24, 's_7_24', 's_7_27', 's_7_28', 's_3_8', 5, 's_5_8', 10, 's_8_10', 's_8_14', 15, 's_8_15', 's_8_16', 's_8_23', 29, 's_8_29', 12, 's_12_13', 's_13_25', 1, 's_1_16', 4, 's_4_16', 's_5_16', 's_14_16', 's_16_17', 's_16_19', 's_16_20', 22, 's_16_22', 's_16_29', 's_3_19', 's_4_19', 's_5_19', 's_9_19', 's_15_19', 's_19_20', 's_19_28', 's_3_20', 's_4_20', 's_9_20', 's_11_20', 's_14_20', 18, 's_18_20', 's_20_27', 's_10_23', 's_11_23', 's_21_23', 's_22_23', 's_23_24', 's_23_28', 's_23_29', 's_11_25', 's_15_25', 's_25_26', 's_25_28', 's_5_26', 's_9_26', 's_4_27', 's_10_27', 's_18_27', 's_1_5', 's_1_12', 's_1_15', 's_1_21', 's_1_28', 's_5_18', 's_5_21', 's_5_22', 's_5_28', 's_12_18', 's_9_15', 's_15_17', 's_4_21', 's_11_21', 's_14_21', 's_24_28', 's_3_10', 's_3_14', 's_3_24', 's_9_11', 's_9_14', 's_9_22', 's_11_22', 's_10_18', 's_10_29', 's_14_17']</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
         <is>
           <t>[0, 2, 6, 7, 8, 13, 16, 19, 20, 23, 25, 26, 27, 3, 9, 11, 21, 28, 14, 17, 24, 5, 10, 15, 29, 12, 1, 4, 22, 18]</t>
         </is>
@@ -1289,12 +1177,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>[0, 2, 4, 5, 7, 8, 12, 13, 16, 18, 23, 32, 33, 36, 14, 34, 17, 21, 25, 26, 28, 29, 31, 6, 10, 20, 24, 35, 1, 3, 15, 27, 38, 9, 37, 11, 19, 30, 39, 22]</t>
+          <t>[0, 2, 4, 5, 7, 8, 12, 13, 16, 18, 23, 32, 33, 36, 1, 3, 6, 9, 20, 21, 31, 37, 38, 39, 14, 34, 17, 25, 26, 28, 29, 10, 24, 35, 19, 15, 27, 22, 11, 30]</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>[(0, 2), (0, 4), (0, 5), (0, 7), (0, 8), (0, 12), (0, 13), (0, 16), (0, 18), (0, 23), (0, 32), (0, 33), (0, 36), (0, 0), (2, 12), (2, 14), (2, 18), (2, 34), (2, 2), (4, 12), (4, 17), (4, 18), (4, 21), (4, 25), (4, 26), (4, 28), (4, 29), (4, 31), (4, 34), (4, 4), (5, 6), (5, 10), (5, 20), (5, 21), (5, 23), (5, 24), (5, 26), (5, 33), (5, 35), (5, 5), (7, 1), (7, 3), (7, 8), (7, 10), (7, 13), (7, 15), (7, 20), (7, 26), (7, 27), (7, 31), (7, 32), (7, 38), (7, 7), (8, 12), (8, 25), (8, 28), (8, 32), (8, 35), (8, 8), (12, 9), (12, 17), (12, 21), (12, 24), (12, 28), (12, 34), (12, 35), (12, 37), (12, 38), (12, 12), (13, 9), (13, 11), (13, 14), (13, 16), (13, 18), (13, 19), (13, 21), (13, 27), (13, 29), (13, 30), (13, 35), (13, 39), (13, 13), (16, 1), (16, 6), (16, 10), (16, 11), (16, 18), (16, 20), (16, 22), (16, 32), (16, 36), (16, 16), (18, 6), (18, 21), (18, 24), (18, 27), (18, 30), (18, 35), (18, 36), (18, 39), (18, 18), (23, 1), (23, 14), (23, 19), (23, 33), (23, 37), (23, 39), (23, 23), (32, 3), (32, 6), (32, 14), (32, 33), (32, 37), (32, 38), (32, 32), (33, 6), (33, 9), (33, 22), (33, 26), (33, 36), (33, 33), (36, 10), (36, 14), (36, 21), (36, 29), (36, 35), (36, 38), (36, 39), (36, 36), (14, 3), (14, 20), (14, 37), (14, 39), (14, 11), (14, 15), (14, 27), (14, 35), (14, 14), (34, 10), (34, 22), (34, 24), (34, 28), (34, 34), (17, 20), (17, 38), (17, 22), (17, 24), (17, 25), (17, 29), (17, 30), (17, 17), (21, 1), (21, 6), (21, 11), (21, 27), (21, 28), (21, 31), (21, 35), (21, 38), (21, 21), (25, 38), (25, 11), (25, 19), (25, 22), (25, 28), (25, 29), (25, 25), (26, 38), (26, 24), (26, 27), (26, 28), (26, 35), (26, 26), (28, 6), (28, 20), (28, 38), (28, 19), (28, 24), (28, 29), (28, 30), (28, 28), (29, 6), (29, 31), (29, 37), (29, 22), (29, 24), (29, 35), (29, 29), (31, 1), (31, 3), (31, 10), (31, 30), (31, 31), (6, 1), (6, 10), (6, 19), (6, 24), (6, 35), (6, 6), (10, 22), (10, 24), (10, 35), (10, 10), (20, 1), (20, 3), (20, 37), (20, 20), (24, 9), (24, 38), (24, 11), (24, 22), (24, 24), (35, 37), (35, 38), (35, 15), (35, 27), (35, 35), (1, 3), (1, 9), (1, 37), (1, 38), (1, 39), (1, 1), (3, 3), (15, 37), (15, 38), (15, 15), (27, 9), (27, 38), (27, 19), (27, 30), (27, 27), (38, 39), (38, 38), (9, 9), (37, 11), (37, 19), (37, 30), (37, 37), (11, 39), (11, 11), (19, 39), (19, 22), (19, 19), (30, 39), (30, 22), (30, 30), (39, 22), (39, 39), (22, 22)]</t>
+          <t>[(0, 2), (0, 4), (0, 5), (0, 7), (0, 8), (0, 12), (0, 13), (0, 16), (0, 18), (0, 23), (0, 32), (0, 33), (0, 36), (2, 12), (2, 14), (2, 18), (2, 34), (4, 12), (4, 17), (4, 18), (4, 21), (4, 25), (4, 26), (4, 28), (4, 29), (4, 31), (4, 34), (5, 6), (5, 10), (5, 20), (5, 21), (5, 23), (5, 24), (5, 26), (5, 33), (5, 35), (7, 1), (7, 3), (7, 8), (7, 10), (7, 13), (7, 15), (7, 20), (7, 26), (7, 27), (7, 31), (7, 32), (7, 38), (8, 12), (8, 25), (8, 28), (8, 32), (8, 35), (12, 9), (12, 17), (12, 21), (12, 24), (12, 28), (12, 34), (12, 35), (12, 37), (12, 38), (13, 9), (13, 11), (13, 14), (13, 16), (13, 18), (13, 19), (13, 21), (13, 27), (13, 29), (13, 30), (13, 35), (13, 39), (16, 1), (16, 6), (16, 10), (16, 11), (16, 18), (16, 20), (16, 22), (16, 32), (16, 36), (18, 6), (18, 21), (18, 24), (18, 27), (18, 30), (18, 35), (18, 36), (18, 39), (23, 1), (23, 14), (23, 19), (23, 33), (23, 37), (23, 39), (32, 3), (32, 6), (32, 14), (32, 33), (32, 37), (32, 38), (33, 6), (33, 9), (33, 22), (33, 26), (33, 36), (36, 10), (36, 14), (36, 21), (36, 29), (36, 35), (36, 38), (36, 39), (1, 3), (1, 6), (1, 9), (1, 20), (1, 21), (1, 31), (1, 37), (1, 38), (1, 39), (3, 14), (3, 20), (3, 31), (6, 10), (6, 19), (6, 21), (6, 24), (6, 28), (6, 29), (6, 35), (9, 24), (9, 27), (20, 14), (20, 17), (20, 28), (20, 37), (21, 11), (21, 27), (21, 28), (21, 31), (21, 35), (21, 38), (31, 10), (31, 29), (31, 30), (37, 11), (37, 14), (37, 15), (37, 19), (37, 29), (37, 30), (37, 35), (38, 15), (38, 17), (38, 24), (38, 25), (38, 26), (38, 27), (38, 28), (38, 35), (38, 39), (39, 11), (39, 14), (39, 19), (39, 22), (39, 30), (14, 11), (14, 15), (14, 27), (14, 35), (34, 10), (34, 22), (34, 24), (34, 28), (17, 22), (17, 24), (17, 25), (17, 29), (17, 30), (25, 11), (25, 19), (25, 22), (25, 28), (25, 29), (26, 24), (26, 27), (26, 28), (26, 35), (28, 19), (28, 24), (28, 29), (28, 30), (29, 22), (29, 24), (29, 35), (10, 22), (10, 24), (10, 35), (24, 11), (24, 22), (35, 15), (35, 27), (19, 22), (19, 27), (27, 30), (22, 30)]</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -1309,14 +1197,14 @@
         <v>0.002534468157697533</v>
       </c>
       <c r="J6" t="n">
-        <v>0.02290896074454122</v>
+        <v>0.02827309236947791</v>
       </c>
       <c r="K6" t="n">
         <v>0.3205128205128205</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[(0, 2), (0, 's_0_2'), (0, 4), (0, 's_0_4'), (0, 5), (0, 's_0_5'), (0, 7), (0, 's_0_7'), (0, 8), (0, 's_0_8'), (0, 12), (0, 's_0_12'), (0, 13), (0, 's_0_13'), (0, 16), (0, 's_0_16'), (0, 18), (0, 's_0_18'), (0, 23), (0, 's_0_23'), (0, 32), (0, 's_0_32'), (0, 33), (0, 's_0_33'), (0, 36), (0, 's_0_36'), (0, 's_0_0'), (0, 0), (2, 's_0_2'), (2, 12), (2, 's_2_12'), (2, 14), (2, 's_2_14'), (2, 18), (2, 's_2_18'), (2, 34), (2, 's_2_34'), (2, 's_2_2'), (2, 2), ('s_0_2', 's_0_2'), (4, 's_0_4'), (4, 12), (4, 's_4_12'), (4, 17), (4, 's_4_17'), (4, 18), (4, 's_4_18'), (4, 21), (4, 's_4_21'), (4, 25), (4, 's_4_25'), (4, 26), (4, 's_4_26'), (4, 28), (4, 's_4_28'), (4, 29), (4, 's_4_29'), (4, 31), (4, 's_4_31'), (4, 34), (4, 's_4_34'), (4, 's_4_4'), (4, 4), ('s_0_4', 's_0_4'), (5, 's_0_5'), (5, 6), (5, 's_5_6'), (5, 10), (5, 's_5_10'), (5, 20), (5, 's_5_20'), (5, 21), (5, 's_5_21'), (5, 23), (5, 's_5_23'), (5, 24), (5, 's_5_24'), (5, 26), (5, 's_5_26'), (5, 33), (5, 's_5_33'), (5, 35), (5, 's_5_35'), (5, 's_5_5'), (5, 5), ('s_0_5', 's_0_5'), (7, 's_0_7'), (7, 1), (7, 's_7_1'), (7, 3), (7, 's_7_3'), (7, 8), (7, 's_7_8'), (7, 10), (7, 's_7_10'), (7, 13), (7, 's_7_13'), (7, 15), (7, 's_7_15'), (7, 20), (7, 's_7_20'), (7, 26), (7, 's_7_26'), (7, 27), (7, 's_7_27'), (7, 31), (7, 's_7_31'), (7, 32), (7, 's_7_32'), (7, 38), (7, 's_7_38'), (7, 's_7_7'), (7, 7), ('s_0_7', 's_0_7'), (8, 's_0_8'), (8, 's_7_8'), (8, 12), (8, 's_8_12'), (8, 25), (8, 's_8_25'), (8, 28), (8, 's_8_28'), (8, 32), (8, 's_8_32'), (8, 35), (8, 's_8_35'), (8, 's_8_8'), (8, 8), ('s_0_8', 's_0_8'), (12, 's_0_12'), (12, 's_2_12'), (12, 's_4_12'), (12, 's_8_12'), (12, 9), (12, 's_12_9'), (12, 17), (12, 's_12_17'), (12, 21), (12, 's_12_21'), (12, 24), (12, 's_12_24'), (12, 28), (12, 's_12_28'), (12, 34), (12, 's_12_34'), (12, 35), (12, 's_12_35'), (12, 37), (12, 's_12_37'), (12, 38), (12, 's_12_38'), (12, 's_12_12'), (12, 12), ('s_0_12', 's_0_12'), (13, 's_0_13'), (13, 's_7_13'), (13, 9), (13, 's_13_9'), (13, 11), (13, 's_13_11'), (13, 14), (13, 's_13_14'), (13, 16), (13, 's_13_16'), (13, 18), (13, 's_13_18'), (13, 19), (13, 's_13_19'), (13, 21), (13, 's_13_21'), (13, 27), (13, 's_13_27'), (13, 29), (13, 's_13_29'), (13, 30), (13, 's_13_30'), (13, 35), (13, 's_13_35'), (13, 39), (13, 's_13_39'), (13, 's_13_13'), (13, 13), ('s_0_13', 's_0_13'), (16, 's_0_16'), (16, 's_13_16'), (16, 1), (16, 's_16_1'), (16, 6), (16, 's_16_6'), (16, 10), (16, 's_16_10'), (16, 11), (16, 's_16_11'), (16, 18), (16, 's_16_18'), (16, 20), (16, 's_16_20'), (16, 22), (16, 's_16_22'), (16, 32), (16, 's_16_32'), (16, 36), (16, 's_16_36'), (16, 's_16_16'), (16, 16), ('s_0_16', 's_0_16'), (18, 's_0_18'), (18, 's_2_18'), (18, 's_4_18'), (18, 's_13_18'), (18, 's_16_18'), (18, 6), (18, 's_18_6'), (18, 21), (18, 's_18_21'), (18, 24), (18, 's_18_24'), (18, 27), (18, 's_18_27'), (18, 30), (18, 's_18_30'), (18, 35), (18, 's_18_35'), (18, 36), (18, 's_18_36'), (18, 39), (18, 's_18_39'), (18, 's_18_18'), (18, 18), ('s_0_18', 's_0_18'), (23, 's_0_23'), (23, 's_5_23'), (23, 1), (23, 's_23_1'), (23, 14), (23, 's_23_14'), (23, 19), (23, 's_23_19'), (23, 33), (23, 's_23_33'), (23, 37), (23, 's_23_37'), (23, 39), (23, 's_23_39'), (23, 's_23_23'), (23, 23), ('s_0_23', 's_0_23'), (32, 's_0_32'), (32, 's_7_32'), (32, 's_8_32'), (32, 's_16_32'), (32, 3), (32, 's_32_3'), (32, 6), (32, 's_32_6'), (32, 14), (32, 's_32_14'), (32, 33), (32, 's_32_33'), (32, 37), (32, 's_32_37'), (32, 38), (32, 's_32_38'), (32, 's_32_32'), (32, 32), ('s_0_32', 's_0_32'), (33, 's_0_33'), (33, 's_5_33'), (33, 's_23_33'), (33, 's_32_33'), (33, 6), (33, 's_33_6'), (33, 9), (33, 's_33_9'), (33, 22), (33, 's_33_22'), (33, 26), (33, 's_33_26'), (33, 36), (33, 's_33_36'), (33, 's_33_33'), (33, 33), ('s_0_33', 's_0_33'), (36, 's_0_36'), (36, 's_16_36'), (36, 's_18_36'), (36, 's_33_36'), (36, 10), (36, 's_36_10'), (36, 14), (36, 's_36_14'), (36, 21), (36, 's_36_21'), (36, 29), (36, 's_36_29'), (36, 35), (36, 's_36_35'), (36, 38), (36, 's_36_38'), (36, 39), (36, 's_36_39'), (36, 's_36_36'), (36, 36), ('s_0_36', 's_0_36'), ('s_0_0', 's_0_0'), ('s_2_12', 's_2_12'), (14, 's_2_14'), (14, 's_13_14'), (14, 's_23_14'), (14, 's_32_14'), (14, 's_36_14'), (14, 3), (14, 's_14_3'), (14, 20), (14, 's_14_20'), (14, 37), (14, 's_14_37'), (14, 39), (14, 's_14_39'), (14, 11), (14, 's_14_11'), (14, 15), (14, 's_14_15'), (14, 27), (14, 's_14_27'), (14, 35), (14, 's_14_35'), (14, 's_14_14'), (14, 14), ('s_2_14', 's_2_14'), ('s_2_18', 's_2_18'), (34, 's_2_34'), (34, 's_4_34'), (34, 's_12_34'), (34, 10), (34, 's_34_10'), (34, 22), (34, 's_34_22'), (34, 24), (34, 's_34_24'), (34, 28), (34, 's_34_28'), (34, 's_34_34'), (34, 34), ('s_2_34', 's_2_34'), ('s_2_2', 's_2_2'), ('s_4_12', 's_4_12'), (17, 's_4_17'), (17, 's_12_17'), (17, 20), (17, 's_17_20'), (17, 38), (17, 's_17_38'), (17, 22), (17, 's_17_22'), (17, 24), (17, 's_17_24'), (17, 25), (17, 's_17_25'), (17, 29), (17, 's_17_29'), (17, 30), (17, 's_17_30'), (17, 's_17_17'), (17, 17), ('s_4_17', 's_4_17'), ('s_4_18', 's_4_18'), (21, 's_4_21'), (21, 's_5_21'), (21, 's_12_21'), (21, 's_13_21'), (21, 's_18_21'), (21, 's_36_21'), (21, 1), (21, 's_21_1'), (21, 6), (21, 's_21_6'), (21, 11), (21, 's_21_11'), (21, 27), (21, 's_21_27'), (21, 28), (21, 's_21_28'), (21, 31), (21, 's_21_31'), (21, 35), (21, 's_21_35'), (21, 38), (21, 's_21_38'), (21, 's_21_21'), (21, 21), ('s_4_21', 's_4_21'), (25, 's_4_25'), (25, 's_8_25'), (25, 's_17_25'), (25, 38), (25, 's_25_38'), (25, 11), (25, 's_25_11'), (25, 19), (25, 's_25_19'), (25, 22), (25, 's_25_22'), (25, 28), (25, 's_25_28'), (25, 29), (25, 's_25_29'), (25, 's_25_25'), (25, 25), ('s_4_25', 's_4_25'), (26, 's_4_26'), (26, 's_5_26'), (26, 's_7_26'), (26, 's_33_26'), (26, 38), (26, 's_26_38'), (26, 24), (26, 's_26_24'), (26, 27), (26, 's_26_27'), (26, 28), (26, 's_26_28'), (26, 35), (26, 's_26_35'), (26, 's_26_26'), (26, 26), ('s_4_26', 's_4_26'), (28, 's_4_28'), (28, 's_8_28'), (28, 's_12_28'), (28, 's_34_28'), (28, 's_21_28'), (28, 's_25_28'), (28, 's_26_28'), (28, 6), (28, 's_28_6'), (28, 20), (28, 's_28_20'), (28, 38), (28, 's_28_38'), (28, 19), (28, 's_28_19'), (28, 24), (28, 's_28_24'), (28, 29), (28, 's_28_29'), (28, 30), (28, 's_28_30'), (28, 's_28_28'), (28, 28), ('s_4_28', 's_4_28'), (29, 's_4_29'), (29, 's_13_29'), (29, 's_36_29'), (29, 's_17_29'), (29, 's_25_29'), (29, 's_28_29'), (29, 6), (29, 's_29_6'), (29, 31), (29, 's_29_31'), (29, 37), (29, 's_29_37'), (29, 22), (29, 's_29_22'), (29, 24), (29, 's_29_24'), (29, 35), (29, 's_29_35'), (29, 's_29_29'), (29, 29), ('s_4_29', 's_4_29'), (31, 's_4_31'), (31, 's_7_31'), (31, 's_21_31'), (31, 's_29_31'), (31, 1), (31, 's_31_1'), (31, 3), (31, 's_31_3'), (31, 10), (31, 's_31_10'), (31, 30), (31, 's_31_30'), (31, 's_31_31'), (31, 31), ('s_4_31', 's_4_31'), ('s_4_34', 's_4_34'), ('s_4_4', 's_4_4'), (6, 's_5_6'), (6, 's_16_6'), (6, 's_18_6'), (6, 's_32_6'), (6, 's_33_6'), (6, 's_21_6'), (6, 's_28_6'), (6, 's_29_6'), (6, 1), (6, 's_6_1'), (6, 10), (6, 's_6_10'), (6, 19), (6, 's_6_19'), (6, 24), (6, 's_6_24'), (6, 35), (6, 's_6_35'), (6, 's_6_6'), (6, 6), ('s_5_6', 's_5_6'), (10, 's_5_10'), (10, 's_7_10'), (10, 's_16_10'), (10, 's_36_10'), (10, 's_34_10'), (10, 's_31_10'), (10, 's_6_10'), (10, 22), (10, 's_10_22'), (10, 24), (10, 's_10_24'), (10, 35), (10, 's_10_35'), (10, 's_10_10'), (10, 10), ('s_5_10', 's_5_10'), (20, 's_5_20'), (20, 's_7_20'), (20, 's_16_20'), (20, 's_14_20'), (20, 's_17_20'), (20, 's_28_20'), (20, 1), (20, 's_20_1'), (20, 3), (20, 's_20_3'), (20, 37), (20, 's_20_37'), (20, 's_20_20'), (20, 20), ('s_5_20', 's_5_20'), ('s_5_21', 's_5_21'), ('s_5_23', 's_5_23'), (24, 's_5_24'), (24, 's_12_24'), (24, 's_18_24'), (24, 's_34_24'), (24, 's_17_24'), (24, 's_26_24'), (24, 's_28_24'), (24, 's_29_24'), (24, 's_6_24'), (24, 's_10_24'), (24, 9), (24, 's_24_9'), (24, 38), (24, 's_24_38'), (24, 11), (24, 's_24_11'), (24, 22), (24, 's_24_22'), (24, 's_24_24'), (24, 24), ('s_5_24', 's_5_24'), ('s_5_26', 's_5_26'), ('s_5_33', 's_5_33'), (35, 's_5_35'), (35, 's_8_35'), (35, 's_12_35'), (35, 's_13_35'), (35, 's_18_35'), (35, 's_36_35'), (35, 's_14_35'), (35, 's_21_35'), (35, 's_26_35'), (35, 's_29_35'), (35, 's_6_35'), (35, 's_10_35'), (35, 37), (35, 's_35_37'), (35, 38), (35, 's_35_38'), (35, 15), (35, 's_35_15'), (35, 27), (35, 's_35_27'), (35, 's_35_35'), (35, 35), ('s_5_35', 's_5_35'), ('s_5_5', 's_5_5'), (1, 's_7_1'), (1, 's_16_1'), (1, 's_23_1'), (1, 's_21_1'), (1, 's_31_1'), (1, 's_6_1'), (1, 's_20_1'), (1, 3), (1, 's_1_3'), (1, 9), (1, 's_1_9'), (1, 37), (1, 's_1_37'), (1, 38), (1, 's_1_38'), (1, 39), (1, 's_1_39'), (1, 's_1_1'), (1, 1), ('s_7_1', 's_7_1'), (3, 's_7_3'), (3, 's_32_3'), (3, 's_14_3'), (3, 's_31_3'), (3, 's_20_3'), (3, 's_1_3'), (3, 's_3_3'), (3, 3), ('s_7_3', 's_7_3'), ('s_7_8', 's_7_8'), ('s_7_10', 's_7_10'), ('s_7_13', 's_7_13'), (15, 's_7_15'), (15, 's_14_15'), (15, 's_35_15'), (15, 37), (15, 's_15_37'), (15, 38), (15, 's_15_38'), (15, 's_15_15'), (15, 15), ('s_7_15', 's_7_15'), ('s_7_20', 's_7_20'), ('s_7_26', 's_7_26'), (27, 's_7_27'), (27, 's_13_27'), (27, 's_18_27'), (27, 's_14_27'), (27, 's_21_27'), (27, 's_26_27'), (27, 's_35_27'), (27, 9), (27, 's_27_9'), (27, 38), (27, 's_27_38'), (27, 19), (27, 's_27_19'), (27, 30), (27, 's_27_30'), (27, 's_27_27'), (27, 27), ('s_7_27', 's_7_27'), ('s_7_31', 's_7_31'), ('s_7_32', 's_7_32'), (38, 's_7_38'), (38, 's_12_38'), (38, 's_32_38'), (38, 's_36_38'), (38, 's_17_38'), (38, 's_21_38'), (38, 's_25_38'), (38, 's_26_38'), (38, 's_28_38'), (38, 's_24_38'), (38, 's_35_38'), (38, 's_1_38'), (38, 's_15_38'), (38, 's_27_38'), (38, 39), (38, 's_38_39'), (38, 's_38_38'), (38, 38), ('s_7_38', 's_7_38'), ('s_7_7', 's_7_7'), ('s_8_12', 's_8_12'), ('s_8_25', 's_8_25'), ('s_8_28', 's_8_28'), ('s_8_32', 's_8_32'), ('s_8_35', 's_8_35'), ('s_8_8', 's_8_8'), (9, 's_12_9'), (9, 's_13_9'), (9, 's_33_9'), (9, 's_24_9'), (9, 's_1_9'), (9, 's_27_9'), (9, 's_9_9'), (9, 9), ('s_12_9', 's_12_9'), ('s_12_17', 's_12_17'), ('s_12_21', 's_12_21'), ('s_12_24', 's_12_24'), ('s_12_28', 's_12_28'), ('s_12_34', 's_12_34'), ('s_12_35', 's_12_35'), (37, 's_12_37'), (37, 's_23_37'), (37, 's_32_37'), (37, 's_14_37'), (37, 's_29_37'), (37, 's_20_37'), (37, 's_35_37'), (37, 's_1_37'), (37, 's_15_37'), (37, 11), (37, 's_37_11'), (37, 19), (37, 's_37_19'), (37, 30), (37, 's_37_30'), (37, 's_37_37'), (37, 37), ('s_12_37', 's_12_37'), ('s_12_38', 's_12_38'), ('s_12_12', 's_12_12'), ('s_13_9', 's_13_9'), (11, 's_13_11'), (11, 's_16_11'), (11, 's_14_11'), (11, 's_21_11'), (11, 's_25_11'), (11, 's_24_11'), (11, 's_37_11'), (11, 39), (11, 's_11_39'), (11, 's_11_11'), (11, 11), ('s_13_11', 's_13_11'), ('s_13_14', 's_13_14'), ('s_13_16', 's_13_16'), ('s_13_18', 's_13_18'), (19, 's_13_19'), (19, 's_23_19'), (19, 's_25_19'), (19, 's_28_19'), (19, 's_6_19'), (19, 's_27_19'), (19, 's_37_19'), (19, 39), (19, 's_19_39'), (19, 22), (19, 's_19_22'), (19, 's_19_19'), (19, 19), ('s_13_19', 's_13_19'), ('s_13_21', 's_13_21'), ('s_13_27', 's_13_27'), ('s_13_29', 's_13_29'), (30, 's_13_30'), (30, 's_18_30'), (30, 's_17_30'), (30, 's_28_30'), (30, 's_31_30'), (30, 's_27_30'), (30, 's_37_30'), (30, 39), (30, 's_30_39'), (30, 22), (30, 's_30_22'), (30, 's_30_30'), (30, 30), ('s_13_30', 's_13_30'), ('s_13_35', 's_13_35'), (39, 's_13_39'), (39, 's_18_39'), (39, 's_23_39'), (39, 's_36_39'), (39, 's_14_39'), (39, 's_1_39'), (39, 's_38_39'), (39, 's_11_39'), (39, 's_19_39'), (39, 's_30_39'), (39, 22), (39, 's_39_22'), (39, 's_39_39'), (39, 39), ('s_13_39', 's_13_39'), ('s_13_13', 's_13_13'), ('s_16_1', 's_16_1'), ('s_16_6', 's_16_6'), ('s_16_10', 's_16_10'), ('s_16_11', 's_16_11'), ('s_16_18', 's_16_18'), ('s_16_20', 's_16_20'), (22, 's_16_22'), (22, 's_33_22'), (22, 's_34_22'), (22, 's_17_22'), (22, 's_25_22'), (22, 's_29_22'), (22, 's_10_22'), (22, 's_24_22'), (22, 's_19_22'), (22, 's_30_22'), (22, 's_39_22'), (22, 's_22_22'), (22, 22), ('s_16_22', 's_16_22'), ('s_16_32', 's_16_32'), ('s_16_36', 's_16_36'), ('s_16_16', 's_16_16'), ('s_18_6', 's_18_6'), ('s_18_21', 's_18_21'), ('s_18_24', 's_18_24'), ('s_18_27', 's_18_27'), ('s_18_30', 's_18_30'), ('s_18_35', 's_18_35'), ('s_18_36', 's_18_36'), ('s_18_39', 's_18_39'), ('s_18_18', 's_18_18'), ('s_23_1', 's_23_1'), ('s_23_14', 's_23_14'), ('s_23_19', 's_23_19'), ('s_23_33', 's_23_33'), ('s_23_37', 's_23_37'), ('s_23_39', 's_23_39'), ('s_23_23', 's_23_23'), ('s_32_3', 's_32_3'), ('s_32_6', 's_32_6'), ('s_32_14', 's_32_14'), ('s_32_33', 's_32_33'), ('s_32_37', 's_32_37'), ('s_32_38', 's_32_38'), ('s_32_32', 's_32_32'), ('s_33_6', 's_33_6'), ('s_33_9', 's_33_9'), ('s_33_22', 's_33_22'), ('s_33_26', 's_33_26'), ('s_33_36', 's_33_36'), ('s_33_33', 's_33_33'), ('s_36_10', 's_36_10'), ('s_36_14', 's_36_14'), ('s_36_21', 's_36_21'), ('s_36_29', 's_36_29'), ('s_36_35', 's_36_35'), ('s_36_38', 's_36_38'), ('s_36_39', 's_36_39'), ('s_36_36', 's_36_36'), ('s_14_3', 's_14_3'), ('s_14_20', 's_14_20'), ('s_14_37', 's_14_37'), ('s_14_39', 's_14_39'), ('s_14_11', 's_14_11'), ('s_14_15', 's_14_15'), ('s_14_27', 's_14_27'), ('s_14_35', 's_14_35'), ('s_14_14', 's_14_14'), ('s_34_10', 's_34_10'), ('s_34_22', 's_34_22'), ('s_34_24', 's_34_24'), ('s_34_28', 's_34_28'), ('s_34_34', 's_34_34'), ('s_17_20', 's_17_20'), ('s_17_38', 's_17_38'), ('s_17_22', 's_17_22'), ('s_17_24', 's_17_24'), ('s_17_25', 's_17_25'), ('s_17_29', 's_17_29'), ('s_17_30', 's_17_30'), ('s_17_17', 's_17_17'), ('s_21_1', 's_21_1'), ('s_21_6', 's_21_6'), ('s_21_11', 's_21_11'), ('s_21_27', 's_21_27'), ('s_21_28', 's_21_28'), ('s_21_31', 's_21_31'), ('s_21_35', 's_21_35'), ('s_21_38', 's_21_38'), ('s_21_21', 's_21_21'), ('s_25_38', 's_25_38'), ('s_25_11', 's_25_11'), ('s_25_19', 's_25_19'), ('s_25_22', 's_25_22'), ('s_25_28', 's_25_28'), ('s_25_29', 's_25_29'), ('s_25_25', 's_25_25'), ('s_26_38', 's_26_38'), ('s_26_24', 's_26_24'), ('s_26_27', 's_26_27'), ('s_26_28', 's_26_28'), ('s_26_35', 's_26_35'), ('s_26_26', 's_26_26'), ('s_28_6', 's_28_6'), ('s_28_20', 's_28_20'), ('s_28_38', 's_28_38'), ('s_28_19', 's_28_19'), ('s_28_24', 's_28_24'), ('s_28_29', 's_28_29'), ('s_28_30', 's_28_30'), ('s_28_28', 's_28_28'), ('s_29_6', 's_29_6'), ('s_29_31', 's_29_31'), ('s_29_37', 's_29_37'), ('s_29_22', 's_29_22'), ('s_29_24', 's_29_24'), ('s_29_35', 's_29_35'), ('s_29_29', 's_29_29'), ('s_31_1', 's_31_1'), ('s_31_3', 's_31_3'), ('s_31_10', 's_31_10'), ('s_31_30', 's_31_30'), ('s_31_31', 's_31_31'), ('s_6_1', 's_6_1'), ('s_6_10', 's_6_10'), ('s_6_19', 's_6_19'), ('s_6_24', 's_6_24'), ('s_6_35', 's_6_35'), ('s_6_6', 's_6_6'), ('s_10_22', 's_10_22'), ('s_10_24', 's_10_24'), ('s_10_35', 's_10_35'), ('s_10_10', 's_10_10'), ('s_20_1', 's_20_1'), ('s_20_3', 's_20_3'), ('s_20_37', 's_20_37'), ('s_20_20', 's_20_20'), ('s_24_9', 's_24_9'), ('s_24_38', 's_24_38'), ('s_24_11', 's_24_11'), ('s_24_22', 's_24_22'), ('s_24_24', 's_24_24'), ('s_35_37', 's_35_37'), ('s_35_38', 's_35_38'), ('s_35_15', 's_35_15'), ('s_35_27', 's_35_27'), ('s_35_35', 's_35_35'), ('s_1_3', 's_1_3'), ('s_1_9', 's_1_9'), ('s_1_37', 's_1_37'), ('s_1_38', 's_1_38'), ('s_1_39', 's_1_39'), ('s_1_1', 's_1_1'), ('s_3_3', 's_3_3'), ('s_15_37', 's_15_37'), ('s_15_38', 's_15_38'), ('s_15_15', 's_15_15'), ('s_27_9', 's_27_9'), ('s_27_38', 's_27_38'), ('s_27_19', 's_27_19'), ('s_27_30', 's_27_30'), ('s_27_27', 's_27_27'), ('s_38_39', 's_38_39'), ('s_38_38', 's_38_38'), ('s_9_9', 's_9_9'), ('s_37_11', 's_37_11'), ('s_37_19', 's_37_19'), ('s_37_30', 's_37_30'), ('s_37_37', 's_37_37'), ('s_11_39', 's_11_39'), ('s_11_11', 's_11_11'), ('s_19_39', 's_19_39'), ('s_19_22', 's_19_22'), ('s_19_19', 's_19_19'), ('s_30_39', 's_30_39'), ('s_30_22', 's_30_22'), ('s_30_30', 's_30_30'), ('s_39_22', 's_39_22'), ('s_39_39', 's_39_39'), ('s_22_22', 's_22_22')]</t>
+          <t>[(0, 2), (0, 's_0_2'), (0, 4), (0, 's_0_4'), (0, 5), (0, 's_0_5'), (0, 7), (0, 's_0_7'), (0, 8), (0, 's_0_8'), (0, 12), (0, 's_0_12'), (0, 13), (0, 's_0_13'), (0, 16), (0, 's_0_16'), (0, 18), (0, 's_0_18'), (0, 23), (0, 's_0_23'), (0, 32), (0, 's_0_32'), (0, 33), (0, 's_0_33'), (0, 36), (0, 's_0_36'), (0, 0), (2, 's_0_2'), (2, 12), (2, 's_2_12'), (2, 14), (2, 's_2_14'), (2, 18), (2, 's_2_18'), (2, 34), (2, 's_2_34'), (2, 2), ('s_0_2', 's_0_2'), (4, 's_0_4'), (4, 12), (4, 's_4_12'), (4, 17), (4, 's_4_17'), (4, 18), (4, 's_4_18'), (4, 21), (4, 's_4_21'), (4, 25), (4, 's_4_25'), (4, 26), (4, 's_4_26'), (4, 28), (4, 's_4_28'), (4, 29), (4, 's_4_29'), (4, 31), (4, 's_4_31'), (4, 34), (4, 's_4_34'), (4, 4), ('s_0_4', 's_0_4'), (5, 's_0_5'), (5, 6), (5, 's_5_6'), (5, 10), (5, 's_5_10'), (5, 20), (5, 's_5_20'), (5, 21), (5, 's_5_21'), (5, 23), (5, 's_5_23'), (5, 24), (5, 's_5_24'), (5, 26), (5, 's_5_26'), (5, 33), (5, 's_5_33'), (5, 35), (5, 's_5_35'), (5, 5), ('s_0_5', 's_0_5'), (7, 's_0_7'), (7, 1), (7, 's_1_7'), (7, 3), (7, 's_3_7'), (7, 8), (7, 's_7_8'), (7, 10), (7, 's_7_10'), (7, 13), (7, 's_7_13'), (7, 15), (7, 's_7_15'), (7, 20), (7, 's_7_20'), (7, 26), (7, 's_7_26'), (7, 27), (7, 's_7_27'), (7, 31), (7, 's_7_31'), (7, 32), (7, 's_7_32'), (7, 38), (7, 's_7_38'), (7, 7), ('s_0_7', 's_0_7'), (8, 's_0_8'), (8, 's_7_8'), (8, 12), (8, 's_8_12'), (8, 25), (8, 's_8_25'), (8, 28), (8, 's_8_28'), (8, 32), (8, 's_8_32'), (8, 35), (8, 's_8_35'), (8, 8), ('s_0_8', 's_0_8'), (12, 's_0_12'), (12, 's_2_12'), (12, 's_4_12'), (12, 's_8_12'), (12, 9), (12, 's_9_12'), (12, 17), (12, 's_12_17'), (12, 21), (12, 's_12_21'), (12, 24), (12, 's_12_24'), (12, 28), (12, 's_12_28'), (12, 34), (12, 's_12_34'), (12, 35), (12, 's_12_35'), (12, 37), (12, 's_12_37'), (12, 38), (12, 's_12_38'), (12, 12), ('s_0_12', 's_0_12'), (13, 's_0_13'), (13, 's_7_13'), (13, 9), (13, 's_9_13'), (13, 11), (13, 's_11_13'), (13, 14), (13, 's_13_14'), (13, 16), (13, 's_13_16'), (13, 18), (13, 's_13_18'), (13, 19), (13, 's_13_19'), (13, 21), (13, 's_13_21'), (13, 27), (13, 's_13_27'), (13, 29), (13, 's_13_29'), (13, 30), (13, 's_13_30'), (13, 35), (13, 's_13_35'), (13, 39), (13, 's_13_39'), (13, 13), ('s_0_13', 's_0_13'), (16, 's_0_16'), (16, 's_13_16'), (16, 1), (16, 's_1_16'), (16, 6), (16, 's_6_16'), (16, 10), (16, 's_10_16'), (16, 11), (16, 's_11_16'), (16, 18), (16, 's_16_18'), (16, 20), (16, 's_16_20'), (16, 22), (16, 's_16_22'), (16, 32), (16, 's_16_32'), (16, 36), (16, 's_16_36'), (16, 16), ('s_0_16', 's_0_16'), (18, 's_0_18'), (18, 's_2_18'), (18, 's_4_18'), (18, 's_13_18'), (18, 's_16_18'), (18, 6), (18, 's_6_18'), (18, 21), (18, 's_18_21'), (18, 24), (18, 's_18_24'), (18, 27), (18, 's_18_27'), (18, 30), (18, 's_18_30'), (18, 35), (18, 's_18_35'), (18, 36), (18, 's_18_36'), (18, 39), (18, 's_18_39'), (18, 18), ('s_0_18', 's_0_18'), (23, 's_0_23'), (23, 's_5_23'), (23, 1), (23, 's_1_23'), (23, 14), (23, 's_14_23'), (23, 19), (23, 's_19_23'), (23, 33), (23, 's_23_33'), (23, 37), (23, 's_23_37'), (23, 39), (23, 's_23_39'), (23, 23), ('s_0_23', 's_0_23'), (32, 's_0_32'), (32, 's_7_32'), (32, 's_8_32'), (32, 's_16_32'), (32, 3), (32, 's_3_32'), (32, 6), (32, 's_6_32'), (32, 14), (32, 's_14_32'), (32, 33), (32, 's_32_33'), (32, 37), (32, 's_32_37'), (32, 38), (32, 's_32_38'), (32, 32), ('s_0_32', 's_0_32'), (33, 's_0_33'), (33, 's_5_33'), (33, 's_23_33'), (33, 's_32_33'), (33, 6), (33, 's_6_33'), (33, 9), (33, 's_9_33'), (33, 22), (33, 's_22_33'), (33, 26), (33, 's_26_33'), (33, 36), (33, 's_33_36'), (33, 33), ('s_0_33', 's_0_33'), (36, 's_0_36'), (36, 's_16_36'), (36, 's_18_36'), (36, 's_33_36'), (36, 10), (36, 's_10_36'), (36, 14), (36, 's_14_36'), (36, 21), (36, 's_21_36'), (36, 29), (36, 's_29_36'), (36, 35), (36, 's_35_36'), (36, 38), (36, 's_36_38'), (36, 39), (36, 's_36_39'), (36, 36), ('s_0_36', 's_0_36'), ('s_2_12', 's_2_12'), (14, 3), (14, 20), (14, 37), (14, 39), (14, 's_2_14'), (14, 's_13_14'), (14, 's_14_23'), (14, 's_14_32'), (14, 's_14_36'), (14, 's_3_14'), (14, 's_14_20'), (14, 's_14_37'), (14, 's_14_39'), (14, 11), (14, 's_11_14'), (14, 15), (14, 's_14_15'), (14, 27), (14, 's_14_27'), (14, 35), (14, 's_14_35'), (14, 14), ('s_2_14', 's_2_14'), ('s_2_18', 's_2_18'), (34, 's_2_34'), (34, 's_4_34'), (34, 's_12_34'), (34, 10), (34, 's_10_34'), (34, 22), (34, 's_22_34'), (34, 24), (34, 's_24_34'), (34, 28), (34, 's_28_34'), (34, 34), ('s_2_34', 's_2_34'), ('s_4_12', 's_4_12'), (17, 20), (17, 38), (17, 's_4_17'), (17, 's_12_17'), (17, 's_17_20'), (17, 's_17_38'), (17, 22), (17, 's_17_22'), (17, 24), (17, 's_17_24'), (17, 25), (17, 's_17_25'), (17, 29), (17, 's_17_29'), (17, 30), (17, 's_17_30'), (17, 17), ('s_4_17', 's_4_17'), ('s_4_18', 's_4_18'), (21, 1), (21, 6), (21, 's_4_21'), (21, 's_5_21'), (21, 's_12_21'), (21, 's_13_21'), (21, 's_18_21'), (21, 's_21_36'), (21, 's_1_21'), (21, 's_6_21'), (21, 11), (21, 's_11_21'), (21, 27), (21, 's_21_27'), (21, 28), (21, 's_21_28'), (21, 31), (21, 's_21_31'), (21, 35), (21, 's_21_35'), (21, 38), (21, 's_21_38'), (21, 21), ('s_4_21', 's_4_21'), (25, 38), (25, 's_4_25'), (25, 's_8_25'), (25, 's_25_38'), (25, 's_17_25'), (25, 11), (25, 's_11_25'), (25, 19), (25, 's_19_25'), (25, 22), (25, 's_22_25'), (25, 28), (25, 's_25_28'), (25, 29), (25, 's_25_29'), (25, 25), ('s_4_25', 's_4_25'), (26, 38), (26, 's_4_26'), (26, 's_5_26'), (26, 's_7_26'), (26, 's_26_33'), (26, 's_26_38'), (26, 24), (26, 's_24_26'), (26, 27), (26, 's_26_27'), (26, 28), (26, 's_26_28'), (26, 35), (26, 's_26_35'), (26, 26), ('s_4_26', 's_4_26'), (28, 6), (28, 20), (28, 38), (28, 's_4_28'), (28, 's_8_28'), (28, 's_12_28'), (28, 's_6_28'), (28, 's_20_28'), (28, 's_21_28'), (28, 's_28_38'), (28, 's_28_34'), (28, 's_25_28'), (28, 's_26_28'), (28, 19), (28, 's_19_28'), (28, 24), (28, 's_24_28'), (28, 29), (28, 's_28_29'), (28, 30), (28, 's_28_30'), (28, 28), ('s_4_28', 's_4_28'), (29, 6), (29, 31), (29, 37), (29, 's_4_29'), (29, 's_13_29'), (29, 's_29_36'), (29, 's_6_29'), (29, 's_29_31'), (29, 's_29_37'), (29, 's_17_29'), (29, 's_25_29'), (29, 's_28_29'), (29, 22), (29, 's_22_29'), (29, 24), (29, 's_24_29'), (29, 35), (29, 's_29_35'), (29, 29), ('s_4_29', 's_4_29'), (31, 1), (31, 3), (31, 's_4_31'), (31, 's_7_31'), (31, 's_1_31'), (31, 's_3_31'), (31, 's_21_31'), (31, 10), (31, 's_10_31'), (31, 's_29_31'), (31, 30), (31, 's_30_31'), (31, 31), ('s_4_31', 's_4_31'), ('s_4_34', 's_4_34'), (6, 1), (6, 's_5_6'), (6, 's_6_16'), (6, 's_6_18'), (6, 's_6_32'), (6, 's_6_33'), (6, 's_1_6'), (6, 10), (6, 's_6_10'), (6, 19), (6, 's_6_19'), (6, 's_6_21'), (6, 24), (6, 's_6_24'), (6, 's_6_28'), (6, 's_6_29'), (6, 35), (6, 's_6_35'), (6, 6), ('s_5_6', 's_5_6'), (10, 's_5_10'), (10, 's_7_10'), (10, 's_10_16'), (10, 's_10_36'), (10, 's_6_10'), (10, 's_10_31'), (10, 's_10_34'), (10, 22), (10, 's_10_22'), (10, 24), (10, 's_10_24'), (10, 35), (10, 's_10_35'), (10, 10), ('s_5_10', 's_5_10'), (20, 1), (20, 3), (20, 's_5_20'), (20, 's_7_20'), (20, 's_16_20'), (20, 's_1_20'), (20, 's_3_20'), (20, 's_14_20'), (20, 's_17_20'), (20, 's_20_28'), (20, 37), (20, 's_20_37'), (20, 20), ('s_5_20', 's_5_20'), ('s_5_21', 's_5_21'), ('s_5_23', 's_5_23'), (24, 9), (24, 38), (24, 's_5_24'), (24, 's_12_24'), (24, 's_18_24'), (24, 's_6_24'), (24, 's_9_24'), (24, 's_24_38'), (24, 's_24_34'), (24, 's_17_24'), (24, 's_24_26'), (24, 's_24_28'), (24, 's_24_29'), (24, 's_10_24'), (24, 11), (24, 's_11_24'), (24, 22), (24, 's_22_24'), (24, 24), ('s_5_24', 's_5_24'), ('s_5_26', 's_5_26'), ('s_5_33', 's_5_33'), (35, 37), (35, 38), (35, 's_5_35'), (35, 's_8_35'), (35, 's_12_35'), (35, 's_13_35'), (35, 's_18_35'), (35, 's_35_36'), (35, 's_6_35'), (35, 's_21_35'), (35, 's_35_37'), (35, 's_35_38'), (35, 's_14_35'), (35, 's_26_35'), (35, 's_29_35'), (35, 's_10_35'), (35, 15), (35, 's_15_35'), (35, 27), (35, 's_27_35'), (35, 35), ('s_5_35', 's_5_35'), (1, 's_1_7'), (1, 's_1_16'), (1, 's_1_23'), (1, 3), (1, 's_1_3'), (1, 's_1_6'), (1, 9), (1, 's_1_9'), (1, 's_1_20'), (1, 's_1_21'), (1, 's_1_31'), (1, 37), (1, 's_1_37'), (1, 38), (1, 's_1_38'), (1, 39), (1, 's_1_39'), (1, 1), ('s_1_7', 's_1_7'), (3, 's_3_7'), (3, 's_3_32'), (3, 's_1_3'), (3, 's_3_14'), (3, 's_3_20'), (3, 's_3_31'), (3, 3), ('s_3_7', 's_3_7'), ('s_7_8', 's_7_8'), ('s_7_10', 's_7_10'), ('s_7_13', 's_7_13'), (15, 37), (15, 38), (15, 's_7_15'), (15, 's_15_37'), (15, 's_15_38'), (15, 's_14_15'), (15, 's_15_35'), (15, 15), ('s_7_15', 's_7_15'), ('s_7_20', 's_7_20'), ('s_7_26', 's_7_26'), (27, 9), (27, 38), (27, 19), (27, 's_7_27'), (27, 's_13_27'), (27, 's_18_27'), (27, 's_9_27'), (27, 's_21_27'), (27, 's_27_38'), (27, 's_14_27'), (27, 's_26_27'), (27, 's_27_35'), (27, 's_19_27'), (27, 30), (27, 's_27_30'), (27, 27), ('s_7_27', 's_7_27'), ('s_7_31', 's_7_31'), ('s_7_32', 's_7_32'), (38, 's_7_38'), (38, 's_12_38'), (38, 's_32_38'), (38, 's_36_38'), (38, 's_1_38'), (38, 's_21_38'), (38, 's_15_38'), (38, 's_17_38'), (38, 's_24_38'), (38, 's_25_38'), (38, 's_26_38'), (38, 's_27_38'), (38, 's_28_38'), (38, 's_35_38'), (38, 39), (38, 's_38_39'), (38, 38), ('s_7_38', 's_7_38'), ('s_8_12', 's_8_12'), ('s_8_25', 's_8_25'), ('s_8_28', 's_8_28'), ('s_8_32', 's_8_32'), ('s_8_35', 's_8_35'), (9, 's_9_12'), (9, 's_9_13'), (9, 's_9_33'), (9, 's_1_9'), (9, 's_9_24'), (9, 's_9_27'), (9, 9), ('s_9_12', 's_9_12'), ('s_12_17', 's_12_17'), ('s_12_21', 's_12_21'), ('s_12_24', 's_12_24'), ('s_12_28', 's_12_28'), ('s_12_34', 's_12_34'), ('s_12_35', 's_12_35'), (37, 's_12_37'), (37, 's_23_37'), (37, 's_32_37'), (37, 's_1_37'), (37, 's_20_37'), (37, 11), (37, 's_11_37'), (37, 's_14_37'), (37, 's_15_37'), (37, 19), (37, 's_19_37'), (37, 's_29_37'), (37, 30), (37, 's_30_37'), (37, 's_35_37'), (37, 37), ('s_12_37', 's_12_37'), ('s_12_38', 's_12_38'), ('s_9_13', 's_9_13'), (11, 39), (11, 's_11_13'), (11, 's_11_16'), (11, 's_11_21'), (11, 's_11_37'), (11, 's_11_39'), (11, 's_11_14'), (11, 's_11_25'), (11, 's_11_24'), (11, 11), ('s_11_13', 's_11_13'), ('s_13_14', 's_13_14'), ('s_13_16', 's_13_16'), ('s_13_18', 's_13_18'), (19, 39), (19, 's_13_19'), (19, 's_19_23'), (19, 's_6_19'), (19, 's_19_37'), (19, 's_19_39'), (19, 's_19_25'), (19, 's_19_28'), (19, 22), (19, 's_19_22'), (19, 's_19_27'), (19, 19), ('s_13_19', 's_13_19'), ('s_13_21', 's_13_21'), ('s_13_27', 's_13_27'), ('s_13_29', 's_13_29'), (30, 39), (30, 22), (30, 's_13_30'), (30, 's_18_30'), (30, 's_30_31'), (30, 's_30_37'), (30, 's_30_39'), (30, 's_17_30'), (30, 's_28_30'), (30, 's_27_30'), (30, 's_22_30'), (30, 30), ('s_13_30', 's_13_30'), ('s_13_35', 's_13_35'), (39, 's_13_39'), (39, 's_18_39'), (39, 's_23_39'), (39, 's_36_39'), (39, 's_1_39'), (39, 's_38_39'), (39, 's_11_39'), (39, 's_14_39'), (39, 's_19_39'), (39, 22), (39, 's_22_39'), (39, 's_30_39'), (39, 39), ('s_13_39', 's_13_39'), ('s_1_16', 's_1_16'), ('s_6_16', 's_6_16'), ('s_10_16', 's_10_16'), ('s_11_16', 's_11_16'), ('s_16_18', 's_16_18'), ('s_16_20', 's_16_20'), (22, 's_16_22'), (22, 's_22_33'), (22, 's_22_39'), (22, 's_22_34'), (22, 's_17_22'), (22, 's_22_25'), (22, 's_22_29'), (22, 's_10_22'), (22, 's_22_24'), (22, 's_19_22'), (22, 's_22_30'), (22, 22), ('s_16_22', 's_16_22'), ('s_16_32', 's_16_32'), ('s_16_36', 's_16_36'), ('s_6_18', 's_6_18'), ('s_18_21', 's_18_21'), ('s_18_24', 's_18_24'), ('s_18_27', 's_18_27'), ('s_18_30', 's_18_30'), ('s_18_35', 's_18_35'), ('s_18_36', 's_18_36'), ('s_18_39', 's_18_39'), ('s_1_23', 's_1_23'), ('s_14_23', 's_14_23'), ('s_19_23', 's_19_23'), ('s_23_33', 's_23_33'), ('s_23_37', 's_23_37'), ('s_23_39', 's_23_39'), ('s_3_32', 's_3_32'), ('s_6_32', 's_6_32'), ('s_14_32', 's_14_32'), ('s_32_33', 's_32_33'), ('s_32_37', 's_32_37'), ('s_32_38', 's_32_38'), ('s_6_33', 's_6_33'), ('s_9_33', 's_9_33'), ('s_22_33', 's_22_33'), ('s_26_33', 's_26_33'), ('s_33_36', 's_33_36'), ('s_10_36', 's_10_36'), ('s_14_36', 's_14_36'), ('s_21_36', 's_21_36'), ('s_29_36', 's_29_36'), ('s_35_36', 's_35_36'), ('s_36_38', 's_36_38'), ('s_36_39', 's_36_39'), ('s_1_3', 's_1_3'), ('s_1_6', 's_1_6'), ('s_1_9', 's_1_9'), ('s_1_20', 's_1_20'), ('s_1_21', 's_1_21'), ('s_1_31', 's_1_31'), ('s_1_37', 's_1_37'), ('s_1_38', 's_1_38'), ('s_1_39', 's_1_39'), ('s_3_14', 's_3_14'), ('s_3_20', 's_3_20'), ('s_3_31', 's_3_31'), ('s_6_10', 's_6_10'), ('s_6_19', 's_6_19'), ('s_6_21', 's_6_21'), ('s_6_24', 's_6_24'), ('s_6_28', 's_6_28'), ('s_6_29', 's_6_29'), ('s_6_35', 's_6_35'), ('s_9_24', 's_9_24'), ('s_9_27', 's_9_27'), ('s_14_20', 's_14_20'), ('s_17_20', 's_17_20'), ('s_20_28', 's_20_28'), ('s_20_37', 's_20_37'), ('s_11_21', 's_11_21'), ('s_21_27', 's_21_27'), ('s_21_28', 's_21_28'), ('s_21_31', 's_21_31'), ('s_21_35', 's_21_35'), ('s_21_38', 's_21_38'), ('s_10_31', 's_10_31'), ('s_29_31', 's_29_31'), ('s_30_31', 's_30_31'), ('s_11_37', 's_11_37'), ('s_14_37', 's_14_37'), ('s_15_37', 's_15_37'), ('s_19_37', 's_19_37'), ('s_29_37', 's_29_37'), ('s_30_37', 's_30_37'), ('s_35_37', 's_35_37'), ('s_15_38', 's_15_38'), ('s_17_38', 's_17_38'), ('s_24_38', 's_24_38'), ('s_25_38', 's_25_38'), ('s_26_38', 's_26_38'), ('s_27_38', 's_27_38'), ('s_28_38', 's_28_38'), ('s_35_38', 's_35_38'), ('s_38_39', 's_38_39'), ('s_11_39', 's_11_39'), ('s_14_39', 's_14_39'), ('s_19_39', 's_19_39'), ('s_22_39', 's_22_39'), ('s_30_39', 's_30_39'), ('s_11_14', 's_11_14'), ('s_14_15', 's_14_15'), ('s_14_27', 's_14_27'), ('s_14_35', 's_14_35'), ('s_10_34', 's_10_34'), ('s_22_34', 's_22_34'), ('s_24_34', 's_24_34'), ('s_28_34', 's_28_34'), ('s_17_22', 's_17_22'), ('s_17_24', 's_17_24'), ('s_17_25', 's_17_25'), ('s_17_29', 's_17_29'), ('s_17_30', 's_17_30'), ('s_11_25', 's_11_25'), ('s_19_25', 's_19_25'), ('s_22_25', 's_22_25'), ('s_25_28', 's_25_28'), ('s_25_29', 's_25_29'), ('s_24_26', 's_24_26'), ('s_26_27', 's_26_27'), ('s_26_28', 's_26_28'), ('s_26_35', 's_26_35'), ('s_19_28', 's_19_28'), ('s_24_28', 's_24_28'), ('s_28_29', 's_28_29'), ('s_28_30', 's_28_30'), ('s_22_29', 's_22_29'), ('s_24_29', 's_24_29'), ('s_29_35', 's_29_35'), ('s_10_22', 's_10_22'), ('s_10_24', 's_10_24'), ('s_10_35', 's_10_35'), ('s_11_24', 's_11_24'), ('s_22_24', 's_22_24'), ('s_15_35', 's_15_35'), ('s_27_35', 's_27_35'), ('s_19_22', 's_19_22'), ('s_19_27', 's_19_27'), ('s_27_30', 's_27_30'), ('s_22_30', 's_22_30')]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -1324,130 +1212,90 @@
           <t>[(0, 2), (0, 4), (0, 5), (0, 7), (0, 8), (0, 12), (0, 13), (0, 16), (0, 18), (0, 23), (0, 32), (0, 33), (0, 36), (0, 0), (2, 12), (2, 14), (2, 18), (2, 34), (2, 2), (4, 12), (4, 17), (4, 18), (4, 21), (4, 25), (4, 26), (4, 28), (4, 29), (4, 31), (4, 34), (4, 4), (5, 6), (5, 10), (5, 20), (5, 21), (5, 23), (5, 24), (5, 26), (5, 33), (5, 35), (5, 5), (7, 1), (7, 3), (7, 8), (7, 10), (7, 13), (7, 15), (7, 20), (7, 26), (7, 27), (7, 31), (7, 32), (7, 38), (7, 7), (8, 12), (8, 25), (8, 28), (8, 32), (8, 35), (8, 8), (12, 9), (12, 17), (12, 21), (12, 24), (12, 28), (12, 34), (12, 35), (12, 37), (12, 38), (12, 12), (13, 9), (13, 11), (13, 14), (13, 16), (13, 18), (13, 19), (13, 21), (13, 27), (13, 29), (13, 30), (13, 35), (13, 39), (13, 13), (16, 1), (16, 6), (16, 10), (16, 11), (16, 18), (16, 20), (16, 22), (16, 32), (16, 36), (16, 16), (18, 6), (18, 21), (18, 24), (18, 27), (18, 30), (18, 35), (18, 36), (18, 39), (18, 18), (23, 1), (23, 14), (23, 19), (23, 33), (23, 37), (23, 39), (23, 23), (32, 3), (32, 6), (32, 14), (32, 33), (32, 37), (32, 38), (32, 32), (33, 6), (33, 9), (33, 22), (33, 26), (33, 36), (33, 33), (36, 10), (36, 14), (36, 21), (36, 29), (36, 35), (36, 38), (36, 39), (36, 36), (14, 3), (14, 20), (14, 37), (14, 39), (14, 11), (14, 15), (14, 27), (14, 35), (14, 14), (34, 10), (34, 22), (34, 24), (34, 28), (34, 34), (17, 20), (17, 38), (17, 22), (17, 24), (17, 25), (17, 29), (17, 30), (17, 17), (21, 1), (21, 6), (21, 11), (21, 27), (21, 28), (21, 31), (21, 35), (21, 38), (21, 21), (25, 38), (25, 11), (25, 19), (25, 22), (25, 28), (25, 29), (25, 25), (26, 38), (26, 24), (26, 27), (26, 28), (26, 35), (26, 26), (28, 6), (28, 20), (28, 38), (28, 19), (28, 24), (28, 29), (28, 30), (28, 28), (29, 6), (29, 31), (29, 37), (29, 22), (29, 24), (29, 35), (29, 29), (31, 1), (31, 3), (31, 10), (31, 30), (31, 31), (6, 1), (6, 10), (6, 19), (6, 24), (6, 35), (6, 6), (10, 22), (10, 24), (10, 35), (10, 10), (20, 1), (20, 3), (20, 37), (20, 20), (24, 9), (24, 38), (24, 11), (24, 22), (24, 24), (35, 37), (35, 38), (35, 15), (35, 27), (35, 35), (1, 3), (1, 9), (1, 37), (1, 38), (1, 39), (1, 1), (3, 3), (15, 37), (15, 38), (15, 15), (27, 9), (27, 38), (27, 19), (27, 30), (27, 27), (38, 39), (38, 38), (9, 9), (37, 11), (37, 19), (37, 30), (37, 37), (11, 39), (11, 11), (19, 39), (19, 22), (19, 19), (30, 39), (30, 22), (30, 30), (39, 22), (39, 39), (22, 22)]</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="N6" t="n">
+        <v>538.46</v>
+      </c>
+      <c r="O6" t="n">
+        <v>132.14</v>
+      </c>
+      <c r="P6" t="n">
+        <v>20.84245073795319</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>1.908885955810547</v>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>{0: [4714, 4713, 4712, 4711, 385, 386, 388, 387], 2: [609, 4788], 's_0_2': [654], 4: [372, 820, 821, 5176, 5177, 5178], 's_0_4': [5116], 5: [958, 5285, 1078, 1077, 1076, 1075, 4775, 940], 's_0_5': [969], 7: [309, 310, 311, 313, 312, 569, 5462, 5461], 's_0_7': [4756], 8: [1138, 4726, 4727, 4728, 4729, 4730, 1137, 1136, 1135], 's_0_8': [714], 12: [942, 4803, 5194, 730, 731, 732, 5193], 's_0_12': [834], 13: [641, 4951, 537, 5012, 4952, 535, 536], 's_0_13': [5011], 16: [5341, 432, 431, 4654, 4653, 4652, 4651, 429, 430], 's_0_16': [459], 18: [595, 596, 4999, 4998, 4996, 4997], 's_0_18': [371], 23: [5389, 5386, 5387, 5388], 's_0_23': [5371], 32: [403, 5401, 5402, 703, 5405, 5404, 5403], 's_0_32': [5266], 33: [5327, 553, 552, 551, 4819, 4818, 4817, 550], 's_0_33': [4816], 36: [745, 4877, 759, 760, 670, 715, 4878], 's_0_36': [4876], 's_2_12': [4773], 14: [624, 625, 628, 627, 626], 's_2_14': [4697], 's_2_18': [580], 34: [4789, 910, 4848, 4849], 's_2_34': [700], 's_4_12': [822], 17: [1092, 5149, 1033, 1032, 5150], 's_4_17': [5134], 's_4_18': [597], 21: [4936, 4937, 4938, 1018, 1017, 1016, 1015, 4940, 4939], 's_4_21': [5179], 25: [987, 5225, 5224, 957, 4909, 956], 's_4_25': [4894], 26: [492, 5254, 5253, 5251, 5252], 's_4_26': [342], 28: [868, 4850, 1120, 1121, 5060, 867, 866, 5059], 's_4_28': [4954], 29: [716, 5086, 5087, 5090, 5089, 5088], 's_4_29': [446], 31: [5071, 5340, 279, 280, 282, 281], 's_4_31': [5131], 's_4_34': [835], 6: [898, 4685, 999, 5374, 1003, 1002, 1000, 1001], 's_5_6': [5344], 10: [4681, 864, 984, 985, 4684, 4683, 4682], 's_5_10': [939], 20: [508, 959, 5432, 5435, 5434, 5433], 's_5_20': [5465], 's_5_21': [4865], 's_5_23': [5390], 24: [702, 4790, 1045, 1046, 5268, 5269, 5270, 1047], 's_5_24': [5135], 's_5_26': [5255], 's_5_33': [4820], 35: [789, 793, 790, 791, 5222, 5223, 792, 5329, 5330], 's_5_35': [1108], 1: [5221, 447, 448, 5495, 5494, 5493, 5492], 's_1_7': [5355, 297], 3: [5447, 328, 5446], 's_3_7': [419], 's_7_8': [324], 's_7_10': [4696], 's_7_13': [538], 15: [5523, 5522], 's_7_15': [554], 's_7_20': [5477], 's_7_26': [5281, 357], 27: [672, 566, 568, 5147, 5162, 567], 's_7_27': [5146], 's_7_31': [4845], 's_7_32': [374, 373], 38: [4906, 4907, 5104, 779, 778, 777, 776, 4908], 's_7_38': [4891], 's_8_12': [804], 's_8_25': [1122], 's_8_28': [4805], 's_8_32': [1123], 's_8_35': [5331], 9: [5133, 402, 5132], 's_9_12': [747], 's_12_17': [5120], 's_12_21': [850], 's_12_24': [733], 's_12_28': [5058], 's_12_34': [819], 's_12_35': [4863], 37: [5105, 5478, 1061, 1062, 1063, 5480, 5479, 838], 's_12_37': [5195], 's_12_38': [5028], 's_9_13': [401], 11: [1106, 4970, 4967, 4968, 4969], 's_11_13': [491], 's_13_14': [4862], 's_13_16': [534], 's_13_18': [356], 19: [748, 5300, 913, 5298, 5297, 5299], 's_13_19': [5282], 's_13_21': [265], 's_13_27': [5207], 's_13_29': [521], 30: [5041, 5042, 971, 5044, 5043], 's_13_30': [581], 's_13_35': [5013], 39: [5027, 658, 657, 655, 656], 's_13_39': [5192], 's_1_16': [5191], 's_6_16': [1029], 's_10_16': [354], 's_11_16': [445], 's_16_18': [4981], 's_16_20': [493], 22: [5283, 5284, 879, 880, 881, 882], 's_16_22': [894], 's_16_32': [5356], 's_16_36': [669], 's_6_18': [4984], 's_18_21': [970], 's_18_24': [1031], 's_18_27': [4982], 's_18_30': [506], 's_18_35': [805], 's_18_36': [4758], 's_18_39': [4832], 's_1_23': [973], 's_14_23': [5372], 's_19_23': [418], 's_23_33': [523], 's_23_37': [673], 's_23_39': [643], 's_3_32': [404], 's_6_32': [5420], 's_14_32': [5313], 's_32_33': [5312], 's_32_37': [1048], 's_32_38': [5448], 's_6_33': [1014], 's_9_33': [5117], 's_22_33': [895], 's_26_33': [477], 's_33_36': [775], 's_10_36': [4623], 's_14_36': [4743], 's_21_36': [490], 's_29_36': [671], 's_35_36': [4698], 's_36_38': [460], 's_36_39': [4847], 's_3_14': [613], 's_14_20': [5417], 's_14_37': [5463], 's_14_39': [5118], 's_11_14': [610], 's_14_15': [5537], 's_14_27': [5072], 's_14_35': [5328], 's_10_34': [4760, 4759], 's_22_34': [4774], 's_24_34': [4834], 's_28_34': [865], 's_17_20': [5450], 's_17_38': [762], 's_17_22': [897], 's_17_24': [1093], 's_17_25': [5239, 5240], 's_17_29': [986], 's_17_30': [836], 's_1_21': [884, 5539], 's_6_21': [5209], 's_11_21': [911], 's_21_27': [4922], 's_21_28': [4895], 's_21_31': [295], 's_21_35': [4924], 's_21_38': [761], 's_25_38': [912], 's_11_25': [4910], 's_19_25': [972], 's_22_25': [837], 's_25_28': [4926, 4925], 's_25_29': [5074], 's_26_38': [5208, 717], 's_24_26': [5267], 's_26_27': [507], 's_26_28': [852], 's_26_35': [943], 's_6_28': [5373], 's_20_28': [5449], 's_28_38': [5464], 's_19_28': [5314], 's_24_28': [1105], 's_28_29': [1166], 's_28_30': [926], 's_6_29': [5075], 's_29_31': [296], 's_29_37': [1107], 's_22_29': [896], 's_24_29': [687, 686], 's_29_35': [5073], 's_1_31': [5236], 's_3_31': [5311], 's_10_31': [294], 's_30_31': [5056], 's_1_6': [5510], 's_6_10': [4745], 's_6_19': [5359], 's_6_24': [928], 's_6_35': [5315], 's_10_22': [4699], 's_10_24': [4804], 's_10_35': [4744], 's_1_20': [463, 5536], 's_3_20': [478], 's_20_37': [914], 's_9_24': [5148], 's_24_38': [763], 's_11_24': [4955], 's_22_24': [807], 's_35_37': [853], 's_35_38': [806], 's_15_35': [5538], 's_27_35': [582], 's_1_3': [327], 's_1_9': [5206], 's_1_37': [929], 's_1_38': [5509], 's_1_39': [5508], 's_15_37': [808], 's_15_38': [764], 's_9_27': [5161], 's_27_38': [4892], 's_19_27': [522], 's_27_30': [5057], 's_38_39': [5103], 's_11_37': [5015], 's_19_37': [5419], 's_30_37': [5045], 's_11_39': [640], 's_19_39': [612, 5357], 's_19_22': [583], 's_30_39': [4953, 746], 's_22_30': [941, 5014], 's_22_39': [642]}</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>{0: [4699, 923, 924], 2: [877, 4354], 4: [4399, 787], 5: [4517, 4519, 4518], 7: [4622, 4624, 4623, 803], 8: [834, 832, 833], 12: [578, 4384, 4383], 13: [939, 4565, 4563, 4564], 16: [4548, 954, 4549], 18: [4698, 4353, 773, 774], 23: [894, 893], 32: [4743, 4654, 699, 4653], 33: [638, 4609, 4608], 36: [4533, 4534], 14: [879, 4489, 878], 34: [982, 4324, 862], 17: [697, 4339, 4338], 21: [4368, 653, 652], 25: [802, 4308], 26: [4398, 594, 593], 28: [4444, 4442, 4443], 29: [4458, 698], 31: [758, 759], 6: [684, 4413, 683], 10: [4487, 4488, 863], 20: [967, 968], 24: [743, 742, 4293], 35: [4429, 668, 4428], 1: [4595, 4593, 4594], 3: [864, 4638, 4639], 15: [4684, 4683, 669], 27: [4579, 4578], 38: [729, 727, 728], 9: [4292, 623, 622], 37: [4474, 909, 4459, 908], 11: [953, 847, 938, 4369], 19: [848, 4414], 30: [712, 713, 4473], 39: [983, 4503, 4504], 22: [818, 817]}</t>
         </is>
       </c>
       <c r="T6" t="n">
-        <v>589.37</v>
+        <v>475</v>
       </c>
       <c r="U6" t="n">
-        <v>133.46</v>
+        <v>115</v>
       </c>
       <c r="V6" t="n">
-        <v>19.02752828598022</v>
+        <v>33.7059805393219</v>
       </c>
       <c r="W6" t="n">
-        <v>1.370362997055054</v>
+        <v>2.888305902481079</v>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>{0: [3536, 2042, 3460, 1546, 1547, 3458, 3459], 2: [3068, 3263, 1651, 3070, 3069, 1725, 3129], 's_0_2': [1545], 4: [1500, 3231, 3232, 3338, 1501], 's_0_4': [1592], 5: [2056, 3850, 1894, 3311, 3670, 1893, 3310, 1891, 1892], 's_0_5': [1848, 3535], 7: [1369, 1801, 1368, 1367, 3427, 3428, 3429, 3726, 1802], 's_0_7': [1562], 8: [3518, 3517], 's_0_8': [1638], 12: [1610, 1605, 1609, 1606, 1607, 1608], 's_0_12': [3473], 13: [4045, 3594, 1925, 1924, 3369, 3610, 1921, 1922, 1923], 's_0_13': [1818], 16: [1775, 1771, 1772, 1774, 1773], 's_0_16': [3474], 18: [3295, 3294, 3293, 1531, 1532, 3488, 1488, 1489, 1490], 's_0_18': [3457], 23: [2118, 2119, 3715, 3716], 's_0_23': [3521], 32: [2028, 1696, 1697, 3550, 3549, 1413, 3547, 3548], 's_0_32': [3278], 33: [2089, 2088, 2086, 2087], 's_0_33': [3565], 36: [3399, 3400, 2026, 3265, 1907, 3505, 1951, 1952], 's_0_36': [3415], 's_0_0': [3537], 's_2_12': [3218], 14: [3519, 1995, 1996, 1997, 3520, 3865, 2000, 1999, 1998], 's_2_14': [1980], 's_2_18': [1652], 34: [1515, 3053, 3051, 3052], 's_2_34': [1650], 's_2_2': [1845], 's_4_12': [3233], 17: [1516, 1517, 3637, 3668, 1520, 1519, 1518], 's_4_17': [3382], 's_4_18': [3308], 21: [1834, 3639, 1788, 3246, 3247, 3248, 3355, 1787, 3354, 1681], 's_4_21': [1411], 25: [1625, 1624, 1622, 1623], 's_4_25': [3353], 26: [3096, 3235, 1981, 3100, 3097, 3098, 3099], 's_4_26': [1441], 28: [1335, 1336, 3848, 1549, 1548, 3592, 1337, 1338, 3591], 's_4_28': [1321], 29: [1428, 1427, 3411, 1472, 3412, 3414, 3413], 's_4_29': [1487], 31: [1280, 1279, 1276, 1277, 1278], 's_4_31': [3216], 's_4_34': [1471, 1470], 's_4_4': [1426], 6: [3322, 3323, 2163, 2162, 3326, 2164, 3324, 3325], 's_5_6': [2101], 10: [3186, 3187, 1936, 3189, 3188], 's_5_10': [3250], 20: [3880, 3877, 3878, 3879], 's_5_20': [1985], 's_5_21': [3640], 's_5_23': [3700], 24: [3669, 1698, 3638, 1575, 1576, 1577, 1699, 1578], 's_5_24': [3849], 's_5_26': [1890], 's_5_33': [3341], 35: [3114, 1831, 1832, 1443, 3577, 3578, 3579, 1833], 's_5_35': [3384], 's_5_5': [2131], 1: [1309, 2104, 3761, 3756, 3757, 3758, 1864, 3759, 3760], 's_7_1': [1249], 3: [1684, 1653, 1654, 3771, 3772, 3773], 's_7_3': [1234], 's_7_8': [1398, 3561], 's_7_10': [3204], 's_7_13': [3219], 15: [3489, 1803], 's_7_15': [1727], 's_7_20': [3892], 's_7_26': [1816], 27: [1880, 3895, 1875, 1876, 1877, 1879, 1878], 's_7_27': [3249], 's_7_31': [3426], 's_7_32': [1412], 38: [3445, 3712, 1353, 1352, 1755, 1756, 1757, 3442, 3444, 3443], 's_7_38': [3487], 's_7_7': [3725], 's_8_12': [1593], 's_8_25': [3533], 's_8_28': [1322], 's_8_32': [1502], 's_8_35': [1458], 's_8_8': [1293, 3456], 9: [3923, 3925, 3924], 's_12_9': [1595], 's_12_17': [4043], 's_12_21': [3383], 's_12_24': [3158], 's_12_28': [3653], 's_12_34': [3128], 's_12_35': [3113], 37: [1715, 1712, 3685, 3684, 1714, 3714, 1713, 3728], 's_12_37': [3563], 's_12_38': [3713, 3698], 's_12_12': [3968], 's_13_9': [1955], 11: [3745, 3743, 3744], 's_13_11': [2043], 's_13_14': [3655], 's_13_16': [3954], 's_13_18': [1906], 19: [3787, 3788, 3791, 3790, 3789], 's_13_19': [3805], 's_13_21': [1817], 's_13_27': [1940], 's_13_29': [1937], 30: [1445, 1550, 3939, 3938, 3937, 3936], 's_13_30': [1895], 's_13_35': [3175], 39: [3940, 2015, 3730, 2012, 2013, 2014], 's_13_39': [3595, 1968], 's_13_13': [4046], 's_16_1': [3774], 's_16_6': [3309], 's_16_10': [1786], 's_16_11': [3729], 's_16_18': [3279], 's_16_20': [1790], 22: [3821, 3820, 3818, 1380, 3819, 1381, 1382, 1383, 1384, 3817], 's_16_22': [3834], 's_16_32': [3504], 's_16_36': [3564], 's_16_16': [3969], 's_18_6': [1591], 's_18_21': [1667], 's_18_24': [3367], 's_18_27': [1861], 's_18_30': [3967, 1355], 's_18_35': [3622], 's_18_36': [1966, 3220], 's_18_39': [2041, 3370], 's_18_18': [1530], 's_23_1': [2149], 's_23_14': [1969], 's_23_19': [3806], 's_23_33': [3775], 's_23_37': [3609, 1863], 's_23_39': [3671], 's_23_23': [2120], 's_32_3': [3534], 's_32_6': [3491], 's_32_14': [3580], 's_32_33': [2072], 's_32_37': [1953], 's_32_38': [1414], 's_32_32': [2057], 's_33_6': [3611], 's_33_9': [2074], 's_33_22': [3836], 's_33_26': [2071], 's_33_36': [3266], 's_33_33': [3881], 's_36_10': [3190], 's_36_14': [1862], 's_36_21': [1847], 's_36_29': [3398], 's_36_35': [3115], 's_36_38': [1967], 's_36_39': [3385], 's_36_36': [3176], 's_14_3': [3864], 's_14_20': [1835], 's_14_37': [1938], 's_14_39': [3625], 's_14_11': [1954], 's_14_15': [1668], 's_14_27': [3130], 's_14_35': [3160], 's_14_14': [2920], 's_34_10': [1350], 's_34_22': [3067], 's_34_24': [3143], 's_34_28': [1320], 's_34_34': [1230], 's_17_20': [1504], 's_17_38': [3652], 's_17_22': [3802], 's_17_24': [3217], 's_17_25': [3503], 's_17_29': [3277], 's_17_30': [4102], 's_17_17': [3907], 's_21_1': [1789], 's_21_6': [1366], 's_21_11': [1819], 's_21_27': [3654], 's_21_28': [3262, 3261], 's_21_31': [1261], 's_21_35': [1728], 's_21_38': [1982], 's_21_21': [1201], 's_25_38': [3368], 's_25_11': [1639], 's_25_19': [3803], 's_25_22': [1640], 's_25_28': [3608], 's_25_29': [1637], 's_25_25': [1626], 's_26_38': [1740], 's_26_24': [1560], 's_26_27': [3234], 's_26_28': [3112, 3111], 's_26_35': [1785], 's_26_26': [3236], 's_28_6': [3307], 's_28_20': [3893], 's_28_38': [1323], 's_28_19': [1564], 's_28_24': [1563], 's_28_29': [3396], 's_28_30': [1475], 's_28_28': [3471], 's_29_6': [1292], 's_29_31': [1262], 's_29_37': [3727, 1444, 3667], 's_29_22': [3532], 's_29_24': [3397], 's_29_35': [3472], 's_29_29': [1232], 's_31_1': [3651], 's_31_3': [1264], 's_31_10': [3201], 's_31_30': [3951], 's_31_31': [3666], 's_6_1': [3701], 's_6_10': [1741], 's_6_19': [2179], 's_6_24': [1561], 's_6_35': [1442], 's_6_6': [3401], 's_10_22': [1396, 1397], 's_10_24': [3202], 's_10_35': [1860], 's_10_10': [3185], 's_20_1': [1534], 's_20_3': [1324], 's_20_37': [1729], 's_20_20': [3876], 's_24_9': [3908], 's_24_38': [1758], 's_24_11': [1669], 's_24_22': [1579], 's_24_24': [3022], 's_35_37': [1908], 's_35_38': [3502], 's_35_15': [3490], 's_35_27': [3264], 's_35_35': [3576], 's_1_3': [1594], 's_1_9': [2105], 's_1_37': [3804], 's_1_38': [1429], 's_1_39': [3866], 's_1_1': [2299], 's_3_3': [3699], 's_15_37': [1804], 's_15_38': [1742], 's_15_15': [3624], 's_27_9': [1970, 3910], 's_27_38': [3084], 's_27_19': [1909], 's_27_30': [3894, 1820], 's_27_27': [3039], 's_38_39': [3430], 's_38_38': [3697, 3696], 's_9_9': [1745], 's_37_11': [1984], 's_37_19': [1744], 's_37_30': [3983, 3984], 's_37_37': [4088], 's_11_39': [2058], 's_11_11': [1759], 's_19_39': [2029], 's_19_22': [2239], 's_19_19': [3792], 's_30_39': [1910, 3970], 's_30_22': [1655], 's_30_30': [1551], 's_39_22': [3835], 's_39_39': [2016], 's_22_22': [3127]}</t>
+          <t>[564, 544, 544, 531, 544, 582, 537, 532, 491, 513, 534, 549, 558, 499, 503, 527, 526, 533, 512, 552, 569, 578, 540, 504, 503, 520, 551, 543, 515, 537, 530, 613, 569, 570, 566, 523, 567, 508, 552, 569, 573, 559, 540, 578, 506, 518, 533, 546, 600, 527, 527, 527, 521, 520, 570, 534, 541, 505, 538, 575, 509, 537, 544, 494, 523, 524, 548, 509, 522, 546, 494, 475, 521, 510, 523, 549, 495, 520, 571, 554, 523, 535, 600, 535, 544, 508, 505, 597, 578, 547, 531, 539, 559, 554, 577, 520, 521, 588, 529, 548]</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>{0: [1407, 4985, 1406, 4986], 2: [5077], 4: [1393, 1391, 1392], 5: [5060, 1302, 5061, 1301], 7: [5331, 1271, 1272, 1273], 8: [5210, 5212, 5211], 12: [5332, 5092, 1453, 1452], 13: [1256, 1258, 1257], 16: [1061, 5121, 5120], 18: [1467, 5106, 5107], 23: [5270, 1076, 1077], 32: [1121, 1123, 1122], 33: [1241, 5045, 5047, 5046], 36: [1211, 1212], 14: [5075, 1332, 1331, 5076], 34: [1345, 1421, 4957], 17: [5301, 5302], 21: [5197, 5195, 5196], 25: [1362, 5257], 26: [5166, 1361], 28: [1422, 5137], 29: [5287, 5286], 31: [1167, 5361, 5360], 6: [5015, 1377, 1376, 5016], 10: [5032, 1166, 5030, 5031], 20: [5136, 1197, 1196], 24: [1346, 1347], 35: [1228, 5152, 1227, 5151], 1: [1152, 1151], 3: [5345, 5346], 15: [4926, 1137, 1136], 27: [5391, 1288, 1287], 38: [5242, 5240, 5241, 1242], 9: [5090, 5091], 37: [5317, 1138, 5316], 11: [5256, 5255, 1062], 19: [1182, 5272, 5271], 30: [5181, 1318, 1317], 39: [5225, 5227, 5226], 22: [5122, 1437, 1436]}</t>
+          <t>[122, 132, 129, 126, 128, 127, 135, 131, 143, 126, 134, 126, 136, 135, 138, 133, 134, 139, 147, 135, 129, 119, 139, 136, 130, 131, 135, 141, 123, 132, 139, 149, 130, 129, 128, 133, 115, 127, 125, 132, 125, 130, 121, 129, 134, 126, 142, 142, 126, 133, 131, 132, 125, 132, 131, 129, 132, 125, 122, 143, 140, 130, 136, 136, 132, 148, 128, 137, 138, 129, 140, 128, 137, 131, 127, 125, 135, 130, 128, 128, 124, 131, 137, 158, 139, 132, 129, 135, 124, 131, 137, 130, 135, 145, 131, 138, 126, 122, 127, 132]</t>
         </is>
       </c>
       <c r="Z6" t="n">
-        <v>532</v>
+        <v>27.14027161681223</v>
       </c>
       <c r="AA6" t="n">
-        <v>118</v>
+        <v>6.853473645539246</v>
       </c>
       <c r="AB6" t="n">
-        <v>33.19077444076538</v>
+        <v>1</v>
       </c>
       <c r="AC6" t="n">
-        <v>1.101470947265625</v>
+        <v>1</v>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>[{0: [4487, 683, 684, 4743, 745, 5196, 5195, 5194, 5193, 747, 746], 2: [985, 987, 986], 's_0_2': [972], 4: [4972, 1166, 5178, 1375, 1376, 5181, 5179, 5180], 's_0_4': [867], 5: [4732, 4731, 4730, 999, 1000, 4970, 716, 4968, 4969], 's_0_5': [5073], 7: [1342, 4356, 551, 550, 549, 548, 4352, 4353, 4354, 4355], 's_0_7': [4472], 8: [4414, 4744, 4459, 877, 4460, 879, 878], 's_0_8': [4413, 668], 12: [1073, 5150, 1077, 1074, 1075, 5061, 1076, 5060], 's_0_12': [1047], 13: [4985, 4984, 4442, 911, 910, 909, 4443, 4564, 863], 's_0_13': [4457], 16: [625, 624, 623, 622, 4398, 4400, 4281, 4399, 4280, 1057], 's_0_16': [4637], 18: [4519, 957, 953, 5045, 5044, 956, 954, 955], 's_0_18': [5209], 23: [504, 5103, 5102, 505, 5027, 5026, 506], 's_0_23': [4742], 32: [4666, 834, 744, 4667, 789, 4668], 's_0_32': [669], 33: [1164, 4761, 400, 4757, 4758, 4760, 4759], 's_0_33': [580], 36: [1287, 1282, 4746, 1283, 1284, 1285, 1286, 4956, 4955], 's_0_36': [5211], 's_0_0': [5197], 's_2_12': [5300], 14: [941, 5162, 656, 654, 4909, 4908, 655], 's_2_14': [4894], 's_2_18': [5135], 34: [1436, 1571, 5108, 5105, 5106, 5107], 's_2_34': [5120], 's_2_2': [5285], 's_4_12': [1181], 17: [1328, 1329, 5152, 4491, 1331, 1330], 's_4_17': [1392], 's_4_18': [1001], 21: [4879, 1314, 1315, 4881, 4880, 5224, 5225, 1017, 1016, 1015], 's_4_21': [1167], 25: [4639, 1345, 4867, 4866, 1210, 4638, 1209, 4640], 's_4_25': [4882], 26: [804, 806, 4832, 4833, 805], 's_4_26': [5163], 28: [848, 1107, 1106, 4925, 5210, 849, 850, 4924], 's_4_28': [1092], 29: [4565, 1089, 1090, 4942, 1405, 1406, 5001, 5000, 1091], 's_4_29': [4897], 31: [881, 4417, 5089, 5090, 1418, 1419, 1420, 1421, 5092, 5091], 's_4_31': [882], 's_4_34': [1302], 's_4_4': [5136], 6: [923, 924, 4699, 4702, 4701, 4700], 's_5_6': [1374], 10: [4295, 1358, 4987, 4507, 1510, 1509, 1508, 4296, 4297, 1507], 's_5_10': [1524], 20: [5016, 5015, 5014, 4937, 4938, 731, 5013], 's_5_20': [640], 's_5_21': [4717, 4716], 's_5_23': [581], 24: [1435, 4822, 4821, 4818, 4819, 1194, 4820], 's_5_24': [1495], 's_5_26': [5028], 's_5_33': [1014], 35: [4474, 4715, 4802, 4803, 4804, 1045, 1044, 4506, 4505, 1043], 's_5_35': [4685], 's_5_5': [4733], 1: [821, 536, 4550, 4997, 4998, 4549, 818, 819, 820], 's_7_1': [5057], 3: [686, 835, 4954, 4952, 4953], 's_7_3': [4967], 's_7_8': [967], 's_7_10': [4357], 's_7_13': [563], 15: [4683, 4862, 610, 4682, 609], 's_7_15': [4877], 's_7_20': [4922], 's_7_26': [4847], 27: [4490, 1103, 4489, 893, 896, 895, 5104, 894], 's_7_27': [908], 's_7_31': [1298], 's_7_32': [564], 38: [4787, 4788, 4792, 4791, 4790, 4789], 's_7_38': [4772], 's_7_7': [4387], 's_8_12': [1058], 's_8_25': [4624], 's_8_28': [4729], 's_8_32': [833, 832], 's_8_35': [1088], 's_8_8': [4249], 9: [4669, 1119, 4670], 's_12_9': [1059], 's_12_17': [5151], 's_12_21': [1032], 's_12_24': [4805], 's_12_28': [5075], 's_12_34': [1031], 's_12_35': [4745], 37: [728, 4593, 4850, 4712, 4713, 4849, 4848, 729, 730], 's_12_37': [4835], 's_12_38': [4775], 's_12_12': [1078], 's_13_9': [4654], 11: [5223, 762, 758, 759, 760, 761], 's_13_11': [4473], 's_13_14': [4563, 653], 's_13_16': [593], 's_13_18': [4444], 19: [4607, 4608, 4611, 4610, 4609], 's_13_19': [714, 713], 's_13_21': [1150], 's_13_27': [4999], 's_13_29': [1061], 30: [4432, 1238, 4428, 4429, 4431, 4430], 's_13_30': [637], 's_13_35': [5029, 1046], 39: [701, 1268, 5058, 1269, 1270, 776, 4939, 4940, 4941, 1271], 's_13_39': [926], 's_13_13': [698], 's_16_1': [817], 's_16_6': [4385, 4384], 's_16_10': [1312], 's_16_11': [4235, 4234, 757], 's_16_18': [938], 's_16_20': [596, 4892], 22: [1252, 1256, 1255, 4641, 1253, 1254], 's_16_22': [4401], 's_16_32': [4652], 's_16_36': [1267], 's_16_16': [4310], 's_18_6': [4534], 's_18_21': [5239], 's_18_24': [865, 4864], 's_18_27': [5074], 's_18_30': [4415], 's_18_35': [4504], 's_18_36': [5046], 's_18_39': [1121], 's_18_18': [866], 's_23_1': [521], 's_23_14': [5087, 567], 's_23_19': [4592], 's_23_33': [4816], 's_23_37': [490, 489], 's_23_39': [641], 's_23_23': [4981], 's_32_3': [790], 's_32_6': [4684], 's_32_14': [4728], 's_32_33': [399], 's_32_37': [534], 's_32_38': [429], 's_32_32': [4665], 's_33_6': [1224], 's_33_9': [969], 's_33_22': [4776], 's_33_26': [595], 's_33_36': [1149], 's_33_33': [4726], 's_36_10': [4311, 4312], 's_36_14': [970], 's_36_21': [5226, 5241], 's_36_29': [1391, 4957], 's_36_35': [4521], 's_36_38': [1179], 's_36_39': [4386], 's_36_36': [4236], 's_14_3': [5118], 's_14_20': [670], 's_14_37': [4773], 's_14_39': [5043], 's_14_11': [657], 's_14_15': [611], 's_14_27': [5059], 's_14_35': [4910], 's_14_14': [687], 's_34_10': [4958], 's_34_22': [5121], 's_34_24': [1570], 's_34_28': [1137], 's_34_34': [1467], 's_17_20': [5031], 's_17_38': [4777], 's_17_22': [4536], 's_17_24': [1344], 's_17_25': [4911], 's_17_29': [4986], 's_17_30': [1208, 4551], 's_17_17': [5153], 's_21_1': [822], 's_21_6': [1299], 's_21_11': [4878], 's_21_27': [897], 's_21_28': [1122], 's_21_31': [4567], 's_21_35': [1313], 's_21_38': [1300], 's_21_21': [1316, 1317, 1318], 's_25_38': [1225], 's_25_11': [4623], 's_25_19': [774], 's_25_22': [4896], 's_25_28': [4926], 's_25_29': [1360], 's_25_25': [4927], 's_26_38': [715], 's_26_24': [4834, 880], 's_26_27': [5119], 's_26_28': [4653], 's_26_35': [535], 's_26_26': [807], 's_28_6': [864], 's_28_20': [5030], 's_28_38': [1030], 's_28_19': [4594], 's_28_24': [1105], 's_28_29': [4895], 's_28_30': [4488, 773], 's_28_28': [4458], 's_29_6': [1404], 's_29_31': [5077], 's_29_37': [4851], 's_29_22': [4836], 's_29_24': [1390], 's_29_35': [4535], 's_29_29': [4865], 's_31_1': [851], 's_31_3': [5088], 's_31_10': [4657], 's_31_30': [4462, 4461], 's_31_31': [4582], 's_6_1': [4579], 's_6_10': [4687], 's_6_19': [939], 's_6_24': [1434], 's_6_35': [984], 's_6_6': [1449], 's_10_22': [4626, 4627], 's_10_24': [4763, 1480, 4837], 's_10_35': [4613, 4612, 1343], 's_10_10': [4598], 's_20_1': [5012], 's_20_3': [430], 's_20_37': [700], 's_20_20': [416], 's_24_9': [1120], 's_24_38': [1465], 's_24_11': [775], 's_24_22': [4686], 's_24_24': [1554], 's_35_37': [925], 's_35_38': [520], 's_35_15': [4817], 's_35_27': [1028], 's_35_35': [1148], 's_1_3': [836], 's_1_9': [1104], 's_1_37': [4548], 's_1_38': [565, 566], 's_1_39': [671], 's_1_1': [5072], 's_3_3': [491], 's_15_37': [579], 's_15_38': [459], 's_15_15': [4727], 's_27_9': [1118], 's_27_38': [4774], 's_27_19': [968], 's_27_30': [1223], 's_27_27': [4475], 's_38_39': [1240], 's_38_38': [1359], 's_9_9': [4671], 's_37_11': [4863], 's_37_19': [594], 's_37_30': [743], 's_37_37': [4518], 's_11_39': [777], 's_11_11': [5222], 's_19_39': [4596], 's_19_22': [1239], 's_19_19': [4606], 's_30_39': [4416], 's_30_22': [4476], 's_30_30': [802], 's_39_22': [4566], 's_39_39': [1272], 's_22_22': [4251]}, {0: [909, 625, 1197, 913, 910, 911, 626, 5133, 5134, 5210, 5209, 912], 2: [686, 491, 5026, 5027], 's_0_2': [5072], 4: [430, 5206, 849, 850, 342, 341, 4996, 4997, 4848, 4847, 610], 's_0_4': [4879], 5: [779, 5466, 687, 688, 5465, 5464, 5463], 's_0_5': [914], 7: [5583, 4669, 969, 970, 971, 972, 973, 988, 989, 5585, 5584], 's_0_7': [4849], 8: [4652, 4655, 4653, 924, 4654], 's_0_8': [4549], 12: [326, 5105, 5104, 5101, 5102, 5103, 699, 700, 701], 's_0_12': [4953], 13: [4711, 400, 401, 402, 837, 5300, 5299, 5298, 5297, 403], 's_0_13': [5284], 16: [4591, 4592, 943, 942, 941, 940, 4714, 4713, 4712, 519], 's_0_16': [5389], 18: [804, 805, 5119, 5058, 807, 806], 's_0_18': [5208], 23: [5525, 1059, 1060, 1064, 1061, 1063, 1062], 's_0_23': [5360], 32: [627, 5598, 4667, 4666, 444, 445, 446, 447, 734, 733, 5328, 5327], 's_0_32': [732], 33: [5237, 462, 5311, 5312, 5315, 1002, 5314, 5313], 's_0_33': [5316], 36: [553, 550, 5043, 5042, 552, 551], 's_0_36': [5057], 's_0_0': [5211], 's_2_12': [5117], 14: [4801, 504, 505, 506, 507, 508, 5447, 554, 5522, 1049, 5524, 5523], 's_2_14': [4981], 's_2_18': [671], 34: [4968, 4967, 4950, 4951, 4952], 's_2_34': [371], 's_2_2': [4982], 's_4_12': [4803], 17: [4621, 354, 355, 387, 386, 4906], 's_4_17': [5221], 's_4_18': [4774], 21: [775, 5028, 778, 777, 4971, 4970, 4969, 776], 's_4_21': [851], 25: [4639, 4635, 4636, 4638, 4637], 's_4_25': [4623], 26: [944, 5434, 5433, 5432, 5267, 5462, 494, 492, 5341, 493], 's_4_26': [5161], 28: [5223, 4563, 729, 643, 642, 730, 641, 4863, 640], 's_4_28': [745], 29: [5180, 954, 955, 5146, 5147, 5148, 5149, 1077, 5150, 957, 956], 's_4_29': [4684], 31: [1000, 1138, 1123, 4894, 1137, 4895, 1136], 's_4_31': [865], 's_4_34': [416], 's_4_4': [5281], 6: [5061, 5060, 703, 702, 5163, 821, 5059], 's_5_6': [5478], 10: [5405, 5404, 673, 5357, 5356, 5355, 206, 207, 5403, 208], 's_5_10': [838], 20: [1154, 1153, 1152, 1151, 1149, 4700, 1089, 4610, 4609, 1150, 4608, 4607, 4606], 's_5_20': [1167, 1168], 's_5_21': [5388, 853], 's_5_23': [5480], 24: [582, 4845, 5179, 5178, 295, 250, 251, 5175, 5177, 5176], 's_5_24': [5162], 's_5_26': [929], 's_5_33': [1048], 35: [5372, 5373, 823, 927, 1119, 1120, 1121, 5371, 1122, 5240, 5239, 822], 's_5_35': [613], 's_5_5': [5481], 1: [4729, 5285, 5075, 1109, 1108, 4730, 1105, 1106, 1107], 's_7_1': [5510], 3: [5450, 854, 1124, 5599, 5600], 's_7_3': [959], 's_7_8': [4699], 's_7_10': [674], 's_7_13': [987], 15: [4772, 4773, 715, 926, 4909, 4908], 's_7_15': [4999], 's_7_20': [968], 's_7_26': [749], 27: [4819, 895, 899, 898, 897, 896], 's_7_27': [5554], 's_7_31': [985], 's_7_32': [719], 38: [373, 372, 5086, 5087, 879, 880, 881, 5089, 5088], 's_7_38': [4804], 's_7_7': [659], 's_8_12': [714], 's_8_25': [774], 's_8_28': [594], 's_8_32': [654], 's_8_35': [4670], 's_8_8': [1224], 9: [1046, 1047, 5269, 5270], 's_12_9': [5120], 's_12_17': [5041], 's_12_21': [4998], 's_12_24': [5116], 's_12_28': [4698], 's_12_34': [311], 's_12_35': [1092], 37: [534, 535, 4937, 1196, 5015, 5014, 5013, 731, 4938], 's_12_37': [566, 567], 's_12_38': [611], 's_12_12': [698], 's_13_9': [928], 11: [4577, 4878, 4877, 414, 4876, 415], 's_13_11': [4846, 475], 's_13_14': [5191], 's_13_16': [4757], 's_13_18': [836], 19: [1271, 1270, 4791, 4790, 4789, 4861, 4862, 579, 580, 4788], 's_13_19': [370], 's_13_21': [763], 's_13_27': [5359, 1017], 's_13_29': [672], 30: [596, 595, 835, 834, 4815, 4816, 4817, 4818], 's_13_30': [294], 's_13_35': [5224], 39: [4745, 4741, 4742, 4744, 624, 4743], 's_13_39': [309], 's_13_13': [5011], 's_16_1': [4760], 's_16_6': [5044], 's_16_10': [5419], 's_16_11': [458], 's_16_18': [789], 's_16_20': [248], 22: [4726, 278, 279, 282, 281, 4995, 280], 's_16_22': [443, 4501], 's_16_32': [669], 's_16_36': [565], 's_16_16': [459], 's_18_6': [791], 's_18_21': [5253], 's_18_24': [656], 's_18_27': [5509, 808], 's_18_30': [4939], 's_18_35': [5193], 's_18_36': [716], 's_18_39': [4759], 's_18_18': [803], 's_23_1': [4865], 's_23_14': [5630], 's_23_19': [1075, 4850], 's_23_33': [5330], 's_23_37': [5030], 's_23_39': [1074], 's_23_23': [4925], 's_32_3': [5538], 's_32_6': [704], 's_32_14': [764], 's_32_33': [598], 's_32_37': [4922], 's_32_38': [5266], 's_32_32': [644], 's_33_6': [718], 's_33_9': [958], 's_33_22': [297], 's_33_26': [432], 's_33_36': [5282], 's_33_33': [223], 's_36_10': [568], 's_36_14': [628, 5417], 's_36_21': [761], 's_36_29': [521, 522, 5132, 431], 's_36_35': [5387], 's_36_38': [536], 's_36_39': [4802], 's_36_36': [5252], 's_14_3': [869], 's_14_20': [5615], 's_14_37': [4787], 's_14_39': [4682], 's_14_11': [4831], 's_14_15': [4907], 's_14_27': [5539], 's_14_35': [5521, 463], 's_14_14': [539, 5492], 's_34_10': [4965], 's_34_22': [191], 's_34_24': [265], 's_34_28': [655], 's_34_34': [56], 's_17_20': [428], 's_17_38': [5071], 's_17_22': [4921], 's_17_24': [4905], 's_17_25': [399], 's_17_29': [5131], 's_17_30': [340], 's_17_17': [4891], 's_21_1': [1076], 's_21_6': [1256], 's_21_11': [760], 's_21_27': [5329], 's_21_28': [5418], 's_21_31': [1165], 's_21_35': [4956], 's_21_38': [866], 's_21_21': [1211], 's_25_38': [4624], 's_25_11': [564], 's_25_19': [4622], 's_25_22': [293], 's_25_28': [744], 's_25_29': [939], 's_25_25': [159], 's_26_38': [5386], 's_26_24': [537], 's_26_27': [883], 's_26_28': [5268], 's_26_35': [658], 's_26_26': [5551], 's_28_6': [5448], 's_28_20': [4593], 's_28_38': [5073], 's_28_19': [4832], 's_28_24': [5192], 's_28_29': [4864], 's_28_30': [670], 's_28_28': [5508], 's_29_6': [852], 's_29_31': [5151], 's_29_37': [1181, 1182, 5195], 's_29_22': [296], 's_29_24': [266], 's_29_35': [5225], 's_29_29': [953], 's_31_1': [5000], 's_31_3': [1139], 's_31_10': [5420], 's_31_30': [820], 's_31_31': [4926], 's_6_1': [1001], 's_6_10': [5358], 's_6_19': [1090, 1091], 's_6_24': [747], 's_6_35': [867], 's_6_6': [1346], 's_10_22': [5160], 's_10_24': [205], 's_10_35': [538], 's_10_10': [4920], 's_20_1': [5390], 's_20_3': [1169], 's_20_37': [5121], 's_20_20': [5691], 's_24_9': [1032], 's_24_38': [986], 's_24_11': [4875], 's_24_22': [5025], 's_24_24': [5055], 's_35_37': [5106], 's_35_38': [882], 's_35_15': [4910], 's_35_27': [5494], 's_35_35': [5370, 268], 's_1_3': [5570], 's_1_9': [4940, 1045], 's_1_37': [5076], 's_1_38': [5090, 1166], 's_1_39': [1044], 's_1_1': [4731], 's_3_3': [5601], 's_15_37': [746], 's_15_38': [4954], 's_15_15': [790], 's_27_9': [5254], 's_27_38': [4984], 's_27_19': [1014], 's_27_30': [4924], 's_27_27': [1030], 's_38_39': [894], 's_38_38': [374], 's_9_9': [4955], 's_37_11': [460], 's_37_19': [581], 's_37_30': [520], 's_37_37': [5046], 's_11_39': [385], 's_11_11': [413], 's_19_39': [4758], 's_19_22': [4727], 's_19_19': [578], 's_30_39': [220], 's_30_22': [4800], 's_30_30': [325], 's_39_22': [4756], 's_39_39': [4746], 's_22_22': [4470]}, {0: [1047, 5101, 5102, 5254, 867, 5179, 5178, 5193, 747, 5103], 2: [5149, 838, 836, 837], 's_0_2': [5239], 4: [4729, 972, 971, 969, 4954, 4955, 970], 's_0_4': [866], 5: [5298, 612, 4487, 608, 609, 611, 610], 's_0_5': [717], 7: [4668, 4667, 4666, 297, 295, 296, 294, 4665], 's_0_7': [281], 8: [446, 443, 444, 445], 's_0_8': [4996, 341], 12: [4560, 4561, 821, 820, 458, 4562, 4563, 4564, 819, 818], 's_0_12': [822], 13: [4635, 958, 519, 4636, 4637, 4638, 1033, 5344, 4639, 1029, 1030, 1031, 1032], 's_0_13': [5150, 942, 943], 16: [325, 4891, 401, 5389, 402, 5388, 5387, 5386, 403], 's_0_16': [792, 5314, 913], 18: [703, 5433, 5434, 5435, 1078, 5330, 1119, 1120, 1121, 1122, 5240, 1002], 's_0_18': [5255], 23: [912, 5224, 5222, 5223], 's_0_23': [852], 32: [5086, 5055, 326, 5025, 192, 189, 190, 191], 's_0_32': [5116], 33: [5118, 5119, 896, 894, 4605, 4606, 895, 4607, 4608, 4609], 's_0_33': [806], 36: [4997, 658, 5357, 655, 657, 656], 's_0_36': [5133], 's_0_0': [521], 's_2_12': [5044], 14: [5269, 371, 372, 373, 311, 312, 807, 4951, 5268, 5267, 5266], 's_2_14': [5329], 's_2_18': [823], 34: [955, 956, 4984, 5074, 881], 's_2_34': [882], 's_2_2': [5523], 's_4_12': [4714], 17: [4939, 776, 5207, 5208, 777], 's_4_17': [4969], 's_4_18': [5209], 21: [4850, 940, 4848, 4847, 219, 220, 4849, 4846, 4845], 's_4_21': [4775], 25: [551, 5026, 491, 5042, 4924, 761, 5043], 's_4_25': [805], 26: [624, 623, 849, 4593, 714, 4623], 's_4_26': [4624, 968], 28: [1000, 910, 4880, 4879, 4878, 5132, 552, 5087, 5088, 716, 715], 's_4_28': [4804], 29: [669, 4818, 4817, 670, 597, 596, 4953, 671], 's_4_29': [4819], 31: [148, 4684, 147, 146, 145, 144, 4683, 4682, 4681, 4680], 's_4_31': [984], 's_4_34': [5014], 's_4_4': [973], 6: [340, 4895, 4695, 339, 4696, 1165, 1164, 4700, 4699, 4698, 564, 4697], 's_5_6': [563], 10: [5328, 718, 5358, 5359, 1017, 1016, 1015, 1014, 4654, 4653, 744], 's_5_10': [4578], 20: [5250, 5251, 537, 5297, 418], 's_5_20': [5177], 's_5_21': [625], 's_5_23': [642], 24: [4770, 4771, 4772, 4773, 5060, 459, 5059, 5058, 701, 700], 's_5_24': [5057], 's_5_26': [4743], 's_5_33': [638], 35: [4535, 4534, 4968, 4967, 4966, 4533, 4532, 280, 4531, 279, 278], 's_5_35': [533], 's_5_5': [593], 1: [4650, 249, 462, 250, 251, 252, 5190, 5191], 's_7_1': [5281], 3: [116, 117, 163, 5311, 5310], 's_7_3': [5340], 's_7_8': [4651], 's_7_10': [4652], 's_7_13': [4669, 954], 15: [265, 4906, 4905], 's_7_15': [4980], 's_7_20': [282], 's_7_26': [699], 27: [4710, 566, 4712, 567, 568, 4711, 565, 5402, 5403, 5404], 's_7_27': [309], 's_7_31': [684], 's_7_32': [5175], 38: [4592, 161, 4787, 4909, 4908, 4907, 504, 505, 5010, 5011, 506], 's_7_38': [549], 's_7_7': [4936], 's_8_12': [4471], 's_8_25': [4937], 's_8_28': [5117], 's_8_32': [5041], 's_8_35': [4876], 's_8_8': [442], 9: [160, 158, 159], 's_12_9': [173], 's_12_17': [835], 's_12_21': [4864], 's_12_24': [4774], 's_12_28': [925, 924], 's_12_34': [5104], 's_12_35': [4565, 1089], 37: [702, 5160, 5161, 5148, 5147, 428, 429, 430, 432, 431], 's_12_37': [4486], 's_12_38': [473], 's_12_12': [98], 's_13_9': [4620], 11: [4921, 4922, 489, 4801, 490], 's_13_11': [4621], 's_13_14': [5270], 's_13_16': [928], 's_13_18': [5345], 19: [492, 5253, 897, 1091, 1092, 1093, 5300, 763, 5252, 5299], 's_13_19': [5405], 's_13_21': [4745], 's_13_27': [5419], 's_13_29': [4622], 30: [883, 5479, 5283, 5478, 628, 5235, 5236, 5237, 627], 's_13_30': [5480], 's_13_35': [1013], 39: [384, 5464, 385, 5463, 5462, 386, 387, 5176, 507, 508], 's_13_39': [5465], 's_13_13': [4640], 's_16_1': [463], 's_16_6': [324], 's_16_10': [1018], 's_16_11': [355], 's_16_18': [5390], 's_16_20': [538], 22: [4998, 734, 733, 5073, 731, 732], 's_16_22': [748], 's_16_32': [4890], 's_16_36': [583], 's_16_16': [1003], 's_18_6': [4865], 's_18_21': [4835], 's_18_24': [5045], 's_18_27': [853], 's_18_30': [5432], 's_18_35': [4550], 's_18_36': [5448], 's_18_39': [914], 's_18_18': [4566], 's_23_1': [477], 's_23_14': [987], 's_23_19': [5225], 's_23_33': [927], 's_23_37': [582], 's_23_39': [5221], 's_23_23': [5194], 's_32_3': [193, 5325], 's_32_6': [4741, 4740], 's_32_14': [4950], 's_32_33': [204], 's_32_37': [207], 's_32_38': [5115], 's_32_32': [4935], 's_33_6': [579], 's_33_9': [4590], 's_33_22': [791], 's_33_26': [803], 's_33_36': [641], 's_33_33': [54], 's_36_10': [5313], 's_36_14': [598], 's_36_21': [4832], 's_36_29': [581], 's_36_35': [536], 's_36_38': [640], 's_36_39': [523], 's_36_36': [5493], 's_14_3': [388], 's_14_20': [5371], 's_14_37': [342], 's_14_39': [5206], 's_14_11': [236], 's_14_15': [221], 's_14_27': [808], 's_14_35': [4952], 's_14_14': [5284], 's_34_10': [5029], 's_34_22': [851], 's_34_24': [986], 's_34_28': [5089], 's_34_34': [985], 's_17_20': [5192], 's_17_38': [790], 's_17_22': [5163], 's_17_24': [911], 's_17_25': [926], 's_17_29': [775], 's_17_30': [672], 's_17_17': [4938], 's_21_1': [310, 4815], 's_21_6': [1075], 's_21_11': [535], 's_21_27': [205], 's_21_28': [4833], 's_21_31': [865, 864], 's_21_35': [4530, 4545], 's_21_38': [4591], 's_21_21': [4760], 's_25_38': [880], 's_25_11': [4892], 's_25_19': [4925], 's_25_22': [762], 's_25_28': [5013], 's_25_29': [550], 's_25_25': [5027], 's_26_38': [850, 4894], 's_26_24': [4788], 's_26_27': [4727], 's_26_28': [4759], 's_26_35': [653], 's_26_26': [4728], 's_28_6': [1105, 4715], 's_28_20': [5162], 's_28_38': [5072], 's_28_19': [4940], 's_28_24': [4863], 's_28_29': [4803], 's_28_30': [626], 's_28_28': [999, 998, 4520], 's_29_6': [834], 's_29_31': [654], 's_29_37': [4816], 's_29_22': [730], 's_29_24': [745], 's_29_35': [746], 's_29_29': [4713], 's_31_1': [5085], 's_31_3': [5445], 's_31_10': [774], 's_31_30': [132], 's_31_31': [5145], 's_6_1': [264], 's_6_10': [759], 's_6_19': [4910], 's_6_24': [114], 's_6_35': [4547], 's_6_6': [4861], 's_10_22': [5418], 's_10_24': [1001], 's_10_35': [909], 's_10_10': [5285], 's_20_1': [177], 's_20_3': [223], 's_20_37': [5356], 's_20_20': [238], 's_24_9': [175], 's_24_38': [520], 's_24_11': [370], 's_24_22': [686], 's_24_24': [5061], 's_35_37': [4546], 's_35_38': [475], 's_35_15': [416], 's_35_27': [4726], 's_35_35': [1163], 's_1_3': [5265], 's_1_9': [174], 's_1_37': [5282], 's_1_38': [5040], 's_1_39': [357], 's_1_1': [248], 's_3_3': [328], 's_15_37': [266], 's_15_38': [206], 's_15_15': [4860], 's_27_9': [4725], 's_27_38': [4742], 's_27_19': [5327, 493], 's_27_30': [793], 's_27_27': [534], 's_38_39': [4981], 's_38_38': [176], 's_9_9': [157], 's_37_11': [4757], 's_37_19': [687], 's_37_30': [237], 's_37_37': [222], 's_11_39': [4831], 's_11_11': [488], 's_19_39': [764], 's_19_22': [5373], 's_19_19': [5135], 's_30_39': [868], 's_30_22': [5508], 's_30_30': [629], 's_39_22': [749], 's_39_39': [404], 's_22_22': [5553]}, {0: [998, 4489, 968, 969, 972, 505, 4877, 4878, 4879, 970, 971], 2: [403, 5315, 5312, 5314, 5313], 's_0_2': [987], 4: [5115, 5118, 5119, 490, 491, 5116, 5117], 's_0_4': [4892], 5: [4728, 4725, 4726, 504, 4727], 's_0_5': [730], 7: [367, 4606, 368, 369, 4834, 4833, 4832, 4831, 370, 4876], 's_0_7': [820], 8: [895, 612, 5074, 5191, 5192, 5193, 896, 897, 5194], 's_0_8': [5254], 12: [295, 4953, 508, 507, 506, 4951, 4952], 's_0_12': [625], 13: [850, 849, 4471, 4472, 4473, 848], 's_0_13': [4474], 16: [877, 878, 4744, 4576, 4577, 4849, 4578, 4579, 909, 910], 's_0_16': [4624], 18: [864, 5027, 5028, 4654, 4652, 837, 836, 835, 834, 4653], 's_0_18': [5044], 23: [4860, 594, 595, 4861, 4862], 's_0_23': [610], 32: [4504, 4999, 985, 984, 983, 982, 682, 4339, 4338], 's_0_32': [986], 33: [700, 4608, 699, 939, 4639, 4638], 's_0_33': [4595], 36: [503, 908, 744, 4412, 4414, 743, 4413], 's_0_36': [893], 's_0_0': [4490], 's_2_12': [5341], 14: [5251, 357, 356, 355, 4323, 637, 4457, 4456, 353, 354], 's_2_14': [418], 's_2_18': [822], 34: [5266, 326, 5190, 327], 's_2_34': [432], 's_2_2': [5328], 's_4_12': [521], 17: [927, 5224, 5223, 371, 372, 5222, 5221], 's_4_17': [387], 's_4_18': [5026], 21: [791, 460, 459, 790, 789, 4697, 728, 729, 4698], 's_4_21': [4981], 25: [5149, 5146, 582, 5148, 5147], 's_4_25': [5072], 26: [746, 535, 597, 596, 4938, 429, 430, 4937], 's_4_26': [656, 5162], 28: [386, 911, 5059, 701, 5058, 5057, 5056, 5055, 266], 's_4_28': [101], 29: [5102, 5103, 772, 773, 774, 775, 776, 777, 5104], 's_4_29': [536], 31: [131, 130, 129, 128, 4369, 4368, 4367, 4366, 4365, 127], 's_4_31': [146], 's_4_34': [207], 's_4_4': [57], 6: [489, 176, 175, 174, 4590, 4591, 4592, 4593, 4594, 818], 's_5_6': [159], 10: [132, 147, 5235, 222, 221, 4562, 4561, 219, 220], 's_5_10': [4710], 20: [307, 308, 4891, 310, 309], 's_5_20': [4711], 's_5_21': [624], 's_5_23': [415], 24: [5085, 714, 715, 641, 5086, 716, 5087, 5088], 's_5_24': [4713], 's_5_26': [565, 4787], 's_5_33': [609, 4743], 35: [611, 5012, 4741, 4742, 502, 551, 550, 549, 4352, 4427, 548], 's_5_35': [385], 's_5_5': [99], 1: [4637, 564, 291, 292, 293, 4547, 4546], 's_7_1': [4545, 248], 3: [4230, 636, 4233, 4231, 4232], 's_7_3': [4246], 's_7_8': [865, 866], 's_7_10': [234], 's_7_13': [383], 15: [4277, 352, 4276], 's_7_15': [4261], 's_7_20': [4771], 's_7_26': [4681], 27: [4622, 4666, 4667, 4519, 4518, 668, 669], 's_7_27': [4651], 's_7_31': [4605], 's_7_32': [1015], 38: [447, 441, 446, 445, 444, 443, 442, 4397, 4398], 's_7_38': [4351], 's_7_7': [4835], 's_8_12': [5206], 's_8_25': [702], 's_8_28': [4954], 's_8_32': [881], 's_8_35': [5013, 821], 's_8_8': [807], 9: [4863, 655, 653, 654], 's_12_9': [4968], 's_12_17': [4966], 's_12_21': [475], 's_12_24': [311], 's_12_28': [236], 's_12_34': [4980], 's_12_35': [5011], 37: [4294, 4293, 4291, 4830, 205, 204, 203, 4292, 202, 4290], 's_12_37': [280], 's_12_38': [4996], 's_12_12': [5447], 's_13_9': [638], 11: [4815, 4816, 4801, 4802, 762, 761, 4803, 760], 's_13_11': [4818], 's_13_14': [398], 's_13_16': [623], 's_13_18': [4864], 19: [399, 338, 339, 251, 250, 249, 279, 4695, 4696], 's_13_19': [4486], 's_13_21': [4488], 's_13_27': [608], 's_13_29': [4429], 30: [952, 953, 954, 4714, 957, 956, 955], 's_13_30': [4909], 's_13_35': [578], 39: [4760, 4759, 4758, 518, 519, 4757, 4756], 's_13_39': [4487], 's_13_13': [4443, 832], 's_16_1': [278], 's_16_6': [924], 's_16_10': [458], 's_16_11': [4774], 's_16_18': [804], 's_16_20': [323], 22: [1044, 1045, 1046, 5175, 5176, 5177, 5178, 5179, 1047], 's_16_22': [4819], 's_16_32': [892], 's_16_36': [698], 's_16_16': [4384], 's_18_6': [759], 's_18_21': [4924], 's_18_24': [5089], 's_18_27': [833], 's_18_30': [5239], 's_18_35': [671], 's_18_36': [4668], 's_18_39': [894], 's_18_18': [5299], 's_23_1': [4532], 's_23_14': [593], 's_23_19': [4875], 's_23_33': [579], 's_23_37': [4800, 325], 's_23_39': [580], 's_23_23': [115], 's_32_3': [742], 's_32_6': [817], 's_32_14': [4307], 's_32_33': [4610], 's_32_37': [802], 's_32_38': [667], 's_32_32': [4324], 's_33_6': [4609], 's_33_9': [4788], 's_33_22': [4775, 940], 's_33_26': [4908], 's_33_36': [4623], 's_33_33': [1013], 's_36_10': [488], 's_36_14': [4458], 's_36_21': [4683], 's_36_29': [4533], 's_36_35': [563], 's_36_38': [457], 's_36_39': [745], 's_36_36': [4415, 1088], 's_14_3': [652, 651], 's_14_20': [4455], 's_14_37': [757], 's_14_39': [533], 's_14_11': [340], 's_14_15': [697, 4278], 's_14_27': [683], 's_14_35': [413], 's_14_14': [5281, 373], 's_34_10': [5265], 's_34_22': [342], 's_34_24': [5071], 's_34_28': [5101], 's_34_34': [282], 's_17_20': [4921], 's_17_38': [4906, 401], 's_17_22': [912], 's_17_24': [567], 's_17_25': [852], 's_17_29': [747], 's_17_30': [942], 's_17_17': [5225], 's_21_1': [684], 's_21_6': [534], 's_21_11': [4939], 's_21_27': [4428], 's_21_28': [4969], 's_21_31': [4353], 's_21_35': [4382, 4383], 's_21_38': [4922], 's_21_21': [4907], 's_25_38': [5132], 's_25_11': [5208, 5207, 537], 's_25_19': [5131], 's_25_22': [867], 's_25_28': [281], 's_25_29': [402], 's_25_25': [882], 's_26_38': [428], 's_26_24': [5133], 's_26_27': [670], 's_26_28': [566], 's_26_35': [640, 4982], 's_26_26': [598], 's_28_6': [5025], 's_28_20': [4890, 265], 's_28_38': [5041, 416], 's_28_19': [5040], 's_28_24': [806], 's_28_29': [5073], 's_28_30': [4984], 's_28_28': [191], 's_29_6': [4564], 's_29_31': [758], 's_29_37': [4308], 's_29_22': [5105], 's_29_24': [686], 's_29_35': [552], 's_29_29': [4219], 's_31_1': [277], 's_31_3': [337], 's_31_10': [4905], 's_31_30': [4354], 's_31_31': [144], 's_6_1': [473], 's_6_10': [263, 4530], 's_6_19': [4650], 's_6_24': [160, 161], 's_6_35': [4740], 's_6_6': [4785], 's_10_22': [162], 's_10_24': [5070], 's_10_35': [235], 's_10_10': [5280], 's_20_1': [4381], 's_20_3': [322], 's_20_37': [4665], 's_20_20': [4440], 's_24_9': [4773], 's_24_38': [431], 's_24_11': [4998], 's_24_22': [717], 's_24_24': [732, 733], 's_35_37': [427], 's_35_38': [472], 's_35_15': [547], 's_35_27': [4442], 's_35_35': [501], 's_1_3': [276], 's_1_9': [4548], 's_1_37': [4305], 's_1_38': [4156], 's_1_39': [4607], 's_1_1': [294], 's_3_3': [232], 's_15_37': [532], 's_15_38': [622, 621], 's_15_15': [351], 's_27_9': [4503], 's_27_38': [414, 4531], 's_27_19': [384], 's_27_30': [938], 's_27_27': [4563, 713], 's_38_39': [517], 's_38_38': [712, 4263], 's_9_9': [4997], 's_37_11': [190], 's_37_19': [4680], 's_37_30': [937], 's_37_37': [1042], 's_11_39': [400], 's_11_11': [763], 's_19_39': [264], 's_19_22': [5160], 's_19_19': [4621], 's_30_39': [4745], 's_30_22': [5135], 's_30_30': [5150], 's_39_22': [5060, 1091, 1090], 's_39_39': [4761], 's_22_22': [5045]}, {0: [5150, 940, 4906, 4907, 4908, 4909, 943, 942, 941], 2: [4877, 580, 4802, 700, 730, 609, 4773], 's_0_2': [625], 4: [4666, 429, 430, 5163, 5162, 5161, 431], 's_0_4': [5164], 5: [4756, 4757, 4758, 5224, 5014, 4759, 912, 911, 910], 's_0_5': [5194], 7: [956, 955, 954, 4610, 4609, 4608, 506, 5072, 5071, 356, 355, 354, 4606, 4607], 's_0_7': [957], 8: [4864, 4865, 4790, 1076, 1075], 's_0_8': [4775], 12: [623, 624, 969, 535, 4819, 749, 748, 4817, 4818, 747, 746, 745], 's_0_12': [880], 13: [325, 4980, 326, 327, 328, 5476, 5225, 1077, 5478, 5479, 5477, 5480, 1078], 's_0_13': [1047], 16: [670, 340, 4832, 235, 4830, 491, 490, 4831], 's_0_16': [445], 18: [311, 310, 4800, 4695, 4801, 444, 4579, 4578, 4577, 399, 4696], 's_0_18': [4951, 280], 23: [972, 5403, 5330, 958, 5404], 's_0_23': [5300], 32: [5102, 821, 5103, 5105, 5104], 's_0_32': [986], 33: [4984, 5255, 5465, 1003, 998, 999, 1000, 1002, 1001], 's_0_33': [4804], 36: [460, 4892, 4715, 1044, 505, 504, 4624, 4623, 4622, 4620, 4621], 's_0_36': [939], 's_0_0': [4849], 's_2_12': [4848], 14: [1105, 701, 5357, 5358, 5359, 1017, 1106, 5058, 5059, 5060, 1016], 's_2_14': [731], 's_2_18': [608], 34: [4684, 4683, 4682, 4681, 222, 221, 220, 4815, 294], 's_2_34': [4697], 's_2_2': [4713], 's_4_12': [4816], 17: [5117, 568, 563, 5222, 567, 566, 564, 565], 's_4_17': [507], 's_4_18': [384], 21: [4594, 4549, 5056, 416, 415, 414, 4546, 4547, 760, 759, 4548], 's_4_21': [4891], 25: [1153, 1152, 1151, 4651, 4652, 4653, 4654, 4655, 1149, 1150], 's_4_25': [459], 26: [5090, 867, 5089, 5088, 5073, 5178, 732], 's_4_26': [5133, 672], 28: [4744, 4968, 4969, 849, 850, 851, 5553, 854, 853, 852], 's_4_28': [4967], 29: [462, 5206, 342, 341, 4698, 654, 655, 4982, 4981], 's_4_29': [656], 31: [5176, 403, 401, 5146, 5147, 402], 's_4_31': [5086], 's_4_34': [5160], 's_4_4': [687], 6: [5282, 524, 4772, 4639, 4638, 4637, 519, 523, 522, 521, 520], 's_5_6': [534], 10: [263, 264, 265, 5281, 267, 266], 's_5_10': [249], 20: [595, 822, 5193, 5192, 596, 597], 's_5_20': [5239], 's_5_21': [909], 's_5_23': [987], 24: [804, 4591, 4729, 717, 716, 715, 714, 4592, 718, 4593, 669, 4728], 's_5_24': [278, 279], 's_5_26': [881], 's_5_33': [4760], 35: [686, 160, 1015, 4999, 4998, 4997, 4996, 475, 4846, 4845], 's_5_35': [400], 's_5_5': [489], 1: [764, 551, 5026, 5027, 5028, 763, 762, 761], 's_7_1': [5029], 3: [5177, 5012, 627, 626], 's_7_3': [5011], 's_7_8': [4955], 's_7_10': [5070], 's_7_13': [5116], 15: [4939, 4940], 's_7_15': [4925], 's_7_20': [594], 's_7_26': [5087], 27: [924, 925, 926, 929, 928, 927], 's_7_27': [4669], 's_7_31': [5041], 's_7_32': [552], 38: [4894, 4954, 896, 895, 894, 893, 4489, 4487, 4488], 's_7_38': [803], 's_7_7': [4595], 's_8_12': [4820], 's_8_25': [4791], 's_8_28': [4970], 's_8_32': [1061], 's_8_35': [1014], 's_8_8': [4866], 9: [5433, 959, 5434], 's_12_9': [734], 's_12_17': [4922], 's_12_21': [4833], 's_12_24': [984], 's_12_28': [5208], 's_12_34': [789], 's_12_35': [4847], 37: [5327, 5328, 790, 791, 5329, 793, 792], 's_12_37': [733], 's_12_38': [865], 's_12_12': [819], 's_13_9': [944], 11: [5180, 1167, 1166, 5000, 4878, 4879, 4880, 1165], 's_13_11': [5210], 's_13_14': [5270], 's_13_16': [4936], 's_13_18': [5025, 176], 19: [1079, 5525, 5522, 808, 5524, 5523], 's_13_19': [569], 's_13_21': [4861], 's_13_27': [914], 's_13_29': [5266], 30: [5101, 372, 373, 313, 5372, 5509, 5508, 628, 5416, 5417], 's_13_30': [463], 's_13_35': [250], 39: [833, 4534, 4535, 1119, 1120, 1121, 1122, 1123, 5373, 5374, 1033, 5405], 's_13_39': [1032], 's_13_13': [268], 's_16_1': [550], 's_16_6': [4952], 's_16_10': [4875], 's_16_11': [640], 's_16_18': [370, 369], 's_16_20': [4938], 22: [613, 297, 252, 223, 5340, 5451, 5341, 492, 493, 5447, 5448, 5449, 5450], 's_16_22': [295, 296], 's_16_32': [671], 's_16_36': [234], 's_16_16': [236], 's_18_6': [579], 's_18_21': [683], 's_18_24': [159, 4590], 's_18_27': [4564], 's_18_30': [312], 's_18_35': [4921, 4920], 's_18_36': [189], 's_18_39': [848], 's_18_18': [324, 323, 4561], 's_23_1': [5418], 's_23_14': [913], 's_23_19': [988], 's_23_33': [973], 's_23_37': [883], 's_23_39': [5315], 's_23_23': [5419], 's_32_3': [5013], 's_32_6': [536], 's_32_14': [1107], 's_32_33': [5120], 's_32_37': [806], 's_32_38': [866], 's_32_32': [1031], 's_33_6': [1013], 's_33_9': [5510], 's_33_22': [1094], 's_33_26': [5254], 's_33_36': [983, 4565], 's_33_33': [4520], 's_36_10': [4635], 's_36_14': [1135, 1136], 's_36_21': [4636], 's_36_29': [4743, 699], 's_36_35': [205, 204], 's_36_38': [968], 's_36_39': [1043], 's_36_36': [174], 's_14_3': [641], 's_14_20': [807], 's_14_37': [583], 's_14_39': [5030], 's_14_11': [5240], 's_14_15': [1091], 's_14_27': [5044], 's_14_35': [1046], 's_14_14': [5360], 's_34_10': [4890], 's_34_22': [5220], 's_34_24': [834], 's_34_28': [4699], 's_34_34': [4680], 's_17_20': [4712], 's_17_38': [548], 's_17_22': [5237], 's_17_24': [4727], 's_17_25': [549], 's_17_29': [5221], 's_17_30': [5402], 's_17_17': [562], 's_21_1': [371], 's_21_6': [744], 's_21_11': [775], 's_21_27': [4789], 's_21_28': [4774], 's_21_31': [4937], 's_21_35': [161, 5055], 's_21_38': [713, 4443], 's_21_21': [4531], 's_25_38': [879], 's_25_11': [5015], 's_25_19': [5540], 's_25_22': [1168], 's_25_28': [864], 's_25_29': [4667], 's_25_25': [5420], 's_26_38': [5149, 897, 882], 's_26_24': [5223], 's_26_27': [5299], 's_26_28': [5284], 's_26_35': [5118], 's_26_26': [1137], 's_28_6': [5552], 's_28_20': [5269], 's_28_38': [5074], 's_28_19': [869], 's_28_24': [4803], 's_28_29': [4953], 's_28_30': [719], 's_28_28': [5614], 's_29_6': [774], 's_29_31': [5297], 's_29_37': [5312], 's_29_22': [5356], 's_29_24': [729], 's_29_35': [610], 's_29_29': [357], 's_31_1': [446], 's_31_3': [5148], 's_31_10': [251], 's_31_30': [5401], 's_31_31': [5191], 's_6_1': [5057], 's_6_10': [5131, 5132], 's_6_19': [5537], 's_6_24': [653], 's_6_35': [4862], 's_6_6': [538, 539], 's_10_22': [388, 5386], 's_10_24': [309, 4650], 's_10_35': [4905], 's_10_10': [4530], 's_20_1': [777], 's_20_3': [5207], 's_20_37': [642], 's_20_20': [598], 's_24_9': [703], 's_24_38': [638], 's_24_11': [4730, 1090], 's_24_22': [5463], 's_24_24': [219], 's_35_37': [5043], 's_35_38': [835], 's_35_15': [776], 's_35_</t>
+          <t>[22.41586661338806, 21.22614026069641, 11.925055265426636, 17.575570583343506, 17.86868381500244, 12.501160621643066, 25.99880361557007, 31.30040979385376, 57.01960563659668, 15.96935510635376, 32.493196964263916, 17.41078472137451, 11.378475189208984, 22.261898040771484, 20.088332176208496, 18.218420267105103, 25.00328040122986, 21.879677772521973, 19.90427827835083, 29.66428780555725, 18.655328273773193, 13.357178688049316, 32.138351917266846, 41.82378530502319, 26.467851638793945, 35.35292959213257, 24.956265687942505, 27.689016580581665, 27.271931648254395, 32.38490104675293, 19.369263172149658, 11.311038255691528, 13.417658805847168, 13.241601467132568, 19.347644090652466, 28.058809280395508, 16.999776601791382, 23.35080099105835, 13.127259492874146, 21.33750081062317, 19.047412633895874, 14.59726881980896, 15.100475788116455, 14.130224704742432, 17.940375566482544, 17.547006607055664, 31.551339626312256, 27.868627786636353, 15.615024328231812, 31.607417345046997, 25.75628924369812, 18.634746551513672, 26.824950218200684, 24.71854519844055, 19.746604442596436, 22.601799964904785, 11.49241852760315, 22.871469497680664, 25.15409541130066, 26.09713387489319, 18.330068111419678, 11.883667230606079, 23.250046014785767, 20.927736043930054, 34.53120970726013, 16.529052257537842, 16.87854242324829, 15.499851703643799, 24.363864183425903, 26.735021829605103, 23.96262001991272, 33.7059805393219, 23.723427772521973, 29.1303927898407, 28.92953610420227, 20.75716543197632, 20.746752738952637, 24.110805988311768, 16.96973443031311, 16.866915702819824, 11.848808765411377, 18.907697677612305, 15.692572593688965, 30.01745367050171, 15.580776691436768, 29.404669523239136, 27.6116623878479, 16.993005752563477, 15.663578748703003, 13.015208005905151, 16.703418254852295, 24.56422710418701, 21.99783229827881, 22.40062713623047, 18.714409589767456, 20.43033790588379, 27.04928731918335, 15.06744122505188, 40.16705775260925, 15.242068529129028]</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>[{0: [3103, 3101, 3102], 2: [3118, 2537, 2536], 4: [2310, 2311], 5: [2205, 2206], 7: [3385, 2102, 2100, 2101], 8: [3040, 2116, 2115], 12: [2431, 2430, 3041, 3042], 13: [3162, 3251, 2191], 16: [2340, 3237, 2342, 2341], 18: [2446, 3131, 2445, 3133, 3132], 23: [3266, 2400, 3267, 2401], 32: [2415, 3296, 3297, 2416], 33: [2130, 3056, 3057], 36: [2370, 2372, 2371], 14: [3341, 2236, 3343, 3342], 34: [2535, 3088, 3087], 17: [3327, 3328], 21: [3012, 3011, 2162, 2161, 2160], 25: [3311, 2266, 3312], 26: [3176, 2250, 3178, 3177], 28: [2221, 3147, 3086, 2220], 29: [3117, 2357, 2356], 31: [2072, 2312, 3432, 3431], 6: [2326, 2997, 2325], 10: [2071, 3072, 3071, 2070], 20: [3446, 3357, 2207], 24: [3026, 2281, 2280], 35: [3190, 2462, 2461, 3191, 3192], 1: [2177, 3282, 3281], 3: [3235, 2086, 2087], 15: [2055, 2056], 27: [2981, 2147, 2146, 2145], 38: [3207, 3326, 2131, 3206], 9: [2176, 2175], 37: [3370, 3372, 2251, 3371], 11: [3236], 19: [3222, 3221], 30: [3387, 2192, 3386], 39: [3447, 2295, 2296, 2297], 22: [2387, 3252, 2385, 2386]}, {0: [1395, 1397, 1396], 2: [3427, 1367], 4: [3276, 3277], 5: [1623, 1592, 3457, 3458], 7: [1562, 3471, 3472, 3473], 8: [3231, 1337, 1336], 12: [3397, 3396, 1262, 1261], 13: [3216, 1532, 1531, 3217], 16: [1605, 1306, 3143, 3142], 18: [1488, 3112, 1487, 1486], 23: [3353, 3352], 32: [1380, 1382, 1381], 33: [1366, 3338, 3337], 36: [1637, 1636, 3098, 1500, 3097], 14: [3441, 3443, 1502, 1427, 3442], 34: [3158, 1472, 1471], 17: [1186, 3307, 3306], 21: [1352, 1350, 1351], 25: [3187, 1231, 3186], 26: [1411, 1412], 28: [1246, 3202, 3201], 29: [3096, 1277, 1276], 31: [3367, 1307, 3366], 6: [3171, 3172, 1622, 1621, 3173], 10: [1575, 1577, 1576], 20: [1515, 1517, 3308, 1516], 24: [1591, 3261, 3263, 3262], 35: [3413, 3411, 3412], 1: [1607, 3322, 3323, 1606], 3: [3383, 3381, 3382], 15: [3501, 1247], 27: [1443, 1547, 3488, 3487], 38: [3502, 1456, 1457, 1458], 9: [1321, 1322], 37: [3128, 3426, 3127, 1291, 1292], 11: [3082, 1426, 1425], 19: [1545, 1546], 30: [1441, 1442], 39: [1501, 3232], 22: [3248, 3246, 3247]}, {0: [648, 3901, 649, 3902], 2: [3767, 634], 4: [363, 364, 3977, 365, 3976], 5: [3782, 3708, 589], 7: [500, 498, 3751, 499], 8: [469], 12: [3886, 3888, 3887], 13: [590, 3811, 3812], 16: [575, 574], 18: [3843, 410, 3842], 23: [3662, 3663], 32: [3796, 3798, 3797], 33: [3858, 3963, 725, 724], 36: [604, 3826, 3827], 14: [558, 560, 559], 34: [3918, 3828, 3978, 694, 695], 17: [425, 320, 3961], 21: [528, 530, 529], 25: [3766, 334, 335, 3946], 26: [484, 485, 3962], 28: [680, 3916, 3917], 29: [453, 350, 349, 3736], 31: [708, 3573, 3571, 3572], 6: [3721, 679, 3722], 10: [3752, 3753, 709], 20: [380, 379, 3632, 3631], 24: [664, 3931, 665, 3932], 35: [3856, 513, 3857, 515, 514], 1: [3646, 618, 3647], 3: [3482, 409, 408], 15: [3601, 3602], 27: [454, 3872], 38: [438, 4022, 440, 439], 9: [3873, 619], 37: [603, 740, 739, 3677, 3678], 11: [3948, 3947], 19: [394, 395], 30: [423, 424], 39: [3707, 545, 544], 22: [319, 3691, 3693, 3692]}, {0: [2245, 2247, 2246], 2: [4961, 5051, 2187, 2186], 4: [5053, 5036, 5037, 2456], 5: [2307, 5171, 5172], 7: [4886, 2471, 4887, 4888, 2470], 8: [2472, 5186, 5187], 12: [2396, 5231, 5232, 2397], 13: [4977, 4978, 2381], 16: [2576, 5068, 5066, 5067], 18: [2306, 4962], 23: [2157, 2156, 2155, 4841], 32: [4856, 2142, 2141, 2140], 33: [5217, 5216], 36: [2351, 5157, 2352], 14: [4901, 4903, 2305, 4902], 34: [5052], 17: [5023, 5021, 5022], 21: [2502, 5248, 2336, 2337, 5247], 25: [5143, 5158, 2441], 26: [5112, 2382, 5113], 28: [5006, 2426, 5007, 2425], 29: [5083, 2291, 5082], 31: [2501, 2500], 6: [4857, 2320, 2322, 2321], 10: [5098, 2260, 5097, 2261], 20: [2230, 2231], 24: [2366, 5202, 2367], 35: [5127, 2201, 2202], 1: [4916, 4918, 2335, 4917], 3: [4873, 4871, 4872], 15: [4783, 4782, 2200], 27: [2485, 2486, 4991, 4992], 38: [2215, 2216, 5142, 5081, 2217], 9: [4976, 5201, 2171, 2172], 37: [2290, 4933, 4932], 11: [5203, 2546, 2547], 19: [2440, 4842, 2455], 30: [4963, 2531], 39: [4948, 2275, 4947], 22: [2410, 2412, 2411]}, {0: [2693, 2692, 4287, 4288, 4289], 2: [4409], 4: [2632, 4364], 5: [2646, 4529, 2647, 2648], 7: [4184, 2436, 4182, 4183], 8: [2572], 12: [4394, 4303, 2603, 2602], 13: [2421, 2423, 2422], 16: [4152, 2376, 2378, 4302, 2377], 18: [4319, 2587, 4317, 4318], 23: [4589, 4588, 2483], 32: [4272, 4198, 2451], 33: [2392, 2393, 4528, 4527], 36: [4407, 2347, 2348], 14: [4137, 2481, 4408, 2482], 34: [4484, 2723], 17: [2618, 2617], 21: [4467, 4468, 2767, 4469], 25: [2558, 4453, 2573], 26: [4258, 2631, 4259], 28: [4514, 4244, 2662, 2663], 29: [4377, 2437, 4379, 4378], 31: [4214, 2708, 2707], 6: [2543, 4273, 4213, 2542], 10: [2737, 2738, 4497, 4498, 4499], 20: [2616, 4153, 4154], 24: [2512, 4483, 2513], 35: [2677, 4334, 4332, 4333], 1: [4482, 2363, 4229, 4228, 2362, 4227], 3: [4168, 2586], 15: [4363, 2467, 2466], 27: [2408, 2406, 2407], 38: [4347, 4349, 2557, 4348], 9: [2333, 2364, 4558, 4557], 37: [2496, 2498, 2497], 11: [4393, 2528], 19: [4512, 2468, 4513], 30: [4424, 4423], 39: [2452, 4452], 22: [2678, 4439, 4438]}, {0: [5337, 2128, 5335, 5336], 2: [5412, 5472, 2308], 4: [2247, 5441, 2248], 5: [5245, 2052, 5306], 7: [1932, 5305, 1843], 8: [5394, 5395], 12: [5516, 5396, 2143, 2144], 13: [1977, 1979, 1978], 16: [5529, 5605, 1933, 1934], 18: [5410, 5411], 23: [2068, 2067], 32: [5274, 1859, 1858], 33: [2097, 5290, 5291], 36: [1994, 1993], 14: [5471, 2009, 5470], 34: [5351, 2293], 17: [5454, 5455, 5456], 21: [2023, 5440, 2024], 25: [2114, 2113], 26: [5216, 5214, 5215], 28: [2008, 5364, 5365, 5366, 2232], 29: [2188, 2189, 5591, 5590, 1949], 31: [5261, 1948, 1947, 5260], 6: [2039, 2038, 5275], 10: [5322, 5320, 5321], 20: [5244, 1888, 1887], 24: [5276, 2158, 2157], 35: [1964, 1902, 1903, 5515], 1: [5230, 5199, 1918, 1917], 3: [5469, 1738, 5379, 5378], 15: [1844], 27: [1962, 1963], 38: [1872, 1873, 5486, 5485], 9: [2142, 5200, 5201], 37: [5500, 2098, 5501], 11: [2159, 5530, 5531], 19: [5381, 5380], 30: [2233, 5425, 5426], 39: [5546, 5544, 2083, 5545], 22: [2173, 5606, 2174]}, {0: [1293, 3337, 1291, 1292], 2: [1263, 3606], 4: [3336, 1203, 1202], 5: [1516, 1442, 3442, 1517], 7: [1457, 1456, 3186, 3187], 8: [3245, 3172, 1126, 3171], 12: [1173, 3591, 1127, 1128, 3590], 13: [3200, 1351, 1352, 3201, 1350], 16: [1397, 1396], 18: [3500, 3502, 3501], 23: [3246, 3247], 32: [3232, 1306, 3231], 33: [3367, 1428, 1426, 1427], 36: [3397, 1247, 3396], 14: [1278, 1276, 1277], 34: [3471, 3470], 17: [1186, 3351], 21: [1547, 3488, 3486, 3487], 25: [3321, 1141], 26: [1458, 3518, 3516, 3517], 28: [3380, 1216, 1218, 1217], 29: [1261, 3441, 1262], 31: [3410, 3411, 3412], 6: [3382, 1381, 3381, 1382], 10: [3352, 1322, 1321], 20: [3262, 3261], 24: [1383, 3562, 1187, 3561, 3560], 35: [3427, 3426, 1170, 1171, 1172], 1: [1473, 1471, 3276, 3277, 1472], 3: [3112, 1487, 3111, 1486], 15: [3097, 1200, 3096], 27: [3185, 1111, 1112, 1113, 3531], 38: [3156, 1233, 1230, 1232, 1231], 9: [3607, 1398, 3532], 37: [3230, 3290, 1201, 3291], 11: [3456, 3322, 1337, 1336], 19: [1411, 3306, 3307], 30: [3215, 1066, 1067], 39: [1367, 3216, 1366], 22: [1307, 3366, 3365, 1052, 1053]}, {0: [3425, 946, 947, 3424], 2: [3230, 1112, 1111], 4: [1067, 3349, 1022, 3350], 5: [3170, 3169], 7: [3183, 3394, 3393, 767, 766], 8: [3363, 3423, 736, 737], 12: [3378, 3379, 3380], 13: [1037, 1035, 1036], 16: [855, 3110, 3109], 18: [1066, 3034, 1005, 3155], 23: [841, 3094, 840], 32: [3199, 825, 3198], 33: [3259, 975, 976], 36: [887, 885, 886], 14: [3080, 1110, 3078, 3079], 34: [872, 3229, 871], 17: [1052, 3334, 3335], 21: [3290, 3289, 795, 796, 3288], 25: [750, 752, 751], 26: [3184, 1021], 28: [3215, 1006, 3213, 3214], 29: [3305, 3438, 932, 3439], 31: [3348, 722, 721], 6: [931, 3124, 3125], 10: [3228, 3244, 856], 20: [811, 810], 24: [961, 960], 35: [900, 901, 3364, 902], 1: [3139, 3138], 3: [3108, 3033, 705], 15: [2959, 765], 27: [992, 990, 3245, 991], 38: [1020, 781, 3049, 780, 3048], 9: [1097, 3140, 1096], 37: [3154, 915, 917, 916], 11: [3065, 3063, 3064], 19: [1126, 3095, 2974, 2975, 1065], 30: [3408, 3409, 3410, 1081, 1082], 39: [1080, 870, 2990, 2989], 22: [3319, 3320, 1051, 1050]}, {0: [4366, 563, 4368, 4367], 2: [4399, 398, 4398, 4397], 4: [4291, 561, 562, 4292], 5: [427, 532, 4382], 7: [607, 606, 4143, 4142], 8: [457, 4261, 456], 12: [773, 4172, 4173, 772], 13: [680, 682, 681], 16: [4321, 4323, 517, 4322], 18: [4293, 4098, 4158, 712, 711], 23: [411, 413, 412], 32: [4427, 470, 471, 472], 33: [4351, 4353, 4352], 36: [4128, 728, 726, 727], 14: [4023, 4022, 397, 396], 34: [4171, 4396, 352, 351], 17: [4201, 531, 4202], 21: [667, 4263, 4262], 25: [366, 367], 26: [502, 501], 28: [620, 4156, 4157, 621], 29: [4113, 4111, 4112], 31: [576, 577], 6: [4428, 696, 697, 4383, 622], 10: [4246, 4248, 4247], 20: [548, 546, 547], 24: [4278, 426, 4276, 4277], 35: [4232, 801, 4234, 4233], 1: [4052, 4053, 742, 741], 3: [3993, 591, 3992], 15: [4141, 441], 27: [4187, 665, 4188, 666], 38: [516, 651, 4126, 4127], 9: [637, 757, 4338], 37: [4217, 487, 486], 11: [382, 4307, 4306], 19: [4068, 4066, 4067], 30: [4096, 4097], 39: [4083, 4082, 381, 4081], 22: [4231, 336, 337]}, {0: [4418, 4627, 1584, 1583], 2: [4417, 1327], 4: [4447, 1598, 4448], 5: [4823, 4822, 1508, 1509], 7: [4807, 4793, 1494, 1495], 8: [1645, 1643, 1644], 12: [1522, 4432, 4434, 4433], 13: [1465, 4764, 4763, 4762], 16: [4567, 1464], 18: [1450, 1448, 1449], 23: [4626, 4717, 1404], 32: [4671, 4673, 4672], 33: [4719, 1659, 1658, 4718, 1660], 36: [1479, 4688, 4687], 14: [4686, 4821, 1328, 1329], 34: [1507, 4461, 4462, 4463], 17: [4643, 4538, 1687, 1688], 21: [4507, 1434, 1433], 25: [1357, 1673, 4372, 4373], 26: [1599, 1538, 4613], 28: [1703, 1403, 4523, 4522], 29: [1554, 4478, 1553, 4477], 31: [1613, 4747, 1614, 4748], 6: [4657, 1628, 1629, 4658], 10: [1568, 4568], 20: [1285, 1284, 4536, 4537], 24: [1748, 4582, 4583, 4584], 35: [4777, 4778, 1523, 1524], 1: [4704, 4703, 4701, 4702], 3: [1344, 4806], 15: [1420, 4792], 27: [4731, 4734, 4732, 4733], 38: [1417, 1418, 4642, 1419], 9: [1793, 1794], 37: [4476, 1298, 1299, 1300], 11: [1374, 1372, 4641, 1373], 19: [4656, 1358, 1359], 30: [1764, 1733, 4597, 4598, 4599], 39: [4612, 1389], 22: [1388, 4493, 1463, 4491, 4492]}, {0: [2573, 4454, 4452, 4453], 2: [4707, 4722, 2318, 2319], 4: [2407, 4467, 4468], 5: [2587, 4633, 2588], 7: [2393, 2394, 4784, 4783, 2395], 8: [4379, 4377, 4378], 12: [4647, 2378, 2379], 13: [2695, 2693, 2694], 16: [4679, 2574, 4678], 18: [2558, 4709, 4708, 2559], 23: [2632, 2634, 2633], 32: [2725, 2782, 2783, 2784, 4814], 33: [2604, 2603, 4499, 4498], 36: [2710, 2708, 2709], 14: [4769, 2380, 4768], 34: [4497, 2333], 17: [4438, 4439], 21: [2648, 4603, 4604, 2649], 25: [2528, 2529], 26: [4424, 4362, 2602, 4363], 28: [2798, 4484, 2348, 4482, 4483], 29: [2543, 4529, 4528], 31: [4527, 2409, 2408], 6: [4649, 4648, 2544], 10: [4572, 4574, 4573], 20: [2498, 2500, 2499], 24: [4543, 2437, 2439, 2438], 35: [2454, 2452, 4619, 4618, 2453], 1: [4694, 4692, 4693], 3: [2349, 4813, 4812, 2350], 15: [2424, 2423], 27: [2680, 2678, 2679], 38: [2724, 2723, 4512, 4514, 4513], 9: [4724, 4723, 2469], 37: [2483, 4754, 4753, 2484], 11: [2664, 2530, 4739, 4738], 19: [2513, 4664, 4663, 2514], 30: [4588, 2663, 4589], 39: [4544, 2619, 2618], 22: [4559, 2468, 4558]}, {0: [1407, 4985, 1406, 4986], 2: [5077], 4: [1393, 1391, 1392], 5: [5060, 1302, 5061, 1301], 7: [5331, 1271, 1272, 1273], 8: [5210, 5212, 5211], 12: [5332, 5092, 1453, 1452], 13: [1256, 1258, 1257], 16: [1061, 5121, 5120], 18: [1467, 5106, 5107], 23: [5270, 1076, 1077], 32: [1121, 1123, 1122], 33: [1241, 5045, 5047, 5046], 36: [1211, 1212], 14: [5075, 1332, 1331, 5076], 34: [1345, 1421, 4957], 17: [5301, 5302], 21: [5197, 5195, 5196], 25: [1362, 5257], 26: [5166, 1361], 28: [1422, 5137], 29: [5287, 5286], 31: [1167, 5361, 5360], 6: [5015, 1377, 1376, 5016], 10: [5032, 1166, 5030, 5031], 20: [5136, 1197, 1196], 24: [1346, 1347], 35: [1228, 5152, 1227, 5151], 1: [1152, 1151], 3: [5345, 5346], 15: [4926, 1137, 1136], 27: [5391, 1288, 1287], 38: [5242, 5240, 5241, 1242], 9: [5090, 5091], 37: [5317, 1138, 5316], 11: [5256, 5255, 1062], 19: [1182, 5272, 5271], 30: [5181, 1318, 1317], 39: [5225, 5227, 5226], 22: [5122, 1437, 1436]}, {0: [2526, 4017, 4019, 4018], 2: [2781, 2780, 2779], 4: [2677, 4409, 2527, 2632, 4318], 5: [2466, 2465, 4048], 7: [2480, 3944, 3943, 3942], 8: [3958, 2406, 3957, 2405], 12: [3989, 2631, 2630], 13: [2764, 4154, 2765, 2766], 16: [4139, 4137, 4138], 18: [2675, 4109, 2676], 23: [4122, 3988, 2435, 2436], 32: [2705, 3854, 3853, 2376, 2375], 33: [3898, 3899, 2585, 2584], 36: [4078, 4079, 2570, 2571], 14: [3824, 3823, 2541, 2540], 34: [2752, 4273, 4274], 17: [4288], 21: [3883, 3884, 2645, 2647, 2646], 25: [4259, 2497, 4258], 26: [4228, 2421, 4034, 4033, 2420], 28: [2542, 4182, 4184, 4183], 29: [4244, 2661, 2662], 31: [4334, 2735, 2736, 2737], 6: [4049, 2707, 2706], 10: [4199, 2481, 4198], 20: [2512, 2511, 2510, 3913], 24: [4213, 2572, 4214], 35: [4167, 4169, 4168], 1: [2751, 4003, 4004], 3: [3914, 2750], 15: [2451, 2450, 3973, 3974], 27: [4064, 2720, 2721], 38: [2614, 2616, 2615], 9: [2691, 2690], 37: [4108, 2599, 2601, 2600], 11: [4094, 2496, 4093], 19: [2557, 4153, 2556], 30: [2796, 4229, 4289, 2722], 39: [4124, 4123], 22: [2586]}, {0: [3470, 3468, 3469, 840, 841, 842], 2: [872, 3454, 3455], 4: [1005, 3034, 705, 3032, 3033], 5: [630, 3064, 3063], 7: [1036, 3320, 3318, 3319], 8: [3259, 3184, 947, 946], 12: [3289, 855, 857, 856], 13: [885, 887, 3168, 886, 3169], 16: [782, 916, 917, 3408, 3409], 18: [3453, 3452, 615, 616, 617], 23: [3273, 632, 631], 32: [3424, 811, 812], 33: [795, 3227, 3228, 796], 36: [902, 3123, 901, 3124], 14: [3335, 3333, 3334], 34: [3080, 3290, 992, 990, 991], 17: [3094, 3095], 21: [3109, 3108, 3153, 645], 25: [3182, 825, 3183], 26: [3062, 3303, 600, 601], 28: [720, 945, 3049, 3047, 3048], 29: [1035, 931, 3139, 3140], 31: [975, 976], 6: [3212, 735, 736, 3214, 3213], 10: [870, 3198, 871, 3199], 20: [3065, 1020, 1022, 1021], 24: [810, 3079, 3138, 3078, 675], 35: [3348, 3350, 780, 781, 3349], 1: [646, 1006, 3377, 3378, 3379], 3: [977, 1037, 3394], 15: [737], 27: [691, 692], 38: [3093, 721, 3393, 722], 9: [3288, 676], 37: [3274, 3364, 3438, 3439, 932], 11: [3423, 647, 587, 586, 3407], 19: [3363, 750, 751, 752], 30: [960, 961, 3243, 3242, 3244], 39: [768, 766, 767], 22: [1081, 3154, 3155]}, {0: [4294, 995, 997, 996], 2: [3993, 4293, 741, 742], 4: [1116, 1117, 4070, 4071], 5: [4400], 7: [772, 4025, 4024, 4113, 771], 8: [4099, 936], 12: [980, 4083, 4084], 13: [4280, 4278, 4279], 16: [4308, 1027, 4310, 4309], 18: [4323, 4325, 862, 4324], 23: [981, 982], 32: [4204, 937, 1026, 4205], 33: [1073, 1058, 938, 4430], 36: [4190, 1103, 1102], 14: [727, 4189, 4188], 34: [3995, 3994], 17: [1145, 3980, 3979, 815], 21: [4355, 1041, 1042], 25: [4146, 4100, 1206, 1207], 26: [1070, 1072, 1071], 28: [906, 4130, 4129], 29: [4114, 1146, 4115], 31: [4160, 4158, 4159], 6: [1011, 4415, 1012], 10: [1086, 1088, 1087], 20: [4399, 4128, 816, 817], 24: [967, 4235, 965, 966], 35: [4385, 4384, 891, 892], 1: [4340, 4339, 922, 921], 3: [4234, 801], 15: [4069, 861], 27: [4143, 4250, 786, 4249], 38: [785, 1101, 4055, 4054], 9: [846, 4354, 847], 37: [4174, 876, 4219], 11: [4265, 877, 4263, 4264], 19: [1161, 4144, 4145], 30: [757, 4040, 4039, 756], 39: [4220, 951, 952], 22: [4175, 1057, 1055, 1056]}, {0: [3109, 3110], 2: [930, 931], 4: [3215, 1050, 3170, 1051], 5: [3273, 3274, 975, 3335, 976], 7: [3378, 960, 961, 3379], 8: [1066, 1005, 3155], 12: [945, 2975, 1035, 1036], 13: [3093, 3095, 916, 3094], 16: [825, 842, 841, 3169], 18: [1081, 3124, 3125], 23: [631, 3108, 630], 32: [735, 840, 3034, 3033], 33: [1155, 3050, 795, 3048, 3049], 36: [3439, 885, 886, 887], 14: [721, 720, 3004, 3003], 34: [3305, 932], 17: [3213, 3214], 21: [947, 946], 25: [3080, 811, 810, 3079], 26: [991, 990], 28: [3318, 3319, 3320], 29: [3018, 3019, 1021, 1020], 31: [3245, 3243, 3244], 6: [1097, 3139, 1096, 3140], 10: [676, 3290, 3289, 3288], 20: [692, 691, 3168], 24: [3260, 1006], 35: [3199, 902, 900, 901], 1: [646, 3348, 3350, 3349], 3: [737, 736], 15: [3064, 915], 27: [3183, 3185, 3184], 38: [872, 870, 3229, 871], 9: [3351, 3065, 1141, 1140], 37: [645, 3063, 765, 2974], 11: [3259, 855, 3198, 856], 19: [3154, 766, 767], 30: [780, 781], 39: [3334, 752, 3228, 751], 22: [1022, 3364, 796, 3363]}, {0: [4614, 1781, 1779, 1780], 2: [4629, 4628], 4: [4735, 1974, 4599, 4600], 5: [4838, 2095, 4840, 4839], 7: [1764, 4868, 1765, 4869], 8: [1870, 4824, 1869], 12: [2034, 1839, 4688, 4690, 4689], 13: [4915, 4914, 4913, 1705], 16: [1811, 4975, 4974], 18: [1676, 1674, 1675], 23: [1825, 4734], 32: [4958, 1690, 4960, 4959], 33: [4779, 1961, 1960, 4780], 36: [5065, 5063, 5064], 14: [1599, 1646, 1645, 4733], 34: [1809], 17: [1749, 4720, 4719], 21: [4569, 1661, 1660, 1659], 25: [1794, 1795], 26: [4870, 2005, 5019, 5020, 2006], 28: [1824, 4659, 1914, 4765], 29: [4749, 4750, 1991, 1990], 31: [4793, 1733, 4794, 1734], 6: [4944, 1915, 4945], 10: [1856, 4554, 1854, 1855], 20: [1810, 4763, 4764], 24: [4795, 4703, 4704, 1975, 1884], 35: [2035, 5003, 2036, 5004, 5005], 1: [1735, 4883, 4884], 3: [1555, 1554], 15: [4988, 1720], 27: [5018, 1630, 1631], 38: [4853, 4854, 1841, 1840], 9: [1539, 1570, 4778], 37: [1601, 1600, 1719, 4823], 11: [4930, 4928, 4929], 19: [1945, 4808, 4809], 30: [4658, 1615, 4718, 1614], 39: [1826, 4898, 4900, 4899], 22: [4673, 1900, 4674, 1899]}, {0: [1264, 4087, 4086, 1266, 1265], 2: [4041, 4042], 4: [1323, 1324, 3696, 3697], 5: [3938, 4058, 3937, 1535], 7: [3788, 3786, 3787], 8: [1459, 3801, 3802], 12: [1338, 1340, 1339], 13: [3848, 3920, 3847, 3846, 1174], 16: [3923, 3922, 3921], 18: [3816, 1296, 1295], 23: [1475, 1476], 32: [1520, 1518, 1519], 33: [3968, 3966, 3967], 36: [3876, 1430, 3878, 3877], 14: [3727, 4043, 1564, 1565], 34: [1325], 17: [1353, 1354, 1355, 4101], 21: [1534, 1249, 3772, 3771], 25: [3666, 3667, 1309], 26: [1445, 1444], 28: [3952, 3951, 1279, 1280], 29: [1386, 1383, 1385, 1384], 31: [1608, 1593, 3683, 1294, 3682], 6: [1491, 3997, 3996, 1250], 10: [1609, 4027, 4028, 1610], 20: [4102, 1504, 3863, 1505], 24: [3983, 3981, 3982], 35: [1549, 3908, 3906, 1460, 3907], 1: [1489, 3893, 1490], 3: [3698, 1594], 15: [1699, 3833], 27: [3757, 1204, 3755, 3756], 38: [3711, 3712, 3713, 1624, 1625], 9: [1144, 3892, 1205, 3891], 37: [3861, 3862, 3832, 1429], 11: [1413, 1415, 1414], 19: [4012, 1368, 1369, 1370], 30: [3726, 1234], 39: [1399, 3817, 1640, 3818], 22: [1235, 1310, 1400, 3936]}, {0: [2319, 4602, 2304, 2302, 2303], 2: [2289, 2559, 4707, 4708], 4: [4451, 4453, 4452], 5: [4377, 2394, 2392, 2393], 7: [4362, 2362, 2364, 2363], 8: [2379, 4557], 12: [4572, 2648, 4574, 4573], 13: [2272, 4512, 2273, 4513], 16: [2242, 4301, 4302, 4303], 18: [2287, 2288], 23: [4288, 4286, 2482, 4287], 32: [2632, 2633, 4647, 4648], 33: [2514, 2483, 2484, 4603], 36: [4437, 4439, 4438], 14: [4198, 4318, 2558, 2557], 34: [2574, 2573], 17: [2497, 2498], 21: [4542, 2318], 25: [2529, 4558, 2587, 2588], 26: [2422, 2423], 28: [2378, 4468, 4467], 29: [4348, 2468, 2467], 31: [4347, 2347, 2349, 2348], 6: [4422, 4423, 4424], 10: [2617, 4587, 4588, 4589, 2618], 20: [2542, 2377, 4257, 4258], 24: [4496, 2663, 4497, 4498], 35: [4483, 2333, 4481, 4482], 1: [2317, 4392, 2437, 4393], 3: [2631, 4272, 4273], 15: [2153, 4317, 4316, 2152], 27: [4527, 4528], 38: [4619, 2499, 2407, 2408, 4618], 9: [2438], 37: [2451, 2453, 2452], 11: [4543, 2602, 2603], 19: [2527, 4363, 2528], 30: [4407, 2543, 4408], 39: [2257, 4332, 4333], 22: [4378, 2512, 2513]}, {0: [2543, 2542, 4078, 2541], 2: [4482, 4483, 4484], 4: [2393, 4513, 4512], 5: [2468, 2466, 2467], 7: [2676, 4228, 4229], 8: [2451, 4258], 12: [4259, 2722, 4423, 4424, 2723], 13: [4318, 2573, 2572], 16: [2526, 2528, 2527], 18: [4303, 2603, 2602], 23: [4439, 4438], 32: [4154, 4153], 33: [2483, 2481, 2482], 36: [4409, 4408], 14: [2691, 2693, 2692, 4244], 34: [4377, 4527, 2423, 2422], 17: [4212, 4422, 2347, 2348], 21: [2407, 4349, 4348, 4347, 2392], 25: [4257, 2317, 2318], 26: [2511, 2363, 2362, 4183, 4182], 28: [4362, 2377, 2378], 29: [2452, 4453, 4452], 31: [2663, 2707, 2708, 4514], 6: [2586, 2587, 4363], 10: [2677, 4378, 4379], 20: [4213, 4214], 24: [2436, 4302, 2437], 35: [2496, 4334, 4333, 2497], 1: [4138, 2631, 4364, 2632], 3: [2661, 4184], 15: [4123, 4124], 27: [2557], 38: [2512, 4287, 2601, 4288], 9: [4199, 4198], 37: [2646, 2648, 2647], 11: [4469, 4467, 4468], 19: [4497, 2558, 4498], 30: [2662, 4272, 4273], 39: [2616, 2618, 2617], 22: [4394, 4392, 4393]}, {0: [3609, 3608, 1607, 1608], 2: [1563, 3668], 4: [3638, 1861, 1862, 3639, 1863], 5: [1548, 1546, 3473, 1547], 7: [1502, 3488, 3489], 8: [3490, 1832, 1833], 12: [1847, 3577, 3578, 3579, 1848], 13: [3308, 1592, 1591], 16: [3368, 1743, 1742, 3444], 18: [3383, 1622, 1624, 1623], 23: [1682, 3443], 32: [3505, 1787, 1818, 3504], 33: [3562, 3564, 3563], 36: [1756, 1758, 1757], 14: [1516, 1637, 3354, 1562, 3353], 34: [3549, 1698, 3669, 1788], 17: [1921, 3594, 1922, 1923], 21: [3279, 1532, 1531, 3278], 25: [1982, 3370, 3369], 26: [3474, 1802, 1804, 1803], 28: [3458, 1876, 1877, 3459], 29: [1891, 3293, 3294, 3295], 31: [3412, 1576, 1577, 1578], 6: [1652, 1653], 10: [1473, 3624, 3622, 3623], 20: [3593, 1638], 24: [3518, 3519, 3520, 1892], 35: [1472, 3325, 3324, 3323], 1: [3547, 3548], 3: [3503, 1517], 15: [3427, 3428], 27: [1712, 3397, 3398], 38: [3430, 3429, 1727, 1726], 9: [1488, 1487], 37: [1668, 1667], 11: [3399, 3309, 1817], 19: [1937, 3413, 3414], 30: [1593, 3535, 3533, 3534], 39: [3234, 3233, 1697, 1696], 22: [1773, 1771, 1772]}, {0: [998, 999, 4969, 4970, 1000], 2: [4968, 4832, 654, 655], 4: [4683, 4774, 790, 789], 5: [4595, 4760, 1059], 7: [803, 4639, 4638, 4700, 1044], 8: [4624, 4623], 12: [864, 4730, 4729, 4728], 13: [4984, 5060, 1046, 1045], 16: [924, 4849, 925], 18: [4833, 985, 4834], 23: [1091, 1090], 32: [760, 759, 4669, 4668], 33: [1089, 4610, 4609], 36: [1029, 1031, 1030], 14: [4865, 4863, 4864], 34: [699, 4699, 4698], 17: [4773, 731, 4803, 730], 21: [4880, 4878, 955, 4879], 25: [833, 4654, 834, 4653], 26: [4684, 4685], 28: [894, 895, 4894], 29: [819, 820, 4999, 4998], 31: [744, 4818, 745], 6: [941, 939, 940], 10: [4743, 4745, 4744], 20: [670, 4594, 4593, 669], 24: [984, 4713, 4715, 4714], 35: [909, 4819, 910, 4759], 1: [804, 4788, 4790, 4789], 3: [4758, 715, 714], 15: [1149, 4820, 1075], 27: [4910, 4909, 849, 850], 38: [1015, 4804, 4775, 1014], 9: [1104, 1105, 1106], 37: [879, 4925, 4924, 880], 11: [969, 970], 19: [851, 4955, 4954, 835], 30: [5075, 5074, 865, 866], 39: [805, 4940, 4939], 22: [774, 4848, 775]}, {0: [5362, 1632, 5363, 1633], 2: [5258, 1542], 4: [5094, 5152, 5153, 5154, 1721], 5: [1663, 1662], 7: [1751, 1753, 5259, 1752], 8: [5197, 5198], 12: [5032, 1571, 5288, 1572], 13: [5318, 1812, 1813, 5319], 16: [5305, 5303, 5304], 18: [1601, 1603, 1602], 23: [1678], 32: [1722], 33: [5348, 5347], 36: [1618, 1616, 1617], 14: [5273, 1843, 5274], 34: [1541], 17: [1573, 1452, 1453, 5392], 21: [1857, 5243, 5244], 25: [1437, 1438, 5439, 5438, 5437], 26: [1498, 1497, 5109, 5108], 28: [5017, 5018, 1738, 1737, 1736], 29: [5184, 5182, 5183], 31: [1767, 1768], 6: [1648, 1647, 5213], 10: [5139, 1587, 5138], 20: [1858, 5393, 5394], 24: [1422, 5167, 5168], 35: [5078, 1707, 1706], 1: [1872, 5333, 5334, 5335], 3: [1873, 1844, 1723, 5454], 15: [1796, 1842, 5079], 27: [1828, 5123, 5124, 1827], 38: [5227, 5229, 5228], 9: [1482, 1483], 37: [5289, 1798, 1797], 11: [1783, 5169, 1782], 19: [1693, 5409, 5408], 30: [5424, 5423], 39: [1887, 1888, 5378, 5379], 22: [5377, 1558, 1556, 1557]}, {0: [2141, 2142, 5172, 5171], 2: [5068, 5067, 5066], 4: [2380, 4827, 4826, 2140], 5: [4992, 4991], 7: [5096, 5098, 2426, 5097], 8: [5126, 2111, 2110], 12: [4946, 2170, 2171, 5051], 13: [2365, 2367, 2366], 16: [2080, 2081, 5187, 5186, 5185], 18: [2456, 2455, 4857], 23: [5202, 2321, 2322], 32: [5083, 5081, 5082], 33: [5143, 2471, 2472], 36: [2441, 4963, 2440], 14: [2201, 2231, 5022, 5021], 34: [2186, 4901, 2125], 17: [2215, 4812, 4811], 21: [5053, 2381, 5052], 25: [2320, 4796, 4797], 26: [2485, 2486], 28: [4931, 4932, 4933], 29: [4873, 2305, 4872], 31: [5216, 2292, 2290, 2291], 6: [2395, 2397, 2396], 10: [4916, 2425, 4917], 20: [2217, 2216], 24: [4842, 2245, 4841], 35: [4871, 5007, 5006, 2230], 1: [5157, 2411, 5158], 3: [2202], 15: [4782, 4781, 2156, 2155], 27: [5113, 2336, 5112], 38: [2335, 2547, 2546, 4947, 4948], 9: [2337, 2246, 5142], 37: [2306, 5037, 5036], 11: [2352, 2350, 2351], 19: [5127, 2261, 4902, 2260], 30: [4856, 4962, 2275], 39: [2410, 4977, 4978], 22: [4798, 2470, 4888, 4886, 4887]}, {0: [1447, 4190, 4191, 4192], 2: [1432, 1431], 4: [1446, 1235, 4042, 4041], 5: [1356, 4267, 4266], 7: [4341, 1133, 4340, 1132], 8: [1056, 1057], 12: [1400, 1401, 4207, 1297, 4310, 4311], 13: [1252, 4206, 1250, 1251], 16: [1207, 1205, 1206], 18: [4222, 3996, 1325, 1326], 23: [4070, 1371, 1370, 4071, 4072], 32: [4177, 4176, 4175], 33: [4162, 1462, 1461], 36: [4252, 4251], 14: [996, 4235, 4237, 4236], 34: [1430, 1415, 4027], 17: [1070, 1130, 3951, 3950], 21: [1282, 1236, 4221], 25: [1265, 1055, 3966, 3965], 26: [4012, 4011, 1312, 1311], 28: [1295, 4115, 4116, 1296], 29: [4145, 1145, 1146], 31: [4010, 1160, 1162, 1161], 6: [4147, 4146, 1221], 10: [4102, 4401, 4402, 1416, 1417], 20: [4265, 1071, 1072], 24: [4100, 1355, 4101], 35: [4282, 4281, 1222, 4280], 1: [4085, 1117, 1116], 3: [1012, 4160, 1011], 15: [1103, 1237, 4386, 4385], 27: [1087, 4131, 4130, 1085, 1086], 38: [4295, 1192, 1190, 1191], 9: [1386, 4086], 37: [1100, 1102, 1101], 11: [4025, 1267, 4026, 1266], 19: [3982, 1220, 3980, 3981], 30: [3936, 3935], 39: [1175, 1176], 22: [4056, 1340, 4057]}, {0: [5161, 5160, 179, 178, 177], 2: [449, 5580, 5581], 4: [479, 5550, 5552, 644, 5551], 5: [5190, 462, 5191], 7: [5385, 568, 5282, 5281, 239, 238], 8: [5565, 5445, 208, 209], 12: [5597, 5595, 5596], 13: [253, 5478, 5475, 5477, 5476], 16: [492, 5236, 5237, 612, 613], 18: [5147, 314, 312, 313, 5146], 23: [388, 387, 5206, 5207], 32: [297, 5265, 5266], 33: [523, 5267, 5162, 522], 36: [5402, 5400, 5401], 14: [5356, 448, 447], 34: [629, 5582], 17: [464, 5386, 463], 21: [327, 329, 5311, 328], 25: [5567, 494, 659, 5566], 26: [5372, 5222, 643, 642, 5223], 28: [5448, 554, 5446, 5447], 29: [403, 404], 31: [419, 5251, 418], 6: [5221, 432, 5298, 553, 5297], 10: [628, 627, 5252], 20: [374, 372, 373], 24: [507, 5327, 509, 5371, 508], 35: [477, 5341, 164, 163, 5340], 1: [672, 5461, 673, 5463, 5462], 3: [446, 5177, 357, 5176], 15: [5355], 27: [268, 5522, 5520, 5521], 38: [5537, 5536, 223, 224, 5535], 9: [5432, 569], 37: [194, 193, 5415, 5416, 5417, 5418], 11: [5312, 493], 19: [657, 5387, 658], 30: [5505, 5507, 5506], 39: [5357, 537, 539, 538], 22: [524, 5493, 5492]}, {0: [4873, 4872, 2365, 2364, 2363], 2: [2320, 2485, 4842], 4: [4737, 4887, 4783, 2395], 5: [2348, 2528, 4482, 2633, 4483], 7: [2499, 2498, 4557, 4558], 8: [4662, 2380, 2379], 12: [4857, 2423, 4933, 2425, 2424], 13: [4452, 4453, 2649, 2648], 16: [4874, 2709, 4754, 2710], 18: [4888, 4889, 2755, 2754, 4559, 2663], 23: [4527, 4528], 32: [2274, 4752, 4753], 33: [4439, 4438, 4437, 2304, 2303], 36: [2678, 2679, 4617, 4618, 4619], 14: [2558, 2559, 2319, 4692, 4693], 34: [4829, 4827, 4828], 17: [2407, 2408, 4798, 2409], 21: [2635, 4768, 2634, 4769], 25: [4813, 4812], 26: [4408, 2394, 2393], 28: [4497, 2437, 2439, 2438], 29: [4724, 2545, 4723], 31: [2483, 2484, 4739, 4738], 6: [2784, 2349, 4709, 4708, 4707], 10: [2769, 4543, 4544, 2768], 20: [4484, 2708, 4424, 4423], 24: [2452, 2453, 2455, 2454], 35: [4649, 4647, 2664, 4648], 1: [2544, 4633, 2543, 4634, 2694], 3: [4603, 2468, 2469], 15: [4663], 27: [4678, 2574, 2573, 4468, 4467], 38: [2530, 4573, 2529], 9: [2422, 4393], 37: [2513, 2514, 2515], 11: [4588, 4589, 4604, 2589, 2588], 19: [4498, 2604, 2603], 30: [4512, 4514, 4513], 39: [4574, 4529, 2693], 22: [2619, 4302, 4303, 2618, 2617]}, {0: [1892, 1893, 1804, 3744], 2: [1757, 3399, 3398], 4: [3547, 3548, 3549], 5: [3459, 1819, 1818], 7: [3729, 1832, 1834, 1833], 8: [3490, 3639, 1863, 1862], 12: [1608, 1607, 3579, 3578], 13: [3772, 1879, 3774, 3773], 16: [1789, 1788], 18: [3669, 1759, 1758], 23: [3700, 3698, 3699], 32: [1803, 1787, 3474], 33: [3685, 1848, 1849], 36: [3683, 3684], 14: [1714, 1712, 1713], 34: [1878, 1877], 17: [1562, 1682, 3458], 21: [1727, 1729, 3743, 1728], 25: [1564, 3638, 1563], 26: [3804, 1743, 1744], 28: [1413, 3607, 3609, 3608], 29: [1654, 1653], 31: [3504, 1907, 3505], 6: [3592, 3594, 3593], 10: [3429, 1773, 1772], 20: [3519, 3610, 3520, 1968], 24: [3564, 1593, 3563], 35: [1742, 3489, 1669, 1668], 1: [3713, 3714, 3715, 3640, 1908], 3: [2058, 2057, 3444, 3445], 15: [3653, 3654], 27: [3788, 3789], 38: [3728, 3473, 3803, 1638, 1639], 9: [3790, 1938, 1939], 37: [3625, 1548, 3624, 3623], 11: [1549, 3849, 1594, 3848], 19: [1578, 1579], 30: [1697, 1699, 1698], 39: [3757, 1624, 3758], 22: [1623, 3535, 3533, 3534]}, {0: [306, 4185, 4186, 4187], 2: [4065, 172, 171], 4: [203, 4336, 4335, 202], 5: [426, 4110, 4111], 7: [366, 4201, 367], 8: [338, 4156, 336, 337], 12: [4125, 292, 291], 13: [246, 247, 4382, 4381], 16: [233, 231, 232], 18: [4350, 4352, 307, 4351], 23: [516, 4202], 32: [4097, 4095, 4096], 33: [503, 501, 4261, 502], 36: [456, 4275, 4276], 14: [4277, 4066, 4067, 532, 531], 34: [173, 4455], 17: [4410, 4412, 4411], 21: [321, 322], 25: [427, 4456], 26: [4247, 127, 4245, 4246], 28: [188, 4366, 4365], 29: [4426, 382, 383], 31: [201, 4140, 381, 4141], 6: [4291, 187, 186, 4290], 10: [4216, 262, 261], 20: [4170, 218, 217, 216], 24: [276, 277], 35: [4231, 412, 4232], 1: [4050, 4052, 4051], 3: [4021, 260], 15: [350, 3991, 411], 27: [4322, 4320, 4321], 38: [353, 351, 4396, 352], 9: [156, 4260, 157], 37: [4171, 440, 441], 11: [442, 4307, 4305, 4306], 19: [397, 398], 30: [472, 471, 4367, 4126], 39: [488, 4397, 4081, 486, 487], 22: [308, 4440, 4441]}, {0: [4053, 4054, 1041, 4055], 2: [4220, 966], 4: [3995, 4203, 4204, 4205, 1056, 1055], 5: [801, 799, 3933, 800], 7: [829, 861, 4098, 830], 8: [4114, 4113], 12: [755, 4234, 4235, 756, 757], 13: [1026, 1025, 3964, 3965], 16: [3979, 816, 815], 18: [4025, 3814, 952, 951, 950], 23: [995, 4070, 4069, 4068], 32: [891, 4083, 4084], 33: [4189, 4188, 681], 36: [981, 979, 980], 14: [3934, 876, 4174, 874, 875], 34: [636, 4219, 4218], 17: [860, 3993, 3994], 21: [3920, 3919, 3918], 25: [936, 1040, 4040], 26: [846, 844, 845], 28: [742, 4039, 740, 741, 4038], 29: [3875, 3873, 3874], 31: [711, 710], 6: [4127, 4129, 4128, 725, 726], 10: [4159, 4158], 20: [4143, 906, 4144], 24: [3813, 3844, 786, 785, 784], 35: [1085, 771, 3860, 3859, 770], 1: [695, 4010, 4009, 4008], 3: [696, 4173], 15: [3769, 3799, 889], 27: [814, 3904, 3903], 38: [3948, 890, 3949], 9: [3902, 3963, 680], 37: [4145, 1009, 1011, 1010], 11: [3845, 935], 19: [3828, 3829, 3830, 3980, 1115], 30: [3888, 3890, 3889], 39: [964, 965], 22: [4099, 922, 920, 921]}, {0: [1968, 3595, 1970, 1969], 2: [1894, 3805], 4: [3730, 3731], 5: [3865, 2165, 3866], 7: [3670, 2345, 3671, 3672, 2344], 8: [2073], 12: [3642, 3700, 3641, 3640, 1984], 13: [2148, 3850, 2149, 3851], 16: [4002, 4000, 4001, 2150], 18: [3895, 2179, 2180, 3896], 23: [3715, 2000, 1999, 3685], 32: [2088, 2090, 2089], 33: [3942, 3940, 3941], 36: [3970, 2195, 2075, 3971], 14: [2060, 2059, 2058, 3686, 3687], 34: [2031, 2029, 2030], 17: [3732, 2359, 2360, 3897], 21: [2118, 3986, 2120, 2119], 25: [3626, 3702, 2223], 26: [2015, 2014], 28: [3776, 3655, 2164, 3656], 29: [3792, 2284, 3852], 31: [2299, 3987, 2300], 6: [2255, 3910, 2254, 3911], 10: [3881, 3882], 20: [3956, 2268, 2270, 2269], 24: [2225, 1954, 3835, 2224, 3836], 35: [3790, 2074, 3791], 1: [2330, 3925, 3926, 3927], 3: [2346, 4031, 4032], 15: [2194], 27: [2238, 3820, 2239, 3821], 38: [2210, 3745, 3746, 2209], 9: [1985], 37: [3760, 2328, 2329, 3762, 3761], 11: [2135, 2133, 2134], 19: [2253, 3717, 3716], 30: [3806, 3807], 39: [2105, 3775, 3701, 2104], 22: [4046, 4047, 2314, 2315]}, {0: [5120, 1046, 5209, 1047], 2: [1136, 1045, 1030, 4910], 4: [1241, 5122, 5121], 5: [1167, 5060, 1166], 7: [1303, 5255, 1227, 5256], 8: [1376, 1377, 5210, 5211], 12: [1196, 5016, 5014, 5015], 13: [1106, 1108, 1107], 16: [5285, 1017, 5075, 1016], 18: [1121, 5090, 1123, 1122], 23: [5359, 1001, 1002], 32: [5376, 5375, 1092, 1093], 33: [5269, 5271, 5270], 36: [5405, 1061, 1062, 1063], 14: [5135, 1033, 1031, 1032], 34: [4911, 1271, 1272], 17: [5092, 1317, 5091], 21: [5076, 1182, 5030, 1181], 25: [1346, 5047, 5046], 26: [5136, 1211, 1212], 28: [1288, 1286, 1287], 29: [5195, 5152, 5196, 1302], 31: [5317, 1332, 1331], 6: [5316, 1137, 1138], 10: [5179, 5181, 5180], 20: [5240, 5241], 24: [1361, 5106, 5107], 35: [5150, 5151, 1242], 1: [5346, 5344, 1197, 5345], 3: [5225, 5226], 15: [1243, 5420, 5421], 27: [5302, 5300, 5301], 38: [1256, 5406, 1257, 1258], 9: [5105, 987, 986], 37: [5315, 1076, 1078, 1077], 11: [1151, 5045], 19: [5360, 5361, 1347], 30: [5390, 5391, 1318], 39: [5332, 5330, 1152, 5331], 22: [1406, 1407, 5287, 1273, 5286]}, {0: [1032, 5240, 1167</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>[577, 598, 592, 585, 612, 587, 578, 653, 609, 615, 585, 576, 614, 583, 587, 575, 591, 561, 586, 587, 580, 593, 574, 599, 575, 588, 606, 587, 602, 574, 561, 561, 548, 611, 622, 557, 554, 585, 557, 554, 532, 662, 576, 589, 546, 602, 635, 588, 583, 583, 587, 577, 604, 634, 600, 550, 605, 559, 607, 563, 588, 583, 625, 619, 601, 639, 577, 604, 629, 586, 617, 638, 607, 627, 562, 579, 659, 587, 575, 571, 594, 604, 592, 576, 605, 631, 566, 538, 583, 584, 558, 563, 603, 562, 596, 579, 572, 581, 598, 558]</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>[133, 130, 127, 132, 131, 123, 141, 136, 136, 140, 137, 118, 135, 155, 133, 134, 139, 139, 134, 124, 135, 138, 124, 130, 139, 151, 152, 130, 130, 140, 135, 135, 127, 149, 130, 129, 125, 136, 144, 138, 127, 135, 131, 133, 131, 128, 126, 131, 132, 121, 130, 124, 129, 126, 140, 136, 139, 124, 125, 134, 122, 122, 131, 136, 128, 135, 137, 132, 129, 132, 128, 138, 141, 127, 129, 141, 129, 130, 133, 130, 130, 133, 128, 123, 136, 145, 137, 152, 131, 130, 131, 142, 150, 128, 138, 126, 151, 144, 133, 132]</t>
-        </is>
+          <t>[1.6625113487243652, 1.9390292167663574, 1.4789783954620361, 2.9375765323638916, 2.0075018405914307, 2.985349655151367, 1.7945563793182373, 1.4265046119689941, 2.4031927585601807, 2.4082133769989014, 1.7461261749267578, 2.83158802986145, 1.6064908504486084, 2.8140363693237305, 1.5839533805847168, 1.245661973953247, 2.185072660446167, 2.032407760620117, 0.9030394554138184, 1.385160207748413, 1.3342080116271973, 2.712493419647217, 1.6024935245513916, 0.9927964210510254, 2.343881130218506, 1.2360732555389404, 1.4889051914215088, 1.403932809829712, 1.6416053771972656, 0.8741812705993652, 1.7117092609405518, 1.7332885265350342, 2.514055013656616, 3.04793119430542, 2.0753650665283203, 1.5336976051330566, 2.888305902481079, 2.395442247390747, 1.3685219287872314, 1.2308645248413086, 2.859231948852539, 0.9496307373046875, 2.1298739910125732, 2.4211196899414062, 1.4886796474456787, 2.346733331680298, 1.3443360328674316, 2.004361152648926, 2.099306583404541, 1.6191675662994385, 1.2798938751220703, 2.7310783863067627, 1.9969723224639893, 1.0911805629730225, 1.8787426948547363, 2.312145948410034, 2.5361099243164062, 1.6546049118041992, 1.277308702468872, 1.2051968574523926, 1.0788681507110596, 2.023848533630371, 1.6109974384307861, 1.623262882232666, 2.9495317935943604, 0.9431965351104736, 2.1581296920776367, 1.6569583415985107, 1.25803542137146, 1.3993299007415771, 1.3975446224212646, 3.015129327774048, 2.224008560180664, 1.6765048503875732, 2.4402990341186523, 2.865541458129883, 1.3673980236053467, 4.4167115688323975, 1.1707477569580078, 3.2855615615844727, 4.268656492233276, 1.2180325984954834, 2.4960248470306396, 1.9486846923828125, 2.122032403945923, 2.408773899078369, 2.2054481506347656, 2.1937496662139893, 2.4968674182891846, 1.6183910369873047, 1.8621165752410889, 1.5093748569488525, 1.57204008102417, 2.521735429763794, 2.570600986480713, 2.666222333908081, 1.7922489643096924, 2.5203607082366943, 2.565200090408325, 2.614882707595825]</t>
+        </is>
+      </c>
+      <c r="AF6" t="n">
+        <v>880</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>250</v>
       </c>
       <c r="AH6" t="n">
-        <v>25.72333570904054</v>
+        <v>250</v>
       </c>
       <c r="AI6" t="n">
-        <v>7.412002278586925</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL6" t="inlineStr">
-        <is>
-          <t>[21.202367305755615, 17.12324547767639, 11.41109824180603, 26.641306400299072, 19.684669017791748, 15.411335229873657, 22.664333820343018, 15.611384630203247, 27.57191276550293, 18.05035662651062, 21.992186307907104, 26.24391531944275, 25.530449151992798, 20.51543140411377, 12.202906847000122, 21.471049070358276, 15.22265625, 24.40701389312744, 22.343660354614258, 12.797702074050903, 20.785868406295776, 15.712550640106201, 16.348380088806152, 15.90837836265564, 30.91939377784729, 14.271824836730957, 20.754175662994385, 14.066508293151855, 13.41293978691101, 21.1462459564209, 25.56670832633972, 26.477521181106567, 26.22222638130188, 10.190853357315063, 15.25717282295227, 20.649556636810303, 14.901387691497803, 17.486640453338623, 24.12067675590515, 26.95597529411316, 33.19077444076538, 15.970278263092041, 19.157680988311768, 25.90647578239441, 23.794183492660522, 9.722698450088501, 11.986931562423706, 23.094684600830078, 12.35834264755249, 25.693645238876343, 23.568758010864258, 18.237729787826538, 14.97902226448059, 16.277510166168213, 26.14507555961609, 13.802763938903809, 12.480957746505737, 22.38634181022644, 28.232869863510132, 34.39499568939209, 14.877748489379883, 14.79174280166626, 24.22863483428955, 18.72968578338623, 20.916091918945312, 23.64266061782837, 16.40866994857788, 16.21902823448181, 16.312846183776855, 24.728204250335693, 13.890604019165039, 13.896397590637207, 17.4173846244812, 28.71347665786743, 31.4583420753479, 20.133112907409668, 14.148967027664185, 20.761720418930054, 19.12813377380371, 16.6443350315094, 21.300541877746582, 15.796643495559692, 14.348553895950317, 15.833485841751099, 18.631818056106567, 19.385186672210693, 20.885730743408203, 21.800116300582886, 17.273578643798828, 18.92692279815674, 18.92389178276062, 19.688615560531616, 29.645623683929443, 20.386237382888794, 17.135771989822388, 9.217562437057495, 15.658275365829468, 11.368450164794922, 19.414942026138306, 17.63179636001587]</t>
-        </is>
-      </c>
-      <c r="AM6" t="inlineStr">
-        <is>
-          <t>[1.0044102668762207, 1.6007425785064697, 1.1873817443847656, 1.2449455261230469, 0.8067021369934082, 1.1749553680419922, 1.134737491607666, 0.9295828342437744, 1.9970622062683105, 1.1505405902862549, 1.4689610004425049, 1.101470947265625, 0.8441252708435059, 0.8388116359710693, 1.3667569160461426, 1.0146079063415527, 1.7736458778381348, 1.8985340595245361, 1.173868179321289, 1.0486533641815186, 2.19638729095459, 0.9357469081878662, 2.2362613677978516, 1.449674367904663, 1.7411456108093262, 1.0583229064941406, 1.122087001800537, 1.5435740947723389, 0.8958888053894043, 0.9741184711456299, 2.99871563911438, 1.996805191040039, 1.8416290283203125, 0.8415234088897705, 1.3742225170135498, 1.3411743640899658, 1.400406837463379, 1.8691587448120117, 1.8389756679534912, 0.6694011688232422, 1.1134183406829834, 1.4523849487304688, 1.6596362590789795, 1.4095592498779297, 1.3576102256774902, 1.4411389827728271, 1.1810414791107178, 2.3012735843658447, 1.2500252723693848, 1.6653423309326172, 1.1228086948394775, 1.8272557258605957, 0.9650394916534424, 1.3804936408996582, 0.8707263469696045, 1.0841221809387207, 2.2486557960510254, 2.014078140258789, 2.04750657081604, 1.9975807666778564, 0.8363842964172363, 2.0888357162475586, 1.694915533065796, 1.6606450080871582, 1.0727767944335938, 1.4036571979522705, 1.6111137866973877, 1.5541424751281738, 2.4081358909606934, 1.8343546390533447, 2.303412675857544, 1.3931350708007812, 1.1362810134887695, 2.4246842861175537, 1.2590429782867432, 1.4284203052520752, 1.0504505634307861, 1.3791401386260986, 0.7984826564788818, 1.3464727401733398, 1.1701838970184326, 2.5152785778045654, 1.057816505432129, 1.42724609375, 1.4972069263458252, 1.1411957740783691, 1.194103717803955, 0.8449912071228027, 1.771437168121338, 1.563765048980713, 1.0156464576721191, 1.1369049549102783, 0.807525634765625, 1.0129642486572266, 1.2409553527832031, 1.1947929859161377, 2.5205588340759277, 1.3739690780639648, 2.1215670108795166, 1.0146527290344238]</t>
-        </is>
-      </c>
-      <c r="AN6" t="n">
-        <v>960</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>250</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>290</v>
-      </c>
-      <c r="AQ6" t="n">
         <v>40</v>
       </c>
-      <c r="AR6" t="inlineStr">
-        <is>
-          <t>[0, 2, 's_0_2', 4, 's_0_4', 5, 's_0_5', 7, 's_0_7', 8, 's_0_8', 12, 's_0_12', 13, 's_0_13', 16, 's_0_16', 18, 's_0_18', 23, 's_0_23', 32, 's_0_32', 33, 's_0_33', 36, 's_0_36', 's_0_0', 's_2_12', 14, 's_2_14', 's_2_18', 34, 's_2_34', 's_2_2', 's_4_12', 17, 's_4_17', 's_4_18', 21, 's_4_21', 25, 's_4_25', 26, 's_4_26', 28, 's_4_28', 29, 's_4_29', 31, 's_4_31', 's_4_34', 's_4_4', 6, 's_5_6', 10, 's_5_10', 20, 's_5_20', 's_5_21', 's_5_23', 24, 's_5_24', 's_5_26', 's_5_33', 35, 's_5_35', 's_5_5', 1, 's_7_1', 3, 's_7_3', 's_7_8', 's_7_10', 's_7_13', 15, 's_7_15', 's_7_20', 's_7_26', 27, 's_7_27', 's_7_31', 's_7_32', 38, 's_7_38', 's_7_7', 's_8_12', 's_8_25', 's_8_28', 's_8_32', 's_8_35', 's_8_8', 9, 's_12_9', 's_12_17', 's_12_21', 's_12_24', 's_12_28', 's_12_34', 's_12_35', 37, 's_12_37', 's_12_38', 's_12_12', 's_13_9', 11, 's_13_11', 's_13_14', 's_13_16', 's_13_18', 19, 's_13_19', 's_13_21', 's_13_27', 's_13_29', 30, 's_13_30', 's_13_35', 39, 's_13_39', 's_13_13', 's_16_1', 's_16_6', 's_16_10', 's_16_11', 's_16_18', 's_16_20', 22, 's_16_22', 's_16_32', 's_16_36', 's_16_16', 's_18_6', 's_18_21', 's_18_24', 's_18_27', 's_18_30', 's_18_35', 's_18_36', 's_18_39', 's_18_18', 's_23_1', 's_23_14', 's_23_19', 's_23_33', 's_23_37', 's_23_39', 's_23_23', 's_32_3', 's_32_6', 's_32_14', 's_32_33', 's_32_37', 's_32_38', 's_32_32', 's_33_6', 's_33_9', 's_33_22', 's_33_26', 's_33_36', 's_33_33', 's_36_10', 's_36_14', 's_36_21', 's_36_29', 's_36_35', 's_36_38', 's_36_39', 's_36_36', 's_14_3', 's_14_20', 's_14_37', 's_14_39', 's_14_11', 's_14_15', 's_14_27', 's_14_35', 's_14_14', 's_34_10', 's_34_22', 's_34_24', 's_34_28', 's_34_34', 's_17_20', 's_17_38', 's_17_22', 's_17_24', 's_17_25', 's_17_29', 's_17_30', 's_17_17', 's_21_1', 's_21_6', 's_21_11', 's_21_27', 's_21_28', 's_21_31', 's_21_35', 's_21_38', 's_21_21', 's_25_38', 's_25_11', 's_25_19', 's_25_22', 's_25_28', 's_25_29', 's_25_25', 's_26_38', 's_26_24', 's_26_27', 's_26_28', 's_26_35', 's_26_26', 's_28_6', 's_28_20', 's_28_38', 's_28_19', 's_28_24', 's_28_29', 's_28_30', 's_28_28', 's_29_6', 's_29_31', 's_29_37', 's_29_22', 's_29_24', 's_29_35', 's_29_29', 's_31_1', 's_31_3', 's_31_10', 's_31_30', 's_31_31', 's_6_1', 's_6_10', 's_6_19', 's_6_24', 's_6_35', 's_6_6', 's_10_22', 's_10_24', 's_10_35', 's_10_10', 's_20_1', 's_20_3', 's_20_37', 's_20_20', 's_24_9', 's_24_38', 's_24_11', 's_24_22', 's_24_24', 's_35_37', 's_35_38', 's_35_15', 's_35_27', 's_35_35', 's_1_3', 's_1_9', 's_1_37', 's_1_38', 's_1_39', 's_1_1', 's_3_3', 's_15_37', 's_15_38', 's_15_15', 's_27_9', 's_27_38', 's_27_19', 's_27_30', 's_27_27', 's_38_39', 's_38_38', 's_9_9', 's_37_11', 's_37_19', 's_37_30', 's_37_37', 's_11_39', 's_11_11', 's_19_39', 's_19_22', 's_19_19', 's_30_39', 's_30_22', 's_30_30', 's_39_22', 's_39_39', 's_22_22']</t>
-        </is>
-      </c>
-      <c r="AS6" t="inlineStr">
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>[0, 2, 's_0_2', 4, 's_0_4', 5, 's_0_5', 7, 's_0_7', 8, 's_0_8', 12, 's_0_12', 13, 's_0_13', 16, 's_0_16', 18, 's_0_18', 23, 's_0_23', 32, 's_0_32', 33, 's_0_33', 36, 's_0_36', 's_2_12', 14, 's_2_14', 's_2_18', 34, 's_2_34', 's_4_12', 17, 's_4_17', 's_4_18', 21, 's_4_21', 25, 's_4_25', 26, 's_4_26', 28, 's_4_28', 29, 's_4_29', 31, 's_4_31', 's_4_34', 6, 's_5_6', 10, 's_5_10', 20, 's_5_20', 's_5_21', 's_5_23', 24, 's_5_24', 's_5_26', 's_5_33', 35, 's_5_35', 1, 's_1_7', 3, 's_3_7', 's_7_8', 's_7_10', 's_7_13', 15, 's_7_15', 's_7_20', 's_7_26', 27, 's_7_27', 's_7_31', 's_7_32', 38, 's_7_38', 's_8_12', 's_8_25', 's_8_28', 's_8_32', 's_8_35', 9, 's_9_12', 's_12_17', 's_12_21', 's_12_24', 's_12_28', 's_12_34', 's_12_35', 37, 's_12_37', 's_12_38', 's_9_13', 11, 's_11_13', 's_13_14', 's_13_16', 's_13_18', 19, 's_13_19', 's_13_21', 's_13_27', 's_13_29', 30, 's_13_30', 's_13_35', 39, 's_13_39', 's_1_16', 's_6_16', 's_10_16', 's_11_16', 's_16_18', 's_16_20', 22, 's_16_22', 's_16_32', 's_16_36', 's_6_18', 's_18_21', 's_18_24', 's_18_27', 's_18_30', 's_18_35', 's_18_36', 's_18_39', 's_1_23', 's_14_23', 's_19_23', 's_23_33', 's_23_37', 's_23_39', 's_3_32', 's_6_32', 's_14_32', 's_32_33', 's_32_37', 's_32_38', 's_6_33', 's_9_33', 's_22_33', 's_26_33', 's_33_36', 's_10_36', 's_14_36', 's_21_36', 's_29_36', 's_35_36', 's_36_38', 's_36_39', 's_1_3', 's_1_6', 's_1_9', 's_1_20', 's_1_21', 's_1_31', 's_1_37', 's_1_38', 's_1_39', 's_3_14', 's_3_20', 's_3_31', 's_6_10', 's_6_19', 's_6_21', 's_6_24', 's_6_28', 's_6_29', 's_6_35', 's_9_24', 's_9_27', 's_14_20', 's_17_20', 's_20_28', 's_20_37', 's_11_21', 's_21_27', 's_21_28', 's_21_31', 's_21_35', 's_21_38', 's_10_31', 's_29_31', 's_30_31', 's_11_37', 's_14_37', 's_15_37', 's_19_37', 's_29_37', 's_30_37', 's_35_37', 's_15_38', 's_17_38', 's_24_38', 's_25_38', 's_26_38', 's_27_38', 's_28_38', 's_35_38', 's_38_39', 's_11_39', 's_14_39', 's_19_39', 's_22_39', 's_30_39', 's_11_14', 's_14_15', 's_14_27', 's_14_35', 's_10_34', 's_22_34', 's_24_34', 's_28_34', 's_17_22', 's_17_24', 's_17_25', 's_17_29', 's_17_30', 's_11_25', 's_19_25', 's_22_25', 's_25_28', 's_25_29', 's_24_26', 's_26_27', 's_26_28', 's_26_35', 's_19_28', 's_24_28', 's_28_29', 's_28_30', 's_22_29', 's_24_29', 's_29_35', 's_10_22', 's_10_24', 's_10_35', 's_11_24', 's_22_24', 's_15_35', 's_27_35', 's_19_22', 's_19_27', 's_27_30', 's_22_30']</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
         <is>
           <t>[0, 2, 4, 5, 7, 8, 12, 13, 16, 18, 23, 32, 33, 36, 14, 34, 17, 21, 25, 26, 28, 29, 31, 6, 10, 20, 24, 35, 1, 3, 15, 27, 38, 9, 37, 11, 19, 30, 39, 22]</t>
         </is>
@@ -1466,12 +1314,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>[0, 7, 17, 21, 23, 25, 27, 30, 34, 41, 47, 9, 13, 14, 15, 29, 36, 5, 12, 18, 19, 20, 28, 35, 39, 40, 49, 8, 4, 11, 37, 42, 43, 1, 2, 3, 10, 26, 46, 48, 16, 24, 32, 38, 45, 31, 33, 22, 6, 44]</t>
+          <t>[0, 7, 17, 21, 23, 25, 27, 30, 34, 41, 47, 1, 2, 4, 10, 13, 18, 26, 28, 29, 42, 48, 3, 5, 6, 8, 11, 22, 39, 40, 44, 45, 9, 15, 19, 24, 49, 20, 31, 33, 12, 14, 16, 32, 36, 38, 46, 35, 37, 43]</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>[(0, 7), (0, 17), (0, 21), (0, 23), (0, 25), (0, 27), (0, 30), (0, 34), (0, 41), (0, 47), (0, 0), (7, 9), (7, 13), (7, 14), (7, 15), (7, 25), (7, 29), (7, 36), (7, 7), (17, 5), (17, 9), (17, 12), (17, 14), (17, 15), (17, 18), (17, 19), (17, 20), (17, 28), (17, 29), (17, 35), (17, 39), (17, 40), (17, 41), (17, 49), (17, 17), (21, 8), (21, 18), (21, 23), (21, 34), (21, 21), (23, 4), (23, 5), (23, 9), (23, 11), (23, 13), (23, 20), (23, 30), (23, 34), (23, 36), (23, 37), (23, 39), (23, 42), (23, 43), (23, 23), (25, 1), (25, 2), (25, 3), (25, 10), (25, 12), (25, 20), (25, 26), (25, 37), (25, 40), (25, 42), (25, 46), (25, 48), (25, 25), (27, 1), (27, 4), (27, 8), (27, 10), (27, 14), (27, 15), (27, 16), (27, 18), (27, 24), (27, 29), (27, 32), (27, 37), (27, 38), (27, 39), (27, 43), (27, 45), (27, 27), (30, 4), (30, 8), (30, 19), (30, 40), (30, 42), (30, 30), (34, 1), (34, 2), (34, 3), (34, 9), (34, 15), (34, 18), (34, 28), (34, 29), (34, 31), (34, 33), (34, 34), (41, 1), (41, 3), (41, 4), (41, 14), (41, 18), (41, 29), (41, 32), (41, 46), (41, 41), (47, 10), (47, 12), (47, 22), (47, 29), (47, 32), (47, 37), (47, 43), (47, 46), (47, 47), (9, 4), (9, 10), (9, 18), (9, 26), (9, 42), (9, 48), (9, 3), (9, 40), (9, 15), (9, 16), (9, 24), (9, 32), (9, 35), (9, 36), (9, 37), (9, 9), (13, 1), (13, 10), (13, 11), (13, 15), (13, 24), (13, 28), (13, 31), (13, 37), (13, 38), (13, 39), (13, 46), (13, 13), (14, 10), (14, 28), (14, 48), (14, 5), (14, 8), (14, 11), (14, 22), (14, 45), (14, 19), (14, 31), (14, 37), (14, 14), (15, 26), (15, 29), (15, 42), (15, 3), (15, 12), (15, 20), (15, 31), (15, 36), (15, 37), (15, 38), (15, 46), (15, 15), (29, 1), (29, 4), (29, 10), (29, 18), (29, 6), (29, 11), (29, 12), (29, 16), (29, 19), (29, 38), (29, 29), (36, 28), (36, 6), (36, 39), (36, 40), (36, 12), (36, 16), (36, 35), (36, 36), (5, 2), (5, 4), (5, 10), (5, 48), (5, 12), (5, 39), (5, 40), (5, 45), (5, 5), (12, 18), (12, 39), (12, 49), (12, 33), (12, 16), (12, 38), (12, 43), (12, 46), (12, 12), (18, 1), (18, 6), (18, 11), (18, 19), (18, 20), (18, 28), (18, 38), (18, 40), (18, 45), (18, 46), (18, 48), (18, 18), (19, 28), (19, 3), (19, 6), (19, 8), (19, 40), (19, 44), (19, 32), (19, 33), (19, 37), (19, 49), (19, 19), (20, 4), (20, 26), (20, 39), (20, 44), (20, 45), (20, 35), (20, 38), (20, 20), (28, 1), (28, 26), (28, 8), (28, 40), (28, 42), (28, 43), (28, 45), (28, 28), (35, 26), (35, 8), (35, 22), (35, 40), (35, 24), (35, 32), (35, 38), (35, 37), (35, 35), (39, 2), (39, 8), (39, 31), (39, 33), (39, 49), (39, 39), (40, 2), (40, 42), (40, 11), (40, 24), (40, 31), (40, 33), (40, 37), (40, 44), (40, 40), (49, 10), (49, 3), (49, 6), (49, 16), (49, 49), (8, 2), (8, 48), (8, 3), (8, 8), (4, 1), (4, 2), (4, 6), (4, 24), (4, 31), (4, 33), (4, 42), (4, 48), (4, 4), (11, 2), (11, 26), (11, 48), (11, 22), (11, 32), (11, 33), (11, 37), (11, 11), (37, 26), (37, 42), (37, 48), (37, 45), (37, 31), (37, 37), (42, 1), (42, 6), (42, 16), (42, 31), (42, 42), (43, 22), (43, 16), (43, 38), (43, 43), (1, 2), (1, 10), (1, 26), (1, 48), (1, 1), (2, 3), (2, 6), (2, 22), (2, 26), (2, 44), (2, 45), (2, 2), (3, 48), (3, 24), (3, 3), (10, 26), (10, 32), (10, 48), (10, 10), (26, 33), (26, 44), (26, 26), (46, 6), (46, 44), (46, 31), (46, 38), (46, 46), (48, 33), (48, 48), (16, 6), (16, 22), (16, 33), (16, 32), (16, 16), (24, 45), (24, 24), (32, 6), (32, 22), (32, 44), (32, 38), (32, 32), (38, 6), (38, 22), (38, 44), (38, 38), (45, 22), (45, 45), (31, 6), (31, 44), (31, 33), (31, 31), (33, 22), (33, 33), (22, 22), (6, 6), (44, 44)]</t>
+          <t>[(0, 7), (0, 17), (0, 21), (0, 23), (0, 25), (0, 27), (0, 30), (0, 34), (0, 41), (0, 47), (7, 9), (7, 13), (7, 14), (7, 15), (7, 25), (7, 29), (7, 36), (17, 5), (17, 9), (17, 12), (17, 14), (17, 15), (17, 18), (17, 19), (17, 20), (17, 28), (17, 29), (17, 35), (17, 39), (17, 40), (17, 41), (17, 49), (21, 8), (21, 18), (21, 23), (21, 34), (23, 4), (23, 5), (23, 9), (23, 11), (23, 13), (23, 20), (23, 30), (23, 34), (23, 36), (23, 37), (23, 39), (23, 42), (23, 43), (25, 1), (25, 2), (25, 3), (25, 10), (25, 12), (25, 20), (25, 26), (25, 37), (25, 40), (25, 42), (25, 46), (25, 48), (27, 1), (27, 4), (27, 8), (27, 10), (27, 14), (27, 15), (27, 16), (27, 18), (27, 24), (27, 29), (27, 32), (27, 37), (27, 38), (27, 39), (27, 43), (27, 45), (30, 4), (30, 8), (30, 19), (30, 40), (30, 42), (34, 1), (34, 2), (34, 3), (34, 9), (34, 15), (34, 18), (34, 28), (34, 29), (34, 31), (34, 33), (41, 1), (41, 3), (41, 4), (41, 14), (41, 18), (41, 29), (41, 32), (41, 46), (47, 10), (47, 12), (47, 22), (47, 29), (47, 32), (47, 37), (47, 43), (47, 46), (1, 2), (1, 4), (1, 10), (1, 13), (1, 18), (1, 26), (1, 28), (1, 29), (1, 42), (1, 48), (2, 3), (2, 4), (2, 5), (2, 6), (2, 8), (2, 11), (2, 22), (2, 26), (2, 39), (2, 40), (2, 44), (2, 45), (4, 5), (4, 6), (4, 9), (4, 20), (4, 24), (4, 29), (4, 31), (4, 33), (4, 42), (4, 48), (10, 5), (10, 9), (10, 13), (10, 14), (10, 26), (10, 29), (10, 32), (10, 48), (10, 49), (13, 11), (13, 15), (13, 24), (13, 28), (13, 31), (13, 37), (13, 38), (13, 39), (13, 46), (18, 6), (18, 9), (18, 11), (18, 12), (18, 19), (18, 20), (18, 28), (18, 29), (18, 38), (18, 40), (18, 45), (18, 46), (18, 48), (26, 9), (26, 11), (26, 15), (26, 20), (26, 28), (26, 33), (26, 35), (26, 37), (26, 44), (28, 8), (28, 14), (28, 19), (28, 36), (28, 40), (28, 42), (28, 43), (28, 45), (29, 6), (29, 11), (29, 12), (29, 15), (29, 16), (29, 19), (29, 38), (42, 6), (42, 9), (42, 15), (42, 16), (42, 31), (42, 37), (42, 40), (48, 3), (48, 5), (48, 8), (48, 9), (48, 11), (48, 14), (48, 33), (48, 37), (3, 8), (3, 9), (3, 15), (3, 19), (3, 24), (3, 49), (5, 12), (5, 14), (5, 39), (5, 40), (5, 45), (6, 16), (6, 19), (6, 31), (6, 32), (6, 36), (6, 38), (6, 46), (6, 49), (8, 14), (8, 19), (8, 35), (8, 39), (11, 14), (11, 22), (11, 32), (11, 33), (11, 37), (11, 40), (22, 14), (22, 16), (22, 32), (22, 33), (22, 35), (22, 38), (22, 43), (22, 45), (39, 12), (39, 20), (39, 31), (39, 33), (39, 36), (39, 49), (40, 9), (40, 19), (40, 24), (40, 31), (40, 33), (40, 35), (40, 36), (40, 37), (40, 44), (44, 19), (44, 20), (44, 31), (44, 32), (44, 38), (44, 46), (45, 14), (45, 20), (45, 24), (45, 37), (9, 15), (9, 16), (9, 24), (9, 32), (9, 35), (9, 36), (9, 37), (15, 12), (15, 20), (15, 31), (15, 36), (15, 37), (15, 38), (15, 46), (19, 14), (19, 32), (19, 33), (19, 37), (19, 49), (24, 35), (49, 12), (49, 16), (20, 35), (20, 38), (31, 14), (31, 33), (31, 37), (31, 46), (33, 12), (33, 16), (12, 16), (12, 36), (12, 38), (12, 43), (12, 46), (14, 37), (16, 32), (16, 36), (16, 43), (32, 35), (32, 38), (36, 35), (38, 35), (38, 43), (38, 46), (35, 37)]</t>
         </is>
       </c>
       <c r="G7" t="n">
@@ -1486,14 +1334,14 @@
         <v>0.002534468157697533</v>
       </c>
       <c r="J7" t="n">
-        <v>0.01631613369591408</v>
+        <v>0.01957706432887099</v>
       </c>
       <c r="K7" t="n">
         <v>0.3004081632653061</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>[(0, 7), (0, 's_0_7'), (0, 17), (0, 's_0_17'), (0, 21), (0, 's_0_21'), (0, 23), (0, 's_0_23'), (0, 25), (0, 's_0_25'), (0, 27), (0, 's_0_27'), (0, 30), (0, 's_0_30'), (0, 34), (0, 's_0_34'), (0, 41), (0, 's_0_41'), (0, 47), (0, 's_0_47'), (0, 's_0_0'), (0, 0), (7, 's_0_7'), (7, 9), (7, 's_7_9'), (7, 13), (7, 's_7_13'), (7, 14), (7, 's_7_14'), (7, 15), (7, 's_7_15'), (7, 25), (7, 's_7_25'), (7, 29), (7, 's_7_29'), (7, 36), (7, 's_7_36'), (7, 's_7_7'), (7, 7), ('s_0_7', 's_0_7'), (17, 's_0_17'), (17, 5), (17, 's_17_5'), (17, 9), (17, 's_17_9'), (17, 12), (17, 's_17_12'), (17, 14), (17, 's_17_14'), (17, 15), (17, 's_17_15'), (17, 18), (17, 's_17_18'), (17, 19), (17, 's_17_19'), (17, 20), (17, 's_17_20'), (17, 28), (17, 's_17_28'), (17, 29), (17, 's_17_29'), (17, 35), (17, 's_17_35'), (17, 39), (17, 's_17_39'), (17, 40), (17, 's_17_40'), (17, 41), (17, 's_17_41'), (17, 49), (17, 's_17_49'), (17, 's_17_17'), (17, 17), ('s_0_17', 's_0_17'), (21, 's_0_21'), (21, 8), (21, 's_21_8'), (21, 18), (21, 's_21_18'), (21, 23), (21, 's_21_23'), (21, 34), (21, 's_21_34'), (21, 's_21_21'), (21, 21), ('s_0_21', 's_0_21'), (23, 's_0_23'), (23, 's_21_23'), (23, 4), (23, 's_23_4'), (23, 5), (23, 's_23_5'), (23, 9), (23, 's_23_9'), (23, 11), (23, 's_23_11'), (23, 13), (23, 's_23_13'), (23, 20), (23, 's_23_20'), (23, 30), (23, 's_23_30'), (23, 34), (23, 's_23_34'), (23, 36), (23, 's_23_36'), (23, 37), (23, 's_23_37'), (23, 39), (23, 's_23_39'), (23, 42), (23, 's_23_42'), (23, 43), (23, 's_23_43'), (23, 's_23_23'), (23, 23), ('s_0_23', 's_0_23'), (25, 's_0_25'), (25, 's_7_25'), (25, 1), (25, 's_25_1'), (25, 2), (25, 's_25_2'), (25, 3), (25, 's_25_3'), (25, 10), (25, 's_25_10'), (25, 12), (25, 's_25_12'), (25, 20), (25, 's_25_20'), (25, 26), (25, 's_25_26'), (25, 37), (25, 's_25_37'), (25, 40), (25, 's_25_40'), (25, 42), (25, 's_25_42'), (25, 46), (25, 's_25_46'), (25, 48), (25, 's_25_48'), (25, 's_25_25'), (25, 25), ('s_0_25', 's_0_25'), (27, 's_0_27'), (27, 1), (27, 's_27_1'), (27, 4), (27, 's_27_4'), (27, 8), (27, 's_27_8'), (27, 10), (27, 's_27_10'), (27, 14), (27, 's_27_14'), (27, 15), (27, 's_27_15'), (27, 16), (27, 's_27_16'), (27, 18), (27, 's_27_18'), (27, 24), (27, 's_27_24'), (27, 29), (27, 's_27_29'), (27, 32), (27, 's_27_32'), (27, 37), (27, 's_27_37'), (27, 38), (27, 's_27_38'), (27, 39), (27, 's_27_39'), (27, 43), (27, 's_27_43'), (27, 45), (27, 's_27_45'), (27, 's_27_27'), (27, 27), ('s_0_27', 's_0_27'), (30, 's_0_30'), (30, 's_23_30'), (30, 4), (30, 's_30_4'), (30, 8), (30, 's_30_8'), (30, 19), (30, 's_30_19'), (30, 40), (30, 's_30_40'), (30, 42), (30, 's_30_42'), (30, 's_30_30'), (30, 30), ('s_0_30', 's_0_30'), (34, 's_0_34'), (34, 's_21_34'), (34, 's_23_34'), (34, 1), (34, 's_34_1'), (34, 2), (34, 's_34_2'), (34, 3), (34, 's_34_3'), (34, 9), (34, 's_34_9'), (34, 15), (34, 's_34_15'), (34, 18), (34, 's_34_18'), (34, 28), (34, 's_34_28'), (34, 29), (34, 's_34_29'), (34, 31), (34, 's_34_31'), (34, 33), (34, 's_34_33'), (34, 's_34_34'), (34, 34), ('s_0_34', 's_0_34'), (41, 's_0_41'), (41, 's_17_41'), (41, 1), (41, 's_41_1'), (41, 3), (41, 's_41_3'), (41, 4), (41, 's_41_4'), (41, 14), (41, 's_41_14'), (41, 18), (41, 's_41_18'), (41, 29), (41, 's_41_29'), (41, 32), (41, 's_41_32'), (41, 46), (41, 's_41_46'), (41, 's_41_41'), (41, 41), ('s_0_41', 's_0_41'), (47, 's_0_47'), (47, 10), (47, 's_47_10'), (47, 12), (47, 's_47_12'), (47, 22), (47, 's_47_22'), (47, 29), (47, 's_47_29'), (47, 32), (47, 's_47_32'), (47, 37), (47, 's_47_37'), (47, 43), (47, 's_47_43'), (47, 46), (47, 's_47_46'), (47, 's_47_47'), (47, 47), ('s_0_47', 's_0_47'), ('s_0_0', 's_0_0'), (9, 's_7_9'), (9, 's_17_9'), (9, 's_23_9'), (9, 's_34_9'), (9, 4), (9, 's_9_4'), (9, 10), (9, 's_9_10'), (9, 18), (9, 's_9_18'), (9, 26), (9, 's_9_26'), (9, 42), (9, 's_9_42'), (9, 48), (9, 's_9_48'), (9, 3), (9, 's_9_3'), (9, 40), (9, 's_9_40'), (9, 15), (9, 's_9_15'), (9, 16), (9, 's_9_16'), (9, 24), (9, 's_9_24'), (9, 32), (9, 's_9_32'), (9, 35), (9, 's_9_35'), (9, 36), (9, 's_9_36'), (9, 37), (9, 's_9_37'), (9, 's_9_9'), (9, 9), ('s_7_9', 's_7_9'), (13, 's_7_13'), (13, 's_23_13'), (13, 1), (13, 's_13_1'), (13, 10), (13, 's_13_10'), (13, 11), (13, 's_13_11'), (13, 15), (13, 's_13_15'), (13, 24), (13, 's_13_24'), (13, 28), (13, 's_13_28'), (13, 31), (13, 's_13_31'), (13, 37), (13, 's_13_37'), (13, 38), (13, 's_13_38'), (13, 39), (13, 's_13_39'), (13, 46), (13, 's_13_46'), (13, 's_13_13'), (13, 13), ('s_7_13', 's_7_13'), (14, 's_7_14'), (14, 's_17_14'), (14, 's_27_14'), (14, 's_41_14'), (14, 10), (14, 's_14_10'), (14, 28), (14, 's_14_28'), (14, 48), (14, 's_14_48'), (14, 5), (14, 's_14_5'), (14, 8), (14, 's_14_8'), (14, 11), (14, 's_14_11'), (14, 22), (14, 's_14_22'), (14, 45), (14, 's_14_45'), (14, 19), (14, 's_14_19'), (14, 31), (14, 's_14_31'), (14, 37), (14, 's_14_37'), (14, 's_14_14'), (14, 14), ('s_7_14', 's_7_14'), (15, 's_7_15'), (15, 's_17_15'), (15, 's_27_15'), (15, 's_34_15'), (15, 's_9_15'), (15, 's_13_15'), (15, 26), (15, 's_15_26'), (15, 29), (15, 's_15_29'), (15, 42), (15, 's_15_42'), (15, 3), (15, 's_15_3'), (15, 12), (15, 's_15_12'), (15, 20), (15, 's_15_20'), (15, 31), (15, 's_15_31'), (15, 36), (15, 's_15_36'), (15, 37), (15, 's_15_37'), (15, 38), (15, 's_15_38'), (15, 46), (15, 's_15_46'), (15, 's_15_15'), (15, 15), ('s_7_15', 's_7_15'), ('s_7_25', 's_7_25'), (29, 's_7_29'), (29, 's_17_29'), (29, 's_27_29'), (29, 's_34_29'), (29, 's_41_29'), (29, 's_47_29'), (29, 's_15_29'), (29, 1), (29, 's_29_1'), (29, 4), (29, 's_29_4'), (29, 10), (29, 's_29_10'), (29, 18), (29, 's_29_18'), (29, 6), (29, 's_29_6'), (29, 11), (29, 's_29_11'), (29, 12), (29, 's_29_12'), (29, 16), (29, 's_29_16'), (29, 19), (29, 's_29_19'), (29, 38), (29, 's_29_38'), (29, 's_29_29'), (29, 29), ('s_7_29', 's_7_29'), (36, 's_7_36'), (36, 's_23_36'), (36, 's_9_36'), (36, 's_15_36'), (36, 28), (36, 's_36_28'), (36, 6), (36, 's_36_6'), (36, 39), (36, 's_36_39'), (36, 40), (36, 's_36_40'), (36, 12), (36, 's_36_12'), (36, 16), (36, 's_36_16'), (36, 35), (36, 's_36_35'), (36, 's_36_36'), (36, 36), ('s_7_36', 's_7_36'), ('s_7_7', 's_7_7'), (5, 's_17_5'), (5, 's_23_5'), (5, 's_14_5'), (5, 2), (5, 's_5_2'), (5, 4), (5, 's_5_4'), (5, 10), (5, 's_5_10'), (5, 48), (5, 's_5_48'), (5, 12), (5, 's_5_12'), (5, 39), (5, 's_5_39'), (5, 40), (5, 's_5_40'), (5, 45), (5, 's_5_45'), (5, 's_5_5'), (5, 5), ('s_17_5', 's_17_5'), ('s_17_9', 's_17_9'), (12, 's_17_12'), (12, 's_25_12'), (12, 's_47_12'), (12, 's_15_12'), (12, 's_29_12'), (12, 's_36_12'), (12, 's_5_12'), (12, 18), (12, 's_12_18'), (12, 39), (12, 's_12_39'), (12, 49), (12, 's_12_49'), (12, 33), (12, 's_12_33'), (12, 16), (12, 's_12_16'), (12, 38), (12, 's_12_38'), (12, 43), (12, 's_12_43'), (12, 46), (12, 's_12_46'), (12, 's_12_12'), (12, 12), ('s_17_12', 's_17_12'), ('s_17_14', 's_17_14'), ('s_17_15', 's_17_15'), (18, 's_17_18'), (18, 's_21_18'), (18, 's_27_18'), (18, 's_34_18'), (18, 's_41_18'), (18, 's_9_18'), (18, 's_29_18'), (18, 's_12_18'), (18, 1), (18, 's_18_1'), (18, 6), (18, 's_18_6'), (18, 11), (18, 's_18_11'), (18, 19), (18, 's_18_19'), (18, 20), (18, 's_18_20'), (18, 28), (18, 's_18_28'), (18, 38), (18, 's_18_38'), (18, 40), (18, 's_18_40'), (18, 45), (18, 's_18_45'), (18, 46), (18, 's_18_46'), (18, 48), (18, 's_18_48'), (18, 's_18_18'), (18, 18), ('s_17_18', 's_17_18'), (19, 's_17_19'), (19, 's_30_19'), (19, 's_14_19'), (19, 's_29_19'), (19, 's_18_19'), (19, 28), (19, 's_19_28'), (19, 3), (19, 's_19_3'), (19, 6), (19, 's_19_6'), (19, 8), (19, 's_19_8'), (19, 40), (19, 's_19_40'), (19, 44), (19, 's_19_44'), (19, 32), (19, 's_19_32'), (19, 33), (19, 's_19_33'), (19, 37), (19, 's_19_37'), (19, 49), (19, 's_19_49'), (19, 's_19_19'), (19, 19), ('s_17_19', 's_17_19'), (20, 's_17_20'), (20, 's_23_20'), (20, 's_25_20'), (20, 's_15_20'), (20, 's_18_20'), (20, 4), (20, 's_20_4'), (20, 26), (20, 's_20_26'), (20, 39), (20, 's_20_39'), (20, 44), (20, 's_20_44'), (20, 45), (20, 's_20_45'), (20, 35), (20, 's_20_35'), (20, 38), (20, 's_20_38'), (20, 's_20_20'), (20, 20), ('s_17_20', 's_17_20'), (28, 's_17_28'), (28, 's_34_28'), (28, 's_13_28'), (28, 's_14_28'), (28, 's_36_28'), (28, 's_18_28'), (28, 's_19_28'), (28, 1), (28, 's_28_1'), (28, 26), (28, 's_28_26'), (28, 8), (28, 's_28_8'), (28, 40), (28, 's_28_40'), (28, 42), (28, 's_28_42'), (28, 43), (28, 's_28_43'), (28, 45), (28, 's_28_45'), (28, 's_28_28'), (28, 28), ('s_17_28', 's_17_28'), ('s_17_29', 's_17_29'), (35, 's_17_35'), (35, 's_9_35'), (35, 's_36_35'), (35, 's_20_35'), (35, 26), (35, 's_35_26'), (35, 8), (35, 's_35_8'), (35, 22), (35, 's_35_22'), (35, 40), (35, 's_35_40'), (35, 24), (35, 's_35_24'), (35, 32), (35, 's_35_32'), (35, 38), (35, 's_35_38'), (35, 37), (35, 's_35_37'), (35, 's_35_35'), (35, 35), ('s_17_35', 's_17_35'), (39, 's_17_39'), (39, 's_23_39'), (39, 's_27_39'), (39, 's_13_39'), (39, 's_36_39'), (39, 's_5_39'), (39, 's_12_39'), (39, 's_20_39'), (39, 2), (39, 's_39_2'), (39, 8), (39, 's_39_8'), (39, 31), (39, 's_39_31'), (39, 33), (39, 's_39_33'), (39, 49), (39, 's_39_49'), (39, 's_39_39'), (39, 39), ('s_17_39', 's_17_39'), (40, 's_17_40'), (40, 's_25_40'), (40, 's_30_40'), (40, 's_9_40'), (40, 's_36_40'), (40, 's_5_40'), (40, 's_18_40'), (40, 's_19_40'), (40, 's_28_40'), (40, 's_35_40'), (40, 2), (40, 's_40_2'), (40, 42), (40, 's_40_42'), (40, 11), (40, 's_40_11'), (40, 24), (40, 's_40_24'), (40, 31), (40, 's_40_31'), (40, 33), (40, 's_40_33'), (40, 37), (40, 's_40_37'), (40, 44), (40, 's_40_44'), (40, 's_40_40'), (40, 40), ('s_17_40', 's_17_40'), ('s_17_41', 's_17_41'), (49, 's_17_49'), (49, 's_12_49'), (49, 's_19_49'), (49, 's_39_49'), (49, 10), (49, 's_49_10'), (49, 3), (49, 's_49_3'), (49, 6), (49, 's_49_6'), (49, 16), (49, 's_49_16'), (49, 's_49_49'), (49, 49), ('s_17_49', 's_17_49'), ('s_17_17', 's_17_17'), (8, 's_21_8'), (8, 's_27_8'), (8, 's_30_8'), (8, 's_14_8'), (8, 's_19_8'), (8, 's_28_8'), (8, 's_35_8'), (8, 's_39_8'), (8, 2), (8, 's_8_2'), (8, 48), (8, 's_8_48'), (8, 3), (8, 's_8_3'), (8, 's_8_8'), (8, 8), ('s_21_8', 's_21_8'), ('s_21_18', 's_21_18'), ('s_21_23', 's_21_23'), ('s_21_34', 's_21_34'), ('s_21_21', 's_21_21'), (4, 's_23_4'), (4, 's_27_4'), (4, 's_30_4'), (4, 's_41_4'), (4, 's_9_4'), (4, 's_29_4'), (4, 's_5_4'), (4, 's_20_4'), (4, 1), (4, 's_4_1'), (4, 2), (4, 's_4_2'), (4, 6), (4, 's_4_6'), (4, 24), (4, 's_4_24'), (4, 31), (4, 's_4_31'), (4, 33), (4, 's_4_33'), (4, 42), (4, 's_4_42'), (4, 48), (4, 's_4_48'), (4, 's_4_4'), (4, 4), ('s_23_4', 's_23_4'), ('s_23_5', 's_23_5'), ('s_23_9', 's_23_9'), (11, 's_23_11'), (11, 's_13_11'), (11, 's_14_11'), (11, 's_29_11'), (11, 's_18_11'), (11, 's_40_11'), (11, 2), (11, 's_11_2'), (11, 26), (11, 's_11_26'), (11, 48), (11, 's_11_48'), (11, 22), (11, 's_11_22'), (11, 32), (11, 's_11_32'), (11, 33), (11, 's_11_33'), (11, 37), (11, 's_11_37'), (11, 's_11_11'), (11, 11), ('s_23_11', 's_23_11'), ('s_23_13', 's_23_13'), ('s_23_20', 's_23_20'), ('s_23_30', 's_23_30'), ('s_23_34', 's_23_34'), ('s_23_36', 's_23_36'), (37, 's_23_37'), (37, 's_25_37'), (37, 's_27_37'), (37, 's_47_37'), (37, 's_9_37'), (37, 's_13_37'), (37, 's_14_37'), (37, 's_15_37'), (37, 's_19_37'), (37, 's_35_37'), (37, 's_40_37'), (37, 's_11_37'), (37, 26), (37, 's_37_26'), (37, 42), (37, 's_37_42'), (37, 48), (37, 's_37_48'), (37, 45), (37, 's_37_45'), (37, 31), (37, 's_37_31'), (37, 's_37_37'), (37, 37), ('s_23_37', 's_23_37'), ('s_23_39', 's_23_39'), (42, 's_23_42'), (42, 's_25_42'), (42, 's_30_42'), (42, 's_9_42'), (42, 's_15_42'), (42, 's_28_42'), (42, 's_40_42'), (42, 's_4_42'), (42, 's_37_42'), (42, 1), (42, 's_42_1'), (42, 6), (42, 's_42_6'), (42, 16), (42, 's_42_16'), (42, 31), (42, 's_42_31'), (42, 's_42_42'), (42, 42), ('s_23_42', 's_23_42'), (43, 's_23_43'), (43, 's_27_43'), (43, 's_47_43'), (43, 's_12_43'), (43, 's_28_43'), (43, 22), (43, 's_43_22'), (43, 16), (43, 's_43_16'), (43, 38), (43, 's_43_38'), (43, 's_43_43'), (43, 43), ('s_23_43', 's_23_43'), ('s_23_23', 's_23_23'), (1, 's_25_1'), (1, 's_27_1'), (1, 's_34_1'), (1, 's_41_1'), (1, 's_13_1'), (1, 's_29_1'), (1, 's_18_1'), (1, 's_28_1'), (1, 's_4_1'), (1, 's_42_1'), (1, 2), (1, 's_1_2'), (1, 10), (1, 's_1_10'), (1, 26), (1, 's_1_26'), (1, 48), (1, 's_1_48'), (1, 's_1_1'), (1, 1), ('s_25_1', 's_25_1'), (2, 's_25_2'), (2, 's_34_2'), (2, 's_5_2'), (2, 's_39_2'), (2, 's_40_2'), (2, 's_8_2'), (2, 's_4_2'), (2, 's_11_2'), (2, 's_1_2'), (2, 3), (2, 's_2_3'), (2, 6), (2, 's_2_6'), (2, 22), (2, 's_2_22'), (2, 26), (2, 's_2_26'), (2, 44), (2, 's_2_44'), (2, 45), (2, 's_2_45'), (2, 's_2_2'), (2, 2), ('s_25_2', 's_25_2'), (3, 's_25_3'), (3, 's_34_3'), (3, 's_41_3'), (3, 's_9_3'), (3, 's_15_3'), (3, 's_19_3'), (3, 's_49_3'), (3, 's_8_3'), (3, 's_2_3'), (3, 48), (3, 's_3_48'), (3, 24), (3, 's_3_24'), (3, 's_3_3'), (3, 3), ('s_25_3', 's_25_3'), (10, 's_25_10'), (10, 's_27_10'), (10, 's_47_10'), (10, 's_9_10'), (10, 's_13_10'), (10, 's_14_10'), (10, 's_29_10'), (10, 's_5_10'), (10, 's_49_10'), (10, 's_1_10'), (10, 26), (10, 's_10_26'), (10, 32), (10, 's_10_32'), (10, 48), (10, 's_10_48'), (10, 's_10_10'), (10, 10), ('s_25_10', 's_25_10'), ('s_25_12', 's_25_12'), ('s_25_20', 's_25_20'), (26, 's_25_26'), (26, 's_9_26'), (26, 's_15_26'), (26, 's_20_26'), (26, 's_28_26'), (26, 's_35_26'), (26, 's_11_26'), (26, 's_37_26'), (26, 's_1_26'), (26, 's_2_26'), (26, 's_10_26'), (26, 33), (26, 's_26_33'), (26, 44), (26, 's_26_44'), (26, 's_26_26'), (26, 26), ('s_25_26', 's_25_26'), ('s_25_37', 's_25_37'), ('s_25_40', 's_25_40'), ('s_25_42', 's_25_42'), (46, 's_25_46'), (46, 's_41_46'), (46, 's_47_46'), (46, 's_13_46'), (46, 's_15_46'), (46, 's_12_46'), (46, 's_18_46'), (46, 6), (46, 's_46_6'), (46, 44), (46, 's_46_44'), (46, 31), (46, 's_46_31'), (46, 38), (46, 's_46_38'), (46, 's_46_46'), (46, 46), ('s_25_46', 's_25_46'), (48, 's_25_48'), (48, 's_9_48'), (48, 's_14_48'), (48, 's_5_48'), (48, 's_18_48'), (48, 's_8_48'), (48, 's_4_48'), (48, 's_11_48'), (48, 's_37_48'), (48, 's_1_48'), (48, 's_3_48'), (48, 's_10_48'), (48, 33), (48, 's_48_33'), (48, 's_48_48'), (48, 48), ('s_25_48', 's_25_48'), ('s_25_25', 's_25_25'), ('s_27_1', 's_27_1'), ('s_27_4', 's_27_4'), ('s_27_8', 's_27_8'), ('s_27_10', 's_27_10'), ('s_27_14', 's_27_14'), ('s_27_15', 's_27_15'), (16, 's_27_16'), (16, 's_9_16'), (16, 's_29_16'), (16, 's_36_16'), (16, 's_12_16'), (16, 's_49_16'), (16, 's_42_16'), (16, 's_43_16'), (16, 6), (16, 's_16_6'), (16, 22), (16, 's_16_22'), (16, 33), (16, 's_16_33'), (16, 32), (16, 's_16_32'), (16, 's_16_16'), (16, 16), ('s_27_16', 's_27_16'), ('s_27_18', 's_27_18'), (24, 's_27_24'), (24, 's_9_24'), (24, 's_13_24'), (24, 's_35_24'), (24, 's_40_24'), (24, 's_4_24'), (24, 's_3_24'), (24, 45), (24, 's_24_45'), (24, 's_24_24'), (24, 24), ('s_27_24', 's_27_24'), ('s_27_29', 's_27_29'), (32, 's_27_32'), (32, 's_41_32'), (32, 's_47_32'), (32, 's_9_32'), (32, 's_19_32'), (32, 's_35_32'), (32, 's_11_32'), (32, 's_10_32'), (32, 's_16_32'), (32, 6), (32, 's_32_6'), (32, 22), (32, 's_32_22'), (32, 44), (32, 's_32_44'), (32, 38), (32, 's_32_38'), (32, 's_32_32'), (32, 32), ('s_27_32', 's_27_32'), ('s_27_37', 's_27_37'), (38, 's_27_38'), (38, 's_13_38'), (38, 's_15_38'), (38, 's_29_38'), (38, 's_12_38'), (38, 's_18_38'), (38, 's_20_38'), (38, 's_35_38'), (38, 's_43_38'), (38, 's_46_38'), (38, 's_32_38'), (38, 6), (38, 's_38_6'), (38, 22), (38, 's_38_22'), (38, 44), (38, 's_38_44'), (38, 's_38_38'), (38, 38), ('s_27_38', 's_27_38'), ('s_27_39', 's_27_39'), ('s_27_43', 's_27_43'), (45, 's_27_45'), (45, 's_14_45'), (45, 's_5_45'), (45, 's_18_45'), (45, 's_20_45'), (45, 's_28_45'), (45, 's_37_45'), (45, 's_2_45'), (45, 's_24_45'), (45, 22), (45, 's_45_22'), (45, 's_45_45'), (45, 45), ('s_27_45', 's_27_45'), ('s_27_27', 's_27_27'), ('s_30_4', 's_30_4'), ('s_30_8', 's_30_8'), ('s_30_19', 's_30_19'), ('s_30_40', 's_30_40'), ('s_30_42', 's_30_42'), ('s_30_30', 's_30_30'), ('s_34_1', 's_34_1'), ('s_34_2', 's_34_2'), ('s_34_3', 's_34_3'), ('s_34_9', 's_34_9'), ('s_34_15', 's_34_15'), ('s_34_18', 's_34_18'), ('s_34_28', 's_34_28'), ('s_34_29', 's_34_29'), (31, 's_34_31'), (31, 's_13_31'), (31, 's_14_31'), (31, 's_15_31'), (31, 's_39_31'), (31, 's_40_31'), (31, 's_4_31'), (31, 's_37_31'), (31, 's_42_31'), (31, 's_46_31'), (31, 6), (31, 's_31_6'), (31, 44), (31, 's_31_44'), (31, 33), (31, 's_31_33'), (31, 's_31_31'), (31, 31), ('s_34_31', 's_34_31'), (33, 's_34_33'), (33, 's_12_33'), (33, 's_19_33'), (33, 's_39_33'), (33, 's_40_33'), (33, 's_4_33'), (33, 's_11_33'), (33, 's_26_33'), (33, 's_48_33'), (33, 's_16_33'), (33, 's_31_33'), (33, 22), (33, 's_33_22'), (33, 's_33_33'), (33, 33), ('s_34_33', 's_34_33'), ('s_34_34', 's_34_34'), ('s_41_1', 's_41_1'), ('s_41_3', 's_41_3'), ('s_41_4', 's_41_4'), ('s_41_14', 's_41_14'), ('s_41_18', 's_41_18'), ('s_41_29', 's_41_29'), ('s_41_32', 's_41_32'), ('s_41_46', 's_41_46'), ('s_41_41', 's_41_41'), ('s_47_10', 's_47_10'), ('s_47_12', 's_47_12'), (22, 's_47_22'), (22, 's_14_22'), (22, 's_35_22'), (22, 's_11_22'), (22, 's_43_22'), (22, 's_2_22'), (22, 's_16_22'), (22, 's_32_22'), (22, 's_38_22'), (22, 's_45_22'), (22, 's_33_22'), (22, 's_22_22'), (22, 22), ('s_47_22', 's_47_22'), ('s_47_29', 's_47_29'), ('s_47_32', 's_47_32'), ('s_47_37', 's_47_37'), ('s_47_43', 's_47_43'), ('s_47_46', 's_47_46'), ('s_47_47', 's_47_47'), ('s_9_4', 's_9_4'), ('s_9_10', 's_9_10'), ('s_9_18', 's_9_18'), ('s_9_26', 's_9_26'), ('s_9_42', 's_9_42'), ('s_9_48', 's_9_48'), ('s_9_3', 's_9_3'), ('s_9_40', 's_9_40'), ('s_9_15', 's_9_15'), ('s_9_16', 's_9_16'), ('s_9_24', 's_9_24'), ('s_9_32', 's_9_32'), ('s_9_35', 's_9_35'), ('s_9_36', 's_9_36'), ('s_9_37', 's_9_37'), ('s_9_9', 's_9_9'), ('s_13_1', 's_13_1'), ('s_13_10', 's_13_10'), ('s_13_11', 's_13_11'), ('s_13_15', 's_13_15'), ('s_13_24', 's_13_24'), ('s_13_28', 's_13_28'), ('s_13_31', 's_13_31'), ('s_13_37', 's_13_37'), ('s_13_38', 's_13_38'), ('s_13_39', 's_13_39'), ('s_13_46', 's_13_46'), ('s_13_13', 's_13_13'), ('s_14_10', 's_14_10'), ('s_14_28', 's_14_28'), ('s_14_48', 's_14_48'), ('s_14_5', 's_14_5'), ('s_14_8', 's_14_8'), ('s_14_11', 's_14_11'), ('s_14_22', 's_14_22'), ('s_14_45', 's_14_45'), ('s_14_19', 's_14_19'), ('s_14_31', 's_14_31'), ('s_14_37', 's_14_37'), ('s_14_14', 's_14_14'), ('s_15_26', 's_15_26'), ('s_15_29', 's_15_29'), ('s_15_42', 's_15_42'), ('s_15_3', 's_15_3'), ('s_15_12', 's_15_12'), ('s_15_20', 's_15_20'), ('s_15_31', 's_15_31'), ('s_15_36', 's_15_36'), ('s_15_37', 's_15_37'), ('s_15_38', 's_15_38'), ('s_15_46', 's_15_46'), ('s_15_15', 's_15_15'), ('s_29_1', 's_29_1'), ('s_29_4', 's_29_4'), ('s_29_10', 's_29_10'), ('s_29_18', 's_29_18'), (6, 's_29_6'), (6, 's_36_6'), (6, 's_18_6'), (6, 's_19_6'), (6, 's_49_6'), (6, 's_4_6'), (6, 's_42_6'), (6, 's_2_6'), (6, 's_46_6'), (6, 's_16_6'), (6, 's_32_6'), (6, 's_38_6'), (6, 's_31_6'), (6, 's_6_6'), (6, 6), ('s_29_6', 's_29_6'), ('s_29_11', 's_29_11'), ('s_29_12', 's_29_12'), ('s_29_16', 's_29_16'), ('s_29_19', 's_29_19'), ('s_29_38', 's_29_38'), ('s_29_29', 's_29_29'), ('s_36_28', 's_36_28'), ('s_36_6', 's_36_6'), ('s_36_39', 's_36_39'), ('s_36_40', 's_36_40'), ('s_36_12', 's_36_12'), ('s_36_16', 's_36_16'), ('s_36_35', 's_36_35'), ('s_36_36', 's_36_36'), ('s_5_2', 's_5_2'), ('s_5_4', 's_5_4'), ('s_5_10', 's_5_10'), ('s_5_48', 's_5_48'), ('s_5_12', 's_5_12'), ('s_5_39', 's_5_39'), ('s_5_40', 's_5_40'), ('s_5_45', 's_5_45'), ('s_5_5', 's_5_5'), ('s_12_18', 's_12_18'), ('s_12_39', 's_12_39'), ('s_12_49', 's_12_49'), ('s_12_33', 's_12_33'), ('s_12_16', 's_12_16'), ('s_12_38', 's_12_38'), ('s_12_43', 's_12_43'), ('s_12_46', 's_12_46'), ('s_12_12', 's_12_12'), ('s_18_1', 's_18_1'), ('s_18_6', 's_18_6'), ('s_18_11', 's_18_11'), ('s_18_19', 's_18_19'), ('s_18_20', 's_18_20'), ('s_18_28', 's_18_28'), ('s_18_38', 's_18_38'), ('s_18_40', 's_18_40'), ('s_18_45', 's_18_45'), ('s_18_46', 's_18_46'), ('s_18_48', 's_18_48'), ('s_18_18', 's_18_18'), ('s_19_28', 's_19_28'), ('s_19_3', 's_19_3'), ('s_19_6', 's_19_6'), ('s_19_8', 's_19_8'), ('s_19_40', 's_19_40'), (44, 's_19_44'), (44, 's_20_44'), (44, 's_40_44'), (44, 's_2_44'), (44, 's_26_44'), (44, 's_46_44'), (44, 's_32_44'), (44, 's_38_44'), (44, 's_31_44'), (44, 's_44_44'), (44, 44), ('s_19_44', 's_19_44'), ('s_19_32', 's_19_32'), ('s_19_33', 's_19_33'), ('s_19_37', 's_19_37'), ('s_19_49', 's_19_49'), ('s_19_19', 's_19_19'), ('s_20_4', 's_20_4'), ('s_20_26', 's_20_26'), ('s_20_39', 's_20_39'), ('s_20_44', 's_20_44'), ('s_20_45', 's_20_45'), ('s_20_35', 's_20_35'), ('s_20_38', 's_20_38'), ('s_20_20', 's_20_20'), ('s_28_1', 's_28_1'), ('s_28_26', 's_28_26'), ('s_28_8', 's_28_8'), ('s_28_40', 's_28_40'), ('s_28_42', 's_28_42'), ('s_28_43', 's_28_43'), ('s_28_45', 's_28_45'), ('s_28_28', 's_28_28'), ('s_35_26', 's_35_26'), ('s_35_8', 's_35_8'), ('s_35_22', 's_35_22'), ('s_35_40', 's_35_40'), ('s_35_24', 's_35_24'), ('s_35_32', 's_35_32'), ('s_35_38', 's_35_38'), ('s_35_37', 's_35_37'), ('s_35_35', 's_35_35'), ('s_39_2', 's_39_2'), ('s_39_8', 's_39_8'), ('s_39_31', 's_39_31'), ('s_39_33', 's_39_33'), ('s_39_49', 's_39_49'), ('s_39_39', 's_39_39'), ('s_40_2', 's_40_2'), ('s_40_42', 's_40_42'), ('s_40_11', 's_40_11'), ('s_40_24', 's_40_24'), ('s_40_31', 's_40_31'), ('s_40_33', 's_40_33'), ('s_40_37', 's_40_37'), ('s_40_44', 's_40_44'), ('s_40_40', 's_40_40'), ('s_49_10', 's_49_10'), ('s_49_3', 's_49_3'), ('s_49_6', 's_49_6'), ('s_49_16', 's_49_16'), ('s_49_49', 's_49_49'), ('s_8_2', 's_8_2'), ('s_8_48', 's_8_48'), ('s_8_3', 's_8_3'), ('s_8_8', 's_8_8'), ('s_4_1', 's_4_1'), ('s_4_2', 's_4_2'), ('s_4_6', 's_4_6'), ('s_4_24', 's_4_24'), ('s_4_31', 's_4_31'), ('s_4_33', 's_4_33'), ('s_4_42', 's_4_42'), ('s_4_48', 's_4_48'), ('s_4_4', 's_4_4'), ('s_11_2', 's_11_2'), ('s_11_26', 's_11_26'), ('s_11_48', 's_11_48'), ('s_11_22', 's_11_22'), ('s_11_32', 's_11_32'), ('s_11_33', 's_11_33'), ('s_11_37', 's_11_37'), ('s_11_11', 's_11_11'), ('s_37_26', 's_37_26'), ('s_37_42', 's_37_42'), ('s_37_48', 's_37_48'), ('s_37_45', 's_37_45'), ('s_37_31', 's_37_31'), ('s_37_37', 's_37_37'), ('s_42_1', 's_42_1'), ('s_42_6', 's_42_6'), ('s_42_16', 's_42_16'), ('s_42_31', 's_42_31'), ('s_42_42', 's_42_42'), ('s_43_22', 's_43_22'), ('s_43_16', 's_43_16'), ('s_43_38', 's_43_38'), ('s_43_43', 's_43_43'), ('s_1_2', 's_1_2'), ('s_1_10', 's_1_10'), ('s_1_26', 's_1_26'), ('s_1_48', 's_1_48'), ('s_1_1', 's_1_1'), ('s_2_3', 's_2_3'), ('s_2_6', 's_2_6'), ('s_2_22', 's_2_22'), ('s_2_26', 's_2_26'), ('s_2_44', 's_2_44'), ('s_2_45', 's_2_45'), ('s_2_2', 's_2_2'), ('s_3_48', 's_3_48'), ('s_3_24', 's_3_24'), ('s_3_3', 's_3_3'), ('s_10_26', 's_10_26'), ('s_10_32', 's_10_32'), ('s_10_48', 's_10_48'), ('s_10_10', 's_10_10'), ('s_26_33', 's_26_33'), ('s_26_44', 's_26_44'), ('s_26_26', 's_26_26'), ('s_46_6', 's_46_6'), ('s_46_44', 's_46_44'), ('s_46_31', 's_46_31'), ('s_46_38', 's_46_38'), ('s_46_46', 's_46_46'), ('s_48_33', 's_48_33'), ('s_48_48', 's_48_48'), ('s_16_6', 's_16_6'), ('s_16_22', 's_16_22'), ('s_16_33', 's_16_33'), ('s_16_32', 's_16_32'), ('s_16_16', 's_16_16'), ('s_24_45', 's_24_45'), ('s_24_24', 's_24_24'), ('s_32_6', 's_32_6'), ('s_32_22', 's_32_22'), ('s_32_44', 's_32_44'), ('s_32_38', 's_32_38'), ('s_32_32', 's_32_32'), ('s_38_6', 's_38_6'), ('s_38_22', 's_38_22'), ('s_38_44', 's_38_44'), ('s_38_38', 's_38_38'), ('s_45_22', 's_45_22'), ('s_45_45', 's_45_45'), ('s_31_6', 's_31_6'), ('s_31_44', 's_31_44'), ('s_31_33', 's_31_33'), ('s_31_31', 's_31_31'), ('s_33_22', 's_33_22'), ('s_33_33', 's_33_33'), ('s_22_22', 's_22_22'), ('s_6_6', 's_6_6'), ('s_44_44', 's_44_44')]</t>
+          <t>[(0, 7), (0, 's_0_7'), (0, 17), (0, 's_0_17'), (0, 21), (0, 's_0_21'), (0, 23), (0, 's_0_23'), (0, 25), (0, 's_0_25'), (0, 27), (0, 's_0_27'), (0, 30), (0, 's_0_30'), (0, 34), (0, 's_0_34'), (0, 41), (0, 's_0_41'), (0, 47), (0, 's_0_47'), (0, 0), (7, 's_0_7'), (7, 9), (7, 's_7_9'), (7, 13), (7, 's_7_13'), (7, 14), (7, 's_7_14'), (7, 15), (7, 's_7_15'), (7, 25), (7, 's_7_25'), (7, 29), (7, 's_7_29'), (7, 36), (7, 's_7_36'), (7, 7), ('s_0_7', 's_0_7'), (17, 's_0_17'), (17, 5), (17, 's_5_17'), (17, 9), (17, 's_9_17'), (17, 12), (17, 's_12_17'), (17, 14), (17, 's_14_17'), (17, 15), (17, 's_15_17'), (17, 18), (17, 's_17_18'), (17, 19), (17, 's_17_19'), (17, 20), (17, 's_17_20'), (17, 28), (17, 's_17_28'), (17, 29), (17, 's_17_29'), (17, 35), (17, 's_17_35'), (17, 39), (17, 's_17_39'), (17, 40), (17, 's_17_40'), (17, 41), (17, 's_17_41'), (17, 49), (17, 's_17_49'), (17, 17), ('s_0_17', 's_0_17'), (21, 's_0_21'), (21, 8), (21, 's_8_21'), (21, 18), (21, 's_18_21'), (21, 23), (21, 's_21_23'), (21, 34), (21, 's_21_34'), (21, 21), ('s_0_21', 's_0_21'), (23, 's_0_23'), (23, 's_21_23'), (23, 4), (23, 's_4_23'), (23, 5), (23, 's_5_23'), (23, 9), (23, 's_9_23'), (23, 11), (23, 's_11_23'), (23, 13), (23, 's_13_23'), (23, 20), (23, 's_20_23'), (23, 30), (23, 's_23_30'), (23, 34), (23, 's_23_34'), (23, 36), (23, 's_23_36'), (23, 37), (23, 's_23_37'), (23, 39), (23, 's_23_39'), (23, 42), (23, 's_23_42'), (23, 43), (23, 's_23_43'), (23, 23), ('s_0_23', 's_0_23'), (25, 's_0_25'), (25, 's_7_25'), (25, 1), (25, 's_1_25'), (25, 2), (25, 's_2_25'), (25, 3), (25, 's_3_25'), (25, 10), (25, 's_10_25'), (25, 12), (25, 's_12_25'), (25, 20), (25, 's_20_25'), (25, 26), (25, 's_25_26'), (25, 37), (25, 's_25_37'), (25, 40), (25, 's_25_40'), (25, 42), (25, 's_25_42'), (25, 46), (25, 's_25_46'), (25, 48), (25, 's_25_48'), (25, 25), ('s_0_25', 's_0_25'), (27, 's_0_27'), (27, 1), (27, 's_1_27'), (27, 4), (27, 's_4_27'), (27, 8), (27, 's_8_27'), (27, 10), (27, 's_10_27'), (27, 14), (27, 's_14_27'), (27, 15), (27, 's_15_27'), (27, 16), (27, 's_16_27'), (27, 18), (27, 's_18_27'), (27, 24), (27, 's_24_27'), (27, 29), (27, 's_27_29'), (27, 32), (27, 's_27_32'), (27, 37), (27, 's_27_37'), (27, 38), (27, 's_27_38'), (27, 39), (27, 's_27_39'), (27, 43), (27, 's_27_43'), (27, 45), (27, 's_27_45'), (27, 27), ('s_0_27', 's_0_27'), (30, 's_0_30'), (30, 's_23_30'), (30, 4), (30, 's_4_30'), (30, 8), (30, 's_8_30'), (30, 19), (30, 's_19_30'), (30, 40), (30, 's_30_40'), (30, 42), (30, 's_30_42'), (30, 30), ('s_0_30', 's_0_30'), (34, 's_0_34'), (34, 's_21_34'), (34, 's_23_34'), (34, 1), (34, 's_1_34'), (34, 2), (34, 's_2_34'), (34, 3), (34, 's_3_34'), (34, 9), (34, 's_9_34'), (34, 15), (34, 's_15_34'), (34, 18), (34, 's_18_34'), (34, 28), (34, 's_28_34'), (34, 29), (34, 's_29_34'), (34, 31), (34, 's_31_34'), (34, 33), (34, 's_33_34'), (34, 34), ('s_0_34', 's_0_34'), (41, 's_0_41'), (41, 's_17_41'), (41, 1), (41, 's_1_41'), (41, 3), (41, 's_3_41'), (41, 4), (41, 's_4_41'), (41, 14), (41, 's_14_41'), (41, 18), (41, 's_18_41'), (41, 29), (41, 's_29_41'), (41, 32), (41, 's_32_41'), (41, 46), (41, 's_41_46'), (41, 41), ('s_0_41', 's_0_41'), (47, 's_0_47'), (47, 10), (47, 's_10_47'), (47, 12), (47, 's_12_47'), (47, 22), (47, 's_22_47'), (47, 29), (47, 's_29_47'), (47, 32), (47, 's_32_47'), (47, 37), (47, 's_37_47'), (47, 43), (47, 's_43_47'), (47, 46), (47, 's_46_47'), (47, 47), ('s_0_47', 's_0_47'), (9, 4), (9, 10), (9, 18), (9, 26), (9, 42), (9, 48), (9, 3), (9, 40), (9, 's_7_9'), (9, 's_9_17'), (9, 's_9_23'), (9, 's_9_34'), (9, 's_4_9'), (9, 's_9_10'), (9, 's_9_18'), (9, 's_9_26'), (9, 's_9_42'), (9, 's_9_48'), (9, 's_3_9'), (9, 's_9_40'), (9, 15), (9, 's_9_15'), (9, 16), (9, 's_9_16'), (9, 24), (9, 's_9_24'), (9, 32), (9, 's_9_32'), (9, 35), (9, 's_9_35'), (9, 36), (9, 's_9_36'), (9, 37), (9, 's_9_37'), (9, 9), ('s_7_9', 's_7_9'), (13, 1), (13, 10), (13, 's_7_13'), (13, 's_13_23'), (13, 's_1_13'), (13, 's_10_13'), (13, 11), (13, 's_11_13'), (13, 15), (13, 's_13_15'), (13, 24), (13, 's_13_24'), (13, 28), (13, 's_13_28'), (13, 31), (13, 's_13_31'), (13, 37), (13, 's_13_37'), (13, 38), (13, 's_13_38'), (13, 39), (13, 's_13_39'), (13, 46), (13, 's_13_46'), (13, 13), ('s_7_13', 's_7_13'), (14, 10), (14, 28), (14, 48), (14, 5), (14, 8), (14, 11), (14, 22), (14, 45), (14, 19), (14, 31), (14, 's_7_14'), (14, 's_14_17'), (14, 's_14_27'), (14, 's_14_41'), (14, 's_10_14'), (14, 's_14_28'), (14, 's_14_48'), (14, 's_5_14'), (14, 's_8_14'), (14, 's_11_14'), (14, 's_14_22'), (14, 's_14_45'), (14, 's_14_19'), (14, 's_14_31'), (14, 37), (14, 's_14_37'), (14, 14), ('s_7_14', 's_7_14'), (15, 26), (15, 29), (15, 42), (15, 3), (15, 's_7_15'), (15, 's_15_17'), (15, 's_15_27'), (15, 's_15_34'), (15, 's_13_15'), (15, 's_15_26'), (15, 's_15_29'), (15, 's_15_42'), (15, 's_3_15'), (15, 's_9_15'), (15, 12), (15, 's_12_15'), (15, 20), (15, 's_15_20'), (15, 31), (15, 's_15_31'), (15, 36), (15, 's_15_36'), (15, 37), (15, 's_15_37'), (15, 38), (15, 's_15_38'), (15, 46), (15, 's_15_46'), (15, 15), ('s_7_15', 's_7_15'), ('s_7_25', 's_7_25'), (29, 1), (29, 4), (29, 10), (29, 18), (29, 's_7_29'), (29, 's_17_29'), (29, 's_27_29'), (29, 's_29_34'), (29, 's_29_41'), (29, 's_29_47'), (29, 's_1_29'), (29, 's_4_29'), (29, 's_10_29'), (29, 's_18_29'), (29, 6), (29, 's_6_29'), (29, 11), (29, 's_11_29'), (29, 12), (29, 's_12_29'), (29, 's_15_29'), (29, 16), (29, 's_16_29'), (29, 19), (29, 's_19_29'), (29, 38), (29, 's_29_38'), (29, 29), ('s_7_29', 's_7_29'), (36, 28), (36, 6), (36, 39), (36, 40), (36, 12), (36, 16), (36, 's_7_36'), (36, 's_23_36'), (36, 's_28_36'), (36, 's_6_36'), (36, 's_36_39'), (36, 's_36_40'), (36, 's_9_36'), (36, 's_15_36'), (36, 's_12_36'), (36, 's_16_36'), (36, 35), (36, 's_35_36'), (36, 36), ('s_7_36', 's_7_36'), (5, 2), (5, 4), (5, 10), (5, 48), (5, 's_5_17'), (5, 's_5_23'), (5, 's_2_5'), (5, 's_4_5'), (5, 's_5_10'), (5, 's_5_48'), (5, 12), (5, 's_5_12'), (5, 's_5_14'), (5, 39), (5, 's_5_39'), (5, 40), (5, 's_5_40'), (5, 45), (5, 's_5_45'), (5, 5), ('s_5_17', 's_5_17'), ('s_9_17', 's_9_17'), (12, 18), (12, 39), (12, 49), (12, 33), (12, 's_12_17'), (12, 's_12_25'), (12, 's_12_47'), (12, 's_12_18'), (12, 's_12_29'), (12, 's_5_12'), (12, 's_12_39'), (12, 's_12_15'), (12, 's_12_49'), (12, 's_12_33'), (12, 16), (12, 's_12_16'), (12, 's_12_36'), (12, 38), (12, 's_12_38'), (12, 43), (12, 's_12_43'), (12, 46), (12, 's_12_46'), (12, 12), ('s_12_17', 's_12_17'), ('s_14_17', 's_14_17'), ('s_15_17', 's_15_17'), (18, 1), (18, 's_17_18'), (18, 's_18_21'), (18, 's_18_27'), (18, 's_18_34'), (18, 's_18_41'), (18, 's_1_18'), (18, 6), (18, 's_6_18'), (18, 's_9_18'), (18, 11), (18, 's_11_18'), (18, 's_12_18'), (18, 19), (18, 's_18_19'), (18, 20), (18, 's_18_20'), (18, 28), (18, 's_18_28'), (18, 's_18_29'), (18, 38), (18, 's_18_38'), (18, 40), (18, 's_18_40'), (18, 45), (18, 's_18_45'), (18, 46), (18, 's_18_46'), (18, 48), (18, 's_18_48'), (18, 18), ('s_17_18', 's_17_18'), (19, 28), (19, 3), (19, 6), (19, 8), (19, 40), (19, 44), (19, 's_17_19'), (19, 's_19_30'), (19, 's_18_19'), (19, 's_19_28'), (19, 's_19_29'), (19, 's_3_19'), (19, 's_6_19'), (19, 's_8_19'), (19, 's_19_40'), (19, 's_19_44'), (19, 's_14_19'), (19, 32), (19, 's_19_32'), (19, 33), (19, 's_19_33'), (19, 37), (19, 's_19_37'), (19, 49), (19, 's_19_49'), (19, 19), ('s_17_19', 's_17_19'), (20, 4), (20, 26), (20, 39), (20, 44), (20, 45), (20, 's_17_20'), (20, 's_20_23'), (20, 's_20_25'), (20, 's_4_20'), (20, 's_18_20'), (20, 's_20_26'), (20, 's_20_39'), (20, 's_20_44'), (20, 's_20_45'), (20, 's_15_20'), (20, 35), (20, 's_20_35'), (20, 38), (20, 's_20_38'), (20, 20), ('s_17_20', 's_17_20'), (28, 1), (28, 26), (28, 's_17_28'), (28, 's_28_34'), (28, 's_1_28'), (28, 's_13_28'), (28, 's_18_28'), (28, 's_26_28'), (28, 8), (28, 's_8_28'), (28, 's_14_28'), (28, 's_19_28'), (28, 's_28_36'), (28, 40), (28, 's_28_40'), (28, 42), (28, 's_28_42'), (28, 43), (28, 's_28_43'), (28, 45), (28, 's_28_45'), (28, 28), ('s_17_28', 's_17_28'), ('s_17_29', 's_17_29'), (35, 26), (35, 8), (35, 22), (35, 40), (35, 24), (35, 32), (35, 38), (35, 's_17_35'), (35, 's_26_35'), (35, 's_8_35'), (35, 's_22_35'), (35, 's_35_40'), (35, 's_9_35'), (35, 's_24_35'), (35, 's_20_35'), (35, 's_32_35'), (35, 's_35_36'), (35, 's_35_38'), (35, 37), (35, 's_35_37'), (35, 35), ('s_17_35', 's_17_35'), (39, 2), (39, 8), (39, 's_17_39'), (39, 's_23_39'), (39, 's_27_39'), (39, 's_2_39'), (39, 's_13_39'), (39, 's_5_39'), (39, 's_8_39'), (39, 's_12_39'), (39, 's_20_39'), (39, 31), (39, 's_31_39'), (39, 33), (39, 's_33_39'), (39, 's_36_39'), (39, 49), (39, 's_39_49'), (39, 39), ('s_17_39', 's_17_39'), (40, 2), (40, 42), (40, 11), (40, 's_17_40'), (40, 's_25_40'), (40, 's_30_40'), (40, 's_2_40'), (40, 's_18_40'), (40, 's_28_40'), (40, 's_40_42'), (40, 's_5_40'), (40, 's_11_40'), (40, 's_9_40'), (40, 's_19_40'), (40, 24), (40, 's_24_40'), (40, 31), (40, 's_31_40'), (40, 33), (40, 's_33_40'), (40, 's_35_40'), (40, 's_36_40'), (40, 37), (40, 's_37_40'), (40, 44), (40, 's_40_44'), (40, 40), ('s_17_40', 's_17_40'), ('s_17_41', 's_17_41'), (49, 10), (49, 3), (49, 6), (49, 's_17_49'), (49, 's_10_49'), (49, 's_3_49'), (49, 's_6_49'), (49, 's_39_49'), (49, 's_19_49'), (49, 's_12_49'), (49, 16), (49, 's_16_49'), (49, 49), ('s_17_49', 's_17_49'), (8, 2), (8, 48), (8, 3), (8, 's_8_21'), (8, 's_8_27'), (8, 's_8_30'), (8, 's_2_8'), (8, 's_8_28'), (8, 's_8_48'), (8, 's_3_8'), (8, 's_8_14'), (8, 's_8_19'), (8, 's_8_35'), (8, 's_8_39'), (8, 8), ('s_8_21', 's_8_21'), ('s_18_21', 's_18_21'), ('s_21_23', 's_21_23'), ('s_21_34', 's_21_34'), (4, 1), (4, 2), (4, 's_4_23'), (4, 's_4_27'), (4, 's_4_30'), (4, 's_4_41'), (4, 's_1_4'), (4, 's_2_4'), (4, 's_4_5'), (4, 6), (4, 's_4_6'), (4, 's_4_9'), (4, 's_4_20'), (4, 24), (4, 's_4_24'), (4, 's_4_29'), (4, 31), (4, 's_4_31'), (4, 33), (4, 's_4_33'), (4, 42), (4, 's_4_42'), (4, 48), (4, 's_4_48'), (4, 4), ('s_4_23', 's_4_23'), ('s_5_23', 's_5_23'), ('s_9_23', 's_9_23'), (11, 2), (11, 26), (11, 48), (11, 's_11_23'), (11, 's_2_11'), (11, 's_11_13'), (11, 's_11_18'), (11, 's_11_26'), (11, 's_11_29'), (11, 's_11_48'), (11, 's_11_14'), (11, 22), (11, 's_11_22'), (11, 32), (11, 's_11_32'), (11, 33), (11, 's_11_33'), (11, 37), (11, 's_11_37'), (11, 's_11_40'), (11, 11), ('s_11_23', 's_11_23'), ('s_13_23', 's_13_23'), ('s_20_23', 's_20_23'), ('s_23_30', 's_23_30'), ('s_23_34', 's_23_34'), ('s_23_36', 's_23_36'), (37, 26), (37, 42), (37, 48), (37, 45), (37, 31), (37, 's_23_37'), (37, 's_25_37'), (37, 's_27_37'), (37, 's_37_47'), (37, 's_13_37'), (37, 's_26_37'), (37, 's_37_42'), (37, 's_37_48'), (37, 's_11_37'), (37, 's_37_40'), (37, 's_37_45'), (37, 's_9_37'), (37, 's_15_37'), (37, 's_19_37'), (37, 's_31_37'), (37, 's_14_37'), (37, 's_35_37'), (37, 37), ('s_23_37', 's_23_37'), ('s_23_39', 's_23_39'), (42, 1), (42, 's_23_42'), (42, 's_25_42'), (42, 's_30_42'), (42, 's_1_42'), (42, 's_4_42'), (42, 's_28_42'), (42, 6), (42, 's_6_42'), (42, 's_9_42'), (42, 's_15_42'), (42, 16), (42, 's_16_42'), (42, 31), (42, 's_31_42'), (42, 's_37_42'), (42, 's_40_42'), (42, 42), ('s_23_42', 's_23_42'), (43, 22), (43, 16), (43, 38), (43, 's_23_43'), (43, 's_27_43'), (43, 's_43_47'), (43, 's_28_43'), (43, 's_22_43'), (43, 's_12_43'), (43, 's_16_43'), (43, 's_38_43'), (43, 43), ('s_23_43', 's_23_43'), (1, 's_1_25'), (1, 's_1_27'), (1, 's_1_34'), (1, 's_1_41'), (1, 2), (1, 's_1_2'), (1, 's_1_4'), (1, 10), (1, 's_1_10'), (1, 's_1_13'), (1, 's_1_18'), (1, 26), (1, 's_1_26'), (1, 's_1_28'), (1, 's_1_29'), (1, 's_1_42'), (1, 48), (1, 's_1_48'), (1, 1), ('s_1_25', 's_1_25'), (2, 's_2_25'), (2, 's_2_34'), (2, 's_1_2'), (2, 3), (2, 's_2_3'), (2, 's_2_4'), (2, 's_2_5'), (2, 6), (2, 's_2_6'), (2, 's_2_8'), (2, 's_2_11'), (2, 22), (2, 's_2_22'), (2, 26), (2, 's_2_26'), (2, 's_2_39'), (2, 's_2_40'), (2, 44), (2, 's_2_44'), (2, 45), (2, 's_2_45'), (2, 2), ('s_2_25', 's_2_25'), (3, 48), (3, 's_3_25'), (3, 's_3_34'), (3, 's_3_41'), (3, 's_2_3'), (3, 's_3_48'), (3, 's_3_8'), (3, 's_3_9'), (3, 's_3_15'), (3, 's_3_19'), (3, 24), (3, 's_3_24'), (3, 's_3_49'), (3, 3), ('s_3_25', 's_3_25'), (10, 's_10_25'), (10, 's_10_27'), (10, 's_10_47'), (10, 's_1_10'), (10, 's_5_10'), (10, 's_9_10'), (10, 's_10_13'), (10, 's_10_14'), (10, 26), (10, 's_10_26'), (10, 's_10_29'), (10, 32), (10, 's_10_32'), (10, 48), (10, 's_10_48'), (10, 's_10_49'), (10, 10), ('s_10_25', 's_10_25'), ('s_12_25', 's_12_25'), ('s_20_25', 's_20_25'), (26, 's_25_26'), (26, 's_1_26'), (26, 's_2_26'), (26, 's_10_26'), (26, 's_9_26'), (26, 's_11_26'), (26, 's_15_26'), (26, 's_20_26'), (26, 's_26_28'), (26, 33), (26, 's_26_33'), (26, 's_26_35'), (26, 's_26_37'), (26, 44), (26, 's_26_44'), (26, 26), ('s_25_26', 's_25_26'), ('s_25_37', 's_25_37'), ('s_25_40', 's_25_40'), ('s_25_42', 's_25_42'), (46, 6), (46, 44), (46, 31), (46, 38), (46, 's_25_46'), (46, 's_41_46'), (46, 's_46_47'), (46, 's_13_46'), (46, 's_18_46'), (46, 's_6_46'), (46, 's_44_46'), (46, 's_15_46'), (46, 's_31_46'), (46, 's_12_46'), (46, 's_38_46'), (46, 46), ('s_25_46', 's_25_46'), (48, 's_25_48'), (48, 's_1_48'), (48, 's_4_48'), (48, 's_10_48'), (48, 's_18_48'), (48, 's_3_48'), (48, 's_5_48'), (48, 's_8_48'), (48, 's_9_48'), (48, 's_11_48'), (48, 's_14_48'), (48, 33), (48, 's_33_48'), (48, 's_37_48'), (48, 48), ('s_25_48', 's_25_48'), ('s_1_27', 's_1_27'), ('s_4_27', 's_4_27'), ('s_8_27', 's_8_27'), ('s_10_27', 's_10_27'), ('s_14_27', 's_14_27'), ('s_15_27', 's_15_27'), (16, 6), (16, 22), (16, 33), (16, 's_16_27'), (16, 's_16_29'), (16, 's_16_42'), (16, 's_6_16'), (16, 's_16_22'), (16, 's_9_16'), (16, 's_16_49'), (16, 's_16_33'), (16, 's_12_16'), (16, 32), (16, 's_16_32'), (16, 's_16_36'), (16, 's_16_43'), (16, 16), ('s_16_27', 's_16_27'), ('s_18_27', 's_18_27'), (24, 45), (24, 's_24_27'), (24, 's_4_24'), (24, 's_13_24'), (24, 's_3_24'), (24, 's_24_40'), (24, 's_24_45'), (24, 's_9_24'), (24, 's_24_35'), (24, 24), ('s_24_27', 's_24_27'), ('s_27_29', 's_27_29'), (32, 6), (32, 22), (32, 44), (32, 's_27_32'), (32, 's_32_41'), (32, 's_32_47'), (32, 's_10_32'), (32, 's_6_32'), (32, 's_11_32'), (32, 's_22_32'), (32, 's_32_44'), (32, 's_9_32'), (32, 's_19_32'), (32, 's_16_32'), (32, 's_32_35'), (32, 38), (32, 's_32_38'), (32, 32), ('s_27_32', 's_27_32'), ('s_27_37', 's_27_37'), (38, 6), (38, 22), (38, 44), (38, 's_27_38'), (38, 's_13_38'), (38, 's_18_38'), (38, 's_29_38'), (38, 's_6_38'), (38, 's_22_38'), (38, 's_38_44'), (38, 's_15_38'), (38, 's_20_38'), (38, 's_12_38'), (38, 's_32_38'), (38, 's_35_38'), (38, 's_38_43'), (38, 's_38_46'), (38, 38), ('s_27_38', 's_27_38'), ('s_27_39', 's_27_39'), ('s_27_43', 's_27_43'), (45, 22), (45, 's_27_45'), (45, 's_2_45'), (45, 's_18_45'), (45, 's_28_45'), (45, 's_5_45'), (45, 's_22_45'), (45, 's_14_45'), (45, 's_20_45'), (45, 's_24_45'), (45, 's_37_45'), (45, 45), ('s_27_45', 's_27_45'), ('s_4_30', 's_4_30'), ('s_8_30', 's_8_30'), ('s_19_30', 's_19_30'), ('s_30_40', 's_30_40'), ('s_30_42', 's_30_42'), ('s_1_34', 's_1_34'), ('s_2_34', 's_2_34'), ('s_3_34', 's_3_34'), ('s_9_34', 's_9_34'), ('s_15_34', 's_15_34'), ('s_18_34', 's_18_34'), ('s_28_34', 's_28_34'), ('s_29_34', 's_29_34'), (31, 6), (31, 44), (31, 's_31_34'), (31, 's_4_31'), (31, 's_13_31'), (31, 's_31_42'), (31, 's_6_31'), (31, 's_31_39'), (31, 's_31_40'), (31, 's_31_44'), (31, 's_15_31'), (31, 's_14_31'), (31, 33), (31, 's_31_33'), (31, 's_31_37'), (31, 's_31_46'), (31, 31), ('s_31_34', 's_31_34'), (33, 22), (33, 's_33_34'), (33, 's_4_33'), (33, 's_26_33'), (33, 's_33_48'), (33, 's_11_33'), (33, 's_22_33'), (33, 's_33_39'), (33, 's_33_40'), (33, 's_19_33'), (33, 's_31_33'), (33, 's_12_33'), (33, 's_16_33'), (33, 33), ('s_33_34', 's_33_34'), ('s_1_41', 's_1_41'), ('s_3_41', 's_3_41'), ('s_4_41', 's_4_41'), ('s_14_41', 's_14_41'), ('s_18_41', 's_18_41'), ('s_29_41', 's_29_41'), ('s_32_41', 's_32_41'), ('s_41_46', 's_41_46'), ('s_10_47', 's_10_47'), ('s_12_47', 's_12_47'), (22, 's_22_47'), (22, 's_2_22'), (22, 's_11_22'), (22, 's_14_22'), (22, 's_16_22'), (22, 's_22_32'), (22, 's_22_33'), (22, 's_22_35'), (22, 's_22_38'), (22, 's_22_43'), (22, 's_22_45'), (22, 22), ('s_22_47', 's_22_47'), ('s_29_47', 's_29_47'), ('s_32_47', 's_32_47'), ('s_37_47', 's_37_47'), ('s_43_47', 's_43_47'), ('s_46_47', 's_46_47'), ('s_1_2', 's_1_2'), ('s_1_4', 's_1_4'), ('s_1_10', 's_1_10'), ('s_1_13', 's_1_13'), ('s_1_18', 's_1_18'), ('s_1_26', 's_1_26'), ('s_1_28', 's_1_28'), ('s_1_29', 's_1_29'), ('s_1_42', 's_1_42'), ('s_1_48', 's_1_48'), ('s_2_3', 's_2_3'), ('s_2_4', 's_2_4'), ('s_2_5', 's_2_5'), (6, 's_2_6'), (6, 's_4_6'), (6, 's_6_18'), (6, 's_6_29'), (6, 's_6_42'), (6, 's_6_16'), (6, 's_6_19'), (6, 's_6_31'), (6, 's_6_32'), (6, 's_6_36'), (6, 's_6_38'), (6, 's_6_46'), (6, 's_6_49'), (6, 6), ('s_2_6', 's_2_6'), ('s_2_8', 's_2_8'), ('s_2_11', 's_2_11'), ('s_2_22', 's_2_22'), ('s_2_26', 's_2_26'), ('s_2_39', 's_2_39'), ('s_2_40', 's_2_40'), (44, 's_2_44'), (44, 's_26_44'), (44, 's_40_44'), (44, 's_19_44'), (44, 's_20_44'), (44, 's_31_44'), (44, 's_32_44'), (44, 's_38_44'), (44, 's_44_46'), (44, 44), ('s_2_44', 's_2_44'), ('s_2_45', 's_2_45'), ('s_4_5', 's_4_5'), ('s_4_6', 's_4_6'), ('s_4_9', 's_4_9'), ('s_4_20', 's_4_20'), ('s_4_24', 's_4_24'), ('s_4_29', 's_4_29'), ('s_4_31', 's_4_31'), ('s_4_33', 's_4_33'), ('s_4_42', 's_4_42'), ('s_4_48', 's_4_48'), ('s_5_10', 's_5_10'), ('s_9_10', 's_9_10'), ('s_10_13', 's_10_13'), ('s_10_14', 's_10_14'), ('s_10_26', 's_10_26'), ('s_10_29', 's_10_29'), ('s_10_32', 's_10_32'), ('s_10_48', 's_10_48'), ('s_10_49', 's_10_49'), ('s_11_13', 's_11_13'), ('s_13_15', 's_13_15'), ('s_13_24', 's_13_24'), ('s_13_28', 's_13_28'), ('s_13_31', 's_13_31'), ('s_13_37', 's_13_37'), ('s_13_38', 's_13_38'), ('s_13_39', 's_13_39'), ('s_13_46', 's_13_46'), ('s_6_18', 's_6_18'), ('s_9_18', 's_9_18'), ('s_11_18', 's_11_18'), ('s_12_18', 's_12_18'), ('s_18_19', 's_18_19'), ('s_18_20', 's_18_20'), ('s_18_28', 's_18_28'), ('s_18_29', 's_18_29'), ('s_18_38', 's_18_38'), ('s_18_40', 's_18_40'), ('s_18_45', 's_18_45'), ('s_18_46', 's_18_46'), ('s_18_48', 's_18_48'), ('s_9_26', 's_9_26'), ('s_11_26', 's_11_26'), ('s_15_26', 's_15_26'), ('s_20_26', 's_20_26'), ('s_26_28', 's_26_28'), ('s_26_33', 's_26_33'), ('s_26_35', 's_26_35'), ('s_26_37', 's_26_37'), ('s_26_44', 's_26_44'), ('s_8_28', 's_8_28'), ('s_14_28', 's_14_28'), ('s_19_28', 's_19_28'), ('s_28_36', 's_28_36'), ('s_28_40', 's_28_40'), ('s_28_42', 's_28_42'), ('s_28_43', 's_28_43'), ('s_28_45', 's_28_45'), ('s_6_29', 's_6_29'), ('s_11_29', 's_11_29'), ('s_12_29', 's_12_29'), ('s_15_29', 's_15_29'), ('s_16_29', 's_16_29'), ('s_19_29', 's_19_29'), ('s_29_38', 's_29_38'), ('s_6_42', 's_6_42'), ('s_9_42', 's_9_42'), ('s_15_42', 's_15_42'), ('s_16_42', 's_16_42'), ('s_31_42', 's_31_42'), ('s_37_42', 's_37_42'), ('s_40_42', 's_40_42'), ('s_3_48', 's_3_48'), ('s_5_48', 's_5_48'), ('s_8_48', 's_8_48'), ('s_9_48', 's_9_48'), ('s_11_48', 's_11_48'), ('s_14_48', 's_14_48'), ('s_33_48', 's_33_48'), ('s_37_48', 's_37_48'), ('s_3_8', 's_3_8'), ('s_3_9', 's_3_9'), ('s_3_15', 's_3_15'), ('s_3_19', 's_3_19'), ('s_3_24', 's_3_24'), ('s_3_49', 's_3_49'), ('s_5_12', 's_5_12'), ('s_5_14', 's_5_14'), ('s_5_39', 's_5_39'), ('s_5_40', 's_5_40'), ('s_5_45', 's_5_45'), ('s_6_16', 's_6_16'), ('s_6_19', 's_6_19'), ('s_6_31', 's_6_31'), ('s_6_32', 's_6_32'), ('s_6_36', 's_6_36'), ('s_6_38', 's_6_38'), ('s_6_46', 's_6_46'), ('s_6_49', 's_6_49'), ('s_8_14', 's_8_14'), ('s_8_19', 's_8_19'), ('s_8_35', 's_8_35'), ('s_8_39', 's_8_39'), ('s_11_14', 's_11_14'), ('s_11_22', 's_11_22'), ('s_11_32', 's_11_32'), ('s_11_33', 's_11_33'), ('s_11_37', 's_11_37'), ('s_11_40', 's_11_40'), ('s_14_22', 's_14_22'), ('s_16_22', 's_16_22'), ('s_22_32', 's_22_32'), ('s_22_33', 's_22_33'), ('s_22_35', 's_22_35'), ('s_22_38', 's_22_38'), ('s_22_43', 's_22_43'), ('s_22_45', 's_22_45'), ('s_12_39', 's_12_39'), ('s_20_39', 's_20_39'), ('s_31_39', 's_31_39'), ('s_33_39', 's_33_39'), ('s_36_39', 's_36_39'), ('s_39_49', 's_39_49'), ('s_9_40', 's_9_40'), ('s_19_40', 's_19_40'), ('s_24_40', 's_24_40'), ('s_31_40', 's_31_40'), ('s_33_40', 's_33_40'), ('s_35_40', 's_35_40'), ('s_36_40', 's_36_40'), ('s_37_40', 's_37_40'), ('s_40_44', 's_40_44'), ('s_19_44', 's_19_44'), ('s_20_44', 's_20_44'), ('s_31_44', 's_31_44'), ('s_32_44', 's_32_44'), ('s_38_44', 's_38_44'), ('s_44_46', 's_44_46'), ('s_14_45', 's_14_45'), ('s_20_45', 's_20_45'), ('s_24_45', 's_24_45'), ('s_37_45', 's_37_45'), ('s_9_15', 's_9_15'), ('s_9_16', 's_9_16'), ('s_9_24', 's_9_24'), ('s_9_32', 's_9_32'), ('s_9_35', 's_9_35'), ('s_9_36', 's_9_36'), ('s_9_37', 's_9_37'), ('s_12_15', 's_12_15'), ('s_15_20', 's_15_20'), ('s_15_31', 's_15_31'), ('s_15_36', 's_15_36'), ('s_15_37', 's_15_37'), ('s_15_38', 's_15_38'), ('s_15_46', 's_15_46'), ('s_14_19', 's_14_19'), ('s_19_32', 's_19_32'), ('s_19_33', 's_19_33'), ('s_19_37', 's_19_37'), ('s_19_49', 's_19_49'), ('s_24_35', 's_24_35'), ('s_12_49', 's_12_49'), ('s_16_49', 's_16_49'), ('s_20_35', 's_20_35'), ('s_20_38', 's_20_38'), ('s_14_31', 's_14_31'), ('s_31_33', 's_31_33'), ('s_31_37', 's_31_37'), ('s_31_46', 's_31_46'), ('s_12_33', 's_12_33'), ('s_16_33', 's_16_33'), ('s_12_16', 's_12_16'), ('s_12_36', 's_12_36'), ('s_12_38', 's_12_38'), ('s_12_43', 's_12_43'), ('s_12_46', 's_12_46'), ('s_14_37', 's_14_37'), ('s_16_32', 's_16_32'), ('s_16_36', 's_16_36'), ('s_16_43', 's_16_43'), ('s_32_35', 's_32_35'), ('s_32_38', 's_32_38'), ('s_35_36', 's_35_36'), ('s_35_38', 's_35_38'), ('s_38_43', 's_38_43'), ('s_38_46', 's_38_46'), ('s_35_37', 's_35_37')]</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1501,136 +1349,96 @@
           <t>[(0, 7), (0, 17), (0, 21), (0, 23), (0, 25), (0, 27), (0, 30), (0, 34), (0, 41), (0, 47), (0, 0), (7, 9), (7, 13), (7, 14), (7, 15), (7, 25), (7, 29), (7, 36), (7, 7), (17, 5), (17, 9), (17, 12), (17, 14), (17, 15), (17, 18), (17, 19), (17, 20), (17, 28), (17, 29), (17, 35), (17, 39), (17, 40), (17, 41), (17, 49), (17, 17), (21, 8), (21, 18), (21, 23), (21, 34), (21, 21), (23, 4), (23, 5), (23, 9), (23, 11), (23, 13), (23, 20), (23, 30), (23, 34), (23, 36), (23, 37), (23, 39), (23, 42), (23, 43), (23, 23), (25, 1), (25, 2), (25, 3), (25, 10), (25, 12), (25, 20), (25, 26), (25, 37), (25, 40), (25, 42), (25, 46), (25, 48), (25, 25), (27, 1), (27, 4), (27, 8), (27, 10), (27, 14), (27, 15), (27, 16), (27, 18), (27, 24), (27, 29), (27, 32), (27, 37), (27, 38), (27, 39), (27, 43), (27, 45), (27, 27), (30, 4), (30, 8), (30, 19), (30, 40), (30, 42), (30, 30), (34, 1), (34, 2), (34, 3), (34, 9), (34, 15), (34, 18), (34, 28), (34, 29), (34, 31), (34, 33), (34, 34), (41, 1), (41, 3), (41, 4), (41, 14), (41, 18), (41, 29), (41, 32), (41, 46), (41, 41), (47, 10), (47, 12), (47, 22), (47, 29), (47, 32), (47, 37), (47, 43), (47, 46), (47, 47), (9, 4), (9, 10), (9, 18), (9, 26), (9, 42), (9, 48), (9, 3), (9, 40), (9, 15), (9, 16), (9, 24), (9, 32), (9, 35), (9, 36), (9, 37), (9, 9), (13, 1), (13, 10), (13, 11), (13, 15), (13, 24), (13, 28), (13, 31), (13, 37), (13, 38), (13, 39), (13, 46), (13, 13), (14, 10), (14, 28), (14, 48), (14, 5), (14, 8), (14, 11), (14, 22), (14, 45), (14, 19), (14, 31), (14, 37), (14, 14), (15, 26), (15, 29), (15, 42), (15, 3), (15, 12), (15, 20), (15, 31), (15, 36), (15, 37), (15, 38), (15, 46), (15, 15), (29, 1), (29, 4), (29, 10), (29, 18), (29, 6), (29, 11), (29, 12), (29, 16), (29, 19), (29, 38), (29, 29), (36, 28), (36, 6), (36, 39), (36, 40), (36, 12), (36, 16), (36, 35), (36, 36), (5, 2), (5, 4), (5, 10), (5, 48), (5, 12), (5, 39), (5, 40), (5, 45), (5, 5), (12, 18), (12, 39), (12, 49), (12, 33), (12, 16), (12, 38), (12, 43), (12, 46), (12, 12), (18, 1), (18, 6), (18, 11), (18, 19), (18, 20), (18, 28), (18, 38), (18, 40), (18, 45), (18, 46), (18, 48), (18, 18), (19, 28), (19, 3), (19, 6), (19, 8), (19, 40), (19, 44), (19, 32), (19, 33), (19, 37), (19, 49), (19, 19), (20, 4), (20, 26), (20, 39), (20, 44), (20, 45), (20, 35), (20, 38), (20, 20), (28, 1), (28, 26), (28, 8), (28, 40), (28, 42), (28, 43), (28, 45), (28, 28), (35, 26), (35, 8), (35, 22), (35, 40), (35, 24), (35, 32), (35, 38), (35, 37), (35, 35), (39, 2), (39, 8), (39, 31), (39, 33), (39, 49), (39, 39), (40, 2), (40, 42), (40, 11), (40, 24), (40, 31), (40, 33), (40, 37), (40, 44), (40, 40), (49, 10), (49, 3), (49, 6), (49, 16), (49, 49), (8, 2), (8, 48), (8, 3), (8, 8), (4, 1), (4, 2), (4, 6), (4, 24), (4, 31), (4, 33), (4, 42), (4, 48), (4, 4), (11, 2), (11, 26), (11, 48), (11, 22), (11, 32), (11, 33), (11, 37), (11, 11), (37, 26), (37, 42), (37, 48), (37, 45), (37, 31), (37, 37), (42, 1), (42, 6), (42, 16), (42, 31), (42, 42), (43, 22), (43, 16), (43, 38), (43, 43), (1, 2), (1, 10), (1, 26), (1, 48), (1, 1), (2, 3), (2, 6), (2, 22), (2, 26), (2, 44), (2, 45), (2, 2), (3, 48), (3, 24), (3, 3), (10, 26), (10, 32), (10, 48), (10, 10), (26, 33), (26, 44), (26, 26), (46, 6), (46, 44), (46, 31), (46, 38), (46, 46), (48, 33), (48, 48), (16, 6), (16, 22), (16, 33), (16, 32), (16, 16), (24, 45), (24, 24), (32, 6), (32, 22), (32, 44), (32, 38), (32, 32), (38, 6), (38, 22), (38, 44), (38, 38), (45, 22), (45, 45), (31, 6), (31, 44), (31, 33), (31, 31), (33, 22), (33, 33), (22, 22), (6, 6), (44, 44)]</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>NaN</t>
-        </is>
+      <c r="N7" t="n">
+        <v>881.48</v>
+      </c>
+      <c r="O7" t="n">
+        <v>222.71</v>
+      </c>
+      <c r="P7" t="n">
+        <v>57.64735054969788</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>4.715132236480713</v>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>{0: [4791, 1509, 1287, 1286, 4732, 4731, 1285], 7: [1303, 5302, 1029, 1437, 4760, 4761, 4762, 1436, 1435, 1434], 's_0_7': [4672], 17: [1422, 849, 5152, 5151, 5150, 5149, 850, 851, 853, 852], 's_0_17': [1272], 21: [1192, 1194, 1193], 's_0_21': [1179], 23: [4386, 1207, 1208, 1061, 5000, 1077, 5180, 1212, 1211, 1209, 1210, 4881], 's_0_23': [4971], 25: [5345, 1152, 5087, 5088, 5089, 5090, 1315, 1316, 5031, 5030, 1151], 's_0_25': [5016], 27: [532, 1481, 1482, 5242, 5241, 5240, 5239, 867, 533, 534, 535, 536, 537, 5177, 5178], 's_0_27': [1480], 30: [1224, 4640, 4638, 4639], 's_0_30': [1225], 34: [1164, 4742, 926, 925, 4746, 4745, 4743, 4744], 's_0_34': [1239], 41: [568, 5402, 913, 4717, 1495, 1496, 1497, 1498, 5407, 5406, 5405, 5403, 5404], 's_0_41': [1524], 47: [5002, 5001, 1243, 1242, 1241], 's_0_47': [4986], 9: [4250, 1027, 5163, 5120, 4400, 938, 939, 940, 941, 942, 5164], 's_7_9': [4595], 13: [5450, 1313, 4432, 1139, 1138, 1137, 1136, 1418, 1419, 1420, 4942, 4941], 's_7_13': [4657], 14: [4847, 5391, 5390, 5389, 5388, 5387, 594, 595, 596, 597, 598], 's_7_14': [1318], 15: [5344, 1090, 1017, 5062, 5061, 1091, 5060, 1016], 's_7_15': [5047], 's_7_25': [5032], 29: [607, 608, 609, 5287, 5286, 5045, 1001, 1002, 5285, 5284, 5283, 612, 611, 610], 's_7_29': [1362], 36: [4954, 4955, 982, 983, 984, 985], 's_7_36': [4610], 5: [5106, 5105, 5104, 552, 5102, 5103], 's_5_17': [5134, 777], 's_9_17': [5119], 12: [883, 1331, 5077, 1346, 1045, 5076, 5075, 5359, 1048, 1047, 1046], 's_12_17': [1181], 's_14_17': [868], 's_15_17': [5135], 18: [4326, 4443, 5313, 5314, 837, 836, 835, 4325, 4324, 834, 833, 832], 's_17_18': [848], 19: [775, 4626, 4624, 4623, 774, 4579, 699, 4608, 998, 4625, 879], 's_17_19': [4594], 20: [1093, 428, 429, 5300, 5299, 5298, 5297, 432, 431, 430], 's_17_20': [1062], 28: [4687, 4686, 4685, 4996, 4997, 4998, 820, 4684, 819], 's_17_28': [4924], 's_17_29': [1407], 35: [4295, 4816, 4817, 654, 4728, 1147, 1148, 1149, 4730, 4729], 's_17_35': [864], 39: [460, 897, 1345, 4836, 896, 4907, 4834, 4908, 4835, 894, 895, 4909], 's_17_39': [4969], 40: [727, 728, 729, 986, 5059, 5058, 731, 730], 's_17_40': [4818], 's_17_41': [5419], 49: [4551, 1302, 1299, 1301, 1300], 's_17_49': [1317], 8: [759, 564, 4670, 4667, 4669, 4668], 's_8_21': [4655], 's_18_21': [4341], 's_21_23': [4596], 's_21_34': [4820], 4: [5282, 1088, 522, 521, 520, 519, 4637, 653, 4518, 773, 4384, 4385], 's_4_23': [4370, 4371], 's_5_23': [1107], 's_9_23': [4970], 11: [1135, 701, 4880, 4877, 700, 4878, 4879], 's_11_23': [1165], 's_13_23': [4387], 's_20_23': [5255], 's_23_30': [4611], 's_23_34': [4805], 's_23_36': [4956], 37: [5042, 5043, 5316, 5270, 1123, 4653, 789, 790, 791, 792, 5269, 5268], 's_23_37': [5271], 's_23_39': [4850], 42: [4458, 4459, 1028, 4535, 5195, 1122, 1121, 1120, 1119], 's_23_42': [1118, 4401], 43: [1344, 4806, 1257, 1256, 1255], 's_23_43': [4926], 1: [658, 5225, 5224, 5223, 657, 5192, 5191, 402, 400, 401], 's_1_25': [567], 2: [4726, 4593, 4666, 4592, 503, 506, 505, 4727, 504], 's_2_25': [5072], 3: [804, 4712, 1252, 1253, 4641, 1254, 1074, 4713, 4714, 4716, 4715], 's_3_25': [1314], 10: [1452, 5212, 5208, 1092, 1347, 5209, 1228, 1227, 5211, 5210], 's_10_25': [5346], 's_12_25': [1196], 's_20_25': [5086], 26: [353, 4561, 369, 370, 4831, 4832, 5194, 5193, 747, 640, 5133, 641], 's_25_26': [656], 's_25_37': [5360], 's_25_40': [686], 's_25_42': [1182], 46: [4444, 4445, 1388, 878, 1392, 1391, 1390, 4446, 1389], 's_25_46': [4747], 48: [5161, 762, 763, 5253, 669, 670, 5162, 671, 672], 's_25_48': [5073], 's_1_27': [4952], 's_4_27': [4787], 's_8_27': [4562], 's_10_27': [5197], 's_14_27': [5252], 's_15_27': [5179], 16: [1106, 4910, 4790, 4897, 4896, 4895, 1058, 1059, 1060], 's_16_27': [4912], 's_18_27': [821], 24: [667, 4352, 4353, 4354, 4356, 4355], 's_24_27': [4277], 's_27_29': [4367], 32: [4718, 910, 909, 908, 4489, 4490, 4492, 1553, 1554, 4491, 1555, 5167, 1556], 's_27_32': [5108], 's_27_37': [687], 38: [593, 1376, 1375, 1374, 1373, 4507, 4501, 4502, 4503, 4504, 4506, 4505], 's_27_38': [4442], 's_27_39': [4892], 's_27_43': [5226], 45: [5012, 583, 582, 581, 577, 578, 579, 580], 's_27_45': [4307], 's_4_30': [803], 's_8_30': [1089], 's_19_30': [818], 's_30_40': [744], 's_30_42': [1013], 's_1_34': [415], 's_2_34': [459], 's_3_34': [745], 's_9_34': [4984], 's_15_34': [5014], 's_18_34': [4759], 's_28_34': [969], 's_29_34': [5044], 31: [953, 4582, 4581, 4580, 958, 957, 956, 955, 954], 's_31_34': [4819], 33: [880, 551, 4937, 4940, 4939, 4938], 's_33_34': [550], 's_1_41': [5433, 703], 's_3_41': [1494, 4642], 's_4_41': [523, 538], 's_14_41': [823], 's_18_41': [688], 's_29_41': [733], 's_32_41': [4748], 's_41_46': [1404], 's_10_47': [5481], 's_12_47': [5091], 22: [1465, 1271, 1270, 624, 4773, 4774, 4777, 4776, 4775], 's_22_47': [1466], 's_29_47': [5301], 's_32_47': [4987], 's_37_47': [5331], 's_43_47': [1258], 's_46_47': [5196], 's_4_9': [4399], 's_9_10': [717], 's_9_18': [1087], 's_9_26': [732], 's_9_42': [5121], 's_9_48': [702], 's_3_9': [4251], 's_9_40': [971], 's_9_15': [1076], 's_9_16': [4565], 's_9_24': [1072], 's_9_32': [4549], 's_9_35': [1102], 's_9_36': [4534], 's_9_37': [806], 's_1_13': [5448, 5449], 's_10_13': [5466], 's_11_13': [1150], 's_13_15': [5015], 's_13_24': [1327], 's_13_28': [4701, 4702], 's_13_31': [4567], 's_13_37': [1124], 's_13_38': [4522], 's_13_39': [1360], 's_13_46': [4537], 's_10_14': [5375], 's_14_28': [4982], 's_14_48': [748], 's_5_14': [5237], 's_8_14': [4652], 's_11_14': [4862], 's_14_22': [625], 's_14_45': [5372], 's_14_19': [4848], 's_14_31': [5374], 's_14_37': [1288], 's_15_26': [987], 's_15_29': [5046], 's_15_42': [4865], 's_3_15': [1105], 's_12_15': [1033], 's_15_20': [943], 's_15_31': [5330], 's_15_36': [1015], 's_15_37': [972], 's_15_38': [1361], 's_15_46': [1406], 's_1_29': [822], 's_4_29': [4487], 's_10_29': [1453], 's_18_29': [5315], 6: [4477, 4476, 4412, 4413, 1238, 997, 4416, 4414, 4415], 's_6_29': [4428], 's_11_29': [5118], 's_12_29': [928], 's_16_29': [1000], 's_19_29': [4578], 's_29_38': [1377], 's_28_36': [761], 's_6_36': [967], 's_36_39': [4894], 's_36_40': [4953], 's_12_36': [1031], 's_16_36': [4430], 's_35_36': [4294], 's_2_5': [491], 's_4_5': [553], 's_5_10': [927], 's_5_48': [626], 's_5_12': [1166], 's_5_39': [881], 's_5_40': [866], 's_5_45': [5222], 's_12_18': [5358], 's_12_39': [1330], 's_12_49': [5137], 's_12_33': [4849], 's_12_16': [4925], 's_12_38': [5122], 's_12_43': [5166], 's_12_46': [5181], 's_1_18': [627], 's_6_18': [4429], 's_11_18': [4833], 's_18_19': [4564], 's_18_20': [5312, 418], 's_18_28': [4699], 's_18_38': [758], 's_18_40': [4339, 4338], 's_18_45': [5328], 's_18_46': [1342], 's_18_48': [5329], 44: [4474, 4471, 4473, 4472], 's_19_28': [1284], 's_3_19': [1343], 's_6_19': [893], 's_8_19': [924], 's_19_40': [4698], 's_19_44': [863], 's_19_32': [4609], 's_19_33': [4789], 's_19_37': [714], 's_19_49': [1269], 's_4_20': [4636], 's_20_26': [4711], 's_20_39': [4906], 's_20_44': [4486], 's_20_45': [5011], 's_20_35': [4801], 's_20_38': [443], 's_1_28': [4981], 's_26_28': [371], 's_8_28': [1014], 's_28_40': [716], 's_28_42': [1104], 's_28_43': [1359], 's_28_45': [566], 's_26_35': [340], 's_8_35': [999], 's_22_35': [760], 's_35_40': [4758], 's_24_35': [1222], 's_32_35': [4475], 's_35_38': [1163], 's_35_37': [4683], 's_2_39': [4846], 's_8_39': [4654], 's_31_39': [5029], 's_33_39': [4922], 's_39_49': [4972], 's_2_40': [5057], 's_40_42': [698, 4533], 's_11_40': [4803], 's_24_40': [4248], 's_31_40': [5074], 's_33_40': [776], 's_37_40': [5013], 's_40_44': [743], 's_10_49': [5107], 's_3_49': [4671], 's_6_49': [4536], 's_16_49': [4911], 's_2_8': [549], 's_8_48': [4622], 's_3_8': [1044], 's_1_4': [403], 's_2_4': [507], 's_4_6': [518], 's_4_24': [652, 4398], 's_4_31': [4519], 's_4_33': [4967], 's_4_42': [787], 's_4_48': [5207], 's_2_11': [565], 's_11_26': [4863], 's_11_48': [4968], 's_11_22': [4788], 's_11_32': [4864], 's_11_33': [490], 's_11_37': [805], 's_26_37': [882], 's_37_42': [1197], 's_37_48': [778], 's_37_45': [5267], 's_31_37': [5254], 's_1_42': [1167], 's_6_42': [802], 's_16_42': [4700], 's_31_42': [4566], 's_22_43': [1329], 's_16_43': [1240], 's_38_43': [4792], 's_1_2': [5026], 's_1_10': [912], 's_1_26': [642], 's_1_48': [5357, 673], 's_2_3': [489], 's_2_6': [4427], 's_2_22': [4772], 's_2_26': [4441], 's_2_44': [488], 's_2_45': [4532], 's_3_48': [684], 's_3_24': [1237], 's_10_26': [1032], 's_10_32': [5182], 's_10_48': [807], 's_26_33': [655], 's_26_44': [368], 's_6_46': [1283], 's_44_46': [1043], 's_31_46': [1403], 's_38_46': [1372], 's_33_48': [5027], 's_6_16': [1073], 's_16_22': [1405], 's_16_33': [1030], 's_16_32': [4898], 's_24_45': [4383], 's_6_32': [1583], 's_22_32': [4778], 's_32_44': [4488], 's_32_38': [4508], 's_6_38': [398], 's_22_38': [623], 's_38_44': [713], 's_22_45': [4682], 's_6_31': [1223], 's_31_44': [968], 's_31_33': [4804], 's_22_33': [1075]}</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>NaN</t>
+          <t>{0: [2051, 2052], 7: [5022, 5020, 5021], 17: [5263, 5260, 5262, 5261], 21: [2067, 2007, 5230], 23: [5245, 5007, 5006, 1992, 1991, 5005], 25: [5323, 2021, 2022, 2023, 5322, 5321], 27: [2261, 5111, 5113, 5112], 30: [2065, 2066, 5065], 34: [5217, 5216, 5215], 41: [5292, 2038, 5291], 47: [5126, 5127, 5128], 9: [2293, 5157, 2291, 2292], 13: [2171, 4978, 4977, 4976], 14: [2143, 2141, 2142], 15: [5247, 2383, 2381, 2382], 29: [5278, 2126, 2127, 5276, 5277], 36: [2306, 5082], 5: [5202, 2307, 5200, 5201], 12: [2425, 2428, 2427, 2426], 18: [2441, 2442, 5350, 5351, 5352], 19: [5141, 2112, 5472, 5471, 2113], 20: [5367, 1993, 5365, 5366], 28: [4991, 2230, 2233, 2232, 2231], 35: [2366, 5142, 2368, 2367], 39: [2413, 2410, 2411, 2412], 40: [5037, 2097, 2096, 5035, 5036], 49: [5380, 5381, 2533, 5382, 5383], 8: [5185, 5187, 5186], 4: [2247, 5066, 2245, 2246], 11: [5336, 2156, 2157, 2158], 37: [2203, 2201, 5246, 2202], 42: [4961, 2351, 4963, 4962], 43: [2486, 4992], 1: [4990, 2083, 2080, 2082, 2081], 2: [5233, 5231, 2353, 2352, 5232], 3: [2323, 2322], 10: [5156, 5081, 2173, 2172], 26: [5410, 5412, 5411], 46: [2518, 2516, 5293, 2517], 48: [5172, 5170, 5171], 16: [2546, 2548, 5158, 2547, 5083], 24: [5097, 5067, 2321], 32: [5428, 5427, 2187, 2188, 5426], 38: [5143, 2398, 2396, 2397], 45: [2218, 5096, 2217], 31: [1977, 1976, 5050, 5053, 5052, 5051], 33: [2456, 2308, 5337, 5338, 2457], 22: [5248, 5396, 2532, 5397, 2487, 2488], 6: [2336, 2337, 5306, 5308, 5307], 44: [5473, 5413, 2471, 2472, 2473]}</t>
         </is>
       </c>
       <c r="T7" t="n">
-        <v>950.09</v>
+        <v>791</v>
       </c>
       <c r="U7" t="n">
-        <v>224.72</v>
+        <v>201</v>
       </c>
       <c r="V7" t="n">
-        <v>54.33702790737152</v>
+        <v>49.66722178459167</v>
       </c>
       <c r="W7" t="n">
-        <v>3.719246745109558</v>
+        <v>8.642152547836304</v>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>{0: [5265, 253, 252, 251, 247, 248, 249, 250], 7: [175, 176, 179, 178, 177], 's_0_7': [5370], 17: [4866, 1259, 1258, 1257, 1254, 1255, 1256, 5091, 5085, 5086, 5088, 5089, 5087, 5090], 's_0_17': [5070], 21: [4756, 4757], 's_0_21': [4741], 23: [308, 309, 310, 311, 312, 5190, 5191, 5192, 5193, 1107, 5195, 5194], 's_0_23': [4440], 25: [145, 713, 714, 715, 4908, 4905, 4906, 4907], 's_0_25': [4875], 27: [4815, 608, 609, 5076, 5075, 1046, 1045, 4816, 4817, 4818, 4819], 's_0_27': [264], 30: [563, 503, 4426, 4427], 's_0_30': [4411], 34: [220, 221, 4951, 4956, 4952, 4953, 939, 4699, 969, 970, 4955, 4954], 's_0_34': [4725], 41: [5506, 5508, 5512, 5511, 5507, 5510, 5509], 's_0_41': [268], 47: [867, 5374, 5282, 914, 913, 5281, 5284, 5283], 's_0_47': [267], 's_0_0': [4320], 9: [192, 191, 4845, 190, 4865, 4864, 865, 864, 4668, 189, 4665, 4666, 4667], 's_7_9': [4965], 13: [4743, 4995, 4996, 5237, 582, 579, 580, 581, 4997], 's_7_13': [4980], 14: [569, 4802, 5447, 4832, 534, 5310, 535, 536, 537, 538, 5312, 5311], 's_7_14': [5325], 15: [265, 1196, 266, 5161, 5162, 611, 5160, 612, 5271, 1197, 5360, 5359, 5358, 703, 5313], 's_7_15': [4860], 's_7_25': [4770], 29: [5520, 5521, 5522, 5523, 5524, 5525, 1241, 4986, 1391, 1392, 1393, 5452, 5451, 1198], 's_7_29': [5535], 36: [1033, 1032, 174, 1031, 1030, 1029, 1028, 4459, 173, 4455, 4456, 4457, 4458], 's_7_36': [158, 159, 160], 's_7_7': [5655], 5: [1061, 4804, 4806, 4805, 1105, 1106, 5042, 5043, 5044, 5045], 's_17_5': [971], 's_17_9': [206, 205, 207], 12: [551, 5012, 1183, 5285, 1182, 1002, 1001, 5013, 5014, 5015, 1181], 's_17_12': [552], 's_17_14': [5072], 's_17_15': [402], 18: [524, 5495, 5494, 4787, 519, 520, 521, 522, 823, 523, 5387, 5388], 's_17_18': [5496], 19: [4881, 4637, 653, 1346, 1345, 1344, 1343, 4577, 4578, 4579, 4580, 4581, 4582], 's_17_19': [4626], 20: [5301, 776, 777, 778, 5418, 1138, 5420, 5419], 's_17_20': [763, 762], 28: [1149, 4731, 4730, 4636, 489, 4727, 4729, 4728], 's_17_28': [4776], 's_17_29': [5526], 35: [5299, 4640, 4639, 897, 896, 894, 4924, 895], 's_17_35': [4641], 39: [5332, 1118, 627, 5328, 5329, 5330, 5331, 1119, 1120, 1121, 1122, 1123], 's_17_39': [1332, 5211], 40: [807, 4414, 4607, 806, 805, 458, 802, 4517, 4518, 804, 803], 's_17_40': [5073], 's_17_41': [1244], 49: [1377, 5031, 5016, 5107, 1375, 1376], 's_17_49': [1302], 's_17_17': [101], 8: [459, 4685, 4684, 4686, 564, 4682, 4683], 's_21_8': [504], 's_21_18': [4742], 's_21_23': [324], 's_21_34': [235], 's_21_21': [339], 4: [863, 5302, 4485, 1363, 4486, 4487, 4488, 4489, 4490, 4491, 1362, 1361, 1360, 1359, 1358], 's_23_4': [5196], 's_23_5': [5041], 's_23_9': [4635], 11: [418, 689, 688, 5297, 5135, 432, 5134, 5133, 687, 672, 5298], 's_23_11': [927], 's_23_13': [507], 's_23_20': [5208], 's_23_30': [323], 's_23_34': [4966], 's_23_36': [4650], 37: [968, 4534, 4533, 4532, 4531, 4576, 5251, 297, 296, 295, 294, 293], 's_23_37': [5056], 's_23_39': [1137, 1136, 4910], 42: [356, 4621, 4921, 355, 353, 354], 's_23_42': [5101], 43: [955, 956, 958, 957], 's_23_43': [5209], 's_23_23': [5206], 1: [4398, 4397, 413, 414, 4696, 429, 430, 448, 4351, 447, 446, 5011, 431], 's_25_1': [371], 2: [953, 733, 732, 4354, 4353, 731, 730, 729, 728], 's_25_2': [4833], 3: [4698, 4564, 1289, 759, 1288, 1287, 1286, 1285, 4565, 4566, 1284], 's_25_3': [4623], 10: [4985, 610, 4942, 912, 911, 4937, 4938, 4939, 1091, 4941, 4940], 's_25_10': [655], 's_25_12': [566], 's_25_20': [761], 26: [622, 5270, 4428, 4429, 1167, 1166, 1164, 4655, 923, 5136, 1165, 924, 4654], 's_25_26': [4413], 's_25_37': [4548], 's_25_40': [4443], 's_25_42': [4891], 46: [4846, 4847, 643, 642, 641, 640], 's_25_46': [445], 48: [760, 597, 789, 593, 594, 4502, 4789, 4788, 4862, 596, 595], 's_25_48': [4892], 's_25_25': [115], 's_27_1': [607], 's_27_4': [623], 's_27_8': [999], 's_27_10': [1016, 5179], 's_27_14': [670], 's_27_15': [5241, 1317], 16: [866, 5116, 5117, 5118, 1467, 5122, 5121, 5120, 5119], 's_27_16': [1092], 's_27_18': [400], 24: [833, 4595, 4593, 4594], 's_27_24': [4608], 's_27_29': [5077], 32: [929, 5479, 882, 883, 4791, 1225, 4850, 4849, 880, 881], 's_27_32': [4984], 's_27_37': [279], 38: [1075, 4968, 4969, 4970, 5435, 5449, 5450, 5390, 1078, 1077, 1076], 's_27_38': [5060], 's_27_39': [4820], 's_27_43': [4834], 45: [5267, 5268, 983, 984, 985, 5269, 988, 987, 986], 's_27_45': [4925], 's_27_27': [340], 's_30_4': [233], 's_30_8': [4562], 's_30_19': [488], 's_30_40': [457], 's_30_42': [338], 's_30_30': [4425], 's_34_1': [5025, 5026], 's_34_2': [938], 's_34_3': [4971], 's_34_9': [219], 's_34_15': [5055], 's_34_18': [4967], 's_34_28': [879], 's_34_29': [4957], 31: [790, 5252, 4878, 4877, 383, 384, 385, 4801, 492, 491, 490], 's_34_31': [506], 33: [4879, 717, 1133, 5178, 821, 820, 4505, 4504, 818, 819], 's_34_33': [4549], 's_34_34': [834], 's_41_1': [5492], 's_41_3': [1274], 's_41_4': [5497], 's_41_14': [628], 's_41_18': [509, 5582], 's_41_29': [1214], 's_41_32': [764], 's_41_46': [658], 's_41_41': [1394], 's_47_10': [5239], 's_47_12': [5375], 22: [5404, 851, 852, 5372, 5373, 853], 's_47_22': [5464], 's_47_29': [5539], 's_47_32': [5584], 's_47_37': [282], 's_47_43': [5344], 's_47_46': [657], 's_47_47': [822], 's_9_4': [188], 's_9_10': [1150], 's_9_18': [444], 's_9_26': [4669], 's_9_42': [369], 's_9_48': [910], 's_9_3': [669], 's_9_40': [399], 's_9_15': [5175], 's_9_16': [5115], 's_9_24': [774], 's_9_32': [1000], 's_9_35': [4744], 's_9_36': [4575], 's_9_37': [234], 's_9_9': [204], 's_13_1': [4981], 's_13_10': [416], 's_13_11': [671], 's_13_15': [5027], 's_13_24': [684], 's_13_28': [699], 's_13_31': [5222], 's_13_37': [5236], 's_13_38': [686], 's_13_39': [583], 's_13_46': [460], 's_13_13': [4758], 's_14_10': [4922], 's_14_28': [4697], 's_14_48': [4652], 's_14_5': [5057], 's_14_8': [4622], 's_14_11': [5327], 's_14_22': [613], 's_14_45': [553], 's_14_19': [654], 's_14_31': [5102], 's_14_37': [373], 's_14_14': [102], 's_15_26': [5210], 's_15_29': [5272, 1407], 's_15_42': [4936], 's_15_3': [5286], 's_15_12': [5226], 's_15_20': [673], 's_15_31': [5176], 's_15_36': [1093, 5300], 's_15_37': [281], 's_15_38': [1048], 's_15_46': [5103], 's_15_15': [342], 's_29_1': [5537, 5536], 's_29_4': [5257], 's_29_10': [1240], 's_29_18': [5538], 6: [1406, 4726, 1405, 415, 4772, 4773, 4774, 4775, 1060, 4895, 4896, 1330, 4927], 's_29_6': [5001], 's_29_11': [674], 's_29_12': [5540], 's_29_16': [5227], 's_29_19': [5287, 1347], 's_29_38': [1139], 's_29_29': [1243], 's_36_28': [4715], 's_36_6': [4880], 's_36_39': [5225], 's_36_40': [787], 's_36_12': [5256, 5255], 's_36_16': [5105], 's_36_35': [1044], 's_36_36': [172], 's_5_2': [746], 's_5_4': [1374], 's_5_10': [1390], 's_5_48': [4790], 's_5_12': [1151], 's_5_39': [1135], 's_5_40': [4803], 's_5_45': [4745], 's_5_5': [4807], 's_12_18': [1003], 's_12_39': [626], 's_12_49': [5030], 's_12_33': [716], 's_12_16': [1211], 's_12_38': [5345], 's_12_43': [943], 's_12_46': [656], 's_12_12': [5466], 's_18_1': [5132], 's_18_6': [565], 's_18_11': [5552], 's_18_19': [4592, 549], 's_18_20': [808], 's_18_28': [4712], 's_18_38': [1109], 's_18_40': [518], 's_18_45': [5389, 928], 's_18_46': [793, 5433], 's_18_48': [505], 's_18_18': [1064], 's_19_28': [1329], 's_19_3': [4536], 's_19_6': [4972], 's_19_8': [1299], 's_19_40': [848], 44: [5152, 5151, 5150, 5148, 791, 5149], 's_19_44': [5137], 's_19_32': [4851], 's_19_33': [1073], 's_19_37': [878], 's_19_49': [5166], 's_19_19': [1433], 's_20_4': [1273, 5376], 's_20_26': [5316], 's_20_39': [718], 's_20_44': [1242], 's_20_45': [5253], 's_20_35': [898], 's_20_38': [1168], 's_20_20': [1153], 's_28_1': [4651], 's_28_26': [1074], 's_28_8': [624], 's_28_40': [4713], 's_28_42': [443], 's_28_43': [940], 's_28_45': [4714], 's_28_28': [1315], 's_35_26': [1163], 's_35_8': [1059], 's_35_22': [5224], 's_35_40': [893], 's_35_24': [1089], 's_35_32': [4999], 's_35_38': [926], 's_35_37': [4624], 's_35_35': [1193], 's_39_2': [4401, 4400], 's_39_8': [4700], 's_39_31': [598], 's_39_33': [4431], 's_39_49': [5106], 's_39_39': [4370, 1057], 's_40_2': [743], 's_40_42': [4471], 's_40_11': [5223], 's_40_24': [4473], 's_40_31': [4606], 's_40_33': [4609], 's_40_37': [683], 's_40_44': [5163], 's_40_40': [4293], 's_49_10': [1301], 's_49_3': [5181], 's_49_6': [4897], 's_49_16': [5092], 's_49_49': [5062], 's_8_2': [744], 's_8_48': [4547], 's_8_3': [4701], 's_8_8': [1239], 's_4_1': [398], 's_4_2': [908], 's_4_6': [4836], 's_4_24': [998], 's_4_31': [368], 's_4_33': [1043], 's_4_42': [428], 's_4_48': [473], 's_4_4': [4537], 's_11_2': [5403], 's_11_26': [1047], 's_11_48': [5207], 's_11_22': [5371], 's_11_32': [5478], 's_11_33': [5177], 's_11_37': [5266], 's_11_11': [5401], 's_37_26': [668], 's_37_42': [357], 's_37_48': [533], 's_37_45': [4610], 's_37_31': [4591], 's_37_37': [5340], 's_42_1': [352], 's_42_6': [4771], 's_42_16': [341], 's_42_31': [4561], 's_42_42': [4920], 's_43_22': [5254], 's_43_16': [942], 's_43_38': [5315], 's_43_43': [4894], 's_1_2': [4352], 's_1_10': [401], 's_1_26': [578], 's_1_48': [4501], 's_1_1': [4441, 4442], 's_2_3': [758], 's_2_6': [700, 4863], 's_2_22': [748], 's_2_26': [4444], 's_2_44': [5028], 's_2_45': [982], 's_2_2': [952], 's_3_48': [4653], 's_3_24': [954], 's_3_3': [5541], 's_10_26': [4926], 's_10_32': [1015], 's_10_48': [475], 's_10_10': [1420], 's_26_33': [817], 's_26_44': [1272], 's_26_26': [1108], 's_46_6': [550], 's_46_44': [5058], 's_46_31': [4831], 's_46_38': [5448], 's_46_46': [5493], 's_48_33': [4759], 's_48_48': [4383], 's_16_6': [1331], 's_16_22': [4998], 's_16_33': [5059], 's_16_32': [4792, 1465, 1466], 's_16_16': [5197], 's_24_45': [4519], 's_24_24': [849], 's_32_6': [4911, 1210], 's_32_22': [838], 's_32_44': [5104], 's_32_38': [5480], 's_32_32': [1270], 's_38_6': [4835], 's_38_22': [868], 's_38_44': [1062], 's_38_38': [1018], 's_45_22': [5434], 's_45_45': [5465], 's_31_6': [775], 's_31_44': [5147], 's_31_33': [4848], 's_31_31': [493], 's_33_22': [5074], 's_33_33': [4475], 's_22_22': [854], 's_6_6': [1451], 's_44_44': [1437]}</t>
+          <t>[878, 896, 845, 915, 852, 886, 887, 886, 892, 889, 909, 935, 882, 903, 978, 849, 803, 906, 828, 900, 902, 949, 904, 844, 868, 862, 882, 877, 889, 856, 934, 853, 886, 866, 902, 884, 920, 893, 811, 913, 832, 889, 830, 849, 869, 856, 811, 886, 929, 819, 825, 861, 874, 923, 971, 907, 864, 872, 838, 861, 856, 898, 860, 951, 930, 872, 863, 844, 861, 791, 896, 888, 856, 916, 842, 902, 847, 864, 856, 911, 969, 926, 853, 884, 955, 909, 913, 914, 894, 854, 894, 854, 916, 953, 861, 825, 899, 896, 856, 839]</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>{0: [4903, 2335, 4902], 7: [4841, 4842], 17: [2410, 5096, 5097, 2412, 2411], 21: [2274, 4812, 4811], 23: [2470, 5306, 5307, 5308, 2472, 2471], 25: [2424, 2427, 2426, 4991, 2425, 4992], 27: [2305, 2306, 5200, 5201, 2307], 30: [2439, 4797, 4798], 34: [5292, 2353, 2350, 2352, 2351], 41: [4917, 4916], 47: [1991, 4901, 4900], 9: [2485, 2486, 5111, 5112, 5113], 13: [4781, 2140, 2142, 2141], 14: [2155, 5006, 2157, 2156], 15: [2455, 2456, 5276, 2457, 5277, 5278], 29: [2245, 2246, 2247], 36: [2606, 2380, 2381, 5053, 5052], 5: [5247, 2082, 5246], 12: [1992, 2382, 5172, 5170, 5171], 18: [2170, 5232, 5231, 2171, 2172], 19: [5185, 5186, 2259, 2260, 2261], 20: [2336, 5068, 5066, 5067], 28: [4870, 4873, 4871, 4872], 35: [4961, 4963, 4962], 39: [2232, 5051, 2231], 40: [2337, 2440, 2441, 5187], 49: [2112, 2111], 8: [2230, 4782, 2229], 4: [2292, 2290, 5036, 2291], 11: [4933, 4931, 4932], 37: [5217, 2216, 2217, 5216], 42: [5037, 2365, 2367, 2366], 43: [5305, 1962, 1960, 1961], 1: [2080, 4887, 4886], 2: [2320, 5126, 5127, 2322, 2321], 3: [2454, 2110, 4825, 4827, 4826], 10: [2081, 5022, 5021, 5020], 26: [5007, 2397, 2395, 2396], 46: [4990, 2127, 2125, 2126], 48: [2200, 2202, 2201], 16: [4948, 5035, 2036, 2051, 4947, 4946], 24: [2215, 2275, 4857, 4856], 32: [2022, 4915, 2021], 38: [5005, 2095, 5261, 2097, 2096], 45: [2185, 2187, 2186], 31: [2531, 2532, 5156, 5158, 5157], 33: [2546, 2547, 5142, 5143], 22: [5095, 2065, 5141, 2066], 6: [5080, 5083, 5081, 5082], 44: [4978, 4976, 4977]}</t>
+          <t>[218, 224, 224, 212, 212, 242, 237, 225, 226, 218, 212, 223, 218, 224, 222, 219, 237, 228, 225, 218, 226, 225, 227, 224, 239, 220, 229, 239, 217, 227, 207, 224, 222, 215, 226, 205, 240, 213, 232, 215, 215, 232, 214, 233, 232, 224, 205, 234, 231, 223, 229, 213, 213, 221, 231, 226, 215, 207, 232, 241, 235, 220, 217, 206, 225, 216, 225, 222, 216, 219, 233, 220, 231, 222, 219, 215, 226, 232, 203, 229, 219, 212, 210, 234, 228, 232, 230, 226, 201, 238, 203, 219, 223, 218, 227, 229, 220, 216, 224, 224]</t>
         </is>
       </c>
       <c r="Z7" t="n">
-        <v>880</v>
+        <v>37.95650887076636</v>
       </c>
       <c r="AA7" t="n">
-        <v>199</v>
+        <v>9.148930499950762</v>
       </c>
       <c r="AB7" t="n">
-        <v>63.26925468444824</v>
+        <v>1</v>
       </c>
       <c r="AC7" t="n">
-        <v>3.133347749710083</v>
+        <v>1</v>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>[{0: [1452, 716, 1092, 582, 5123, 5122, 5121, 5118, 5119, 5120], 7: [4523, 1541, 1540, 1537, 1538, 1539], 's_0_7': [5108], 17: [5222, 4401, 537, 536, 535, 4832, 655, 4400, 4399, 4398, 654, 652, 653], 's_0_17': [5072], 21: [806, 5012, 5178, 821, 5013], 's_0_21': [717], 23: [1043, 822, 778, 1044, 4940, 4760, 984, 5253, 5254, 987, 986, 985], 's_0_23': [5150], 25: [1479, 1242, 1318, 837, 5239, 5240, 5241, 1317, 1316, 4672, 1315, 4762, 1344, 4671], 's_0_25': [5242], 27: [893, 5062, 1181, 5015, 715, 4937, 5061, 4938, 894, 895, 4939, 1031, 5014, 911], 's_0_27': [581], 30: [5056, 5060, 506, 5057, 5059, 5058], 's_0_30': [836], 34: [462, 504, 594, 4727, 5206, 595, 596, 642, 5207, 5133, 597], 's_0_34': [5237], 41: [4882, 1192, 1601, 1450, 4822, 4823, 1600, 1599, 1598, 4415, 4418, 4416, 4417], 's_0_41': [1616], 47: [1093, 5348, 5347, 5344, 1243, 5345, 5346], 's_0_47': [1453], 's_0_0': [5148], 9: [610, 4968, 834, 835, 4969, 4970, 4971, 4973, 1417, 1418, 1419, 1420, 1421, 4972], 's_7_9': [4958], 13: [443, 4621, 473, 4517, 1525, 4518, 4519, 4520, 4807, 1524, 1523, 4522, 4521], 's_7_13': [1554], 14: [4952, 4861, 475, 4862, 4863, 4864, 4853, 4852, 4851, 4850, 1120, 4865], 's_7_14': [1555], 15: [4742, 4743, 4908, 700, 699, 698, 697, 4308, 4312, 4311, 4310, 4309], 's_7_15': [1567, 4343], 's_7_25': [4613], 29: [5267, 5268, 5269, 5270, 5271, 1273, 1272, 1507, 1508, 1509, 5166, 5167, 1511, 1510], 's_7_29': [4778], 36: [1088, 4592, 4598, 4597, 4596, 4593, 4594, 1089, 4595], 's_7_36': [1553], 's_7_7': [4508], 5: [538, 384, 1048, 385, 5389, 5388, 5387, 386, 387, 388, 5386], 's_17_5': [5221], 's_17_9': [4847], 12: [5407, 4550, 4549, 4548, 4547, 5406, 5405, 5404, 5403, 5402, 493, 492, 491, 490, 489, 488], 's_17_12': [5252], 's_17_14': [4922], 's_17_15': [4338, 787], 18: [4387, 4386, 4385, 672, 938, 939, 940, 941, 942, 5164, 5161, 5162, 5163], 's_17_18': [1207], 19: [4703, 4702, 4701, 4700, 521, 520, 519, 4697, 4698, 4699], 's_17_19': [4622], 20: [5223, 972, 5330, 5329, 4458, 792, 791, 790, 848, 849, 850, 4833], 's_17_20': [4457], 28: [563, 567, 866, 4998, 4997, 564, 565, 566], 's_17_28': [4877], 's_17_29': [612], 35: [863, 862, 4373, 637, 4372, 4371, 4366, 4367, 4368, 4369, 4370], 's_17_35': [593], 39: [4776, 4775, 4774, 325, 4771, 4772, 608, 609, 4773], 's_17_39': [4472], 40: [5027, 5026, 357, 4656, 4655, 773, 774, 356, 355, 354, 4651, 4652, 4654, 4653], 's_17_40': [4683], 's_17_41': [953], 49: [1147, 1256, 1255, 1148, 4611, 1254], 's_17_49': [1118, 4475], 's_17_17': [982], 8: [5011, 4996, 413, 414, 415, 4967, 5042, 5041, 416], 's_21_8': [5043], 's_21_18': [852], 's_21_23': [5179], 's_21_34': [5177], 's_21_21': [551], 4: [1583, 1584, 4718, 5090, 4717, 4716, 4715, 5495, 1013, 1018, 1017, 1016, 1014, 1015], 's_23_4': [4685], 's_23_5': [943], 's_23_9': [4909], 11: [1253, 4898, 4897, 4837, 4581, 4834, 1405, 1269, 1270, 4835, 4836], 's_23_11': [1090], 's_23_13': [983], 's_23_20': [807], 's_23_30': [5044], 's_23_34': [702], 's_23_36': [1059], 37: [5449, 908, 909, 897, 896, 4984, 4744, 910, 4849, 898, 970], 's_23_37': [882], 's_23_39': [969], 42: [999, 1000, 762, 5032, 5031, 5030, 761, 4924, 4925, 1106], 's_23_42': [1060], 43: [5074, 5075, 1138, 1137], 's_23_43': [5089], 's_23_23': [913], 1: [5103, 5104, 5105, 1078, 1077, 1073, 1074, 1075, 1076], 's_25_1': [927], 2: [1389, 4777, 1390, 1391, 1392, 1393, 5376, 371, 372, 373, 5371, 5372, 5373, 5374, 5375], 's_25_2': [5107], 3: [819, 925, 1240, 4792, 4791, 4790, 4787, 4788, 4789], 's_25_3': [4806], 10: [5316, 1734, 5390, 1735, 1705, 4988, 4987, 4986, 1123, 1122, 1121, 4985], 's_25_10': [1241], 's_25_12': [1303], 's_25_20': [5299], 26: [1676, 1675, 1674, 4562, 4569, 4568, 4563, 1374, 1373, 4567, 4564, 4565, 4566], 's_25_26': [4673], 's_25_37': [5314], 's_25_40': [1314], 's_25_42': [1107], 46: [1363, 1357, 1358, 1359, 1362, 1361, 1360], 's_25_46': [5302], 48: [1045, 1210, 4896, 4895, 4894, 4816, 4817, 4818, 865], 's_25_48': [4881], 's_25_25': [1343], 's_27_1': [881], 's_27_4': [5029], 's_27_8': [401], 's_27_10': [5180], 's_27_14': [460], 's_27_15': [640], 16: [5136, 1194, 4761, 1288, 1287, 5046, 1284, 5211, 1285, 1286], 's_27_16': [1196], 's_27_18': [671, 670], 24: [4639, 877, 878, 4714, 879], 's_27_24': [892], 's_27_29': [1346], 32: [5198, 1406, 5047, 1451, 1628, 1629, 1630, 4927, 1633, 1632, 1631, 4928], 's_27_32': [1466], 's_27_37': [956], 38: [1557, 743, 744, 745, 746, 747, 5197, 5196, 5195, 5194, 5193], 's_27_38': [912], 's_27_39': [505], 's_27_43': [1046], 45: [775, 5418, 4533, 729, 733, 4713, 732, 730, 731], 's_27_45': [4534], 's_27_27': [4414], 's_30_4': [1001], 's_30_8': [611], 's_30_19': [5117], 's_30_40': [626], 's_30_42': [1091], 's_30_30': [5102], 's_34_1': [656], 's_34_2': [5191], 's_34_3': [459], 's_34_9': [4953], 's_34_15': [4728], 's_34_18': [507], 's_34_28': [4637], 's_34_29': [627], 31: [1482, 1483, 5362, 1423, 444, 1481, 5467, 5466, 5463, 5465, 5462, 5464, 448, 447, 445, 446], 's_34_31': [5132], 33: [5087, 5086, 341, 340, 339, 338, 579, 4486, 578, 1193, 4490, 4489, 4488, 4487], 's_34_33': [4578], 's_34_34': [5357], 's_41_1': [1058], 's_41_3': [4793], 's_41_4': [1012], 's_41_14': [1465], 's_41_18': [1133], 's_41_29': [4433], 's_41_32': [1615], 's_41_46': [1372], 's_41_41': [4419], 's_47_10': [5360], 's_47_12': [1258], 22: [4492, 1139, 734, 5478, 5479, 5480, 5481, 4491, 1298, 1299, 1183, 1182, 1300, 1301, 1302, 5226], 's_47_22': [1197], 's_47_29': [1167], 's_47_32': [5363], 's_47_37': [883], 's_47_43': [5255], 's_47_46': [5361], 's_47_47': [1244], 's_9_4': [4462], 's_9_10': [4974], 's_9_18': [1432], 's_9_26': [4582], 's_9_42': [1586], 's_9_48': [1136], 's_9_3': [4729], 's_9_40': [624, 625, 4982], 's_9_15': [4668], 's_9_16': [4956], 's_9_24': [4759], 's_9_32': [1646], 's_9_35': [4357], 's_9_36': [4612], 's_9_37': [4848], 's_9_9': [4237], 's_13_1': [4506, 4505], 's_13_10': [4808], 's_13_11': [4732, 1495], 's_13_15': [4503], 's_13_24': [4504], 's_13_28': [548], 's_13_31': [5002], 's_13_37': [923], 's_13_38': [728], 's_13_39': [4502], 's_13_46': [4537], 's_13_13': [4748], 's_14_10': [1345], 's_14_28': [820], 's_14_48': [1150], 's_14_5': [4831], 's_14_8': [430], 's_14_11': [1570], 's_14_22': [4866], 's_14_45': [760], 's_14_19': [1179, 4746], 's_14_31': [4846], 's_14_37': [4879], 's_14_14': [295], 's_15_26': [713], 's_15_29': [1522], 's_15_42': [805], 's_15_3': [550], 's_15_12': [4907], 's_15_20': [817], 's_15_31': [429], 's_15_36': [1087], 's_15_37': [5134, 777, 776], 's_15_38': [4413], 's_15_46': [1492, 4342], 's_15_15': [1477], 's_29_1': [1002, 5300], 's_29_4': [4642], 's_29_10': [5151], 's_29_18': [522], 6: [4610, 1422, 1104, 1105, 4730, 4731, 1329, 5138, 5137, 1331, 1330], 's_29_6': [1467], 's_29_11': [4912], 's_29_12': [553], 's_29_16': [5391], 's_29_19': [4763, 1614], 's_29_38': [1047], 's_29_29': [4297], 's_36_28': [4607], 's_36_6': [1328, 4641, 4640], 's_36_39': [4608], 's_36_40': [399], 's_36_12': [759], 's_36_16': [1224], 's_36_35': [638], 's_36_36': [1464], 's_5_2': [5131], 's_5_4': [1049], 's_5_10': [5315], 's_5_48': [370], 's_5_12': [5341], 's_5_39': [4906], 's_5_40': [4951], 's_5_45': [658], 's_5_5': [523], 's_12_18': [673], 's_12_39': [4682], 's_12_49': [4535], 's_12_33': [4666], 's_12_16': [5421], 's_12_38': [1332, 1333], 's_12_43': [5420], 's_12_46': [5422], 's_12_12': [4546], 's_18_1': [1072], 's_18_6': [1103], 's_18_11': [1252], 's_18_19': [954], 's_18_20': [5209], 's_18_28': [4999], 's_18_38': [957], 's_18_40': [342], 's_18_45': [687, 5298], 's_18_46': [4402], 's_18_48': [4819], 's_18_18': [1313], 's_19_28': [4667], 's_19_3': [804], 's_19_6': [1029], 's_19_8': [4757], 's_19_40': [534], 44: [4428, 4429, 4430, 4431, 4432, 5017, 1436, 1435, 1433, 1434], 's_19_44': [4687], 's_19_32': [1644], 's_19_33': [518], 's_19_37': [4684], 's_19_49': [1119], 's_19_19': [4704], 's_20_4': [5285], 's_20_26': [4579], 's_20_39': [789], 's_20_44': [802], 's_20_45': [763], 's_20_35': [832], 's_20_38': [5208], 's_20_20': [853], 's_28_1': [701], 's_28_26': [4577], 's_28_8': [4412], 's_28_40': [549], 's_28_42': [4954], 's_28_43': [851], 's_28_45': [4532], 's_28_28': [4382], 's_35_26': [1673], 's_35_8': [4351], 's_35_22': [4356], 's_35_40': [4473], 's_35_24': [4339], 's_35_32': [4358], 's_35_38': [4383], 's_35_37': [4354], 's_35_35': [427], 's_39_2': [4936], 's_39_8': [4891], 's_39_31': [4876], 's_39_33': [623], 's_39_49': [1149], 's_39_39': [4815], 's_40_2': [5146], 's_40_42': [686, 5073], 's_40_11': [1404], 's_40_24': [864], 's_40_31': [5176], 's_40_33': [4756], 's_40_37': [4669], 's_40_44': [4657], 's_40_40': [5101], 's_49_10': [5106], 's_49_3': [1239], 's_49_6': [4911], 's_49_16': [4626], 's_49_49': [5076], 's_8_2': [4981], 's_8_48': [4801], 's_8_3': [400], 's_8_8': [4427], 's_4_1': [5045], 's_4_2': [1003], 's_4_6': [5091], 's_4_24': [4474], 's_4_31': [1109], 's_4_33': [998], 's_4_42': [4955], 's_4_48': [4910], 's_4_4': [5496], 's_11_2': [4867], 's_11_26': [4838], 's_11_48': [1225], 's_11_22': [1268], 's_11_32': [4913], 's_11_33': [1223], 's_11_37': [955], 's_11_11': [4899], 's_37_26': [924], 's_37_42': [5149], 's_37_48': [926], 's_37_45': [5419], 's_37_31': [823], 's_37_37': [944], 's_42_1': [1061], 's_42_6': [1571, 1572], 's_42_16': [5016], 's_42_31': [1496], 's_42_42': [5000], 's_43_22': [5301], 's_43_16': [5286], 's_43_38': [5210], 's_43_43': [971], 's_1_2': [1063], 's_1_10': [5225], 's_1_26': [4580], 's_1_48': [4805], 's_1_1': [4445], 's_2_3': [4821], 's_2_6': [5001], 's_2_22': [1168], 's_2_26': [1388], 's_2_44': [4957], 's_2_45': [748], 's_2_2': [374], 's_3_48': [4804], 's_3_24': [880], 's_3_3': [4926], 's_10_26': [4794], 's_10_32': [4929], 's_10_48': [1165], 's_10_10': [4689], 's_26_33': [683], 's_26_44': [5018], 's_26_26': [1778], 's_46_6': [5152], 's_46_44': [4507], 's_46_31': [5257], 's_46_38': [1377], 's_46_46': [4476], 's_48_33': [580], 's_48_48': [1209], 's_16_6': [5181], 's_16_22': [5256], 's_16_33': [4536], 's_16_32': [1407], 's_16_16': [1289], 's_24_45': [4638], 's_24_24': [4264], 's_32_6': [4942], 's_32_22': [4493], 's_32_44': [5092, 5093], 's_32_38': [5273], 's_32_32': [5408], 's_38_6': [5212, 1587], 's_38_22': [1212], 's_38_44': [1556], 's_38_38': [4758], 's_45_22': [688], 's_45_45': [668], 's_31_6': [1497], 's_31_44': [5077], 's_31_33': [4711], 's_31_31': [554], 's_33_22': [4551], 's_33_33': [4456], 's_22_22': [5448], 's_6_6': [1617], 's_44_44': [4477]}, {0: [1497, 4959, 5047, 4958, 1496, 1495, 1494, 4451, 4450, 4449, 1778, 4584, 4583], 7: [1317, 1406, 5122], 's_0_7': [1436], 17: [4596, 4850, 1209, 1498, 5275, 5274, 5273, 5272, 5271, 1212, 1211, 1210], 's_0_17': [5046], 21: [1751, 1811, 5050, 5049], 's_0_21': [4974], 23: [1947, 1946, 4977, 4976, 4975, 1856, 1855, 1597, 1598, 1599, 4718, 4719], 's_0_23': [4717], 25: [1572, 1016, 5075, 5076, 1781, 5079, 1571, 5078, 5077], 's_0_25': [1601], 27: [4766, 2140, 2139, 2138, 1269, 4466, 4465, 4464, 4463, 1268, 4462, 4461, 4460, 1058], 's_0_27': [2183], 30: [2198, 2201, 4856, 2200, 2199], 's_0_30': [2213, 2214], 34: [5018, 4749, 1674, 1676, 1675], 's_0_34': [1659], 41: [1208, 1658, 4509, 4508, 1178, 4506, 4507], 's_0_41': [4434], 47: [5212, 957, 5135, 4837, 1465, 1466, 1467, 5136, 5137], 's_0_47': [1523, 1524, 1525], 's_0_0': [4452], 9: [1825, 5186, 5185, 2005, 4869, 4870, 1196, 5180, 5181, 5182, 5183, 5184, 1915, 1916], 's_7_9': [1302], 13: [4970, 4971, 2364, 2365, 2366, 2367, 4972, 4973, 1586, 5093, 5094, 5095, 5096, 2363, 5097], 's_7_13': [4957], 14: [1853, 5001, 5002, 1962, 5003, 5004, 5005, 1961, 1960, 1959, 1958, 4420], 's_7_14': [1391], 15: [1284, 5016, 1616, 1617, 5258, 5257, 1362, 4670, 4671, 1359, 1361, 1360], 's_7_15': [5196], 's_7_25': [5091], 29: [1238, 4733, 4732, 4476, 1373, 1374, 5345, 5346, 1377, 1376, 1375], 's_7_29': [5211], 36: [1930, 4824, 1316, 1315, 4820, 4821, 4823, 4822], 's_7_36': [1405], 's_7_7': [5121], 5: [1767, 5289, 1752, 2097, 5232, 5231, 5230, 5229], 's_17_5': [1887], 's_17_9': [5030], 12: [1073, 1074, 5377, 5376, 5379, 5375, 1933, 1075, 1678, 1076, 5378, 1077, 1078], 's_17_12': [5195], 's_17_14': [5000], 's_17_15': [1707], 18: [1644, 1553, 4550, 1163, 4611, 4612, 4613, 4614, 4615, 1989, 1990, 1991, 1993, 1992], 's_17_18': [1239], 19: [2078, 2079, 2080, 2081, 2082, 5316, 5317, 5318, 4886, 5319, 5320, 5321], 's_17_19': [1182], 20: [5059, 5171, 5150, 5170, 1976, 1977, 5305, 5304, 5303, 5302, 5301, 5300, 987, 986], 's_17_20': [5151], 28: [2125, 2124, 4707, 4706, 4705, 4704, 4703, 4702, 4701, 4700, 999, 4819], 's_17_28': [1254], 's_17_29': [1318], 35: [4926, 4927, 4928, 4929, 2126, 5035, 5034, 1826], 's_17_35': [1150], 39: [5394, 5110, 2019, 1948, 2020, 4885, 5364, 1902, 1901, 1900], 's_17_39': [1917], 40: [4629, 2112, 2111, 4630, 2108, 1570, 2109, 2110, 4855, 4854, 4853, 4851, 4852], 's_17_40': [5291, 2038], 's_17_41': [4640], 49: [1603, 5393, 5392], 's_17_49': [1483], 's_17_17': [1499], 8: [4661, 2229, 2230, 4914, 4915, 4916], 's_21_8': [2006], 's_21_18': [5065], 's_21_23': [2036], 's_21_34': [5019], 's_21_21': [4988], 4: [5172, 1884, 4477, 1508, 1509, 2337, 2336, 2335, 4797, 4793, 4794, 4796, 4795], 's_23_4': [4478], 's_23_5': [1857], 's_23_9': [4839], 11: [1898, 4522, 4523, 4527, 4526, 4554, 1748, 4524, 4525], 's_23_11': [4553], 's_23_13': [2141], 's_23_20': [5290], 's_23_30': [2216], 's_23_34': [4538], 's_23_36': [4809], 37: [5226, 5227, 1482, 5124, 2289, 2290, 2291, 5123, 2288, 5127, 5225, 5126, 5125], 's_23_37': [2321], 's_23_39': [4720], 42: [5152, 5154, 5155, 5156, 5153, 5157, 4722, 4782, 2261, 2260, 2259], 's_23_42': [5140], 43: [4955, 942, 941, 940, 4403, 4402, 4401, 4400, 938, 939], 's_23_43': [1612], 's_23_23': [4298], 1: [1422, 1421, 1420, 4780, 4779, 4778, 1342, 1343, 1344, 4777], 's_25_1': [4987], 2: [4895, 1812, 5109, 1796, 4896, 4897, 4495, 4494, 1793, 1794, 1795, 4898, 4899], 's_25_2': [1691], 3: [5348, 4599, 1718, 1719, 1720, 5261, 5260, 5259, 1722, 1721], 's_25_3': [5064], 10: [5334, 4626, 1299, 1300, 1663, 1301, 1662, 5243, 5242, 5241, 1242, 1241, 5061], 's_25_10': [1452], 's_25_12': [1107, 5210], 's_25_20': [5074], 26: [5015, 1388, 4582, 4581, 1121, 1119, 1120, 1135, 5060, 1047, 1046, 1045, 4865], 's_25_26': [1001], 's_25_37': [5092], 's_25_40': [1780], 's_25_42': [1556], 46: [4625, 4836, 4835, 1089, 1090, 1105, 4745, 4776, 1061, 1060, 4775], 's_25_46': [5090], 48: [4960, 5245, 4930, 5244, 1842, 1839, 1840, 1841], 's_25_48': [1782], 's_25_25': [1151], 's_27_1': [4356], 's_27_4': [1583], 's_27_8': [4826], 's_27_10': [4551], 's_27_14': [1897], 's_27_15': [1314, 4641], 16: [4388, 1633, 1632, 1631, 1628, 1629, 1630], 's_27_16': [1643], 's_27_18': [1162], 24: [2155, 5111, 2157, 2156], 's_27_24': [2154], 's_27_29': [4431], 32: [5362, 1705, 4942, 5138, 4448, 1763, 1764, 1765, 1542, 1541, 1540, 4943, 4944], 's_27_32': [1702], 's_27_37': [4646], 38: [1690, 985, 1555, 4883, 4565, 4882, 4881, 4880, 4999, 1013, 1014, 1015], 's_27_38': [4520], 's_27_39': [4601], 's_27_43': [1088], 45: [5020, 5021, 2307, 2306, 2305, 2047, 2048, 2049, 4810, 4811], 's_27_45': [4841], 's_27_27': [4446], 's_30_4': [4962], 's_30_8': [4932], 's_30_19': [4721], 's_30_40': [5051], 's_30_42': [2350, 4857], 's_30_30': [4602], 's_34_1': [5017], 's_34_2': [1646], 's_34_3': [4643], 's_34_9': [1736], 's_34_15': [5063], 's_34_18': [4658], 's_34_28': [1749], 's_34_29': [1660], 31: [2274, 4692, 4691, 4690, 4689, 4746, 4747, 1419, 4687, 4688], 's_34_31': [1734], 33: [4567, 1703, 2169, 4490, 1133, 4571, 4570, 4569, 4568, 4416, 4417, 4418, 1568], 's_34_33': [4628], 's_34_34': [4673], 's_41_1': [4536], 's_41_3': [1688], 's_41_4': [1883], 's_41_14': [4510], 's_41_18': [1358], 's_41_29': [1313], 's_41_32': [4493], 's_41_46': [1193], 's_41_41': [1403], 's_47_10': [1257], 's_47_12': [5105], 22: [4912, 4345, 4344, 1435, 1434, 1433, 4447, 1537, 4419, 1687, 4343], 's_47_22': [4807], 's_47_29': [5107], 's_47_32': [5167], 's_47_37': [1227], 's_47_43': [5194], 's_47_46': [1062], 's_47_47': [5089], 's_9_4': [5187], 's_9_10': [1392], 's_9_18': [4735], 's_9_26': [1166, 5045], 's_9_42': [1706], 's_9_48': [4765], 's_9_3': [2142], 's_9_40': [1870], 's_9_15': [1587], 's_9_16': [5168], 's_9_24': [2172], 's_9_32': [4734], 's_9_35': [1827], 's_9_36': [1810], 's_9_37': [2202], 's_9_9': [1137], 's_13_1': [5032], 's_13_10': [1256], 's_13_11': [2348], 's_13_15': [1286], 's_13_24': [2187], 's_13_28': [2349], 's_13_31': [4752], 's_13_37': [4572], 's_13_38': [1510], 's_13_39': [5080], 's_13_46': [1106], 's_13_13': [4497], 's_14_10': [4986], 's_14_28': [1854], 's_14_48': [4600], 's_14_5': [5215], 's_14_8': [2095], 's_14_11': [4555], 's_14_22': [1867], 's_14_45': [4540], 's_14_19': [4480], 's_14_31': [1974], 's_14_37': [1931], 's_14_14': [4390], 's_15_26': [4566], 's_15_29': [1283], 's_15_42': [1602], 's_15_3': [5198], 's_15_12': [1363], 's_15_20': [5288], 's_15_31': [1149], 's_15_36': [1179], 's_15_37': [5108], 's_15_38': [4669], 's_15_46': [1104], 's_15_15': [1059], 's_29_1': [4806], 's_29_4': [4537], 's_29_10': [1298], 's_29_18': [1389], 6: [4656, 5467, 1423, 1554, 1333, 1332, 1331, 4763, 4762, 1329, 1330], 's_29_6': [5166], 's_29_11': [4521], 's_29_12': [1393], 's_29_16': [1645], 's_29_19': [1243], 's_29_38': [1480], 's_29_29': [1093], 's_36_28': [1164], 's_36_6': [5031], 's_36_39': [4945], 's_36_40': [1450], 's_36_12': [4805], 's_36_16': [4808], 's_36_35': [1255], 's_36_36': [1539], 's_5_2': [1813], 's_5_4': [2382], 's_5_10': [5139], 's_5_48': [5246], 's_5_12': [1768], 's_5_39': [1828], 's_5_40': [2127], 's_5_45': [5247], 's_5_5': [5350], 's_12_18': [5410], 's_12_39': [5455], 's_12_49': [5408], 's_12_33': [4505], 's_12_16': [1648], 's_12_38': [4760], 's_12_43': [1072], 's_12_46': [5120], 's_12_12': [1183], 's_18_1': [4597], 's_18_6': [1404], 's_18_11': [1733], 's_18_19': [2008], 's_18_20': [2007], 's_18_28': [1809], 's_18_38': [1028], 's_18_40': [5200], 's_18_45': [4675], 's_18_46': [4535], 's_18_48': [4750], 's_18_18': [4549], 's_19_28': [4736], 's_19_3': [2067], 's_19_6': [1438], 's_19_8': [4660], 's_19_40': [5066], 44: [4941, 1273, 1270, 1271, 1272], 's_19_44': [5331], 's_19_32': [1453], 's_19_33': [4556], 's_19_37': [1152], 's_19_49': [1753], 's_19_19': [2077], 's_20_4': [5306, 5307], 's_20_26': [5285], 's_20_39': [1858], 's_20_44': [5286], 's_20_45': [2292], 's_20_35': [2066], 's_20_38': [5029, 911], 's_20_20': [5254], 's_28_1': [4686], 's_28_26': [4730], 's_28_8': [4901], 's_28_40': [1944], 's_28_42': [2319], 's_28_43': [4654], 's_28_45': [4751], 's_28_28': [2394], 's_35_26': [1136], 's_35_8': [4990, 4991], 's_35_22': [1481], 's_35_40': [5081], 's_35_24': [5036], 's_35_32': [1390], 's_35_38': [1225], 's_35_37': [2096], 's_35_35': [4925, 956], 's_39_2': [5199], 's_39_8': [2021], 's_39_31': [1899], 's_39_33': [4586], 's_39_49': [5363], 's_39_39': [5395], 's_40_2': [4913], 's_40_42': [5141], 's_40_11': [4645, 4644], 's_40_24': [4931], 's_40_31': [1824], 's_40_33': [4541], 's_40_37': [4631], 's_40_44': [1240], 's_40_40': [2113], 's_49_10': [5333], 's_49_3': [1618], 's_49_6': [5391], 's_49_16': [5423], 's_49_49': [1528], 's_8_2': [4900], 's_8_48': [1945], 's_8_3': [1735], 's_8_8': [4662], 's_4_1': [4781], 's_4_2': [4674], 's_4_6': [4672], 's_4_24': [5112], 's_4_31': [2094], 's_4_33': [1507], 's_4_42': [5006, 5007], 's_4_48': [4659], 's_4_4': [5037], 's_11_2': [2033], 's_11_26': [1418], 's_11_48': [1838], 's_11_22': [1747], 's_11_32': [1613], 's_11_33': [1913], 's_11_37': [2303], 's_11_11': [2273], 's_37_26': [1122], 's_37_42': [4887], 's_37_48': [2022], 's_37_45': [5067], 's_37_31': [2304], 's_37_37': [4617], 's_42_1': [1437], 's_42_6': [1346], 's_42_16': [1647], 's_42_31': [2409], 's_42_42': [4783], 's_43_22': [1582], 's_43_16': [1522], 's_43_38': [4639], 's_43_43': [4354], 's_1_2': [1615], 's_1_10': [4716], 's_1_26': [1328], 's_1_48': [1975], 's_1_1': [1341], 's_2_3': [1779], 's_2_6': [4764], 's_2_22': [1792], 's_2_26': [4910], 's_2_44': [4911], 's_2_45': [2063], 's_2_2': [1943], 's_3_48': [1872], 's_3_24': [5276], 's_3_3': [5262], 's_10_26': [4956], 's_10_32': [1557], 's_10_48': [1737], 's_10_10': [1664], 's_26_33': [4491], 's_26_44': [4761], 's_26_26': [5014], 's_46_6': [4655], 's_46_44': [1165], 's_46_31': [1224], 's_46_38': [4685], 's_46_46': [4744], 's_48_33': [4585], 's_48_48': [1797], 's_16_6': [4748], 's_16_22': [1627], 's_16_33': [4433], 's_16_32': [4868], 's_16_16': [1634], 's_24_45': [5216], 's_24_24': [5201], 's_32_6': [1345], 's_32_22': [1717], 's_32_44': [5361], 's_32_38': [4884], 's_32_32': [5347], 's_38_6': [4866], 's_38_22': [4867], 's_38_44': [4940], 's_38_38': [4564], 's_45_22': [2062], 's_45_45': [5277], 's_31_6': [4657], 's_31_44': [1285], 's_31_33': [2034], 's_31_31': [2184], 's_33_22': [1448], 's_33_33': [1132], 's_22_22': [2002], 's_6_6': [1424], 's_44_44': [1274]}, {0: [1207, 1208, 1209, 1210, 4997, 4998, 4999, 5000, 1211], 7: [477, 1165, 1166, 1167, 5267, 5268, 5269, 5270], 's_0_7': [4956], 17: [928, 816, 817, 818, 819, 5404, 5403, 5402, 568, 567, 566, 565, 4804, 4803, 4802], 's_0_17': [551], 21: [4263, 4265, 4264], 's_0_21': [1222], 23: [1454, 758, 757, 5015, 5016, 5017, 4204, 4205, 4206, 4207, 1447, 1448, 1449, 1450, 5014, 1451, 1452, 1453], 's_0_23': [5030], 25: [4597, 1388, 1389, 1390, 5120, 5121, 5122, 5108, 5107, 1391], 's_0_25': [5001], 27: [4941, 4789, 895, 5508, 5522, 643, 642, 4940, 4832, 641, 4939, 4938, 4942, 640], 's_0_27': [4926], 30: [5028, 807, 805, 5013, 806], 's_0_30': [761], 34: [4310, 4232, 636, 4233, 4234, 4235, 4250, 1058, 1056, 1057], 's_0_34': [4280], 41: [4698, 654, 5012, 4758, 597, 596, 4817, 595], 's_0_41': [686], 47: [745, 5193, 4968, 746, 747, 5390, 5389, 5388, 748], 's_0_47': [731], 's_0_0': [776], 9: [5057, 1313, 4371, 4370, 4369, 4368, 4367, 508, 502, 503, 507, 506, 505, 504], 's_7_9': [5191], 13: [1198, 5240, 1197, 4732, 1480, 5241, 5242, 1481, 1482], 's_7_13': [5195], 14: [4549, 4972, 4773, 4774, 1360, 1105, 4836, 4835, 924, 925, 4834], 's_7_14': [4971], 15: [1362, 5346, 441, 442, 443, 444, 445, 446, 447, 5327, 5328, 5329, 5330, 5331, 987, 1243], 's_7_15': [1108], 's_7_25': [5106], 29: [608, 487, 488, 489, 4682, 5161, 687, 673, 672, 5162, 611, 610, 609], 's_7_29': [492], 36: [997, 5132, 5477, 4416, 4415, 4414, 4413, 538, 537, 536, 535, 534, 533, 4412], 's_7_36': [5252], 's_7_7': [5266], 5: [1060, 4775, 982, 4518, 4519, 984, 983], 's_17_5': [1045], 's_17_9': [4967], 12: [5463, 5432, 1030, 1031, 1032, 1033, 988, 613, 5478, 5479, 5480], 's_17_12': [898], 's_17_14': [4699], 's_17_15': [718], 18: [849, 4729, 4727, 520, 5209, 519, 848, 5207, 522, 5208, 4728, 4715, 4714, 4716, 521, 847], 's_17_18': [4219, 846], 19: [5317, 5316, 5314, 5074, 4787, 4788, 5315, 700, 4833, 835, 837, 836], 's_17_19': [760], 20: [882, 883, 1496, 5153, 973, 5419, 5420, 5421, 1393, 1497, 1498, 5422], 's_17_20': [868], 28: [1087, 4293, 4294, 4295, 4973, 1423, 1422, 5182, 1556, 1555, 1554, 1553, 1552, 4297, 4296], 's_17_28': [4339, 922, 4279], 's_17_29': [4892], 35: [999, 4341, 5075, 1224, 1237, 1138, 1137, 1136, 1135, 1238, 1239, 4745, 4746], 's_17_35': [5405], 39: [808, 4458, 5496, 5495, 5494, 5493, 5492, 404, 403, 713, 4578, 4577, 399, 400, 401, 402], 's_17_39': [463], 40: [1088, 4806, 5299, 5300, 5301, 1257, 1256, 4430, 4431, 1253, 1254, 1255], 's_17_40': [778], 's_17_41': [598], 49: [656, 659, 5313, 658, 657], 's_17_49': [583], 's_17_17': [4113], 8: [4924, 790, 789, 4670, 4669, 4668, 727, 728, 729], 's_21_8': [4278], 's_21_18': [862], 's_21_23': [786], 's_21_34': [742], 's_21_21': [1191], 4: [4323, 4608, 716, 715, 1511, 1510, 1509, 1508, 1507, 4327, 4326, 4325, 4324, 832, 714, 4638, 833], 's_23_4': [4338], 's_23_5': [981], 's_23_9': [4402], 11: [4622, 4623, 4624, 4626, 4760, 4970, 1076, 1075, 1404, 1074, 4625], 's_23_11': [956], 's_23_13': [5197], 's_23_20': [5467], 's_23_30': [5029], 's_23_34': [4115, 1176], 's_23_36': [4417], 37: [1012, 4460, 940, 5194, 4849, 942, 5239, 912, 4459, 908, 909, 911, 910], 's_23_37': [926], 's_23_39': [773], 42: [5356, 5357, 5358, 822, 5063, 5062, 5061, 5060, 5059, 821], 's_23_42': [1316], 43: [5448, 5452, 5449, 5450, 1228, 5451], 's_23_43': [1469], 's_23_23': [1431], 1: [804, 4653, 4793, 759, 1644, 4581, 4580, 4579, 4683, 1645, 4582, 4583, 1646, 1629, 1630], 's_25_1': [4598], 2: [4474, 5134, 5135, 5137, 1376, 1375, 4700, 4701, 1299, 4473, 4612, 4475, 5136, 4476, 1374, 1373], 's_25_2': [1181], 3: [491, 5102, 4820, 1147, 1148, 1149, 1150, 4985, 5103, 5104, 5105, 1061], 's_25_3': [4986], 10: [4847, 1465, 1464, 5027, 581, 4537, 4536, 4535, 580, 579, 4532, 4533, 4534], 's_25_10': [1314], 's_25_12': [1046], 's_25_20': [5123], 26: [4627, 4357, 1372, 4461, 4356, 5257, 1437, 1436, 1435, 4462, 1434, 1433], 's_25_26': [4747], 's_25_37': [5119], 's_25_40': [4432], 's_25_42': [1586], 46: [5221, 5222, 5223, 5226, 5225, 957, 5224], 's_25_46': [1287], 48: [879, 4547, 594, 4593, 1269, 4596, 4595, 4594], 's_25_48': [4656], 's_25_25': [1571], 's_27_1': [774, 775], 's_27_4': [5088], 's_27_8': [834], 's_27_10': [4982], 's_27_14': [4790], 's_27_15': [4831], 16: [1304, 5601, 370, 371, 5600, 5447, 569, 372, 373, 374, 5596, 5599, 5598, 5597], 's_27_16': [689], 's_27_18': [894], 24: [4822, 4821, 1342, 1343, 1345, 4731, 1344], 's_27_24': [1240], 's_27_29': [5298], 32: [295, 1120, 431, 430, 4880, 971, 970, 4879, 4878, 4877, 4876], 's_27_32': [550], 's_27_37': [4894], 38: [779, 1227, 1392, 5181, 1196, 5433, 703, 702, 5177, 5180, 5179, 5178], 's_27_38': [5509], 's_27_39': [524], 's_27_43': [749], 45: [1300, 1301, 1466, 1015, 4898, 4897, 4895, 4896], 's_27_45': [4927], 's_27_27': [704], 's_30_4': [4908], 's_30_8': [4954], 's_30_19': [4848], 's_30_40': [792], 's_30_42': [851], 's_30_30': [5284], 's_34_1': [4490, 1193], 's_34_2': [1073], 's_34_3': [4520], 's_34_9': [4262, 4261], 's_34_15': [4218, 4217], 's_34_18': [4249], 's_34_28': [937], 's_34_29': [4247], 31: [5196, 1332, 1331, 1329, 1328, 1330, 4506, 279, 278, 4501, 4502, 4503, 4504, 4505], 's_34_31': [1117, 1118], 33: [4311, 5435, 1154, 1153, 1152, 1151, 5045, 5046, 1286, 1285, 1284, 1283, 1282], 's_34_33': [4251], 's_34_34': [471, 470], 's_41_1': [699], 's_41_3': [5087], 's_41_4': [669], 's_41_14': [4759], 's_41_18': [4862], 's_41_29': [4712], 's_41_32': [670], 's_41_46': [582], 's_41_41': [4907], 's_47_10': [744], 's_47_12': [5374], 22: [1089, 1094, 1090, 1091, 1093, 1092], 's_47_22': [5375], 's_47_29': [4953], 's_47_32': [625], 's_47_37': [867], 's_47_43': [853], 's_47_46': [762], 's_47_47': [5373], 's_9_4': [1312], 's_9_10': [4697], 's_9_18': [5206], 's_9_26': [4387], 's_9_42': [5341], 's_9_48': [593], 's_9_3': [4996], 's_9_40': [1103], 's_9_15': [4757], 's_9_16': [493], 's_9_24': [1327], 's_9_32': [4981], 's_9_35': [4491], 's_9_36': [532], 's_9_37': [1133], 's_9_9': [622], 's_13_1': [4733], 's_13_10': [1479], 's_13_11': [1358, 1359], 's_13_15': [5406], 's_13_24': [1495], 's_13_28': [4763], 's_13_31': [5256], 's_13_37': [1047], 's_13_38': [5271], 's_13_39': [1182, 1183], 's_13_46': [1122], 's_13_13': [5540], 's_14_10': [4882], 's_14_28': [4837], 's_14_48': [4639], 's_14_5': [923], 's_14_8': [954], 's_14_11': [1106], 's_14_22': [4550], 's_14_45': [1405], 's_14_19': [624], 's_14_31': [4957], 's_14_37': [4850], 's_14_14': [1406], 's_15_26': [5272], 's_15_29': [4742], 's_15_42': [733], 's_15_3': [5011], 's_15_12': [5359], 's_15_20': [5391], 's_15_31': [4696], 's_15_36': [427], 's_15_37': [913], 's_15_38': [688], 's_15_46': [1242], 's_15_15': [4336], 's_29_1': [4652], 's_29_4': [4743], 's_29_10': [671], 's_29_18': [4667], 6: [5044, 340, 341, 280, 281, 296, 297, 5041, 626, 791, 5043, 5042], 's_29_6': [5160], 's_29_11': [4621], 's_29_12': [5387], 's_29_16': [387], 's_29_19': [459], 's_29_38': [5253], 's_29_29': [549, 548], 's_36_28': [877, 878], 's_36_6': [5131], 's_36_39': [4457], 's_36_40': [4385], 's_36_12': [554], 's_36_16': [419], 's_36_35': [1177], 's_36_36': [5297], 's_5_2': [1028, 4565], 's_5_4': [638], 's_5_10': [968], 's_5_48': [1059], 's_5_12': [4819], 's_5_39': [683], 's_5_40': [4400], 's_5_45': [4910], 's_5_5': [4309], 's_12_18': [523, 5417, 478], 's_12_39': [959], 's_12_49': [5537], 's_12_33': [5255], 's_12_16': [989], 's_12_38': [5464], 's_12_43': [1078], 's_12_46': [612], 's_12_12': [614], 's_18_1': [4713], 's_18_6': [5146, 5147], 's_18_11': [969], 's_18_19': [4772], 's_18_20': [972], 's_18_28': [4852, 4851, 1270], 's_18_38': [732], 's_18_40': [4776, 1164, 1163], 's_18_45': [1014], 's_18_46': [1002], 's_18_48': [4744], 's_18_18': [4726], 's_19_28': [1438], 's_19_3': [490], 's_19_6': [429, 4801], 's_19_8': [4818], 's_19_40': [1017], 44: [1016, 5093, 5092, 5091, 5089, 5090], 's_19_44': [896], 's_19_32': [865], 's_19_33': [1063], 's_19_37': [4864], 's_19_49': [5073], 's_19_19': [5332], 's_20_4': [5138], 's_20_26': [5167], 's_20_39': [1003], 's_20_44': [1647], 's_20_45': [5032], 's_20_35': [1123], 's_20_38': [5434], 's_20_20': [1572], 's_28_1': [4688], 's_28_26': [1432], 's_28_8': [4308], 's_28_40': [1192], 's_28_42': [1541], 's_28_43': [5437], 's_28_45': [1525], 's_28_28': [1587], 's_35_26': [4342], 's_35_8': [1179], 's_35_22': [5210], 's_35_40': [5151], 's_35_24': [4686], 's_35_32': [1121], 's_35_38': [5286], 's_35_37': [955], 's_35_35': [4266], 's_39_2': [743], 's_39_8': [4548], 's_39_31': [458], 's_39_33': [1168], 's_39_49': [5312], 's_39_39': [5566], 's_40_2': [897], 's_40_42': [763], 's_40_11': [4805], 's_40_24': [4881], 's_40_31': [1223, 4521], 's_40_33': [4911], 's_40_37': [943], 's_40_44': [1241], 's_40_40': [4807], 's_49_10': [655], 's_49_3': [5118], 's_49_6': [5148], 's_49_16': [644], 's_49_49': [5658], 's_8_2': [1044, 4654], 's_8_48': [4563], 's_8_3': [1194], 's_8_8': [4398], 's_4_1': [4928], 's_4_2': [4867], 's_4_6': [5058], 's_4_24': [1524], 's_4_31': [4507], 's_4_33': [1267], 's_4_42': [5047], 's_4_48': [4637], 's_4_4': [1522], 's_11_2': [1013], 's_11_26': [4702], 's_11_48': [939], 's_11_22': [4925], 's_11_32': [4761], 's_11_33': [4641], 's_11_37': [4969], 's_11_11': [1178], 's_37_26': [4355], 's_37_42': [941], 's_37_48': [4609], 's_37_45': [4984], 's_37_31': [938], 's_37_37': [4384], 's_42_1': [1631], 's_42_6': [5163], 's_42_16': [388], 's_42_31': [1346], 's_42_42': [823], 's_43_22': [5360], 's_43_16': [1229], 's_43_38': [793], 's_43_43': [1319], 's_1_2': [998], 's_1_10': [1418], 's_1_26': [1583], 's_1_48': [4684], 's_1_1': [1643], 's_2_3': [4685], 's_2_6': [5133], 's_2_22': [5150], 's_2_26': [4912], 's_2_44': [1361], 's_2_45': [1467], 's_2_2': [777], 's_3_48': [4611], 's_3_24': [4730], 's_3_3': [4640], 's_10_26': [4642], 's_10_32': [5026], 's_10_48': [1119], 's_10_10': [4531], 's_26_33': [1268], 's_26_44': [1421], 's_26_26': [1357], 's_46_6': [627], 's_46_44': [1272], 's_46_31': [1317], 's_46_38': [1062], 's_46_46': [5227], 's_48_33': [4671], 's_48_48': [4551], 's_16_6': [5236], 's_16_22': [1109], 's_16_33': [1169], 's_16_32': [4891], 's_16_16': [299], 's_24_45': [1570], 's_24_24': [1539], 's_32_6': [4845], 's_32_22': [4955], 's_32_44': [986], 's_32_38': [5176], 's_32_32': [475], 's_38_6': [701], 's_38_22': [1107], 's_38_44': [927], 's_38_38': [764], 's_45_22': [4865], 's_45_45': [4899], 's_31_6': [4771], 's_31_44': [5076], 's_31_33': [5031], 's_31_31': [4485], 's_33_22': [5555], 's_33_33': [5705], 's_22_22': [5525], 's_6_6': [326, 327, 5190], 's_44_44': [5094]}, {0: [996, 995, 3723, 4055, 4054, 785, 781, 782, 783, 784], 7: [758, 757, 753, 754, 756, 4429, 755], 's_0_7': [3648], 17: [1160, 3980, 392, 3979, 3978, 3982, 394, 395, 3976, 393, 3981, 3977], 's_0_17': [3963], 21: [709, 3857, 3858], 's_0_21': [3859], 23: [3949, 4023, 3183, 691, 692, 1207, 4280, 4279, 4278, 697, 696, 693, 694, 3948, 695], 's_0_23': [4053], 25: [1205, 1296, 1295, 4178, 4177, 1416, 1415, 3889, 3769, 994, 3890, 3891, 3892], 's_0_25': [3768], 27: [3514, 1247, 4233, 4234, 4235, 3516, 1248, 1249, 1250, 1251, 1252, 3515, 4236], 's_0_27': [4056], 30: [4024, 4025, 1100, 1101], 's_0_30': [921], 34: [1189, 1188, 501, 453, 648, 500, 499, 498, 3662, 3666, 3665, 3664, 3663], 's_0_34': [769], 41: [3713, 4043, 4041, 1595, 1594, 1548, 4042, 4040], 's_0_41': [1010], 47: [841, 3394, 3288, 3290, 3289, 933, 932], 's_0_47': [3273], 's_0_0': [846], 9: [3425, 4354, 4353, 3424, 812, 3543, 3542, 843, 528, 4352, 532, 531, 530, 529], 's_7_9': [817], 13: [1263, 4431, 3679, 3680, 3681, 1338, 1192, 4326, 1342, 1264, 3786, 1341, 1340, 1339], 's_7_13': [4430], 14: [4173, 682, 681, 680, 980, 979, 3799, 678, 679, 3798], 's_7_14': [4158], 15: [4191, 3484, 4388, 4387, 1327, 1326, 1325, 1324, 919, 1323, 3606, 918, 3604, 3605], 's_7_15': [3694], 's_7_25': [770], 29: [1283, 1282, 3467, 1281, 3468, 1280, 3469, 1279, 3470, 3471, 1278], 's_7_29': [3453], 36: [1053, 1052, 3350, 768, 767, 3349, 3348, 3347, 3346, 302, 303, 304, 305], 's_7_36': [3558], 's_7_7': [4503], 5: [3227, 511, 381, 3527, 3722, 380, 3828, 512, 513, 3826, 3827, 514], 's_17_5': [408], 's_17_9': [3512], 12: [3330, 3331, 3336, 3335, 874, 873, 3286, 872, 3334, 3333, 3332, 422, 421], 's_17_12': [3302], 's_17_14': [665], 's_17_15': [3966], 18: [1461, 1462, 437, 438, 439, 440, 441, 442, 4397, 4398, 4399, 4400, 4401, 4402, 1463], 's_17_18': [3796], 19: [3810, 410, 3811</t>
+          <t>[60.90292286872864, 60.367132902145386, 60.10868048667908, 25.12303638458252, 60.63820743560791, 39.3959641456604, 57.96503281593323, 43.36915326118469, 60.94960594177246, 60.08281373977661, 60.574636936187744, 52.96138072013855, 61.03238558769226, 60.22406792640686, 26.304267406463623, 50.62888979911804, 60.57561755180359, 60.59284472465515, 55.742136001586914, 57.81824588775635, 52.14940571784973, 37.797128677368164, 36.5156307220459, 60.5747287273407, 60.25340676307678, 60.95748543739319, 60.61593985557556, 37.74830508232117, 50.511730670928955, 60.72650909423828, 45.47265076637268, 60.27928876876831, 60.38705897331238, 60.64099144935608, 60.42351031303406, 57.7498414516449, 46.746829986572266, 32.76058650016785, 42.702500343322754, 53.54858756065369, 60.373024463653564, 38.36473536491394, 52.54418325424194, 60.30771565437317, 55.95404314994812, 42.97668218612671, 60.508172273635864, 60.15338325500488, 51.53297257423401, 61.01070976257324, 57.544859647750854, 48.30012226104736, 40.512839555740356, 46.997708320617676, 37.735970973968506, 60.60769605636597, 60.25596046447754, 41.31668210029602, 60.84594011306763, 49.320152044296265, 61.25083541870117, 50.42956733703613, 60.82823467254639, 30.68811345100403, 34.09960103034973, 46.9245285987854, 60.722832918167114, 35.107173442840576, 58.35650897026062, 49.667221784591675, 44.1021728515625, 43.784549951553345, 60.952670097351074, 55.81160545349121, 60.48659610748291, 30.967498779296875, 60.45810508728027, 61.12547969818115, 56.63964247703552, 60.36851930618286, 25.50247073173523, 60.555126428604126, 60.54286026954651, 56.10061836242676, 60.12129616737366, 60.99593663215637, 38.463398694992065, 61.200695753097534, 60.825417041778564, 60.18255400657654, 41.327094078063965, 59.95753026008606, 60.3663809299469, 24.607553958892822, 54.57161092758179, 53.69917130470276, 43.38887310028076, 54.78499507904053, 60.23981046676636, 35.256892919540405]</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>[{0: [2510, 3899, 3897, 3898], 7: [2555, 2553, 2554], 17: [2507, 3838, 2508, 2509], 21: [2330, 3882], 23: [2270, 3658, 3657, 2269, 2268], 25: [3869, 2614, 2612, 2613], 27: [2358, 2359, 2254, 2404, 3792], 30: [3988, 3987], 34: [2492, 2493, 3883, 2495, 2494], 41: [2599, 2597, 2598], 47: [3747, 3746, 3476, 2210, 2209, 2208], 9: [3764, 2525, 2523, 3763, 2524], 13: [3628, 2538, 2540, 2539], 14: [2345, 2344, 3733, 3732], 15: [2584, 3612, 3613, 2583], 29: [3507, 3509, 2389, 2388, 3508], 36: [3643, 2447, 2448], 5: [3854, 3853, 3852, 2298, 2299], 12: [3687, 2313, 3403, 3402, 2312], 18: [2329, 2328, 3553, 3552], 19: [2570, 2568, 2569], 20: [3704, 2253, 3702, 3703], 28: [3762, 3793, 2449], 35: [3956, 2195, 2194, 2193, 3492, 3493], 39: [3674, 3672, 3673], 40: [3824, 2432, 3823, 2435, 2433, 2434], 49: [3748, 2627, 2628], 8: [2374, 2660, 3958, 3957, 2375], 4: [3583, 2285, 3582, 2343, 2284, 2283, 3537], 11: [3776, 2645, 2644, 3778, 2164, 3777], 37: [2720, 2735, 3929, 3926, 3927, 3928], 42: [2480, 2478, 3868, 2479], 43: [2223, 3761, 3731, 2179], 1: [3809, 3807, 3808], 2: [3972, 2688, 2689, 2690, 3974, 3973], 3: [2630, 2629, 3884], 10: [2419, 3689, 3688, 2418], 26: [3494, 3614, 3794, 2719, 2718], 46: [3479, 2582, 3477, 3478], 48: [2658, 3839, 2659], 16: [2178, 2237, 3568, 3567, 3566], 24: [3911, 3913, 3912], 32: [3463, 2163, 2417, 3462, 3461], 38: [2373, 3626, 3627], 45: [2315, 2314], 31: [2462, 2465, 2463, 2464], 33: [3597, 2643, 3598], 22: [3596, 3719, 3718, 2238, 3717], 6: [2222, 3522, 3524, 3523], 44: [2674, 2673, 3539, 3538]}, {0: [1963, 1962], 7: [5186, 2112, 5185], 17: [5503, 2428, 5425, 5427, 5426], 21: [1947, 5155], 23: [5171, 1782, 5170, 5169], 25: [5276, 5275], 27: [5574, 1859, 5472, 5471, 5470], 30: [5096, 2096, 1961, 5020], 34: [1888, 5290, 1887, 5215, 5214], 41: [2353, 5320, 5322, 5321], 47: [2159, 5604, 1964, 5606, 5605], 9: [2083, 2081, 5231, 5232, 2082], 13: [2202, 5560, 5561, 2203, 2204], 14: [2127, 2129, 2128], 15: [2113, 5364, 5365, 5366], 29: [1844, 1977, 1978, 5485], 36: [2309, 2307, 2308], 5: [5247, 2008, 2007, 5246, 5245], 12: [5622, 5621, 1904, 5620, 1902, 1903], 18: [5456, 1932, 5455, 1933], 19: [2219, 2217, 5350, 5351, 2218], 20: [2039, 5575, 1992, 1993, 1994], 28: [1934, 5502, 5500, 5501], 35: [2084, 2099, 5651, 5547, 5546, 2144], 39: [5576, 2294, 2292, 2293], 40: [2097, 5487, 5486, 2098], 49: [2414, 5217, 5262, 5352, 2413, 2412], 8: [2324, 2323, 2322, 5157, 5156], 4: [1858, 5126, 1843, 1842, 5125], 11: [1783, 5379, 5381, 5380], 37: [5545, 2022, 2023, 2024], 42: [2053, 2051, 5230, 2052], 43: [5244, 1872, 5515, 1873], 1: [2069, 2066, 5200, 2068, 2067], 2: [5291, 2172, 2174, 2173], 3: [2187, 2247, 5216], 10: [2158, 5260, 2157, 5261], 26: [2188, 5516, 2189], 46: [5559, 1919, 1917, 1918], 48: [2141, 5141, 2143, 2142], 16: [5439, 2248, 5440, 5442, 5441], 24: [5592, 5127, 2367, 2369, 5292, 2368], 32: [2234, 2232, 2233], 38: [1948, 1979, 1949, 5636, 5635], 45: [2009, 5591, 5590], 31: [5307, 2038, 5305, 5306], 33: [5394, 5396, 5395], 22: [5529, 2263, 5530, 5531], 6: [5338, 5335, 2338, 5337, 5336], 44: [5410, 5411]}, {0: [1792, 4299, 1598, 4568, 1597, 4298], 7: [4703, 4868, 1630, 1628, 1629], 17: [1538, 4523, 4524, 4526, 4525], 21: [4313, 1837, 4314], 23: [1687, 1688, 4690, 1944, 4615, 4614], 25: [2005, 1644, 1645, 4853, 4854, 4855], 27: [4496, 2123, 4495, 4493, 4494], 30: [4718, 4613, 1600, 1599], 34: [4705, 4661, 1942, 4360, 4660, 2019, 2018], 41: [2048, 4344, 4345, 2047, 1958, 4421, 4465], 47: [4448, 1614, 1612, 1613], 9: [4373, 2035, 2034, 4374, 4375, 2033], 13: [2215, 1855, 4736, 4869, 4870, 2020, 4735], 14: [2228, 4511, 4508, 4509, 4510], 15: [2063, 2124, 4645, 4643, 4644], 29: [4587, 4583, 4584, 4585, 4586], 36: [1747, 4704, 1748, 1749], 5: [1884, 1883], 12: [1780, 4733, 1778, 4734, 1779], 18: [4478, 4481, 4480, 4479, 1928, 1927], 19: [1912, 1913, 4823, 4824, 1914], 20: [4538, 4570, 1703, 4569], 28: [4434, 4435, 4436, 2154, 2153], 35: [4674, 1823, 1824], 39: [1870, 1868, 1869], 40: [2138, 2139, 1825, 4721, 4719, 4720], 49: [1583, 1584, 4689, 1539, 4822, 4688], 8: [1915, 4838, 4839, 1840, 1838, 1839], 4: [4630, 1898, 4628, 4629], 11: [4781, 4749, 2093, 2094, 4750, 4751], 37: [2110, 4691, 4449, 4450, 2109, 2108], 42: [4601, 4598, 4599, 4600], 43: [1777, 1988, 4388, 4389, 4390], 1: [4856, 4631, 2185, 4706, 2183, 2184], 2: [2049, 1794, 4766, 4764, 4765], 3: [4840, 4793, 4794, 4795, 1959, 1960], 10: [4553, 4554, 2214, 4556, 4555], 26: [4676, 2004, 4675], 46: [1735, 4658, 1732, 1733, 1734], 48: [2078, 2079, 4809, 4810], 16: [1660, 4673, 1658, 1659], 24: [1808, 1810, 1809], 32: [1719, 1717, 4404, 1718], 38: [4659, 1854, 4359, 1853], 45: [4539, 1793], 31: [4915, 1974, 1973, 4914, 1975], 33: [1989, 1990, 4779, 1899, 4780], 22: [4358, 4419, 1675, 1674, 1673], 6: [1762, 1765, 1764, 1763], 44: [2170, 2169, 4463, 4541, 4540, 4464, 1943]}, {0: [2202, 2382, 5114, 5111, 5112, 5113], 7: [2547, 2546, 5069, 5068], 17: [5232, 4828, 4827, 2397, 2396, 2395], 21: [2229, 2230, 5127, 2231], 23: [4978, 5052, 5051, 2380, 2381], 25: [2649, 2651, 2650], 27: [2666, 2667, 4646, 4647, 4648, 2665, 2664], 30: [4901, 4706, 2109, 2201, 4736, 2200], 34: [5083, 2516, 2532, 2515, 5128], 41: [5233, 2561, 2562], 47: [4961, 2140, 5096, 2141], 9: [2426, 5158, 5159, 2712, 2709, 2710, 2711], 13: [5007, 2634, 5008, 2635], 14: [2472, 2469, 4857, 2471, 2470], 15: [5129, 4829, 2679, 4874, 2681, 2680], 29: [5099, 2576, 2577, 5097, 5098], 36: [2440, 4919, 4917, 4918], 5: [5053, 2529, 2531, 2530], 12: [4843, 4844, 4841, 2336, 2335, 4842], 18: [2724, 5142, 5143, 2725, 2726, 2727, 5144], 19: [2319, 4797, 2322, 2321, 2320], 20: [4798, 4634, 4633, 2500, 2499], 28: [4722, 2514, 2439, 4724, 4723], 35: [2394, 2275, 2274, 4619, 2273, 4617, 4618], 39: [2366, 4663, 4662, 2365, 2364], 40: [2425, 4769, 4707, 4768, 2424], 49: [2367, 2411, 5082], 8: [4754, 4753, 4752], 4: [4904, 4902, 2589, 2590, 4903], 11: [2155, 4931, 4934, 4933, 4932], 37: [2125, 4889, 4886, 4887, 2545, 4888], 42: [4739, 4737, 4738], 43: [4977, 2214, 2216, 4721, 4826, 2215], 1: [2606, 4979, 2604, 2605], 2: [4993, 4992, 2456, 2454, 4873, 2455], 3: [5037, 5038, 2694, 2695, 2696, 5039], 10: [2486, 5021, 5023, 5022], 26: [2485, 4709, 4708, 2484], 46: [2410, 4964, 4962, 4963], 48: [4858, 2621, 2619, 2620], 16: [2289, 2290, 5067, 2291], 24: [2693, 2423, 4573, 2633, 2588, 4574], 32: [5174, 5173, 4991, 2245, 2246, 5171, 5172], 38: [4947, 4949, 4948], 45: [2453, 2544, 4604, 4603, 4602], 31: [4782, 2409, 4784, 4783], 33: [4811, 4813, 4812], 22: [4872, 2306, 2304, 4856, 2305], 6: [2352, 2350, 2351], 44: [2260, 4693, 4692, 2259]}, {0: [1287, 746, 5121, 5120, 747, 5118, 5119], 7: [1196, 1198, 1197], 17: [791, 792, 5375, 5374, 5373, 793], 21: [5193], 23: [5194, 1033, 1031, 1032], 25: [1288, 5299, 1017, 5300, 5301], 27: [5464, 5465, 1076, 1078, 1077], 30: [1000, 701, 970, 4999, 4998], 34: [5420, 5419, 821, 822, 823], 41: [762, 5208, 5210, 5209], 47: [1241, 5106], 9: [1047, 5178, 5180, 5179], 13: [5358, 5359, 5360], 14: [5314, 763, 5481, 5480, 5479, 764], 15: [1106, 1107, 5389, 5390, 1108], 29: [1153, 5345, 1150, 1151, 1152], 36: [5241, 5239, 5240], 5: [5525, 1034, 854, 5524, 5523], 12: [1168, 1166, 1167], 18: [5451, 717, 718, 5450, 5448, 5449], 19: [881, 4969, 1063, 1062, 1061, 4970], 20: [5406, 837, 838, 5405, 5404], 28: [5074, 914, 913, 912], 35: [5223, 5225, 5224], 39: [5331, 5330, 988, 986, 987], 40: [5013, 869, 868, 866, 5284, 867], 49: [5028, 5030, 5029], 8: [702, 5270, 5269, 5268], 4: [1001, 5255, 1003, 1002], 11: [5285, 1094, 1092, 1093], 37: [807, 1046, 5105, 806, 5104], 42: [1016, 5015, 911, 5014], 43: [1302, 5075, 5076], 1: [896, 5329, 5344, 897, 898], 2: [884, 5435, 882, 5434, 883], 3: [5149, 928, 926, 927], 10: [4956, 4955, 4954, 853, 852, 851], 26: [5164, 941, 5089, 943, 942], 46: [5361, 5466, 5391, 5211, 1242, 1243], 48: [973, 971, 5254, 972], 16: [5286, 4985, 5091, 1212, 1211], 24: [5495, 5494, 779, 777, 778], 32: [1121, 5090, 1122], 38: [5226, 5195, 1228, 1227], 45: [808, 5509], 31: [5059, 1138, 1137, 1136, 1139, 5060], 33: [956, 1091, 5045, 5044], 22: [5510, 1272, 5151, 5150, 959, 958, 957], 6: [1048, 1258, 1123, 5315, 1181, 1182, 5316], 44: [836, 5136, 5134, 5135]}, {0: [804, 4668], 7: [880, 4773, 4775, 4774], 17: [624, 548, 549, 4699, 4698, 4697], 21: [4759, 4758], 23: [864, 863, 4415, 4413, 4414], 25: [4489, 4669, 967, 968, 969], 27: [4683, 760, 757, 758, 759], 30: [4652, 4653], 34: [4715, 4714, 698, 699, 789, 4713], 41: [4593, 774, 4594, 4595, 998], 47: [4323, 803, 802, 801], 9: [877, 879, 878], 13: [4235, 952, 955, 954, 953], 14: [4547, 578, 579, 654, 4667], 15: [938, 4803, 819, 4684, 939], 29: [4367, 727, 728, 4368, 730, 729], 36: [895, 892, 894, 893], 5: [668, 669], 12: [4457, 4459, 4458], 18: [1042, 4743, 4744, 4745, 1043, 1044], 19: [4742, 517, 519, 518], 20: [4279, 924, 922, 923], 28: [4565, 4562, 4564, 653, 4563], 35: [834, 4579, 832, 833], 39: [684, 683, 682, 4233, 4234], 40: [4639, 563, 564, 4638, 4637], 49: [4397, 743, 4398], 8: [4757, 4623, 534, 4622], 4: [4428, 849, 848, 4429], 11: [4520, 4519, 4517, 4518], 37: [909, 908, 4352, 4353, 4354], 42: [4430, 1027, 1028, 4654, 1029], 43: [4338, 652], 1: [713, 4504, 4505, 4503], 2: [4488, 621, 622, 623, 4487], 3: [4534, 745, 4532, 4533, 744], 10: [4472, 4474, 4473], 26: [818, 4369, 817], 46: [997, 4385, 982, 4324], 48: [4550, 638, 4549, 4548], 16: [4250, 773, 667, 4248, 772, 4249], 24: [714, 4729, 4728], 32: [594, 4382, 4384, 593, 4383], 38: [786, 787, 4400, 4399], 45: [4610, 4608, 4609], 31: [4443, 4444, 4442, 636, 637], 33: [4308, 4427, 4578, 4307, 532, 533, 4577], 22: [609, 4293, 608, 607, 4292], 6: [697, 4262, 4264, 847, 4263], 44: [562, 4277, 862, 4278]}, {0: [5226, 5228, 1467, 5227], 7: [1421, 1751, 5076, 5077, 5079, 5078], 17: [1709, 1708, 1452, 1453, 5393, 5392], 21: [1406, 5242, 1407], 23: [1616, 5257, 1618, 5259, 5258, 1617], 25: [1331, 1334, 1333, 5196, 1332], 27: [1273, 1272, 5106, 5110, 5109, 5108, 5107], 30: [1364, 1362, 1363], 34: [5091, 5094, 5093, 5092], 41: [5124, 5123, 5122], 47: [5199, 5229, 1783, 1782], 9: [1469, 5557, 1842, 1843, 1844, 5559, 5558], 13: [5288, 1303, 5287, 1422], 14: [1647, 1649, 1648], 15: [5289, 1739, 1736, 5333, 1738, 1737, 5334], 29: [5301, 5305, 5302, 1706, 1707, 5303, 5304], 36: [1754, 1753, 1752], 5: [5136, 1227, 1228, 5408, 5407, 5406], 12: [1932, 5151, 5152, 5155, 5154, 5153], 18: [1349, 5601, 5602, 1497, 1498, 1499], 19: [5317, 5318, 1798, 5319], 20: [1587, 5168, 5167, 5166], 28: [1346, 1347, 5364, 5363, 5361, 5362], 35: [1769, 1767, 1768], 39: [5139, 5138, 1361, 5137], 40: [1557, 1558, 5647, 5649, 5648, 1559], 49: [5439, 5438, 5437, 5376, 5391, 1392, 1393], 8: [5183, 5182, 1377, 1376, 5181], 4: [1454, 5452, 5482, 1436, 1437, 1438], 11: [1589, 5603, 1633, 1634], 37: [5421, 5424, 5423, 5422], 42: [1243, 1244, 1619, 5543, 1513, 5542, 5541], 43: [1858, 5169, 1857], 1: [1317, 1319, 1318], 2: [1571, 5467, 1572, 1573, 5468], 3: [1302, 5241, 1182, 5331, 5332, 1423, 1424], 10: [1784, 5499, 5498, 5497, 5496, 1289, 1288, 5271], 26: [5586, 5469, 5587, 5588, 1662, 1663, 1664], 46: [5197, 1632, 5198], 48: [5513, 1378, 5512], 16: [1693, 5484, 1829, 1827, 1828], 24: [1304, 5573, 5481, 1274, 5572, 5571], 32: [5604, 5409, 1812, 1814, 1813], 38: [1541, 5214, 1542, 5212, 5213], 45: [1257, 1259, 5348, 1258, 5346, 5347], 31: [1601, 1604, 1602, 5453, 1603], 33: [5528, 5527, 1482, 1483, 1484], 22: [5272, 1678, 5273, 5274], 6: [5379, 5377, 5378, 1722, 1723], 44: [5320, 1872, 5243, 5244]}, {0: [678, 3678, 3573, 3243, 691, 693, 692], 7: [3033, 3032, 3543, 797, 795, 796], 17: [3363, 3360, 677, 3361, 3362], 21: [3528, 723], 23: [647, 3408, 3405, 3406, 3407], 25: [3061, 3062, 3063, 780, 781], 27: [766, 767, 768, 3601, 3602, 3603], 30: [648, 3570, 3571, 3572], 34: [3289, 3198, 3587, 841, 842, 843, 3588], 41: [3107, 571, 3182, 3333, 646, 645], 47: [256, 3240, 3242, 3241], 9: [3616, 751, 752, 3617, 3618, 753], 13: [512, 510, 511], 14: [3558, 3557, 602, 3348, 3257, 601], 15: [435, 436, 3153, 3151, 3154, 3152], 29: [3228, 3226, 556, 631, 3227], 36: [437, 588, 3541, 3542], 5: [525, 527, 526], 12: [315, 316, 558, 557, 3317, 3316], 18: [303, 465, 466, 528, 3526, 3527, 467], 19: [573, 3302, 572, 3303], 20: [300, 301, 302], 28: [886, 887, 3451, 3454, 3453, 3452], 35: [3467, 393, 3468, 332, 3466], 39: [632, 3436, 3437, 3438], 40: [360, 3272, 3271, 363, 361, 362], 49: [3376, 587, 3377], 8: [618, 617, 616], 4: [213, 212, 211, 3123, 3122, 3124, 3121], 11: [452, 3347, 451], 37: [270, 3166, 483, 482, 481, 3167], 42: [3045, 288, 287, 286, 3091, 285], 43: [273, 271, 272], 1: [676, 3169, 3046, 3047, 630, 3168], 2: [542, 3288, 3286, 3285, 3287], 3: [3318, 3273, 736, 737], 10: [495, 586, 3092, 3093], 26: [721, 722, 3421, 3422, 782, 3423], 46: [3213, 331, 3210, 3212, 3211], 48: [3139, 615, 600, 3138, 450, 3137], 16: [376, 3346, 378, 377], 24: [513, 3511, 663, 738, 3513, 3512], 32: [498, 496, 3331, 3332, 497], 38: [3482, 348, 346, 3481, 347], 45: [3496, 3497, 543], 31: [420, 662, 661, 3196, 541, 3197], 33: [3586, 406, 407, 3556, 408], 22: [422, 3256, 421], 6: [391, 3391, 392], 44: [3420, 3195, 226, 3301, 227]}, {0: [3828, 3903, 757, 756, 755], 7: [846, 4052, 4054, 4053], 17: [772, 3992, 3993, 771], 21: [3827], 23: [4111, 4113, 590, 591, 4112], 25: [487, 4249, 4382, 4383, 4384, 847], 27: [4293, 335, 336, 337, 4292, 4291], 30: [3901, 3902], 34: [3844, 3843, 3842, 546, 545], 41: [4186, 4188, 4187], 47: [4263, 726, 727], 9: [352, 4126, 4128, 351, 4127], 13: [622, 620, 4248, 621], 14: [410, 3991, 411, 413, 412], 15: [4068, 3963, 606, 605, 3961, 3962], 29: [472, 725, 3978, 3977, 470, 471], 36: [4217, 815, 816, 4219, 4218], 5: [4007, 4006, 382, 381], 12: [922, 921, 4039, 4083, 4008, 785], 18: [4038, 4037, 4096, 456, 454, 455], 19: [861, 860, 3933, 3931, 530, 3932], 20: [533, 532, 4097, 4098, 531], 28: [395, 4234, 396, 4233, 4232, 397], 35: [773, 368, 817, 4351, 4352, 4353, 4354], 39: [380, 800, 3948, 3946, 3947], 40: [4397, 563, 560, 561, 562], 49: [576, 665, 575, 3917], 8: [4336, 3826, 367, 4156, 365, 366], 4: [517, 515, 4067, 516], 11: [636, 4276, 4277], 37: [652, 4171, 4172, 4174, 651, 4173], 42: [3872, 502, 501, 500], 43: [4458, 786, 787], 1: [4247, 547], 2: [439, 442, 440, 441], 3: [3916, 427, 424, 426, 425], 10: [4324, 4321, 577, 4323, 4322], 26: [4306, 4307, 666, 667], 46: [892, 4189, 891, 890, 4023, 4024], 48: [4262, 4261], 16: [713, 3873, 710, 712, 711], 24: [4366, 4367], 32: [862, 801, 697, 4278], 38: [740, 741, 742, 743], 45: [4428, 383, 4501, 457, 398, 4427], 31: [485, 4157, 4203, 486, 4204, 4202], 33: [4338, 4082, 680, 682, 681], 22: [4368, 637, 4412, 728, 4413], 6: [4158, 696, 3887, 3888, 695], 44: [4141, 4144, 4143, 4142]}, {0: [1773, 4149, 1774, 1775, 1776], 7: [3909, 1879], 17: [1716, 1669, 1670, 1671, 4133], 21: [1924, 1923, 3549], 23: [3849, 1759, 3744, 3743], 25: [1819, 3759, 3756, 3757, 3758], 27: [1806, 3682, 3683, 1805, 1804, 3684], 30: [1880, 4045, 3774, 1940, 1939], 34: [3715, 1609, 3712, 3713, 3714], 41: [1822, 4224, 4223, 1490, 1491, 1492], 47: [4101, 1865, 4102, 4104, 4103], 9: [3789, 1534, 3787, 3788], 13: [1656, 3906, 1655, 3907, 3908], 14: [3967, 3968, 1834, 1835, 3969], 15: [1579, 3819, 3818], 29: [3832, 3833, 1864, 3834], 36: [4089, 4194, 1789, 1790, 1791], 5: [1413, 3639, 3637, 1698, 3638], 12: [1731, 1728, 1730, 1729], 18: [3862, 3863, 3865, 3864], 19: [1564, 1565, 4044, 4043], 20: [4162, 4163, 1624, 1625, 1626], 28: [1429, 3999, 3998, 1430, 3997], 35: [1459, 4088, 4087, 1461, 1460], 39: [1788, 1654, 3668, 3669], 40: [3984, 3983, 1414, 1415, 3982], 49: [3697, 3699, 3698], 8: [3726, 3727, 3729, 3728], 4: [3895, 3892, 3893, 1699, 3894], 11: [3922, 3923, 1685, 1684], 37: [3848, 1518, 1520, 1519], 42: [3772, 3773], 43: [3879, 1761, 1760], 1: [1504, 1489, 3802], 2: [3937, 1474, 1475], 3: [4042, 1400, 3817, 1399], 10: [1353, 1355, 1354], 26: [3877, 1610, 1549, 3878], 46: [4028, 4029, 1820, 1821], 48: [1445, 3652, 1444], 16: [1715, 3804, 1713, 1714], 24: [1369, 1323, 3847, 1324], 32: [4072, 4074, 4073, 1535], 38: [1850, 3954, 3952, 3953], 45: [1476, 1383, 1384, 1385, 4012], 31: [1639, 1640, 1641], 33: [3593, 1595, 1594, 3653, 1593], 22: [1505, 4059, 1596, 4058], 6: [1746, 3938, 1744, 1745], 44: [4148, 1550, 1551]}, {0: [1622, 1606, 3322, 3323], 7: [1639, 1637, 1638], 17: [1381, 1384, 1382, 1383], 21: [1321, 1216, 1171, 3261], 23: [1188, 1187, 1186, 3307, 3306], 25: [1623, 3533, 3530, 3531, 3532], 27: [3443, 1547, 3725, 3726, 3727, 1548], 30: [3351, 3352, 1336], 34: [1129, 3321, 1127, 1128], 41: [3635, 3636, 3637, 1607, 1608, 3638], 47: [3473, 1531, 3397, 1532], 9: [3485, 1458, 3488, 3486, 3487], 13: [1399, 1323, 3713, 3711, 3712], 14: [3668, 3667, 3666, 1353], 15: [3623, 3620, 3621, 3622], 29: [3428, 1023, 1022, 3425, 3427, 3426], 36: [3548, 3547, 1426, 1427, 1428], 5: [1339, 3740, 3741, 1338], 12: [1054, 3382, 3381, 1053, 1052, 3380], 18: [1201, 1203, 3442, 3441, 1202], 19: [1097, 1307, 3410, 1352, 3411], 20: [3575, 3576, 1367, 1368], 28: [3367, 1398, 3365, 3366, 1397], 35: [3455, 3458, 3456, 3457], 39: [1429, 3698, 3697, 3696, 3650, 1143], 40: [1337, 3516, 3517], 49: [3201, 3200, 1066, 1067, 1068], 8: [1219, 1218, 1217], 4: [1292, 1294, 3471, 1293], 11: [1248, 3562, 3560, 1322, 3561], 37: [3396, 1262, 1264, 1263], 42: [1246, 3291, 3290, 1113, 1112], 43: [1576, 1546, 1501, 3308], 1: [1247, 1231, 1232, 1234, 3651, 1233], 2: [3518, 3755, 1473, 3756, 3757, 1474], 3: [1099, 3590, 1098], 10: [1652, 1653, 3608, 3605, 3606, 3607], 26: [1443, 3591, 1563, 3592], 46: [1516, 3472, 1518, 1517], 48: [1173, 3501, 1172], 16: [3230, 1562, 3231, 1561, 3232], 24: [3470, 1158, 1157], 32: [1502, 3413, 3412], 38: [3652, 1489, 1487, 1488], 45: [3681, 1309, 3682], 31: [3336, 3337, 1414, 1413, 1412], 33: [3771, 1279, 1276, 1278, 1277], 22: [1459, 3772, 1577, 1578, 1579], 6: [1472, 1396, 3276, 1457, 3277], 44: [3503, 3502]}, {0: [5484, 1811, 1812, 5559, 1814, 1813], 7: [5064, 5063, 5061, 5062], 17: [1317, 1318, 1319, 5558, 5557, 5556], 21: [5334], 23: [1799, 1798, 1797, 5304, 5301, 5302, 5303], 25: [5213, 5407, 5408, 5409, 1721, 1722, 1723], 27: [5543, 5076, 5077, 5078, 1664, 1662, 1663], 30: [1739, 5574, 5482, 1454, 5572, 5573], 34: [5319, 1649, 1648, 5318], 41: [5287, 5288, 1767, 5289], 47: [1781, 5046, 4959, 5047, 4958, 1481], 9: [1271, 1272, 5438, 5437, 1378, 5541, 1273, 1274], 13: [1558, 5017, 1556, 1557], 14: [5588, 1631, 1634, 1633, 5587, 1632], 15: [5316, 5317, 1362, 5016, 1361], 29: [1540, 5361, 5362, 1541, 1542], 36: [1331, 1333, 1332], 5: [5256, 5259, 1678, 5257, 5258], 12: [5210, 1572, 1301, 1302, 5212, 5211], 18: [4986, 4987, 4988, 1751, 1752, 1753, 1754], 19: [1391, 1394, 1392, 1393], 20: [1796, 5122, 5124, 5123], 28: [5528, 1574, 5526, 5527], 35: [5466, 5121, 5421, 1258, 5226, 1256, 1257], 39: [5271, 5272, 1436, 1437], 40: [1619, 1617, 1618, 5378, 5377, 5376], 49: [1407, 5166], 8: [1738, 1737, 5196, 5197, 5198], 4: [1244, 1364, 5571, 5602, 1482, 1483, 1484], 11: [5274, 5002, 5108, 1586, 5273, 1587], 37: [1438, 1782, 1783, 5469, 5467, 5468], 42: [1303, 5391, 1363], 43: [5525, 1183, 1181, 1182], 1: [1768, 1573, 5392, 5393], 2: [1499, 5347, 1497, 1498], 3: [5241, 1647, 5244, 5242, 5243], 10: [5167, 5168, 1603, 1601, 1602], 26: [1528, 5107, 1452, 5422, 1453], 46: [5154, 5153, 1346, 5152], 48: [5513, 5423, 5514, 1707, 1708], 16: [5286, 5406, 1287, 1288], 24: [5139, 1376, 5138, 5136, 5137], 32: [1511, 5181, 5183, 5182], 38: [5030, 1466, 1406, 5032, 5031], 45: [1827, 1828, 1829, 5498, 5499], 31: [1347, 5331, 1377, 5333, 5332], 33: [1289, 5451, 5453, 5452, 1421, 1422, 1423], 22: [5094, 1211, 5091, 5093, 5092], 6: [5151, 5346, 1241, 1242, 1243], 44: [5228, 5227, 1467]}, {0: [3727, 3728, 3730, 3729], 7: [3668, 3893, 1475, 1474], 17: [1926, 1924, 1925], 21: [2104, 3836, 2090, 2089], 23: [1893, 1894, 4046, 4045, 1895], 25: [3774, 3669, 1819], 27: [3578, 3579, 1880, 1879, 1878], 30: [4076, 2060, 2058, 2059], 34: [3804, 3805, 3760, 2014], 41: [1699, 1639, 3744, 1698, 3743], 47: [1491, 1490, 1489, 3639, 3638, 3637], 9: [3713, 1985, 3714, 3715, 1984], 13: [1851, 4015, 3907, 4014, 3908, 1745], 14: [3895, 3894, 1776, 1775], 15: [1743, 1744, 3863, 3865, 3864], 29: [1519, 3757, 3759, 3758], 36: [1609, 1610, 4044, 4043], 5: [1836, 1834, 3954, 1835], 12: [3953, 1669, 3820, 3819, 1670, 3818], 18: [1534, 1774, 3835, 3833, 3834], 19: [3983, 4075, 4074, 1685, 1684], 20: [1999, 1970, 1969, 3699, 3700], 28: [1953, 1954, 1955, 4029, 4030], 35: [1563, 4000, 3999, 1564, 1565, 3998], 39: [1971, 1730, 4059, 4060], 40: [2029, 3790, 3788, 3789], 49: [3939, 3938], 8: [1986, 4089, 1956, 2045, 4090], 4: [1805, 1804, 3686, 3685, 3684], 11: [3880, 1938, 1939, 1941, 1940], 37: [3593, 1865, 1864, 3594, 1863], 42: [3655, 3654, 1579, 1578, 3653], 43: [4102, 1671, 4104, 4103], 1: [1848, 1850, 3670, 1849], 2: [3985, 1758, 1759, 3984, 1760], 3: [1789, 1791, 1790], 10: [1910, 3640, 1908, 1909], 26: [1593, 3610, 3608, 1713, 3609], 46: [3773, 1504, 3772], 48: [1820, 3970, 3969], 16: [4133, 3803, 1623, 1624, 1626, 1625], 24: [2031, 2030, 3924, 3925], 32: [1550, 3624, 1549, 3625, 1548, 3623], 38: [1653, 1656, 1655, 1654], 45: [4120, 3850, 2000, 2001], 31: [1729, 1728], 33: [1716, 3879, 1714, 1715], 22: [4119, 1806, 4087, 4088, 4149, 1761], 6: [1640, 3849, 3848], 44: [1595, 3698, 3923, 1594]}, {0: [1390, 1420, 4941, 4942], 7: [4850, 4881, 5000, 1212, 1210, 1211], 17: [1345, 1062, 1061, 4985, 4986], 21: [1465, 1480, 4882], 23: [4896, 4897, 1481, 1482, 1483, 5422], 25: [1136, 1138, 1137], 27: [1330, 1332, 1331], 30: [1393, 1392, 1391], 34: [1647, 1646, 4866, 4867, 1525, 4928], 41: [4987, 1438, 1435, 1437, 1436], 47: [5092, 1451, 1452], 9: [1167, 1166, 1165, 4926, 1240, 1241], 13: [1663, 1662, 5076, 1467, 5077, 5078], 14: [1346, 5273, 5272, 5271, 1347], 15: [4851, 1362, 1361, 1360], 29: [1557, 5210, 5211, 5213, 5212], 36: [1242, 5227, 5226], 5: [1063, 1303, 1228, 5420, 5421], 12: [1375, 1376, 5375, 5376, 1378, 1377], 18: [4911, 1587, 1586, 5002, 4912, 1466], 19: [1077, 1076, 5015, 5047, 5046, 1181], 20: [4956, 4957, 1618, 1617, 4958, 1616], 28: [1255, 1258, 1257, 1256], 35: [1273, 1271, 1272], 39: [5289, 5288, 5287, 5286, 5285], 40: [5255, 5258, 5257, 5256], 49: [1106, 1108, 1107, 5240], 8: [1405, 5001, 1407, 1406], 4: [5334, 1182, 5331, 5333, 5332], 11: [5377, 1571, 1572, 1573], 37: [4971, 1423, 4972, 1421, 1422], 42: [5363, 5362, 1288, 5360, 5361], 43: [5032, 5031], 1: [1601, 5301, 5302, 1602, 1648, 5303], 2: [5151, 1318, 5153, 5152, 1317], 3: [5123, 1092, 5120, 5122, 5121], 10: [5107, 5106, 1123, 1122], 26: [5345, 5348, 5346, 5347], 46: [5180, 5181, 5182], 48: [5198, 1227, 5197, 5196, 5195], 16: [5061, 5030, 1198, 1197, 1196], 24: [1152, 1151, 5091, 5090], 32: [5136, 5138, 5137], 38: [1555, 5166, 1556, 5167], 45: [5228, 5316, 1542, 5317, 5318], 31: [5183, 1633, 5242, 5243, 1632], 33: [5062, 5063, 1706, 1707], 22: [1301, 5016, 1541, 5017], 6: [5241, 1286, 1287], 44: [1511, 5108, 1498, 1497]}, {0: [2622, 2471, 2621, 5098, 5099], 7: [4961, 4964, 4963, 4962], 17: [2518, 5127, 2517, 5128, 2516], 21: [5143, 5144], 23: [2682, 5156, 5159, 5157, 5158], 25: [4977, 4978, 2503, 2502, 2501], 27: [2561, 2562, 5427, 5428, 2563], 30: [5084, 2757, 5233, 5234], 34: [5097, 2398, 2397], 41: [5217, 5218], 47: [4842, 2456, 2455], 9: [2428, 2427, 5066, 5067, 2425, 2426], 13: [4948, 4949, 2590, 2592, 2591], 14: [5276, 5277, 2486, 2487, 5278], 15: [5036, 2606, 5038, 2396, 5037], 29: [2320, 2321, 2323, 2322], 36: [2188, 5096, 2186, 2187], 5: [2248, 2246, 2247], 12: [2531, 5053, 5051, 5052], 18: [4901, 2383, 2382, 2381, 4902], 19: [5249, 5248, 5246, 5247], 20: [2203, 2201, 2202], 28: [2172, 5081, 2411, 5083, 5082], 35: [5381, 5382, 2578, 5383], 39: [2141, 2142, 5203, 5202, 5201], 40: [5324, 2637, 5021, 5022, 5023, 2636], 49: [2293, 2291, 2292], 8: [2547, 2548], 4: [2473, 5186, 5187, 2472], 11: [5309, 5307, 5308], 37: [5112, 2533, 5188, 5113, 2532], 42: [2440, 5323, 2441, 2442], 43: [4918, 4917, 2261, 2260], 1: [5351, 2412, 5353, 5352], 2: [2158, 2143, 2353, 5366, 5368, 5367], 3: [2608, 2607, 5262, 5263], 10: [5339, 5337, 2457, 5338], 26: [2216, 2217, 2218], 46: [2350, 2352, 2351, 4947], 48: [5294, 5292, 5293], 16: [5006, 5007, 5008], 24: [2698, 2593, 5473, 5474], 32: [2335, 2338, 4992, 2337, 2336], 38: [2577, 2576, 4932, 4933, 4934], 45: [2173, 5413, 5412, 5411], 31: [5171, 5173, 5172], 33: [2306, 5142, 2307], 22: [2365, 2366, 2368, 2367], 6: [2230, 5322, 2232, 2231], 44: [2157, 2156, 2275, 4991]}, {0: [4688, 4583, 1630, 1629], 7: [4870, 4868, 4869], 17: [4750, 1748, 4748, 1749, 4749], 21: [4763, 1810, 4764], 23: [1703, 1809, 4598, 4600, 4599], 25: [4689, 1780, 1778, 1779], 27: [1869, 4645, 1867, 1868, 4643, 4644], 30: [4586, 4585, 4584], 34: [1674, 4823, 1675], 41: [4703, 1583, 1584], 47: [4537, 4538, 1568], 9: [1735, 1732, 4734, 1733, 1734], 13: [4884, 4885, 2003, 2004, 2005], 14: [1856, 1855, 4705, 1854, 4704], 15: [1765, 1762, 1764, 1763], 29: [4854, 4853, 1600, 1598, 4733, 1599], 36: [1615, 4673, 1613, 1614], 5: [4960, 1900, 4510, 1899, 1898], 12: [1628, 4509, 4508], 18: [1643, 1645, 4839, 1644, 4838], 19: [1808, 1719, 4494, 1718, 4493], 20: [1687, 4630, 1688, 4629, 4628], 28: [4810, 1524, 4807, 4809, 4808], 35: [4613, 1988, 4614, 4615, 1989], 39: [4525, 4523, 4524], 40: [2034, 4658, 4659, 4660, 2079], 49: [1540, 4492, 4477, 1539, 1538], 8: [4765, 1913, 1914], 4: [1659, 4795, 4794, 1660], 11: [1943, 1944, 1945], 37: [4539, 2063, 4540], 42: [4359, 1840, 1839, 1838], 43: [4642, 4507, 1522, 1523], 1: [1884, 4718, 4720, 4719], 2: [2048, 2049, 1990, 4824, 4825], 3: [4672, 1509, 4780, 4779, 4778], 10: [1553, 1554, 1555, 4898, 4899, 1870], 26: [1958, 4914, 4915, 1960, 1959], 46: [1928, 4435, 4433, 4434], 48: [1826, 1825, 4674, 1824], 16: [1537, 4464, 4462, 4463], 24: [4735, 1975, 4675, 1974], 32: [1552, 4418, 4420, 4419], 38: [1597, 4390, 4388, 1717, 4389], 45: [4840, 2020, 2018, 2019], 31: [4569, 4571, 1883, 4570], 33: [1793, 4555, 4553, 4554], 22: [2047, 4447, 1853, 4448, 4450, 4449], 6: [4480, 1658, 4479, 1673, 4478], 44: [1972, 2078, 1973, 4495]}, {0: [2522, 3404, 2432, 3402, 3403], 7: [3523, 3524], 17: [3479, 3478, 3477], 21: [3569, 2717, 2718], 23: [2402, 3492, 3494, 3493], 25: [3193, 2703, 2702, 2567, 3314, 3614, 2656], 27: [2222, 2221, 3329, 3328, 3327], 30: [3748, 2657, 2658, 2659], 34: [2687, 3358, 3359], 41: [2536, 2537, 2538], 47: [3732, 3731, 2164, 3401, 2163, 2162], 9: [2253, 3657, 2374, 2371, 2372, 2373], 13: [2386, 2388, 2387], 14: [3313, 3207, 2478, 2477, 2476], 15: [2551, 2552, 3508, 3509, 2553], 29: [3238, 2611, 2612, 3733, 2613], 36: [2417, 2418], 5: [2356, 2358, 2357], 12: [2568, 3629, 3626, 2328, 3628, 3627], 18: [3566, 3567, 3568, 2596, 2597], 19: [2581, 2582, 2583, 3672, 3673, 3674], 20: [3464, 3462, 2523, 3463], 28: [3416, 2298, 2297, 2296, 2416, 3282], 35: [2281, 2282, 3642, 2283], 39: [3446, 2327, 3447], 40: [3192, 3747, 2344, 2343, 2342, 2341], 49: [3702, 3476, 2209, 2208, 2207], 8: [3344, 3342, 3343], 4: [3164, 2625, 2626, 3552, 3553, 2627], 11: [3491, 2148, 2147, 2146, 3237, 3236], 37: [3433, 3432, 3431, 2072], 42: [2508, 3373, 2507, 2415, 3178, 2506], 43: [2238, 2237], 1: [3297, 2431, 3299, 3298], 2: [2446, 3386, 3388, 3387], 3: [2206, 3266, 2521, 2401, 3268, 3267], 10: [2192, 3281, 3223, 3222, 3221, 2236], 26: [3296, 3613, 2177, 2178, 3612, 3611], 46: [3581, 2643, 3582, 2628, 3583], 48: [3254, 2071, 3251, 3253, 2251, 3252], 16: [3689, 3688, 2223, 3687], 24: [2326, 3162, 3163], 32: [3461, 3598, 2193, 3596, 3597], 38: [3539, 3537, 3538], 45: [2313, 3357, 2311, 2312], 31: [3434, 3417, 3418, 2642], 33: [2461, 3372, 2463, 2462], 22: [2268, 3507, 3371, 3312, 2267, 2266], 6: [2492, 3703, 2493, 2494], 44: [2447, 2448]}, {0: [3827, 439, 201, 3826, 200, 3825], 7: [575, 3962], 17: [4381, 560, 561, 562, 4382, 563], 21: [3811, 3810, 185], 23: [3945, 277, 274, 275, 276], 25: [3960, 3961, 351, 350], 27: [440, 4247, 441], 30: [262, 4305, 202], 34: [424, 3902, 3900, 3901], 41: [454, 3887], 47: [3992, 590, 591, 4158, 4157], 9: [485, 4232, 487, 4231, 486], 13: [4171, 620, 621, 606, 4172], 14: [4427, 455, 457, 456], 15: [472, 469, 470, 471], 29: [500, 501, 502, 4261], 36: [4080, 4081, 605, 4082], 5: [398, 4366, 306, 307], 12: [4083, 4051, 4052, 711, 4053], 18: [413, 410, 411, 412], 19: [4263, 4396, 4262, 4397, 532], 20: [246, 245, 3857, 3856, 244], 28: [4276, 427, 4412, 425, 426], 35: [3990, 3872, 3871, 216, 215], 39: [531, 4203, 4201, 4202], 40: [3991, 4275, 292, 290, 291], 49: [4128, 4383, 697, 696], 8: [186, 187, 442, 217, 4320, 4321], 4: [4245, 3886, 365, 366, 367, 4246], 11: [4277, 4351, 4352, 4322, 517], 37: [4456, 338, 4155, 4156, 336, 337], 42: [4306, 4066, 382, 381], 43: [3946, 3947, 785, 3948, 786], 1: [395, 4336, 397, 396], 2: [322, 4095, 320, 321], 3: [4218, 4216, 545, 546, 547, 4217], 10: [652, 651, 4125, 4126, 4127], 26: [4350, 172, 3931, 171, 170, 3930], 46: [577, 576, 530, 4006, 4007], 48: [352, 4291, 4292], 16: [4069, 4067, 4068], 24: [3977, 3976, 3975], 32: [4233, 4248, 3888, 3873, 682, 680, 681], 38: [4110, 4113, 4111, 4112], 45: [4142, 155, 4005, 231, 4141, 4140], 31: [4186, 4187, 515, 516], 33: [335, 667, 666, 665, 3917, 3916], 22: [636, 4143, 741, 4023, 4021, 4022], 6: [847, 846, 4096, 4097, 4098], 44: [727, 305, 726, 4038, 4036, 4037]}, {0: [2802, 2801, 5024, 4873, 4874, 2785, 2786], 7: [2831, 5399, 5219, 2832, 2833], 17: [5038, 2772, 5039, 2771], 21: [2470, 4798], 23: [2488, 2487, 4978, 2485, 2486], 25: [2472, 4994, 4993, 4992, 2471], 27: [2515, 5128, 2518, 2517, 2516], 30: [5022, 5023], 34: [2695, 4887, 2440, 4889, 4888], 41: [2682, 2681], 47: [2713, 5354], 9: [5397, 2665, 2666, 2667, 2668, 5398], 13: [2711, 2712, 5247, 5248, 5249], 14: [2847, 2846, 2321, 5007, 5009, 5008], 15: [5369, 5368, 2635, 2636, 2637], 29: [2698, 5129, 2696, 2697], 36: [2427, 5218, 5217], 5: [2548, 2546, 2547], 12: [5353, 2607, 5083, 2606], 18: [5054, 2605, 4918, 4919, 2742, 2741], 19: [5099, 2411, 5097, 5098], 20: [5189, 2337, 5188, 5187], 28: [2562, 4902, 4903, 2561], 35: [5082, 2291, 2292, 5264, 5262, 5263], 39: [5052, 2592, 5053, 2591], 40: [2576, 5428, 2577, 2578], 49: [2441, 5036, 5037], 8: [2380, 5067, 4963, 2381], 4: [5159, 2425, 2426, 5158], 11: [5069, 2457, 2455, 5068, 2456], 37: [5308, 5309, 2620, 2621, 2622], 42: [2351, 4947, 4949, 4948], 43: [5338, 2563, 5339], 1: [2365, 4857, 4858, 4979, 2590], 2: [2533, 2532, 2530, 2531], 3: [5144, 5143, 2260, 2261, 5142], 10: [5384, 5383, 5382, 2366, 2367, 2368], 26: [5127, 2336, 4843, 4842, 2335], 46: [2756, 5084, 2758, 2757], 48: [4934, 4932, 2410, 4933], 16: [5324, 2246, 2247, 5323, 2245, 5322], 24: [5427, 2382, 2383], 32: [5232, 5233, 2728, 2727, 5234], 38: [5277, 2442, 2743, 5279, 5278], 45: [5174, 5172, 5173], 31: [2650, 2651, 5113, 5114], 33: [2503, 2502, 2500, 2501], 22: [2322, 5294, 5293, 5292], 6: [2398, 2396, 2397, 5204, 5203, 5202], 44: [5414, 5413, 5412, 2353, 2352, 5112]}, {0: [3472, 1350, 1352, 1351], 7: [1278, 962, 3515, 3517, 3516], 17: [3409, 1158, 1157, 3411, 3410], 21: [1320, 3112, 3111], 23: [3605, 3606, 1486, 1487, 1488, 3607], 25: [3351, 1276, 3367, 3366, 1277], 27: [1187, 3530, 3532, 3531], 30: [1444, 3711, 1353, 3712], 34: [3202, 3201, 3200, 1021, 3199], 41: [3485, 3487, 3486], 47: [3335, 3337, 3336], 9: [3500, 1170, 1083, 1082, 3186, 3185, 1081], 13: [3575, 1321, 1322, 1323, 3576], 14: [1306, 3306, 1307, 1458, 1457, 3307], 15: [3469, 3471, 1022, 3470], 29: [1038, 1037, 3246, 3245, 1036], 36: [993, 933, 934, 3739], 5: [1366, 1368, 1367], 12: [1262, 1263, 3591, 3590, 3589], 18: [1294, 1291, 1293, 3441, 1292], 19: [1008, 1188, 3622, 3620, 3621], 20: [1247, 1248], 28: [3740, 3741, 3442, 1399, 1398, 1396, 1397], 35: [932, 3427, 3426, 3424, 3425], 39: [3559, 3562, 3560, 3561], 40: [1084, 1516, 1517, 1518, 3650, 3651, 3652], 49: [1231, 1233, 1232], 8: [1441, 1443, 1442], 4: [1249, 1171, 3726, 3725, 1173, 1172], 11: [3260, 3262, 3261], 37: [1219, 1216, 1218, 1217], 42: [3545, 1112, 1114, 1113], 43: [3592, 1427, 1428], 1: [1111, 992, 991, 3216, 3215, 3214], 2: [3502, 1335, 1336, 1338, 1337], 3: [1007, 1006, 1005, 3172, 3171, 3170], 10: [3365, 1186, 3277, 1246, 3276], 26: [1129, 1126, 1127, 3501, 1128], 46: [1204, 1202, 1203], 48: [3322, 1201, 3321], 16: [3382, 3381, 3380, 3379, 948, 947], 24: [3455, 1054, 1051, 1053, 1052], 32: [3187, 3637, 1411, 1413, 1412], 38: [977, 978, 3667, 3666, 1023, 3665], 45: [3457, 3456], 31: [3770, 3305, 1097, 1098, 1099], 33: [1068, 1067, 3230, 1066], 22: [3231, 1383, 3352, 1381, 1382], 6: [949, 3682, 3680, 3681], 44: [3635, 3636]}, {0: [2154, 4752, 2319, 2035, 4750, 4751], 7: [2215, 2217, 2216], 17: [2155, 5080, 5081, 2156], 21: [2005, 4765], 23: [1869, 1870, 4977, 4976, 4975], 25: [2320, 4870, 4871, 4872], 27: [1975, 4842, 4841, 4840], 30: [5005, 2036], 34: [1899, 1901, 1900], 41: [4857, 4855, 4856], 47: [2409, 2365, 4737], 9: [4827, 4826, 4825, 4824, 1795, 4899], 13: [2006, 2007, 2292, 5186, 5185], 14: [1962, 4812, 4811, 4810, 1960, 1961], 15: [2020, 5067, 5066, 2051, 5065, 2021], 29: [4915, 2410, 2411, 4916, 4917], 36: [</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>[932, 890, 952, 964, 918, 952, 921, 906, 945, 1031, 1000, 919, 935, 938, 919, 961, 927, 900, 919, 913, 959, 961, 958, 950, 977, 940, 999, 1017, 910, 990, 909, 887, 990, 927, 980, 984, 955, 920, 962, 977, 964, 952, 930, 968, 931, 935, 941, 989, 955, 960, 956, 954, 1025, 893, 946, 939, 893, 960, 926, 910, 880, 913, 978, 954, 894, 981, 992, 931, 941, 1081, 936, 948, 1001, 939, 989, 946, 958, 964, 969, 941, 883, 1007, 950, 1000, 908, 932, 950, 993, 952, 982, 955, 942, 970, 930, 926, 999, 916, 881, 980, 996]</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>[208, 207, 243, 240, 225, 214, 249, 243, 229, 207, 221, 249, 220, 223, 203, 215, 222, 230, 219, 224, 223, 212, 225, 210, 229, 227, 211, 225, 231, 218, 221, 237, 220, 221, 231, 213, 229, 222, 231, 221, 203, 242, 221, 223, 231, 211, 226, 225, 229, 230, 224, 235, 226, 229, 213, 221, 244, 209, 234, 221, 243, 237, 230, 223, 227, 209, 215, 216, 224, 231, 219, 218, 228, 250, 226, 230, 227, 233, 213, 209, 231, 212, 231, 243, 263, 228, 199, 211, 226, 244, 209, 236, 209, 230, 209, 223, 233, 247, 220, 215]</t>
-        </is>
+          <t>[3.0324337482452393, 7.605472803115845, 2.871635913848877, 4.787048578262329, 8.54765796661377, 3.3995132446289062, 4.422792196273804, 5.932949542999268, 4.643215894699097, 7.813405513763428, 5.50854229927063, 11.405491590499878, 3.938908576965332, 5.461305379867554, 4.190269947052002, 7.660758972167969, 2.381101369857788, 8.33068299293518, 6.844806671142578, 4.856736183166504, 5.1558756828308105, 6.07828950881958, 3.276534080505371, 2.4024999141693115, 2.721935987472534, 5.05341100692749, 4.487309455871582, 5.69313383102417, 4.221601724624634, 6.523714065551758, 5.370956659317017, 5.577910661697388, 2.909867763519287, 3.095127820968628, 5.31394362449646, 5.900859355926514, 2.6045351028442383, 7.89505410194397, 5.682848930358887, 4.387810468673706, 11.339157581329346, 2.9098966121673584, 5.3250439167022705, 4.091111183166504, 2.3704535961151123, 3.9470887184143066, 3.2195944786071777, 7.669661998748779, 7.136152267456055, 4.319780111312866, 3.0618855953216553, 10.655011415481567, 6.4566686153411865, 5.946972131729126, 7.719345569610596, 4.180140256881714, 9.673887491226196, 5.172270774841309, 3.7846992015838623, 5.390903472900391, 3.119191884994507, 4.210273504257202, 6.115856409072876, 6.384482145309448, 4.616524696350098, 4.48347282409668, 3.239455223083496, 2.934675693511963, 3.4376919269561768, 5.552026033401489, 3.43912410736084, 5.111489534378052, 3.23044753074646, 3.5724244117736816, 4.260251522064209, 2.528724193572998, 3.475013256072998, 7.008441925048828, 5.3094165325164795, 3.1710877418518066, 4.632193326950073, 4.246231317520142, 6.168186902999878, 3.367288827896118, 5.282670497894287, 3.89880633354187, 3.541198253631592, 5.98030948638916, 8.642152547836304, 7.315213441848755, 6.3314759731292725, 5.78587532043457, 4.641846179962158, 3.6435563564300537, 6.010741710662842, 3.5223946571350098, 6.3978271484375, 6.2874977588653564, 3.0787198543548584, 4.404331207275391]</t>
+        </is>
+      </c>
+      <c r="AF7" t="n">
+        <v>1322</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>368</v>
       </c>
       <c r="AH7" t="n">
-        <v>36.11488263133008</v>
+        <v>368</v>
       </c>
       <c r="AI7" t="n">
-        <v>11.90796355216105</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL7" t="inlineStr">
-        <is>
-          <t>[55.54072332382202, 87.21537041664124, 65.2913293838501, 24.98943281173706, 45.570876598358154, 49.0337872505188, 51.74196720123291, 96.30105948448181, 72.25069618225098, 36.21541929244995, 44.536646366119385, 52.37589645385742, 63.59989404678345, 67.30353927612305, 77.5811619758606, 46.83509063720703, 74.76074123382568, 72.98611426353455, 60.810713052749634, 60.06945037841797, 65.32670712471008, 67.14547610282898, 47.601123094558716, 66.99491810798645, 77.05387330055237, 53.96953797340393, 41.02799439430237, 30.154779195785522, 81.10278987884521, 44.522128105163574, 40.64310002326965, 62.81629228591919, 36.844605684280396, 73.10185217857361, 52.3443865776062, 37.92685627937317, 39.855217695236206, 54.115241050720215, 41.679449796676636, 41.53893828392029, 64.66213202476501, 59.346620082855225, 51.30195713043213, 50.66285848617554, 54.48108220100403, 62.64045333862305, 55.912933588027954, 54.192973613739014, 63.34813928604126, 74.78139925003052, 37.66552472114563, 58.99678349494934, 29.015008211135864, 35.20820689201355, 66.06011652946472, 53.051913261413574, 75.95918297767639, 39.88374090194702, 71.35197877883911, 82.67455720901489, 63.26925468444824, 61.707324266433716, 35.322250843048096, 43.77687358856201, 75.99945402145386, 59.22379779815674, 56.47948360443115, 94.76505160331726, 71.98441290855408, 29.08835220336914, 42.8342080116272, 67.0741138458252, 45.413280963897705, 91.3551299571991, 54.172523021698, 51.12741041183472, 36.55331778526306, 93.87054634094238, 42.62156367301941, 45.566954374313354, 85.67571878433228, 44.48027849197388, 34.68355989456177, 42.15486431121826, 87.16092300415039, 58.272828340530396, 46.21805787086487, 67.6047956943512, 44.17249631881714, 41.54749608039856, 43.808664083480835, 38.46893811225891, 42.1409068107605, 56.61925005912781, 66.544851064682, 28.565345764160156, 70.05952548980713, 37.32827138900757, 64.9146728515625, 59.30778241157532]</t>
-        </is>
-      </c>
-      <c r="AM7" t="inlineStr">
-        <is>
-          <t>[2.9470365047454834, 2.117743968963623, 2.931302785873413, 2.0055181980133057, 3.641345977783203, 5.411850929260254, 5.1623663902282715, 2.6140713691711426, 3.158367395401001, 7.622862100601196, 4.308040142059326, 3.807116985321045, 4.907686471939087, 5.253502368927002, 4.023576736450195, 7.032364130020142, 5.707158803939819, 2.1161320209503174, 2.719886064529419, 6.0631420612335205, 4.279545307159424, 5.491664886474609, 2.6734352111816406, 4.021744251251221, 6.061335325241089, 3.861811637878418, 4.76082444190979, 4.438096284866333, 4.257365465164185, 3.307382822036743, 4.183989524841309, 4.003809213638306, 4.004135370254517, 3.4554450511932373, 2.3493382930755615, 4.915064573287964, 1.969552755355835, 2.019904613494873, 4.727254629135132, 3.5656206607818604, 3.5841474533081055, 1.737703800201416, 4.277407646179199, 2.3167102336883545, 3.948988199234009, 7.190643310546875, 2.5809576511383057, 5.887145757675171, 2.070012092590332, 2.3965086936950684, 6.69754958152771, 3.7918508052825928, 3.1360604763031006, 2.2826039791107178, 4.193027019500732, 3.7299110889434814, 3.10435152053833, 8.774941682815552, 2.617234230041504, 2.8813984394073486, 3.541252374649048, 5.390315771102905, 2.909367084503174, 4.377321720123291, 1.996891975402832, 5.195709466934204, 3.7867021560668945, 2.5552306175231934, 4.531709432601929, 3.953594207763672, 5.435537099838257, 5.027769565582275, 2.149747610092163, 1.639617919921875, 2.6196646690368652, 3.738994598388672, 2.3482658863067627, 2.0701212882995605, 4.120977163314819, 4.8634934425354, 3.7085824012756348, 7.130875587463379, 2.7438652515411377, 3.2174317836761475, 1.9996140003204346, 3.598555564880371, 3.133347749710083, 2.329434394836426, 4.6702117919921875, 3.2976126670837402, 4.943619966506958, 3.0643930435180664, 4.67376446723938, 3.3447093963623047, 2.9650397300720215, 2.4372127056121826, 4.09052038192749, 1.948474645614624, 2.3378970623016357, 4.364195346832275]</t>
-        </is>
-      </c>
-      <c r="AN7" t="n">
-        <v>1422</v>
-      </c>
-      <c r="AO7" t="n">
-        <v>368</v>
-      </c>
-      <c r="AP7" t="n">
-        <v>418</v>
-      </c>
-      <c r="AQ7" t="n">
         <v>50</v>
       </c>
-      <c r="AR7" t="inlineStr">
-        <is>
-          <t>[0, 7, 's_0_7', 17, 's_0_17', 21, 's_0_21', 23, 's_0_23', 25, 's_0_25', 27, 's_0_27', 30, 's_0_30', 34, 's_0_34', 41, 's_0_41', 47, 's_0_47', 's_0_0', 9, 's_7_9', 13, 's_7_13', 14, 's_7_14', 15, 's_7_15', 's_7_25', 29, 's_7_29', 36, 's_7_36', 's_7_7', 5, 's_17_5', 's_17_9', 12, 's_17_12', 's_17_14', 's_17_15', 18, 's_17_18', 19, 's_17_19', 20, 's_17_20', 28, 's_17_28', 's_17_29', 35, 's_17_35', 39, 's_17_39', 40, 's_17_40', 's_17_41', 49, 's_17_49', 's_17_17', 8, 's_21_8', 's_21_18', 's_21_23', 's_21_34', 's_21_21', 4, 's_23_4', 's_23_5', 's_23_9', 11, 's_23_11', 's_23_13', 's_23_20', 's_23_30', 's_23_34', 's_23_36', 37, 's_23_37', 's_23_39', 42, 's_23_42', 43, 's_23_43', 's_23_23', 1, 's_25_1', 2, 's_25_2', 3, 's_25_3', 10, 's_25_10', 's_25_12', 's_25_20', 26, 's_25_26', 's_25_37', 's_25_40', 's_25_42', 46, 's_25_46', 48, 's_25_48', 's_25_25', 's_27_1', 's_27_4', 's_27_8', 's_27_10', 's_27_14', 's_27_15', 16, 's_27_16', 's_27_18', 24, 's_27_24', 's_27_29', 32, 's_27_32', 's_27_37', 38, 's_27_38', 's_27_39', 's_27_43', 45, 's_27_45', 's_27_27', 's_30_4', 's_30_8', 's_30_19', 's_30_40', 's_30_42', 's_30_30', 's_34_1', 's_34_2', 's_34_3', 's_34_9', 's_34_15', 's_34_18', 's_34_28', 's_34_29', 31, 's_34_31', 33, 's_34_33', 's_34_34', 's_41_1', 's_41_3', 's_41_4', 's_41_14', 's_41_18', 's_41_29', 's_41_32', 's_41_46', 's_41_41', 's_47_10', 's_47_12', 22, 's_47_22', 's_47_29', 's_47_32', 's_47_37', 's_47_43', 's_47_46', 's_47_47', 's_9_4', 's_9_10', 's_9_18', 's_9_26', 's_9_42', 's_9_48', 's_9_3', 's_9_40', 's_9_15', 's_9_16', 's_9_24', 's_9_32', 's_9_35', 's_9_36', 's_9_37', 's_9_9', 's_13_1', 's_13_10', 's_13_11', 's_13_15', 's_13_24', 's_13_28', 's_13_31', 's_13_37', 's_13_38', 's_13_39', 's_13_46', 's_13_13', 's_14_10', 's_14_28', 's_14_48', 's_14_5', 's_14_8', 's_14_11', 's_14_22', 's_14_45', 's_14_19', 's_14_31', 's_14_37', 's_14_14', 's_15_26', 's_15_29', 's_15_42', 's_15_3', 's_15_12', 's_15_20', 's_15_31', 's_15_36', 's_15_37', 's_15_38', 's_15_46', 's_15_15', 's_29_1', 's_29_4', 's_29_10', 's_29_18', 6, 's_29_6', 's_29_11', 's_29_12', 's_29_16', 's_29_19', 's_29_38', 's_29_29', 's_36_28', 's_36_6', 's_36_39', 's_36_40', 's_36_12', 's_36_16', 's_36_35', 's_36_36', 's_5_2', 's_5_4', 's_5_10', 's_5_48', 's_5_12', 's_5_39', 's_5_40', 's_5_45', 's_5_5', 's_12_18', 's_12_39', 's_12_49', 's_12_33', 's_12_16', 's_12_38', 's_12_43', 's_12_46', 's_12_12', 's_18_1', 's_18_6', 's_18_11', 's_18_19', 's_18_20', 's_18_28', 's_18_38', 's_18_40', 's_18_45', 's_18_46', 's_18_48', 's_18_18', 's_19_28', 's_19_3', 's_19_6', 's_19_8', 's_19_40', 44, 's_19_44', 's_19_32', 's_19_33', 's_19_37', 's_19_49', 's_19_19', 's_20_4', 's_20_26', 's_20_39', 's_20_44', 's_20_45', 's_20_35', 's_20_38', 's_20_20', 's_28_1', 's_28_26', 's_28_8', 's_28_40', 's_28_42', 's_28_43', 's_28_45', 's_28_28', 's_35_26', 's_35_8', 's_35_22', 's_35_40', 's_35_24', 's_35_32', 's_35_38', 's_35_37', 's_35_35', 's_39_2', 's_39_8', 's_39_31', 's_39_33', 's_39_49', 's_39_39', 's_40_2', 's_40_42', 's_40_11', 's_40_24', 's_40_31', 's_40_33', 's_40_37', 's_40_44', 's_40_40', 's_49_10', 's_49_3', 's_49_6', 's_49_16', 's_49_49', 's_8_2', 's_8_48', 's_8_3', 's_8_8', 's_4_1', 's_4_2', 's_4_6', 's_4_24', 's_4_31', 's_4_33', 's_4_42', 's_4_48', 's_4_4', 's_11_2', 's_11_26', 's_11_48', 's_11_22', 's_11_32', 's_11_33', 's_11_37', 's_11_11', 's_37_26', 's_37_42', 's_37_48', 's_37_45', 's_37_31', 's_37_37', 's_42_1', 's_42_6', 's_42_16', 's_42_31', 's_42_42', 's_43_22', 's_43_16', 's_43_38', 's_43_43', 's_1_2', 's_1_10', 's_1_26', 's_1_48', 's_1_1', 's_2_3', 's_2_6', 's_2_22', 's_2_26', 's_2_44', 's_2_45', 's_2_2', 's_3_48', 's_3_24', 's_3_3', 's_10_26', 's_10_32', 's_10_48', 's_10_10', 's_26_33', 's_26_44', 's_26_26', 's_46_6', 's_46_44', 's_46_31', 's_46_38', 's_46_46', 's_48_33', 's_48_48', 's_16_6', 's_16_22', 's_16_33', 's_16_32', 's_16_16', 's_24_45', 's_24_24', 's_32_6', 's_32_22', 's_32_44', 's_32_38', 's_32_32', 's_38_6', 's_38_22', 's_38_44', 's_38_38', 's_45_22', 's_45_45', 's_31_6', 's_31_44', 's_31_33', 's_31_31', 's_33_22', 's_33_33', 's_22_22', 's_6_6', 's_44_44']</t>
-        </is>
-      </c>
-      <c r="AS7" t="inlineStr">
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>[0, 7, 's_0_7', 17, 's_0_17', 21, 's_0_21', 23, 's_0_23', 25, 's_0_25', 27, 's_0_27', 30, 's_0_30', 34, 's_0_34', 41, 's_0_41', 47, 's_0_47', 9, 's_7_9', 13, 's_7_13', 14, 's_7_14', 15, 's_7_15', 's_7_25', 29, 's_7_29', 36, 's_7_36', 5, 's_5_17', 's_9_17', 12, 's_12_17', 's_14_17', 's_15_17', 18, 's_17_18', 19, 's_17_19', 20, 's_17_20', 28, 's_17_28', 's_17_29', 35, 's_17_35', 39, 's_17_39', 40, 's_17_40', 's_17_41', 49, 's_17_49', 8, 's_8_21', 's_18_21', 's_21_23', 's_21_34', 4, 's_4_23', 's_5_23', 's_9_23', 11, 's_11_23', 's_13_23', 's_20_23', 's_23_30', 's_23_34', 's_23_36', 37, 's_23_37', 's_23_39', 42, 's_23_42', 43, 's_23_43', 1, 's_1_25', 2, 's_2_25', 3, 's_3_25', 10, 's_10_25', 's_12_25', 's_20_25', 26, 's_25_26', 's_25_37', 's_25_40', 's_25_42', 46, 's_25_46', 48, 's_25_48', 's_1_27', 's_4_27', 's_8_27', 's_10_27', 's_14_27', 's_15_27', 16, 's_16_27', 's_18_27', 24, 's_24_27', 's_27_29', 32, 's_27_32', 's_27_37', 38, 's_27_38', 's_27_39', 's_27_43', 45, 's_27_45', 's_4_30', 's_8_30', 's_19_30', 's_30_40', 's_30_42', 's_1_34', 's_2_34', 's_3_34', 's_9_34', 's_15_34', 's_18_34', 's_28_34', 's_29_34', 31, 's_31_34', 33, 's_33_34', 's_1_41', 's_3_41', 's_4_41', 's_14_41', 's_18_41', 's_29_41', 's_32_41', 's_41_46', 's_10_47', 's_12_47', 22, 's_22_47', 's_29_47', 's_32_47', 's_37_47', 's_43_47', 's_46_47', 's_1_2', 's_1_4', 's_1_10', 's_1_13', 's_1_18', 's_1_26', 's_1_28', 's_1_29', 's_1_42', 's_1_48', 's_2_3', 's_2_4', 's_2_5', 6, 's_2_6', 's_2_8', 's_2_11', 's_2_22', 's_2_26', 's_2_39', 's_2_40', 44, 's_2_44', 's_2_45', 's_4_5', 's_4_6', 's_4_9', 's_4_20', 's_4_24', 's_4_29', 's_4_31', 's_4_33', 's_4_42', 's_4_48', 's_5_10', 's_9_10', 's_10_13', 's_10_14', 's_10_26', 's_10_29', 's_10_32', 's_10_48', 's_10_49', 's_11_13', 's_13_15', 's_13_24', 's_13_28', 's_13_31', 's_13_37', 's_13_38', 's_13_39', 's_13_46', 's_6_18', 's_9_18', 's_11_18', 's_12_18', 's_18_19', 's_18_20', 's_18_28', 's_18_29', 's_18_38', 's_18_40', 's_18_45', 's_18_46', 's_18_48', 's_9_26', 's_11_26', 's_15_26', 's_20_26', 's_26_28', 's_26_33', 's_26_35', 's_26_37', 's_26_44', 's_8_28', 's_14_28', 's_19_28', 's_28_36', 's_28_40', 's_28_42', 's_28_43', 's_28_45', 's_6_29', 's_11_29', 's_12_29', 's_15_29', 's_16_29', 's_19_29', 's_29_38', 's_6_42', 's_9_42', 's_15_42', 's_16_42', 's_31_42', 's_37_42', 's_40_42', 's_3_48', 's_5_48', 's_8_48', 's_9_48', 's_11_48', 's_14_48', 's_33_48', 's_37_48', 's_3_8', 's_3_9', 's_3_15', 's_3_19', 's_3_24', 's_3_49', 's_5_12', 's_5_14', 's_5_39', 's_5_40', 's_5_45', 's_6_16', 's_6_19', 's_6_31', 's_6_32', 's_6_36', 's_6_38', 's_6_46', 's_6_49', 's_8_14', 's_8_19', 's_8_35', 's_8_39', 's_11_14', 's_11_22', 's_11_32', 's_11_33', 's_11_37', 's_11_40', 's_14_22', 's_16_22', 's_22_32', 's_22_33', 's_22_35', 's_22_38', 's_22_43', 's_22_45', 's_12_39', 's_20_39', 's_31_39', 's_33_39', 's_36_39', 's_39_49', 's_9_40', 's_19_40', 's_24_40', 's_31_40', 's_33_40', 's_35_40', 's_36_40', 's_37_40', 's_40_44', 's_19_44', 's_20_44', 's_31_44', 's_32_44', 's_38_44', 's_44_46', 's_14_45', 's_20_45', 's_24_45', 's_37_45', 's_9_15', 's_9_16', 's_9_24', 's_9_32', 's_9_35', 's_9_36', 's_9_37', 's_12_15', 's_15_20', 's_15_31', 's_15_36', 's_15_37', 's_15_38', 's_15_46', 's_14_19', 's_19_32', 's_19_33', 's_19_37', 's_19_49', 's_24_35', 's_12_49', 's_16_49', 's_20_35', 's_20_38', 's_14_31', 's_31_33', 's_31_37', 's_31_46', 's_12_33', 's_16_33', 's_12_16', 's_12_36', 's_12_38', 's_12_43', 's_12_46', 's_14_37', 's_16_32', 's_16_36', 's_16_43', 's_32_35', 's_32_38', 's_35_36', 's_35_38', 's_38_43', 's_38_46', 's_35_37']</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
         <is>
           <t>[0, 7, 17, 21, 23, 25, 27, 30, 34, 41, 47, 9, 13, 14, 15, 29, 36, 5, 12, 18, 19, 20, 28, 35, 39, 40, 49, 8, 4, 11, 37, 42, 43, 1, 2, 3, 10, 26, 46, 48, 16, 24, 32, 38, 45, 31, 33, 22, 6, 44]</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>